<commit_message>
Refactor and fix all data file names - move old data files to archive folder - change file names - supersites_region_geom.geojson - supersites_location_geom_2024.geojson - supersites_geom_2024.xlsx - venues_all_years_fixed.xlsx - supersite_map.js
</commit_message>
<xml_diff>
--- a/data/supersites_geom_2024.xlsx
+++ b/data/supersites_geom_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,65 +446,55 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.1</t>
+          <t>Venue</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>address</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Venue</t>
+          <t>organization</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>address</t>
+          <t>website</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>organization</t>
+          <t>google_map_link</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>website</t>
+          <t>google_map_name</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>google_map_link</t>
+          <t>lat</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>google_map_name</t>
+          <t>lon</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>lat</t>
+          <t>google_map_url</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>lon</t>
+          <t>website_url</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>google_map_url</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>website_url</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>location_geom</t>
         </is>
@@ -524,55 +514,49 @@
           <t>POLYGON ((-105.3383475896821 40.25279579827692, -105.3382794314722 40.25524525249802, -105.3381412199228 40.25881617856658, -105.3381829609955 40.26243240924209, -105.3381828979697 40.26243567209774, -105.3478002549402 40.26237901406024, -105.3479202448766 40.26237941764173, -105.3480531934493 40.2623798651291, -105.3480609959063 40.26237989068174, -105.3483753054478 40.26238094047059, -105.3483831137831 40.26238096600925, -105.3502716880137 40.26238727182132, -105.3502795316186 40.26238729727766, -105.3574027486471 40.26241077828855, -105.3620853399815 40.26241822105709, -105.3620933905265 40.26241823335076, -105.3672010594676 40.26242613784095, -105.3672092063966 40.26242615889559, -105.3719103561596 40.26243791500907, -105.3719185889108 40.26243793582719, -105.3766294256697 40.26244652003982, -105.3766298418329 40.26244652138401, -105.3768931198172 40.26244699532722, -105.3769018181211 40.26244701088236, -105.3814089843745 40.26106398454443, -105.3814148842667 40.26106217584215, -105.3856822884296 40.25975451154127, -105.389306418282 40.25868505833365, -105.3893126034273 40.25868324139569, -105.3920579591849 40.25787665318066, -105.3920641982831 40.25787481993468, -105.3924852901653 40.25775109572469, -105.3924896028312 40.25774982805633, -105.392492463916 40.25774917956623, -105.3924926331846 40.25774918422654, -105.3925017878451 40.25774940437503, -105.3942308924439 40.25779098039329, -105.3942396415731 40.25779119102752, -105.3962976245635 40.25784063924261, -105.3963064113209 40.25784085065493, -105.3969000271832 40.25785510728947, -105.3969088233486 40.25785531866444, -105.4015359961488 40.25796628527932, -105.4015360784346 40.25796628624992, -105.404327806051 40.25801654858331, -105.4043367140068 40.25801670905149, -105.4059574231582 40.25804585556789, -105.4059663605099 40.2580460159345, -105.4107477294264 40.25813203184654, -105.4155198889819 40.25829770498576, -105.4155290636505 40.25829802329604, -105.4203330852328 40.25846415434641, -105.4251861794957 40.25840726140195, -105.4251953382348 40.25840715384359, -105.4294812217399 40.2583567394641, -105.4294904615783 40.25835663071469, -105.4295536757102 40.25835588566847, -105.4295629143729 40.25835577691257, -105.4298646896997 40.25835280079793, -105.4299225583033 40.25835581509605, -105.4299320479088 40.25835630897658, -105.4305133050051 40.25838657975033, -105.4305228051982 40.25838707448938, -105.4306757416342 40.25839503849969, -105.4306852441799 40.2583955341274, -105.4307426027005 40.25839852069145, -105.430752107599 40.25839901541449, -105.4308077781424 40.25840191357626, -105.4308172818664 40.25840240829324, -105.4322794064476 40.25847853230823, -105.4322889360531 40.25847902872076, -105.4323419078253 40.25848178857227, -105.4323514409584 40.25848228498171, -105.4324151589678 40.25848560045744, -105.4324246932774 40.2584860968615, -105.4345929559632 40.25859894893045, -105.4346025279193 40.25859944787823, -105.4369612784415 40.25872217258483, -105.4369708915756 40.25872267225978, -105.4393363255669 40.25884516486855, -105.4409258012767 40.25883700876198, -105.4409352809209 40.25883695956276, -105.4434546744453 40.25882398712621, -105.4434642011069 40.25882393864347, -105.4443764377183 40.25881922909699, -105.4443859820117 40.25881918054682, -105.4462974984619 40.25880928571338, -105.4463070780196 40.25880923612055, -105.4476086573605 40.25880271230612, -105.4522696778767 40.25889905814066, -105.4522794676884 40.2588992603134, -105.457320490272 40.25900313029224, -105.4620166225517 40.2590381363858, -105.4620265441448 40.25903821079019, -105.4638404081088 40.25905168042018, -105.4638503614461 40.25905175377748, -105.4671613666072 40.25907632231434, -105.4714882186452 40.25913474836782, -105.4714983353781 40.25913488415101, -105.4763999511735 40.25920087241619, -105.4764101572673 40.2592010095895, -105.4808091579479 40.25926021774424, -105.4808194451724 40.25926035544283, -105.4856590016976 40.25932525952785, -105.4900841554215 40.25936213161643, -105.4900945931585 40.25936221806891, -105.4914674244207 40.25937362026658, -105.4914778868478 40.25937370749673, -105.4949090741289 40.25940296772085, -105.4993103492368 40.25992138523038, -105.4993210915308 40.25992265066251, -105.5029085134606 40.26034512851926, -105.502931935669 40.26034788652174, -105.5041307628281 40.26048828783482, -105.5088612768845 40.26059839940055, -105.5088719511472 40.26059864715346, -105.5136047435574 40.26070861601637, -105.5136154296108 40.26070886513165, -105.5183519417781 40.26081923745897, -105.5183626384468 40.26081948703492, -105.5231001382505 40.26092971894171, -105.5246476950239 40.2609710938596, -105.525269431533 40.26098771039094, -105.5273444115898 40.26104314285998, -105.5273551400827 40.26104342942336, -105.5274352605084 40.26104556924201, -105.5274459878262 40.26104585489666, -105.5321867141913 40.2611723584543, -105.5321974533053 40.26117264456591, -105.5325643454667 40.2611824271107, -105.5325750857591 40.26118271228633, -105.5358139134438 40.2612686678133, -105.5374657135926 40.26131247066026, -105.5374700080801 40.26131258454924, -105.5374807589939 40.26131286926624, -105.5376060021513 40.26131618794863, -105.5376167542434 40.26131647535446, -105.5377707903809 40.26132060406002, -105.5377815436505 40.2613208923508, -105.5420407296155 40.26143500096256, -105.5420510583876 40.26143505394957, -105.5420123310872 40.26132699564431, -105.5419533310875 40.25691899504218, -105.5418693303538 40.25068399588682, -105.5417913293522 40.24484599488542, -105.5417703294095 40.24320999597101, -105.5418212665354 40.24069807142973, -105.5420429039838 40.2322667322377, -105.542057627296 40.22872637662191, -105.5420562713165 40.22872637531357, -105.5420822364319 40.22507980477056, -105.5420823229212 40.22506767874194, -105.5420808495041 40.22506765406047, -105.5419590751946 40.22506557191936, -105.5419484417806 40.22506555326001, -105.5405764553367 40.22506318763808, -105.5385255461858 40.22505961624928, -105.5374809703504 40.2250577834895, -105.5373800222655 40.2250576054056, -105.536760204845 40.22505651522585, -105.5364318357178 40.22505593462795, -105.5364251454815 40.22505592322528, -105.5360637775385 40.22505528352068, -105.5353538558136 40.22505402382836, -105.5344553890728 40.22505242161549, -105.5326910735317 40.22504859983672, -105.5326820404199 40.22504857987344, -105.5326825303639 40.22418840574673, -105.5326967674883 40.2233561262393, -105.5326849473221 40.2214446523428, -105.5326849358092 40.22144269979285, -105.5333207578963 40.22144445293673, -105.5338911592008 40.22144602273305, -105.5348769137664 40.22144872610919, -105.5360049453737 40.2214518136923, -105.5360297782496 40.21982080776719, -105.5364610049816 40.21977874858243, -105.536469145231 40.2197779543675, -105.5364659849748 40.21975632326548, -105.5364658151693 40.21975515971221, -105.5378566567431 40.21962890467403, -105.5379291219123 40.21962350240685, -105.5379809748795 40.21961963612427, -105.5398831425591 40.21944693342513, -105.5411373910101 40.21826779544625, -105.5422084115658 40.21794388539156, -105.5422524668593 40.21422603345813, -105.5422526119581 40.21421377049138, -105.5326985284376 40.21419413237972, -105.5326895026425 40.21419411331591, -105.5326894995797 40.21419262998702, -105.5326902668153 40.21217981128849, -105.5326905761208 40.21136213502758, -105.5326905760758 40.21136204136256, -105.5326909158406 40.21046358966055, -105.5404398525206 40.21053711938241, -105.5422860075863 40.21055412132916, -105.5422953313193 40.21055420708196, -105.5423441034594 40.20698849445215, -105.5423441045886 40.20698842150102, -105.5469038813974 40.20702247197197, -105.5471669256137 40.20702443013139, -105.5471762500321 40.20702449927905, -105.5471710649767 40.20342824622806, -105.5471617411033 40.203428251832, -105.5424019515685 40.20343087127191, -105.542401834668 40.20341858226157, -105.5423929265994 40.20341858732859, -105.5423024628827 40.19394992984792, -105.5422970925746 40.19338779750338, -105.542297092536 40.19338773536003, -105.5422833975938 40.19195401206859, -105.5422833975333 40.19195391480071, -105.5422758519701 40.1911640951709, -105.5422571009006 40.18920076026023, -105.5422569890588 40.18918897106952, -105.541762862168 40.1891617345586, -105.5375946466315 40.18889544853639, -105.5375677880135 40.18893092853408, -105.537254321171 40.18934499589563, -105.5372715249519 40.18934647278628, -105.5375223216064 40.1893679950532, -105.5375224677095 40.18937951494874, -105.5375433224156 40.1910399954814, -105.5375101454505 40.19106602720946, -105.5375025897888 40.19185229996346, -105.537495561658 40.19258391871914, -105.5349909777208 40.19246710871604, -105.5349371865247 40.19249180670148, -105.5348823209668 40.19251699672893, -105.5346356497051 40.19259680260618, -105.5343393829121 40.19281390637015, -105.5342271532779 40.19272517011618, -105.5342180715312 40.19271798939261, -105.5342183360385 40.19269518000148, -105.5342183473157 40.19269425235101, -105.5342193376537 40.19260852935302, -105.5342198678148 40.19256285923371, -105.5342200411473 40.19254790514945, -105.5341957862916 40.19255495433799, -105.5341047369489 40.19258913845898, -105.5340122329798 40.19262441809995, -105.5339501238616 40.19264610006633, -105.533890165039 40.19266779307718, -105.5338179414305 40.19269327228345, -105.5337565232855 40.19271606081569, -105.533684251341 40.19274374108799, -105.5336515583924 40.19275577849825, -105.5336459058447 40.19275785969391, -105.5336091149603 40.19277140683688, -105.5335304733625 40.19279520175227, -105.5334323856855 40.19282329373202, -105.5333357318797 40.19285139332066, -105.5332445784334 40.19289053114875, -105.5331549173888 40.1929269242624, -105.5330790606768 40.1929545853694, -105.5330083598834 40.19297567307023, -105.5329570730651 40.19299410915016, -105.5328935660998 40.19301413198865, -105.5328294254024 40.19303029578, -105.5328098787648 40.19303559882346, -105.5328006690869 40.1930380970772, -105.5328018956497 40.19294170518686, -105.5328019262174 40.19293933922767, -105.5328090737093 40.1923771568957, -105.5328092241853 40.19236530368316, -105.5327720701403 40.19236356970227, -105.5327628767569 40.19236313910528, -105.5327760272405 40.19144611821562, -105.5328026033848 40.18959315645375, -105.5328144473783 40.1887670954498, -105.5328252743849 40.18844763660821, -105.5328252778692 40.18844755645122, -105.5328963810823 40.18678931519381, -105.532976230018 40.18492700366666, -105.5330262556054 40.1837602446121, -105.5331269808046 40.18141083850799, -105.5332266806333 40.17753671869425, -105.5332269975165 40.17752442499798, -105.5331662580995 40.17752449827886, -105.5331568626344 40.17752450998029, -105.5331893193217 40.17646799626176, -105.5332742031089 40.1738843189681, -105.5332746068535 40.17387203604751, -105.5332652858553 40.17387203873018, -105.5258340931253 40.17387231809113, -105.5258247721261 40.17387231837259, -105.5238776530766 40.17387231186575, -105.5237857437776 40.17749800315436, -105.5237651645466 40.17831101269118, -105.5237510683669 40.17886786445666, -105.5237454789506 40.17908870192743, -105.5237413580885 40.17925150068127, -105.5237197330747 40.18010577977868, -105.5237041709683 40.18072051517435, -105.5236896753479 40.18129311342297, -105.523688178229 40.1812930930153, -105.523680357985 40.181292988343, -105.5224378823772 40.18127630972313, -105.5224377955276 40.18127643582816, -105.522435320304 40.18127999739902, -105.5222435741154 40.18127382730909, -105.5222435283211 40.18127382641728, -105.522236754261 40.18127360796668, -105.5208006874244 40.18122739465633, -105.5207705453987 40.18122672640443, -105.5138093385616 40.18107228813918, -105.5115988430433 40.18102320894966, -105.5066788071574 40.18091382279687, -105.5037971648563 40.18084965648772, -105.4988689323545 40.18060051532034, -105.4942254027887 40.18036558420872, -105.4942081234937 40.18036470973328, -105.4938523205461 40.18035299938223, -105.4938523169958 40.18035330559622, -105.4938123200268 40.18389599982997, -105.4938093397902 40.1838958852905, -105.493803003558 40.18389564358236, -105.4916169415424 40.18381225335324, -105.4913673103303 40.18380308278645, -105.4890342964373 40.18371735136233, -105.4887108236855 40.18370645233315, -105.4858596675139 40.18361035232417, -105.4843017355777 40.18355781209871, -105.4842927315417 40.18355750826427, -105.4842923359611 40.18291119120383, -105.4842919357208 40.18225457717938, -105.4842909836418 40.18069288673419, -105.484290852698 40.18047691385383, -105.4842905938626 40.18005209836011, -105.4842904845098 40.17987483273979, -105.4842904768209 40.17986236891954, -105.4821456944617 40.17990478346833, -105.4809104417855 40.17992919131213, -105.4809046495147 40.17992930563622, -105.479611783183 40.17995483837693, -105.4796026937846 40.17995501780022, -105.4796152483834 40.17796396985926, -105.4796240684069 40.17656529689094, -105.4796805373642 40.17330482726621, -105.4797733872597 40.16988566754004, -105.4797734359278 40.16988387259018, -105.4797873653326 40.16937091048318, -105.479787691759 40.16935887360058, -105.4752042504024 40.16923656802826, -105.4750210361202 40.17237698847438, -105.4750206722191 40.17238323337168, -105.4750032321987 40.1726821562563, -105.4749708600473 40.17323704782745, -105.4727391684574 40.17317988978623, -105.471439289043 40.1731465768118, -105.4711861857428 40.17314008889846, -105.470709432716 40.1731278654992, -105.470200732758 40.17311482223527, -105.4701498775658 40.17311351851009, -105.4701398981323 40.17311326375602, -105.470147089627 40.17302417969756, -105.4701471120568 40.17302390050776, -105.4703235422809 40.17083798352486, -105.4704014266738 40.1698729832864, -105.4704561694049 40.16919470380456, -105.4704672528061 40.1690710003927, -105.4705125686798 40.16856524699041, -105.4707617862852 40.16578366217297, -105.4707617910061 40.16578360363307, -105.4708146541582 40.16519354991458, -105.470815740543 40.16518143398583, -105.46628891067 40.16510477709761, -105.4661484313311 40.16510540791135, -105.4661390192035 40.16575318835307, -105.4661360291954 40.16575316856382, -105.4661360034201 40.16575542373876, -105.4661389863847 40.16575544352597, -105.4661041161459 40.16599498340007, -105.4659122147164 40.16731319895921, -105.4656564837945 40.16906980083949, -105.4654595827187 40.17042224296217, -105.4654156772836 40.17072380804591, -105.4653390047136 40.17125043193705, -105.4650859317025 40.17298856399155, -105.4650278923397 40.17298779802273, -105.465020799437 40.17303651100915, -105.4650205696819 40.17303809154707, -105.4639674508512 40.17302419196477, -105.4551151660433 40.17290698011092, -105.4548676764149 40.17289810889962, -105.4460938038541 40.17258326152695, -105.4460938893231 40.17258504211464, -105.4461030764639 40.17277599101477, -105.4464328855671 40.17963012402592, -105.4467706877612 40.18691469756227, -105.4467707570555 40.18691618453304, -105.4562018644992 40.18738200961488, -105.4654274239811 40.18748873382307, -105.4654337392727 40.18798117173748, -105.4660768702116 40.18800936007144, -105.4655238635754 40.19500728610073, -105.4649952892548 40.20169467125756, -105.4649758233132 40.20194092921771, -105.4474170601683 40.20137233213854, -105.4472734418836 40.20136766994612, -105.447226697916 40.22921312441949, -105.4391980447536 40.22936945487155, -105.4216202374492 40.22919080099819, -105.4200940059783 40.22911348585162, -105.4156150536366 40.22888699158656, -105.4156135450612 40.22912913839541, -105.415475085733 40.22912771340392, -105.4154249119026 40.22912767673616, -105.4154032237782 40.23260784691084, -105.4146656795209 40.23257685252141, -105.4110641024067 40.23242806717199, -105.4110586742406 40.23267442569232, -105.4109241110912 40.23266878334061, -105.4107917390044 40.23854881554955, -105.4106350047693 40.24360757533661, -105.4077967243588 40.24357879200166, -105.4078014258309 40.24362964482339, -105.4076809304183 40.24362842117775, -105.4061610915533 40.24361252845856, -105.4062353345834 40.2472014281798, -105.4061687067422 40.24720049697125, -105.3969333339457 40.24707105012143, -105.3966897457939 40.24346376519367, -105.3957980869377 40.24345499160201, -105.3920182790535 40.24341772408644, -105.3920307022783 40.24383753423813, -105.3920155279506 40.24341610220183, -105.3920154663501 40.24337721060778, -105.3772575504983 40.24783662782211, -105.3579966972145 40.24799691433613, -105.3385839153525 40.24791229438405, -105.3385811986579 40.24812077097913, -105.338448737321 40.25124619151066, -105.3384298201 40.25169256512352, -105.3384279523157 40.25173657136099, -105.3383900936446 40.25262978135259, -105.3383510062346 40.25260183093391, -105.3383475896821 40.25279579827692))</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Allenspark Fire Station</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>14861 CO-7, Allenspark, CO 80510</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
-          <t>14861 CO-7, Allenspark, CO 80510</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>http://www.allensparkfire.com/</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>Allenspark Fire Protection</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>40.19712777610975</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-105.5279141785934</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>http://www.allensparkfire.com/</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Allenspark Fire Protection</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>40.19712777610975</v>
-      </c>
-      <c r="M2" t="n">
-        <v>-105.5279141785934</v>
-      </c>
       <c r="N2" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>http://www.allensparkfire.com/</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
         <is>
           <t>POINT (-105.5279141785934 40.19712777610975)</t>
         </is>
@@ -592,59 +576,53 @@
           <t>POLYGON ((-105.1462091902176 40.1287254615651, -105.1463811910671 40.1286814612758, -105.1465091905153 40.1286324608168, -105.1466521909948 40.12851646037345, -105.1467601907007 40.12837346040647, -105.1469681918037 40.12816546030267, -105.1471681902714 40.12801146050332, -105.1473611912454 40.12789646119431, -105.1474471915002 40.12785746102228, -105.1476831913874 40.12780346061299, -105.1478051914117 40.1277864601138, -105.1479051910319 40.12776446140642, -105.1480411907711 40.12775946117674, -105.148131047267 40.12775946111901, -105.1483701909708 40.12775946068273, -105.1484921909401 40.12776446038666, -105.1486281913429 40.12777546030672, -105.1488141912797 40.12775946127093, -105.1489711913174 40.12773246071522, -105.1490791919685 40.12769346043497, -105.1493501918869 40.12752346094415, -105.1498021911529 40.12714446046252, -105.1501191918396 40.1269784605735, -105.1503821911598 40.12695246089658, -105.1508891916811 40.12694046027134, -105.1513948839501 40.12694194872075, -105.1527758874465 40.12694600356159, -105.154300191837 40.12695046002028, -105.1548092204482 40.12693493214863, -105.1549821926101 40.12692646047514, -105.1550255475185 40.12692646026373, -105.1552101930545 40.12692646033931, -105.155437192927 40.12695445958236, -105.1555461931968 40.12695945989714, -105.1556001924722 40.12702245971152, -105.1555921921127 40.12707946011266, -105.15561919262 40.12719845979632, -105.1556931920723 40.12731245959085, -105.1557801926516 40.12740145928399, -105.1559481928024 40.12743746043777, -105.1563391925392 40.1276614597395, -105.1565141933392 40.12771445982453, -105.1565956562976 40.12772766228106, -105.1568041930755 40.12776145992218, -105.1571021940422 40.12773645947969, -105.1572911938164 40.12771146007818, -105.1574571934914 40.12767945991541, -105.1576939255081 40.12766480027194, -105.1578931932202 40.12765245913534, -105.1581221932529 40.12766346026724, -105.1583881937712 40.12771545958289, -105.1587271935286 40.12775946009889, -105.1590381943059 40.12775145938977, -105.1591931935459 40.12775345958096, -105.159295194393 40.12773946004652, -105.1593321942806 40.12776146020572, -105.1593099156614 40.12782736753463, -105.1593961945012 40.12792145999537, -105.1594101940028 40.12802046036595, -105.1593961948648 40.12808645966798, -105.1593311943713 40.12824045994564, -105.1593241941156 40.12833945963551, -105.1593311935832 40.1284274605238, -105.1594381937382 40.12879546005235, -105.1594881935436 40.12887746060884, -105.159567194188 40.1289214593066, -105.159667193892 40.12894945954594, -105.1598101948547 40.12896045970615, -105.1599321943844 40.1289494599988, -105.1601261845107 40.12889596708893, -105.1602477556501 40.1288630990707, -105.1603761943632 40.1288334601072, -105.1604831934606 40.12878445990846, -105.1620093210164 40.12797305594989, -105.1625441952281 40.1276864588521, -105.1627091942639 40.12764845894845, -105.1627731945469 40.12760446023837, -105.1628381942516 40.1275384598923, -105.1629311946616 40.12746646007216, -105.1633531947814 40.12731345908721, -105.1636321946816 40.12720345937235, -105.1644421950803 40.12692945902451, -105.1648051947436 40.12681345989837, -105.1653700089539 40.12664755526463, -105.1658119066372 40.12652845903283, -105.1665941954893 40.12633345884351, -105.1665751958297 40.1268584592293, -105.1665921947485 40.12690745915487, -105.166642195758 40.12696145922249, -105.1667081954379 40.12699345858284, -105.1667741949328 40.12700345879298, -105.1687057057889 40.12700441568506, -105.1687951961079 40.12700445884948, -105.1688701962396 40.1270274592329, -105.168898196283 40.12704245954604, -105.1689571957668 40.12709045909411, -105.1689921957212 40.12714645870656, -105.1690031954348 40.12720745836092, -105.1689281965424 40.13055845919673, -105.1689125986237 40.1306329048518, -105.1689124571838 40.13066294718519, -105.168948196977 40.1306634594016, -105.1763945382965 40.13068560471505, -105.1783901991411 40.13068445895293, -105.1784921990268 40.13071445866245, -105.1785511991025 40.13076045923802, -105.1785684592082 40.13078897836895, -105.1785641690483 40.13079204933064, -105.1785020389263 40.13084705429363, -105.1784840588681 40.13086786763377, -105.1784548908681 40.13091006260262, -105.178444049129 40.13093391475787, -105.1784339246554 40.13095694572148, -105.178427016947 40.13098108442205, -105.1784229738302 40.13100413231251, -105.1784189256439 40.1310280042764, -105.1784180942343 40.13105298307757, -105.1784131673081 40.13194404858856, -105.1783999480014 40.13330396605977, -105.1783991396833 40.1337020124477, -105.1784048791175 40.13377395099028, -105.1783991093832 40.13408688368758, -105.1783958547979 40.13492689429661, -105.1783961618531 40.13508913406532, -105.1783948972642 40.13528101768208, -105.1783940230415 40.13644990497878, -105.178390832764 40.13742799644631, -105.1783857569761 40.13792377194132, -105.1783856925215 40.13792375374909, -105.1783808185894 40.13938497043898, -105.178379409163 40.13975199673494, -105.1783763784656 40.14133788851696, -105.1783763779464 40.14133799839369, -105.1783713737261 40.14226699561438, -105.1783533903674 40.14336199241301, -105.1783493436875 40.14413299714823, -105.1783547608992 40.14414764583766, -105.178355161728 40.14414850346271, -105.1783513876863 40.14416088307052, -105.1783507230336 40.14416221146657, -105.1783483399981 40.14435999722787, -105.1783373495214 40.14522699350773, -105.178337307856 40.14535299840424, -105.1783402810778 40.14660499955411, -105.1783343699196 40.1478468345418, -105.1783342828933 40.1478649966097, -105.1783342685619 40.14786827670135, -105.1783322539086 40.14912099754154, -105.1783316896897 40.14922173345824, -105.1783252470594 40.15034799549664, -105.1783262111119 40.15130500003102, -105.1783232044195 40.15240999729076, -105.1783233146343 40.15242367651192, -105.1783301522852 40.15303800468062, -105.1783291792601 40.15375999780937, -105.1783012893748 40.15590656871396, -105.1783011802659 40.1559149983927, -105.1783005822134 40.15597644463524, -105.1782971626988 40.15633399335119, -105.1782960871354 40.15719749425114, -105.1782960854515 40.15719884340366, -105.1782960843966 40.15719956301125, -105.1782951121814 40.15799899804473, -105.178294217315 40.15818577184383, -105.1782870964684 40.15965399674796, -105.1782862950887 40.15989422276495, -105.1782860862953 40.15995699669625, -105.1782851194905 40.16030891223458, -105.1782850786808 40.16032399691657, -105.178284679339 40.16043600372073, -105.1782749234563 40.16315591889484, -105.178274033215 40.16340399540454, -105.1782655161564 40.1650051485672, -105.1782579902131 40.16641899487397, -105.1782538706628 40.16695343985297, -105.1735772011636 40.16694246349251, -105.1735112021403 40.16875746475598, -105.1735104074165 40.16876894654175, -105.1734888774345 40.16876895687698, -105.1734876717343 40.1687689579743, -105.1734854970979 40.16912908258862, -105.1734767013714 40.17058610997677, -105.1734766984293 40.17058819044085, -105.1734768239046 40.17088245964705, -105.1734768197971 40.17088453830642, -105.1733657812711 40.17083213172842, -105.1733576954174 40.17082828027013, -105.1729529231051 40.17063241614367, -105.1728205681745 40.1705683728318, -105.1728195198593 40.17056786550766, -105.1687255340658 40.16858670852341, -105.1687256438738 40.1685916425322, -105.1687231045455 40.16859477217606, -105.1677518350548 40.16979169341922, -105.1677465944088 40.16979815123889, -105.167035661948 40.17067421828263, -105.167026766362 40.17067109176306, -105.1670240178124 40.17067447924944, -105.1669332093008 40.17078637943621, -105.1669304607418 40.17078976692029, -105.1668896186171 40.17084009214113, -105.1668985520034 40.17084317464879, -105.1668943955052 40.17084829540469, -105.1668849048761 40.17085999075397, -105.1665201919034 40.17073175740313, -105.1665174951051 40.17073080935722, -105.1664129896231 40.17079382714124, -105.1650199693466 40.17032183177924, -105.1642709600386 40.17007883540592, -105.1642169582605 40.17006083511097, -105.1640679558686 40.16999983608142, -105.1638209526211 40.16989583642651, -105.1637179519749 40.16985083726004, -105.1635209475333 40.16973283788921, -105.1631259398792 40.16948983996239, -105.1622709235831 40.1688868436568, -105.161120902206 40.16807485153609, -105.1602088846895 40.16741385793949, -105.1599118790576 40.16721485751804, -105.1598118775726 40.1671618596847, -105.1596798760458 40.16712085952145, -105.1595208740774 40.16707385977891, -105.1593498721462 40.16705286010649, -105.1572978539927 40.16702986225165, -105.1562688454048 40.16703286263721, -105.1551078351645 40.16704986397507, -105.1546488300367 40.16705586518081, -105.1546488353165 40.16705898771062, -105.154647999395 40.16705899872255, -105.1546530002739 40.17018099915842, -105.1546569998319 40.17225799859407, -105.1546569996872 40.17249899848197, -105.1546589995688 40.17417299912417, -105.1546599342045 40.17417298750612, -105.1546620818144 40.17647724158829, -105.1546629131087 40.17736968103145, -105.1538534119111 40.17702152067658, -105.1538401553576 40.17416747340352, -105.1471472878128 40.17412208832916, -105.1308240275999 40.16707106507126, -105.1308251696132 40.16745401704761, -105.1308248690956 40.16770711920258, -105.1308339090772 40.16841512361963, -105.130829951995 40.16861687941822, -105.130829023898 40.16878789975995, -105.1308268264415 40.16899487857084, -105.130825096449 40.16911593337741, -105.130826950711 40.16923590355137, -105.1308328523583 40.16953294692157, -105.1308381211171 40.16968312372387, -105.1308380730325 40.1698239502182, -105.1308520529194 40.17054487184136, -105.130858089966 40.17094897815058, -105.1308571509205 40.17105603681589, -105.1308601753751 40.17135609075753, -105.1308610970434 40.17144997901022, -105.1308640602036 40.17169513068922, -105.1308731301453 40.17200206767621, -105.1308830569357 40.17234908671396, -105.1308980849702 40.1728770261307, -105.130890136097 40.17308892735598, -105.1308928515666 40.17318199632658, -105.1308981571233 40.1736550034996, -105.1308978484933 40.17384386824337, -105.1308928914898 40.17403189495574, -105.130896930049 40.17421089176275, -105.1308961355192 40.17475305743081, -105.1309030890619 40.17558211464502, -105.1309011192309 40.1758791343955, -105.1309108852502 40.17618991643079, -105.130907895079 40.17667497536176, -105.1309089894072 40.17686906099571, -105.1309088561322 40.17768491898182, -105.1309031473364 40.17900092566963, -105.1308910444444 40.1812969306925, -105.1308898627142 40.181442199769, -105.1309021056735 40.18314994122324, -105.1308979191687 40.1841851230857, -105.1309039419183 40.18465813085619, -105.1309051019469 40.18497190483541, -105.1309110183405 40.18513498587469, -105.1309118354979 40.18564393849361, -105.1309191252318 40.18634507253613, -105.1309188689071 40.186986063103, -105.1309220276749 40.18759110388334, -105.1309130611667 40.18812198620383, -105.1309169704838 40.1885889481708, -105.1288573477865 40.18857997484698, -105.1256918879809 40.18856611215961, -105.121360830748 40.18856299055086, -105.1194899230949 40.18855492662844, -105.1190850825382 40.1885568881324, -105.1186970917979 40.1885539619918, -105.1183019485997 40.18854991306068, -105.1179300587332 40.18854813537448, -105.1174969479037 40.18854890001953, -105.1172141737779 40.18854906207515, -105.1167671242837 40.18854593391976, -105.1158580022557 40.18853797614679, -105.1146671019506 40.18854389517986, -105.1145858430134 40.18854499691239, -105.1134489979368 40.18854998659783, -105.1133670179578 40.18855190824585, -105.1125820027335 40.18856108520247, -105.1125329666713 40.18856092088617, -105.1120540599835 40.18855794243968, -105.1120313601333 40.18760194311961, -105.112017894645 40.18707819066701, -105.112011570436 40.18673288206929, -105.1120085237062 40.186557607745, -105.1119319115066 40.18487960280919, -105.1119049061916 40.18402300359683, -105.1119118919206 40.18367686408679, -105.1119091664257 40.18315088404788, -105.1119081200098 40.18251894680662, -105.1118759946224 40.18181388411318, -105.1118629926047 40.18127002597253, -105.1115040224316 40.18126909494015, -105.1113569308159 40.18126805117004, -105.1112559916314 40.18126990755782, -105.1101640174649 40.18126520655875, -105.1089940736708 40.18126612354689, -105.1086240113595 40.18126487136174, -105.1084361110251 40.18126505829095, -105.1080911123929 40.18126196732355, -105.1072020949942 40.18126004898254, -105.106833109551 40.18125797063896, -105.106641973712 40.18126088969616, -105.1059451380013 40.18126098709274, -105.1052980584674 40.18125987759827, -105.1051319899099 40.18126013369076, -105.1047898365833 40.18126006333194, -105.1044011718303 40.18125708676741, -105.1036499481707 40.18125506224674, -105.1033940415842 40.18125610659184, -105.1027139937316 40.18126200709273, -105.1023829530066 40.18125894705506, -105.1023970324222 40.18093204823994, -105.102413175028 40.18019091209275, -105.1024151073728 40.17943188442915, -105.1024348285392 40.17795588288692, -105.1024359298053 40.17764513457093, -105.102446985836 40.17691688312216, -105.1024459726393 40.17647792955385, -105.1024538771325 40.17579907983215, -105.1024659300747 40.1745939986924, -105.1024928436826 40.1739690192746, -105.1024948495252 40.17393196664215, -105.1024508498185 40.17392907018132, -105.1023799809039 40.17393102219533, -105.101211927436 40.17392892050625, -105.1001161310761 40.17393199790583, -105.0998391512321 40.17393103942207, -105.0989699184054 40.17392802714794, -105.0981518434555 40.1739279313386, -105.0979528772734 40.17392696481058, -105.0977370735687 40.17392895919532, -105.0974990948966 40.17392895400177, -105.0964931512326 40.17392709427654, -105.0963270854283 40.17393008282001, -105.0957541527641 40.17392890476933, -105.0955101015059 40.1739269531794, -105.0950699350661 40.17392596063161, -105.0947811388498 40.17392604651604, -105.0933063695626 40.17394767675843, -105.0930905495083 40.1739629603663, -105.0930355022931 40.17396373747397, -105.093035412355 40.17395404356559, -105.093035999663 40.17395399970057, -105.0930759995535 40.17368299823816, -105.0931459999594 40.17231399916508, -105.0931330003842 40.17149199908522, -105.093151000261 40.17065999832266, -105.0931500001353 40.17054199825319, -105.0931479994263 40.17023599850143, -105.0931369991391 40.16900499892864, -105.0931339988095 40.16872599950739, -105.0931369998561 40.16781299868737, -105.0931289996238 40.16735399928291, -105.093122999789 40.1669069989264, -105.0931319995954 40.16601699884203, -105.0931289999454 40.16569099842605, -105.0931259993862 40.16516199880555, -105.0931569991541 40.16423199918421, -105.0931480029145 40.16392408767742, -105.0931479999207 40.16392399940396, -105.0931469291512 40.16390871444782, -105.0931039998199 40.16329599907725, -105.0931040000302 40.16325199822559, -105.0931050114934 40.1631399988786, -105.0931050119728 40.16313991872316, -105.0931070004038 40.1623779989626, -105.0931070011848 40.1623778683723, -105.0931070642517 40.16237164155648, -105.0931129997678 40.16178000016573, -105.0931149989175 40.16163199930823, -105.0931069993422 40.16131200006891, -105.0931069998108 40.1613119217147, -105.0930749990154 40.16110699945172, -105.0930749994591 40.16106100006206, -105.093074999123 40.16093800027746, -105.0930969990843 40.16066999982127, -105.0930949991611 40.1604880000312, -105.0931024819559 40.16045158549526, -105.0931099998072 40.16041499996014, -105.0931679955306 40.16027501197318, -105.0933151831979 40.16027514992445, -105.0941529994326 40.16027600012808, -105.0942474912358 40.16027599866759, -105.0943463028096 40.16027599968295, -105.0944589999225 40.16027599890212, -105.0946219991399 40.16027500002095, -105.0948714164467 40.16027221347903, -105.0951589994661 40.16026899899504, -105.095906860969 40.16024372245906, -105.0960168884854 40.16023999747829, -105.0960170000153 40.16023999516622, -105.0960982895062 40.16023918860394, -105.0967180002406 40.1602330001241, -105.0998739874729 40.16022399957189, -105.1010630001934 40.16022199906198, -105.1010699280626 40.16022203558438, -105.1010700959203 40.16022203616376, -105.101072318054 40.16022203122495, -105.1024143180025 40.16022903062637, -105.1025380465539 40.16023089182191, -105.1025414551247 40.16023094317227, -105.1037689994997 40.16021099846859, -105.1049759993214 40.16020199886749, -105.1051399994199 40.16020099938218, -105.1051399989076 40.16020108764328, -105.1051400004159 40.16025199911635, -105.1051410002289 40.16030099923575, -105.1051503173048 40.16030096622104, -105.1068299991866 40.16029499859334, -105.1073450001184 40.16022799895545, -105.1077819997477 40.16013699863746, -105.1082079998631 40.16001999929222, -105.108461998888 40.15992999885013, -105.1086199994601 40.15987499865997, -105.1090149994251 40.15970599910182, -105.1093910002993 40.15951199882478, -105.1097429994652 40.15929699888233, -105.1100720003185 40.15905999866217, -105.1103729990311 40.15880299892639, -105.1104429993529 40.15873099894289, -105.1106439998662 40.15852399914743, -105.113046069445 40.15615724048531, -105.1131817329908 40.15603004308861, -105.1131833166732 40.1560310309896, -105.1132350662543 40.15598003692975, -105.1171083166701 40.15216303071296, -105.1174373163797 40.15206603050657, -105.1176343172161 40.15199203009031, -105.1178293167799 40.15191002952171, -105.1180609815329 40.15179809088321, -105.1180673167806 40.15179502982453, -105.1181203168223 40.15176802990709, -105.1182913165957 40.15165502930292, -105.1183783160733 40.15159102880732, -105.1185163167286 40.15147502962919, -105.1186593166722 40.15133602907218, -105.1187093166785 40.15128002911514, -105.1191113168914 40.1508870293791, -105.1196193162772 40.15040603050766, -105.1198893170867 40.15014302898289, -105.1201383165571 40.14990102921602, -105.1208303159887 40.14919902937343, -105.1212533161005 40.14879703059298, -105.1214593168065 40.1485880297608, -105.1214633158546 40.14837802926677, -105.1214643159671 40.14822102985509, -105.1214713155419 40.14797502969255, -105.1219613160375 40.14750802952513, -105.1243203153778 40.14526002966053, -105.1247883151495 40.14478902902466, -105.1303313154118 40.13922902808567, -105.1303923142009 40.13916902875051, -105.1308769439179 40.13869433055886, -105.1308803144594 40.13869102876136, -105.1308803139455 40.13859202915448, -105.1308793142346 40.13849702881259, -105.1308863138307 40.13833002958336, -105.1308973153534 40.13793402935524, -105.1308973195819 40.13793389877544, -105.1309083153879 40.13760103000428, -105.1309613147293 40.13428302934808, -105.1309633151163 40.13416902954575, -105.1309663158803 40.13407590265542, -105.131264018241 40.13407590214059, -105.1351949880881 40.13406190558131, -105.1355969920545 40.13406290499365, -105.136218990986 40.13406390604963, -105.1383481339877 40.1340678960071, -105.1387142130814 40.13405542457127, -105.1387601569389 40.13397838399309, -105.1388641599894 40.13379438525001, -105.1394061770989 40.13283739637802, -105.1396172542842 40.13246945491051, -105.1399113154917 40.13199350715775, -105.1400313152862 40.13181050557099, -105.1402873438578 40.13141953294432, -105.1404134075242 40.13123259600766, -105.1404134914445 40.13123248008579, -105.1405674928146 40.13101869438201, -105.1409685953441 40.13051183984713, -105.1410715897065 40.13039683245281, -105.1412255205253 40.13022372772332, -105.1414536901801 40.12994403235987, -105.1416416731433 40.12976299450775, -105.1433827002903 40.12803805788978, -105.1443716376531 40.12710336772473, -105.1446938377278 40.12679883459163, -105.1447137065043 40.12678007314066, -105.1448846966432 40.12662004649052, -105.1451267445326 40.1263892194086, -105.1456327957312 40.12596286157071, -105.1456423360221 40.12643537867292, -105.1456487281823 40.12675200170747, -105.1456168014993 40.12884799589443, -105.1456167647361 40.12885442637872, -105.1456271903526 40.12885446106298, -105.1457651912196 40.12883446131615, -105.1459941909125 40.12876946043333, -105.1462091902176 40.1287254615651))</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Altona MS</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>4600 Clover Basin Dr, Longmont, CO 80503</t>
+        </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Altona MS</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>4600 Clover Basin Dr, Longmont, CO 80503</t>
+          <t>https://ams.svvsd.org/</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>Altona Middle School</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>40.14448266991539</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-105.1626179175455</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
           <t>https://ams.svvsd.org/</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Altona Middle School</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>40.14448266991539</v>
-      </c>
-      <c r="M3" t="n">
-        <v>-105.1626179175455</v>
-      </c>
       <c r="N3" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>https://ams.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
         <is>
           <t>POINT (-105.1626179175455 40.14448266991539)</t>
         </is>
@@ -664,59 +642,53 @@
           <t>POLYGON ((-105.1295199780874 40.13072688132058, -105.129739962766 40.13072788110647, -105.1308018207651 40.13073588184478, -105.131019817435 40.13074388165322, -105.1310098430939 40.13155699817882, -105.1310003956401 40.13199844572109, -105.130988858237 40.13253599608295, -105.1309879188726 40.13259022536034, -105.1309708325789 40.13358999631841, -105.1309568622919 40.13407299670184, -105.1309663158803 40.13407590265542, -105.1309633151163 40.13416902954575, -105.1309613147293 40.13428302934808, -105.1309083153879 40.13760103000428, -105.1308973195819 40.13793389877544, -105.1308973153534 40.13793402935524, -105.1308863138307 40.13833002958336, -105.1308793142346 40.13849702881259, -105.1308803139455 40.13859202915448, -105.1308803144594 40.13869102876136, -105.1308769439179 40.13869433055886, -105.1303923142009 40.13916902875051, -105.1303313154118 40.13922902808567, -105.1247883151495 40.14478902902466, -105.1243203153778 40.14526002966053, -105.1219613160375 40.14750802952513, -105.1214713155419 40.14797502969255, -105.1214643159671 40.14822102985509, -105.1214633158546 40.14837802926677, -105.1214593168065 40.1485880297608, -105.1212533161005 40.14879703059298, -105.1208303159887 40.14919902937343, -105.1201383165571 40.14990102921602, -105.1198893170867 40.15014302898289, -105.1196193162772 40.15040603050766, -105.1191113168914 40.1508870293791, -105.1187093166785 40.15128002911514, -105.1186593166722 40.15133602907218, -105.1185163167286 40.15147502962919, -105.1183783160733 40.15159102880732, -105.1182913165957 40.15165502930292, -105.1181203168223 40.15176802990709, -105.1180673167806 40.15179502982453, -105.1180609815329 40.15179809088321, -105.1178293167799 40.15191002952171, -105.1176343172161 40.15199203009031, -105.1174373163797 40.15206603050657, -105.1171083166701 40.15216303071296, -105.1131833166732 40.1560310309896, -105.1131817329908 40.15603004308861, -105.1130460729817 40.15615723779523, -105.1106439998662 40.15852399914743, -105.1104429993529 40.15873099894289, -105.1103729990311 40.15880299892639, -105.1100720003185 40.15905999866217, -105.1097429994652 40.15929699888233, -105.1093910002993 40.15951199882478, -105.1090149994251 40.15970599910182, -105.1086199994601 40.15987499865997, -105.108461998888 40.15992999885013, -105.1082079998631 40.16001999929222, -105.1077819997477 40.16013699863746, -105.1073450001184 40.16022799895545, -105.1068299991866 40.16029499859334, -105.1051503173048 40.16030096622104, -105.1051410002289 40.16030099923575, -105.1051400004159 40.16025199911635, -105.1051399989076 40.16020108764328, -105.1051399994199 40.16020099938218, -105.1049759993214 40.16020199886749, -105.1037689994997 40.16021099846859, -105.1025414551247 40.16023094317227, -105.1025380465539 40.16023089182191, -105.1024143180025 40.16022903062637, -105.101072318054 40.16022203122495, -105.1010700959203 40.16022203616376, -105.1010699280626 40.16022203558438, -105.1010630001934 40.16022199906198, -105.0998739874729 40.16022399957189, -105.0967180002406 40.1602330001241, -105.0960982895062 40.16023918860394, -105.0960170000153 40.16023999516622, -105.0960168884854 40.16023999747829, -105.095906860969 40.16024372245906, -105.0951589994661 40.16026899899504, -105.0948714164467 40.16027221347903, -105.0946219991399 40.16027500002095, -105.0944589999225 40.16027599890212, -105.0943463028096 40.16027599968295, -105.0942474912358 40.16027599866759, -105.0941529994326 40.16027600012808, -105.0933151831979 40.16027514992445, -105.0931679955306 40.16027501197318, -105.0931099998072 40.16041499996014, -105.0931024819559 40.16045158549526, -105.0930949991611 40.1604880000312, -105.0930969990843 40.16066999982127, -105.093074999123 40.16093800027746, -105.0930749994591 40.16106100006206, -105.0930749990154 40.16110699945172, -105.0931069998108 40.1613119217147, -105.0931069993422 40.16131200006891, -105.0931149989175 40.16163199930823, -105.0931129997678 40.16178000016573, -105.0931070642517 40.16237164155648, -105.0931070011848 40.1623778683723, -105.0925199158311 40.16237689791628, -105.0917190936679 40.16238697525812, -105.0909838252546 40.16238410086513, -105.089468094328 40.16239711982808, -105.0886809584908 40.16239212456986, -105.0881623938254 40.1623954782369, -105.0881598089886 40.16280928973737, -105.0881648387267 40.16306998948579, -105.0881668740553 40.16350208512876, -105.0881650625537 40.16356494168014, -105.0881693626968 40.16382478228903, -105.0881761464068 40.16392102833853, -105.083609519032 40.16392308127849, -105.0829128177578 40.16392203457659, -105.0813998304982 40.16392203444205, -105.0807888352324 40.1639220337433, -105.0802848402826 40.16392203294821, -105.0795948459216 40.16388103180415, -105.0787978532788 40.16380003091128, -105.0775498655427 40.16357702807103, -105.0756918859996 40.16302902328239, -105.0744968993014 40.16262302002178, -105.0739259058449 40.16241901849396, -105.0730759142553 40.16213901527696, -105.0719189271613 40.16175401236442, -105.0705369421375 40.16129000865394, -105.0694629539653 40.16092000499503, -105.0694111630307 40.16090422372054, -105.0687409608614 40.16070000328342, -105.0678959694674 40.1604240008717, -105.067322977026 40.16013699897744, -105.066765552507 40.15964313063317, -105.0662970046367 40.1588843247345, -105.064919505624 40.15935175545492, -105.064296309749 40.15959008850385, -105.0634333444827 40.15986251985857, -105.062539016009 40.16009099355082, -105.0606010313516 40.16022699272562, -105.0580710513005 40.16025799056519, -105.0553377713311 40.16028796999728, -105.0553382965441 40.16019791122213, -105.0553387559006 40.1601157733564, -105.0553383718875 40.15647913976149, -105.0553382920939 40.15571473362403, -105.0553382659259 40.15546513428482, -105.0553379947871 40.15282923958088, -105.0553386499967 40.15257631307534, -105.055340783666 40.15175194196998, -105.0553462127781 40.14965381974552, -105.055348545721 40.14875222591935, -105.0553554845123 40.14607040548283, -105.0553568117257 40.14555727121959, -105.0553581629 40.14497257258469, -105.0553735349496 40.13831543018563, -105.0553734627153 40.13826344007112, -105.055393108424 40.1382658753683, -105.0570841697421 40.13820687462603, -105.0623920537045 40.13814787912667, -105.0630970281733 40.13814387787887, -105.0644970736709 40.13812287925889, -105.0646163718572 40.1381387740668, -105.0647026837377 40.13816640688852, -105.0647902892207 40.13821288423826, -105.0648822428967 40.13829711858007, -105.0649247890964 40.13837338792121, -105.0649496601588 40.13851303311695, -105.0649012584268 40.13969700518675, -105.0649223983107 40.13978009284535, -105.0649318121612 40.13979936609553, -105.064944699213 40.13982145163131, -105.0650172912994 40.139897965545, -105.0651172543858 40.13995483397098, -105.0652349113323 40.13998458559128, -105.0728341139191 40.13987189343821, -105.0737770801883 40.13984989482434, -105.0742440761428 40.13984499868648, -105.0742413915201 40.13481684621029, -105.0745131984398 40.13479486487819, -105.0762711360049 40.13472286783558, -105.077656234461 40.13468386293215, -105.0799831751011 40.13457186759719, -105.0831630652203 40.13445687173049, -105.0832755753651 40.13446682896835, -105.0846750309919 40.13445787330612, -105.0879403055598 40.13442385884984, -105.0887041365292 40.13437587163286, -105.0899250393446 40.13434187663415, -105.0905391301851 40.13433687298826, -105.0920430472559 40.13429687652557, -105.0927490541487 40.13428987731798, -105.0930212415033 40.13428686643668, -105.0932020045514 40.13427787787717, -105.0940880142722 40.13427987836944, -105.0944050049201 40.13427896522876, -105.0944350199997 40.134278878763, -105.094924071347 40.13427687757695, -105.0960260840791 40.13426087793793, -105.100395113552 40.13418487869186, -105.1024960005596 40.13413300172339, -105.1025130341002 40.13316287731691, -105.1025130798614 40.13316287747433, -105.1041803847008 40.13315484466681, -105.1044939964566 40.13312987928641, -105.1055759631424 40.13312799972009, -105.1055759857053 40.13312511863367, -105.1055770144187 40.13300287849541, -105.1085152097078 40.13299386796137, -105.1086315304633 40.13298881317525, -105.1087220040101 40.13297863883014, -105.1088964020049 40.13293936322003, -105.1089796055062 40.13291013523579, -105.1090587413161 40.13287489693305, -105.1091328252846 40.13283461228306, -105.1092018368701 40.13278836166751, -105.1092647735506 40.13273806278027, -105.1093205768746 40.13268270513078, -105.1093585944797 40.13263279385802, -105.1093701834689 40.13263246468068, -105.1096519310758 40.13263086368207, -105.1098582235746 40.1326323161728, -105.1103350195741 40.13263517546018, -105.110591834876 40.13263671418122, -105.1109074261621 40.13263860431368, -105.111021497991 40.13263928746463, -105.1115905511339 40.13264209640875, -105.1119701840193 40.13263846362696, -105.1119769681384 40.13240697386129, -105.1119826842302 40.13221195301501, -105.1119871837674 40.13205846401782, -105.1121931826917 40.1319974642461, -105.1122250359624 40.13198450641528, -105.1122248807698 40.13196726034626, -105.1123102126654 40.13194232418207, -105.1126460873139 40.13184417366759, -105.1130752163228 40.13171876581113, -105.1134884683498 40.13159766957149, -105.1138787565874 40.13160434794801, -105.1142691989206 40.13161076343259, -105.1146592764502 40.13161717097666, -105.1150500767831 40.13162358771766, -105.1152464520673 40.13162554514241, -105.1155191846595 40.13164146329787, -105.1167491843696 40.13166446387874, -105.1167582823744 40.13069277850736, -105.1190737172402 40.13069586675535, -105.1190789667365 40.13069587415787, -105.1190837455796 40.13069590702754, -105.1196690057948 40.13069987439082, -105.1214287020073 40.13069788718315, -105.1214388421045 40.13069787537972, -105.1214389852497 40.1306978758488, -105.125637981124 40.13071087844324, -105.1295199780874 40.13072688132058))</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>4</v>
-      </c>
-      <c r="E4" t="n">
-        <v>4</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Burlington Elementary</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1051 S Pratt Pkwy, Longmont, CO 80501</t>
+        </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Burlington Elementary</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1051 S Pratt Pkwy, Longmont, CO 80501</t>
+          <t>http://bes.svvsd.org/</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
+          <t>Burlington Elementary School</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>40.1466539913149</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-105.108633248163</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
           <t>http://bes.svvsd.org/</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Burlington Elementary School</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>40.1466539913149</v>
-      </c>
-      <c r="M4" t="n">
-        <v>-105.108633248163</v>
-      </c>
       <c r="N4" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>http://bes.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
         <is>
           <t>POINT (-105.108633248163 40.1466539913149)</t>
         </is>
@@ -736,59 +708,53 @@
           <t>POLYGON ((-105.2583845261048 40.01916806167687, -105.2583845465005 40.01820405441318, -105.2583835533824 40.017841051784, -105.2583967697713 40.01738897110558, -105.258420544823 40.01462569237854, -105.2630299591908 40.01461696725389, -105.2630753109644 40.01461633090538, -105.2638765422727 40.01460508854388, -105.2646558644589 40.01461288522881, -105.2657616256185 40.01461332253763, -105.2662260626349 40.01461196195721, -105.2678219770818 40.01460804739548, -105.2689819637891 40.01460406242605, -105.270220141546 40.01459912551402, -105.2716550449331 40.01459291590101, -105.2725519067238 40.01458809993736, -105.2736219240902 40.0145838908234, -105.2746458800721 40.01458095527774, -105.2760611408061 40.01457602595389, -105.2764250735946 40.01453802385365, -105.2773539185385 40.01436001199994, -105.2775250367717 40.01432794849211, -105.278005899344 40.01423306829994, -105.2782030961592 40.01419611210767, -105.278663968713 40.01410393231048, -105.2786769521653 40.01410055096331, -105.2786822492777 40.01411631803115, -105.278851249496 40.01459531880194, -105.2788752505237 40.01466131864607, -105.2789422504309 40.01484831880367, -105.2790212496877 40.01506431947683, -105.279283131531 40.01582838979826, -105.2792882488983 40.01584331888502, -105.2793182480616 40.01593431868323, -105.2795172500427 40.01656331893992, -105.2796422519211 40.01688331794094, -105.2797922499383 40.0173063188877, -105.2800122511694 40.01792531871845, -105.280344103938 40.01889429097838, -105.2840818920156 40.01812191122571, -105.2839600121989 40.01782410420856, -105.2838869444426 40.01755905605179, -105.2837991589066 40.01709413112621, -105.2840110981352 40.01704713596685, -105.2841060700353 40.01702607643248, -105.2850088672696 40.01684712918449, -105.2852128642166 40.01680605680808, -105.2865308262578 40.01653288651573, -105.2866812529073 40.01650245354258, -105.2878670067061 40.0162528717229, -105.2885419939298 40.01611983770974, -105.2891551001181 40.01599098183944, -105.2904817987244 40.01572217487955, -105.2916482773999 40.01546871123976, -105.2924838834105 40.01529960385942, -105.2929311934506 40.01520907552712, -105.2932648974691 40.01514153813964, -105.2935522291935 40.01508380053187, -105.2940456558378 40.01498431869415, -105.2941799322994 40.01493717604964, -105.2942962425791 40.01484536492688, -105.2945651847544 40.01463397060598, -105.2948050566042 40.01443646962085, -105.2948669406371 40.01436130597801, -105.2949106525785 40.01428611088715, -105.2949149278989 40.01420590378106, -105.2949111667633 40.01415099338725, -105.2948850709373 40.01404306065437, -105.2948279437313 40.01392601395955, -105.2948950990359 40.01391405477982, -105.2951188286011 40.01383593998661, -105.2955889946644 40.01372696689724, -105.2959720191087 40.01362689650804, -105.2966129379867 40.013483906396, -105.2968701231647 40.01343988732408, -105.2972629400945 40.01340708693889, -105.297280077546 40.01340711706504, -105.2975649848486 40.01340487234885, -105.2978951689382 40.01342411927098, -105.2981560643021 40.0134531259425, -105.2984361789157 40.01350193131028, -105.2987091069599 40.01356691986554, -105.2989748438362 40.01364891574665, -105.2990971694855 40.01369387506902, -105.2994309509394 40.01382595114303, -105.2996880626172 40.01392796986438, -105.3000011606622 40.01405287069223, -105.300067868143 40.0140719279547, -105.300254092653 40.01412001668933, -105.3005359990144 40.01416799685423, -105.300684149682 40.01417292017293, -105.3008359183136 40.01416110284114, -105.3009841703811 40.01413088704314, -105.3010065439604 40.01412285491573, -105.3010146521981 40.01412034528163, -105.3010158302282 40.01400687156732, -105.3010182134563 40.01377743388108, -105.3012170449381 40.01365994277487, -105.3012511657355 40.01363978016212, -105.3012602122003 40.01363443507628, -105.3013157480595 40.01351102356379, -105.3013862127445 40.01335443432603, -105.3014422127245 40.01298943465143, -105.3014430498437 40.01295818709555, -105.3014855972748 40.01291567214673, -105.3016445781594 40.01279315270759, -105.301669611214 40.01277386057978, -105.3018438953327 40.01265106276252, -105.3018840442789 40.01258892735918, -105.3019098151939 40.01254904485556, -105.3019510380944 40.012454651744, -105.3020538088907 40.01231838041662, -105.3021905057177 40.01225039243434, -105.3023609783213 40.0122379765276, -105.3024963718175 40.01215354095651, -105.3025641030316 40.01212000680025, -105.3028339352925 40.01201999358893, -105.302871088117 40.01201209624642, -105.3030868287403 40.01197513103055, -105.3032639351221 40.01196500016254, -105.3034049259969 40.01197512435276, -105.3035260492263 40.01198695187986, -105.3036140681767 40.01199799158061, -105.3039102543303 40.01202602940209, -105.305557109506 40.01218191783366, -105.3057609542073 40.0121850065404, -105.3059319946257 40.01217403816238, -105.3061630807291 40.01213901500693, -105.3063570745538 40.01209102548007, -105.3065429044971 40.01202600142455, -105.3076141292119 40.01157813163452, -105.3077088271884 40.01154589495262, -105.3079238782443 40.01149903669649, -105.3080870674058 40.01148613185906, -105.308331942269 40.01149806925132, -105.3085360305202 40.01154095864429, -105.3087150704405 40.01160411941821, -105.3088508945874 40.01167407305289, -105.3089869755116 40.01177998905509, -105.3091108765658 40.01190098145004, -105.3091959108223 40.0120048916048, -105.3093011218043 40.01217087461801, -105.3095111066217 40.01265986544916, -105.3095949315841 40.01281400891951, -105.309699132441 40.01295912720237, -105.3098229913196 40.01309604135331, -105.3099480980261 40.01320694391978, -105.3102739955811 40.01344789402713, -105.3118234160897 40.01453544148655, -105.3120567925063 40.01470010708103, -105.312361933919 40.01489993781325, -105.3125289085233 40.0149733016851, -105.3127352332546 40.01504169007535, -105.3129480200329 40.0150804391507, -105.3130960043414 40.01509110681246, -105.3132370369799 40.01508886480606, -105.3133744223811 40.01507836676347, -105.3135317804734 40.01504298074446, -105.3136827254333 40.01498525341332, -105.3138217195852 40.01490369158279, -105.3139311537581 40.01480613317056, -105.3140840267508 40.01465100213418, -105.3141580699373 40.01454765470404, -105.314161100045 40.01453610243495, -105.3142523826783 40.01432569713389, -105.3144299782174 40.0138658864271, -105.3145150378233 40.01370213541934, -105.3146211428467 40.01354500553955, -105.3147468556418 40.01339806550179, -105.3152511428208 40.01293713504057, -105.3153959888806 40.01284293193758, -105.3155440900743 40.01275764490002, -105.3157016044707 40.01269236446624, -105.3158787245793 40.01264979891742, -105.3161049520235 40.01262999701227, -105.3162930090429 40.01263710205752, -105.3164618248755 40.012656038649, -105.3166248808208 40.01269308423035, -105.3170811216146 40.01283491108664, -105.3185478949735 40.0133129701069, -105.318734015863 40.01340412766929, -105.3188769358608 40.01349604118355, -105.3190030450923 40.01360000856643, -105.3190590450488 40.01365991406973, -105.319111985134 40.01371602570779, -105.3192538759621 40.01392707882941, -105.3194131462352 40.01418208192421, -105.3196241265045 40.01445912624737, -105.3197259873269 40.0145528964566, -105.3197746679137 40.01458662986119, -105.3198439456211 40.01463488779377, -105.3200051121442 40.01471392747337, -105.3201231738931 40.01475693671951, -105.3202769540203 40.01479396174955, -105.3205160984978 40.01481794203936, -105.3206771327974 40.01481187808569, -105.3207571317286 40.01480212051062, -105.3210079447452 40.01473305728056, -105.3215281528368 40.01458809318348, -105.3215913105161 40.01457452082933, -105.3216871073137 40.01455786734842, -105.3218510178522 40.0145441209512, -105.3219609779378 40.01454511395445, -105.3221377392204 40.01457308621488, -105.3221690399934 40.01457700548138, -105.3223699117416 40.01462810094041, -105.3225621678807 40.01469702558393, -105.3228649500641 40.01482486826393, -105.3233328044708 40.01505322987001, -105.323660104682 40.01519062698569, -105.3238888151895 40.01526805234592, -105.3241205694507 40.01532592516624, -105.3241648728118 40.01538111073737, -105.3242303884762 40.01548755042216, -105.3244247008065 40.01574628088172, -105.3245436788014 40.01591887528656, -105.3245492477389 40.0159269544882, -105.3246059212577 40.01602909790676, -105.3247017555202 40.01622526479302, -105.3247730382696 40.01643244347468, -105.3248041000856 40.01657168709549, -105.3248219629255 40.01670913457539, -105.3248553573099 40.01687431775166, -105.3249133701591 40.01707073862386, -105.3249952481318 40.0172958282551, -105.3250760460801 40.01745401497376, -105.3252098556754 40.0176254206745, -105.3253212573837 40.01774829766252, -105.3255659482411 40.01799501028366, -105.3257195021807 40.01817081069291, -105.3258066509846 40.01828485840267, -105.3258460155857 40.01835697437657, -105.3259681394613 40.01858573655364, -105.3260399610972 40.01874900580488, -105.3261540656113 40.01894792884458, -105.3262193760422 40.01910160164122, -105.3263929273057 40.0195099539127, -105.3264250268082 40.01966400709756, -105.3264778781707 40.01980107190855, -105.3265102510802 40.01985978085294, -105.3265528701127 40.01993707119846, -105.326870866398 40.0204130156731, -105.3269570457379 40.02050291279555, -105.3270988940789 40.02060497193763, -105.3274174830837 40.02081711266219, -105.3275899041758 40.02100756890201, -105.3276826272177 40.02115700281578, -105.3277198721696 40.02124929852239, -105.3277770989521 40.02139110936605, -105.3278828940231 40.021773946245, -105.3279280546751 40.02198896183513, -105.3279869488215 40.0221389376397, -105.3281110299227 40.02235105094308, -105.3281758228844 40.02243234016946, -105.3283149827645 40.02260693121875, -105.3284389778593 40.02271198198343, -105.3287591164508 40.02291395380421, -105.3288938247745 40.02301901997969, -105.3290120195943 40.02315892566909, -105.3290941141536 40.02331387534033, -105.3291661187661 40.02350587084195, -105.329187860145 40.02366402561023, -105.3291856108905 40.0237299462356, -105.3291851632656 40.02374308334997, -105.3292105083722 40.02393861410442, -105.3292580015209 40.02409411493859, -105.3293400314355 40.02426807343316, -105.3293850744826 40.02433971920112, -105.329517076826 40.0245221086009, -105.3296581319994 40.02466094949524, -105.3297101574987 40.0247041251023, -105.3298849343158 40.02478097424918, -105.330075850617 40.02482902161795, -105.3301448347398 40.02483905198635, -105.3303063677034 40.02486253821598, -105.3305089314445 40.02490174321267, -105.3307188932055 40.02497976589941, -105.3311201805862 40.02514192076426, -105.3313211016588 40.02521297880104, -105.3315614094424 40.02528981493634, -105.3316864080329 40.02530226875604, -105.3318593114162 40.02530661078252, -105.3320268883447 40.02527797201461, -105.3322212954186 40.02522737817259, -105.3323144391407 40.0251865241619, -105.3324583090925 40.02512342117116, -105.3326207608531 40.02505003162955, -105.3327166037238 40.02501949364788, -105.3328488509051 40.02500107885299, -105.3329530767121 40.0250179756226, -105.3330761532333 40.02506509655677, -105.3334181797729 40.02523387018027, -105.3336921200928 40.0253378996183, -105.3338808648359 40.02539134594898, -105.3341307947925 40.02544487907239, -105.3342930478431 40.0254532928835, -105.3344340886531 40.02543304437418, -105.3345139544222 40.02540861718986, -105.3346764107789 40.02533318028983, -105.3348588869171 40.02521323380916, -105.3349301769176 40.02516213123148, -105.334942439392 40.0251533413287, -105.3351340153575 40.02508456072082, -105.3352794641085 40.02507572510495, -105.3354306917962 40.02509896697647, -105.3355180506154 40.02513393951381, -105.3358146694223 40.02529351858141, -105.3360870116539 40.02543283740193, -105.3366797666057 40.02573373858232, -105.3368153907778 40.02580180617613, -105.3369393034369 40.0258639947272, -105.3370898293551 40.02596861159827, -105.337211444122 40.02608962972621, -105.3372945325549 40.02622374646779, -105.3373147386148 40.02627063395128, -105.337421175453 40.02647877096612, -105.3374981735376 40.026582085771, -105.3376050923685 40.02666898418729, -105.3377398955795 40.02674301993157, -105.3378653071847 40.02677945552124, -105.3379240857469 40.02679433669536, -105.3381088963428 40.02683907028913, -105.3381922987373 40.02687609862392, -105.3382659791816 40.02691977176665, -105.3383043922788 40.02695517610391, -105.3383708887366 40.02703599359061, -105.3383777622052 40.02713038225339, -105.338366843368 40.02723611127646, -105.3383566309992 40.0272642467565, -105.3382529574146 40.02752611738724, -105.338225780298 40.02763739410864, -105.3382170012274 40.02773192113717, -105.3382338601833 40.02783799351767, -105.3383062021897 40.02799593461113, -105.338404047229 40.02811187719205, -105.3384651416272 40.02816304037792, -105.3385772570687 40.02823389648423, -105.3387027374635 40.02828469390063, -105.3388570775456 40.02831510567995, -105.3390817408703 40.0283388001672, -105.339237772709 40.02837330724666, -105.3393408026778 40.02842274061585, -105.339427070937 40.0284871535725, -105.3395271463893 40.02860730522766, -105.3395743309235 40.02869523638033, -105.3395908092224 40.02880027047129, -105.3395907679906 40.02884567393286, -105.3395316310671 40.02907021534642, -105.3395313939624 40.0291709390978, -105.3395785284584 40.029280301116, -105.3396758483765 40.02938759113305, -105.3398070717007 40.02948011247911, -105.34001105511 40.02959898763005, -105.34015883881 40.02966944762828, -105.3403328781856 40.02971994667367, -105.3404849920475 40.02972509898724, -105.3406360896496 40.02970691478322, -105.3410469038371 40.02961451122763, -105.341183063898 40.02960005782608, -105.3413729948086 40.02962008481045, -105.3415028859989 40.02966089163202, -105.3416609109556 40.02973495466169, -105.3418081666057 40.02983288521217, -105.3419061589185 40.02992388512177, -105.3420809641687 40.03015389630465, -105.342137060486 40.03029507504125, -105.3421488596493 40.03044031811095, -105.3421403156747 40.03055896510004, -105.3421095060823 40.0306210722046, -105.3420716051278 40.03069511489726, -105.3419991759212 40.03077501854443, -105.341919419521 40.03083712699294, -105.3418300778567 40.03089928889136, -105.3415005965306 40.03112171569501, -105.3410174858492 40.03147037200236, -105.3408471369649 40.03159443563352, -105.340665615881 40.03172705505519, -105.3405288206844 40.03180830358372, -105.3403725243837 40.03188309433408, -105.3402050811774 40.03195572768927, -105.3399985277202 40.03206259515791, -105.3398923459022 40.03216531452311, -105.3398401151529 40.03228710789242, -105.339815900834 40.03266454513719, -105.3397910481914 40.03276958840173, -105.3397623867686 40.03289592220633, -105.3397648869638 40.0330180815536, -105.3398021263316 40.03310402182879, -105.3398648639367 40.03318323722127, -105.3399094257732 40.03320258646184, -105.3399874379754 40.03322412473215, -105.3400861009968 40.03322904669189, -105.3404129451709 40.03319600779776, -105.340606091903 40.03321988353994, -105.3407891693523 40.03327394200747, -105.3409739123984 40.03337906294917, -105.3411214760025 40.03350214896666, -105.3414135867008 40.03377043530846, -105.3416446218389 40.03392719713566, -105.3418169530248 40.03404894816423, -105.3419979269082 40.03425771521409, -105.3420729438595 40.03436925697198, -105.3421506900844 40.03450652043009, -105.3422027158252 40.03456991529723, -105.3422675171242 40.0346224063464, -105.3423343685873 40.03464821394812, -105.3424653436751 40.03467410999632, -105.3429150731083 40.03468705674727, -105.3431410697753 40.03471591391834, -105.3433656111949 40.03478463226877, -105.3435020608055 40.03485553907074, -105.3438695438839 40.03508748923305, -105.3440168467119 40.03514205613806, -105.3440255978391 40.03514317666856, -105.3441489464593 40.03515897953323, -105.3442811158003 40.03514598153194, -105.3445051287401 40.03510592924802, -105.3447008653332 40.03509301643103, -105.3448968898014 40.03511112379889, -105.3450871457833 40.0351531064796, -105.3453108748094 40.03523795776137, -105.3454389324795 40.03530511152007, -105.3455861725568 40.0354181365134, -105.3457001544155 40.0355508806632, -105.3457428449966 40.03562395961514, -105.3458831215092 40.03597388322648, -105.345896628054 40.03615305911401, -105.3458797746984 40.03628602631347, -105.3457491322696 40.03663309661266, -105.3457611032644 40.03670887964498, -105.3458098776353 40.03677702573989, -105.3458869092818 40.03682599243626, -105.3459829278598 40.03684890616413, -105.3461322249344 40.0368457054413, -105.3466198830052 40.03677206577161, -105.3467530710819 40.03678294877792, -105.3468751210049 40.03682401467811, -105.3469760397207 40.03689195387994, -105.3471355108481 40.03703348689576, -105.3472691705876 40.0371086708003, -105.3472744176314 40.03710968647263, -105.3474308076592 40.03714103151144, -105.3475785708468 40.03714336947589, -105.3481836375957 40.03712059375427, -105.348392981334 40.03713896938038, -105.3485029214573 40.03716601706564, -105.348603897788 40.03720897453926, -105.3486919822502 40.03726701348017, -105.3487650432671 40.0373360133605, -105.3488319497072 40.03744288818694, -105.3488511085128 40.03750001347461, -105.348856789205 40.03820800949617, -105.3487067298522 40.03821232955207, -105.3477914050935 40.03821638893005, -105.3474817926258 40.03821722291953, -105.3468614299469 40.03822512838605, -105.3450104181683 40.03829153532944, -105.3450179171597 40.03868015700185, -105.3460405482716 40.0386437539853, -105.3461031168401 40.03898908284479, -105.3453268746833 40.03901948006025, -105.3452802180325 40.03911018389644, -105.345271517239 40.03912433761808, -105.3452452833364 40.03915814157467, -105.3452130574343 40.03918918870853, -105.3451781010895 40.03921517142847, -105.3451448277192 40.03923480953083, -105.3451089087152 40.03925177274996, -105.3450576487383 40.03926988529709, -105.3450069768098 40.03928187960952, -105.344961760615 40.03928819273935, -105.3449089508063 40.03929064807553, -105.3448494533033 40.03928712489946, -105.3447950264157 40.03927776511058, -105.3447425347318 40.03926247803446, -105.3446092328436 40.03929490292018, -105.3445765512982 40.03930516501039, -105.344539877266 40.03932120387111, -105.3444846960346 40.03935795158987, -105.3444426165169 40.03940586426801, -105.344423128196 40.03944725428348, -105.3444160073502 40.03949552391189, -105.3444275517575 40.03955601888752, -105.3444731759986 40.03968833424123, -105.3444965572211 40.03975520013649, -105.3445205624492 40.03981616221999, -105.3445578084813 40.03989778498795, -105.3446376646379 40.04003968424905, -105.3447276531524 40.04016680845205, -105.344795157412 40.04024733253993, -105.3448549167217 40.04031071675156, -105.3448484541613 40.04055274004725, -105.3448541691076 40.0406499600528, -105.3448674149786 40.04072253855343, -105.3448882399842 40.04079357632659, -105.3449216829459 40.04087332410908, -105.3449704426995 40.04095811087339, -105.3446364322639 40.04102959990085, -105.3446007162516 40.04104340376086, -105.3445703711054 40.04106466860651, -105.3445493695219 40.04108914063158, -105.3445380231417 40.04111119661664, -105.3445343361066 40.04112275146215, -105.3445311011553 40.04114724832418, -105.3445392814093 40.04121096396332, -105.3419896303343 40.04121709476975, -105.3422755387781 40.04337513429397, -105.3465131388534 40.04343423722576, -105.3501117189857 40.04341854173573, -105.3509604583964 40.04341720319611, -105.351061685705 40.04341728708226, -105.3544519058515 40.04524596662837, -105.355091416096 40.04556889885021, -105.3559880623356 40.04583041298836, -105.3567595372542 40.04599519383382, -105.3579301381531 40.04606086270712, -105.3600970053326 40.04564174739976, -105.3606742433043 40.0468628855719, -105.3621557651074 40.04965424089358, -105.3639920692559 40.05282887853546, -105.3641080684391 40.05289587827868, -105.3797250233372 40.06069585746808, -105.3900870057658 40.06584284178945, -105.3912861257657 40.07092499987773, -105.3914749402041 40.07083101793872, -105.3920811145549 40.07050298994405, -105.3925910222121 40.07026600808574, -105.3937980289077 40.06981087854467, -105.3940840170989 40.06972192263695, -105.3946001680771 40.06959803960483, -105.3947989293112 40.06953590537677, -105.3948919023455 40.06948987079981, -105.394964868722 40.06944107368035, -105.395060070696 40.06933903984681, -105.3952621280964 40.06899113614033, -105.3955138612367 40.0686358647477, -105.3957139250865 40.06842109885081, -105.3959568633348 40.06820609746421, -105.3961321294408 40.06808409464642, -105.3965509251752 40.06782505281563, -105.3967590498075 40.06770994229892, -105.3970411697905 40.06757211203932, -105.3973890575354 40.06741704540752, -105.3979349933502 40.06719105257222, -105.3989681210101 40.0668320704148, -105.3993949116376 40.0667119298152, -105.4001279456997 40.06656295502956, -105.400853036919 40.06646804795456, -105.401574842874 40.0664209000962, -105.4031081030495 40.06634588138125, -105.4033760986539 40.06632908658128, -105.4036001268962 40.06632597936235, -105.4039354886404 40.06629270998662, -105.4039684530764 40.06628998415017, -105.4041299199174 40.06627663574243, -105.4042548603106 40.06623819278212, -105.4043540234276 40.06619888982722, -105.4044344048956 40.06614050729836, -105.4045148499365 40.06603666564356, -105.4047389400583 40.06573287074457, -105.4047829657393 40.06567608181868, -105.4049212700939 40.06553693910522, -105.4051253441126 40.06542981958253, -105.4053520055905 40.06532884620861, -105.4056105037759 40.06528097971057, -105.4058260373516 40.06528440260607, -105.4060288655031 40.0653072983951, -105.4061852130406 40.0653236615075, -105.4063458769007 40.0652750842445, -105.4065446697525 40.06515834714913, -105.406676242775 40.06503075664818, -105.4068038590952 40.06490576206056, -105.4069109925564 40.06477432561354, -105.4072568691801 40.06434998263192, -105.4075520798087 40.0638858471748, -105.4076144271041 40.06375352486941, -105.4076986539011 40.06358322723908, -105.4077424376704 40.06351872295893, -105.4078528920384 40.06344490160728, -105.407979736912 40.06339954278057, -105.4081488124669 40.06337694790046, -105.4081993022081 40.06354259319305, -105.4082583191018 40.06365304293325, -105.4083384376527 40.06378623987003, -105.4086252315054 40.0642215866695, -105.4087813728473 40.06439056211295, -105.4089458907069 40.06461799217212, -105.4091018907903 40.06489412393282, -105.4092368182365 40.06512802479963, -105.4093225643208 40.06526853688391, -105.409504095397 40.06548498442051, -105.4098262734777 40.06579167091841, -105.4100664892069 40.06598563197285, -105.4102657157319 40.06612999100079, -105.4104355939177 40.0662923524043, -105.4104999331161 40.06642759351949, -105.4105231868886 40.06658533416806, -105.4111090704269 40.0668027547869, -105.4113230710384 40.06683775452498, -105.4123600762381 40.06670774877939, -105.4126030773382 40.06671874798173, -105.4127710765582 40.06675374711786, -105.4135470770253 40.06717174623984, -105.4143210780151 40.06733974415099, -105.4147190788605 40.06742674212688, -105.4148260788204 40.06747274227973, -105.4149630792546 40.06748474171021, -105.4150690789331 40.06755474126348, -105.4153730784282 40.06789174239631, -105.4157380779817 40.06803174076535, -105.4159660790526 40.06803073976152, -105.417218086706 40.06765573284537, -105.4192990814895 40.06934373178217, -105.4204860820148 40.06988972973171, -105.4213540837626 40.07010972666475, -105.4217650863564 40.07012072544669, -105.4219790865552 40.07007372430561, -105.4224070903935 40.06972272033761, -105.4231560979392 40.06916171416628, -105.4234760999032 40.06905671176163, -105.4241311017381 40.06905570945187, -105.4263101075327 40.06940170123508, -105.4276811134631 40.06938769518695, -105.4296940698257 40.06907550496865, -105.429696726161 40.06942996754758, -105.429694386054 40.06959605113096, -105.4296933119867 40.06967240975321, -105.429641808105 40.06967550540362, -105.4292166920104 40.06972721171748, -105.4288950002293 40.06976633789137, -105.4286274367091 40.0698159315109, -105.428326045251 40.06989903627482, -105.4279288266033 40.07006320863681, -105.427767388902 40.07014234364784, -105.4274301435079 40.07031168907899, -105.427187862742 40.07041321736073, -105.4265850469876 40.07060213368924, -105.4264385616445 40.0706539625285, -105.4262836121072 40.07072092919811, -105.4261582347105 40.07078358879082, -105.4259539328541 40.0709165081871, -105.4258003383412 40.07103107048781, -105.4253944374446 40.07137217887671, -105.4252350299228 40.07147595325737, -105.4243155617368 40.07219115576593, -105.4231393098885 40.07308417705716, -105.4226100060591 40.07339089775018, -105.4222132276659 40.07363857455535, -105.4217252471861 40.07398674410683, -105.4215431642913 40.07408511303873, -105.4211965898197 40.07427234585262, -105.4210308105794 40.07434951045089, -105.4206584442087 40.07448493070384, -105.4202083996824 40.07461261810035, -105.4195352042127 40.07476456033439, -105.4191247017771 40.07482938094511, -105.4189980306713 40.07484611794027, -105.4186447055464 40.07487513225324, -105.4180009566014 40.07488857546316, -105.4177762251645 40.07488622163074, -105.4174610348563 40.0748779494316, -105.4172705764785 40.07488147149702, -105.4170810759536 40.07488206684572, -105.4170306009453 40.07488568808787, -105.4169286974435 40.07489512468741, -105.4167905896386 40.07491916695444, -105.4166333942057 40.07497684600628, -105.4162312907294 40.07517846289863, -105.4159997512771 40.07528949075067, -105.4156196132907 40.07543625610639, -105.4153350203652 40.07550396612029, -105.4151395682494 40.07551491221498, -105.4149634135315 40.07550234559449, -105.4148358409656 40.07547591583315, -105.4146111929816 40.07540552041137, -105.4143570994708 40.07527584758753, -105.4142381667132 40.07519455728776, -105.4139032823823 40.07494558003621, -105.4136444687195 40.07478517666688, -105.413329475767 40.07462253567618, -105.4130705753038 40.0745330917355, -105.4129058764918 40.07449931594424, -105.4127516241002 40.07448895733638, -105.4125773454127 40.07450053023379, -105.4124096976944 40.0745384436123, -105.4122829936822 40.0745807785052, -105.4116113120437 40.07483923530526, -105.4112998081208 40.07492678295778, -105.4111312145296 40.07495957269411, -105.4109493026843 40.07498064805032, -105.4104369611586 40.07499780879358, -105.4099465988038 40.07495572838605, -105.4096666239786 40.07496136200007, -105.4094075828542 40.07497944835027, -105.4087209130649 40.07504255224723, -105.4072133339139 40.07514450001526, -105.4064926228099 40.07519135351045, -105.4058410165122 40.0752136172959, -105.4054705638814 40.0752272141406, -105.40520487196 40.07523357995193, -105.4049353748692 40.07523628450529, -105.4047392325432 40.07521783433648, -105.4045848509388 40.0751897922855, -105.4041947147465 40.07508862949976, -105.403705422345 40.0749653223569, -105.4035454821902 40.07493738955924, -105.4033969451357 40.07492482835819, -105.4031503024901 40.07492901141337, -105.4028950470262 40.07496317992302, -105.4025169204411 40.07501553263012, -105.4023550157805 40.07502929541273, -105.4021645541007 40.07503425519602, -105.4019389002541 40.07501138551396, -105.40168661591 40.074965083188, -105.4015019436022 40.07491810670258, -105.40096224968 40.07475231378992, -105.4007728206619 40.07470313718637, -105.4006128875573 40.0746708105926, -105.4003900881106 40.07465013520603, -105.4001936699258 40.07464511287059, -105.3999920191408 40.0746658845997, -105.3997996016553 40.07470668529642, -105.3996328800538 40.07475774923518, -105.3994223224821 40.0748299894019, -105.3992936939425 40.07487962339136, -105.3991136328338 40.07493506377642, -105.3989345365082 40.07498245837664, -105.3987192795767 40.0750122629322, -105.3984012230241 40.07501125209868, -105.3982545679028 40.07501551265776, -105.3981326490511 40.07503442581616, -105.3980545259296 40.07505922901456, -105.3979649460374 40.07510377494535, -105.3978486566331 40.0751790217227, -105.3973899365647 40.07562852046983, -105.3972817002089 40.0757136836102, -105.397169427459 40.07578848025003, -105.3968792179321 40.0759179797459, -105.3959609054664 40.07622318892043, -105.3953231254621 40.07647233550051, -105.3947619214149 40.07666278952232, -105.3941305833764 40.07686297010658, -105.3939136913895 40.07697539101873, -105.3934575621836 40.07722224613386, -105.3931865114511 40.07731992618486, -105.3929282780375 40.07737354901404, -105.3926318413482 40.07740020380218, -105.3923466903028 40.0774207953173, -105.3919433258007 40.07747300969441, -105.3915512466445 40.07751915932716, -105.3910859383422 40.07751872123406, -105.390588819259 40.07748152648809, -105.3899547533051 40.07738544205882, -105.3895851208953 40.07734591650613, -105.3890560983312 40.07733071977488, -105.3886608422517 40.07736951179238, -105.3882208880001 40.07745722445686, -105.3878287902893 40.07751315322446, -105.3875386890442 40.07756183623066, -105.3871751517061 40.07769123986255, -105.386958188724 40.07783792342001, -105.3868401010417 40.07793818621354, -105.3866996581514 40.07806535888105, -105.386575220841 40.07815092657836, -105.3864348761523 40.07821933925117, -105.3862435609229 40.07827301294386, -105.3861064964615 40.0782851193332, -105.3859439556369 40.07828495884738, -105.3854915187126 40.07820861461854, -105.3852495670619 40.07817436606354, -105.3849689629014 40.07813464671029, -105.384647065656 40.07813677433686, -105.3843346505428 40.07818542609105, -105.3841911614831 40.07822690365325, -105.3838658088119 40.07838571414805, -105.3835116873142 40.07859345906748, -105.3832533311892 40.07871071489546, -105.3828706781617 40.07882784409028, -105.3824975639514 40.07895722236837, -105.3821530389425 40.07914049159699, -105.3818913601033 40.079333636382, -105.3816040092101 40.07962713452685, -105.381316880753 40.07979087291746, -105.3809245713487 40.07995695099259, -105.3802294146402 40.08015943763821, -105.379588467187 40.08034483921757, -105.3792504093654 40.08046689970899, -105.3786411661966 40.08074291496696, -105.3780797871333 40.08098470179396, -105.3777130575363 40.08109693300169, -105.3774866867055 40.08114076234569, -105.3770053036764 40.08120390520853, -105.3766993091122 40.08121582032145, -105.3761925603991 40.08120548435789, -105.3760268068356 40.08121510006245, -105.3757111712446 40.08127107066737, -105.3751786731141 40.08139780561959, -105.3744967961343 40.08157402736211, -105.3735477428702 40.0818006048877, -105.3730416668277 40.08192675278983, -105.3726786466126 40.08199815224141, -105.3724146658471 40.08203164841389, -105.3720517316847 40.08205658721963, -105.3715667481044 40.08210790769671, -105.3712911926056 40.08211536164035, -105.3710047166085 40.08208494329329, -105.3706571489542 40.0819848523058, -105.3701603136584 40.08182251295334, -105.3693330902472 40.08154316557858, -105.3691740018331 40.08149407507, -105.3689732329173 40.08146939130329, -105.3687454792302 40.08146913257269, -105.3682581015067 40.08148550858736, -105.3674792688943 40.08151471573545, -105.3669855945874 40.08156515588454, -105.3666338417142 40.08163741303427, -105.3665354783196 40.08168099405719, -105.3664748780766 40.08172531938194, -105.3664584034446 40.08159014621046, -105.3664654543084 40.08151024750345, -105.3665410705586 40.0813216177777, -105.3666249026477 40.08104341501357, -105.3665924458401 40.08081366575016, -105.3664632649919 40.08064976953737, -105.3662886091598 40.08052481296188, -105.3660390097108 40.08039337010403, -105.3659304079325 40.08034970692742, -105.3658929678842 40.08033465331701, -105.3657461992619 40.08003983094896, -105.3657423068642 40.08003200973842, -105.3656923072547 40.07998801008782, -105.365564750368 40.07986337558394, -105.3655613064671 40.07986000947152, -105.36547830664 40.07972600962538, -105.3654660928458 40.0796893671258, -105.3654633071831 40.0796810104118, -105.365430306542 40.07966001037191, -105.365182305831 40.0795810101703, -105.3650123076826 40.07954700945725, -105.3646413071265 40.07954001023455, -105.3646409597663 40.07954016834047, -105.3644273067806 40.07963700967829, -105.3641503065364 40.07968800899322, -105.3640113064601 40.07968900896079, -105.3640110721188 40.07968893393132, -105.3638723068514 40.07964401110103, -105.3637572863339 40.079587932841, -105.3637380311503 40.07957854522331, -105.3652410674733 40.07915339564261, -105.3652857427266 40.07914075772138, -105.3650620067686 40.07914218420888, -105.364451609022 40.07932611178899, -105.3644452352826 40.0793280334828, -105.3644119629354 40.07914632201314, -105.3643715348942 40.07889535434658, -105.3643097355887 40.07858571793681, -105.3642741451352 40.07840741532311, -105.3642283755162 40.07817809457496, -105.3642159208946 40.0781157013513, -105.3641896030986 40.07800118147891, -105.3641331627319 40.07770186991803, -105.364130402719 40.07768724201821, -105.3639345284794 40.07776073618592, -105.3638318920551 40.07763710989789, -105.3637768699827 40.07764845253151, -105.3628899389825 40.07783129497066, -105.3627564852363 40.07785880595277, -105.362</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E5" t="n">
-        <v>5</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Casey MS</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1301 High St, Boulder, CO 80304</t>
+        </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Casey MS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1301 High St, Boulder, CO 80304</t>
+          <t>http://cam.bvsd.org/</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
+          <t>Casey Middle School</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>40.0228711759357</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-105.2791579470394</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
           <t>http://cam.bvsd.org/</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Casey Middle School</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>40.0228711759357</v>
-      </c>
-      <c r="M5" t="n">
-        <v>-105.2791579470394</v>
-      </c>
       <c r="N5" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>http://cam.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
         <is>
           <t>POINT (-105.2791579470394 40.0228711759357)</t>
         </is>
@@ -808,59 +774,53 @@
           <t>MULTIPOLYGON (((-105.0528254173539 39.97775321191219, -105.0623973749708 39.97372063584294, -105.0649011917563 39.97266558612067, -105.0651118917171 39.97257307983785, -105.0655694045389 39.9723662368725, -105.065843589435 39.97223613527462, -105.0658811416601 39.97221831119657, -105.0661894751648 39.97206622071226, -105.0664943064096 39.97191000920827, -105.0667955519143 39.97174972953768, -105.0669332243926 39.97167371577209, -105.0670931060007 39.97158542816613, -105.0673868899058 39.97141715346223, -105.0676768084355 39.97124496093888, -105.0679627769857 39.97106889804302, -105.0682344853294 39.97089555776282, -105.0682447038632 39.97088902300355, -105.0685225067772 39.97070538868115, -105.068796101087 39.97051804972923, -105.0690654009565 39.9703270653004, -105.0693303228938 39.97013249455646, -105.0695907916381 39.96993439128609, -105.0698467248178 39.9697328236623, -105.0700980436669 39.96952784546108, -105.0703446716672 39.96931952577825, -105.0705865334178 39.96910794272046, -105.0707451313361 39.96896671059965, -105.0710392581784 39.96869541182943, -105.0717161300403 39.96807106305508, -105.0721451917206 39.96767528499866, -105.0748030386571 39.96522348552804, -105.0755271326264 39.96455551191475, -105.0756795819458 39.96441977864863, -105.0760226022435 39.9641223622555, -105.0762591021639 39.96392605437885, -105.0765000134104 39.96373295238015, -105.0765121122001 39.96372358851206, -105.076745267736 39.96354311362378, -105.0769947863516 39.96335659723671, -105.0772484951806 39.96317345786009, -105.0775063177919 39.96299375282862, -105.0777681754329 39.96281753676679, -105.078033987013 39.96264486429067, -105.0782188195883 39.96252897618582, -105.078303672632 39.96247578731922, -105.0785771512385 39.96231035506532, -105.078790249033 39.96218600590304, -105.0788543347446 39.96214861941868, -105.0791351467864 39.96199062961024, -105.0792737237913 39.96191547900955, -105.0794194922649 39.96183643660421, -105.0797072960419 39.96168608153102, -105.0797096277661 39.96168490746428, -105.0799981319371 39.96153978167267, -105.0804681708858 39.96137839815337, -105.0807716778314 39.96128039372289, -105.0810773181376 39.96118649517031, -105.0811351954348 39.96116960736901, -105.0813850402922 39.96109671219882, -105.0816947493415 39.9610110768708, -105.0820063527403 39.96092961045033, -105.0823197567362 39.96085234050275, -105.0826348617594 39.9607792891692, -105.0829515752528 39.9607104804185, -105.0832698046996 39.96064593191601, -105.0834149319631 39.96061856582238, -105.0835894458524 39.96058566578888, -105.0835950222725 39.96058461865386, -105.0835984859981 39.9605839691827, -105.0836019532348 39.96058331972419, -105.0836054181252 39.96058267115772, -105.0836088841913 39.96058202169477, -105.083612350252 39.96058137313233, -105.0836158186588 39.96058072367757, -105.083619282362 39.96058007780842, -105.0836227484114 39.96057943104697, -105.0836262144553 39.96057878518599, -105.0836296828453 39.9605781384328, -105.0836331500594 39.96057749257591, -105.0836366160866 39.96057684941663, -105.08364008446 39.96057620536502, -105.0836435540202 39.96057555861563, -105.0836470188713 39.96057491635244, -105.0836504848872 39.96057427499397, -105.0836539556066 39.96057363004976, -105.0836574192707 39.96057299048394, -105.0836608911548 39.96057234644444, -105.0836643559891 39.9605717068826, -105.0836678278567 39.96057106554482, -105.0836712938558 39.96057042688767, -105.0836747633769 39.96056978644184, -105.0836782317166 39.96056914779295, -105.0836817000507 39.96056851004457, -105.0836851707256 39.96056787230461, -105.0836886390596 39.96056723455608, -105.0836921109103 39.96056659591945, -105.0836955792277 39.96056596087259, -105.0836990510781 39.9605653222358, -105.0837025182251 39.9605646871845, -105.0837059912293 39.96056405125364, -105.0837094583596 39.96056341890407, -105.0837129290119 39.96056278476582, -105.0837163996588 39.96056215152812, -105.0837198714869 39.96056151649324, -105.0837233409632 39.96056088325109, -105.0837268127747 39.96056025091792, -105.0837302810585 39.96055962127388, -105.0837337552162 39.96055898804835, -105.083737227011 39.9605583584168, -105.0837406988058 39.96055772878519, -105.0837441694246 39.96055710004981, -105.0837476412248 39.96055646951731, -105.0837511153602 39.96055583989384, -105.0837545847974 39.96055521295525, -105.0837580589381 39.9605545824309, -105.0837615307161 39.96055395550054, -105.0837650024939 39.96055332857008, -105.0837684742552 39.96055270434148, -105.0837719518849 39.96055207743193, -105.0837754213053 39.96055145319465, -105.0837788989348 39.96055082628491, -105.0837823671848 39.96055020204319, -105.0837858412865 39.96054957782249, -105.0837893153773 39.96054895540301, -105.0837927918197 39.96054833119056, -105.0837962647344 39.96054770966726, -105.0837997388194 39.96054708814808, -105.0838032140748 39.96054646663302, -105.083806690506 39.96054584422146, -105.0838101634205 39.96054522269775, -105.0838136363184 39.96054460387581, -105.0838171092107 39.96054398595449, -105.0838205879769 39.96054336445156, -105.083824057347 39.96054274831861, -105.0838275360967 39.96054212951744, -105.0838310148517 39.96054150981553, -105.0838344865624 39.96054089369068, -105.0838379606137 39.96054027757422, -105.0838414393467 39.96053966147456, -105.0838449145684 39.96053904536213, -105.0838483921307 39.960538429258, -105.083851864995 39.9605378158388, -105.0838553460684 39.9605371997472, -105.0838588212679 39.96053658723688, -105.0838622964727 39.96053597382583, -105.0838657751887 39.96053536042736, -105.0838692503714 39.96053475061868, -105.0838727314336 39.9605341363278, -105.0838762042755 39.96053352651045, -105.0838796818043 39.96053291580925, -105.0838831605036 39.9605323051122, -105.0838866392027 39.96053169441505, -105.0838901143741 39.96053108640699, -105.0838935954139 39.96053047571807, -105.0838970717556 39.96052986771409, -105.083900550438 39.96052925971836, -105.0839040314611 39.96052865173108, -105.0839075066102 39.96052804732509, -105.0839109888036 39.96052743934182, -105.0839144651286 39.96052683403919, -105.0839179461349 39.96052622875342, -105.0839214248005 39.96052562345907, -105.0839249022901 39.96052501906101, -105.0839283844667 39.9605244137791, -105.0839318607694 39.96052381207851, -105.083935341759 39.96052320949416, -105.0839388215782 39.96052260690542, -105.0839423025677 39.96052200432079, -105.0839457847275 39.96052140174031, -105.083949259843 39.96052080273695, -105.0839527443434 39.96052020016469, -105.0839562241459 39.96051960027736, -105.083959706289 39.96051900039836, -105.0839631860858 39.96051840141151, -105.0839666670419 39.96051780423004, -105.0839701480144 39.96051720434649, -105.0839736266242 39.96051660805698, -105.0839771099209 39.96051601088363, -105.0839805943879 39.9605154137144, -105.0839840753383 39.96051481743307, -105.0839875551072 39.96051422294863, -105.0839910407444 39.96051362578331, -105.0839945181669 39.96051303219087, -105.0839980014469 39.96051243771883, -105.0840014870674 39.96051184325513, -105.0840049680009 39.96051124967506, -105.084008447753 39.96051065789194, -105.0840119357142 39.96051006343639, -105.0840154131144 39.96050947344588, -105.0840189010645 39.9605088807914, -105.084022379624 39.96050829260622, -105.0840258663927 39.96050770174858, -105.0840293519908 39.9605071108866, -105.084032831726 39.9605065218047, -105.0840363161426 39.96050593273956, -105.0840398029001 39.96050534368276, -105.0840432861352 39.96050475641453, -105.0840467670241 39.96050417003831, -105.0840502514186 39.96050358457534, -105.0840537405165 39.96050299552659, -105.0840572225701 39.96050241005499, -105.0840607081403 39.96050182369524, -105.0840641913476 39.96050124092958, -105.0840676792585 39.96050065457812, -105.0840711612954 39.96050007180799, -105.0840746480192 39.96049948815401, -105.0840781347376 39.96049890540058, -105.0840816214558 39.96049832264705, -105.0840851046519 39.96049774168201, -105.0840885925404 39.96049715893248, -105.0840920780771 39.96049657797571, -105.0840955624379 39.96049599791521, -105.084099047969 39.96049541785884, -105.0841025381871 39.96049483691866, -105.0841060213608 39.96049425955555, -105.0841095115733 39.96049367951577, -105.0841129982635 39.96049310126449, -105.0841164849483 39.96049252391376, -105.084119971633 39.96049194656296, -105.0841234583011 39.9604913719139, -105.084126947332 39.96049079367064, -105.0841304328296 39.96049021901722, -105.0841339218383 39.96048964437633, -105.084137410847 39.96048906973534, -105.0841409010315 39.96048849419781, -105.0841443830013 39.96048792223324, -105.0841478731802 39.96048734759611, -105.0841513598314 39.96048677564822, -105.0841548488288 39.96048620280799, -105.0841583413319 39.96048563088095, -105.0841618303292 39.96048505804052, -105.0841653157933 39.96048448878988, -105.0841688047685 39.96048391955179, -105.084172296101 39.96048334762011, -105.084175786252 39.96048277748539, -105.0841792728698 39.96048221094053, -105.0841827641856 39.96048164171044, -105.084186253144 39.96048107517378, -105.0841897444597 39.96048050594352, -105.0841932345885 39.96047993941084, -105.0841967235468 39.96047937287384, -105.084200213659 39.9604788090429, -105.0842037049579 39.96047824251414, -105.0842071938996 39.96047767867879, -105.0842106840116 39.96047711484754, -105.0842141752939 39.96047655102036, -105.0842176677466 39.96047598719733, -105.0842211601992 39.96047542337421, -105.0842246467834 39.96047486223177, -105.0842281427526 39.96047429752046, -105.0842316316773 39.96047373638628, -105.0842351229429 39.96047317526042, -105.0842386165491 39.96047261414292, -105.0842421054573 39.96047205571033, -105.0842456002338 39.96047149459685, -105.0842490903123 39.96047093616829, -105.0842525827315 39.96047037774804, -105.0842560774913 39.96046981933619, -105.0842595687235 39.96046926361346, -105.0842630623074 39.96046870609777, -105.084266553545 39.96046814947415, -105.0842700471124 39.96046759466021, -105.0842735418555 39.96046703894973, -105.0842770330929 39.96046648232583, -105.0842805290064 39.96046592661936, -105.0842840190458 39.96046537449425, -105.0842875137723 39.96046482148525, -105.084291009691 39.96046426487781, -105.0842944985435 39.96046371545011, -105.0842979956051 39.9604631633499, -105.0843014903368 39.96046260943984, -105.0843049838761 39.96046205912804, -105.0843084762395 39.96046150971257, -105.084311972114 39.96046096030963, -105.0843154691753 39.9604604082089, -105.0843189638848 39.96045985790089, -105.0843224562315 39.96045931118692, -105.084325955617 39.96045876179622, -105.0843294456338 39.9604582132723, -105.084332941497 39.96045766567005, -105.084336433827 39.96045712165759, -105.0843399355421 39.9604565740762, -105.0843434325701 39.96045602737846, -105.0843469248999 39.9604554833657, -105.0843504219278 39.96045493666776, -105.0843539166038 39.96045439176255, -105.0843574100874 39.9604538504556, -105.0843609117802 39.96045330647613, -105.0843644052637 39.96045276516899, -105.0843679010934 39.9604522229695, -105.0843714004397 39.96045167988194, -105.0843748950935 39.9604511385787, -105.0843783956046 39.96045059639577, -105.0843818890714 39.96045005779001, -105.0843853907528 39.96044951561112, -105.0843888830491 39.96044897700094, -105.0843923823731 39.96044843751532, -105.0843958758232 39.96044790161103, -105.084399377488 39.96044736213367, -105.0844028744492 39.96044682624184, -105.0844063749324 39.9604462885613, -105.084409871899 39.96044575176866, -105.08441336886 39.96044521587651, -105.0844168669913 39.96044467998852, -105.0844203651116 39.96044414590168, -105.0844238655837 39.96044361002188, -105.0844273637038 39.96044307593485, -105.0844308618186 39.96044254274836, -105.0844343622794 39.96044200866955, -105.0844378592126 39.96044147727986, -105.0844413596679 39.96044094410149, -105.0844448577714 39.96044041271587, -105.0844483605509 39.96043988224761, -105.0844518598192 39.96043935176664, -105.0844553579115 39.96043882218198, -105.0844588583501 39.96043829170497, -105.0844623576018 39.9604377639256, -105.0844658615568 39.96043723256042, -105.0844693537751 39.9604367065568, -105.0844728588786 39.96043617879819, -105.0844763604763 39.96043565012621, -105.0844798585408 39.96043512504401, -105.0844833613033 39.96043459727665, -105.0844868605436 39.96043407129777, -105.08449036446 39.96043354623639, -105.084493861343 39.9604330229508, -105.0844973664296 39.9604324978934, -105.0845008668181 39.96043197552092, -105.0845043707397 39.96043144955845, -105.0845078687929 39.96043092627666, -105.0845113679944 39.96043040660159, -105.0845148742347 39.9604298842498, -105.0845183769638 39.96042936188523, -105.084521877341 39.96042884131344, -105.0845253812295 39.96042832075415, -105.0845288827715 39.96042780108701, -105.084532385484 39.96042728142393, -105.084535885839 39.96042676445424, -105.0845393908921 39.96042624479943, -105.0845428912471 39.96042572782954, -105.0845463951242 39.96042520907093, -105.0845498989903 39.9604246921135, -105.0845534028563 39.96042417515598, -105.0845569031947 39.96042366088757, -105.0845604058738 39.96042314662753, -105.0845639132453 39.96042263058297, -105.0845674159353 39.96042211452143, -105.0845709185977 39.96042160296298, -105.0845744247878 39.96042108871516, -105.0845779274502 39.96042057715649, -105.0845814336346 39.96042006380912, -105.0845849386486 39.96041955045742, -105.0845884389701 39.96041903889005, -105.0845919427861 39.96041853003707, -105.0845954524706 39.96041801850324, -105.0845989527754 39.96041750963744, -105.0846024612894 39.96041699809916, -105.0846059651107 39.96041648834515, -105.0846094677397 39.96041598218939, -105.0846129774075 39.96041547335694, -105.0846164765197 39.96041496808895, -105.0846199861873 39.96041445925627, -105.0846234911624 39.96041395220792, -105.0846269961319 39.96041344606006, -105.0846305022718 39.9604129399163, -105.0846340072247 39.9604124364702, -105.0846375180461 39.96041193034313, -105.0846410230044 39.96041142599616, -105.0846445279518 39.96041092345035, -105.0846480352453 39.96041042001222, -105.0846515390111 39.96040991926331, -105.0846550486509 39.96040941493276, -105.084658553587 39.96040891418785, -105.0846620596881 39.96040841434764, -105.0846655681353 39.96040791361514, -105.0846690754121 39.9604074128783, -105.0846725838647 39.96040691124497, -105.0846760887787 39.96040641410207, -105.0846795960389 39.96040591606685, -105.0846831091674 39.96040541535069, -105.0846866093832 39.96040492089254, -105.0846901236711 39.96040442198164, -105.0846936321015 39.96040392395023, -105.0846971358338 39.96040342860376, -105.0847006442421 39.96040293417474, -105.0847041550022 39.96040243795269, -105.0847076657566 39.96040194263121, -105.0847111706537 39.96040144818916, -105.0847146790509 39.96040095556098, -105.084718187448 39.96040046293266, -105.0847217017135 39.96039996762343, -105.0847252042421 39.96039947767574, -105.0847287173152 39.96039898596462, -105.0847322268825 39.96039849334009, -105.0847357340925 39.96039800340896, -105.0847392436433 39.96039751348618, -105.0847427531886 39.96039702446389, -105.0850096380202 39.96035979868915, -105.0850658527888 39.96035196090204, -105.0854661723567 39.96029612401237, -105.0857839598441 39.9602517994901, -105.08581766119 39.96024710027866, -105.0859393187197 39.96023012947124, -105.0863498292124 39.96017287246411, -105.0870446975825 39.96009434918611, -105.0871191644284 39.96008593633609, -105.0872096218029 39.96007571814968, -105.0874111940689 39.96005124220132, -105.08747407241 39.95978207714827, -105.0879262449088 39.95978400035138, -105.0880333812514 39.95978094919757, -105.0880380735751 39.95888622819314, -105.0880382211008 39.95885810821171, -105.088040376847 39.95844732158841, -105.0881544918518 39.95844611011514, -105.088625575105 39.95844758571651, -105.0886640890448 39.95844581560196, -105.0886662517168 39.95824081254283, -105.0886676791558 39.95810768699305, -105.0886681074652 39.95803876706348, -105.088667006154 39.95803876493348, -105.0886669710434 39.95803876480815, -105.0886139490879 39.95803863676791, -105.0886136635223 39.95803863574837, -105.0886129648172 39.95803863415455, -105.0886128489525 39.9580386337409, -105.088156924958 39.9580375355978, -105.0881558248172 39.95803753346706, -105.0880454746665 39.95803347060461, -105.0880445006021 39.9580195635822, -105.0880433829552 39.95801955328184, -105.0879369926213 39.95801852529694, -105.0879358702931 39.9580185149788, -105.0879130844023 39.95801829479073, -105.0879119632444 39.95801828447654, -105.087644656805 39.95801569800683, -105.0876435368176 39.95801568769421, -105.0864090392693 39.95800374277388, -105.0864089196698 39.95800377927178, -105.085944272825 39.95814719484354, -105.085944214198 39.95814721264614, -105.0858422212814 39.95817869446593, -105.0858421626544 39.95817871226845, -105.0853102002613 39.95834290120607, -105.0853101451451 39.95834291902096, -105.0852568616573 39.95835978581623, -105.0852568276513 39.95835979650178, -105.0852142572362 39.95837252275794, -105.0852141728226 39.95837254677202, -105.0851744799152 39.95838380628351, -105.0851743486054 39.95838384363866, -105.0851713683735 39.95838468583803, -105.0851712382503 39.95838472049549, -105.0851282032845 39.95839627148312, -105.0851280286276 39.95839631588745, -105.0850847889214 39.95840727438583, -105.0850845674009 39.95840732672732, -105.0850411288291 39.95841768915476, -105.0850408592745 39.95841774942916, -105.0849972405584 39.95842751675351, -105.0849969218048 39.95842758405593, -105.0849531323029 39.95843675721125, -105.0849527690538 39.95843682795595, -105.0849088216957 39.95844539798203, -105.0849084092641 39.95844547305273, -105.08486432509 39.95845344452852, -105.084863865833 39.95845352123168, -105.0848196530585 39.9584608905839, -105.0848191434705 39.95846096800619, -105.0847748173279 39.95846773258756, -105.0847742609255 39.95846780984096, -105.0847298330974 39.95847397329614, -105.0847292287157 39.95847404947573, -105.0847027555357 39.95847736217756, -105.084702105477 39.95847744359641, -105.0846847144455 39.95847960735617, -105.0846840621009 39.95847967976002, -105.0846394730714 39.95848463571034, -105.0846387715935 39.95848470433415, -105.0845941253996 39.95848905211304, -105.0845933771403 39.95848911516397, -105.0845486842725 39.95849286201446, -105.0845478892426 39.95849291769114, -105.0845031673014 39.95849605647136, -105.0845023278417 39.95849610478225, -105.0844575826417 39.95849864181768, -105.0844566952575 39.95849868004812, -105.084411946718 39.95850061180795, -105.0844110125797 39.95850063996208, -105.0843662724055 39.95850196648848, -105.0843652950352 39.95850198277773, -105.0843205760685 39.95850270952104, -105.0843195519606 39.95850271303195, -105.0842768016851 39.9585028461176, -105.0842748694392 39.95850283644447, -105.0842738021159 39.95850282538841, -105.0842291677117 39.95850235091626, -105.0842290811161 39.95850234880245, -105.084228056008 39.95850232438844, -105.0841834837884 39.95850124847972, -105.0841823300452 39.95850120648842, -105.0841378188191 39.95849953274163, -105.0841366382675 39.95849947263985, -105.0840922289767 39.9584972048054, -105.0840921470791 39.95849720000647, -105.0840909911929 39.95849712558269, -105.084046681476 39.95849426725479, -105.0840454063616 39.95849416808221, -105.0840012149839 39.9584907130241, -105.0840011529878 39.95849070739629, -105.0839998978684 39.95849059208348, -105.0839558329632 39.95848655023193, -105.0839557534282 39.95848654183878, -105.0839544773578 39.95848640753589, -105.0839105506463 39.95848177623136, -105.0839091600622 39.95848161179256, -105.0838653855513 39.95847639739046, -105.0838639576698 39.95847620759785, -105.0838390743395 39.95847291137007, -105.083837605523 39.958472716926, -105.0838203494051 39.95847041014899, -105.083820295618 39.9584704018488, -105.0838188865613 39.95847019591163, -105.0837754562364 39.95846381725983, -105.0837739607767 39.95846357768551, -105.0837307130412 39.95845662325169, -105.0837291908175 39.95845635836152, -105.0836861584315 39.9584488300656, -105.0836861011444 39.95844881995132, -105.0836845965917 39.95844853621046, -105.0836417643307 39.95844043579893, -105.0836401827601 39.95844011485198, -105.0835975938788 39.95843145058738, -105.083597505047 39.95843143135245, -105.0835959715385 39.95843109796932, -105.0835536225104 39.95842187254114, -105.0835535208322 39.95842184875641, -105.0835519734337 39.95842149010389, -105.0835098782986 39.95841170446378, -105.0835097976648 39.95841168435775, -105.0835082013262 39.95841129040186, -105.0834663694259 39.95840094818657, -105.0834663110015 39.95840093266411, -105.0834646692338 39.95840050341751, -105.0834231134047 39.95838961097829, -105.0834230736785 39.95838960002673, -105.0834213876632 39.95838913369234, -105.0833801172471 39.95837769466598, -105.0833783706378 39.95837718488006, -105.0833374008502 39.95836519932185, -105.083335634549 39.95836465613951, -105.0832949770394 39.95835213309849, -105.0832931933815 39.95835155742886, -105.0832528481451 39.9583384978061, -105.0832510541473 39.95833789057515, -105.0832110480427 39.95832430437537, -105.0832092320398 39.95832365923636, -105.0831695767604 39.9583095483035, -105.0831677422527 39.95830886707035, -105.0831284436178 39.95829423682988, -105.0831265976219 39.95829352042862, -105.083089599058 39.95827597494203, -105.0830896020937 39.9582756696281, -105.0830905175779 39.95814383200661, -105.0830917470141 39.95796309669239, -105.0830914379236 39.95791388241516, -105.0830912914456 39.9578828783425, -105.0830916557268 39.9578012227973, -105.0830905532878 39.95780121430522, -105.0827441915763 39.95779842227282, -105.0827430961593 39.95779841380289, -105.0811926774133 39.95778589991825, -105.0811915867279 39.95778588334476, -105.0797086205163 39.95776348378201, -105.079707513408 39.95776347343922, -105.0796278873055 39.95776268671114, -105.0796267977524 39.9577626764316, -105.0765567090186 39.95773230338303, -105.0765556299548 39.95773230031829, -105.0753803964513 39.95772928419706, -105.0753793466463 39.95772928122915, -105.07420410847 39.95772626840448, -105.0742030621761 39.95772626543882, -105.0719823361877 39.95771661303881, -105.0719822955386 39.95771376408718, -105.0719811965841 39.95763613716662, -105.0718814336875 39.95058499173008, -105.071880156866 39.95049172946248, -105.0718823803634 39.9502020119051, -105.0720227034047 39.95021855966071, -105.074243983681 39.95048048858849, -105.0745735205932 39.95052068211166, -105.0753572740584 39.95053202794011, -105.076103921084 39.95054268882134, -105.076548242864 39.95054710934591, -105.0765585879308 39.94919947316338, -105.076573762168 39.94765414067553, -105.0765867743723 39.9464964353545, -105.0766014550372 39.94499877740917, -105.076617719676 39.94333941431218, -105.0767360412157 39.94334022196765, -105.0812630425988 39.9433621325146, -105.0821871148648 39.94335411398962, -105.0860388355787 39.94332055103774, -105.089837629017 39.94329425448934, -105.0905070988288 39.94329150589123, -105.0905381523252 39.94329137849177, -105.0906429394402 39.94329094929207, -105.0908401727396 39.94329100598443, -105.0910515015407 39.94328985775073, -105.0910588121924 39.94240422444584, -105.0910630538564 39.94143533357321, -105.0910619951027 39.94143530369561, -105.0910619178891 39.94143530162019, -105.0909044712291 39.9414271563125, -105.0909043710449 39.94131892761472, -105.0909032136222 39.94006601094053, -105.0909447678353 39.94006555055373, -105.0909399203652 39.93925547113504, -105.0909388888204 39.93925539722021, -105.0909386654367 39.93925538111568, -105.0908988896852 39.93924889918723, -105.0908992109706 39.93920895855562, -105.0909009129949 39.93899798932196, -105.0909023057667 39.93869844672675, -105.0909012831155 39.93869845210159, -105.0908424959132 39.93869504775551, -105.090845184441 39.93815985715184, -105.0908493310474 39.93733416590344, -105.0908557345987 39.93605890767786, -105.0910157459438 39.93605931468678, -105.0918615391184 39.93606134993986, -105.0924035059316 39.93606276275314, -105.0933812509434 39.93606530861484, -105.0936100881903 39.93606736899439, -105.0938741497766 39.9360664242047, -105.0940532611034 39.93606746625473, -105.0941950319923 39.93606829722803, -105.0942317090223 39.936068511994, -105.0944119399563 39.93606956913881, -105.0945908398346 39.93607115000719, -105.09476502367 39.93607269419247, -105.0950355885139 39.93607365200723, -105.0951422560202 39.93606933899665, -105.099991742204 39.93605491013817, -105.1046341365572 39.93611220688962, -105.1081492163309 39.93614206184396, -105.1086808361625 39.93614327640896, -105.109037945844 39.93614408640219, -105.1091476096643 39.93614433425925, -105.1092309617087 39.93614452157765, -105.109237555661 39.93614271109521, -105.109236684834 39.93553881744052, -105.1092370249853 39.93540888430044, -105.1097777212305 39.93505856392756, -105.1108825455564 39.93434273300105, -105.1122097787322 39.93350518891695, -105.1122542835765 39.93347639049676, -105.112298162726 39.93344754492023, -105.1123413922496 39.93341812792112, -105.1123839627366 39.93338814847505, -105.1124258612613 39.93335761644661, -105.1124670725634 39.93332654079186, -105.1125075872323 39.93329493048649, -105.1125473923425 39.93326279539504, -105.1125864726237 39.93323014627482, -105.1126248198305 39.93319699300623, -105.1126624222279 39.93316334185509, -105.112699266845 39.93312921079185, -105.1127353419725 39.93309460157923, -105.1127706323048 39.93305953127903, -105.1128051389664 39.93302400800174, -105.1128388431675 39.93298804429421, -105.1128717343385 39.93295164732695, -105.1129038065386 39.93291483329256, -105.112935043359 39.93287760754068, -105.1129654411784 39.93283998987437, -105.1129949918083 39.93280198026674, -105.113023677573 39.93276360117568, -105.1130514984277 39.93272486070767, -105.113078446138 39.93268576694161, -105.1131045065741 39.93264633604267, -105.1131296761662 39.93260657880734, -105.1131539431397 39.93256650870666, -105.1131773051049 39.93252613473981, -105.1131997491178 39.9324854703738, -105.1132212762678 39.9324445300235, -105.1132418736157 39.9324033262552, -105.1132615340774 39.93236187075425, -105.1132802564333 39.93232017252367, -105.1132980335634 39.93227824955331, -105.1133148583837 39.93223611352849, -105.1133307273246 39.93219377524553, -105.1133456344566 39.93215124909558, -105.113359577355 39.93210855038208, -105.1133725489611 39.9320656862871, -105.1133845491696 39.93202267572452, -105.1133955662373 39.93197952676115, -105.1134056070834 39.93193625743383, -105.113414662279 39.93189288032042, -105.1134227329501 39.9318494035309, -105.113429811982 39.93180584415427, -105.1134359028049 39.93176221661275, -105.1134409983348 39.93171853259142, -105.1134451020171 39.93167480381061, -105.1134482067322 39.93163104825973, -105.113450314771 39.93158727495323, -105.1134514272185 39.93154349920609, -105.1134515416603 39.9314997345202, -105.1134506592019 39.93145599260789, -105.1134487762438 39.931412289669, -105.1134459032609 39.93136863564597, -105.113442030799 39.93132504761954, -105.113437162339 39.9312815310053, -105.1134313012498 39.93123811103305, -105.1134244521873 39.93119479222157, -105.113416610382 39.93115159076657, -105.1134077827836 39.93110851930052, -105.1133979751567 39.93106559315386, -105.1133871804378 39.93102282040854, -105.1133754137557 39.93098021552567, -105.1133626703306 39.93093779650227, -105.113348960637 39.93089557328036, -105.113334278771 39.93085355574722, -105.1133186421806 39.93081176197423, -105.1133020484817 39.93077020005903, -105.1132844999339 39.93072888441935, -105.1132659917676 39.93068783125076, -105.113233333253 39.93062041135646, -105.1131118570121 39.93037915497996, -105.1122051443685 39.9286176515559, -105.112204645089 39.92861698878723, -105.1122038636647 39.92861595039223, -105.1121075772735 39.92848730040697, -105.112107214614 39.92848647687905, -105.1120967981585 39.92846279035226, -105.1120837940408 39.92843332545336, -105.1120587550635 39.92837964708677, -105.1120324811199 39.92832631491299, -105.1120049849938 39.9282733442855, -105.1119762689248 39.92822075322429, -105.1119463480464 39.92816855528933, -105.1119452737562 39.92816676565235, -105.1119152257527 39.92811677120648, -105.1119151561972 39.92811665928968, -105.1119141116025 39.92811499674616, -105.1118829195319 39.92806541184156, -105.1118817643469 39.92806365345461, -105.1118494304382 39.92801449791246, -105.111848236553 39.92801275650742, -105.1118147748001 39.92796403847989, -105.1118135410398 39.92796231495335, -105.1117789525426 39.92791404705239, -105.1117776870397 39.92791235133907, -105.1117419938938 39.92786455705546, -105.1117406873717 39.92786287471342, -105.1117038953714 39.92781556397286, -105.1117025524685 39.92781390222298, -105.111664672062 39.92776708947031, -105.111663293943 39.92776544921718, -105.1116243367531 39.92771914800042, -105.1116229245829 39.92771753014858, -105.1115828952545 39.92767174678695, -105.1115814571705 39.92767016037045, -105.1115403777728 39.9276249228577, -105.1115389009839 39.92762335432344, -105.1114967808562 39.92757866629268, -105.1114967564333 39.92757864099171, -105.1114952746698 39.92757712467863, -105.1114521207296 39.9275330041653, -105.1114505828162 39.92753148766221, -105.1114063367063 39.92748791105097, -105.1114047705602 39.92748642237255, -105.1113594310861 39.92744339416132, -105.1113578471896 39.927441941449, -105.1113115286313 39.92739952596935, -105.1113099106939 39.9273980938567, -105.1112626165257 39.92735629742379, -105.1112609750245 39.92735489495286, -105.1112127180535 39.92731372841661, -105.111212659834 39.92731368048491, -105.1112110529834 39.92731235648804, -105.1111618506854 39.92727183251554, -105.111160165556 39.92727049114104, -105.1111100307173 39.9272306241849, -105.1111100062535 39.92723060608901, -105.1111083231939 39.92722931245594, -105.1110572686417 39.92719010976344, -105.1110572395243 39.92719008714854, -105.1110555422339 39.92718882769187, -105.1110035830733 39.92715030732615, -105.11100184127 39.92714905852634, -105.1109489916877 39.92711119441476, -105.1109472591628 39.92710996005612, -105.1108928284495 39.92707140337049, -105.1108909641212 39.9270703063674, -105.1093961302332 39.92618804064294, -105.1093961314852 39.9261876173348, -105.1093963927524 39.92610719247062, -105.1093970325059 39.92591051920145, -105.1093983533093 39.92550463644266, -105.1097181218421 39.92570515554632, -105.1102888127801 39.92606301804486, -105.110533010465 39.92620741090535, -105.1109611901158 39.92646588786492, -105.1117548190385 39.92701045155007, -105.1118443320229 39.92708224169476, -105.1127892552828 39.92784224790676, -105.1134254430625 39.92836563900499, -105.113704554754 39.92859527303179, -105.1137050251862 39.92859566099454, -105.1137255080341 39.92864659560585, -105.1137262203602 39.92864847858181, -105.1140585185026 39.92932809442664, -105.1142666296578 39.9297534484365, -105.1142675329075 39.92975529512095, -105.1144409722058 39.93010978460534, -105.1144411075297 39.93011005976095, -105.1144418766246 39.9301116330937, -105.1186305278242 39.93297156507604, -105.1186310511322 39.93297192257087, -105.1187423547122 39.93370473330269, -105.1187426310094 39.93370658508118, -105.1187496800574 39.93377277206956, -105.1187554050253 39.93382717399349, -105.1187555828143 39.93382885792241, -105.1187358911118 39.93399247936708, -105.1187356803395 39.93399418722844, -105.1187155377534 39.93415766216859, -105.1187153808925 39.93415893428716, -105.118673946249 39.93423753404684, -105.1186732794773 39.93423877115278, -105.1182594976906 39.93500675201376, -105.1182587942474 39.93500805834684, -105.1186175723289 39.93567414007994, -105.1186184037774 39.93567568026551, -105.1186179894219 39.93603778437812, -105.1186179804826 39.93603959378159, -105.1185991792267 39.93884273667501, -105.1185991667161 39.93884455687426, -105.1185988645399 39.93887769668284, -105.1185988473492 39.93887951686656, -105.1185965575348 39.9391274519986, -105.1185965403389 39.93912927308293, -105.1185957855938 39.93921094994099, -105.1185957683928 39.93921277192599, -105.1185948788888 39.93930872385114, -105.1185948615821 39.93931056474968, -105.1185970663537 39.93942461764238, -105.1185971028635 39.93942645961974, -105.1186016797191 39.93965792092657, -105.1186017162192 39.93965976470523, -105.1186032568698 39.9397377195128, -105.1186032935058 39.93973953897395, -105.1186017200063 39.93990283122475, -105.1186017016353 39.93990465320577, -105.1185787173852 39.94163370729682, -105.1185786931275 39.94163553556272, -105.1185577375591 39.9432111717849, -105.1185561841228 39.94332791779106, -105.1139808884187 39.94334427863482, -105.1139797592105 39.94334428565912, -105.1117289010016 39.94335835641672, -105.1117277916897 39.94335836258531, -105.1115097327091 39.94335971429, -105.1115086222681 39.94335971324735, -105.1113693752345 39.94335951289126, -105.111368241391</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>6</v>
-      </c>
-      <c r="E6" t="n">
-        <v>6</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Centaurus HS</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>10300 W South Boulder Rd, Lafayette, CO 80026</t>
+        </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Centaurus HS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>10300 W South Boulder Rd, Lafayette, CO 80026</t>
+          <t>http://ceh.bvsd.org/</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
+          <t>Centaurus High School</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>39.98635981263706</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-105.1125276640655</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
           <t>http://ceh.bvsd.org/</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Centaurus High School</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>39.98635981263706</v>
-      </c>
-      <c r="M6" t="n">
-        <v>-105.1125276640655</v>
-      </c>
       <c r="N6" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>http://ceh.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
         <is>
           <t>POINT (-105.1125276640655 39.98635981263706)</t>
         </is>
@@ -880,59 +840,53 @@
           <t>POLYGON ((-105.2726881734809 40.03464911391067, -105.2726840628362 40.03406108764794, -105.2726820898275 40.03390296023866, -105.2726760239568 40.0331518655748, -105.2726760357997 40.03272004799683, -105.272671164566 40.03193189473561, -105.2726661710148 40.03160905132167, -105.2726628596342 40.03142401880926, -105.2726558625326 40.03073798238746, -105.2726510020113 40.03005387211383, -105.273645871071 40.030061869293, -105.2741701059328 40.03006097391676, -105.2751321551345 40.03005901118281, -105.276498044355 40.03007099921356, -105.277470066055 40.03007699534945, -105.2781960300691 40.03008690379698, -105.2784088644469 40.03008703905117, -105.2791998402836 40.03009102538928, -105.2793758908887 40.03009191253876, -105.2803029427175 40.03009011263436, -105.2804018518184 40.030093047055, -105.2805939720805 40.03009396023452, -105.2820898563745 40.03010393344913, -105.2820900004695 40.03010393732394, -105.2821084505153 40.03010442340204, -105.28212225549 40.02926831736175, -105.2821221918683 40.02925559915963, -105.2832689344744 40.02923208823412, -105.2844270167391 40.02923096285564, -105.2854201124465 40.02923199133771, -105.2855761122275 40.02924902721826, -105.2855863693432 40.02924869918922, -105.2855862117171 40.02922543814994, -105.2855754584629 40.02732638721953, -105.2855712105374 40.02672743692585, -105.2855692118289 40.02663843724292, -105.2855892107703 40.02642143748587, -105.2856742107215 40.02601043682525, -105.2856822111836 40.02592843665887, -105.2856812109885 40.02583443661324, -105.2856660543705 40.0255160131922, -105.2867490705732 40.02551994347327, -105.2887301598848 40.02552001896971, -105.290043906236 40.02550594671673, -105.2902481507636 40.02550796560364, -105.2915040127181 40.02550612476494, -105.2920939363481 40.025498130862, -105.2925031180585 40.02550902431486, -105.2926069291672 40.02543973575167, -105.2936339345848 40.02541515269726, -105.2962396867081 40.02535273730569, -105.2962396415504 40.02215067912587, -105.2965063930992 40.02212077652984, -105.3009340316972 40.02443523818599, -105.3015129345043 40.02495411241519, -105.3019768726209 40.02523547047512, -105.3036913518517 40.02668039861787, -105.3158896760477 40.03657502954008, -105.3192074195506 40.03913430974992, -105.3199463280383 40.03974204931587, -105.3213194875436 40.04086764115979, -105.3218374986145 40.04129224587619, -105.3223361207968 40.04169918639315, -105.3228326493725 40.0421032961798, -105.3234564439344 40.04261022835578, -105.3235650157017 40.04270601443687, -105.3236279789155 40.04277070698105, -105.3236391294289 40.04281891589837, -105.3237254066363 40.04321419443117, -105.3237860406652 40.04349198382817, -105.3237843665057 40.04387571131006, -105.3237828875122 40.04421431571672, -105.3237823449867 40.0443384818003, -105.3237809310199 40.04466280651826, -105.3237793817299 40.04501725408277, -105.3237789988946 40.04510503603166, -105.3237783998165 40.04528551141335, -105.3237739562574 40.045350713323, -105.3237755669408 40.04610054821104, -105.3237764999897 40.04656136329066, -105.3237777433405 40.04717500970264, -105.3232106563202 40.04719455446896, -105.323221528834 40.04849852044671, -105.3232344307103 40.05085237381964, -105.3237807104702 40.05084289607972, -105.3237746785025 40.05174426081269, -105.323768510175 40.05268741436502, -105.3237595236597 40.05413331629786, -105.3237456249731 40.05636891728329, -105.3237422288764 40.05691517045657, -105.3236649981389 40.05690199939841, -105.3234309988263 40.05688399882967, -105.3232779999172 40.05690299883362, -105.323172998984 40.05698399884937, -105.3231529996911 40.05707399863253, -105.3231499993645 40.05709199885952, -105.3231619998333 40.05718199904416, -105.3232919997439 40.05737999907437, -105.3234339985885 40.05755099881815, -105.3235629988358 40.05765899900364, -105.3235989988297 40.05778499864036, -105.3235999997156 40.05792899912804, -105.3235059990182 40.05802799856036, -105.3233419994831 40.05810999915607, -105.3231779991147 40.05811899852135, -105.3227089981302 40.05811199963112, -105.3222399987181 40.05809499805878, -105.3220289988635 40.05805999885644, -105.321676998539 40.05804299884692, -105.3214079998949 40.05808799885816, -105.3211850003847 40.05818799905649, -105.3210514373444 40.0582376509077, -105.32106095721 40.05823758461141, -105.3221724264569 40.05822988914631, -105.3225816832363 40.05822705158369, -105.3237332159603 40.05821906132902, -105.3244526418999 40.05821394350896, -105.3282194852361 40.05818707363856, -105.3283319969811 40.05818626656585, -105.3292573137716 40.05818135374078, -105.3292665417278 40.05818130434862, -105.3292919364783 40.05818116989376, -105.3319541386962 40.05816256206004, -105.3339319600427 40.05815113377263, -105.3363688276225 40.05813097199744, -105.3372943533713 40.05812628053155, -105.3373097910866 40.05812620232494, -105.3425993028118 40.05804701136856, -105.3442073023861 40.05802301073521, -105.3446489917473 40.05801662437516, -105.3446489909119 40.05801647666802, -105.3446488464446 40.0580006719369, -105.3472232555888 40.05794871736776, -105.3472232182339 40.05796119576863, -105.3472322260892 40.05796101405485, -105.3472271551965 40.05966073692544, -105.3472224896003 40.06133066754241, -105.3486782908329 40.061357989212, -105.3486782404571 40.06137011633922, -105.3486742154388 40.06233587690733, -105.3473107204354 40.06232116573092, -105.3472109110526 40.06235733955729, -105.3470235657521 40.06242702740272, -105.346800850027 40.0625838279675, -105.3467783723339 40.06259127168354, -105.3467801571126 40.06283435827675, -105.3472076899097 40.06342523965154, -105.3472079425455 40.06342548676287, -105.3486885970446 40.06487342811074, -105.3486849106566 40.06487334582209, -105.3486975687233 40.06488572377337, -105.3471897519431 40.06485211464241, -105.3473133623905 40.06933911891326, -105.3473207934553 40.06961740186438, -105.3473209038137 40.06962151345378, -105.3473428026947 40.07044154251917, -105.3473863264873 40.07207482178335, -105.3521890440063 40.07206474065865, -105.3527429298888 40.0720635653864, -105.3527521643292 40.07206354564473, -105.3566839075929 40.0720551235077, -105.3566879098085 40.07206743037823, -105.3569141002044 40.07276297868636, -105.3569186609197 40.07276170632576, -105.3570182822697 40.07273390079512, -105.3570189338859 40.07274851995955, -105.3570658145457 40.07380002971021, -105.3570743376764 40.07380220901534, -105.357075228185 40.07380243798097, -105.357075334534 40.07380483292546, -105.3570756794207 40.07381255367425, -105.3571196919032 40.07479969608959, -105.3571280259499 40.07479762231507, -105.35803786981 40.07457117646017, -105.358117034332 40.07453663682637, -105.3581232652609 40.07453391823564, -105.358847711203 40.0742178328324, -105.3587794465179 40.07430909535827, -105.3588135101471 40.07430030621352, -105.3588112717716 40.07430329631586, -105.3590849558513 40.07423267261267, -105.3592610081719 40.07404768796147, -105.3594411968741 40.07396265795662, -105.3594470525279 40.07397642512769, -105.3594917021376 40.07408138741301, -105.3596075059446 40.0743536065922, -105.359597384184 40.07435795069615, -105.3595915406397 40.07436046088824, -105.3584869030154 40.074834666367, -105.3584826247326 40.07483650293884, -105.3581805956881 40.07496615732713, -105.3571387269635 40.07522658799327, -105.3571567757665 40.07563136333869, -105.3571651961045 40.07563123686058, -105.3580379658965 40.07561815271803, -105.3597576897657 40.07558682392172, -105.3600733286092 40.07558051699573, -105.3600823364097 40.07558033697835, -105.3600943059392 40.07558800966181, -105.3606163062426 40.0762420105657, -105.3612283062352 40.07688201049471, -105.3617303055701 40.07727800991306, -105.3621513056302 40.07752001023393, -105.362650306177 40.07779700989174, -105.3627564852363 40.07785880595277, -105.3628899389825 40.07783129497066, -105.3637768699827 40.07764845253151, -105.3638318920551 40.07763710989789, -105.3639345284794 40.07776073618592, -105.364130402719 40.07768724201821, -105.3641331627319 40.07770186991803, -105.3641896030986 40.07800118147891, -105.3642159208946 40.0781157013513, -105.3642283755162 40.07817809457496, -105.3642741451352 40.07840741532311, -105.3643097355887 40.07858571793681, -105.3643715348942 40.07889535434658, -105.3644119629354 40.07914632201314, -105.3644452352826 40.0793280334828, -105.364451609022 40.07932611178899, -105.3650620067686 40.07914218420888, -105.3652857427266 40.07914075772138, -105.3652410674733 40.07915339564261, -105.3637380311503 40.07957854522331, -105.3637572863339 40.079587932841, -105.3638723068514 40.07964401110103, -105.3640110721188 40.07968893393132, -105.3640113064601 40.07968900896079, -105.3641503065364 40.07968800899322, -105.3644273067806 40.07963700967829, -105.3646409597663 40.07954016834047, -105.3646413071265 40.07954001023455, -105.3650123076826 40.07954700945725, -105.365182305831 40.0795810101703, -105.365430306542 40.07966001037191, -105.3654633071831 40.0796810104118, -105.3654660928458 40.0796893671258, -105.36547830664 40.07972600962538, -105.3655613064671 40.07986000947152, -105.365564750368 40.07986337558394, -105.3656923072547 40.07998801008782, -105.3657423068642 40.08003200973842, -105.3657461992619 40.08003983094896, -105.3658929678842 40.08033465331701, -105.3659703076023 40.08049001044129, -105.3660033070792 40.08058400926235, -105.3651603062312 40.08079800940757, -105.36386330684 40.08112600999898, -105.3614307179702 40.08181077296624, -105.3614136449111 40.08208931510966, -105.361373970351 40.08273668039418, -105.3613838696417 40.08273389398298, -105.3616833691065 40.08264960897541, -105.3616895744276 40.08266268384122, -105.3618231569629 40.08294413896749, -105.3618343745151 40.08296777085793, -105.3618626507548 40.08302734621064, -105.3612294649398 40.08322514258172, -105.3582044235136 40.08420073402425, -105.3580926092154 40.08423693487651, -105.3581270614178 40.08459850432136, -105.3581348601366 40.08459842924469, -105.3591926002434 40.08458815364854, -105.3591925371214 40.08460053741205, -105.3591905319785 40.0849959100054, -105.3573681646263 40.08502614465402, -105.3569189380437 40.08526239120709, -105.3568395193715 40.08711423232176, -105.3556791226172 40.08712097800886, -105.3556774246944 40.08712098849529, -105.354242246951 40.08712931769688, -105.3542328567851 40.08712937248871, -105.3527096423569 40.08713819019081, -105.3527001841789 40.08713824477123, -105.3519880447198 40.08755429373965, -105.3510273451841 40.08805364431768, -105.3510314240971 40.08805658117283, -105.3510339691511 40.08805849111732, -105.3510364707778 40.08806041991922, -105.3510389277868 40.0880623756828, -105.3510405793695 40.08806372697654, -105.3510413472218 40.08806435481455, -105.3510437197018 40.08806635730237, -105.3510460487584 40.0880683768463, -105.3510483355446 40.08807042245434, -105.3510505753798 40.08807248961713, -105.3510527729524 40.08807457924146, -105.3510549200622 40.08807668771413, -105.3510570237446 40.08807881504423, -105.351059080476 40.08808096392912, -105.351061091431 40.08808313346974, -105.3510630566174 40.08808532006347, -105.3510649713371 40.08808752730682, -105.3510668391175 40.08808975070119, -105.351068656435 40.0880919929439, -105.3510704291584 40.08809425134065, -105.3510721502444 40.0880965294849, -105.3510738208755 40.08809882287498, -105.3510754457399 40.08810113241754, -105.3510770166333 40.08810345630074, -105.3510772620555 40.08810383308597, -105.3510785405837 40.08810579813619, -105.3510800410192 40.08810816876191, -105.3510817287355 40.08811069273843, -105.3510833753659 40.08811323737671, -105.3510849820807 40.08811580357887, -105.351086548892 40.08811838594115, -105.3510880757858 40.08812099076799, -105.3510895604248 40.08812361445374, -105.3510910063348 40.08812625340051, -105.3510924076469 40.08812891030255, -105.3510937713965 40.08813158516899, -105.3510950928933 40.08813427799377, -105.3510963697981 40.08813698607194, -105.3510976021068 40.08813971120482, -105.3510987945178 40.08814244979585, -105.3510999482036 40.08814520184658, -105.3511010526129 40.0881479664427, -105.3511021147673 40.08815074989782, -105.3511031346887 40.08815354230494, -105.3511041123671 40.08815634816715, -105.3511050454592 40.08815916658087, -105.351105933969 40.08816199574477, -105.351106776724 40.08816483565742, -105.3511075737242 40.08816768631873, -105.3511083343561 40.08817054503891, -105.3511090421975 40.08817341449873, -105.3511097078077 40.08817629200986, -105.3511103311927 40.08817917487041, -105.3511109029578 40.08818206937269, -105.3511114371899 40.08818496832981, -105.351111919806 40.08818787712743, -105.3511123602068 40.08819078677125, -105.3511127548545 40.08819370626314, -105.3511131061122 40.08819662750032, -105.3511134057638 40.08819955407481, -105.3511136655411 40.08820248329983, -105.3511138760653 40.08820541426265, -105.3511140443603 40.08820835237604, -105.351114163412 40.08821128772411, -105.351114241413 40.08821422752239, -105.3511142701628 40.08821716815781, -105.3511142520106 40.08822010783207, -105.3511141893056 40.08822304474702, -105.3511140808613 40.08822598520552, -105.3511139243503 40.08822892109879, -105.3511137267983 40.08823185693918, -105.3511134800089 40.08823478731219, -105.351113191008 40.08823771673009, -105.3511128527656 40.08824064248196, -105.3511124723156 40.08824356547749, -105.3511120426341 40.08824648030368, -105.3511115695742 40.08824939147138, -105.3511110496261 40.08825229537347, -105.3511104874762 40.08825519381728, -105.3511098760888 40.08825808679372, -105.3511092248507 40.08826097161301, -105.3511085279028 40.08826384646623, -105.3511077805547 40.08826671134739, -105.3511069968658 40.08826957167852, -105.3511061604374 40.08827241933256, -105.3511052865074 40.08827525703119, -105.3511043656989 40.08827808296099, -105.3511034015258 40.0882808989278, -105.3511023951647 40.08828370313181, -105.3511013407563 40.08828649376421, -105.3511002453384 40.08828926993341, -105.3510991053852 40.08829203523749, -105.3510979279441 40.08829478428164, -105.3510967024539 40.08829752065474, -105.3510954347834 40.08830024166259, -105.3510941284525 40.08830294640897, -105.3510927799473 40.08830563308802, -105.3510913869165 40.08830830439874, -105.3510899505349 40.088310959442, -105.3510884766733 40.0883135946227, -105.3510869629747 40.08831621534176, -105.3510854047624 40.08831881528859, -105.3510838090661 40.0883213971742, -105.3510821712054 40.0883239564893, -105.3510804970312 40.08832649864536, -105.3510787818711 40.08832901553052, -105.3510770257072 40.08833151525054, -105.3510752332379 40.08833399420897, -105.3510734009512 40.08833644969923, -105.3510715288491 40.08833888082079, -105.3510696239633 40.08834128938393, -105.3510676816053 40.088343674482, -105.351065699426 40.0883460379133, -105.3510636821256 40.08834837518056, -105.3510616261805 40.08835068898124, -105.3510595374595 40.08835297662093, -105.3510574124448 40.08835523809517, -105.351055252313 40.08835747160411, -105.3510530570523 40.08835968255164, -105.3510508290275 40.08836186193435, -105.3510485693955 40.08836401695893, -105.3510462734738 40.08836614401667, -105.3510439459587 40.08836824041177, -105.3510415833244 40.08837030974222, -105.3509560258479 40.08843761152456, -105.3507798770322 40.08857084662024, -105.3507538096081 40.08863307525191, -105.3507519531502 40.08863799036086, -105.3507511319305 40.08864084523704, -105.3507504935722 40.08864373007083, -105.3507500357499 40.08864663585278, -105.3507497561281 40.08864955807664, -105.3507496605839 40.08865249044558, -105.3507497479682 40.08865542215029, -105.3507500159438 40.08865834958532, -105.3507504680483 40.0886612637487, -105.3507511019483 40.08866415923357, -105.350751910624 40.08866702882577, -105.3507528976031 40.08866986802661, -105.3507540605621 40.08867266692603, -105.3507553959971 40.08867541921492, -105.350756900396 40.08867812218688, -105.3507585679157 40.08868076682799, -105.350760398576 40.0886833441317, -105.3507623876923 40.08868585139007, -105.3507645258996 40.08868828138591, -105.3507648979519 40.08868866373927, -105.3507668167196 40.08869063232233, -105.3507692461027 40.08869289427427, -105.3507718140629 40.08869506093713, -105.3507745112231 40.08869713049755, -105.3507773305537 40.08869910024445, -105.3507802720763 40.08870096027083, -105.350783320557 40.08870270605373, -105.3507864724758 40.08870433848928, -105.3507897254995 40.0887058521706, -105.3507930608822 40.08870723986828, -105.3507965301085 40.0887090870666, -105.3508980689437 40.08877062856219, -105.3509009761502 40.08877209766227, -105.3509038776238 40.08877350731244, -105.3509068038209 40.08877487196231, -105.3509097547317 40.08877619611515, -105.350912730362 40.08877747706896, -105.3509157295431 40.08877871302094, -105.3509187499201 40.08877990847136, -105.3509217926772 40.08878105801779, -105.3509248566341 40.08878216526129, -105.35092793711 40.08878322569265, -105.350931043486 40.08878423932394, -105.3509341651927 40.08878521334669, -105.3509373034264 40.08878613695467, -105.3509404581733 40.0887870164524, -105.3509436294314 40.08878785274052, -105.3509468183891 40.08878863861543, -105.3509500215108 40.08878938217835, -105.3509532376397 40.0887900762226, -105.3509564620774 40.08879072434474, -105.3509596995144 40.08879132655078, -105.3509629511253 40.0887918819416, -105.3509662087037 40.08879238960599, -105.3509694781146 40.08879284865083, -105.3509727546598 40.0887932626727, -105.3509760383511 40.08879362626768, -105.3509793291805 40.08879394303838, -105.3509826283206 40.08879421298629, -105.3509859299085 40.08879443610383, -105.3509892327773 40.08879460968762, -105.3509925416098 40.08879473734624, -105.3509958505506 40.08879481546952, -105.3509991642883 40.08879484496426, -105.351002473436 40.08879482852016, -105.3510057838647 40.0887947625423, -105.3510090932251 40.08879464882887, -105.3510124038607 40.08879448828358, -105.3510157063963 40.08879427819243, -105.3510190055145 40.08879402216397, -105.3510223012154 40.0887937201983, -105.3510255911674 40.08879336598777, -105.3510288730156 40.08879296403265, -105.3510321479246 40.08879251793702, -105.3510354123884 40.08879202229245, -105.3510386675698 40.08879148160367, -105.3510419158218 40.08879089227121, -105.3510451512775 40.08879025608872, -105.3510483774528 40.08878957396133, -105.3510515873119 40.08878884588005, -105.3510547843766 40.08878807004817, -105.3510579662997 40.08878724736322, -105.3510611354167 40.08878638233142, -105.3510642882273 40.08878546684256, -105.3510674200216 40.08878450989691, -105.3510705378526 40.08878350339787, -105.351073635838 40.08878245634416, -105.351076711646 40.08878136242842, -105.3510797711359 40.08878022345936, -105.3510828072641 40.08877904303054, -105.3510858235602 40.08877781574264, -105.3510888164907 40.08877654879628, -105.3510917860694 40.08877523588691, -105.3510947287704 40.08877388061261, -105.3512448646096 40.08871567828783, -105.3512486912542 40.08871387742979, -105.351251635128 40.08871251945109, -105.3512545906727 40.08871118670531, -105.3512575602452 40.0887098737917, -105.3512605403221 40.08870858340758, -105.3512635344228 40.08870731465686, -105.3512665378591 40.08870606663291, -105.3512695517975 40.08870484203913, -105.3512725785854 40.08870363997784, -105.3512756147108 40.08870245774266, -105.3512786625149 40.08870129713789, -105.3512817208154 40.08870016266518, -105.3512847896299 40.08869904621879, -105.3512878689408 40.08869795590442, -105.3512909599343 40.08869688541922, -105.3512940579142 40.088695837459, -105.3512971652179 40.08869481562927, -105.3513002865475 40.08869381453241, -105.3513034125184 40.08869283595745, -105.3513065466482 40.08869187990894, -105.3513096901057 40.08869094818974, -105.3513128440714 40.08869003719879, -105.3513160014997 40.08868915143022, -105.3513191753012 40.08868828549675, -105.3513223490436 40.08868744658238, -105.3513255344688 40.08868662749714, -105.3513287268686 40.08868583634074, -105.3513319239214 40.08868506230241, -105.3513351302921 40.08868431709655, -105.3513383424805 40.0886835926129, -105.3513415639967 40.08868289245849, -105.3513447889775 40.08868221662582, -105.3513480174328 40.08868156061168, -105.3513512563826 40.08868093163021, -105.3513544999716 40.08868032607136, -105.3513577481959 40.08867974573641, -105.3513610010635 40.08867918702274, -105.3513642573977 40.08867865173011, -105.3513675218851 40.08867814166592, -105.3513707898391 40.08867765502278, -105.351374061254 40.08867719450269, -105.3513773396651 40.0886767520043, -105.3513806180192 40.08867633562443, -105.3513839045245 40.08867594537359, -105.3513871886334 40.08867557853625, -105.3513904773837 40.08867523422086, -105.3513937731164 40.08867491423175, -105.3513970699648 40.08867462036259, -105.3514003655933 40.08867434810722, -105.3514036693692 40.08867410378213, -105.3514069719272 40.08867388017016, -105.3514102744283 40.08867368267664, -105.3514135815726 40.08867350680448, -105.3514168910031 40.08867335795441, -105.3514201968706 40.08867322981446, -105.3514235061931 40.08867313049941, -105.3514268213333 40.08867305190653, -105.3514301305556 40.08867299852394, -105.351433442068 40.0886729703622, -105.3514367535353 40.08867296291506, -105.3514400661123 40.08867298428987, -105.3514433751263 40.08867302637476, -105.3514466852559 40.08867309457963, -105.3514499941619 40.08867318619949, -105.3514533041913 40.08867330033678, -105.3514566094714 40.08867344148718, -105.3514599147025 40.08867360515348, -105.3514632187059 40.0886737940361, -105.3514665238309 40.08867400633676, -105.3514698206927 40.08867424384466, -105.3514731186721 40.08867450657194, -105.3514764154318 40.088674790913, -105.3514797051029 40.08867509956215, -105.3514829958916 40.08867543343067, -105.3514862807701 40.08867578890692, -105.3514895644133 40.088676173202, -105.351492839807 40.08867657639993, -105.351496113975 40.0886770039135, -105.3514993869117 40.08867745844471, -105.351502651593 40.08867793458061, -105.3515059103563 40.08867843592677, -105.351509167896 40.08867896068803, -105.3515124206924 40.0886795097604, -105.351515666404 40.08868008133964, -105.3515189050231 40.08868067902834, -105.3515221377321 40.08868129832474, -105.3515253680449 40.08868194103469, -105.3515285912691 40.08868260805275, -105.3515318050615 40.08868329847537, -105.3515350152831 40.08868401321057, -105.351538218422 40.08868474955204, -105.3515414121252 40.08868551109929, -105.351544601087 40.08868629605706, -105.3515477841348 40.08868710442384, -105.351550956584 40.08868793349171, -105.3515541207701 40.08868878776683, -105.3515572778715 40.0886896645488, -105.3517668144786 40.08874223138561, -105.3517712897696 40.08874356918196, -105.3517744433507 40.08874444955605, -105.3517776193232 40.08874527862216, -105.3517808059531 40.08874605996785, -105.3517840102742 40.08874679450269, -105.3517872311274 40.08874747592078, -105.3517904591143 40.08874811231585, -105.3517937024629 40.08874869469192, -105.3517969588061 40.08874923295311, -105.3518002199575 40.08874971718186, -105.3518034929369 40.08875015459225, -105.3518067765795 40.08875054158026, -105.3518100650282 40.08875087543642, -105.3518133582732 40.08875116066397, -105.3518166574911 40.0887513954631, -105.3518199626836 40.08875157893316, -105.3518232679801 40.08875171466919, -105.3518265780846 40.08875179637275, -105.3518298906361 40.08875183124597, -105.3518331997874 40.08875181207614, -105.351836513733 40.08875174517834, -105.3518398242724 40.08875162693941, -105.351843130231 40.08875145825852, -105.3518464339581 40.08875123733741, -105.3518497284121 40.08875096686898, -105.351853025319 40.08875064686825, -105.3518563106055 40.0887502782178, -105.3518595901426 40.08874985732261, -105.3518628604085 40.08874938597948, -105.3518661213993 40.0887488659896, -105.3518693707716 40.08874829644942, -105.3518726108767 40.08874767465998, -105.3518758393555 40.08874700692275, -105.3518790550472 40.08874628783244, -105.3518822532574 40.08874551918425, -105.3518854386629 40.08874470728863, -105.351889048104 40.08874410218412, -105.3518929562721 40.08874362985717, -105.3518968528061 40.08874311518499, -105.3519007388787 40.08874255816904, -105.3519046109777 40.0887419561029, -105.3519084726114 40.08874131349427, -105.3519123167499 40.08874062763223, -105.3519161433971 40.08873989671551, -105.3519199560572 40.08873912705313, -105.3519237430216 40.08873831052417, -105.3519268312332 40.0887368977742, -105.3521297321906 40.08870965310233, -105.3521353584751 40.08870744742942, -105.3521389316516 40.0887062604555, -105.35214258898 40.0887052005799, -105.352146323415 40.08870427229673, -105.3521501244089 40.08870347289052, -105.3521539755295 40.0887028095455, -105.352157868561 40.08870228585356, -105.3521617941243 40.08870190090214, -105.3521657357991 40.08870165647144, -105.3521696806946 40.08870154894242, -105.3521736287951 40.08870158552017, -105.3521775519679 40.0887017616655, -105.3521814513797 40.08870208008177, -105.3521853059354 40.08870253533819, -105.3521891109386 40.08870313013065, -105.3521928558477 40.08870385904178, -105.352196519546 40.08870472654777, -105.3522001044021 40.08870572184397, -105.3522035893053 40.08870684670466, -105.3522069672316 40.08870809571696, -105.3522102276295 40.08870946796671, -105.3522133623026 40.0887109580397, -105.3522163618855 40.08871255871862, -105.352219215825 40.08871426999018, -105.3522219182773 40.08871608284031, -105.3522244551869 40.08871799004599, -105.3522268277186 40.08871999521124, -105.3522290230108 40.08872208120746, -105.3522310328513 40.08872424982536, -105.3522328549184 40.08872649025432, -105.3522344833588 40.08872879798358, -105.352235912325 40.08873116580063, -105.3522371173096 40.08873353963548, -105.3522371383208 40.08873358379383, -105.3522381554927 40.08873604745254, -105.3522389661979 40.08873855137593, -105.3522395610806 40.08874108384367, -105.352239944849 40.08874363675592, -105.352240111642 40.08874620920469, -105.3522400626633 40.08874878678113, -105.3522397955776 40.08875136497907, -105.3522393150947 40.08875393479811, -105.3522386212323 40.08875648813249, -105.3522377175237 40.08875901778155, -105.3522366039846 40.08876151654021, -105.3522352829679 40.08876398080893, -105.3522337603739 40.088766393483, -105.3522320455755 40.08876875817698, -105.3522301350824 40.08877106227742, -105.3522280394693 40.08877329589072, -105.3522257645975 40.08877545992507, -105.3522233151827 40.08877754267818, -105.3522207041373 40.08877953786197, -105.3520968124044 40.08889266474071, -105.3520116371138 40.08897043866074, -105.3520098123099 40.08897269603393, -105.3505603079781 40.0901770108341, -105.3504353074468 40.09028001126072, -105.3501143193342 40.09054518814754, -105.3501030044008 40.09054683514306, -105.3488602740463 40.09072766624689, -105.3477420438011 40.0911531132065, -105.3477390155334 40.0912676727278, -105.3474905654169 40.09126545526282, -105.3473647716007 40.09190101374886, -105.3473760618604 40.09190161138967, -105.3477358623749 40.09192063968359, -105.3480775784211 40.09193222086797, -105.3480752065149 40.09194413324476, -105.3480493301681 40.09207408349272, -105.3480266875468 40.09218004037569, -105.3480266804584 40.09218321693172, -105.3480375101837 40.09218369231485, -105.3481173225404 40.09218719725872, -105.3481261729915 40.09218758627011, -105.3489303591214 40.092222907135, -105.3489536535213 40.09211378066907, -105.3489559026821 40.09210480060535, -105.3514657513061 40.0921898080533, -105.3517804351884 40.0920302926229, -105.351787338956 40.09204363909638, -105.3517906752359 40.09205008747434, -105.3517977978255 40.09205880042371, -105.3517996510527 40.09206238375607, -105.3518824545005 40.0921636816697, -105.351910777043 40.0921732918272, -105.3519259366955 40.09217843592464, -105.3515570003769 40.09260513227046, -105.3497571221252 40.09339322755047, -105.3493959159767 40.09370220408351, -105.3486197191432 40.0943661447682, -105.3485938374456 40.09439569602217, -105.348069812973 40.09441758316737, -105.3477279376078 40.09443076942602, -105.3454396442972 40.09442644731377, -105.3454145566375 40.09442639841708, -105.345406450746 40.09442645331113, -105.3428267490629 40.0944438410692, -105.3409616965941 40.09446173446745, -105.3385806165806 40.09448453710624, -105.338038240879 40.09448972631531, -105.3380597264658 40.09816320496651, -105.3380679597995 40.0999829026921, -105.3380680672347 40.10000677074521, -105.3380762485868 40.10181497668572, -105.333785237299 40.10179680139225, -105.3337278521754 40.10179655756251, -105.3333790260725 40.10179507305974, -105.3286884549565 40.10177504586694, -105.3286846007798 40.10277183683161, -105.3286845468612 40.10278580930287, -105.3286746087921 40.10535684263111, -105.3284493757341 40.1053164531441, -105.3279727853101 40.10523011210574, -105.3276491086925 40.105171102215, -105.3276308985215 40.10516778229127, -105.3241715938379 40.10453703921772, -105.3234060627616 40.10495320304896, -105.3230735027185 40.10513227377913, -105.3227056071184 40.10533036849009, -105.3219837186156 40.10571906357421, -105.319637666022 40.10559853352776, -105.3196340094476 40.10608717073401, -105.319633491415 40.10615609689889, -105.3196328620638 40.10624003657848, -105.3196324203565 40.10629918820222, -105.3196321462285 40.10633581324939, -105.3196164950359 40.10877483107916, -105.3196168898822 40.10882458490146, -105.31961907359 40.10910010517093, -105.3196088120404 40.11007871015286, -105.3195981387719 40.11109660301321, -105.3195867291031 40.1121868781655, -105.3195919018123 40.11259425855098, -105.3196073099071 40.11368319199543, -105.3196427185068 40.11618538426401, -105.3196367383125 40.11705363330758, -105.3196284268623 40.1182610946904, -105.3196215022174 40.11926648962921, -105.3196127185051 40.12054217426306, -105.3196075600112 40.12129130371403, -105.3196046445937 40.12171457176227, -105.3196039198489 40.12181983195664, -105.3195907343885 40.12373976980507, -105.3195996402118 40.1271990756839, -105.3196040280096 40.12890583323124, -105.3196047145051 40.12917274842658, -105.3196092372073 40.13093185442296, -105.3196129903288 40.13171254519044, -105.3196132716022 40.13177111142701, -105.3196444735669 40.13826003807267, -105.3196579593377 40.14029878475719, -105.3196943576456 40.14580098361585, -105.3197968729787 40.15181213863595, -105.3198011602762 40.15206351632045, -105.3198251871729 40.15347217831872, -105.3198628279538 40.15498735145348, -105.3198628290226 40.15498739108313, -105.3199164563804 40.15714591594258, -105.319937660156 40.15871453421283, -105.3199658798908 40.16081322516637, -105.319965912186 40.1608156596316, -105.3199470384802 40.16081628319009, -105.3102029758523 40.16093165450556, -105.3038011272576 40.16070799014367, -105.3005885640191 40.16059547665297, -105.2974028537698 40.16033230682975, -105.2914146194853 40.15983716419294, -105.2823830523645 40.1598017510487, -105.2801049068414 40.15978890188411, -105.2797491442513 40.15978689060664, -105.279438147905 40.15965574319318, -105.2789691635483 40.1595966967908, -105.2786951569143 40.15951033105921, -105.2783387574589 40.15923550989657, -105.2778164113579 40.15894098523002, -105.2776541607318 40.15889359876963, -105.2773907774724 40.1588709397186, -105.2764745864344 40.15871964151842, -105.2759892007606 40.15864821436704, -105.2754891981546 40.15864307329331, -105.2749458418215 40.15860031614835, -105.2738102982743 40.15848967626626, -105.2735568724613 40.15844106713092, -105.2738358838627 40.15824286475723, -105.2741450220795 40.15802193630074, -105.2742468856654 40.15794499676178, -105.2744588801126 40.15777987830076, -105.2746357770759 40.15761080747117, -105.2747344479813 40.15752711641187, -105.2748632858387 40.15741202752761, -105.2750305123632 40.15725926668, -105.2754225917291 40.15688255289814, -105.2758929495494 40.15644495979728, -105.2763959191594 40.15594704292194, -105.2766783327523 40.15567077309503, -105.2781341188324 40.15428111162556, -105.2785179368782 40.15391275991212, -105.2793160425854 40.15314803978234, -105.2794728569717 40.15300092477589, -105.280206041469 40.15228913282684, -105.280836947521 40.15167212428224, -105.2809808922424 40.1515200419104, -105.2811198405698 40.15136410597679, -105.2812509272502 40.15120513605844, -105.2813741570252 40.1510420334142, -105.2814298541274 40.15096500015037, -105.2815369705137 40.15080598366004, -105.2815880233071 40.15072702048, -105.281682976191 40.15056798085986, -105.2817290364374 40.15048406638984, -105.2817718698596 40.1504020677656, -105.2818528863331 40.15023806078776, -105.2819260558769 40.15006690229658, -105.2820759337992 40.1496241186037, -105.2821258875183 40.14944111154255, -105.2821458605589 40.14934808820088, -105.2822096587099 40.14892990318661, -105.2822448240156 40.14826998094643, -105.2822451208162 40.14784201323412, -105.2822360982994 40.14719606295897, -105.28224793464 40.14573292184287, -105.2822446240266 40.14535916374291, -105.2822411001326 40.1</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>7</v>
-      </c>
-      <c r="E7" t="n">
-        <v>7</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Centennial MS</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2205 Norwood Ave, Boulder, CO 80304</t>
+        </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Centennial MS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2205 Norwood Ave, Boulder, CO 80304</t>
+          <t>http://cem.bvsd.org/</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
+          <t>Centennial Middle School</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>40.04506796264024</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-105.2671472290834</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
           <t>http://cem.bvsd.org/</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Centennial Middle School</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>40.04506796264024</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-105.2671472290834</v>
-      </c>
       <c r="N7" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>http://cem.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
         <is>
           <t>POINT (-105.2671472290834 40.04506796264024)</t>
         </is>
@@ -952,59 +906,53 @@
           <t>POLYGON ((-105.1470238512916 39.92761587682738, -105.1470244855684 39.92746831055086, -105.1470393599495 39.92524137222502, -105.147038645905 39.92502944310596, -105.147046321183 39.92186965993315, -105.1470470425149 39.92145044388781, -105.1470531994023 39.91775944655548, -105.1471032891195 39.91405210433869, -105.1473391472332 39.91405215140002, -105.147676653323 39.91405221810871, -105.1511818705786 39.9140528369392, -105.1532334610398 39.91405315098152, -105.1550121913589 39.91405339401757, -105.1560293437166 39.91405351953847, -105.156420131756 39.91405356845262, -105.1597894853714 39.91405668205347, -105.1653843869967 39.91413671650596, -105.1656197775234 39.91414007793439, -105.1657674166974 39.91414214035058, -105.1660335028282 39.91414237825769, -105.1660414667389 39.91414238424149, -105.1660433311038 39.91414238604561, -105.1660586296656 39.91414239888842, -105.1667719578876 39.91414299090538, -105.1672381230998 39.91414337611825, -105.1698987794962 39.91414553623513, -105.1703876457997 39.91414592693626, -105.1750099583544 39.91414955744559, -105.1797462276226 39.91415918540865, -105.183940205586 39.91416757726816, -105.184478826679 39.91416864003449, -105.1907538888507 39.91416762414558, -105.1921136011874 39.91416735873496, -105.1926978672329 39.91416724236024, -105.1933546555779 39.91416710270681, -105.1938763305775 39.91416699469512, -105.1953160550247 39.91416702303262, -105.1971047644128 39.91416703407202, -105.1985745597549 39.91416702150446, -105.1991893697619 39.91416701068361, -105.2006351177575 39.91416696934041, -105.2032744790532 39.91416684927634, -105.2062749820281 39.91414793981343, -105.2062611795562 39.91424142750945, -105.206223179592 39.91428442723124, -105.2055840142236 39.91454527467528, -105.2051264319463 39.91473201341331, -105.2047771484222 39.9148745542603, -105.2046181793619 39.91493942746109, -105.2044351788381 39.9150464284585, -105.2039238798093 39.91526835479848, -105.2036994329652 39.91536577400033, -105.2034951787843 39.91545442818257, -105.2032861789647 39.91558342752357, -105.2029610455153 39.91570919533338, -105.2026927027816 39.91582616438962, -105.2019980528428 39.91613227988852, -105.2013773094024 39.91640582131284, -105.2005472795797 39.91677157902036, -105.199981771958 39.9170207684681, -105.1988809443973 39.91750583145522, -105.1980761776685 39.9178604287125, -105.1977971773725 39.91800542846681, -105.1975931774295 39.91818342841723, -105.1971382584971 39.91865717884937, -105.1969171547176 39.91888743134161, -105.1963542841982 39.91947358440687, -105.1960461779453 39.91979442941913, -105.1960031773458 39.91985842861604, -105.1958741782275 39.91996042930643, -105.1957021779222 39.92016442965017, -105.1956491770346 39.92026642822356, -105.1956271775804 39.92046542890528, -105.1956074363542 39.92104863795893, -105.1955832718303 39.92176253388807, -105.1955539541311 39.92260363188283, -105.1955126848871 39.9235025188834, -105.1954828953945 39.92415135493398, -105.1954701680578 39.92442856826072, -105.1954277266185 39.92535293082255, -105.1953454862046 39.92714404290943, -105.1952731788288 39.9286614295662, -105.1921605878346 39.92866908889513, -105.1912021775201 39.92867143016532, -105.1900135071195 39.92868142556227, -105.1891882146993 39.92868835848437, -105.188280750955 39.92869597460466, -105.1874398749427 39.92870302575108, -105.1862427122102 39.92871305375947, -105.1860781767717 39.92871443107489, -105.1857881765031 39.92869343037078, -105.185584175611 39.92863943112477, -105.1853591757001 39.92871443082796, -105.1851551757211 39.92870443083596, -105.1848971762652 39.92868243096175, -105.1846711757492 39.92865043161049, -105.1843711756133 39.92868243090511, -105.1841991763519 39.92873643054561, -105.1838441764116 39.92869343178848, -105.1818511117197 39.92869648384348, -105.1784019212843 39.92870168376908, -105.1754136393685 39.92870368858787, -105.1754132357649 39.92870368835112, -105.1720714920114 39.92870144219746, -105.1691971726547 39.92869943197082, -105.1689792892025 39.92870089102008, -105.1684020970337 39.92870328012041, -105.1674080147692 39.92870738861864, -105.1666546602336 39.92871548911919, -105.1662549995615 39.92871799924519, -105.1662549969533 39.928718054178, -105.1662548834643 39.92871805655115, -105.1658309152665 39.92871792608083, -105.1660201718075 39.92872443199441, -105.1660261074718 39.92941559118069, -105.166031494597 39.93004289540448, -105.1660381193122 39.93081421993796, -105.1660467016499 39.93181341576487, -105.166056515896 39.93295616617159, -105.1660647969186 39.93392020542746, -105.1660503453821 39.93509378069637, -105.1660326082687 39.93546115149928, -105.166003329776 39.93598570561753, -105.1660033259753 39.93598576505014, -105.1659873030505 39.93626023394562, -105.1659872391716 39.93626133344856, -105.1659871764604 39.93626243299418, -105.1659749417947 39.93647953441914, -105.1659674910183 39.93676935921954, -105.1659572086535 39.93679429393993, -105.1659335404815 39.93685168841169, -105.1658977131763 39.93693353750162, -105.1658600197634 39.93701487859802, -105.1658204732303 39.93709568651817, -105.1657790841984 39.93717594147653, -105.1657358633377 39.93725561378023, -105.1657309930949 39.93726410639616, -105.1657314686866 39.93778700123453, -105.1657621735393 39.94010243415755, -105.1664371723441 39.93963643311929, -105.1669986961005 39.93946070845881, -105.1676961733447 39.939242433397, -105.1693161728545 39.9392404329576, -105.1693041740566 39.94127343310699, -105.1683021747413 39.94321143381614, -105.1664695916308 39.9432063625764, -105.165775173689 39.94320443381061, -105.1657468007817 39.94732775484253, -105.1657421736448 39.94800015855595, -105.1657381741117 39.9485814352014, -105.1663871736281 39.94844043457117, -105.1685594742733 39.94796687370324, -105.1696508514793 39.94772963358609, -105.1696509264492 39.94772961758919, -105.1699691748952 39.94766043485847, -105.1703601751532 39.94872843443577, -105.1702541750417 39.94875143479771, -105.1705001743236 39.94877043461553, -105.1706751750825 39.94883443513947, -105.1708731754645 39.94899843388744, -105.1709821753827 39.94931543455208, -105.1710701754516 39.9496574351276, -105.1713521750109 39.95026343503369, -105.171721175489 39.95026543539605, -105.171721175293 39.95049343486586, -105.1732691751886 39.95049443510379, -105.1737901766914 39.9502784352506, -105.1765441762881 39.95029543509211, -105.1765421764602 39.95049343511674, -105.1777091771583 39.95048843468322, -105.1776542787933 39.95210731667019, -105.1776527450811 39.9521525489294, -105.1776503630244 39.95222278293825, -105.1776494915453 39.95224847092626, -105.1776425915952 39.95225318368962, -105.1776474058934 39.95230996305708, -105.1774426914856 39.95247925641739, -105.1774296504487 39.95249004043743, -105.1774078670555 39.95259250878293, -105.177290609483 39.95332415578926, -105.1772734159885 39.95342058182205, -105.1772613072263 39.95349823162613, -105.1772507335152 39.95357595507921, -105.1772416938306 39.95365372245707, -105.1772370166073 39.95373008711738, -105.1772414131593 39.9538026430856, -105.1772475047739 39.95387510202673, -105.1772552845585 39.95394743780206, -105.1772648208975 39.95401954432493, -105.1772767414146 39.95409060825552, -105.177290313959 39.95416152369918, -105.1773055304672 39.95423226451359, -105.177322394536 39.95430281359553, -105.1773408910587 39.95437314928622, -105.1773575396614 39.95443111644111, -105.1773610213213 39.95444324817128, -105.1773827784174 39.95451308681337, -105.1774061518873 39.95458265077165, -105.1774311360077 39.95465191391003, -105.1774577273785 39.95472085370143, -105.1774859155525 39.95478945300295, -105.1775156877714 39.95485768836055, -105.1775470406094 39.95492554265083, -105.1775799624868 39.95499299062175, -105.1776144429687 39.95506001242811, -105.177648397834 39.95512435329022, -105.1789848485213 39.95766031512748, -105.1789897484092 39.957669611876, -105.178782063112 39.95766574209604, -105.1786071533748 39.95766248214333, -105.1753791767883 39.95758643523679, -105.1753811772785 39.95817043580769, -105.1770375813809 39.95819321332797, -105.1770375221035 39.95820029775011, -105.1770363078439 39.95835052526509, -105.1770358705875 39.9584045834283, -105.1770275234974 39.95943772098945, -105.1767015637337 39.95943301604639, -105.1756586713841 39.95941795615627, -105.1752731802447 39.95941238698667, -105.1751673978478 39.95941085853762, -105.1751515536733 39.96066900909348, -105.1751530130947 39.96066902761821, -105.1752660781159 39.9606704126778, -105.1753197877496 39.96067107019252, -105.1760332411225 39.96066191903108, -105.1780562582363 39.96063407794388, -105.1780563504867 39.96064057285627, -105.1780617120378 39.96101742820876, -105.1780795667658 39.96212243842648, -105.1779603294206 39.96230169761951, -105.1777988506388 39.9622247658564, -105.1777786369145 39.96221513532904, -105.1777779996259 39.96221599908061, -105.1777729991336 39.96222499799526, -105.175195000182 39.96134899884276, -105.1750629987647 39.96129699910314, -105.1718929991997 39.96004699882172, -105.16867899997 39.95862899864169, -105.1677549991503 39.95786999907147, -105.1672029990481 39.95741599921722, -105.1668249995467 39.95710599849211, -105.1661219997786 39.95695499897838, -105.1660599995567 39.9569419984156, -105.1660659997773 39.95698699837227, -105.1661089994848 39.95726499912967, -105.1661250002072 39.95739999859541, -105.1663429988309 39.95789999829524, -105.1663939993887 39.95801599875833, -105.1663729998672 39.95804199855646, -105.1663260779203 39.95809453148716, -105.166280999977 39.95814499912188, -105.1658829843055 39.95798883313223, -105.1657049993032 39.95791899851163, -105.1655459994386 39.95785699862255, -105.1640439992191 39.95727199887524, -105.1635449998441 39.95706699912397, -105.163260000118 39.95693999941128, -105.1629539988249 39.95680199904174, -105.1626729999983 39.95667199866357, -105.1623139998591 39.95649799874107, -105.162090999951 39.95638499933245, -105.1615179991773 39.95607999946219, -105.1612710001578 39.9559439989421, -105.1611820283237 39.95589271854974, -105.1609239990875 39.95574399904351, -105.1605739993225 39.95553199876508, -105.1605070003541 39.955487998663, -105.160507601197 39.95548743481859, -105.160553485336 39.95544433019448, -105.1605729992732 39.95542599889634, -105.1605708372656 39.95542490543037, -105.1604879993213 39.95538299862599, -105.1603829998639 39.95530799832515, -105.1594730000078 39.95466099895394, -105.1568089995898 39.95264699943566, -105.1564621234448 39.95235626096443, -105.155603998905 39.95163699829544, -105.154634999516 39.95082499893148, -105.1545469991415 39.95082499900798, -105.1543240000297 39.95082499846626, -105.1538259995572 39.95043899936822, -105.1526479997484 39.94953399844792, -105.1520270002295 39.94907999894239, -105.1510029999227 39.9483689989986, -105.1505859991704 39.94808599920534, -105.1502339997436 39.94785999905235, -105.1493769991665 39.94730899849206, -105.1487869967502 39.94692837327946, -105.1483709999483 39.94665999878806, -105.1479109994562 39.94636399921564, -105.1470224473384 39.94578389403245, -105.1469689981003 39.94574899894534, -105.1465979998178 39.94550799907834, -105.1444109992605 39.94408999827592, -105.1438049994702 39.94369699936311, -105.1436849993157 39.94361699895295, -105.1435829995349 39.94355199879121, -105.1429179998172 39.94312999953807, -105.1415170000054 39.9422179981579, -105.141208999877 39.9420169995477, -105.1409599991531 39.94185799904378, -105.1405889992587 39.94161999863454, -105.1400129996827 39.94124299866457, -105.1380069982713 39.93995099908016, -105.1376659994644 39.93973899908963, -105.1376101742235 39.93970626003536, -105.1376101662146 39.93970556469871, -105.1376101533659 39.93970445864476, -105.1376092642489 39.9396308257882, -105.1376082126364 39.93954372301226, -105.1376032162488 39.9391298924964, -105.1376002640181 39.93888552805745, -105.1376000835919 39.93887058729946, -105.1375934532797 39.93832156847123, -105.1375901359232 39.9380468199151, -105.137587250081 39.93780781910959, -105.13758090158 39.93728200849577, -105.1375804232843 39.93724229677402, -105.1375796290724 39.93717680439059, -105.1375669599118 39.93612418884327, -105.1375702679211 39.93577373335888, -105.137586602701 39.93404371593252, -105.1375954953071 39.9331018756593, -105.1375976976845 39.93286861358298, -105.1376017361011 39.93244089603266, -105.1376081834016 39.93175509745066, -105.137605376672 39.93128768051638, -105.1376034417805 39.93096545410189, -105.1376029272597 39.93086976333272, -105.1376238948989 39.93013023535828, -105.1376321063676 39.92984063493733, -105.1376407559584 39.92953592366019, -105.1376599462519 39.92897351444855, -105.1376612209119 39.92893150972372, -105.1376618506932 39.92891071719205, -105.138619806365 39.92890769866385, -105.1386248219273 39.92890763964525, -105.1391145604889 39.92890607867842, -105.1423066729647 39.92889593602464, -105.1435950820782 39.92889181774414, -105.1435958776075 39.92889181480177, -105.1436712912503 39.92889157348318, -105.1470184689167 39.92887114754381, -105.1470187184292 39.92881293486509, -105.1470188937999 39.92877200297731, -105.1470238512916 39.92761587682738), (-105.169197172132 39.92863411235809, -105.1691864470017 39.92863672319584, -105.1691971726547 39.92869943197082, -105.169197172132 39.92863411235809))</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>8</v>
-      </c>
-      <c r="E8" t="n">
-        <v>8</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Eldorado K8</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>3351 S Indiana St, Superior, CO 80027</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Eldorado K8</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>3351 S Indiana St, Superior, CO 80027</t>
+          <t>http://el8.bvsd.org/</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
+          <t>Eldorado K-8 School</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>39.921698179021</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-105.161197194222</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
           <t>http://el8.bvsd.org/</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Eldorado K-8 School</t>
-        </is>
-      </c>
-      <c r="L8" t="n">
-        <v>39.921698179021</v>
-      </c>
-      <c r="M8" t="n">
-        <v>-105.161197194222</v>
-      </c>
       <c r="N8" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>http://el8.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
         <is>
           <t>POINT (-105.161197194222 39.921698179021)</t>
         </is>
@@ -1024,59 +972,53 @@
           <t>POLYGON ((-105.0553096519419 40.02197149228508, -105.0553161721816 40.02152862889884, -105.0553212996101 40.02118039422834, -105.0554144707321 40.01485168306485, -105.0554156695371 40.01476968888103, -105.055416567316 40.01468733327196, -105.0554222037575 40.01418812084223, -105.0554725655142 40.00972422301597, -105.0554720783693 40.0096054501175, -105.0554763115184 40.00921806165778, -105.0554777210193 40.00908880877136, -105.0554783834164 40.00902816353494, -105.055478575345 40.00901219736176, -105.0554871758176 40.00854380587615, -105.0554879813757 40.00814947087598, -105.055488010625 40.00814642135131, -105.0554881852632 40.00812897442378, -105.0554887295674 40.00808087222916, -105.0554920362152 40.00777826834898, -105.0554948489156 40.00752250682681, -105.055531007058 40.00563956685976, -105.0555401553612 40.00564045054492, -105.0555902120115 40.00566690495083, -105.0556471557209 40.00567245091049, -105.0557201558533 40.00567145055776, -105.0558361548308 40.00567645117783, -105.0559061543596 40.00567545085779, -105.0559701557746 40.00568045011807, -105.0561221547891 40.00567145049642, -105.0561661556522 40.00563345075564, -105.0561531550697 40.0055424501676, -105.056107155146 40.00544945007372, -105.0571341561924 40.00545445010541, -105.0604611556923 40.00038144912251, -105.0640551537651 40.00037580618888, -105.0678619251848 40.00037085969463, -105.0744775635209 40.00036260693889, -105.074477999321 40.00046599897158, -105.0744799997885 40.0007489983894, -105.0744820000614 40.00248399837474, -105.074475000093 40.00379499887224, -105.0744809997915 40.00389299933561, -105.0744759999931 40.00412799915949, -105.0744768152457 40.00418672611349, -105.0744770006211 40.00419999892615, -105.074476815134 40.00421095567354, -105.0744759988608 40.00425899837897, -105.0744770000379 40.00485699808893, -105.0744799998352 40.00548099818882, -105.0744800693377 40.00549913954058, -105.0744829989317 40.00626690809695, -105.0744829995353 40.0062669990658, -105.0744834354184 40.00666768629058, -105.0744840001084 40.00718699899353, -105.0744840001105 40.00754717649394, -105.0744840004529 40.00754899853014, -105.0744840014802 40.00754920928831, -105.0744959994806 40.00913899920532, -105.0744850002892 40.01025499937742, -105.0744939996588 40.01117199953493, -105.0744939994117 40.01312199935634, -105.0744879997328 40.01486699832747, -105.0750330000281 40.01486599880874, -105.0776729999707 40.01487699919728, -105.0778080003735 40.01487099884424, -105.0780740000252 40.01483699883885, -105.0785220001667 40.0147389989032, -105.0787519998548 40.01470499815898, -105.0790640003765 40.0146869983785, -105.0798880004663 40.01470099918091, -105.0827519996697 40.0147379995101, -105.083827279062 40.01474776707985, -105.0838636006166 40.01474809629242, -105.0838678605798 40.01474813508104, -105.0839630017275 40.01474899892437, -105.084275999784 40.01475199921421, -105.084343261355 40.01475098794224, -105.0844090000323 40.01474999906352, -105.0863749999974 40.01472599885857, -105.0865649991523 40.01472399889266, -105.0905288819658 40.01468199225995, -105.0905289991035 40.0146819917752, -105.0905557415763 40.01468189398261, -105.0924409249201 40.01467444931598, -105.0932924249816 40.01467107691634, -105.0933119998438 40.01467099914053, -105.0940020010792 40.01467199918716, -105.0968210984977 40.01464899904126, -105.0968081659261 40.01339944902477, -105.0977161660674 40.01340144824596, -105.097693165477 40.01108044794793, -105.1029281665798 40.01109144817353, -105.1029321674492 40.01426744896852, -105.1029350211734 40.01499712229778, -105.1029381666813 40.01697244858164, -105.1029531677396 40.0182424491116, -105.1029258020212 40.01922928731726, -105.1028801685531 40.02039944897465, -105.1028411684982 40.02101744933578, -105.1027191685341 40.0229774492492, -105.1026901679704 40.02391744893649, -105.102681714784 40.02523098211869, -105.1026813585937 40.02624327690542, -105.1026851686352 40.02731645051675, -105.1026703866881 40.0282598185744, -105.1026821685567 40.02903745095252, -105.1027065698951 40.02953569354239, -105.1025462936187 40.0295350594423, -105.1025509999655 40.02982099987915, -105.1026589993872 40.0325789998223, -105.1028159251721 40.03659410284713, -105.1028159996535 40.03659599988478, -105.1028159808093 40.03659641862485, -105.1026950932294 40.03923308897296, -105.1026695167741 40.03979091557985, -105.102684106142 40.03979099374556, -105.1026843791355 40.04070640471347, -105.1026843795041 40.04070875362413, -105.1026844241735 40.04085566869285, -105.1026853227765 40.04386122510869, -105.1026792879808 40.04699933304118, -105.1026468422424 40.04711176082813, -105.1026515547724 40.04751510558266, -105.1026531716483 40.0476534526228, -105.1026544039104 40.04765355413717, -105.1030171704752 40.04768345267631, -105.1033391709822 40.04790545288033, -105.1037471714223 40.0480454529342, -105.1041869090785 40.04810254797782, -105.1051951720775 40.0482334531068, -105.1056231709406 40.0481744531596, -105.1064479966728 40.0482222769794, -105.1072881721325 40.04830245271919, -105.1075741724027 40.04816445209948, -105.1084266880845 40.04775137397073, -105.109125173029 40.04741245282467, -105.1096111728036 40.0474164516294, -105.1100331727537 40.04752645257917, -105.1103231729248 40.04751845193728, -105.1107256413342 40.047267544397, -105.1111171727025 40.04702345167325, -105.1111851729639 40.04692845194887, -105.1112241729621 40.04694545172396, -105.111576173255 40.04658445258669, -105.1116441732981 40.04653845179544, -105.1117501733669 40.04650145208792, -105.1118461736203 40.04649345213979, -105.1123371190536 40.04651893042601, -105.1123366900865 40.04658012665188, -105.1123366731379 40.04658248811084, -105.1123354147434 40.04676250668771, -105.1123309979452 40.04739433331647, -105.112330888596 40.04741005387065, -105.1123302681899 40.04749872120584, -105.1123296974318 40.0475803086633, -105.1123229001954 40.04855248897933, -105.1123218382726 40.04870461756659, -105.112392173119 40.04869545288748, -105.1127817580233 40.04864540026167, -105.1141782671779 40.04846883077132, -105.1151371742824 40.04834545259219, -105.1159511368379 40.04820936852636, -105.1180384926233 40.04779473006271, -105.1220411513055 40.04703446196407, -105.1244748378258 40.0465721293676, -105.1281644085359 40.04587100599928, -105.1311570490046 40.04532707446116, -105.1311558744463 40.04547805719804, -105.1311661736642 40.04661103317486, -105.1311759744774 40.04744011431053, -105.1311790599092 40.04779398012801, -105.1311841143478 40.04824612972813, -105.1311891001171 40.04930496819956, -105.1311931055019 40.05054498601775, -105.131205846102 40.05096312075745, -105.1312107819624 40.05257722664825, -105.131211005441 40.05265005956795, -105.1312209170923 40.05372291390245, -105.131216169747 40.05413797270889, -105.1312141679244 40.05437597462971, -105.1312034302793 40.05463055486094, -105.1312059997651 40.05463199871355, -105.1312151333568 40.05463829014283, -105.1312051341252 40.0549272902714, -105.1312061330529 40.05519229072108, -105.131207134803 40.05564929051275, -105.1312051349296 40.05727829088557, -105.1312131325501 40.05874928993782, -105.1312141338369 40.05887029037866, -105.131228134939 40.05974929071716, -105.1312201340746 40.06002129004976, -105.1312141343774 40.06023929086055, -105.1312251347958 40.06072029049393, -105.1312291345053 40.06187129073018, -105.131234134076 40.06223529081105, -105.131220135557 40.06361729016729, -105.1312161352539 40.06423529025914, -105.1312261348082 40.06486429056906, -105.1312181355008 40.06555429029728, -105.1312311345578 40.06758328902276, -105.1312421349654 40.06840629078298, -105.1312471352586 40.06877329065517, -105.1312571353166 40.07052429035368, -105.1312561355187 40.07114629121654, -105.131250135106 40.07142728958371, -105.1312471358889 40.07157529118987, -105.1312769801043 40.07280485163446, -105.1312771363536 40.07281128908546, -105.1313291354456 40.07367829108345, -105.1313121353605 40.07453929131646, -105.1313161362929 40.07558629064913, -105.131364137045 40.08008229048873, -105.1314061367591 40.0827892910741, -105.1314141381591 40.08325728973681, -105.1314231385745 40.08373028926654, -105.1314680581192 40.08735891798165, -105.1314681373808 40.08736529032833, -105.1314686920482 40.08736528489368, -105.1315023083889 40.0879120286511, -105.1315123076631 40.08860202899108, -105.1315573093293 40.09073602900505, -105.131565308569 40.09121302826923, -105.1315713090677 40.09267102844738, -105.1315353089882 40.09441602918015, -105.1315413093822 40.09489902827075, -105.1315033084531 40.09835802848521, -105.13149630911 40.09849502893818, -105.1314753089459 40.09960702888224, -105.1314743099729 40.09982802847355, -105.1314613102898 40.1017110280084, -105.1314603103063 40.10285102851227, -105.1313783109039 40.10663902806576, -105.1313063115642 40.10894602876141, -105.1312713110947 40.10989302815075, -105.1312733098291 40.11046202797889, -105.1312403110973 40.11140002800153, -105.1312113114617 40.11250802867715, -105.1311973097867 40.11310902852121, -105.1311303117171 40.114313029054, -105.1310553120431 40.11535402919674, -105.1310183122412 40.11621802952327, -105.1310173486831 40.11641334503174, -105.1310173105552 40.11642102922118, -105.1310173108496 40.11649802904655, -105.1310243109556 40.11903302886184, -105.131030312504 40.11993502837323, -105.1310413121898 40.12134002807184, -105.1310483121341 40.12350602835088, -105.1310553132711 40.12555802887955, -105.1310573131 40.12712102857881, -105.1310483145869 40.12882902900039, -105.131019817435 40.13074388165322, -105.1308018207651 40.13073588184478, -105.129739962766 40.13072788110647, -105.1295199780874 40.13072688132058, -105.125637981124 40.13071087844324, -105.1214389852497 40.1306978758488, -105.1214388421045 40.13069787537972, -105.1214287020073 40.13069788718315, -105.1196690057948 40.13069987439082, -105.1190837455796 40.13069590702754, -105.1190789667365 40.13069587415787, -105.1190737172402 40.13069586675535, -105.1167582823744 40.13069277850736, -105.1167491843696 40.13166446387874, -105.1155191846595 40.13164146329787, -105.1152464520673 40.13162554514241, -105.1150500767831 40.13162358771766, -105.1146592764502 40.13161717097666, -105.1142691989206 40.13161076343259, -105.1138787565874 40.13160434794801, -105.1134884683498 40.13159766957149, -105.1130752163228 40.13171876581113, -105.1126460873139 40.13184417366759, -105.1122248807698 40.13196726034626, -105.1122250359624 40.13198450641528, -105.1121931826917 40.1319974642461, -105.1119871837674 40.13205846401782, -105.1119826842302 40.13221195301501, -105.1119769681384 40.13240697386129, -105.1119701840193 40.13263846362696, -105.1115905511339 40.13264209640875, -105.111021497991 40.13263928746463, -105.1109074261621 40.13263860431368, -105.110591834876 40.13263671418122, -105.1103350195741 40.13263517546018, -105.1098582235746 40.1326323161728, -105.1096519310758 40.13263086368207, -105.1093701834689 40.13263246468068, -105.1093585944797 40.13263279385802, -105.1093205768746 40.13268270513078, -105.1092647735506 40.13273806278027, -105.1092018368701 40.13278836166751, -105.1091328252846 40.13283461228306, -105.1090587413161 40.13287489693305, -105.1089796055062 40.13291013523579, -105.1088964020049 40.13293936322003, -105.1087220040101 40.13297863883014, -105.1086315304633 40.13298881317525, -105.1085152097078 40.13299386796137, -105.1055770144187 40.13300287849541, -105.1055759857053 40.13312511863367, -105.1055759631424 40.13312799972009, -105.1044939964566 40.13312987928641, -105.1041803847008 40.13315484466681, -105.1025130798614 40.13316287747433, -105.1025130341002 40.13316287731691, -105.1024960005596 40.13413300172339, -105.100395113552 40.13418487869186, -105.0960260840791 40.13426087793793, -105.094924071347 40.13427687757695, -105.0944350199997 40.134278878763, -105.0944050049201 40.13427896522876, -105.0940880142722 40.13427987836944, -105.0932020045514 40.13427787787717, -105.0930212415033 40.13428686643668, -105.0927490541487 40.13428987731798, -105.0920430472559 40.13429687652557, -105.0905391301851 40.13433687298826, -105.0899250393446 40.13434187663415, -105.0887041365292 40.13437587163286, -105.0879403055598 40.13442385884984, -105.0846750309919 40.13445787330612, -105.0832755753651 40.13446682896835, -105.0831630652203 40.13445687173049, -105.0799831751011 40.13457186759719, -105.077656234461 40.13468386293215, -105.0762711360049 40.13472286783558, -105.0745131984398 40.13479486487819, -105.0742413915201 40.13481684621029, -105.0742440761428 40.13984499868648, -105.0737770801883 40.13984989482434, -105.0728341139191 40.13987189343821, -105.0652349113323 40.13998458559128, -105.0651172543858 40.13995483397098, -105.0650172912994 40.139897965545, -105.064944699213 40.13982145163131, -105.0649318121612 40.13979936609553, -105.0649223983107 40.13978009284535, -105.0649012584268 40.13969700518675, -105.0649496601588 40.13851303311695, -105.0649247890964 40.13837338792121, -105.0648822428967 40.13829711858007, -105.0647902892207 40.13821288423826, -105.0647026837377 40.13816640688852, -105.0646163718572 40.1381387740668, -105.0644970736709 40.13812287925889, -105.0630970281733 40.13814387787887, -105.0623920537045 40.13814787912667, -105.0570841697421 40.13820687462603, -105.055393108424 40.1382658753683, -105.0553734627153 40.13826344007112, -105.055373432471 40.13824238373312, -105.0553733597693 40.13819028553863, -105.0553632754563 40.13104290372788, -105.055364943468 40.13045509249489, -105.0553838251001 40.1238012151376, -105.0554011703724 40.12074599216336, -105.0554021173245 40.12057908303889, -105.0554247936661 40.11658455689023, -105.0554252479113 40.11650224198018, -105.0554253132042 40.11642002734557, -105.0554270937738 40.11409009148291, -105.0554307971221 40.10923987562791, -105.0554303061645 40.10813983466713, -105.0554291707098 40.1055942872819, -105.0554283485588 40.10374754276933, -105.0554275913097 40.10204463836374, -105.0554275553799 40.10196193683294, -105.0554275083234 40.10188004134116, -105.0554258013926 40.0987667225997, -105.0554241217421 40.09570511636053, -105.0554235981428 40.09475507605646, -105.0554115838102 40.0876056618749, -105.0554116626656 40.08751615800497, -105.0554120967009 40.08737439782387, -105.0554338942331 40.0802760293785, -105.0554359155676 40.07955726421665, -105.0554393436516 40.07833891985845, -105.0554454483656 40.07616858804563, -105.0554543197811 40.07301208584704, -105.0554524783247 40.07097781636424, -105.0554510471109 40.06937851290341, -105.0554511248211 40.06936354972414, -105.0554693891445 40.06582907619643, -105.0554580642362 40.05842399669204, -105.0554542737668 40.05209778695296, -105.0554563122968 40.05151114401765, -105.0554564529153 40.05147054475928, -105.0554575802229 40.05114448977547, -105.0554617276261 40.04898736880429, -105.0554635752588 40.04802681178261, -105.0554639797832 40.04781621901886, -105.0554654855536 40.04674097808282, -105.0554656988988 40.04658897680252, -105.0554665087686 40.04601063733477, -105.0554691137273 40.04415188527337, -105.0554694939043 40.04386956126768, -105.0554628576467 40.04251422452845, -105.0554558612454 40.04108497102352, -105.0554471109753 40.03929767112174, -105.0554415609123 40.03816398170832, -105.0554342598844 40.03667252329386, -105.0554338426251 40.03658900636015, -105.0554331606792 40.03650690784292, -105.0554302318307 40.03615562906905, -105.0554208607084 40.03503174441796, -105.0554056000837 40.03320149646342, -105.0553923068964 40.03160700942662, -105.0553916639802 40.0315298997633, -105.0553898967095 40.03131800400271, -105.0553734970732 40.02935099038166, -105.0553731474197 40.02930921737802, -105.0553704800526 40.02900128894915, -105.0553096519419 40.02197149228508))</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>10</v>
-      </c>
-      <c r="E9" t="n">
-        <v>10</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Erie MS</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>650 Main St, Erie, CO 80516</t>
+        </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Erie MS</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>650 Main St, Erie, CO 80516</t>
+          <t>https://ems.svvsd.org/</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
+          <t>Erie Middle School</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>40.05101707648438</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-105.0529688258069</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
           <t>https://ems.svvsd.org/</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Erie Middle School</t>
-        </is>
-      </c>
-      <c r="L9" t="n">
-        <v>40.05101707648438</v>
-      </c>
-      <c r="M9" t="n">
-        <v>-105.0529688258069</v>
-      </c>
       <c r="N9" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>https://ems.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
         <is>
           <t>POINT (-105.0529688258069 40.05101707648438)</t>
         </is>
@@ -1096,59 +1038,53 @@
           <t xml:space="preserve">POLYGON ((-105.348856789205 40.03820800949617, -105.3487067298522 40.03821232955207, -105.3477914050935 40.03821638893005, -105.3474817926258 40.03821722291953, -105.3468614299469 40.03822512838605, -105.3450104181683 40.03829153532944, -105.3450179171597 40.03868015700185, -105.3460405482716 40.0386437539853, -105.3461031168401 40.03898908284479, -105.3453268746833 40.03901948006025, -105.3452802180325 40.03911018389644, -105.345271517239 40.03912433761808, -105.3452452833364 40.03915814157467, -105.3452130574343 40.03918918870853, -105.3451781010895 40.03921517142847, -105.3451448277192 40.03923480953083, -105.3451089087152 40.03925177274996, -105.3450576487383 40.03926988529709, -105.3450069768098 40.03928187960952, -105.344961760615 40.03928819273935, -105.3449089508063 40.03929064807553, -105.3448494533033 40.03928712489946, -105.3447950264157 40.03927776511058, -105.3447425347318 40.03926247803446, -105.3446092328436 40.03929490292018, -105.3445765512982 40.03930516501039, -105.344539877266 40.03932120387111, -105.3444846960346 40.03935795158987, -105.3444426165169 40.03940586426801, -105.344423128196 40.03944725428348, -105.3444160073502 40.03949552391189, -105.3444275517575 40.03955601888752, -105.3444731759986 40.03968833424123, -105.3444965572211 40.03975520013649, -105.3445205624492 40.03981616221999, -105.3445578084813 40.03989778498795, -105.3446376646379 40.04003968424905, -105.3447276531524 40.04016680845205, -105.344795157412 40.04024733253993, -105.3448549167217 40.04031071675156, -105.3448484541613 40.04055274004725, -105.3448541691076 40.0406499600528, -105.3448674149786 40.04072253855343, -105.3448882399842 40.04079357632659, -105.3449216829459 40.04087332410908, -105.3449704426995 40.04095811087339, -105.3446364322639 40.04102959990085, -105.3446007162516 40.04104340376086, -105.3445703711054 40.04106466860651, -105.3445493695219 40.04108914063158, -105.3445380231417 40.04111119661664, -105.3445343361066 40.04112275146215, -105.3445311011553 40.04114724832418, -105.3445392814093 40.04121096396332, -105.3419896303343 40.04121709476975, -105.3422755387781 40.04337513429397, -105.3465131388534 40.04343423722576, -105.3501117189857 40.04341854173573, -105.3509604583964 40.04341720319611, -105.351061685705 40.04341728708226, -105.3544519058515 40.04524596662837, -105.355091416096 40.04556889885021, -105.3559880623356 40.04583041298836, -105.3567595372542 40.04599519383382, -105.3579301381531 40.04606086270712, -105.3600970053326 40.04564174739976, -105.3606742433043 40.0468628855719, -105.3621557651074 40.04965424089358, -105.3639920692559 40.05282887853546, -105.3641080684391 40.05289587827868, -105.3797250233372 40.06069585746808, -105.3900870057658 40.06584284178945, -105.3912861257657 40.07092499987773, -105.3914749402041 40.07083101793872, -105.3920811145549 40.07050298994405, -105.3925910222121 40.07026600808574, -105.3937980289077 40.06981087854467, -105.3940840170989 40.06972192263695, -105.3946001680771 40.06959803960483, -105.3947989293112 40.06953590537677, -105.3948919023455 40.06948987079981, -105.394964868722 40.06944107368035, -105.395060070696 40.06933903984681, -105.3952621280964 40.06899113614033, -105.3955138612367 40.0686358647477, -105.3957139250865 40.06842109885081, -105.3959568633348 40.06820609746421, -105.3961321294408 40.06808409464642, -105.3965509251752 40.06782505281563, -105.3967590498075 40.06770994229892, -105.3970411697905 40.06757211203932, -105.3973890575354 40.06741704540752, -105.3979349933502 40.06719105257222, -105.3989681210101 40.0668320704148, -105.3993949116376 40.0667119298152, -105.4001279456997 40.06656295502956, -105.400853036919 40.06646804795456, -105.401574842874 40.0664209000962, -105.4031081030495 40.06634588138125, -105.4033760986539 40.06632908658128, -105.4036001268962 40.06632597936235, -105.4039354886404 40.06629270998662, -105.4039684530764 40.06628998415017, -105.4041299199174 40.06627663574243, -105.4042548603106 40.06623819278212, -105.4043540234276 40.06619888982722, -105.4044344048956 40.06614050729836, -105.4045148499365 40.06603666564356, -105.4047389400583 40.06573287074457, -105.4047829657393 40.06567608181868, -105.4049212700939 40.06553693910522, -105.4051253441126 40.06542981958253, -105.4053520055905 40.06532884620861, -105.4056105037759 40.06528097971057, -105.4058260373516 40.06528440260607, -105.4060288655031 40.0653072983951, -105.4061852130406 40.0653236615075, -105.4063458769007 40.0652750842445, -105.4065446697525 40.06515834714913, -105.406676242775 40.06503075664818, -105.4068038590952 40.06490576206056, -105.4069109925564 40.06477432561354, -105.4072568691801 40.06434998263192, -105.4075520798087 40.0638858471748, -105.4076144271041 40.06375352486941, -105.4076986539011 40.06358322723908, -105.4077424376704 40.06351872295893, -105.4078528920384 40.06344490160728, -105.407979736912 40.06339954278057, -105.4081488124669 40.06337694790046, -105.4081993022081 40.06354259319305, -105.4082583191018 40.06365304293325, -105.4083384376527 40.06378623987003, -105.4086252315054 40.0642215866695, -105.4087813728473 40.06439056211295, -105.4089458907069 40.06461799217212, -105.4091018907903 40.06489412393282, -105.4092368182365 40.06512802479963, -105.4093225643208 40.06526853688391, -105.409504095397 40.06548498442051, -105.4098262734777 40.06579167091841, -105.4100664892069 40.06598563197285, -105.4102657157319 40.06612999100079, -105.4104355939177 40.0662923524043, -105.4104999331161 40.06642759351949, -105.4105231868886 40.06658533416806, -105.4111090704269 40.0668027547869, -105.4113230710384 40.06683775452498, -105.4123600762381 40.06670774877939, -105.4126030773382 40.06671874798173, -105.4127710765582 40.06675374711786, -105.4135470770253 40.06717174623984, -105.4143210780151 40.06733974415099, -105.4147190788605 40.06742674212688, -105.4148260788204 40.06747274227973, -105.4149630792546 40.06748474171021, -105.4150690789331 40.06755474126348, -105.4153730784282 40.06789174239631, -105.4157380779817 40.06803174076535, -105.4159660790526 40.06803073976152, -105.417218086706 40.06765573284537, -105.4192990814895 40.06934373178217, -105.4204860820148 40.06988972973171, -105.4213540837626 40.07010972666475, -105.4217650863564 40.07012072544669, -105.4219790865552 40.07007372430561, -105.4224070903935 40.06972272033761, -105.4231560979392 40.06916171416628, -105.4234760999032 40.06905671176163, -105.4241311017381 40.06905570945187, -105.4263101075327 40.06940170123508, -105.4276811134631 40.06938769518695, -105.4296940698257 40.06907550496865, -105.4296848584402 40.06784624750029, -105.429671773314 40.0661001537952, -105.4296579769224 40.06425909176156, -105.4296368548572 40.06155809847662, -105.4296177827629 40.05856372052644, -105.4298099905968 40.05861586964885, -105.430018256796 40.0586642013499, -105.4304940701495 40.0588180812849, -105.4308276096539 40.05895208149089, -105.4313349350903 40.05921427306927, -105.4316590735046 40.0594648528358, -105.4318892343097 40.0596640133864, -105.4322990968159 40.05986651955405, -105.4329873576576 40.06004930992891, -105.4335605933063 40.06004038995119, -105.434434235593 40.0599712445611, -105.4354783925689 40.05975633761448, -105.435996631219 40.05945534342511, -105.4366632696116 40.0590005622899, -105.4374423829502 40.0583688561975, -105.4380710690886 40.05782633790203, -105.4387283869856 40.0573751360412, -105.439546349493 40.0571235327649, -105.4398747066513 40.05698872465391, -105.4406386271914 40.05675863519146, -105.4417548336166 40.05638679447648, -105.442567773736 40.05613305341807, -105.4442686974679 40.05566339315051, -105.445343246227 40.05543155148678, -105.4460872580018 40.05530049376619, -105.4475361795096 40.05506323819086, -105.4484647042474 40.05492359728375, -105.4497124891264 40.05482749056537, -105.4509974746667 40.054709341968, -105.4519105410676 40.05459009159843, -105.4529452414847 40.05436689697932, -105.4539354331393 40.05422779377801, -105.4543838348087 40.05421363093428, -105.4550889579488 40.05414451371335, -105.4556747016011 40.05404522521154, -105.4556195417862 40.05389977953413, -105.4555785994819 40.05312561237029, -105.4555800785149 40.05277505477387, -105.4556423342693 40.05229494829926, -105.455604087428 40.05216777687549, -105.455363854523 40.05189813544341, -105.4549647203148 40.05156158659062, -105.4547531376207 40.05138317782109, -105.4544031511611 40.05106908044412, -105.4542784159924 40.05074735203495, -105.4542974585342 40.05030084833979, -105.4543602124875 40.0498831708682, -105.4544043076297 40.04934065378175, -105.4543482479448 40.04909096993268, -105.4542109292466 40.04890847082154, -105.4540922782555 40.04883640624273, -105.453598796094 40.04875458782777, -105.4530865461581 40.04871117041102, -105.4526367273778 40.04873019111304, -105.4522869920531 40.04882560463331, -105.4518609877183 40.04893312059847, -105.4515392148404 40.04900042535454, -105.4512371760301 40.04894566223346, -105.4510311076975 40.04881594232108, -105.4506189061122 40.04864772506455, -105.450381521998 40.04862841875691, -105.4500442086895 40.04865036424795, -105.449748527079 40.04863651001132, -105.4494197230372 40.04853976397921, -105.4491713770628 40.0484220791417, -105.4488324815664 40.04824364741962, -105.4484976187861 40.04824101085237, -105.4483742062581 40.04828836479434, -105.4481527085251 40.04847342744434, -105.4480825457048 40.04858899738371, -105.4479574354427 40.04880499423177, -105.4477557093762 40.04894803549239, -105.4475449876894 40.04896804860563, -105.447285091094 40.0489087685434, -105.4470577998178 40.04883339300962, -105.4467455619172 40.04867000817741, -105.4466253298221 40.04859381923382, -105.4463159689591 40.04821745074411, -105.4462490902482 40.04814167709562, -105.4460691639663 40.04793781841308, -105.4459530422406 40.04787097758558, -105.4456060940407 40.04782908762505, -105.4452030334892 40.04782752432455, -105.4447533455736 40.04783846618427, -105.4441126313704 40.0478088560095, -105.4436975850779 40.04781395002598, -105.4430717601619 40.04784941480156, -105.4428542106095 40.04781353540704, -105.4426133763108 40.04766957101944, -105.4424314041075 40.04752003349248, -105.4423133012629 40.04740912390634, -105.4421861847308 40.04730907867685, -105.4419926239673 40.04718895154178, -105.4418061612007 40.04717136530205, -105.4417081954194 40.047182415411, -105.4416026797826 40.04721179966809, -105.4415072036721 40.04724939290262, -105.4414255327156 40.04729616164285, -105.4411577224697 40.04751082582863, -105.4409777288979 40.04763690177953, -105.4407871880504 40.04777450210482, -105.4404879006635 40.04801117476408, -105.4403389720799 40.04814775195113, -105.4401721086119 40.04840903387786, -105.4401067707136 40.04857846009677, -105.4399833163249 40.04911181062739, -105.4398729838371 40.04928598490994, -105.4397192008006 40.04939319049351, -105.4394855114924 40.04943941990325, -105.4392044056712 40.04941046497871, -105.4388636524953 40.04931851093392, -105.438546327513 40.04918193415831, -105.4380767786613 40.04891900617424, -105.437743143361 40.04872791764675, -105.4373933085161 40.04859639978524, -105.4370453058392 40.04845061923234, -105.436850100213 40.04838174734803, -105.4366416043731 40.04822077949636, -105.4364623815374 40.04804718592201, -105.4362633499358 40.04785329407545, -105.4359270011547 40.04771609612432, -105.4356638386845 40.04761770272381, -105.4353588193232 40.04759065426665, -105.4351715745744 40.04763071171844, -105.4349968999914 40.0476738768727, -105.4347454162208 40.04770360844505, -105.4345268098148 40.04765547297004, -105.434388492245 40.04755708258775, -105.4343273663388 40.04749335953326, -105.4342501879127 40.04733242057809, -105.434314678797 40.04709269363552, -105.4345204999711 40.04693740685487, -105.4347929737008 40.04689355559919, -105.434987328464 40.04692391707396, -105.4353581394735 40.04718062489702, -105.4356328975705 40.04730560893702, -105.4361277795634 40.04738267032662, -105.4367424163266 40.04755614551331, -105.4373232663294 40.04777462146167, -105.4378965827389 40.04799394153435, -105.4384082122526 40.04818466005356, -105.4385869413177 40.04827225757087, -105.4387181248332 40.04828192910482, -105.4387681853788 40.04819073376519, -105.4387698323472 40.04798677707445, -105.4388164240695 40.04785346836961, -105.4388570582708 40.04770509858814, -105.4388749958935 40.04751382260495, -105.4389056636208 40.04744816914924, -105.438936292543 40.04738259762316, -105.4390135085617 40.0472337121499, -105.4391753715978 40.04694264036142, -105.4393494826775 40.04675592722637, -105.4394709162605 40.04664744693813, -105.4397443071152 40.0464388139819, -105.4398818573897 40.04630925394687, -105.4400319946386 40.04607407341846, -105.4401119276108 40.04575211954744, -105.4401573906037 40.04555561044507, -105.4401888235684 40.04532997165521, -105.4403184492711 40.04515190537982, -105.4404637006837 40.04504664805176, -105.4410062310046 40.04487488619607, -105.441351219543 40.04480243757087, -105.4416959411179 40.04480147386886, -105.4420395016487 40.04485806074565, -105.4423881029662 40.04493259178905, -105.4426691968809 40.04495673762963, -105.4429191074365 40.04491845168188, -105.4432654711716 40.04476847759636, -105.4434739426463 40.04461030486147, -105.443662898663 40.04442909629897, -105.4437817103438 40.04428511840506, -105.4439256132001 40.04410673258661, -105.4441404970957 40.04401270487976, -105.444329416994 40.04400206228913, -105.444606475449 40.0440694640092, -105.4447865945989 40.04423422180232, -105.4449203593976 40.04436476415748, -105.4451131401293 40.04456520837888, -105.4451744249196 40.0447130948, -105.445220507406 40.04488588584199, -105.4452409774836 40.04505930867118, -105.445308555714 40.04528334672855, -105.4454035915627 40.04552010855499, -105.4454710483879 40.04576237462368, -105.4455283401477 40.04598646261165, -105.4456105755037 40.04613445233301, -105.4458916514732 40.04618739837201, -105.446129018222 40.04621631660641, -105.4463039778235 40.04616358427998, -105.446407424162 40.04602195805321, -105.446667215597 40.0458187188582, -105.4468895653487 40.0456291768839, -105.4471443524481 40.04551644473226, -105.4475418471934 40.04542649938936, -105.4478799981491 40.04537433230562, -105.4482973977438 40.04536749866653, -105.4488277934268 40.04536792065857, -105.4493054526135 40.04542072925156, -105.4496841719427 40.04544973101621, -105.4499403346239 40.04540183080188, -105.4501028615711 40.04525786537818, -105.450179275188 40.04507186814531, -105.4502155530288 40.0449218307571, -105.4502282296804 40.04467217531494, -105.4502221263177 40.04447532385408, -105.4501223199638 40.04427843101776, -105.44994131148 40.04407190199892, -105.449822712307 40.0439470200139, -105.4496354242496 40.04378849942575, -105.4494168828578 40.04365397065786, -105.4492077275886 40.04355080971189, -105.4490446942465 40.04343302515638, -105.4488765011509 40.04324751308347, -105.4486865345227 40.04294787288507, -105.4485806074133 40.04259253785128, -105.448517087676 40.04241607109771, -105.4484560132822 40.04214117014943, -105.4484216352835 40.04183236545518, -105.4484403420923 40.04165558502374, -105.4484503267856 40.04140178460691, -105.4484771618931 40.0411400570128, -105.4484394873438 40.04089571999755, -105.4483385338129 40.04054712281781, -105.4484261968361 40.04026869292268, -105.4485450117775 40.04009590378584, -105.4488563328945 40.03998217976847, -105.4492260106934 40.03992336241087, -105.4493999185044 40.03990184221139, -105.4498007028263 40.03990440851381, -105.4501284912924 40.03993647409516, -105.4505348695174 40.03993307438179, -105.4508376767798 40.03982803620941, -105.4510314426461 40.03965527552067, -105.4512557276107 40.03936568470912, -105.4515151705002 40.0391549643555, -105.4518251986846 40.03901225076601, -105.4522750253273 40.03889240763946, -105.4526248871359 40.03880132893642, -105.4529747678841 40.03868144289466, -105.453237146107 40.0386383383169, -105.4534620325642 40.03861442341547, -105.4537868411229 40.03861935533121, -105.4540054406916 40.03865305122331, -105.4542052675649 40.03873955137311, -105.4542940217177 40.03884616820108, -105.454366795153 40.03897296933693, -105.4544554621322 40.03918807970334, -105.4545109151869 40.03937823169469, -105.4545295258558 40.03957028571636, -105.454487349659 40.0397120164544, -105.4544054341493 40.03994098882126, -105.4542949264418 40.04016001026518, -105.4542279658648 40.04041583399074, -105.4542476615172 40.04072245971157, -105.4542663008047 40.04087130524294, -105.4543486699077 40.04097342704688, -105.4544643931002 40.040968531833, -105.4545805139184 40.04090324200731, -105.4547373974696 40.04076906500305, -105.4548604161138 40.0406947188977, -105.4551222424858 40.04065080284435, -105.4553784604135 40.04046363889831, -105.455659724781 40.04020448362071, -105.4559284862173 40.03995492466868, -105.4562574718578 40.03965648192272, -105.4564090054578 40.03950116242441, -105.456544441536 40.03938317116771, -105.4566409306176 40.03929220433345, -105.4567330166988 40.03921855880425, -105.4568672587436 40.03918028655645, -105.4570091920068 40.03917737460529, -105.4571970735713 40.03920399012449, -105.4574727919017 40.0392091978561, -105.4576742374468 40.03919142832632, -105.4579028156498 40.03916299208306, -105.4580965338489 40.03912512646967, -105.4583214307786 40.03908199761207, -105.4585054251747 40.03903662811377, -105.4586676194872 40.0389573510736, -105.4587712987346 40.03887570672356, -105.4589205871877 40.0387839462538, -105.4589924053408 40.03873263674406, -105.4591488750491 40.03866982801697, -105.459281754371 40.03863528565626, -105.4594378452955 40.03860761423366, -105.4596225164181 40.03856567735592, -105.4598300573352 40.03850206237642, -105.4599893871282 40.03843129178706, -105.4601258643819 40.03835200377073, -105.4602619808966 40.03827793021264, -105.4604027375314 40.03820934932943, -105.4605223438437 40.03817541162056, -105.4606932532367 40.03813578027771, -105.4608392966388 40.0381130381778, -105.4610267088864 40.0380746926612, -105.4612703428166 40.03802676213171, -105.4614515026273 40.03799801562068, -105.4616514018601 40.0379692750558, -105.4617950968508 40.03791650970663, -105.4619726054274 40.03783872995795, -105.4620915575303 40.03779868942447, -105.4623023201674 40.03771283408327, -105.4624873757552 40.037614068235, -105.462680990125 40.03753699153216, -105.4628770812229 40.03750054437869, -105.4631042408409 40.03747206674869, -105.4633246112622 40.03744797986833, -105.4635589055868 40.03743185778323, -105.4636235490246 40.03743105409266, -105.4637816937117 40.03741302606748, -105.4639503426529 40.03741307889101, -105.4640814886207 40.03746113147709, -105.4642376044186 40.03753799884461, -105.4644186940067 40.03763888044522, -105.4644748512307 40.03775412559912, -105.4644935320498 40.03786455874874, -105.464507907916 40.03797734576097, -105.4645360958713 40.03802786540076, -105.4645957267993 40.03805259025746, -105.4647120461754 40.03807107744546, -105.4647745202732 40.03805189114709, -105.4648182696122 40.03800389282083, -105.4648550685247 40.03794835304665, -105.4648811532233 40.0379220071657, -105.4649476205288 40.03784790775509, -105.4650122987282 40.03778012129685, -105.465078759705 40.03771782568425, -105.4652080980914 40.03761629342243, -105.4653431327449 40.0375499005596, -105.4654888673151 40.03750904137418, -105.4656178024517 40.03749645190426, -105.4658131584533 40.03749952982961, -105.4660088678796 40.0375105683452, -105.4661702981009 40.03750814532204, -105.4663217330367 40.03749473846992, -105.4664925413939 40.03748106235036, -105.4666674604658 40.03743310044315, -105.4668236445499 40.03737553198952, -105.467013123584 40.03729241699619, -105.4670695855542 40.03724375496851, -105.4671485419023 40.03718837779355, -105.4672235362509 40.03710677890788, -105.4673192818278 40.0370246661799, -105.4674984575032 40.03692441086024, -105.4676921375748 40.0368236405516, -105.4679095874308 40.03674822793891, -105.4680732248038 40.03673756825309, -105.4682168562857 40.03674696743575, -105.4683792638509 40.03673260892104, -105.4685229377228 40.0367086414703, -105.4686916125601 40.03665107389151, -105.4687915756962 40.03659828794598, -105.4688728038787 40.03653589416309, -105.4688978201256 40.03646868383298, -105.46890064363 40.03636922615923, -105.4688683094032 40.03608649176768, -105.4688294375998 40.03588523171646, -105.4688453914475 40.03575198531156, -105.4689044311294 40.0356668865015, -105.4689419428456 40.03559007772576, -105.4689169763039 40.03555166201114, -105.4688687105725 40.03552112246808, -105.4688380044873 40.03550464314591, -105.4687795777049 40.0355180163664, -105.4687296018647 40.0355324059768, -105.4686733742518 40.03556119791493, -105.4686108936511 40.03560439217124, -105.4684359628538 40.03569076511911, -105.4682860068023 40.03579635096558, -105.4681547858792 40.0359067413368, -105.4679898241449 40.03601471206911, -105.4678578285873 40.03608621465351, -105.4676237554177 40.03613705106031, -105.467331920507 40.03621440190616, -105.4670365504225 40.03627611937569, -105.4667993245486 40.03628512626556, -105.4664259061041 40.03627563525414, -105.4659622339207 40.03622779481458, -105.4657686241495 40.03618452719056, -105.4655562815755 40.03613165095232, -105.4653189563666 40.03607396546633, -105.4651072879263 40.03602165240844, -105.4648750882777 40.03598032150571, -105.4646506937304 40.03592972757208, -105.4644258726802 40.03585283868239, -105.4641948044623 40.0357807496646, -105.463994948226 40.03574227847106, -105.4636166427366 40.03564888337526, -105.4634112977461 40.03563673985305, -105.4631798796471 40.03562788131242, -105.4627395533892 40.03560744655459, -105.4624397267235 40.035631355169, -105.4621398918474 40.03566966614794, -105.4619150074207 40.03571280336544, -105.4616719714894 40.03578798273691, -105.4614169324756 40.03586668451568, -105.4612479840717 40.0359075307685, -105.4609737105466 40.03589837960226, -105.4607032034072 40.03581322166796, -105.4606220451006 40.03574117646026, -105.4605471650208 40.03561631940264, -105.4604515209555 40.03538155913075, -105.4605411771969 40.03516980628697, -105.460745325164 40.03496219663339, -105.4611847842231 40.03470911039988, -105.4615213042833 40.03444444280142, -105.4617724253972 40.03433691517333, -105.4620627975974 40.03428677473638, -105.4621856634314 40.03426018654425, -105.4624639281927 40.03414607807002, -105.4626064878654 40.03402615997216, -105.4626558295333 40.03391856483394, -105.4626843287107 40.03379737847219, -105.4629445889004 40.03354610975452, -105.4631298230737 40.03329166422314, -105.4632530713163 40.03312539363773, -105.4631723676173 40.03300656352572, -105.4630145229104 40.03300203861048, -105.4628089278983 40.0330699704752, -105.462622870385 40.03313041401965, -105.462382416347 40.03320324775477, -105.4622308653884 40.03324942665533, -105.4621123091782 40.03323456402543, -105.4619137414415 40.03324987178478, -105.4615197640719 40.03337876415366, -105.4611247327144 40.03347334016239, -105.4609518658094 40.03350869522491, -105.4605078941259 40.03362493922769, -105.4602885655572 40.03372039648056, -105.4601135314883 40.03379527894455, -105.4598056262865 40.03390250849921, -105.4594550870504 40.03394992648856, -105.4592302812619 40.03386822790948, -105.4590304952082 40.03372892247928, -105.4589306386476 40.03359925412024, -105.4588994919795 40.03346000837385, -105.4589271012316 40.03330786827071, -105.4589510975607 40.03319367744554, -105.4589993853942 40.03306631878111, -105.4590991911509 40.03278360050758, -105.4591199652827 40.03268258496826, -105.4591150188724 40.03259226720602, -105.4590904327338 40.0325011183871, -105.459025065846 40.03237018159784, -105.4588191192251 40.03234372289711, -105.4585877890754 40.0324852542631, -105.4584940642501 40.03254763633696, -105.4582941296471 40.03265799168989, -105.4581254393853 40.03274435218859, -105.4578592433275 40.03283393990661, -105.4575384963822 40.03292249191365, -105.4573638484304 40.03294795724295, -105.4570363191193 40.03302854362433, -105.4568385346368 40.03315678050264, -105.4567821974185 40.03335360847299, -105.456810316454 40.0335063948916, -105.4568163017309 40.03364255787771, -105.4568147670809 40.03380864114875, -105.4567836160767 40.03393792729251, -105.4566574104255 40.03415831783961, -105.4565391460978 40.03424556947021, -105.4564459062538 40.03429220223725, -105.4563455251661 40.03433663644886, -105.4560561887739 40.03443617689543, -105.4558820640041 40.03447194538261, -105.4557134367721 40.03444787492125, -105.4555069673559 40.03437282740676, -105.4553591579345 40.03431072922503, -105.4552213537833 40.03423957512793, -105.4549828448176 40.0341595210442, -105.4547518082643 40.03406340635529, -105.4545894553672 40.03400092681017, -105.4544048394762 40.03389006898158, -105.4542148135177 40.03382793642425, -105.4539275651147 40.03373179865706, -105.4537152263285 40.03369810510524, -105.4535757331263 40.03368906599719, -105.4534339224975 40.03373649996782, -105.4532404333301 40.03384675008265, -105.4530966444898 40.03403873941181, -105.4528996095487 40.03433390838572, -105.4528367976827 40.03440445563236, -105.4527409866604 40.03449518904446, -105.4525621631257 40.03462637055709, -105.4522822055471 40.03474707870705, -105.4520285899935 40.03482274046059, -105.4517953516685 40.03486876177074, -105.4514831856922 40.03491859340362, -105.4511863413582 40.03494227858606, -105.450978883285 40.03494341729687, -105.45071074166 40.03487928414413, -105.4505560733715 40.03482792970555, -105.4503783085403 40.03480474727579, -105.4501840342861 40.0347983500095, -105.4498454715085 40.03480396835326, -105.4493036907586 40.03482404562962, -105.4491090456025 40.03483741109122, -105.4488319062706 40.03484689660222, -105.4486097899218 40.03482264071118, -105.4484766115696 40.03478112902216, -105.4482506454887 40.03465337735646, -105.4481422809494 40.03446165746902, -105.4481362684162 40.03443481097717, -105.4481329205014 40.03422597370815, -105.4481470076392 40.03414109764547, -105.4481260795742 40.03400366028069, -105.4480701046018 40.03385408082433, -105.4479668218472 40.03368427038595, -105.4477793721983 40.03355888403479, -105.4475619122258 40.03350832662646, -105.4472766183654 40.03355603716927, -105.4470286594717 40.03362738453134, -105.4467532642444 40.03366443105853, -105.4464040673902 40.03357560062572, -105.4462047509766 40.03342034703974, -105.4460304452506 40.03321525848548, -105.4458930090361 40.03289636765589, -105.4457851194213 40.03274544416081, -105.4456660007642 40.03260247699643, -105.4453974909924 40.03253882935554, -105.4446410104286 40.03254153280623, -105.4443343926845 40.0324079993765, -105.4441504963008 40.03223680009287, -105.4440493814973 40.03200426787598, -105.4441734651061 40.03145424855277, -105.4443124284151 40.03109085401899, -105.4444913236292 40.03071718412532, -105.4446928182208 40.03043460997001, -105.4447325990232 40.03008338367997, -105.4446249435774 40.02990234691063, -105.4444081617735 40.02975138055803, -105.4440156551388 40.02976707094705, -105.4432925149635 40.02991757979642, -105.4428953339191 40.02995247669094, -105.4423222079109 40.03004926154301, -105.4417223648292 40.03014946061934, -105.4411541727373 40.03024205234754, -105.440751507376 40.03005922461082, -105.4405693242223 40.02980844642548, -105.4405247569878 40.02950330023305, -105.4408239584615 40.02917871927851, -105.4411421879788 40.02891412948831, -105.441529024559 40.02852970729988, -105.4421143146823 40.02801533542056, -105.4424566530376 40.02772811448784, -105.4427645731155 40.02748946811337, -105.4428733963731 40.02729685366441, -105.442856035971 40.02709878718856, -105.442753379335 40.02694066987466, -105.4424740740986 40.02667581247531, -105.4422361561291 40.02641171725879, -105.4421627354118 40.02633215234981, -105.4419899014615 40.02608653720438, -105.4418746425845 40.02586809995525, -105.4417586206913 40.02558237748611, -105.4415278888112 40.02530001926016, -105.4411748071398 40.0251914071028, -105.4409601991724 40.0251496406772, -105.4405059529632 40.02491765159761, -105.4402623567944 40.02491513807523, -105.4400030944076 40.02498272684421, -105.4397966454858 40.02508904976244, -105.4395597793163 40.02530826612527, -105.4393847531026 40.02549418783097, -105.4388881862617 40.02578392638166, -105.4383964394073 40.02608161988581, -105.4381236062599 40.02620263262403, -105.4378150629437 40.02627055208302, -105.4374616035033 40.02636780929908, -105.4371070967812 40.02648420993519, -105.436882284474 40.02647389089999, -105.4365096676688 40.02643308879092, -105.4359709061833 40.02638233037293, -105.4353397279123 40.02626338634593, -105.434560662546 40.02605373725178, -105.4342120425081 40.02594238635933, -105.4339840279204 40.02588647444495, -105.4338078295614 40.0258265830417, -105.4336360797591 40.0257101710548, -105.4334659702456 40.02555939012371, -105.4333209616463 40.02541186218291, -105.4331701377172 40.02536766024828, -105.4329232416404 40.02530635391786, -105.4327884855952 40.02530015376797, -105.4323855395824 40.02538971378622, -105.4321131539127 40.0254310601623, -105.431864312664 40.02545883262779, -105.431596830892 40.02545181137284, -105.4312362792186 40.02535266078985, -105.4309884373621 40.02531084067979, -105.4308018192828 40.0253187176223, -105.4306240087566 40.02533914468896, -105.4304440918217 40.02535833452203, -105.4302921227901 40.02531887724997, -105.4300035208585 40.02531027780987, -105.4291686127435 40.02527695480858, -105.4288489351101 40.0252641769005, -105.4286467628336 40.02526405201116, -105.4284398918819 40.02526030865064, -105.4282505399818 40.02526532921783, -105.4280928649176 40.02528905947762, -105.4279403393489 40.02533865214975, -105.4278456463248 40.02536769199481, -105.427565462158 40.02545363275944, -105.4273723149777 40.02548955524393, -105.4272992408456 40.02550315312805, -105.4271607401996 40.02553472983659, -105.4269397331792 40.02553620222038, -105.4268080952425 40.02553707795469, -105.4266553884723 40.025530481876, -105.4264506883495 40.02552826112606, -105.4262204100254 40.02551554731503, -105.4258348759512 40.02550807146258, -105.4255253832655 40.02549189094529, -105.425336537817 40.02546798904408, -105.425231865712 40.02542433437173, -105.4250448922275 40.02530065309304, -105.4248890756269 40.02500178419848, -105.4244829277462 40.02529516184836, -105.4242888337048 40.02538617480473, -105.4241702737477 40.0253943819846, -105.4241055263623 40.02546890946908, -105.4241320967277 40.02580448864965, -105.4240306161858 40.02596997449884, -105.4238353616644 40.02612328375539, -105.4235583844979 40.0262484968697, -105.4232855239439 40.02628862962832, -105.4228380888603 40.02643746950258, -105.4225416650763 40.02647455585658, -105.4219594939403 40.02663572980704, -105.4205957282032 40.02702669446086, -105.4197519470123 40.02744890804984, -105.4194212648639 40.02804059421167, -105.4184673673066 40.02854728053241, -105.416944467668 40.0296031872475, -105.4101147222736 40.03337543824303, -105.3968760313684 40.03572857755817, -105.394174734267 40.03570604764993, -105.3892469026911 40.03526736561258, -105.3858182204366 40.03487996422837, -105.3839568393852 40.03435439097252, -105.3783727923253 40.03162968231719, -105.3782848636422 40.03160427235456, -105.3780233455173 40.03110744717045, -105.3779293998402 40.030962511854, -105.377849027609 40.03075552266019, -105.3776743587331 40.03060018019208, -105.3776073031798 40.03047597181467, -105.377439515432 40.03024819084041, -105.377318552172 40.03015497304926, -105.3772364880586 40.03010182404736, -105.3758836857723 40.03131424309618, -105.3741650995925 40.03020252129752, -105.3749849405123 40.02941898313524, -105.3759045695671 40.02852069220432, -105.3759343080993 40.02849147923748, -105.3763925710351 40.02793364120749, -105.3755117821475 40.02776524000981, -105.3711961630059 40.02695645121048, -105.3546712500328 40.03672381851344, -105.3538108379241 40.03696897306946, -105.3534381461273 40.03724483790737, -105.3532612450637 40.03799366841366, -105.3532354600683 40.03808060757868, -105.3529609690354 40.03773591963947, -105.3527190080583 40.03748607386943, -105.3525869533672 40.0372800170782, -105.3523828838969 40.03685013532778, -105.3523540487777 40.0368069988163, -105.3522848114288 40.03672236455037, -105.35217505533 40.0366652138417, -105.3520679691729 40.03664396178009, -105.3519211633894 40.03665710662899, -105.3512350652558 40.03690471542134, -105.350752066814 40.0370649058794, -105.3506308648587 40.03712486907259, -105.3505725782028 40.03717210823402, -105.3505319465621 40.03720512829423, -105.3504601218263 40.03730088848148, -105.3503969068409 40.03746386974544, -105.3503780571488 40.03759094744733, -105.3503898767918 40.03773810433935, -105.3504460158685 40.03786994552974, -105.3505489509703 40.03799800425764, -105.3506721684706 40.03816013003582, -105.3507470909403 40.03831630026858, -105.3509839656849 40.03881004263459, </t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>12</v>
-      </c>
-      <c r="E10" t="n">
-        <v>12</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Gold Hill School</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>890 Main St, Boulder, CO 80302</t>
+        </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Gold Hill School</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>890 Main St, Boulder, CO 80302</t>
+          <t>http://ghe.bvsd.org/</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
+          <t>Gold Hill Elementary School</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>40.063366273762</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-105.412472825461</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
           <t>http://ghe.bvsd.org/</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Gold Hill Elementary School</t>
-        </is>
-      </c>
-      <c r="L10" t="n">
-        <v>40.063366273762</v>
-      </c>
-      <c r="M10" t="n">
-        <v>-105.412472825461</v>
-      </c>
       <c r="N10" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>http://ghe.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
         <is>
           <t>POINT (-105.412472825461 40.063366273762)</t>
         </is>
@@ -1168,59 +1104,53 @@
           <t>POLYGON ((-105.3286746087921 40.10535684263111, -105.3285829759231 40.10933249677196, -105.3284764287342 40.12320395037586, -105.338666880128 40.12287074752498, -105.3570154846513 40.1222005135923, -105.3572191082018 40.13342581422324, -105.3574479985069 40.14350680276687, -105.3620470526125 40.14373967239412, -105.3653863238086 40.14390863896946, -105.3724445532802 40.14426314701497, -105.3756249977702 40.14442229898955, -105.3802069307475 40.14393475996678, -105.3846142384698 40.1434086231454, -105.3862709652701 40.14324061297724, -105.3884044813609 40.14302421617785, -105.3910227813257 40.14275859159998, -105.3938559354602 40.14264260717856, -105.3978471903133 40.1426810170485, -105.4016158940963 40.1426539946228, -105.4066619382064 40.14222189343135, -105.4120613755037 40.14185679013661, -105.4179731644263 40.14225905162373, -105.4289403298768 40.14271447214097, -105.4395878986195 40.14311825474861, -105.4401727770837 40.14261598846758, -105.4403537810245 40.14238998659867, -105.4402237421184 40.14213030229881, -105.4398852818033 40.14202560438268, -105.4391855920727 40.14174264501145, -105.4393165432695 40.14129639233892, -105.4395625963222 40.14089103276203, -105.4398186194974 40.14076761273627, -105.4401414380125 40.14074512764935, -105.4405929261264 40.14068677884232, -105.4409967632386 40.14032264183017, -105.4408534704239 40.13999095099267, -105.4408490334069 40.1397371658542, -105.4409085075205 40.13945272425534, -105.441627017672 40.13887924774726, -105.4422207242613 40.13851520124469, -105.4423573790931 40.13831032625852, -105.4423578766834 40.13772282112337, -105.4420495241894 40.13747673476857, -105.4415508498067 40.13774518734458, -105.4412480293186 40.13796819417399, -105.4409217230848 40.13789971366144, -105.4402577275296 40.13721622648192, -105.4398547178956 40.13666039171091, -105.4398429826147 40.13651009378682, -105.4400806386873 40.13616409029089, -105.440282517764 40.13601390299153, -105.4407039510041 40.13585471919701, -105.4410720982984 40.13555887751171, -105.4412266339091 40.13525837165508, -105.4411750208083 40.13502962615528, -105.4405388181168 40.13469784026258, -105.4400879145676 40.13463840129412, -105.4398744863336 40.13443334705769, -105.4401657041598 40.13389608953084, -105.4405278974666 40.13361390997284, -105.4407654448196 40.13337720790327, -105.4407125232153 40.1328261093088, -105.4403627730081 40.13245703042931, -105.4402728914216 40.13220656203799, -105.4400644616442 40.13193095930646, -105.4400899194859 40.13145686664786, -105.4403538378005 40.13138993460992, -105.4406096397451 40.13120850977839, -105.4409832887742 40.13115620496019, -105.4415594082608 40.13093225824515, -105.441792766598 40.13083022495606, -105.4419769745805 40.13066338102513, -105.442261322216 40.13000361890706, -105.4427208929108 40.12940160451431, -105.4427095572324 40.12913991797465, -105.4427675703991 40.12897916774902, -105.4424877633457 40.12872236349825, -105.4418814652586 40.1289485387039, -105.4410267929101 40.12911244475854, -105.44062622681 40.12903535671395, -105.4403426310507 40.12882378520813, -105.4401681268348 40.12794595764182, -105.4401434427004 40.1275423135798, -105.4403271348666 40.12745911950469, -105.4404194428449 40.12688895761845, -105.4407201871724 40.12656877013251, -105.4410708990064 40.1263703374706, -105.4412380885365 40.12606289377323, -105.4414134233512 40.12598610083815, -105.4414711420068 40.12577942124896, -105.441420042683 40.12563999291525, -105.4412759346113 40.12536469040398, -105.4410619516994 40.12512509566417, -105.4410137480186 40.12490314051508, -105.441097430001 40.12464690956161, -105.4414813607216 40.12462788419529, -105.4421071991706 40.1247563359244, -105.442947647063 40.12445436328711, -105.4436769171171 40.12394344283241, -105.4439275358654 40.1236488491693, -105.4445202014138 40.12351459181477, -105.4451130029283 40.12320734603828, -105.4452216943186 40.12296393819889, -105.4455611269561 40.12272303852475, -105.445739396922 40.12263102590813, -105.446039955218 40.12249021602141, -105.4464489749707 40.12238789669911, -105.4469749932546 40.12208061124908, -105.4471671525513 40.12181161128712, -105.4477683125735 40.12145310125752, -105.4479437114356 40.12126738157929, -105.448185771842 40.12121623602334, -105.4483776567044 40.12129961021427, -105.4487616002662 40.12123571340185, -105.4491705174989 40.1212551145804, -105.4495626968083 40.12133857566865, -105.4498965579845 40.12128746567679, -105.4500717861507 40.12132598257076, -105.4503472639266 40.12122359163366, -105.4505059458994 40.1210634885219, -105.4511987403007 40.12090361208407, -105.4518080037448 40.12084620635756, -105.4523171416668 40.12075672224367, -105.4526509209928 40.12081452108134, -105.4530014589959 40.12077622322268, -105.4534186065663 40.12096219016633, -105.4539860841122 40.12098804526939, -105.4543114739603 40.12111631176514, -105.4548953690357 40.12155861384782, -105.4551289863891 40.12164840024029, -105.4553375129245 40.12182146652683, -105.4556211845854 40.12194330604206, -105.4567476952424 40.12218078657261, -105.4571148602626 40.12225139836272, -105.4574820900696 40.12221950024355, -105.4577658308258 40.12223882484343, -105.4579744528898 40.12227093481082, -105.4586420805521 40.12231602393006, -105.4591427629213 40.12241230464112, -105.459426540493 40.12237396365717, -105.4596351523571 40.12242529202669, -105.4598603799639 40.12260476219456, -105.4601857548838 40.12279067271524, -105.4604945657169 40.12275874486985, -105.4606280161351 40.12289974109881, -105.4611287323885 40.12295116506065, -105.4613456231521 40.12312422327806, -105.4615375910474 40.12309865972016, -105.4617545600843 40.12313717276883, -105.4619130583798 40.12326536242697, -105.4622383982413 40.12352815004496, -105.4624136462316 40.12355383483845, -105.4626138907714 40.12365640856648, -105.4626722522616 40.12376534421811, -105.4634983443994 40.12404110236733, -105.4637237036221 40.1240027323586, -105.4640575672274 40.12395158235574, -105.4641327441804 40.12382987558185, -105.4642913426707 40.12377866944794, -105.4644582960157 40.12370824606593, -105.464775458548 40.12366990221442, -105.4649006295363 40.12370197418591, -105.4652261281958 40.12368285213142, -105.4653263239067 40.12359318687636, -105.4654765552431 40.12358041760589, -105.465534927737 40.12367653754603, -105.4657352353888 40.12366378377023, -105.4660107054588 40.12354854214486, -105.4662193640389 40.12352297571797, -105.4664447117113 40.12350382089762, -105.4665866247402 40.12343338716104, -105.4668203139106 40.12342064025405, -105.467245981875 40.12335669309825, -105.4675131398364 40.12316456351811, -105.4677718743203 40.12313260212488, -105.4680472876695 40.12312627150369, -105.4683310322217 40.12315197728206, -105.4684896408024 40.12306873151195, -105.4689653473825 40.12307526653493, -105.4696414409102 40.12288324117313, -105.4703897895339 40.12268154313838, -105.4716698357625 40.12198039095991, -105.4719954824268 40.1215768388424, -105.4722709491116 40.12142314124566, -105.4725463847205 40.12134632501065, -105.4728551832017 40.12131436321324, -105.4730555092523 40.12123112095186, -105.4732224711366 40.12110302336163, -105.4734121622826 40.12123371277409, -105.4737473731746 40.12100852646682, -105.4740469092332 40.12082102645913, -105.4745189206885 40.12052595655688, -105.4754638457052 40.11996697409248, -105.4760371636699 40.11961489194562, -105.4767299243416 40.1192079281799, -105.4772510215974 40.11886296609708, -105.4776018882412 40.118590990685, -105.4790361330383 40.11731092193791, -105.4796448686728 40.11676090215462, -105.4798029604164 40.11659100560805, -105.4799828931568 40.11631707090588, -105.4800680420141 40.11614304270354, -105.4801081295797 40.11600304720499, -105.4801271615554 40.11572194687562, -105.4801321518591 40.11565345599552, -105.480126854251 40.11554900265974, -105.4800709291615 40.11483195882938, -105.4799571387577 40.11392000040892, -105.47994689984 40.11347995026318, -105.4799831084339 40.11315108747889, -105.4800228351893 40.11301603279571, -105.4800750724082 40.11289196174184, -105.4803280011827 40.11237701453049, -105.4807411547071 40.11166993238112, -105.4810369668682 40.11119699196959, -105.481141719745 40.11102902557507, -105.481172888273 40.11097904880864, -105.4816951330304 40.1100400158963, -105.4818546629206 40.10977445435542, -105.4823589838911 40.10893492078437, -105.482582135903 40.10869502801032, -105.4828170706975 40.10851196147547, -105.4830648709474 40.10834509253929, -105.4836849112431 40.10788811373511, -105.484198027461 40.10752006052201, -105.4845709709276 40.10725602731577, -105.4853990868868 40.10667498578111, -105.4858270889044 40.10635687564845, -105.486026963706 40.10620893576657, -105.486304682836 40.10598285091034, -105.4863931105853 40.10589493374012, -105.4865518733471 40.10573710627398, -105.4866348289009 40.10565503613041, -105.4869580787954 40.10529600615231, -105.4870421135721 40.1051768763199, -105.4871983867236 40.10493120199538, -105.487371107932 40.10466301956749, -105.4875799550242 40.10427789721646, -105.4877459068544 40.10386586691835, -105.4877981448226 40.10361990686008, -105.4878260717741 40.10337806193478, -105.4878189785318 40.10306209335884, -105.4877879352173 40.10273596572463, -105.4877500744142 40.10255999741634, -105.4876560960379 40.10233598297891, -105.487465982088 40.10197003253423, -105.4872232530914 40.10196231987193, -105.4870658759538 40.10185095894693, -105.4868196809375 40.10165327938159, -105.4866314968063 40.10150845106372, -105.4864409512302 40.10137037515732, -105.4862588024056 40.101262715445, -105.4860921845815 40.10116130415413, -105.485836424144 40.1010056361766, -105.4849920033265 40.1006347135134, -105.4839093249891 40.10031426319865, -105.4830191331509 40.10007645950926, -105.4820120665893 40.09979723467995, -105.4810633072941 40.09953297116691, -105.4804127682046 40.09934531424202, -105.4798790898619 40.09915212792707, -105.4796824446445 40.09903871820308, -105.479522623448 40.09891664061265, -105.47930842218 40.09870538968306, -105.4791915455861 40.09854274547259, -105.4791229733392 40.09834346283061, -105.4790505879534 40.09799448492377, -105.479052359013 40.09769652549827, -105.4791607602249 40.09740045238264, -105.4794961388154 40.09700293191574, -105.479797634012 40.0967043939273, -105.4801272805915 40.09645000218192, -105.4804192775763 40.09622379676028, -105.4807603604884 40.0959618559625, -105.4810373636038 40.09577718040623, -105.4815054397459 40.09552895692337, -105.4828849789354 40.0947965137981, -105.4834266856064 40.09449934716857, -105.4839563409643 40.09420958858656, -105.4843160786468 40.09401001008721, -105.4849600779124 40.09369009269385, -105.4853886269958 40.09344662435053, -105.4855847413489 40.0933274545906, -105.4857615504926 40.09322955615455, -105.4858563001833 40.09318953431386, -105.4859493892815 40.09312657467158, -105.4860073291051 40.0930647932408, -105.4861085231208 40.09283111166538, -105.4862261265858 40.09261623463396, -105.4862796494349 40.09253696028742, -105.4863440427661 40.09244053089211, -105.4864980044573 40.09217910013354, -105.4865441300771 40.09209076614776, -105.4865734608415 40.09198365362728, -105.4865740605829 40.09184425428345, -105.4865353522169 40.09178458501036, -105.4864553790939 40.09173698668518, -105.4862821973595 40.09160110904213, -105.4861073632745 40.09172768854545, -105.4859915724628 40.09188118251183, -105.4859399173889 40.09224669687541, -105.4855569227272 40.09245426085091, -105.4853991721848 40.09275577199028, -105.4851288304584 40.09284965722114, -105.4848585210306 40.0928001904127, -105.4845881940973 40.09282981365086, -105.484388652141 40.09291629160026, -105.4842631327652 40.09297312031171, -105.4841569490116 40.09291131642115, -105.4838834046625 40.09293599485009, -105.4834812175096 40.09261957708101, -105.4829727683574 40.09258243013446, -105.4827860975529 40.09266890721459, -105.4827313666256 40.09276034651839, -105.482319451568 40.09275534145816, -105.4819042578073 40.09297524606438, -105.4814987763503 40.09297765406125, -105.4813056759049 40.09302705373208, -105.4810578863604 40.09300724067585, -105.4808809131605 40.09292812172586, -105.4800635134075 40.09293045483656, -105.4794326933343 40.09316514307063, -105.4792073022026 40.09326798560966, -105.4790400326163 40.09332819563044, -105.4788469508883 40.09330838774851, -105.4786957308279 40.09320949749731, -105.4783771380855 40.09320449555493, -105.4780746382073 40.09319207991353, -105.4776658860475 40.09334771066776, -105.4775306528645 40.09356765334825, -105.4772474503477 40.09358737055681, -105.4771798253259 40.09371835001559, -105.4770510914053 40.09374303988567, -105.4768934234911 40.09368121997633, -105.4765330558175 40.09349330784084, -105.4760471484061 40.09340423194784, -105.4759119562152 40.0934931799337, -105.47569635047 40.09346841936511, -105.475580499466 40.09346097994491, -105.4754786601035 40.09343640599089, -105.4753745308298 40.0934856524864, -105.474866935992 40.09328879541138, -105.4746087047842 40.09324327275854, -105.4745636236239 40.09331740989728, -105.47428364008 40.09333464918728, -105.4742160376812 40.09339147986027, -105.4741162532533 40.09345077464172, -105.4739263878601 40.09344084558703, -105.473807349652 40.09335431389002, -105.4733664608556 40.09336904298313, -105.4731444341594 40.09330720218613, -105.4729916792803 40.0932286162595, -105.4728645084006 40.0931786152824, -105.4726553723939 40.09307723213188, -105.4724719569328 40.09303517184765, -105.4721758977621 40.0930177995692, -105.4718701942519 40.09297570969477, -105.4716835380748 40.09299049312087, -105.471474831456 40.09294463514954, -105.4710559544133 40.09296597786506, -105.4707674328991 40.0928908421586, -105.4705300663141 40.09290865323496, -105.4703206714044 40.09281923890566, -105.4697115083137 40.09283601095878, -105.4697155590948 40.09300137780273, -105.469580518479 40.09316219136713, -105.4692547133936 40.09320142434954, -105.4689847098194 40.09316435921112, -105.4687893378856 40.09312623647281, -105.468551822928 40.09315517446294, -105.4684076755523 40.09317974872646, -105.4680772432944 40.09316178552184, -105.4678259063069 40.09319388575036, -105.4675976897138 40.09313492541786, -105.4674769094881 40.09306510889996, -105.4673382935705 40.09303567465224, -105.4670449195582 40.09282043987553, -105.466830142165 40.0927503751534, -105.4665508752498 40.09279676225574, -105.466175368936 40.09283502917013, -105.4660133546789 40.09291547457706, -105.4658247582281 40.09295739868286, -105.4654896758057 40.09293227830818, -105.4653501000844 40.09283930116639, -105.4643976530924 40.09280481316541, -105.4631414548872 40.09316059275267, -105.4626582682873 40.09335336468543, -105.4624649122545 40.09357591069848, -105.4617286574722 40.09384614586697, -105.4615178994789 40.09387241055427, -105.4611654802694 40.09384973690847, -105.4610315535357 40.09376359322027, -105.4608583491733 40.0938136841182, -105.460658211982 40.09382791377131, -105.460243147953 40.09372063406089, -105.4599415660822 40.09367039294574, -105.4598018508458 40.09382404415791, -105.459650247651 40.09392369492305, -105.4594387633614 40.0939311501803, -105.4590250747669 40.09403479846681, -105.4585034035345 40.09393072863794, -105.4583682293032 40.09378227417517, -105.457595301498 40.09376715213234, -105.4571117811182 40.09377660859597, -105.4565999711225 40.0935476545582, -105.4562231144058 40.09334734393994, -105.4555297114199 40.09325414451478, -105.455083043723 40.09306095254485, -105.454748087056 40.09285350500218, -105.4544735196476 40.09281765242407, -105.4542315415061 40.09276751534037, -105.4539848272495 40.09283890565887, -105.4537427462525 40.09293889265795, -105.4537315827848 40.09234097421643, -105.4539008079947 40.09109986475135, -105.4544090914951 40.09054553456455, -105.454911908807 40.08989274726373, -105.4542163050892 40.08989247351533, -105.4535787792297 40.08972897229278, -105.4527672945866 40.08965444022031, -105.4525356967895 40.08926849065042, -105.4516859108819 40.08871903688248, -105.4512031061514 40.08837750060519, -105.4507010271719 40.08797659187697, -105.4501216663902 40.08757564758034, -105.4487837599722 40.08707073310003, -105.4486953969671 40.08646003986499, -105.4482595350263 40.08540252877995, -105.4478127204892 40.08505892551648, -105.4479228999761 40.08487798226903, -105.4478072669787 40.08469779895818, -105.4476238579465 40.0846890219965, -105.4475036345719 40.08450405928904, -105.4475897214318 40.08435881224172, -105.4470531159785 40.08438867944763, -105.4469366294201 40.08394907302981, -105.447177440526 40.08384352104201, -105.4471899505661 40.08355873923949, -105.4472465702956 40.0830880661421, -105.4461800763135 40.08279278918044, -105.4450593525014 40.08230016385585, -105.4443783256202 40.08273042306977, -105.4436178451164 40.08239173691055, -105.442816765798 40.08272966012455, -105.4425360960861 40.08319086210443, -105.4420155464476 40.08322135784578, -105.4416144854269 40.08399005819694, -105.4408534971651 40.08423571992876, -105.4391716431737 40.08438862612866, -105.438571195249 40.08420377113308, -105.4377308990862 40.08358819949705, -105.4374515200174 40.08260385368555, -105.4361713659957 40.08140366490991, -105.4352912053459 40.08066502816462, -105.434250820534 40.08001856161342, -105.4332097920201 40.08004872002739, -105.4323160686941 40.07981172585485, -105.4316887331096 40.07964800046999, -105.431048340433 40.07943232741334, -105.4287271625604 40.07844672135369, -105.4285285568764 40.07693954925447, -105.424953062166 40.07568973903737, -105.4238530554861 40.07588974495376, -105.4224688082221 40.07553496080854, -105.4210854863552 40.07510219739299, -105.4210690908914 40.07502410942288, -105.4210379038569 40.07498123368718, -105.4206329695366 40.0749038455992, -105.4204181933324 40.07484263681267, -105.4202083996824 40.07461261810035, -105.4195352042127 40.07476456033439, -105.4191247017771 40.07482938094511, -105.4189980306713 40.07484611794027, -105.4186447055464 40.07487513225324, -105.4180009566014 40.07488857546316, -105.4177762251645 40.07488622163074, -105.4174610348563 40.0748779494316, -105.4172705764785 40.07488147149702, -105.4170810759536 40.07488206684572, -105.4170306009453 40.07488568808787, -105.4169286974435 40.07489512468741, -105.4167905896386 40.07491916695444, -105.4166333942057 40.07497684600628, -105.4162312907294 40.07517846289863, -105.4159997512771 40.07528949075067, -105.4156196132907 40.07543625610639, -105.4153350203652 40.07550396612029, -105.4151395682494 40.07551491221498, -105.4149634135315 40.07550234559449, -105.4148358409656 40.07547591583315, -105.4146111929816 40.07540552041137, -105.4143570994708 40.07527584758753, -105.4142381667132 40.07519455728776, -105.4139032823823 40.07494558003621, -105.4136444687195 40.07478517666688, -105.413329475767 40.07462253567618, -105.4130705753038 40.0745330917355, -105.4129058764918 40.07449931594424, -105.4127516241002 40.07448895733638, -105.4125773454127 40.07450053023379, -105.4124096976944 40.0745384436123, -105.4122829936822 40.0745807785052, -105.4116113120437 40.07483923530526, -105.4112998081208 40.07492678295778, -105.4111312145296 40.07495957269411, -105.4109493026843 40.07498064805032, -105.4104369611586 40.07499780879358, -105.4099465988038 40.07495572838605, -105.4096666239786 40.07496136200007, -105.4094075828542 40.07497944835027, -105.4087209130649 40.07504255224723, -105.4072133339139 40.07514450001526, -105.4064926228099 40.07519135351045, -105.4058410165122 40.0752136172959, -105.4054705638814 40.0752272141406, -105.40520487196 40.07523357995193, -105.4049353748692 40.07523628450529, -105.4047392325432 40.07521783433648, -105.4045848509388 40.0751897922855, -105.4041947147465 40.07508862949976, -105.403705422345 40.0749653223569, -105.4035454821902 40.07493738955924, -105.4033969451357 40.07492482835819, -105.4031503024901 40.07492901141337, -105.4028950470262 40.07496317992302, -105.4025169204411 40.07501553263012, -105.4023550157805 40.07502929541273, -105.4021645541007 40.07503425519602, -105.4019389002541 40.07501138551396, -105.40168661591 40.074965083188, -105.4015019436022 40.07491810670258, -105.40096224968 40.07475231378992, -105.4007728206619 40.07470313718637, -105.4006128875573 40.0746708105926, -105.4003900881106 40.07465013520603, -105.4001936699258 40.07464511287059, -105.3999920191408 40.0746658845997, -105.3997996016553 40.07470668529642, -105.3996328800538 40.07475774923518, -105.3994223224821 40.0748299894019, -105.3992936939425 40.07487962339136, -105.3991136328338 40.07493506377642, -105.3989345365082 40.07498245837664, -105.3987192795767 40.0750122629322, -105.3984012230241 40.07501125209868, -105.3982545679028 40.07501551265776, -105.3981326490511 40.07503442581616, -105.3980545259296 40.07505922901456, -105.3979649460374 40.07510377494535, -105.3978486566331 40.0751790217227, -105.3973899365647 40.07562852046983, -105.3972817002089 40.0757136836102, -105.397169427459 40.07578848025003, -105.3968792179321 40.0759179797459, -105.3959609054664 40.07622318892043, -105.3953231254621 40.07647233550051, -105.3947619214149 40.07666278952232, -105.3941305833764 40.07686297010658, -105.3939136913895 40.07697539101873, -105.3934575621836 40.07722224613386, -105.3931865114511 40.07731992618486, -105.3929282780375 40.07737354901404, -105.3926318413482 40.07740020380218, -105.3923466903028 40.0774207953173, -105.3919433258007 40.07747300969441, -105.3915512466445 40.07751915932716, -105.3910859383422 40.07751872123406, -105.390588819259 40.07748152648809, -105.3899547533051 40.07738544205882, -105.3895851208953 40.07734591650613, -105.3890560983312 40.07733071977488, -105.3886608422517 40.07736951179238, -105.3882208880001 40.07745722445686, -105.3878287902893 40.07751315322446, -105.3875386890442 40.07756183623066, -105.3871751517061 40.07769123986255, -105.386958188724 40.07783792342001, -105.3868401010417 40.07793818621354, -105.3866996581514 40.07806535888105, -105.386575220841 40.07815092657836, -105.3864348761523 40.07821933925117, -105.3862435609229 40.07827301294386, -105.3861064964615 40.0782851193332, -105.3859439556369 40.07828495884738, -105.3854915187126 40.07820861461854, -105.3852495670619 40.07817436606354, -105.3849689629014 40.07813464671029, -105.384647065656 40.07813677433686, -105.3843346505428 40.07818542609105, -105.3841911614831 40.07822690365325, -105.3838658088119 40.07838571414805, -105.3835116873142 40.07859345906748, -105.3832533311892 40.07871071489546, -105.3828706781617 40.07882784409028, -105.3824975639514 40.07895722236837, -105.3821530389425 40.07914049159699, -105.3818913601033 40.079333636382, -105.3816040092101 40.07962713452685, -105.381316880753 40.07979087291746, -105.3809245713487 40.07995695099259, -105.3802294146402 40.08015943763821, -105.379588467187 40.08034483921757, -105.3792504093654 40.08046689970899, -105.3786411661966 40.08074291496696, -105.3780797871333 40.08098470179396, -105.3777130575363 40.08109693300169, -105.3774866867055 40.08114076234569, -105.3770053036764 40.08120390520853, -105.3766993091122 40.08121582032145, -105.3761925603991 40.08120548435789, -105.3760268068356 40.08121510006245, -105.3757111712446 40.08127107066737, -105.3751786731141 40.08139780561959, -105.3744967961343 40.08157402736211, -105.3735477428702 40.0818006048877, -105.3730416668277 40.08192675278983, -105.3726786466126 40.08199815224141, -105.3724146658471 40.08203164841389, -105.3720517316847 40.08205658721963, -105.3715667481044 40.08210790769671, -105.3712911926056 40.08211536164035, -105.3710047166085 40.08208494329329, -105.3706571489542 40.0819848523058, -105.3701603136584 40.08182251295334, -105.3693330902472 40.08154316557858, -105.3691740018331 40.08149407507, -105.3689732329173 40.08146939130329, -105.3687454792302 40.08146913257269, -105.3682581015067 40.08148550858736, -105.3674792688943 40.08151471573545, -105.3669855945874 40.08156515588454, -105.3666338417142 40.08163741303427, -105.3665354783196 40.08168099405719, -105.3664748780766 40.08172531938194, -105.3664584034446 40.08159014621046, -105.3664654543084 40.08151024750345, -105.3665410705586 40.0813216177777, -105.3666249026477 40.08104341501357, -105.3665924458401 40.08081366575016, -105.3664632649919 40.08064976953737, -105.3662886091598 40.08052481296188, -105.3660390097108 40.08039337010403, -105.3659304079325 40.08034970692742, -105.3658929678842 40.08033465331701, -105.3659703076023 40.08049001044129, -105.3660033070792 40.08058400926235, -105.3651603062312 40.08079800940757, -105.36386330684 40.08112600999898, -105.3614307179702 40.08181077296624, -105.3614136449111 40.08208931510966, -105.361373970351 40.08273668039418, -105.3613838696417 40.08273389398298, -105.3616833691065 40.08264960897541, -105.3616895744276 40.08266268384122, -105.3618231569629 40.08294413896749, -105.3618343745151 40.08296777085793, -105.3618626507548 40.08302734621064, -105.3612294649398 40.08322514258172, -105.3582044235136 40.08420073402425, -105.3580926092154 40.08423693487651, -105.3581270614178 40.08459850432136, -105.3581348601366 40.08459842924469, -105.3591926002434 40.08458815364854, -105.3591925371214 40.08460053741205, -105.3591905319785 40.0849959100054, -105.3573681646263 40.08502614465402, -105.3569189380437 40.08526239120709, -105.3568395193715 40.08711423232176, -105.3556791226172 40.08712097800886, -105.3556774246944 40.08712098849529, -105.354242246951 40.08712931769688, -105.3542328567851 40.08712937248871, -105.3527096423569 40.08713819019081, -105.3527001841789 40.08713824477123, -105.3519880447198 40.08755429373965, -105.3510273451841 40.08805364431768, -105.3510314240971 40.08805658117283, -105.3510339691511 40.08805849111732, -105.3510364707778 40.08806041991922, -105.3510389277868 40.0880623756828, -105.3510405793695 40.08806372697654, -105.3510413472218 40.08806435481455, -105.3510437197018 40.08806635730237, -105.3510460487584 40.0880683768463, -105.3510483355446 40.08807042245434, -105.3510505753798 40.08807248961713, -105.3510527729524 40.08807457924146, -105.3510549200622 40.08807668771413, -105.3510570237446 40.08807881504423, -105.351059080476 40.08808096392912, -105.351061091431 40.08808313346974, -105.3510630566174 40.08808532006347, -105.3510649713371 40.08808752730682, -105.3510668391175 40.08808975070119, -105.351068656435 40.0880919929439, -105.3510704291584 40.08809425134065, -105.3510721502444 40.0880965294849, -105.3510738208755 40.08809882287498, -105.3510754457399 40.08810113241754, -105.3510770166333 40.08810345630074, -105.3510772620555 40.08810383308597, -105.3510785405837 40.08810579813619, -105.3510800410192 40.08810816876191, -105.3510817287355 40.08811069273843, -105.3510833753659 40.08811323737671, -105.3510849820807 40.08811580357887, -105.351086548892 40.08811838594115, -105.3510880757858 40.08812099076799, -105.3510895604248 40.08812361445374, -105.3510910063348 40.08812625340051, -105.3510924076469 40.08812891030255, -105.3510937713965 40.08813158516899, -105.3510950928933 40.08813427799377, -105.3510963697981 40.08813698607194, -105.3510976021068 40.08813971120482, -105.3510987945178 40.08814244979585, -105.3510999482036 40.08814520184658, -105.3511010526129 40.0881479664427, -105.3511021147673 40.08815074989782, -105.3511031346887 40.08815354230494, -105.3511041123671 40.08815634816715, -105.3511050454592 40.08815916658087, -105.351105933969 40.08816199574477, -105.351106776724 40.08816483565742, -105.3511075737242 40.08816768631873, -105.3511083343561 40.08817054503891, -105.3511090421975 40.08817341449873, -105.3511097078077 40.08817629200986, -105.3511103311927 40.08817917487041, -105.3511109029578 40.08818206937269, -105.3511114371899 40.08818496832981, -105.351111919806 40.08818787712743, -105.3511123602068 40.08819078677125, -105.3511127548545 40.08819370626314, -105.3511131061122 40.08819662750032, -105.3511134057638 40.08819955407481, -105.3511136655411 40.08820248329983, -105.3511138760653 40.08820541426265, -105.3511140443603 40.08820835237604, -105.351114163412 40.08821128772411, -105.351114241413 40.08821422752239, -105.3511142701628 40.08821716815781, -105.3511142520106 40.08822010783207, -105.3511141893056 40.08822304474702, -105.3511140808613 40.08822598520552, -105.3511139243503 40.08822892109879, -105.3511137267983 40.08823185693918, -105.3511134800089 40.08823478731219, -105.351113191008 40.08823771673009, -105.3511128527656 40.08824064248196, -105.3511124723156 40.08824356547749, -105.3511120426341 40.08824648030368, -105.3511115695742 40.08824939147138, -105.3511110496261 40.08825229537347, -105.3511104874762 40.08825519381728, -105.3511098760888 40.08825808679372, -105.3511092248507 40.08826097161301, -105.3511085279028 40.08826384646623, -105.3511077805547 40.08826671134739, -105.3511069968658 40.08826957167852, -105.3511061604374 40.08827241933256, -105.3511052865074 40.08827525703119, -105.3511043656989 40.08827808296099, -105.3511034015258 40.0882808989278, -105.3511023951647 40.08828370313181, -105.3511013407563 40.08828649376421, -105.3511002453384 40.08828926993341, -105.3510991053852 40.08829203523749, -105.3510979279441 40.08829478428164, -105.3510967024539 40.08829752065474, -105.3510954347834 40.08830024166259, -105.3510941284525 40.08830294640897, -105.3510927799473 40.08830563308802, -105.3510913869165 40.08830830439874, -105.3510899505349 40.088310959442, -105.3510884766733 40.0883135946227, -105.3510869629747 40.08831621534176, -105.3510854047624 40.08831881528859, -105.3510838090661 40.0883213971742, -105.3510821712054 40.0883239564893, -105.3510804970312 40.08832649864536, -105.3510787818711 40.08832901553052, -105.3510770257072 40.08833151525054, -105.3510752332379 40.08833399420897, -105.3510734009512 40.08833644969923, -105.3510715288491 40.08833888082079, -105.3510696239633 40.08834128938393, -105.3510676816053 40.088343674482, -105.351065699426 40.0883460379133, -105.3510636821256 40.08834837518056, -105.3510616261805 40.08835068898124, -105.3510595374595 40.08835297662093, -105.3510574124448 40.08835523809517, -105.351055252313 40.08835747160411, -105.3510530570523 40.08835968255164, -105.3510508290275 40.08836186193435, -105.3510485693955 40.08836401695893, -105.3510462734738 40.08836614401667, -105.3510439459587 40.08836824041177, -105.3510415833244 40.08837030974222, -105.3509560258479 40.08843761152456, -105.3507798770322 40.08857084662024, -105.3507538096081 40.08863307525191, -105.3507519531502 40.08863799036086, -105.3507511319305 40.08864084523704, -105.3507504935722 40.08864373007083, -105.3507500357499 40.08864663585278, -105.3507497561281 40.08864955807664, -105.3507496605839 40.08865249044558, -105.3507497479682 40.08865542215029, -105.3507500159438 40.08865834958532, -105.3507504680483 40.0886612637487, -105.3507511019483 40.08866415923357, -105.350751910624 40.08866702882577, -105.3507528976031 40.08866986802661, -105.3507540605621 40.08867266692603, -105.3507553959971 40.08867541921492, -105.350756900396 40.08867812218688, -105.3507585679157 40.08868076682799, -105.350760398576 40.0886833441317, -105.3507623876923 40.08868585139007, -105.3507645258996 40.08868828138591, -105.3507648979519 40.08868866373927, -105.3507668167196 40.08869063232233, -105.3507692461027 40.08869289427427, -105.3507718140629 40.08869506093713, -105.3507745112231 40.08869713049755, -105.3507773305537 40.08869910024445, -105.3507802720763 40.08870096027083, -105.350783320557 40.08870270605373, -105.3507864724758 40.08870433848928, -105.3507897254995 40.0887058521706, -105.3507930608822 40.08870723986828, -105.3507965301085 40.0887090870666, -105.3508980689437 40.08877062856219, -105.3509009761502 40.08877209766227, -105.3509038776238 40.08877350731244, -105.3509068038209 40.08877487196231, -105.3509097547317 40.08877619611515, -105.350912730362 40.08877747706896, -105.3509157295431 40.08877871302094, -105.3509187499201 40.08877990847136, -105.3509217926772 40.08878105801779, -105.3509248566341 40.08878216526129, -105.35092793711 40.08878322569265, -105.350931043486 40.08878423932394, -105.3509341651927 40.08878521334669, -105.3509373034264 40.08878613695467, -105.3509404581733 40.0887870164524, -105.3509436294314 40.08878785274052, -105.3509468183891 40.08878863861543, -105.3509500215108 40.08878938217835, -105.3509532376397 40.0887900762226, -105.3509564620774 40.08879072434474, -105.3509596995144 40.08879132655078, -105.3509629511253 40.0887918819416, -105.3509662087037 40.08879238960599, -105.3509694781146 40.08879284865083, -105.3509727546598 40.0887932626727, -105.3509760383511 40.08879362626768, -105.3509793291805 40.08879394303838, -105.3509826283206 40.08879421298629, -105.3509859299085 40.08879443610383, -105.3509892327773 40.08879460968762, -105.3509925416098 40.08879473734624, -105.3509958505506 40.08879481546952, -105.3509991642883 40.08879484496426, -105</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>14</v>
-      </c>
-      <c r="E11" t="n">
-        <v>14</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Jamestown School</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>111 Mesa St, Jamestown, CO 80455</t>
+        </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Jamestown School</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>111 Mesa St, Jamestown, CO 80455</t>
+          <t>http://jae.bvsd.org/</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
+          <t>Jamestown Elementary School</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>40.1164318137431</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-105.387802261192</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
           <t>http://jae.bvsd.org/</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Jamestown Elementary School</t>
-        </is>
-      </c>
-      <c r="L11" t="n">
-        <v>40.1164318137431</v>
-      </c>
-      <c r="M11" t="n">
-        <v>-105.387802261192</v>
-      </c>
       <c r="N11" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>http://jae.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
         <is>
           <t>POINT (-105.387802261192 40.1164318137431)</t>
         </is>
@@ -1240,59 +1170,53 @@
           <t>MULTIPOLYGON (((-105.130907895079 40.17667497536176, -105.1309108852502 40.17618991643079, -105.1309011192309 40.1758791343955, -105.1309030890619 40.17558211464502, -105.1308961355192 40.17475305743081, -105.130896930049 40.17421089176275, -105.1308928914898 40.17403189495574, -105.1308978484933 40.17384386824337, -105.1308981571233 40.1736550034996, -105.1308928515666 40.17318199632658, -105.130890136097 40.17308892735598, -105.1308980849702 40.1728770261307, -105.1308830569357 40.17234908671396, -105.1308731301453 40.17200206767621, -105.1308640602036 40.17169513068922, -105.1308610970434 40.17144997901022, -105.1308601753751 40.17135609075753, -105.1308571509205 40.17105603681589, -105.130858089966 40.17094897815058, -105.1308520529194 40.17054487184136, -105.1308380730325 40.1698239502182, -105.1308381211171 40.16968312372387, -105.1308328523583 40.16953294692157, -105.130826950711 40.16923590355137, -105.130825096449 40.16911593337741, -105.1308268264415 40.16899487857084, -105.130829023898 40.16878789975995, -105.130829951995 40.16861687941822, -105.1308339090772 40.16841512361963, -105.1308248690956 40.16770711920258, -105.1308251696132 40.16745401704761, -105.1308240275999 40.16707106507126, -105.1471472878128 40.17412208832916, -105.1538401553576 40.17416747340352, -105.1538534119111 40.17702152067658, -105.1546629131087 40.17736968103145, -105.1546620818144 40.17647724158829, -105.1546599342045 40.17417298750612, -105.1546589995688 40.17417299912417, -105.1546569996872 40.17249899848197, -105.1546569998319 40.17225799859407, -105.1546530002739 40.17018099915842, -105.154647999395 40.16705899872255, -105.1546488353165 40.16705898771062, -105.1546488300367 40.16705586518081, -105.1551078351645 40.16704986397507, -105.1562688454048 40.16703286263721, -105.1572978539927 40.16702986225165, -105.1593498721462 40.16705286010649, -105.1595208740774 40.16707385977891, -105.1596798760458 40.16712085952145, -105.1598118775726 40.1671618596847, -105.1599118790576 40.16721485751804, -105.1602088846895 40.16741385793949, -105.161120902206 40.16807485153609, -105.1622709235831 40.1688868436568, -105.1631259398792 40.16948983996239, -105.1635209475333 40.16973283788921, -105.1637179519749 40.16985083726004, -105.1638209526211 40.16989583642651, -105.1640679558686 40.16999983608142, -105.1642169582605 40.17006083511097, -105.1642709600386 40.17007883540592, -105.1650199693466 40.17032183177924, -105.1664129896231 40.17079382714124, -105.1665174951051 40.17073080935722, -105.1665201919034 40.17073175740313, -105.1668849048761 40.17085999075397, -105.1668943955052 40.17084829540469, -105.1668985520034 40.17084317464879, -105.1668896186171 40.17084009214113, -105.1669304607418 40.17078976692029, -105.1669332093008 40.17078637943621, -105.1670240178124 40.17067447924944, -105.167026766362 40.17067109176306, -105.167035661948 40.17067421828263, -105.1677465944088 40.16979815123889, -105.1677518350548 40.16979169341922, -105.1687231045455 40.16859477217606, -105.1687256438738 40.1685916425322, -105.1687255340658 40.16858670852341, -105.1728195198593 40.17056786550766, -105.1728205681745 40.1705683728318, -105.1729529231051 40.17063241614367, -105.1733576954174 40.17082828027013, -105.1733657812711 40.17083213172842, -105.1734768197971 40.17088453830642, -105.1734768239046 40.17088245964705, -105.1734766984293 40.17058819044085, -105.1734767013714 40.17058610997677, -105.1734876717343 40.1687689579743, -105.1734888774345 40.16876895687698, -105.1735104074165 40.16876894654175, -105.1735112021403 40.16875746475598, -105.1735772011636 40.16694246349251, -105.1782538706628 40.16695343985297, -105.1782449702689 40.1681079937859, -105.178239767373 40.1687701694254, -105.1782249819881 40.17185948877151, -105.1781973695228 40.17705081512157, -105.1781856753826 40.1794676433639, -105.1781825181676 40.17975001998585, -105.1781812588263 40.18010303695387, -105.1781793654503 40.18059104394589, -105.1781684523568 40.18168714946533, -105.1781684669265 40.18183643617814, -105.1781660473366 40.18316294860183, -105.1781498990898 40.18620289633849, -105.1781465206755 40.1865180200456, -105.1781438093425 40.18681401520618, -105.178140520294 40.18717302076964, -105.1781444987996 40.1872194370608, -105.1781439104042 40.18733011805361, -105.1781394025259 40.18737198322795, -105.1781394746657 40.18773489066125, -105.178139841851 40.18809600032777, -105.1781305791092 40.18957200588383, -105.1781304006922 40.18958464219161, -105.1781202084915 40.1900471212033, -105.1780948944239 40.19119569292697, -105.1780936532397 40.19125198092252, -105.1780785993141 40.19253098832572, -105.1780756714483 40.19337646219445, -105.17807555733 40.19340999518588, -105.1780755436376 40.19355999935622, -105.1780754437916 40.19356992676756, -105.1780551400565 40.19491920996467, -105.1780545724636 40.19495698637294, -105.1780511446152 40.19536670668712, -105.1780475346618 40.1958009894524, -105.1780295545943 40.19680784784939, -105.1780344485064 40.19725808820253, -105.1780344787037 40.19764486805438, -105.1780338448599 40.19770630300314, -105.1780338432419 40.19770639666449, -105.1780265031893 40.19837698788592, -105.1780244953112 40.19858399017504, -105.1780244611668 40.19870778033302, -105.1780244603029 40.19882999897617, -105.1780262933825 40.19946629969199, -105.1780294225022 40.20054600094512, -105.1780177912117 40.20209443943981, -105.1780154294347 40.20240789362089, -105.1780170937183 40.20279956093896, -105.1780170986384 40.20280075429105, -105.1780171024931 40.20280167654974, -105.1780171035354 40.20280170447224, -105.1780193743578 40.20332300422022, -105.1780125892502 40.20344194989982, -105.1779985287708 40.20376896198804, -105.1779793391662 40.20578677022317, -105.1779733735186 40.20641786448409, -105.1779725180975 40.20704933316319, -105.1779724928907 40.20706829500229, -105.1779692945993 40.20951299755229, -105.1779642885702 40.21058099413643, -105.1779642880199 40.21058111031635, -105.1779548545939 40.21285325838544, -105.1779462410317 40.21411403975657, -105.1779402743808 40.21444507532357, -105.1779392003615 40.21541000119228, -105.1779391996817 40.21541064063836, -105.1779231113842 40.21602719206967, -105.1779222810411 40.216058878454, -105.1779061898209 40.21830724012914, -105.1779061013509 40.21831971271479, -105.1779001627716 40.21915299099524, -105.1778640906119 40.22388898961723, -105.177864540534 40.22467292051728, -105.1778669788484 40.22911209642017, -105.1778663526854 40.22919784805772, -105.177865003127 40.22937498989583, -105.1778569786166 40.23065399100331, -105.1778535241373 40.23095143561333, -105.1778529903291 40.23099711941484, -105.1778516407136 40.23142737115413, -105.1778499448728 40.23197999479415, -105.1778406387775 40.23204779070896, -105.1778184627386 40.23220092675904, -105.1777991760248 40.23223585886259, -105.1777990753533 40.2322360251985, -105.1777373000234 40.23228598032479, -105.1776563108877 40.23231160004515, -105.1776460005625 40.23231260073759, -105.1766870186988 40.23231559253281, -105.1762842567278 40.23231202562735, -105.1746699443099 40.2322976123188, -105.1733949514683 40.23228760767522, -105.1720667001548 40.23229148153948, -105.1720321683417 40.23229158269653, -105.1720320179274 40.2322915831708, -105.1715299999297 40.2322915883125, -105.1691109836499 40.23229392230051, -105.1684200036398 40.23229458111676, -105.1661308987598 40.2323106876401, -105.1660599158641 40.23231118707495, -105.1652950423296 40.23231656198064, -105.162829047121 40.2323355569361, -105.160993003236 40.23233656725746, -105.1596320574399 40.23234954749802, -105.159631111938 40.2326021603701, -105.159639287903 40.23489116429988, -105.1596411241535 40.23543000233618, -105.1596455377918 40.23602956648127, -105.1596490939906 40.23651103133323, -105.1596522712427 40.23722609101691, -105.1596540870133 40.23763600383838, -105.1596750332671 40.23923601341176, -105.1596793682309 40.23954562245473, -105.1596820218607 40.23973500530968, -105.1596852663667 40.24018047174287, -105.1596852684716 40.24018075544682, -105.1596864522177 40.24038181330056, -105.1597150691784 40.24686193224582, -105.1597140201794 40.24693386583294, -105.1597068877074 40.24714470682556, -105.1596630831104 40.24838283982047, -105.1596334362387 40.24898218808481, -105.1596333787975 40.24898333081097, -105.1596251227761 40.24914994405553, -105.1595390930119 40.25123381788716, -105.1595390876333 40.25123395296526, -105.159436146626 40.25319294047603, -105.1594315084507 40.25329819468507, -105.1594011116351 40.25399307586693, -105.1594193459625 40.25413204204748, -105.1594254824308 40.25417719946864, -105.1594376867242 40.25422352574407, -105.1594480492416 40.25426137441204, -105.1594480757986 40.2542614699565, -105.1595344547845 40.25439932079264, -105.1596523760393 40.25452303893846, -105.1597878147295 40.25460896776644, -105.1599382833191 40.25468036847293, -105.160341656995 40.25483557437291, -105.1603418083376 40.25483563335776, -105.1605874317561 40.25494246474813, -105.1608249922877 40.2550751577644, -105.1610305136834 40.25524053832483, -105.1610515290015 40.25526742410285, -105.1610813427591 40.25530659135412, -105.1611090626313 40.25537858837161, -105.1611188206494 40.25540469905818, -105.1611160671059 40.25552193081968, -105.1610980231822 40.25558792265264, -105.1610768827189 40.25562969209872, -105.16104190423 40.25569596936283, -105.1610295681123 40.25571325316199, -105.1609816117556 40.25576544534216, -105.160838322246 40.25591957105722, -105.1607775160145 40.25598497549689, -105.1607389143321 40.25602649736401, -105.1606064865818 40.25617027131609, -105.1605757980321 40.25620359452309, -105.1599924986764 40.25659730650925, -105.1599989720365 40.25673921994948, -105.1599547792698 40.25678485179284, -105.1598025509507 40.25693200702809, -105.1595811076893 40.2571367624378, -105.1594444833865 40.2572704528118, -105.1594442707474 40.25727066113117, -105.1593850046439 40.25732871936017, -105.1593135897142 40.25741741259193, -105.1592464000906 40.25751418241698, -105.1592073730529 40.25761787627735, -105.1592065780735 40.2576200489465, -105.1592065673312 40.25762008133739, -105.1591639582087 40.2577383241414, -105.1590671169694 40.25811957256996, -105.1588131688499 40.25926007653372, -105.1588050309629 40.25937747332689, -105.1588035176399 40.25938480355556, -105.1587867913851 40.25946585282338, -105.1587732062316 40.25970394070752, -105.1587867235447 40.25988310314099, -105.1588772703448 40.26029735125145, -105.1589371805952 40.26053541613221, -105.1589944087731 40.26086126506672, -105.1590273950741 40.26104527341096, -105.1590403258768 40.26112013450027, -105.1590548541795 40.26120439741041, -105.1590573513478 40.26121887960556, -105.157939095726 40.26123214999929, -105.1579317739117 40.26123219050455, -105.150072849193 40.26127578314014, -105.1500654098023 40.26127582459359, -105.1468465531939 40.26128064035046, -105.1467975327648 40.26128071323016, -105.1467900194693 40.26128072362639, -105.1429453634243 40.26128639073979, -105.1429377925196 40.26128640160884, -105.1406184806711 40.26128976910978, -105.1406108744983 40.26128977971715, -105.1379285346962 40.2612928022528, -105.1379208885625 40.2612928107571, -105.1342613927367 40.26129683485336, -105.1342536901744 40.26129684293716, -105.1314853591348 40.26129978664688, -105.1314776165972 40.2612997953193, -105.1311626635374 40.26130017098836, -105.1311533315791 40.26130018177933, -105.1310555398049 40.26130097878088, -105.1310552670561 40.26130098061338, -105.1310475630141 40.26130104431788, -105.1306819028509 40.26130423180297, -105.1306741940863 40.26130429907008, -105.1302260335092 40.26130820712956, -105.1302183188658 40.26130827434753, -105.1302173595303 40.26130828299087, -105.1302096472331 40.26130835111636, -105.1217148802063 40.26138175606975, -105.121707037398 40.26138182410287, -105.1177053612486 40.26141472727208, -105.115742714383 40.26143086470346, -105.1157347810537 40.26143093023018, -105.1157250642582 40.26143100964919, -105.1157171297533 40.26143107517082, -105.1142641668518 40.26144297225395, -105.114256210008 40.26144303760103, -105.1122949779269 40.26145914831125, -105.1122869928654 40.26145921342841, -105.1100575800509 40.26145729732243, -105.1100495048815 40.26145728993158, -105.108467570751 40.26145589258702, -105.1084594708947 40.26145588500171, -105.1057206751605 40.26145337069362, -105.1057125353351 40.26145336277992, -105.1055764423602 40.26145325215404, -105.1055683013489 40.26145324602741, -105.1029318436331 40.2614507919655, -105.1029236626631 40.26145078371452, -105.1026625533545 40.26145053973125, -105.1024478793076 40.26145187944849, -105.1024397379435 40.26145193344261, -105.1009687718798 40.26146179064328, -105.100960609353 40.26146184446047, -105.1005852751427 40.26146435504149, -105.1005771055564 40.26146440970788, -105.1000227844769 40.26146813525616, -105.1000146066554 40.261468190755, -105.0999062011835 40.26146891936003, -105.0998980221863 40.26146897484655, -105.0931208000076 40.26151409742457, -105.093112518724 40.26151415207208, -105.0880094105433 40.26154786605323, -105.0880010516577 40.26154792095951, -105.085095114039 40.2615670067869, -105.0835872226432 40.26157690882633, -105.0835787990881 40.26157696408129, -105.0835227733561 40.26157732810092, -105.0835143486308 40.2615773824463, -105.0834155232793 40.26157802110299, -105.0834070961972 40.26157807633273, -105.0828514814461 40.26158169068106, -105.0823658167984 40.26158485138247, -105.0740535654481 40.26163893567075, -105.0648359236269 40.26171750422144, -105.0645857591206 40.26171962647721, -105.0645770650161 40.26171970004614, -105.0550981174537 40.26181467832726, -105.0550882881114 40.26180786511199, -105.055089102158 40.2561198963567, -105.0550893227732 40.25454176871278, -105.0550893173981 40.25453828145123, -105.0550786320396 40.24742874159061, -105.0550786266126 40.24742526243025, -105.0550781606866 40.24716273015109, -105.0549125264558 40.23982547279036, -105.0549124708876 40.2398219348914, -105.0549113570069 40.23974294872203, -105.0549114469985 40.23973943660069, -105.0550890166748 40.23277390435145, -105.0550845739097 40.2318966321016, -105.055084557513 40.2318932132323, -105.0550521333209 40.22547414490511, -105.0550521966061 40.22547075966209, -105.0551545759616 40.22001725305361, -105.055154576327 40.22001719721558, -105.0551656190208 40.21909135193408, -105.055165657996 40.21908808908051, -105.0551754353958 40.21826973689463, -105.0551754375666 40.2182695846955, -105.0551754907823 40.21826647950752, -105.0551768073136 40.21818594070018, -105.055175145165 40.21195627749737, -105.055175144372 40.21195298746794, -105.055174874339 40.21095185735524, -105.0551748699924 40.2109485718148, -105.0551659295546 40.20376782758404, -105.0551659250086 40.20376457266076, -105.0551658095187 40.20368024908086, -105.0551658094086 40.20367990683798, -105.0551933208667 40.20367993430043, -105.0557612194496 40.20367601713887, -105.0557639998678 40.20367599809817, -105.0558368854482 40.20367580791534, -105.056911999972 40.20367299893432, -105.0583553984353 40.20363396552585, -105.058538999233 40.20362899881254, -105.0594407995711 40.20360935166872, -105.0594569996611 40.2036089990881, -105.0594589803057 40.20360895889921, -105.0604691792169 40.20358828730067, -105.0605809999359 40.20358599860956, -105.0625290002004 40.20354499890966, -105.0647029999319 40.20349699885044, -105.0647501006766 40.20349602781442, -105.0647763071737 40.20349548788953, -105.0647999996946 40.20349499884104, -105.0649459997082 40.20349199875547, -105.0650095092602 40.20349053724983, -105.0662489993874 40.20346199884766, -105.067296999437 40.20343799958135, -105.0690749998827 40.2033999992119, -105.074014699015 40.20330567887017, -105.0740449135742 40.20330506064477, -105.0741578445987 40.20330274940949, -105.0741613829224 40.20330268048043, -105.074174153481 40.20330244200157, -105.0747471835121 40.20329593233741, -105.0765138346332 40.20327584447682, -105.0776037795497 40.20327547779507, -105.0779601843807 40.2032754757722, -105.0783671987761 40.20327647585538, -105.0783672903983 40.20327647528878, -105.0787342713654 40.20327551513552, -105.0788240199679 40.20327306536132, -105.0790784726884 40.20326612110446, -105.0798893828385 40.20325404710055, -105.0806879610338 40.20324837306046, -105.0816501847357 40.20324047561559, -105.0822069163204 40.20323024316917, -105.0830682814023 40.2032196909061, -105.0835791856489 40.20321847582563, -105.0835981069327 40.20321967515504, -105.0837211863008 40.203227474651, -105.0856447171358 40.20320449576815, -105.0856452363401 40.20320449042337, -105.0877735888691 40.20318643920209, -105.0888532544556 40.20317763229867, -105.0897408380637 40.20317038475633, -105.0904716416781 40.20316441172043, -105.0908696894022 40.20316115619768, -105.0912832223234 40.20316093513956, -105.0914944937617 40.2031624183343, -105.0917522278974 40.20316422728517, -105.0919455217571 40.20316558314721, -105.0921975370513 40.20316735111282, -105.0926146724067 40.20317027581347, -105.0928657727666 40.20317203549725, -105.0930057234746 40.2031730162505, -105.093005727191 40.20317337651804, -105.0930711835685 40.20317401664741, -105.0930820960962 40.20317412349315, -105.0932201875574 40.20317547481145, -105.0932147345931 40.20427675894129, -105.0932105779957 40.2051159902964, -105.0932041876712 40.206406475457, -105.0932022136999 40.20678056108493, -105.0932545485407 40.20678031284936, -105.0954331146536 40.20678761374383, -105.0971599989639 40.20679337055231, -105.0971607119664 40.20679337303581, -105.0976247948587 40.20679491652393, -105.0976247893968 40.20679703029651, -105.0977981545344 40.20679786929404, -105.0977981954315 40.20680406130543, -105.0978192166669 40.20994758211779, -105.0978192638643 40.20995469549757, -105.0978192865362 40.20995801171471, -105.0978221643321 40.21038836945402, -105.1020764826853 40.210400971623, -105.1023781912976 40.21039966129107, -105.1024751480868 40.2103992398415, -105.1024778062865 40.2099546758207, -105.102494799139 40.20914168066236, -105.102465788828 40.20820268604596, -105.1025047847938 40.20772268878633, -105.1025137811899 40.20727069089985, -105.1025437709455 40.20634669622018, -105.1025237636843 40.20571670054039, -105.1025237619839 40.20539370203086, -105.1025210625498 40.20515181087357, -105.1025107002389 40.20422331812248, -105.1022201967591 40.20421818627374, -105.1018961897053 40.20421247454206, -105.1018971891388 40.2032814736801, -105.1024151901731 40.20329347428748, -105.1024483477597 40.20329452110688, -105.1024214449243 40.20329367141449, -105.1024213646419 40.20328751439211, -105.102421336487 40.20328529873123, -105.1024054437498 40.2013562575215, -105.1024006556609 40.20088934679336, -105.1024847271985 40.20065462381238, -105.1024859020631 40.19952909100861, -105.1024319782109 40.19815907813807, -105.1024139175533 40.19696213301737, -105.1023788304601 40.19586093436818, -105.1023809230087 40.19574811518007, -105.1023868541003 40.19503988820251, -105.1023850650994 40.1948559566662, -105.1023748592168 40.19451991641212, -105.1023501276933 40.19385193690373, -105.1023401095519 40.19238187512373, -105.1023480324539 40.19219001707661, -105.1023450792598 40.19183807835071, -105.1023359238445 40.19064912338679, -105.1023129456827 40.18974287047573, -105.102305841591 40.18899891023079, -105.1022938744325 40.18859697923833, -105.1022929712663 40.18856787832284, -105.1022919348154 40.18813304226678, -105.1022951231635 40.18764908370499, -105.1022961545613 40.18759500754209, -105.102314050903 40.18661587375054, -105.102324014524 40.18558510414968, -105.1023359709285 40.18488705328424, -105.1023460249624 40.18414699542499, -105.102370035092 40.18248900592155, -105.1023831548078 40.18140800978896, -105.1023829530066 40.18125894705506, -105.1027139937316 40.18126200709273, -105.1033940415842 40.18125610659184, -105.1036499481707 40.18125506224674, -105.1044011718303 40.18125708676741, -105.1047898365833 40.18126006333194, -105.1051319899099 40.18126013369076, -105.1052980584674 40.18125987759827, -105.1059451380013 40.18126098709274, -105.106641973712 40.18126088969616, -105.106833109551 40.18125797063896, -105.1072020949942 40.18126004898254, -105.1080911123929 40.18126196732355, -105.1084361110251 40.18126505829095, -105.1086240113595 40.18126487136174, -105.1089940736708 40.18126612354689, -105.1101640174649 40.18126520655875, -105.1112559916314 40.18126990755782, -105.1113569308159 40.18126805117004, -105.1115040224316 40.18126909494015, -105.1118629926047 40.18127002597253, -105.1118759946224 40.18181388411318, -105.1119081200098 40.18251894680662, -105.1119091664257 40.18315088404788, -105.1119118919206 40.18367686408679, -105.1119049061916 40.18402300359683, -105.1119319115066 40.18487960280919, -105.1120085237062 40.186557607745, -105.112011570436 40.18673288206929, -105.112017894645 40.18707819066701, -105.1120313601333 40.18760194311961, -105.1120540599835 40.18855794243968, -105.1125329666713 40.18856092088617, -105.1125820027335 40.18856108520247, -105.1133670179578 40.18855190824585, -105.1134489979368 40.18854998659783, -105.1145858430134 40.18854499691239, -105.1146671019506 40.18854389517986, -105.1158580022557 40.18853797614679, -105.1167671242837 40.18854593391976, -105.1172141737779 40.18854906207515, -105.1174969479037 40.18854890001953, -105.1179300587332 40.18854813537448, -105.1183019485997 40.18854991306068, -105.1186970917979 40.1885539619918, -105.1190850825382 40.1885568881324, -105.1194899230949 40.18855492662844, -105.121360830748 40.18856299055086, -105.1256918879809 40.18856611215961, -105.1288573477865 40.18857997484698, -105.1309169704838 40.1885889481708, -105.1309130611667 40.18812198620383, -105.1309220276749 40.18759110388334, -105.1309188689071 40.186986063103, -105.1309191252318 40.18634507253613, -105.1309118354979 40.18564393849361, -105.1309110183405 40.18513498587469, -105.1309051019469 40.18497190483541, -105.1309039419183 40.18465813085619, -105.1308979191687 40.1841851230857, -105.1309021056735 40.18314994122324, -105.1308898627142 40.181442199769, -105.1308910444444 40.1812969306925, -105.1309031473364 40.17900092566963, -105.1309088561322 40.17768491898182, -105.1309089894072 40.17686906099571, -105.130907895079 40.17667497536176), (-105.1311514181201 40.2604706245238, -105.1311533230373 40.26129655853457, -105.1311533315791 40.26130018177933, -105.1311514181201 40.2604706245238), (-105.1263252377158 40.20680501554748, -105.1263252134739 40.20681968499972, -105.126325383258 40.20671719607243, -105.1263252377158 40.20680501554748), (-105.1155968517825 40.20318341103974, -105.1155968269777 40.20318946052415, -105.1155957253303 40.2034586936532, -105.1155968517825 40.20318341103974), (-105.1499563688645 40.20041626554917, -105.1499662706908 40.20210364514212, -105.1499562482724 40.20039565687276, -105.1499563688645 40.20041626554917), (-105.1499554011348 40.19980913608271, -105.1499554011414 40.19980913650229, -105.1499982009238 40.19982447013613, -105.1499554011348 40.19980913608271)), ((-105.083075148123 40.17192712109441, -105.0830780316235 40.17151508279193, -105.0830908276374 40.17077009335227, -105.0830898739331 40.16975794923593, -105.0830891382825 40.16941095828075, -105.0830899607455 40.16886796812796, -105.0830910643746 40.16868788974446, -105.0830930531922 40.16830494684462, -105.0830960976557 40.16792502758191, -105.0830959771383 40.16724395293009, -105.0830878765151 40.16693097503487, -105.0830950003841 40.16658593425269, -105.0831080505025 40.16650005739481, -105.0831190490881 40.16645699775201, -105.0831339771326 40.16641505106289, -105.0831478259643 40.16637392366613, -105.0831681144781 40.16633309328626, -105.0831919525168 40.16629694372924, -105.0832150677106 40.16626188854235, -105.0832439014171 40.16622795275293, -105.0833268254032 40.1661261315451, -105.0834260412004 40.16599307439358, -105.0834769351456 40.1659210605575, -105.0835000500647 40.16588600531175, -105.0835210296103 40.16584902129782, -105.0835398631979 40.16581202954788, -105.0835558587693 40.16577090983481, -105.0835711141966 40.16573390518737, -105.0835959221352 40.16565603140108, -105.083613938554 40.16557703616078, -105.0836220561698 40.16553698593949, -105.0836269525403 40.16549692411329, -105.0836300593452 40.16545713053579, -105.0836106635436 40.16484891209912, -105.0836030415373 40.16460987586909, -105.0836141587786 40.16413802271901, -105.0836161082395 40.16399500687811, -105.083609519032 40.16392308127849, -105.0881761464068 40.16392102833853, -105.0881693626968 40.16382478228903, -105.0881650625537 40.16356494168014, -105.0881668740553 40.16350208512876, -105.0881648387267 40.16306998948579, -105.0881598089886 40.16280928973737, -105.0881623938254 40.1623954782369, -105.0886809584908 40.16239212456986, -105.089468094328 40.16239711982808, -105.0909838252546 40.16238410086513, -105.0917190936679 40.16238697525812, -105.0925199158311 40.16237689791628, -105.0931070011848 40.1623778683723, -105.0931070004038 40.1623779989626, -105.0931050119728 40.16313991872316, -105.0931050114934 40.1631399988786, -105.0931040000302 40.16325199822559, -105.0931039998199 40.16329599907725, -105.0931469291512 40.16390871444782, -105.0931479999207 40.16392399940396, -105.0931480029145 40.16392408767742, -105.0931569991541 40.16423199918421, -105.0931259993862 40.16516199880555, -105.0931289999454 40.16569099842605, -105.0931319995954 40.16601699884203, -105.093122999789 40.1669069989264, -105.0931289996238 40.16735399928291, -105.0931369998561 40.16781299868737, -105.0931339988095 40.16872599950739, -105.0931369991391 40.16900499892864, -105.0931479994263 40.17023599850143, -105.0931500001353 40.17054199825319, -105.093151000261 40.17065999832266, -105.0931330003842 40.17149199908522, -105.0931459999594 40.17231399916508, -105.0930759995535 40.17368299823816, -105.093035999663 40.17395399970057, -105.093035412355 40.17395404356559, -105.0928751701174 40.17396600181887, -105.0928349994319 40.17396899906539, -105.0920962144237 40.17397699684266, -105.0920961416262 40.17397699748644, -105.0920959995587 40.17397699788575, -105.0899358508228 40.17397797709733, -105.0898870002667 40.17397799833534, -105.0892635502055 40.17397922794395, -105.0888742073944 40.17397999371771, -105.0883123178483 40.17397704920117, -105.0883031426125 40.17397700121329, -105.0883029993709 40.17397700160376, -105.088302814376 40.1739809907825, -105.0830771458684 40.17399043991578, -105.0830771760332 40.1739901157939, -105.0830749017534 40.17371888591792, -105.0830759771914 40.17348500237775, -105.0830810478255 40.17329999660924, -105.083080876397 40.17274410150467, -105.083075148123 40.17192712109441)))</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>15</v>
-      </c>
-      <c r="E12" t="n">
-        <v>15</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Longs Peak MS</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1500 14th Ave, Longmont, CO 80501</t>
+        </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Longs Peak MS</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1500 14th Ave, Longmont, CO 80501</t>
+          <t>http://lpms.svvsd.org/</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
+          <t>Longs Peak Middle School</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>40.18399195721774</v>
+      </c>
+      <c r="K12" t="n">
+        <v>-105.117518880356</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
           <t>http://lpms.svvsd.org/</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Longs Peak Middle School</t>
-        </is>
-      </c>
-      <c r="L12" t="n">
-        <v>40.18399195721774</v>
-      </c>
-      <c r="M12" t="n">
-        <v>-105.117518880356</v>
-      </c>
       <c r="N12" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
-        </is>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>http://lpms.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
         <is>
           <t>POINT (-105.117518880356 40.18399195721774)</t>
         </is>
@@ -1312,59 +1236,53 @@
           <t>POLYGON ((-105.1310483121341 40.12350602835088, -105.1310413121898 40.12134002807184, -105.131030312504 40.11993502837323, -105.1310243109556 40.11903302886184, -105.1310173108496 40.11649802904655, -105.1310173105552 40.11642102922118, -105.1310173486831 40.11641334503174, -105.131018259415 40.11641262021929, -105.1310181860247 40.11642745992815, -105.1311001857065 40.11641745990186, -105.1311361855693 40.11640146052148, -105.1311941855785 40.11632246004667, -105.1312731862733 40.11603745969056, -105.1313421735774 40.11588122329221, -105.1313536700491 40.11585518628547, -105.1314091855054 40.11572946035969, -105.1314881866388 40.11547746041233, -105.1315867964692 40.11541012927728, -105.1316741852191 40.11535046009578, -105.1317241867259 40.115191460073, -105.1318891858139 40.11515346003952, -105.1322901860955 40.11511545933612, -105.1322751860538 40.11537845966455, -105.1323321866405 40.11548845960182, -105.1323543636915 40.11550215156709, -105.1324471863394 40.11555946059213, -105.1326261859337 40.11553245951755, -105.1327901954493 40.11544179157702, -105.1330331862589 40.1153074606795, -105.1331191859966 40.11521445939096, -105.1331411856992 40.11488445961638, -105.133234186949 40.1147304599069, -105.1333340990247 40.11463557074746, -105.1334131856659 40.11456046023817, -105.1335362178282 40.11456046070084, -105.1336711859251 40.11456046016362, -105.1338501858913 40.11461045973502, -105.1342361863052 40.11481945914035, -105.134329186555 40.11493445989868, -105.1344361864871 40.11494046008041, -105.1346221871356 40.11477045999761, -105.1346861864186 40.1145994604477, -105.1347221866439 40.11440245982309, -105.1350148427649 40.11403187214655, -105.1350602254513 40.11397440482906, -105.1350801857764 40.1139464596064, -105.135182139388 40.11393135543081, -105.1352747246668 40.11399622867296, -105.1353697140693 40.11414098052226, -105.1354881867362 40.1143364596393, -105.1356101869878 40.11439745989412, -105.1357101866312 40.1143694590412, -105.1357961873731 40.11427645936892, -105.1357961869385 40.11416645986762, -105.1357461861792 40.11397446007563, -105.135839187088 40.11381545968592, -105.135989187307 40.11374945946562, -105.1360886500456 40.11374159503977, -105.1362041868162 40.11373245991339, -105.1363067782619 40.11374563253825, -105.1364611865636 40.11376545914218, -105.136647186488 40.11372745988353, -105.1367132737641 40.1136867910588, -105.1367901873759 40.11363945994061, -105.1368346130924 40.11357172155405, -105.1368911870444 40.11348545902928, -105.136926249788 40.11333338529389, -105.1369771870886 40.1131124602168, -105.1369701872679 40.11299745903131, -105.1369049964273 40.11285831592468, -105.1368341870956 40.11272245868071, -105.1367911864023 40.11260145944513, -105.1366771874476 40.11241445906841, -105.1367061863406 40.11229345931134, -105.1368491873511 40.11220045890114, -105.1369921868139 40.11221745873338, -105.1371491860115 40.11229945967833, -105.1373141862809 40.11240445921667, -105.1373815568126 40.11239409447652, -105.137381607722 40.11239400637307, -105.1374571875025 40.11238245959723, -105.1375501870297 40.11229945883865, -105.1375851861427 40.11219045989127, -105.1375783082322 40.11213281406475, -105.1375641863439 40.11201445996381, -105.1375291873222 40.1118764593884, -105.1375931871308 40.11181145885294, -105.1378641325305 40.11172992844479, -105.1379221864662 40.11171245960098, -105.1380043977404 40.11165544251909, -105.1381346354642 40.11156511596145, -105.1383520505958 40.11141634734895, -105.1385021871975 40.1113174589991, -105.1385885373203 40.11121663711587, -105.1386811865493 40.11110845948276, -105.1387881878956 40.11089445929716, -105.1388881875843 40.1108174596417, -105.1391321875739 40.11077945940796, -105.1392166376191 40.11076175266201, -105.1392452612604 40.11075575100678, -105.139318187819 40.11074045974925, -105.1393678994795 40.11072429438088, -105.1395584243935 40.11066233928282, -105.1396041866986 40.11064745841755, -105.139761662953 40.11061060263292, -105.139933186621 40.11057045894069, -105.1401831872421 40.11054845896744, -105.1402242919559 40.11052569800182, -105.1402249272183 40.11052579274737, -105.1403254691414 40.11047119351303, -105.1404621873911 40.11037345868738, -105.1406051874184 40.11035645826706, -105.1406771869243 40.11047245857907, -105.1407334051194 40.11062448513666, -105.1407481874379 40.11066445856965, -105.140834187162 40.11075245890581, -105.1409411875114 40.11075745877094, -105.1411311766261 40.1106291019769, -105.1413141878553 40.1105054587965, -105.1413481734702 40.11044279920952, -105.1413941070261 40.11035810907864, -105.1414421879518 40.11026945914983, -105.1414707361548 40.11017746660836, -105.1414781867133 40.11015345869473, -105.1415522170272 40.11016179340662, -105.1416291874734 40.11017045872525, -105.1416791872043 40.11020345863564, -105.1417791876447 40.11018145895183, -105.1418291878365 40.11010445836963, -105.1418291876094 40.11005455446081, -105.1418291868519 40.10988545812238, -105.1418336763905 40.10988134348353, -105.1419011880146 40.10981945778273, -105.1419941874593 40.10979745872118, -105.1420791878335 40.10989045903131, -105.1420893355731 40.10999193837458, -105.142101188436 40.11011045872333, -105.142126431106 40.11012005767923, -105.1421721882141 40.11013745854567, -105.1423603463296 40.11012042383983, -105.142415188456 40.11011545817529, -105.1424617281768 40.1101221067335, -105.1425371920236 40.11013288780438, -105.1425655734614 40.11013694209405, -105.1425889933667 40.11014028752435, -105.1426306946563 40.11014624465503, -105.142676579207 40.11015280013385, -105.142723188132 40.11015945870771, -105.1428108591608 40.11016490951189, -105.1429161884725 40.11017145869828, -105.1429648250731 40.11017641491812, -105.1429648182534 40.11017771543015, -105.1429664300369 40.11017657839365, -105.1430731876633 40.11018745855665, -105.1431521881496 40.11013245795137, -105.1431796482247 40.11002829750333, -105.1432101875002 40.10991245887465, -105.1433101881548 40.10983045861817, -105.1433261756351 40.10975684233937, -105.143353188753 40.10963245825586, -105.1433382934257 40.10957753407826, -105.143311550045 40.10947891718003, -105.1432891876009 40.10939645879092, -105.1432609860456 40.10935610828796, -105.1432241877329 40.10930345901374, -105.1432328627724 40.10926008276815, -105.143246187286 40.10919345809153, -105.1433391874849 40.10910545859052, -105.1434139958149 40.10909877173545, -105.1435181878683 40.10908945828713, -105.1436391882093 40.10914945901379, -105.1437251880138 40.10919945804216, -105.1438211598157 40.10919242101242, -105.1438751876574 40.10918845906782, -105.1439693495291 40.10914216706989, -105.1440541880079 40.10910045846919, -105.144096572717 40.10909719816408, -105.144123205141 40.10909515020784, -105.1441548387739 40.1090927168681, -105.1441971870977 40.10908945911586, -105.1442691886938 40.10915545782236, -105.144345777039 40.10927439618445, -105.1443541882314 40.10928745804113, -105.1444693672245 40.10929912209676, -105.1444797799127 40.10930245231871, -105.1444972586797 40.10930194682363, -105.1446208477053 40.10929837426536, -105.1447756584748 40.10929241273082, -105.1448795350452 40.10928805784319, -105.1450518589718 40.10928083304527, -105.145156188375 40.1092764585858, -105.1452858210533 40.10929371331622, -105.1454491885845 40.10931545852137, -105.1456711885987 40.10930945796668, -105.1457684551437 40.10927877952781, -105.1459173643046 40.10923181175473, -105.1459501886296 40.1092214585894, -105.14603607745 40.10920312262454, -105.1461281887017 40.10918345829599, -105.1462641887339 40.10909045812184, -105.1463979289381 40.10907882875447, -105.1465861886723 40.10906245846613, -105.1466952183154 40.10908102655211, -105.146815189195 40.10910145810936, -105.1469201518979 40.10911105121482, -105.1470011879937 40.10911845817668, -105.1470486443322 40.10911952728623, -105.1471561250959 40.10912194792165, -105.1472231888622 40.10912345873804, -105.1472670149087 40.10914467042698, -105.1473230421344 40.10917178706982, -105.1474308225596 40.10922395285124, -105.1474731885267 40.10924445749985, -105.1475425064825 40.10924445742264, -105.1476126056347 40.10924445788622, -105.1476639806363 40.10924445792431, -105.1477521893066 40.10924445771168, -105.1478568619915 40.10927209172333, -105.1480021884751 40.109310458268, -105.1481495371838 40.10931457831904, -105.1483626110154 40.10932053569708, -105.1484881807936 40.10932404681184, -105.1486101887807 40.10932745778867, -105.148681535631 40.10935141047885, -105.1486906073675 40.10935551079681, -105.1487742892276 40.10938470218268, -105.1488282710606 40.10942647438896, -105.1489321887245 40.1095144583186, -105.1489961900791 40.10967345746549, -105.1490951105112 40.10978119433448, -105.1491636738781 40.10981642606204, -105.1492181885192 40.10984345882783, -105.1493760472449 40.1098539470783, -105.1495327897234 40.10986436057436, -105.1498051887075 40.10988245858211, -105.1499037995298 40.10983605366251, -105.1500261889393 40.10977845814232, -105.1500616825502 40.10974049989558, -105.1500969366913 40.10970279759637, -105.1501310738441 40.10966628976156, -105.1501701894573 40.10962445796797, -105.150213190036 40.10948145755771, -105.150192927634 40.10942765734119, -105.1501841896918 40.10940445815319, -105.1501460270222 40.10937066109187, -105.150113914031 40.10934222227647, -105.150035810524 40.10927305377975, -105.1499481896146 40.10919545785707, -105.1499411886424 40.10911345803316, -105.1500271894042 40.10901445758356, -105.1501361731898 40.10894852276716, -105.1501628272604 40.1089323972873, -105.1501829687099 40.10892021131422, -105.1501990355049 40.1089104906731, -105.150216358927 40.10890001008798, -105.1502271897408 40.1088934573679, -105.1502991895659 40.10876745797281, -105.1503701892914 40.10874045812216, -105.1505561895843 40.10874045817922, -105.1507351896093 40.10865745754312, -105.1509501898016 40.10867945738578, -105.1510291895926 40.10873445721234, -105.1511498943537 40.108892914989, -105.1512721889252 40.10905345792743, -105.151443190266 40.10915745838717, -105.1515425217955 40.10915797339747, -105.1516361903776 40.10915845863114, -105.152058189739 40.10899345806407, -105.152168642065 40.10888557367066, -105.1521720437602 40.10888555509551, -105.1521871900507 40.10886745719991, -105.1522441899349 40.10883445806299, -105.1522521895131 40.10872445833751, -105.1522161898024 40.10867445774499, -105.1519151896514 40.1086254581982, -105.1518011892207 40.10854845784844, -105.1518081899357 40.10844445794176, -105.1520521905081 40.10809245803009, -105.1521161891182 40.10785645730169, -105.1522381891769 40.1078014575306, -105.1526961899649 40.10774645807478, -105.1530101897713 40.1076424577811, -105.1531681905297 40.10752745787505, -105.1532041904084 40.10742245698562, -105.1531971895655 40.10730745767818, -105.1530821895656 40.10724745707277, -105.1527891896304 40.10716445739909, -105.1527461895664 40.10708745705721, -105.1528251898034 40.10689545706076, -105.1528251894787 40.1068184572149, -105.1529611896807 40.10678045703483, -105.1532181895994 40.10680245729557, -105.1534041890178 40.10683545695765, -105.153533190452 40.10679645699769, -105.1536831893247 40.10669845729011, -105.1538481902248 40.10664345777509, -105.1543781900811 40.10669245702027, -105.1546631906193 40.10667645674386, -105.1549851905804 40.10658345749179, -105.1551071895624 40.106484457227, -105.1551781906975 40.10638545677693, -105.155372190027 40.10630845692795, -105.1557151895679 40.10621545706669, -105.1564161904518 40.10613345690832, -105.1565797245652 40.10604856929712, -105.1569951900118 40.10582045723518, -105.157138190582 40.10579245659894, -105.157239191129 40.10571045628147, -105.157253190884 40.10562845707536, -105.1571241900853 40.10546345672344, -105.1571241898577 40.1053754563856, -105.1572321903226 40.10529845652795, -105.1576681914213 40.10507845747404, -105.1580761909817 40.10495245717316, -105.1581892413284 40.10490396872007, -105.1584981900914 40.10477145654381, -105.1587201908592 40.10476045668218, -105.1588991905787 40.10458445709242, -105.1589061910858 40.10450845692532, -105.1588201907179 40.10434845704976, -105.1588411915942 40.10426645671227, -105.1590781918603 40.10400245670831, -105.1594259918098 40.10399197542836, -105.1594495599439 40.10886022285561, -105.1594520114176 40.10922888777313, -105.1594718259507 40.11205812132699, -105.159467921669 40.11419687283805, -105.1594566443818 40.11609286922273, -105.1594641412873 40.11689641328065, -105.1609821531084 40.11566321114483, -105.1614528663692 40.11528080007928, -105.1674439177613 40.11003576716704, -105.1685799278165 40.10901976085416, -105.1688417643584 40.10884061707407, -105.1763019499671 40.1023029683946, -105.1770289540793 40.10167497796913, -105.1842254973132 40.09480566330672, -105.1842981568986 40.09474644455597, -105.1847611298219 40.09436911199498, -105.1847691909817 40.09436254127205, -105.1851806430128 40.0943560507158, -105.1851823083869 40.09435602463465, -105.1864923089405 40.09436502536359, -105.1869288298045 40.09436799308698, -105.1869333094328 40.09436802324625, -105.1878489982433 40.09436703406432, -105.1878583084638 40.09436702410904, -105.1878579783739 40.09437328631103, -105.1878581437286 40.09437328585741, -105.1878581347478 40.09437345425398, -105.1878554742897 40.09442402015232, -105.1878551441828 40.09443028595678, -105.1914201445046 40.09443828540665, -105.1941921454042 40.0944432846204, -105.1961591443175 40.09444728514715, -105.1999431444402 40.09446928464906, -105.20004901646 40.0944713051883, -105.2000942419318 40.09447216840297, -105.2004028346573 40.09447194731246, -105.2020925487541 40.09447072187066, -105.204067954345 40.09447526321931, -105.206084292794 40.09448027846468, -105.2067696857456 40.09448197611559, -105.206769231588 40.09440878489543, -105.2067688747363 40.09435139755085, -105.2069082004758 40.09435075068787, -105.2069747075104 40.09435044215074, -105.2069438669998 40.08890529265857, -105.2069481319076 40.08890527106102, -105.2075245971012 40.08890693460845, -105.208456199712 40.08891645102268, -105.2093902465011 40.08891684883024, -105.2102848781325 40.08891722213826, -105.2102854292613 40.08891722262064, -105.2102871823232 40.08891722341717, -105.2102892648914 40.08891722413985, -105.2102906849293 40.08891722500127, -105.2114362013246 40.08891745132185, -105.213437201397 40.08892445097817, -105.2143002021996 40.08892245043239, -105.2148042021617 40.08892745043244, -105.2148588360544 40.08892679371123, -105.2159742024865 40.08892045011142, -105.2162802020392 40.08892045046189, -105.2163292022599 40.08892045018143, -105.216360202134 40.08892145040806, -105.2163692023297 40.08714545077098, -105.2182532019159 40.08714945059754, -105.2182432027494 40.08641344971119, -105.2191138039488 40.0864074176304, -105.2211262032423 40.08639345027048, -105.2211162029895 40.08627444986659, -105.2219812039535 40.08618344991433, -105.2230462031982 40.08603244956893, -105.2246852045713 40.08554044892636, -105.2246712037403 40.08611344976358, -105.2258422045073 40.08612344890279, -105.2258472562248 40.08702557574974, -105.2258472559384 40.08702564690012, -105.2258442047025 40.08817345056035, -105.2258660799562 40.08846674914248, -105.225866596984 40.08846589835929, -105.2259971464311 40.08825128178296, -105.2260951784236 40.08815046645809, -105.2260799511012 40.08815043483378, -105.2260289772142 40.08815032829153, -105.2260301833774 40.08814810745953, -105.2260316128055 40.08814547826421, -105.2260330445643 40.08814285267693, -105.2260344868726 40.08814022801536, -105.226035930357 40.08813760245592, -105.2260373773409 40.08813498140795, -105.2260388290152 40.08813236037112, -105.2260402865523 40.08812973934819, -105.2260417429166 40.08812711832244, -105.2260432086508 40.08812450002085, -105.2260446767192 40.08812188442674, -105.226046152992 40.08811926975269, -105.2260476280957 40.08811665417521, -105.2260491125655 40.08811404222255, -105.2260505993841 40.08811142937476, -105.2260520885404 40.08810881833376, -105.2260535823798 40.08810620910523, -105.2260550832546 40.0881035998933, -105.2260565841257 40.08810099158206, -105.2260580920141 40.08809838779062, -105.2260596034202 40.08809578400751, -105.2260611230379 40.08809317934323, -105.2260626414721 40.08809057737804, -105.2260641669416 40.08808797542954, -105.2260656970834 40.08808537799534, -105.2260672295774 40.08808277876541, -105.2260687690924 40.08808018315465, -105.2260703097799 40.08807758754672, -105.2260718574956 40.08807499375673, -105.2260734087289 40.088072399975, -105.2260749611275 40.0880698079974, -105.2260765193853 40.08806721693423, -105.226078084664 40.08806462949036, -105.2260796499462 40.0880620411458, -105.2260812222603 40.08805945371852, -105.2260827980811 40.08805686900151, -105.2260843809301 40.08805428610243, -105.2260859637863 40.08805170140207, -105.2260875536562 40.08804912212216, -105.2260891482163 40.08804654285341, -105.2260907451214 40.08804396359018, -105.2260923455334 40.08804138703718, -105.2260939506355 40.08803881049528, -105.2260955615934 40.08803623576855, -105.2260971760652 40.08803366195077, -105.2260987916986 40.08803109083762, -105.2261004178852 40.08802851974954, -105.2261020440572 40.08802595226398, -105.2261036725816 40.08802338298269, -105.2261053092994 40.08802081732343, -105.2261069495313 40.08801825257306, -105.2261085932736 40.08801568963229, -105.2261102405372 40.08801312579922, -105.2261118948289 40.0880105637841, -105.2261135491024 40.08800800627216, -105.2261152092496 40.08800544607216, -105.2261168764069 40.08800289219328, -105.226118542406 40.08800033470907, -105.2261202165914 40.08799778264812, -105.2261218943052 40.08799522789362, -105.2261235755077 40.08799268035245, -105.2261252602387 40.08799013011774, -105.226126950829 40.08798758079754, -105.2261286460914 40.08798503599166, -105.2261303460513 40.08798248939556, -105.2261320460038 40.0879799446007, -105.2261337541534 40.08797740252725, -105.2261354658207 40.08797486046209, -105.2261371809875 40.08797232290842, -105.2261388996683 40.08796978626372, -105.2261406218776 40.08796724692545, -105.2261423475865 40.08796471209865, -105.2261440803236 40.08796217908979, -105.2261458165711 40.08795964789051, -105.2261475563434 40.08795711489833, -105.226149300777 40.08795458912228, -105.2261510475738 40.08795205884863, -105.2261528013842 40.08794953399544, -105.2261545551981 40.08794700824161, -105.2261563172056 40.08794448610973, -105.2261580815545 40.08794196488402, -105.2261598505936 40.08793944366944, -105.2261616231395 40.08793692516508, -105.2261634015482 40.08793440667458, -105.2261651799496 40.08793188998534, -105.2261669688859 40.08792937782427, -105.2261687566533 40.08792686475982, -105.2261705502725 40.0879243544111, -105.226172348582 40.08792184407345, -105.2261741480568 40.08791933553987, -105.2261759557322 40.08791682882699, -105.2261777645729 40.08791432391816, -105.2261795792655 40.08791182172511, -105.2261813974722 40.08790932044101, -105.2261832203618 40.08790682096924, -105.2261850455965 40.08790432150305, -105.2261868778629 40.08790182295415, -105.2261887112837 40.08789932891115, -105.2261905517435 40.08789683398418, -105.2261923945412 40.08789434086405, -105.2261942361589 40.08789184954237, -105.226196091833 40.08788936185654, -105.226197947507 40.08788687417072, -105.2261998043462 40.08788438828893, -105.2262016682208 40.08788190242377, -105.226203534426 40.08787942016669, -105.2262054064867 40.08787693972477, -105.2262072808852 40.08787446108968, -105.2262091611538 40.08787198066713, -105.2262110437421 40.0878695065546, -105.2262129298625 40.08786702884783, -105.2262148218203 40.0878645574594, -105.2262167161233 40.08786208607652, -105.2262186162781 40.08785961740938, -105.2262205211268 40.08785714785272, -105.226222428306 40.08785468190413, -105.2262243401755 40.08785221596659, -105.2262262543791 40.08784975273657, -105.2262281732657 40.08784729131887, -105.2262300991841 40.08784483081848, -105.226232023919 40.08784237301715, -105.2262339568581 40.08783991613592, -105.2262358933076 40.08783746106425, -105.2262378332675 40.08783500780219, -105.2262397767451 40.08783255454839, -105.2262417237222 40.08783010580613, -105.2262436742169 40.08782765707216, -105.2262456270494 40.08782521014498, -105.2262475892516 40.08782276594194, -105.2262495549714 40.08782032174722, -105.2262515195077 40.08781788025156, -105.2262534898923 40.08781544237237, -105.2262554673158 40.08781300360911, -105.226257445901 40.08781056755058, -105.2262594326977 40.0878081306108, -105.2262614183 40.08780569907206, -105.2262634085889 40.08780326844501, -105.2262654059096 40.08780083873525, -105.2262674008741 40.08779841172184, -105.2262694052227 40.08779598382996, -105.2262714142507 40.0877935586511, -105.2262734244331 40.08779113797818, -105.2262754393057 40.08778871731626, -105.2262774576886 40.08778629846402, -105.2262794831069 40.0877838796284, -105.2262815085034 40.08778146619655, -105.2262835374175 40.08777905277302, -105.2262855745432 40.08777663846826, -105.2262876128304 40.08777422686813, -105.2262896569624 40.08777181978507, -105.226291699918 40.08776941359987, -105.2262937499053 40.08776700833194, -105.2262958045756 40.08776460487633, -105.2262978662741 40.08776220323865, -105.2262999267926 40.08775980339941, -105.2263019919905 40.08775740627321, -105.2263040642092 40.08775501276614, -105.2263061352625 40.08775261745505, -105.2263082145056 40.08775022666651, -105.2263102972735 40.08774783408501, -105.2263123800232 40.08774544600666, -105.226314467456 40.08774305974064, -105.2263165619241 40.08774067349134, -105.2263186598953 40.08773829085281, -105.2263207637256 40.08773590912882, -105.226322866376 40.08773352920324, -105.2263249737094 40.08773115109006, -105.2263270845495 40.0877287756871, -105.2263292047701 40.08772640030627, -105.2263313249726 40.08772402942868, -105.226333448689 40.08772165945994, -105.2263355759121 40.08771929220145, -105.2263377078255 40.08771692495404, -105.2263398455944 40.08771455952174, -105.2263419810035 40.08771219768641, -105.2263441269622 40.08770983677667, -105.2263462740824 40.08770747857164, -105.2263484247239 40.08770511947421, -105.2263505776958 40.08770276398484, -105.2263527353471 40.08770041120849, -105.226354900023 40.08769806115065, -105.2263570647023 40.08769571019219, -105.2263592363989 40.0876933637535, -105.2263614080953 40.08769101731477, -105.2263635879888 40.08768867359738, -105.2263657702201 40.0876863316868, -105.2263679524405 40.08768399247809, -105.2263701416961 40.08768165328597, -105.2263723344585 40.0876793168041, -105.2263745307277 40.0876769830324, -105.2263767305145 40.08767464926904, -105.2263789361496 40.08767231912204, -105.2263825065714 40.08766855838156, -105.2263977138776 40.0876481506639, -105.2264158800905 40.08762967283475, -105.226434455812 40.08761141663134, -105.2264521500162 40.08759367350561, -105.2264697795498 40.08757626436348, -105.2264878009205 40.08755909752002, -105.2265062070929 40.08754217295839, -105.226524998038 40.0875254978835, -105.2265441631842 40.08750907677334, -105.2265637001611 40.08749291592657, -105.22658359957 40.0874770198241, -105.2266038602236 40.08746139206541, -105.2266244715363 40.08744604073107, -105.2266454253037 40.08743096490092, -105.2266667226549 40.08741617538511, -105.2266883530404 40.08740167125784, -105.2267103070542 40.08738745880117, -105.2267325834878 40.08737354701852, -105.2267551729715 40.08735993318564, -105.226778067272 40.08734662358735, -105.2268012569799 40.08733362540633, -105.2268247444441 40.08732093774738, -105.2268485155578 40.08730856958332, -105.2268725621166 40.08729651999401, -105.226896880574 40.08728479617606, -105.2269214580284 40.08727339899931, -105.2269223132005 40.08727301824765, -105.2269462956309 40.08726233387031, -105.2269713781346 40.08725160165343, -105.226995713506 40.08724120810847, -105.2270202222304 40.08723115271041, -105.2270449570381 40.08722144459034, -105.227069908556 40.08721208192462, -105.2270950662131 40.08720306919137, -105.2271204311677 40.08719440999577, -105.2271459834793 40.08718610609185, -105.2271717266588 40.08717815928905, -105.2271977580158 40.08717057341977, -105.2272236163383 40.08716344466387, -105.2272444844378 40.08716355701311, -105.2272912108504 40.08716386193717, -105.2280258931392 40.08716865993154, -105.2283729549368 40.08717092525384, -105.229337317657 40.08728913118895, -105.2315411374752 40.08755923148525, -105.2315951034686 40.08756556421094, -105.2316492191852 40.08757169551478, -105.2317034632943 40.08757708676092, -105.2317578193674 40.08758174061293, -105.2318122651521 40.08758564981383, -105.2318667865754 40.08758881433079, -105.2319213672231 40.08759123322496, -105.2319759906559 40.08759291186197, -105.2320306369806 40.0875938393878, -105.2320852944376 40.08759402388102, -105.232139950141 40.08759346170912, -105.2321945759326 40.08759215640933, -105.2322491612788 40.08759010255342, -105.2323036897474 40.08758730370593, -105.2323581460858 40.0875837616329, -105.2324125138727 40.08757947719696, -105.2324667696581 40.08757444944327, -105.2325209052109 40.08756868375681, -105.2325748982646 40.08756217648359, -105.2326288764451 40.08755497475301, -105.2326832836757 40.08754720298132, -105.232737453437 40.08753868580036, -105.2327913728077 40.08752942858451, -105.2328450159892 40.08751943127434, -105.232898377103 40.08750869745924, -105.2329514268327 40.08749722707182, -105.2330041639691 40.08748502911613, -105.2330565603615 40.08747210532881, -105.2331086089517 40.08745846109794, -105.2331195646996 40.08745541432238, -105.233160289808 40.08744409547717, -105.2332115864704 40.0874290192368, -105.2332572252643 40.08741486387087, -105.2333106562827 40.0873970203308, -105.2333632162177 40.08737853169327, -105.2334153508784 40.08735934044687, -105.2334670391323 40.08733945284803, -105.2335182680553 40.08731887517195, -105.2335350154684 40.08731185997121, -105.2335198087319 40.087300620841, -105.2334842065225 40.08728144947539, -105.233557508418 40.08725212883198, -105.2336642062275 40.0872094484582, -105.2337498879304 40.08716518662143, -105.2338752055783 40.08710044895112, -105.2340141176357 40.08701357127359, -105.2340547143473 40.08698818193187, -105.234116919408 40.08694927681879, -105.2341742062996 40.08691344866173, -105.2342102060382 40.08689144861766, -105.2342874907976 40.08682176614175, -105.2344114016713 40.08671004247304, -105.2346296381483 40.08650825210744, -105.2347532059639 40.0863524487831, -105.2349272055709 40.08608544943124, -105.2351162069385 40.08560644881669, -105.2351382054217 40.08551144874158, -105.2350852057845 40.0846124484227, -105.2350776389745 40.08420165278985, -105.2350497203358 40.08268589163298, -105.2350032064051 40.08016044862552, -105.2299052044168 40.08008044876753, -105.2334432055741 40.07899144749057, -105.2352892054144 40.07873844737262, -105.2366591894632 40.0785191707074, -105.2370786377037 40.07845203165877, -105.2378132062725 40.07833444783447, -105.2384812068036 40.07833244791702, -105.2403432064991 40.07833344770941, -105.2422160069221 40.0783371534334, -105.2423652076105 40.07833744689923, -105.2435522068469 40.07833844725607, -105.2446880588089 40.07833844686491, -105.2446880583013 40.07833920790986, -105.245048207299 40.07833944731037, -105.2453581543005 40.07833797981056, -105.2453582656843 40.07833797915564, -105.2467352086361 40.07833144715077, -105.2479762077927 40.07832544680577, -105.2505104677892 40.07831279674013, -105.2509901360399 40.07831039739476, -105.2509912135285 40.07831039161324, -105.2528018115011 40.07830197852396, -105.2528020506824 40.07830197723486, -105.2552788447606 40.07829042246069, -105.2603639449122 40.0782650686866, -105.2610523420133 40.07826161962124, -105.2611378514393 40.07826119045901, -105.263475212196 40.07824944591677, -105.2635022120304 40.08020744623987, -105.265906623877 40.08014227963445, -105.2678107184368 40.08009626548748, -105.269120467453 40.08006436083225, -105.270773469619 40.08002883906712, -105.271602868858 40.08001390036796, -105.2722111865051 40.0800029400344, -105.2732488422515 40.07998423568615, -105.2738472151207 40.07997344533944, -105.2741904007602 40.07997698391911, -105.2752363556628 40.07998199733333, -105.2752365174616 40.07998199764835, -105.2752366651909 40.079981997936, -105.2752368011957 40.07998199820081, -105.275236925476 40.07998199844278, -105.2752370110651 40.07998199860944, -105.2760592152198 40.07997644544199, -105.2774492150437 40.079994445459, -105.2774442150245 40.07989344467622, -105.2775032146846 40.07989444554472, -105.277486220627 40.07914765992864, -105.277462332525 40.07819215800942, -105.2774232152314 40.07679644423713, -105.2774182151642 40.07662844439344, -105.277414215237 40.07647944379102, -105.2774795717141 40.0764360956394, -105.2776022148752 40.07633644500343, -105.2777612150901 40.07620044483633, -105.2779022152453 40.07603844420503, -105.2780202147794 40.07579044515734, -105.2783742148064 40.07579144511136, -105.278372214492 40.07653744417692, -105.2782532143109 40.07666244408787, -105.2821112161553 40.07666744386643, -105.2821342160606 40.0791254445771, -105.2822223466844 40.07989150774977, -105.2822036751846 40.07998723360745, -105.2822148038009 40.07998772474011, -105.2822150312255 40.07998773507623, -105.2823430660183 40.07999338222898, -105.2823919994679 40.07989699918794, -105.2823952780968 40.07991484894792, -105.2823021518433 40.08009827885829, -105.2822277607727 40.08031775722681, -105.2821622666328 40.08051098862354, -105.2821612415979 40.08051401375702, -105.2821593066155 40.08068901713151, -105.2821463073063 40.08169901632542, -105.2821403062932 40.0821320170198, -105.2821423070911 40.08263701682382, -105.2821423075853 40.08554501716329, -105.2821623079241 40.08608101577435, -105.2821621432272 40.08608704978086, -105.282162143671 40.08608727764472, -105.2821423153658 40.0868150166831, -105.2821421522846 40.08682127765446, -105.2821479765674 40.08702801532603, -105.2821481523551 40.0870342787379, -105.2821390907224 40.08703424902927, -105.2821441072337 40.08721088474018, -105.282137898842 40.0899340794033, -105.2821399488127 40.09152792746865, -105.2821341594649 40.09311407433201, -105.2821409624091 40.09422807602022, -105.2821221684136 40.09529810758003, -105.2821321056455 40.09710801302935, -105.2821051272783 40.09794304108583, -105.2820501495957 40.09926089139519, -105.282012830953 40.09975193069047, -105.2819761427939 40.10038105317948, -105.2819768350256 40.10072310238548, -105.2819774149438 40.10073831713714, -105.2819782232338 40.10075949547533, -105.2819900265868 40.10106901821791, -105.2819991328603 40.10135096358122, -105.2820498498076 40.10248206645011, -105.2821380164751 40.10397587712918, -105.2821500312105 40.10435500626381, -105.2821711087647 40.10503008189505, -105.2821721304822 40.10538091547843, -105.2821429877803 40.10588597033826, -105.2821100589534 40.10623289769167, -105.2820620998125 40.10658501047332, -105.2820240687228 40.10696212396728, -105.2818538952916 40.10852407589721, -105.28182207568 40.10885892394143, -105.2818161192508 40.10960202947805, -105.2818530515338 40.11001497049595, -105.281895999471 40.11033596102865, -105.282007019785 40.11112595402247, -105.2820288722131 40.11126901713702, -105.2820480529635 40.1114200377739, -105.2821319186914 40.11202687618564, -105.2822329804653 40.1128470466918, -105.2822851112858 40.11342801985863, -105.2822921703681 40.1144629590239, -105.2822860850855 40.11569497494339, -105.2822928240271 40.11638292419469, -105.2822928495963 40.11704588145643, -105.28230101788 40.11773410707254, -105.282302930207 40.11847804797252, -105.2823001360619 40.11979901308963, -105.2823039641844 40.12106206847565, -105.2822998880501 40.12211290531759, -105.2823098954699 40.12368013430066, -105.2823120718964 40.12389398635925, -105.2823138398862 40.12412403384995, -105.2823129161732 40.12418909163625, -105.2823108265935 40.12473098201075, -105.2823120082232 40.12503212758082, -105.2823139370068 40.12565912601642, -105.2823230762417 40.12615601536589, -105.2823149319752 40.12680193517511, -105.2823240983905 40.12807295927798, -105.2823100945402 40.12932087953102, -105.2823079566542 40.1295421346564, -105.2823048796789 40.12994511718988, -105.2823158253697 40.13054797525448, -105.2823018622755 40.13100007518779, -105.28227995875 40.13192213067715, -105.282278130057 40.13238193944374, -105.2822721443784 40.13369411122954, -105.2822869464721 40.13488086839918, -105.2822871155677 40.13605798978642, -105.2822808526307 40.13667399035533, -105.2822689487237 40.13804709279694, -105.2822731345116 40.13942187166376, -105.2822709455559 40.14021796128176, -105.2822679484925 40.14104287330215, -105.2822708529094 40.14181206938772, -105.2822551592731 40.14347505101375, -105.2822531667241 40.14398591947473, -105.2822421489368 40.14497003421873, -105.2822411001326 40.14507407386814, -105.2822446</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>17</v>
-      </c>
-      <c r="E13" t="n">
-        <v>17</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Lyons Middle Senior</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>100 McConnell Dr, Lyons, CO 80540</t>
+        </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Lyons Middle Senior</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>100 McConnell Dr, Lyons, CO 80540</t>
+          <t>https://lmshs.svvsd.org/</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
+          <t>Lyons Middle/Senior High School</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>40.2147599852984</v>
+      </c>
+      <c r="K13" t="n">
+        <v>-105.264461148759</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
           <t>https://lmshs.svvsd.org/</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Lyons Middle/Senior High School</t>
-        </is>
-      </c>
-      <c r="L13" t="n">
-        <v>40.2147599852984</v>
-      </c>
-      <c r="M13" t="n">
-        <v>-105.264461148759</v>
-      </c>
       <c r="N13" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
-        </is>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>https://lmshs.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
         <is>
           <t>POINT (-105.264461148759 40.2147599852984)</t>
         </is>
@@ -1384,59 +1302,53 @@
           <t>MULTIPOLYGON (((-105.1784019212843 39.92870168376908, -105.1818511117197 39.92869648384348, -105.1838441764116 39.92869343178848, -105.1841991763519 39.92873643054561, -105.1843711756133 39.92868243090511, -105.1846711757492 39.92865043161049, -105.1848971762652 39.92868243096175, -105.1851551757211 39.92870443083596, -105.1853591757001 39.92871443082796, -105.185584175611 39.92863943112477, -105.1857881765031 39.92869343037078, -105.1860781767717 39.92871443107489, -105.1862427122102 39.92871305375947, -105.1874398749427 39.92870302575108, -105.188280750955 39.92869597460466, -105.1891882146993 39.92868835848437, -105.1900135071195 39.92868142556227, -105.1912021775201 39.92867143016532, -105.1921605878346 39.92866908889513, -105.1952731788288 39.9286614295662, -105.1953454862046 39.92714404290943, -105.1954277266185 39.92535293082255, -105.1954701680578 39.92442856826072, -105.1954828953945 39.92415135493398, -105.1955126848871 39.9235025188834, -105.1955539541151 39.92260363548544, -105.1955832718303 39.92176253388807, -105.1956074363542 39.92104863795893, -105.1956271775804 39.92046542890528, -105.1956491770346 39.92026642822356, -105.1957021779222 39.92016442965017, -105.1958741782275 39.91996042930643, -105.1960031773458 39.91985842861604, -105.1960461779453 39.91979442941913, -105.1963542841982 39.91947358440687, -105.1969171547176 39.91888743134161, -105.1971382584971 39.91865717884937, -105.1975931774295 39.91818342841723, -105.1977971773725 39.91800542846681, -105.1980761776685 39.9178604287125, -105.1988809443973 39.91750583145522, -105.199981771958 39.9170207684681, -105.2005472795797 39.91677157902036, -105.2013773094024 39.91640582131284, -105.2019980528428 39.91613227988852, -105.2026927027816 39.91582616438962, -105.2029610455153 39.91570919533338, -105.2032861789647 39.91558342752357, -105.2034951787843 39.91545442818257, -105.2036994329652 39.91536577400033, -105.2039238798093 39.91526835479848, -105.2044351788381 39.9150464284585, -105.2046181793619 39.91493942746109, -105.2047771484222 39.9148745542603, -105.2051264319463 39.91473201341331, -105.2055840142236 39.91454527467528, -105.206223179592 39.91428442723124, -105.2062611795562 39.91424142750945, -105.2062749820281 39.91414793981343, -105.2080811675174 39.91413651982791, -105.2081010480463 39.91413639369402, -105.2082326020008 39.91413556073108, -105.2082437405714 39.91413548987958, -105.2127750952919 39.914106703786, -105.2128870458286 39.91410599043611, -105.213645040396 39.91410184790944, -105.2175004417789 39.91408067426644, -105.2189361314345 39.91407275709121, -105.2212525262855 39.91405994110492, -105.2221488638938 39.91405498129632, -105.2316342538218 39.91406393968015, -105.2328366111099 39.91406370115187, -105.2386024786223 39.91406237558283, -105.238920889073 39.91406229633754, -105.2392698990356 39.91406220443915, -105.239915923657 39.91406203514502, -105.2402281491856 39.91406195092515, -105.2405279089477 39.91406186839333, -105.2412789148089 39.91406166045791, -105.2459316121797 39.91403871789947, -105.2501535052445 39.91401773192297, -105.2598916796428 39.91397305810732, -105.2600457617387 39.91397082590954, -105.2654909078388 39.91389125974047, -105.2666177593649 39.91387476217126, -105.2692129079631 39.91383672570182, -105.2759740475008 39.91371767073185, -105.2763431408977 39.91371116039856, -105.2811042377732 39.91371047397082, -105.2816813633473 39.9137103780077, -105.2819189247833 39.91371033909354, -105.2826022004646 39.91371022423816, -105.2838975683199 39.91370999020454, -105.2841657430803 39.91370993925377, -105.2845492353484 39.91370986571884, -105.285848204384 39.91370961828155, -105.2953533084801 39.91370800138991, -105.3000747525567 39.91381446987435, -105.3040421127392 39.91390380243763, -105.3047891203881 39.91392060756144, -105.3067655027752 39.91391296285316, -105.307489992947 39.91391015846362, -105.3138618072536 39.91388526812848, -105.3138945250918 39.91388513907664, -105.3140600078973 39.91388448682844, -105.314962656992 39.91387604616386, -105.3149765887619 39.91388835983841, -105.3228091235898 39.92081034046993, -105.322810999039 39.92081199876494, -105.3230754639435 39.92090816782166, -105.3230946808704 39.92091515582619, -105.3232179993169 39.92095999891312, -105.3236539993554 39.92104899939051, -105.3238185156393 39.92104925748924, -105.3238336179889 39.92104928059182, -105.3238539754728 39.92139180765506, -105.3240379379819 39.92434240818668, -105.3242555787687 39.92783278270667, -105.3240442233703 39.93038144497817, -105.3239541807884 39.93152857193745, -105.3205148429798 39.9317151039824, -105.3191391063055 39.9317901419817, -105.3189277387964 39.93544482213235, -105.3152947463766 39.93560825239187, -105.3150107817862 39.93562102376601, -105.3143742582034 39.93564970797279, -105.3095358144376 39.93550462579071, -105.3071402630428 39.93542705711443, -105.3069899024326 39.93542112842958, -105.3069725184858 39.93542044362167, -105.3069620635541 39.93542003071309, -105.3069103940744 39.93541827429448, -105.3069092683438 39.93541834896335, -105.3069535269843 39.93561751436307, -105.3070365248101 39.93587851262632, -105.3070725234688 39.9360675137267, -105.3070965232637 39.93624851219369, -105.3071325228354 39.9364195118327, -105.3071215214023 39.9365905102257, -105.3070635204184 39.93681550897311, -105.30694751905 39.93696950805576, -105.306818518862 39.93700550812312, -105.3067365183501 39.93702350801441, -105.3065845176777 39.937024507514, -105.3064325177913 39.93698850691153, -105.306303518788 39.93693450642142, -105.3061745181336 39.93687250614514, -105.3060220519166 39.93676488394409, -105.3060215182982 39.93676450657076, -105.3058455198719 39.93655750740345, -105.3057515200265 39.93640450647627, -105.3056685207497 39.9362425084482, -105.3056205223492 39.93609850781798, -105.305585522285 39.9359185082124, -105.3055605239748 39.93568450944846, -105.3055245241444 39.9355225104711, -105.3054775255262 39.93536051092015, -105.3054185257825 39.9352255117001, -105.3053475260123 39.93510851162448, -105.3052649411208 39.93500105239805, -105.3051249998132 39.93487599901849, -105.3049609990574 39.9347679983106, -105.3047729999609 39.93465199848702, -105.3043750004235 39.93447299937178, -105.3041400002485 39.93438299901855, -105.3036249993473 39.9342399993314, -105.3033550004067 39.93418699885896, -105.3031559993366 39.93411499904182, -105.3030620004486 39.9340439989491, -105.3030613571231 39.93404313591987, -105.3030605270924 39.93404250944442, -105.3029665280378 39.93391650971581, -105.3028365281158 39.93377250899461, -105.3027425284081 39.93365550934977, -105.3026955304566 39.93353850908618, -105.3027175305075 39.9333315116956, -105.30274053066 39.93320551125296, -105.3027515328109 39.93302451231442, -105.3027395322691 39.93284451334089, -105.3027385331218 39.93272751349467, -105.3026555343237 39.93254751358649, -105.3025744395126 39.93245850672481, -105.3024929994625 39.93238699899254, -105.3023169997215 39.93232499931828, -105.3019069997756 39.93227199824996, -105.3018019998002 39.93225399901318, -105.3016729997055 39.93221799834335, -105.3015790000119 39.93216399873801, -105.3015777603272 39.93216264201322, -105.3015775337403 39.9321625119282, -105.301471534445 39.93204651279913, -105.3014125343503 39.93194751346691, -105.3013765351856 39.93182151241906, -105.3013755377297 39.93146951471951, -105.3013045384598 39.93132551488237, -105.3012215390554 39.93117251653352, -105.3011395392849 39.9310825154602, -105.300857545551 39.93070551454974, -105.3007179891391 39.93056299355572, -105.3007165416099 39.93056151667432, -105.3005405416353 39.93046251704081, -105.300258541759 39.93035551655753, -105.3000245404921 39.93036451610091, -105.2998255407144 39.93035651574085, -105.2996265409012 39.93035651468055, -105.2994985401073 39.93040251280053, -105.2993585393596 39.93050151340886, -105.2992295378499 39.93054751218898, -105.299124538251 39.93056551160236, -105.2989255374498 39.93058351168081, -105.2986565371699 39.93059350921907, -105.2979425358611 39.93053250925767, -105.2977785362033 39.93052350758106, -105.2976145345236 39.93055150739807, -105.2974745341685 39.93059650677375, -105.29729953411 39.93068750674149, -105.2971125337131 39.93079550503958, -105.2968435314715 39.93091350344232, -105.2967035312445 39.93093250348966, -105.2964925312223 39.93093250195601, -105.2962585312108 39.93088850094149, -105.2960563719337 39.93084592573341, -105.2958585855775 39.93080427208812, -105.295847148283 39.93079930450271, -105.2958119503042 39.93077165856035, -105.2957816844527 39.93075581006419, -105.2957414044352 39.93072857119356, -105.2957219621322 39.9307171523971, -105.2956935960834 39.93069431994228, -105.2956681569902 39.93066919149165, -105.2956372964884 39.93064254121168, -105.2956237638325 39.93062237308391, -105.2955785483912 39.93058333758654, -105.2955471287956 39.93054339167713, -105.2955092928667 39.9304939045054, -105.2954749140355 39.93045847282398, -105.2954526680995 39.9304390844845, -105.2954290224646 39.93041557494557, -105.2954147445271 39.93039897567736, -105.2954068553409 39.93038980647571, -105.2953777926859 39.93036449589522, -105.2953347401986 39.93032679351454, -105.2952763762496 39.93028128041745, -105.295274573325 39.93047988761785, -105.2952722289371 39.93073811110776, -105.2952668936788 39.93105153150454, -105.2952189307569 39.93289754368107, -105.295160662098 39.93513982394448, -105.2951595853357 39.93518128110463, -105.290629040115 39.93519372808762, -105.2860766755759 39.93520076136944, -105.2850264897052 39.93519797944938, -105.2839771732097 39.93519518868442, -105.2829408013373 39.93519241095223, -105.2819004552617 39.93518958664934, -105.2808121864995 39.93519349146156, -105.2800887155675 39.9351960772441, -105.2797114034442 39.93519741970312, -105.278656951618 39.93519510654447, -105.2776168693938 39.93519281778027, -105.2765200120783 39.93519044371492, -105.2764859620717 39.93515834754393, -105.2747866320536 39.93355640077568, -105.2747706478011 39.93361397472692, -105.2747423603218 39.93371587032925, -105.2746861686253 39.93391760425664, -105.274475989006 39.93468847254762, -105.2744480828891 39.93479082274935, -105.2736239195408 39.93479817386874, -105.2736102258134 39.93479829736632, -105.2734198916193 39.93444690778491, -105.2733207529988 39.93449712888253, -105.2732794633518 39.93451804827096, -105.2732929660188 39.9352475981247, -105.273205627434 39.93608284252236, -105.2732054606918 39.93608443275637, -105.2731873820246 39.93625731362162, -105.2723902507118 39.93621108668517, -105.2723284207845 39.93638767363275, -105.2722356958043 39.93638920518273, -105.2721475513831 39.93662031538015, -105.2717721351925 39.93717547281373, -105.2694582864074 39.93778338126474, -105.269458297737 39.93778522313335, -105.2694387046704 39.93779073737785, -105.2694348364191 39.93760893088588, -105.2689722975682 39.93761531931789, -105.2689648067507 39.93697763738977, -105.2689647839754 39.93697572434603, -105.2689642246452 39.93692803967598, -105.268962923301 39.9368175091889, -105.2689627153546 39.93679978651981, -105.2689617639647 39.93671860378159, -105.2691360682297 39.93671834980415, -105.2692993042267 39.93671810942311, -105.2693021532052 39.93671810251961, -105.2693057732006 39.93671809986206, -105.2693212793192 39.93671807597465, -105.2694158873298 39.93671793665199, -105.269415158357 39.93668366514719, -105.2694149432323 39.93667357464245, -105.2694131583252 39.93658960360316, -105.2694128787389 39.93657642911547, -105.2694038140611 39.93615028433254, -105.269402414808 39.93608446232579, -105.2693982096128 39.93584833463098, -105.2693961725226 39.9357908856665, -105.2693921113694 39.93566105214616, -105.2665075813326 39.93595690063123, -105.2665040068149 39.93595730138393, -105.2665004826126 39.93595770043715, -105.2664969572278 39.9359581030905, -105.266493433013 39.93595850574616, -105.2664899076251 39.93595890929992, -105.2664863833918 39.93595931735921, -105.2664828626622 39.93595972722687, -105.2664793372618 39.93596013438296, -105.2664758165229 39.93596054695234, -105.2664722946108 39.93596096041988, -105.2664687703433 39.93596137838583, -105.2664652484343 39.93596179095252, -105.2664617276643 39.93596221252799, -105.2664582069067 39.93596263050073, -105.2664546849667 39.93596305207362, -105.2664511665304 39.93596347545478, -105.2664476457418 39.93596390243377, -105.2664441249563 39.93596432851194, -105.2664406076683 39.93596475819975, -105.266437089201 39.93596519058704, -105.266433573086 39.93596561937634, -105.2664300511118 39.93596605085565, -105.2664265326259 39.93596648864649, -105.2664230188169 39.93596692734742, -105.2664195015009 39.93596736514042, -105.2664159841694 39.93596780743661, -105.2664124691871 39.93596824703551, -105.2664089518402 39.93596869383473, -105.2664054368363 39.93596913973796, -105.2664019241723 39.93596958564577, -105.266398405649 39.93597003424361, -105.2663948906264 39.93597048555044, -105.2663913779468 39.93597093596124, -105.2663878664156 39.93597139267883, -105.2663843513806 39.93597184758794, -105.2663808386793 39.93597230430299, -105.2663773271356 39.9359727646229, -105.2663738167588 39.9359732258457, -105.266370301705 39.93597368615828, -105.2663667913096 39.93597415278479, -105.2663632820903 39.93597461761227, -105.2663597693486 39.93597508603516, -105.2663562636176 39.93597555717412, -105.2663527532096 39.93597602740282, -105.2663492451323 39.93597650033816, -105.2663457347119 39.93597697416924, -105.2663422313052 39.93597744981572, -105.2663387196993 39.93597792814752, -105.2663352127703 39.93597840738936, -105.266331707005 39.93597888843473, -105.2663281988966 39.9359793703759, -105.2663246919396 39.93597985772328, -105.2663211849825 39.93598034507053, -105.2663176803685 39.93598083152179, -105.2663141769121 39.93598132157788, -105.2663106699487 39.93598181072613, -105.266307166483 39.93598230348399, -105.2663036618379 39.93598279894131, -105.2663001595173 39.93598329890657, -105.2662966595521 39.93598379437316, -105.2662931560676 39.93598429253451, -105.2662896514038 39.93598479339534, -105.2662861525683 39.93598530057253, -105.2662826525751 39.93598580414454, -105.2662791514057 39.93598630951543, -105.2662756513939 39.93598681849121, -105.266272150209 39.93598732836514, -105.266268650191 39.93598783914199, -105.2662651501605 39.93598835352134, -105.2662616536368 39.93598886880838, -105.2662581571069 39.93598938589656, -105.2662546570671 39.93598990297759, -105.2662511616978 39.93599042276991, -105.2662476651369 39.93599094886435, -105.2662441674276 39.9359914686517, -105.2662406755496 39.93599199385477, -105.2662371778124 39.93599252174779, -105.2662336847551 39.93599304965022, -105.2662301881878 39.9359935775454, -105.2662266951088 39.93599411175222, -105.2662232020297 39.9359946459589, -105.2662197089536 39.93599517926481, -105.2662162158652 39.93599571617321, -105.2662127227706 39.93599625488281, -105.2662092296635 39.93599679719492, -105.2662057388995 39.93599733861106, -105.2662022504722 39.93599788093246, -105.2661987608564 39.93599842865526, -105.2661952724198 39.93599897367843, -105.2661917816278 39.93599952319996, -105.2661882920026 39.93600007362445, -105.266184805878 39.93600062675795, -105.2661813162435 39.93600117988414, -105.2661778301157 39.93600173391802, -105.2661743416417 39.93600228974835, -105.2661708543161 39.93600285188555, -105.2661673693458 39.93600340952411, -105.2661638866907 39.93600397437252, -105.2661604005318 39.93600453741242, -105.2661569108568 39.93600510224636, -105.2661534352183 39.93600566800936, -105.2661499490345 39.93600623825417, -105.2661464663638 39.93600680760531, -105.2661429836744 39.93600738236026, -105.2661395010035 39.9360079517112, -105.2661360194654 39.93600853187225, -105.2661325367759 39.93600910662686, -105.2661290575778 39.93600968679246, -105.2661255795495 39.9360102669603, -105.2661220991689 39.93601085072593, -105.2661186234713 39.93601143360026, -105.2661151384013 39.93601202005809, -105.2661116626851 39.93601260833614, -105.2661081881356 39.93601319751714, -105.2661047089092 39.93601378578784, -105.2661012331743 39.9360143794695, -105.2660977574361 39.93601497405167, -105.266094281701 39.93601556773311, -105.2660908071143 39.93601616772138, -105.2660873313667 39.93601676500521, -105.2660838591105 39.93601736769999, -105.2660803798405 39.93601796857911, -105.2660769110941 39.93601857128082, -105.2660734399892 39.93601917938152, -105.2660699677142 39.9360197874798, -105.2660664954392 39.93602039557795, -105.2660630243279 39.93602100547969, -105.2660595555442 39.93602161898868, -105.2660560867604 39.93602223249754, -105.2660526156242 39.93602284960421, -105.2660491468249 39.93602346761613, -105.2660456780224 39.9360240865286, -105.266042212739 39.93602470274617, -105.2660387450786 39.93602532976669, -105.2660352797673 39.9360259540899, -105.266031810943 39.93602657930655, -105.2660283467954 39.93602720543321, -105.2660248826354 39.9360278351624, -105.2660214172961 39.93602846759107, -105.2660179554636 39.93602910092739, -105.2660144901242 39.93602973335587, -105.2660110294553 39.93603036849571, -105.2660075652672 39.93603100633023, -105.2660041034067 39.936031647772, -105.2660006415461 39.93603228921371, -105.2659971843715 39.93603292886351, -105.2659937224953 39.93603357480826, -105.2659902641352 39.93603421895872, -105.2659868034165 39.93603486850823, -105.2659833462108 39.93603551716411, -105.2659798866434 39.93603617211975, -105.2659764294376 39.9360368207754, -105.2659729757324 39.93603747214006, -105.2659695184955 39.93603812980206, -105.2659660636017 39.93603878656808, -105.2659626098653 39.93603944693898, -105.265959154959 39.93604010730738, -105.2659557012133 39.93604077038, -105.2659522462883 39.93604143615213, -105.265948794867 39.93604210373254, -105.2659453446218 39.93604276951394, -105.2659418908573 39.93604343799007, -105.2659384405965 39.93604410827455, -105.2659349879833 39.93604478215673, -105.26593154122 39.93604545605076, -105.2659280874274 39.93604613263231, -105.2659246441553 39.93604681193715, -105.2659211915295 39.93604748942159, -105.2659177459143 39.93604816962207, -105.2659143014597 39.93604885252684, -105.2659108546589 39.93604953722802, -105.265907407858 39.93605022192915, -105.2659039633878 39.93605090933685, -105.2659005189051 39.93605160034705, -105.2658970767685 39.93605228956062, -105.2658936322857 39.93605298057061, -105.2658901889604 39.93605367518549, -105.2658867491389 39.93605437160874, -105.265883305798 39.93605507072667, -105.2658798648002 39.93605576894862, -105.2658764249599 39.93605647077545, -105.2658729851226 39.9360571717015, -105.265869544106 39.93605787532707, -105.2658661077569 39.93605858256459, -105.2658626679009 39.93605928889429, -105.2658592303724 39.93605999883125, -105.2658557940076 39.93606071057177, -105.2658523576397 39.9360614232128, -105.2658489247817 39.93606213586093, -105.2658454883982 39.93606285300504, -105.2658420543607 39.93606356835247, -105.2658386214777 39.93606428820551, -105.2658351885885 39.93606500985974, -105.2658317556961 39.93606573241451, -105.2658283251405 39.93606645587457, -105.2658248957456 39.93606718203887, -105.2658214675236 39.9360679073048, -105.26581803694 39.9360686388704, -105.2658146075356 39.93606936773635, -105.2658111769426 39.93607010200375, -105.2658077486987 39.93607083357382, -105.2658043192662 39.93607157054531, -105.2658008933467 39.93607230662324, -105.2657974674086 39.93607304810493, -105.2657940403097 39.93607378688219, -105.2657906190483 39.9360745292739, -105.2657871919276 39.93607527435548, -105.2657837694868 39.93607601944651, -105.2657803470459 39.93607676453749, -105.2657769245864 39.93607751503225, -105.2657735021237 39.93607826642751, -105.2657700831709 39.93607901782988, -105.265766660705 39.9360797701256, -105.2657632417304 39.9360805278323, -105.265759822765 39.93608128283692, -105.265756400268 39.9360820441389, -105.2657529883069 39.93608280366088, -105.2657495704865 39.93608356587281, -105.2657461538298 39.93608432988832, -105.2657427383555 39.9360850903035, -105.2657393228439 39.93608586152641, -105.2657359085178 39.93608662824837, -105.2657324953399 39.93608740127714, -105.2657290810043 39.93608817070079, -105.2657256689838 39.93608894733435, -105.2657222569695 39.93608972216647, -105.2657188449551 39.93609049699854, -105.2657154364382 39.93609127544024, -105.265712027915 39.93609205568313, -105.2657086170456 39.93609283772245, -105.265705207343 39.93609362066471, -105.2657017987949 39.93609440811258, -105.2656983937628 39.9360951937661, -105.2656949863907 39.93609597941475, -105.2656915801607 39.93609677317161, -105.2656881762798 39.93609756423111, -105.2656847712289 39.93609835528819, -105.2656813696723 39.93609915085553, -105.2656779645996 39.93609994821697, -105.2656745642067 39.93610074558782, -105.2656711626345 39.93610154565809, -105.2656677610529 39.93610234843027, -105.2656643594682 39.93610315210301, -105.2656609625663 39.93610395488447, -105.2656575644759 39.93610476306737, -105.2656541640455 39.93610557124546, -105.2656507659549 39.93610637942817, -105.2656473713649 39.93610719031987, -105.2656439744225 39.93610800480935, -105.2656405798231 39.93610881840284, -105.2656371852112 39.9361096355988, -105.26563379059 39.9361104554966, -105.265630395981 39.93611127179175, -105.2656270025235 39.93611209349308, -105.2656236125726 39.93611291610208, -105.2656202226155 39.9361137405123, -105.2656168303091 39.93611456761963, -105.2656134438525 39.93611539473874, -105.2656100527098 39.93611622364953, -105.2656066627245 39.93611705616524, -105.2656032750854 39.9361178868843, -105.2655998885975 39.93611872300951, -105.2655965044526 39.93611955823877, -105.2655931179646 39.9361203943638, -105.2655897337918 39.93612123769871, -105.2655863496405 39.93612207472896, -105.2655829654675 39.93612291806367, -105.2655795824613 39.93612376230131, -105.2655762027855 39.93612465878385, -105.2655728252331 39.93612561831667, -105.2655694523606 39.9361265778589, -105.2655660759718 39.93612753919526, -105.2655627019199 39.93612850143685, -105.2655593290254 39.93612946728336, -105.2655559561215 39.93613043583178, -105.2655525855606 39.93613140348413, -105.2655492126535 39.93613237293297, -105.2655458420708 39.93613334688974, -105.2655424726641 39.93613431904748, -105.2655391020812 39.936135293004, -105.2655357361627 39.93613627147327, -105.2655323667433 39.9361372472333, -105.2655290008123 39.93613822930497, -105.2655256337141 39.93613921047346, -105.2655222712866 39.93614019435339, -105.265518905349 39.93614117822608, -105.2655155429089 39.93614216570838, -105.2655121793018 39.93614315228755, -105.2655088180252 39.93614414157337, -105.2655054543994 39.93614513355626, -105.2655020954503 39.93614612644924, -105.2654987353249 39.93614712114109, -105.265495376357 39.93614811943773, -105.2654920185621 39.93614911683608, -105.2654886584148 39.93615011783218, -105.2654853029473 39.93615111883766, -105.2654819474735 39.93615212164437, -105.2654785919965 39.93615312535166, -105.2654752329909 39.9361541344556, -105.2654718833544 39.93615514087652, -105.2654685278493 39.93615615268938, -105.265465175854 39.93615716450925, -105.2654618285416 39.93615817543794, -105.26545847654 39.93615918905895, -105.2654551233559 39.93616020628009, -105.2654517748516 39.93616122351064, -105.2654484251648 39.93616224434134, -105.2654450813217 39.93616326698513, -105.2654417327986 39.93616428961931, -105.265438387776 39.93616531496251, -105.2654350427533 39.93616634030555, -105.2654316977244 39.93616736744988, -105.2654283526798 39.93616839909735, -105.2654250111482 39.9361694298512, -105.2654216684465 39.9361704606026, -105.2654183280661 39.93617149676256, -105.2654149865156 39.93617253292003, -105.265411644962 39.93617356997804, -105.265408306915 39.93617460794378, -105.2654049700225 39.93617565041504, -105.2654016272738 39.93617669467564, -105.2653982973979 39.93617773806172, -105.2653949593197 39.93617878503358, -105.2653916247574 39.93617983021117, -105.2653882901734 39.93618088169328, -105.2653849555955 39.93618193137394, -105.2653816245151 39.93618298466431, -105.2653782934159 39.93618404335844, -105.2653749670152 39.93618509665813, -105.265371632409 39.93618615444431, -105.2653683013096 39.93618721313818, -105.2653649737138 39.93618827364041, -105.2653616461148 39.93618933504321, -105.2653583196703 39.93619040095154, -105.2653549920587 39.93619146595674, -105.2653516679446 39.93619253457162, -105.2653483449973 39.9361936040894, -105.265345024393 39.93619467271121, -105.2653416967531 39.93619574582191, -105.2653383761269 39.9361968207481, -105.2653350531606 39.93619789566948, -105.2653317336979 39.93619897239912, -105.2653284165597 39.93620005363675, -105.2653250947475 39.93620113306347, -105.2653217799491 39.93620221430564, -105.2653184616281 39.93620329914319, -105.2653151456501 39.93620438308478, -105.2653118296596 39.93620547062889, -105.2653085160059 39.93620655907829, -105.2653052035097 39.93620765113261, -105.2653018898465 39.93620874228376, -105.2652985773439 39.93620983613923, -105.2652952660112 39.93621092999692, -105.2652919570059 39.93621202746192, -105.2652886479943 39.93621312672814, -105.2652853378096 39.93621422689249, -105.2652820287885 39.93621532886046, -105.2652787221042 39.93621643173378, -105.2652754165836 39.93621753641067, -105.2652721110505 39.93621864469008, -105.265268807851 39.93621975477546, -105.2652655058277 39.93622086306181, -105.265262202628 39.93622197314698, -105.265258899419 39.93622308593407, -105.2652555973581 39.93622420502795, -105.2652522988257 39.936225318725, -105.2652490002776 39.93622643692521, -105.2652457005564 39.9362275560236, -105.2652424066789 39.93622867693512, -105.2652391069481 39.93622979873529, -105.2652358118756 39.93623092684947, -105.2652325156484 39.93623205045789, -105.2652292240794 39.9362331803803, -105.2652259278427 39.93623430669049, -105.265222636261 39.93623544021534, -105.2652193481923 39.93623657284661, -105.2652160554374 39.93623770726952, -105.2652127720361 39.93623884351279, -105.2652094757617 39.9362399806303, -105.2652061900108 39.93624111957054, -105.2652029030899 39.93624225850828, -105.2651996184902 39.93624340285459, -105.2651963292012 39.93624454989324, -105.2651930492875 39.93624569244763, -105.2651897635082 39.93624683949325, -105.2647621049353 39.9363846692419, -105.2601074640665 39.93777228649274, -105.2591736798439 39.93805987096734, -105.2588379020683 39.93822555703911, -105.2580742502519 39.93844907086968, -105.2580707972867 39.93845110811252, -105.2580673739306 39.93845205381953, -105.2580639505649 39.93845300222836, -105.2580605306933 39.93845395514767, -105.2580571107959 39.93845491527217, -105.2580536944054 39.93845587630452, -105.2580502779924 39.9384568436414, -105.2580468662467 39.93845781459057, -105.2580434521449 39.93845879003799, -105.2580400438867 39.93845976729891, -105.2580366379397 39.93846075267054, -105.2580332319894 39.93846173894266, -105.2580298295299 39.938462730626, -105.258026427048 39.93846372861379, -105.2580230292365 39.93846472931327, -105.2580196337585 39.93846573181887, -105.2580162382485 39.93846674333088, -105.2580128474185 39.93846775485262, -105.2580094553993 39.93846877177572, -105.2580060668709 39.93846979410996, -105.258002683016 39.93847081825532, -105.2579992991355 39.93847184960574, -105.2579959152486 39.93847288275735, -105.2579925360192 39.93847392222328, -105.2579891591138 39.93847496619729, -105.2579857821988 39.93847601287317, -105.257982407611 39.93847706315647, -105.2579790376903 39.93847811705206, -105.2579756665804 39.93847917634906, -105.2579723001377 39.93848023925836, -105.2579689371794 39.93848130938014, -105.2579655730478 39.93848238040005, -105.2579622147438 39.9384834577367, -105.2579588587702 39.93848453778014, -105.2579555027869 39.93848562052543, -105.2579521502944 39.93848670868189, -105.2579487977826 39.9384878022422, -105.2579454475981 39.9384888994099, -105.2579421032475 39.93849000109308, -105.257938756544 39.93849110637386, -105.2579354145046 39.9384922161676, -105.2579320759623 39.93849332957124, -105.257928738574 39.9384944474805, -105.2579254023428 39.93849556899472, -105.257922071952 39.93849669322312, -105.2579187403624 39.93849782555478, -105.2579154122859 39.93849895699314, -105.2579120888575 39.93850009744771, -105.2579087642589 39.93850123789974, -105.2579054431384 39.93850238736557, -105.257902126701 39.93850353594048, -105.2578988090615 39.93850469351932, -105.2578954949353 39.93850585020486, -105.2578921854698 39.938507012304, -105.257888874815 39.9385081798045, -105.2578855688274 39.93850935091735, -105.2578822663274 39.93851052834204, -105.2578789661674 39.93851170577157, -105.2578756659816 39.93851289040624, -105.2578723716331 39.93851407865567, -105.2578690749285 39.93851527140336, -105.2578657817275 39.93851646595966, -105.2578624943541 39.93851766683271, -105.2578592093078 39.93851887131318, -105.2578559230882 39.93852007669179, -105.2578526450235 39.93852129199465, -105.2578493634487 39.93852250729002, -105.257846088881 39.93852372620268, -105.2578428142877 39.93852495232048, -105.2578395431948 39.9385261811475, -105.2578362756022 39.93852741268378, -105.2578330079936 39.9385286487232, -105.2578297438725 39.9385298910745, -105.2578264832518 39.93853113613503, -105.2578232273047 39.9385323830066, -105.2578199689919 39.9385336370784, -105.2578167165194 39.93853489386431, -105.257813466371 39.93853615515832, -105.2578102197229 39.93853741916158, -105.2578069742255 39.93853868857114, -105.2578037310585 39.9385399606875, -105.2578004925491 39.93854123911814, -105.2577972540331 39.93854251934997, -105.2577940213544 39.93854380319665, -105.2577907886596 39.93854509154649, -105.2577875606224 39.9385463862106, -105.2577843325755 39.93854768357663, -105.2577811103722 39.93854898275616, -105.2577778893132 39.93855028914326, -105.257774671761 39.93855159643829, -105.2577714576964 39.93855291004524, -105.2577682424488 39.9385542272522, -105.2577650318652 39.93855554897218, -105.2577618247852 39.93855687250073, -105.2577586211864 39.93855820414242, -105.2577554210944 39.9385595366921, -105.2577522209926 39.93856087194365, -105.2577490243815 39.93856221260636, -105.2577458300945 39.93856355777719, -105.2577426428114 39.93856490746596, -105.2577394555219 39.93856625895595, -105.2577362693799 39.93856761675286, -105.2577330879082 39.93856897726144, -105.2577299075873 39.93857034317637, -105.2577267342864 39.93857170910593, -105.2577235621267 39.93857308314374, -105.2577203899572 39.93857445988341, -105.257717221288 39.93857583933234, -105.2577140572797 39.93857722419494, -105.2577108956017 39.93857861176435, -105.2577077385877 39.93858000384675, -105.2577045815576 39.9385814004323, -105.2577014303711 39.93858279883143, -105.2576982791653 39.9385842026343, -105.2576951326266 39.93858561004964, -105.2576919895787 39.93858702287611, -105.2576888500344 39.93858843751122, -105.2576857093071 39.93858985574636, -105.2576825732375 39.93859128029582, -105.2576794453418 39.93859270936571, -105.2576763151093 39.93859413752992, -105.257673190701 39.93859557291159, -105.2576700639367 39.93859701279147, -105.2576669465228 39.93859845539296, -105.2576638279292 39.93859990069383, -105.2576607163332 39.93860135231392, -105.2576576035575 39.93860280663348, -105.2576544966254 39.93860426276648, -105.2576513920108 39.93860572520894, -105.257648292057 39.93860719306509, -105.2576451909362 39.93860866001801, -105.2576420968036 39.93861013599214, -105.2576390038407 39.93861161196865, -105.2576359131986 39.93861309335391, -105.2576328272269 39.93861457745087, -105.2576297435759 39.93861606695663, -105.2576266645953 39.93861755917406, -105.2576235891118 39.93861905500142, -105.2576205159523 39.93862055533687, -105.2576174439499 39.93862205927732, -105.2576143777814 39.93862356773325, -105.2576113127733 39.93862507889351, -105.2576082559424 39.93862659367355, -105.2576051967522 39.93862811385245, -105.2576021422355 39.93862963584248, -105.2575990923764 39.93863116414679, -105.2575960436872 39.93863269245352, -105.2575929961391 39.93863422886844, -105.2575899567778 39.9386357662012, -105.2575869197437 39.93863730714142, -105.2575838826838 39.93863885528675, -105.2575808526472 39.93864040254618, -105.2575778237613 39.93864195521184, -105.2575747971961 39.93864351328624, -105.2575717741312 39.93864507406995, -105.2575687580735 39.93864663847096, -105.2575657443462 39.93864820557876, -105.2575627317728 39.93864977719219, -105.2575597238665 39.93865135241801, -105.2575567136041 39.93865293214206, -105.2575537126889 39.93865451548837, -105.2575507164441 39.93865610154639, -105.25754772018 39.93865769300825, -105.2575447262462 39.93865928717691, -105.257541740496 39.93866088316403, -105.2575387535534 39.9386624854532, -105.2575357724478 39.93866409135715, -105.2575327925058 39.93866569906486, -105.257</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>18</v>
-      </c>
-      <c r="E14" t="n">
-        <v>18</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Manhattan MS</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>290 Manhattan Dr, Boulder, CO 80303</t>
+        </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>290 Manhattan Dr, Boulder, CO 80303</t>
+          <t>http://mam.bvsd.org/</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
+          <t>Manhattan Middle School of Arts and Academics</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>39.99410342530379</v>
+      </c>
+      <c r="K14" t="n">
+        <v>-105.2273572175253</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
           <t>http://mam.bvsd.org/</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Manhattan Middle School of Arts and Academics</t>
-        </is>
-      </c>
-      <c r="L14" t="n">
-        <v>39.99410342530379</v>
-      </c>
-      <c r="M14" t="n">
-        <v>-105.2273572175253</v>
-      </c>
       <c r="N14" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>http://mam.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
         <is>
           <t>POINT (-105.2273572175253 39.99410342530379)</t>
         </is>
@@ -1456,59 +1368,53 @@
           <t>POLYGON ((-105.1252489123642 39.97296264565752, -105.1251781675552 39.97293944155944, -105.1250681668962 39.972906441131, -105.1249497653521 39.97287524610411, -105.1249011680386 39.97286244087732, -105.1248531668425 39.97285044186012, -105.1247921674847 39.97283644067091, -105.1246601669836 39.97280844165002, -105.1245523833219 39.97278895695491, -105.1244201369517 39.97276780367894, -105.1242581672639 39.97274644167108, -105.1241911675568 39.97273944124998, -105.1229011674566 39.97270644080103, -105.1217242765111 39.97281619705816, -105.1214051667389 39.9728474415511, -105.1212921660192 39.9728514412086, -105.1211677547576 39.97285530417747, -105.1209041446044 39.97286348814555, -105.1206801658403 39.97287044195357, -105.1203420443671 39.97286990956984, -105.1194881869002 39.97287256612985, -105.1186181657589 39.97287744155079, -105.1186161666875 39.97368444138921, -105.1182721659632 39.97381044163679, -105.118018165306 39.97395344192811, -105.1171981652229 39.97420444199783, -105.1171265636503 39.97423590742287, -105.1158010195454 39.97481841383456, -105.114358165628 39.97545244199855, -105.1140021644149 39.97552144240487, -105.1135711643946 39.97554144292338, -105.113406165381 39.97567644266403, -105.1132631646667 39.97570744192655, -105.1133870040023 39.97608190631396, -105.1133790200561 39.97608188493721, -105.1123831027614 39.97608512830671, -105.1117668377299 39.9760899171973, -105.1108470594524 39.97608530949304, -105.1108412041789 39.97609179069381, -105.1092491642645 39.97610344217862, -105.1092964823203 39.97532071473902, -105.1092904101518 39.97530904500583, -105.1092758343959 39.97528099404412, -105.1092339554898 39.97511696238349, -105.1092260671889 39.97499889140114, -105.1092199916418 39.97462689328338, -105.1092231749659 39.97382200756769, -105.1092751638475 39.97241644265112, -105.1093741622733 39.95969644064292, -105.1093821626999 39.95928944047934, -105.1079021614665 39.95931444023918, -105.1078871611286 39.95851244033037, -105.1081481615724 39.95847244081943, -105.108159162151 39.95790844019832, -105.1081605804928 39.95790194404009, -105.1093269988958 39.95789799857891, -105.1093269879348 39.95789786884638, -105.1145961633331 39.95785343948453, -105.1145691634786 39.96033344011676, -105.1152741627195 39.96032944007523, -105.1152851635068 39.95784843935154, -105.1280631665933 39.95781743936814, -105.1279511266712 39.9541802399316, -105.1279522914871 39.95238450217838, -105.127953497769 39.95054658538529, -105.1279535055246 39.95053550276305, -105.1279608891086 39.94967093417858, -105.1279857222323 39.94676288303474, -105.1280107097569 39.9438364185598, -105.1280154169606 39.94328510754713, -105.1281202734379 39.94328281974127, -105.1281189566972 39.94321673837639, -105.128119170051 39.94275986892613, -105.1281188559567 39.9426128500413, -105.1281179815044 39.94209470227083, -105.1281166731066 39.94131881581806, -105.1281160435918 39.94095694729186, -105.1281027487722 39.93982376694078, -105.1280999834125 39.93958806354111, -105.1281533050244 39.93958961368488, -105.129260217686 39.93962179633774, -105.1305578104314 39.93965950845269, -105.1309208893939 39.93966636177272, -105.1364432759128 39.93974592316794, -105.1370090029643 39.93974203840741, -105.13757654182 39.9397486123599, -105.1376106683007 39.93974719309715, -105.1376101742235 39.93970626003536, -105.1376659994644 39.93973899908963, -105.1380069982713 39.93995099908016, -105.1400129996827 39.94124299866457, -105.1405889992587 39.94161999863454, -105.1409599991531 39.94185799904378, -105.141208999877 39.9420169995477, -105.1415170000054 39.9422179981579, -105.1429179998172 39.94312999953807, -105.1435829995349 39.94355199879121, -105.1436849993157 39.94361699895295, -105.1438049994702 39.94369699936311, -105.1444109992605 39.94408999827592, -105.1465979998178 39.94550799907834, -105.1469689981003 39.94574899894534, -105.1470224473384 39.94578389403245, -105.1479109994562 39.94636399921564, -105.1483709999483 39.94665999878806, -105.1487869967502 39.94692837327946, -105.1493769991665 39.94730899849206, -105.1502339997436 39.94785999905235, -105.1505859991704 39.94808599920534, -105.1510029999227 39.9483689989986, -105.1520270002295 39.94907999894239, -105.1526479997484 39.94953399844792, -105.1538259995572 39.95043899936822, -105.1543240000297 39.95082499846626, -105.1545469991415 39.95082499900798, -105.154634999516 39.95082499893148, -105.155603998905 39.95163699829544, -105.1564621234448 39.95235626096443, -105.1568089995898 39.95264699943566, -105.1594730000078 39.95466099895394, -105.1603829998639 39.95530799832515, -105.1604879993213 39.95538299862599, -105.1605708372656 39.95542490543037, -105.1605729992732 39.95542599889634, -105.160553485336 39.95544433019448, -105.160507601197 39.95548743481859, -105.1605070003541 39.955487998663, -105.1605739993225 39.95553199876508, -105.1609239990875 39.95574399904351, -105.1611820283237 39.95589271854974, -105.1612710001578 39.9559439989421, -105.1615179991773 39.95607999946219, -105.162090999951 39.95638499933245, -105.1623139998591 39.95649799874107, -105.1626729999983 39.95667199866357, -105.1629539988249 39.95680199904174, -105.163260000118 39.95693999941128, -105.1635449998441 39.95706699912397, -105.1640439992191 39.95727199887524, -105.1655459994386 39.95785699862255, -105.1657049993032 39.95791899851163, -105.1658829843055 39.95798883313223, -105.166280999977 39.95814499912188, -105.1663260779203 39.95809453148716, -105.1663729998672 39.95804199855646, -105.1663939993887 39.95801599875833, -105.1663429988309 39.95789999829524, -105.1661250002072 39.95739999859541, -105.1661089994848 39.95726499912967, -105.1660659997773 39.95698699837227, -105.1660599995567 39.9569419984156, -105.1661219997786 39.95695499897838, -105.1668249995467 39.95710599849211, -105.1672029990481 39.95741599921722, -105.1677549991503 39.95786999907147, -105.16867899997 39.95862899864169, -105.1718929991997 39.96004699882172, -105.1750629987647 39.96129699910314, -105.175195000182 39.96134899884276, -105.1777729991336 39.96222499799526, -105.1777779996259 39.96221599908061, -105.1777786369145 39.96221513532904, -105.1777988506388 39.9622247658564, -105.1779603294206 39.96230169761951, -105.1780248042583 39.96220476780362, -105.1780361786519 39.96221443573692, -105.1790331792207 39.9626014355022, -105.1791101784401 39.96248843618227, -105.1800231788606 39.96283243551652, -105.1803891795854 39.96287543542729, -105.1804071788043 39.96288743619242, -105.1804541783631 39.96292043608274, -105.1805011791406 39.96295143559319, -105.1805491783552 39.96298243605077, -105.1806471783964 39.96304143605229, -105.1806971792238 39.96307043532614, -105.1807481784856 39.96309843581128, -105.180799178964 39.96312643537638, -105.1808511790458 39.96315343615423, -105.1809041787385 39.96317943634221, -105.1809571796388 39.96320443587675, -105.1810111789803 39.96322943544858, -105.1810651795186 39.96325343616735, -105.1811201784924 39.96327643628931, -105.1811751798336 39.96329843665993, -105.1812645330557 39.96333272334351, -105.1813451795762 39.96336143602115, -105.1814281797796 39.9633894364229, -105.1815181794293 39.96341743539393, -105.1815991793696 39.96344043598965, -105.1818761791532 39.9635074363657, -105.1820251788167 39.96353643541125, -105.1821201788212 39.96355143678812, -105.1822441795616 39.96356843645984, -105.1823521786804 39.96357643573872, -105.1824941789573 39.96359343521812, -105.1826201798852 39.9636004354759, -105.182745178819 39.96360443634497, -105.1828711795887 39.96360543613775, -105.1829971802545 39.96360343569754, -105.1831221800468 39.96359843587509, -105.1832471796654 39.96358943518963, -105.1833721791185 39.96357743607462, -105.1835581803465 39.96355343554686, -105.183681180111 39.96353243572506, -105.183756179454 39.96352043583736, -105.184684179543 39.96329443567719, -105.1846881802595 39.96256443553224, -105.1851691808371 39.96256443568562, -105.1852781797714 39.96245943558378, -105.1862821800566 39.96244943611252, -105.1867361810641 39.96239743503643, -105.187073180655 39.96230143525784, -105.1872551801046 39.96227843565087, -105.1876121808403 39.9621674358669, -105.1877131813326 39.96209643507789, -105.188260316038 39.96197615552799, -105.1889071811083 39.96174843466853, -105.1892811813567 39.96148043493095, -105.1892731804752 39.96267043497246, -105.1882881813402 39.96279743543808, -105.1875491802892 39.96290443543483, -105.1867561809799 39.96303243590308, -105.1859091799674 39.96319543556243, -105.1852101802556 39.96334743554963, -105.1850871806001 39.96337543512138, -105.1846831809932 39.96346543564761, -105.1846811801298 39.96359143505422, -105.183359179438 39.96390543564833, -105.1831431795536 39.96390943620628, -105.1829501799709 39.96406143557106, -105.1823765858315 39.96435856048586, -105.182328924705 39.96438302610748, -105.1836529999933 39.96489799860698, -105.1845014339616 39.96523026465304, -105.184378790729 39.9663747723468, -105.1843769878934 39.96809980246061, -105.1834828991021 39.96810018023088, -105.1826965883272 39.96810050650755, -105.1827049815247 39.96884194995791, -105.1827443502702 39.97231958783131, -105.1826878500371 39.97232043832547, -105.1825779238971 39.97232006357458, -105.1824693614918 39.97231969607867, -105.1818888682263 39.97232118367459, -105.181313336771 39.97232225425414, -105.1807346165126 39.97232332753696, -105.1802034669848 39.97232431015902, -105.1797370086139 39.9723251692939, -105.1792927120879 39.97232533345959, -105.1782463742659 39.97232158132549, -105.1775629965025 39.97231860602722, -105.1761817574226 39.97231257916473, -105.1754036449972 39.97230917804725, -105.1753349979691 39.97230887841319, -105.1753040182588 39.97230874160383, -105.1753029543753 39.97233821445883, -105.1753000521294 39.97286562741104, -105.1752993592102 39.97299154292094, -105.1752986321791 39.97312339547399, -105.1752986400875 39.97327644619253, -105.1752986424906 39.97332390459598, -105.1752987049537 39.97441934769093, -105.1752970387502 39.97477164542337, -105.1752952276789 39.97514060311426, -105.1752932053162 39.97554706270822, -105.1752933364211 39.97554706487885, -105.1752921268262 39.97576430925468, -105.1752921682676 39.97579225049291, -105.1752957663743 39.97633889713853, -105.1752998415047 39.97695824622881, -105.1753039309026 39.97757977851963, -105.1753066251767 39.97798897490134, -105.1753071625874 39.97807062647465, -105.1753077055884 39.97815307154284, -105.1753102988506 39.97864007456597, -105.1749131590959 39.97863994859521, -105.1746315779191 39.97863985840293, -105.1737145515828 39.97863956374063, -105.1736004540525 39.97863952981174, -105.1713767703544 39.97863884954739, -105.1707601398161 39.97863865429652, -105.1705561331186 39.97863809480832, -105.1698279435228 39.97863609678081, -105.1688872339223 39.97863350366777, -105.1679504485915 39.97863091778471, -105.1660539287566 39.97862565398879, -105.1660529846982 39.97899093757391, -105.1660527537385 39.97906729471996, -105.1660524971388 39.97915319426635, -105.1660513282059 39.97953810432843, -105.1660546877398 39.97987039392753, -105.166056001947 39.98000036722793, -105.1660560052696 39.98000040596588, -105.166057391659 39.98000036044625, -105.1660575394011 39.98000748868384, -105.1660575821633 39.98001166786214, -105.1660576266512 39.98001166799104, -105.166065785029 39.98040377608608, -105.1659816707675 39.98040380617206, -105.165974894609 39.98681212206605, -105.1659751117827 39.98681224608544, -105.165974893996 39.98681224725572, -105.1654436915867 39.98681856417538, -105.165249938283 39.98682086759958, -105.1652483903585 39.98682087571383, -105.1652418264078 39.98717422250558, -105.16525834624 39.98830990071465, -105.1652600612412 39.9884278360004, -105.1652129168158 39.98840770990265, -105.164152903713 39.98795517594412, -105.1640557053296 39.98791588344694, -105.1639629797611 39.98801302742708, -105.1638820078671 39.98807702897645, -105.1636180300277 39.98827007062972, -105.1633738472757 39.98842912912709, -105.1632068468137 39.98856892148969, -105.1631318802227 39.98864501967785, -105.1630340843738 39.98879105290501, -105.1629701445979 39.98894706885007, -105.1629411450479 39.9891100499324, -105.1629369535138 39.98923604238151, -105.1629316619924 39.98939933324853, -105.1630484245457 39.98939258460942, -105.1652800904351 39.98963757722175, -105.165280121269 39.98963940654668, -105.165293913414 39.9904726547182, -105.1644396301791 39.99047469439939, -105.1603292951578 39.99048441784612, -105.1598894223283 39.99048544917379, -105.1582351763826 39.99048931494893, -105.1582367037443 39.99049132434087, -105.1585727934224 39.99093128003249, -105.158249423521 39.99149224398947, -105.1576955197453 39.99206442405352, -105.1570945121236 39.99246391068015, -105.156359603665 39.99274076059307, -105.1561716319405 39.99274373072714, -105.1560127966663 39.99270667940952, -105.1550702284904 39.99239786295302, -105.1548927785468 39.99227636637016, -105.1548910742555 39.99251738266482, -105.1548905001314 39.99259868061086, -105.1548904876865 39.99260044586263, -105.1548798542597 39.99410483914303, -105.1527289655441 39.99412802825835, -105.1527391763146 39.99397744204157, -105.1511885403603 39.99398043009678, -105.1489619720619 39.99399513205215, -105.1467891751321 39.99400744202379, -105.146790174619 39.9941694428106, -105.1466363980306 39.99416436382368, -105.1464615829938 39.99416230126948, -105.1459611770951 39.99455926085398, -105.145432872713 39.99479210016541, -105.1443011561806 39.99478265717581, -105.1442614765063 39.99492166747812, -105.1422639133758 39.99651569716553, -105.1418815666315 39.99705442482142, -105.1415483564617 39.99743752080339, -105.1412987486078 39.99773918448757, -105.1407003492131 39.99804212814589, -105.1405141950552 39.99813279982534, -105.1373344848354 39.99415560978961, -105.1373254730912 39.99414433762385, -105.130985314058 39.99412962806004, -105.1279510944342 39.99413186772644, -105.1277274031719 39.99403166429317, -105.1232577328613 39.99406674611331, -105.1232589140897 39.9941456611968, -105.122814800146 39.9941474397444, -105.1226719071595 39.99394172642054, -105.1225145804866 39.99383477964317, -105.1223849223714 39.99378832326342, -105.1223232452224 39.99378812123183, -105.1223389573864 39.99236704634767, -105.1223383484516 39.99236705245885, -105.1222303531299 39.99236784607286, -105.121007043891 39.9923704175954, -105.1204839651552 39.99237377836661, -105.1199496728335 39.99237720607682, -105.1189229397637 39.99238378801977, -105.1185472892864 39.99238619608135, -105.1185474045477 39.99235909652852, -105.118575976712 39.98710775588565, -105.1185703104926 39.98693549769058, -105.1173699922748 39.98694351032786, -105.1173718857854 39.98689901321579, -105.1173974168023 39.9851484639417, -105.1174133094992 39.98331547110325, -105.1186071665135 39.98330244358745, -105.1185851681232 39.98678444408168, -105.1211532829889 39.9867767735869, -105.1230647672254 39.98677086630205, -105.1252729795815 39.9867354607854, -105.1278491696747 39.98669844278966, -105.1278438505662 39.98611127501945, -105.127841169928 39.98581544210798, -105.1278368922283 39.98539987307798, -105.1278341691096 39.98513544239999, -105.1278081691162 39.98462244192449, -105.1278173436443 39.98417719271642, -105.1278251690041 39.98379744319919, -105.1278411686021 39.98365144210749, -105.1268601685777 39.98365144197767, -105.1268441685182 39.98313644257139, -105.1258921445311 39.98314315953377, -105.1249263230647 39.98314996424318, -105.1242251688294 39.98315444282675, -105.1240021678686 39.98305844296069, -105.1238561683382 39.98296444303244, -105.123744168235 39.98286744302084, -105.1236691677244 39.98278344313378, -105.1235781685477 39.98264044277064, -105.1235830349789 39.98201442443881, -105.123586168347 39.98161144252593, -105.1236411680837 39.98141344271861, -105.1237131684662 39.98127144197014, -105.123848168531 39.98109744278342, -105.1239481684561 39.98099044193104, -105.1239441684502 39.98063844197828, -105.12468924775 39.98064430008328, -105.1250891674626 39.98064744247992, -105.1253301685872 39.98066944203719, -105.1254741692224 39.98069944174981, -105.1256331685554 39.98073244235897, -105.1258431687578 39.98075244156166, -105.1259671694033 39.98075344203813, -105.1261481677718 39.9807394421338, -105.126331169116 39.98070644271509, -105.1264991677584 39.98067244239655, -105.1266091684414 39.98065844226225, -105.1266971688295 39.98065244248855, -105.1267971687024 39.98065044260115, -105.1268901681804 39.98065044284952, -105.1269711680979 39.98065844167844, -105.1270981684207 39.98067544186095, -105.127139392241 39.98068334791111, -105.1271711685487 39.98068944278467, -105.127214375739 39.98069969063391, -105.1273066551089 39.98072157695184, -105.1273271684002 39.98072644199087, -105.1274521692765 39.98074644262105, -105.1275471685854 39.9807554418902, -105.1277031693758 39.98076144258219, -105.1277022727454 39.98065050362139, -105.1277006654453 39.98045161563807, -105.1276992570783 39.98027720192252, -105.1276979486562 39.98011536714193, -105.12769489113 39.97973687298536, -105.1276880805791 39.97925149078886, -105.1276812036791 39.97880423869458, -105.1276742985784 39.97835509150174, -105.1276701687788 39.97808644191434, -105.1271081689285 39.97816144152506, -105.1262311691111 39.97870844220219, -105.1260051674357 39.97884844174765, -105.1255304415947 39.97914450912447, -105.1253541688852 39.97925444189506, -105.1255771679067 39.97947344233817, -105.1243405817918 39.98021614971381, -105.1235891680376 39.98066744275177, -105.1232421681502 39.98033144190374, -105.1225391670139 39.98073944211418, -105.1219081678686 39.98099644262695, -105.120230166672 39.98108244243971, -105.1201190479548 39.97979700902974, -105.1199982265585 39.97824241435777, -105.120213921188 39.9783408640164, -105.1204351430655 39.97840802722106, -105.1206690055671 39.97844805327635, -105.1209279925593 39.97846208286956, -105.1212738234645 39.9784519641494, -105.1218390971384 39.97837997317655, -105.1220440922178 39.97834907560969, -105.1251821045501 39.97776690536398, -105.1271320977502 39.97739411515896, -105.1273435143957 39.97735082326365, -105.1276466084615 39.97708321067033, -105.1276525381961 39.97673399347658, -105.1276644462961 39.97603262125949, -105.1275745938115 39.97544829877226, -105.1274121598896 39.97481223461234, -105.1269897690644 39.97410774900974, -105.1265094311803 39.97363524625856, -105.1259336601506 39.97325526013939, -105.125568498434 39.97308157000424, -105.1254721676893 39.97304244124539, -105.1254030021113 39.97301706732278, -105.1253031669845 39.97298044167606, -105.1252489123642 39.97296264565752), (-105.1278929800003 39.98688710210271, -105.1278667741885 39.9867742542211, -105.1278929788344 39.98688710119829, -105.1278529946731 39.98947786494407, -105.1278929800003 39.98688710210271))</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>19</v>
-      </c>
-      <c r="E15" t="n">
-        <v>19</v>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Monarch HS</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>329 Campus Dr, Louisville, CO 80027</t>
+        </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>329 Campus Dr, Louisville, CO 80027</t>
+          <t>http://moh.bvsd.org/</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
+          <t>Monarch High School</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>39.9520220573069</v>
+      </c>
+      <c r="K15" t="n">
+        <v>-105.141776992356</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
           <t>http://moh.bvsd.org/</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Monarch High School</t>
-        </is>
-      </c>
-      <c r="L15" t="n">
-        <v>39.9520220573069</v>
-      </c>
-      <c r="M15" t="n">
-        <v>-105.141776992356</v>
-      </c>
       <c r="N15" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
-        </is>
-      </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>http://moh.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="P15" t="inlineStr">
         <is>
           <t>POINT (-105.141776992356 39.9520220573069)</t>
         </is>
@@ -1528,59 +1434,53 @@
           <t>POLYGON ((-105.3507120197024 39.96977708492175, -105.3502663555101 39.96962995325117, -105.3499738912252 39.96953306242339, -105.3497927648202 39.96950780452823, -105.349583788853 39.96947178771764, -105.3494212532477 39.96944297880439, -105.34924479809 39.96940700386404, -105.3490962626725 39.96934961793916, -105.3487714009241 39.96919906389083, -105.3486369377627 39.9690809296067, -105.3484932173364 39.96894848511075, -105.3483587404312 39.9688374998723, -105.3482335625351 39.96872295112451, -105.3480852136772 39.96858335152659, -105.347973974335 39.96846882176619, -105.3478347816061 39.96838999925331, -105.347653738839 39.9683289938379, -105.3473891086939 39.96825357959553, -105.3471476832231 39.96818891961232, -105.346920194601 39.96812427673464, -105.3467158863003 39.96808111151876, -105.3465302247974 39.96800937500215, -105.3464235532126 39.96793059408106, -105.3463448281598 39.96781967985631, -105.3463031951509 39.96774098641889, -105.3462013150994 39.96759787164284, -105.3460947908402 39.9674547496716, -105.3458116807017 39.96733641345445, -105.345677049642 39.96729691428796, -105.3454078122883 39.96720719142478, -105.3451943215452 39.96711754282754, -105.344799794762 39.96696688392825, -105.3445631686427 39.96683788403377, -105.3440530565571 39.96644757631712, -105.3438722349838 39.96629362851484, -105.3437703294546 39.96616480941587, -105.3437287659197 39.966057518448, -105.3436874645537 39.96583584560934, -105.3435903286542 39.96565341505423, -105.3434611855153 39.96524932320219, -105.3433549485055 39.96498466743203, -105.3432580364064 39.96470572634975, -105.3432596704031 39.96399440692426, -105.3432090325889 39.96379416665803, -105.3432139409706 39.9636797911035, -105.3433584770403 39.96344764579057, -105.3440104872482 39.96271576210818, -105.3441130822002 39.96254075062669, -105.3441646115461 39.96235137391512, -105.3441696243447 39.9621905291703, -105.3442119288581 39.96197254236927, -105.3443796023165 39.96177617221307, -105.3445844845748 39.96155840560913, -105.3447195684986 39.96139416148351, -105.3447756268418 39.96125483276604, -105.3447388797202 39.96107248443195, -105.3446230140441 39.96095794510541, -105.3444420997995 39.96085046636512, -105.3439919356307 39.96067113365707, -105.3435556196811 39.96053113787423, -105.343360798049 39.96041291535013, -105.3430825891228 39.96019806749968, -105.3428645192128 39.96009053566726, -105.342558426089 39.95988279881342, -105.342340474804 39.95972522305689, -105.3421550957813 39.95954267131271, -105.3419930516309 39.95931368197322, -105.3419145010556 39.95913485006723, -105.3417808581094 39.95867713300948, -105.3417254175696 39.95854837578747, -105.3416888387843 39.95829811186334, -105.3416286954819 39.95819436922678, -105.3415686602473 39.95804415830918, -105.3414855003038 39.95785102185104, -105.3414486570114 39.95771514066693, -105.34143978317 39.95753640426094, -105.3413796242992 39.9574398108651, -105.3411988658981 39.95727156089524, -105.340813971399 39.95700294350355, -105.3407585423853 39.95687061110937, -105.3407823576073 39.95661685560312, -105.3407644374192 39.9563344475167, -105.3407741612119 39.95614858733419, -105.3408163394168 39.95598779399175, -105.340737929226 39.9557517698098, -105.3404224215921 39.95560835426767, -105.339963064055 39.95540754654273, -105.3397169369457 39.9553893318278, -105.3395404716461 39.95537478831839, -105.3393595717931 39.95527087623741, -105.3391972860632 39.95515269194618, -105.3389332719973 39.95484134311943, -105.3387481361285 39.95456584840096, -105.3385674690961 39.95436542476165, -105.3383821243641 39.95417929127716, -105.3380613773924 39.95387922079283, -105.3381922100665 39.9539168925779, -105.3385208374587 39.95402999317365, -105.3389704612986 39.95410320173998, -105.3396355797279 39.95422398497384, -105.3401411453694 39.95431463685155, -105.3405915068032 39.9543867512165, -105.3410226063689 39.95442202475896, -105.3413251764538 39.95446640101372, -105.3415462146834 39.95453170278824, -105.341978907135 39.95476111029183, -105.342318205314 39.95497951658208, -105.3425857909343 39.95514264437324, -105.3431903754274 39.95531610814066, -105.3435986820116 39.95550253670501, -105.3438741990323 39.95558088547542, -105.3440186020231 39.95565550758867, -105.3441136976464 39.95574272423425, -105.3441389977332 39.95581652211911, -105.3441425364855 39.95588635109922, -105.3440711556896 39.95613686272678, -105.3440378720344 39.9564039015618, -105.3440884076289 39.95664703425503, -105.3441827960147 39.95684524841415, -105.3443946158489 39.95709611761605, -105.3446068353019 39.95717269309261, -105.3448191912631 39.95717297927444, -105.3451590792293 39.9571407418311, -105.3454434965831 39.95717430831029, -105.3456695563883 39.95726454891713, -105.3459817638437 39.95741094481667, -105.3462287436664 39.95746034235974, -105.3465296949049 39.95748316629089, -105.3467618157279 39.95753709210727, -105.3471456360077 39.95776202530593, -105.3478214840077 39.95814889463594, -105.3485363790411 39.95860993791083, -105.3487037748324 39.95867567956383, -105.3488962982591 39.95871689126606, -105.3490717285018 39.95871526312619, -105.3492283080394 39.95870384425507, -105.3494911127846 39.95865230559473, -105.3497176360485 39.9586526012469, -105.3499724607688 39.95866380511001, -105.3502291566699 39.95861756977649, -105.3503832841733 39.95857717838697, -105.3506098071917 39.95857747228528, -105.3510048124872 39.9586400226201, -105.351345777182 39.95870917935156, -105.3516733318363 39.95880173663877, -105.3518836686614 39.95878613315444, -105.3520178350116 39.95875210856961, -105.3520746957046 39.95872122336939, -105.3521102839133 39.95867938499769, -105.35212220401 39.95863842500425, -105.3521104398092 39.95860745169789, -105.3520702935195 39.95856915836187, -105.3519260940527 39.95849795111383, -105.3517903015078 39.95841226836524, -105.3516327162817 39.95825478871504, -105.3515030716467 39.95806517346453, -105.3514385408322 39.95783632304158, -105.3514614232365 39.95763062854918, -105.3516543984425 39.95738535951605, -105.3519882100022 39.95711141236313, -105.3522487218811 39.95692587313406, -105.3526579361303 39.95670835306336, -105.3530862636785 39.95657473750998, -105.3533690273359 39.95650551578468, -105.3536895321031 39.9564987737959, -105.3540065873437 39.95656501021908, -105.3544637367979 39.95665966283416, -105.3547191238183 39.95666362646298, -105.3549249516538 39.95662020943129, -105.3552374249272 39.95646773426095, -105.3554859298368 39.95637159505921, -105.3556823119012 39.95632088393366, -105.3558505676371 39.95630145846711, -105.3557992750611 39.95602245334246, -105.3557741141502 39.95576549921196, -105.3557386458138 39.95566937293702, -105.3557060233276 39.95561276915417, -105.3556469662596 39.95556472809908, -105.3555265701328 39.95553835283317, -105.35533130302 39.95549197808626, -105.3551509598883 39.955420341284, -105.354983454261 39.95532837636013, -105.3548194703378 39.95514520178909, -105.3547633005575 39.95493811633833, -105.354806468642 39.95460040077084, -105.3548830434188 39.95440920980376, -105.3549020387573 39.95421263782769, -105.3547589612953 39.95378709435537, -105.3544950960814 39.95337569701889, -105.354328387966 39.95314314435302, -105.3542544405529 39.95297147602072, -105.3544141255283 39.95269311604522, -105.3546227298896 39.95232853300234, -105.3546986643523 39.95203973189982, -105.3546976459791 39.951916725421, -105.354696493764 39.95184504081303, -105.3546691554396 39.95177685194528, -105.3545945513623 39.95167804960032, -105.3543318430792 39.95143562611569, -105.3540492663155 39.95118040016152, -105.3537479616793 39.95090835791643, -105.353706951089 39.95054013413743, -105.3535977264722 39.95029109927498, -105.3534278442595 39.95000483331427, -105.3532453961211 39.94974103325151, -105.3531911033443 39.94957306478888, -105.3531914570367 39.94940864067144, -105.353246801853 39.94908729334558, -105.3534345654886 39.94866188254792, -105.3535091801626 39.94851899837285, -105.3535095024001 39.94836886940653, -105.3533754572079 39.94807201753893, -105.3531236142911 39.94767376819163, -105.3528824496291 39.94735108971799, -105.3528263263688 39.94711130763148, -105.352854191666 39.94687038990777, -105.3528397428303 39.94667371057839, -105.3526547492991 39.94631602639261, -105.3524040429403 39.94599939878466, -105.3522201694978 39.94592290094791, -105.3520502790885 39.94594445355338, -105.3519560576344 39.94598776664162, -105.3518405762703 39.94601937441158, -105.3517208975748 39.94600567457899, -105.3516026725817 39.94597137759611, -105.3514444997917 39.94588811076953, -105.3513546245374 39.94579577849958, -105.3511027920363 39.94548997156586, -105.3509050233133 39.94529359798763, -105.3505838167 39.94513865452713, -105.3503982828856 39.9450347527661, -105.350300970492 39.94493811658024, -105.3502832029022 39.94481336976445, -105.3503120243307 39.94458459468469, -105.3503112624806 39.94448059585778, -105.3502143510659 39.94420166014947, -105.3500575626043 39.94379875040127, -105.3500026987519 39.94362534593829, -105.3498445102611 39.94343981278547, -105.3497053349327 39.9433752893389, -105.3495243107314 39.94333573399553, -105.3493059779342 39.94336762004309, -105.3491340108557 39.94343173423461, -105.3490129147341 39.94359242734798, -105.3487423315608 39.94414969374191, -105.3486259823145 39.94430691253987, -105.3484437905829 39.9444187019977, -105.3482453905888 39.94452739768072, -105.3481372522787 39.94476370979286, -105.3479977654047 39.94483858920728, -105.3478766414147 39.94483201306166, -105.3476077831022 39.94478806418913, -105.3473618750095 39.94468761993063, -105.3470789371956 39.94453354237368, -105.3468933634192 39.94445108312228, -105.3465051621862 39.94434773235889, -105.3463368710556 39.94425756130052, -105.3463274436908 39.94416437045862, -105.3463787208825 39.94407865046045, -105.3464923497525 39.94400257219984, -105.3466895263439 39.94394785691841, -105.3468249318228 39.94390409492455, -105.3469458653255 39.94381846726618, -105.3470014923789 39.94370856024724, -105.3469741140173 39.94364693072029, -105.3468813323513 39.9436039136981, -105.3466264719512 39.94357602811639, -105.3461619038107 39.94351265458335, -105.3458521496769 39.94348923147759, -105.3457354489024 39.94342004628592, -105.3457141629159 39.94332550653542, -105.3457536159009 39.94326998077975, -105.345841741395 39.9432602869895, -105.3459996916824 39.94329175730961, -105.3462238298761 39.94330439209571, -105.3464080083053 39.94323924565847, -105.3464764128338 39.94315766084034, -105.3465029621614 39.9431100037764, -105.3465102514326 39.94306756376609, -105.3464971988181 39.94302076089416, -105.3464276688434 39.94296347566614, -105.3461191802726 39.94278303907976, -105.3459129593672 39.94262678691265, -105.3455888314258 39.94217652562062, -105.3455008873075 39.94208291329695, -105.3453157028288 39.94183245170021, -105.345260220683 39.94172514236121, -105.3452994412459 39.94161807458997, -105.3454790206228 39.94148594525846, -105.3456232594566 39.94136103208576, -105.3456936576798 39.94124233435014, -105.3456794784697 39.94114306213983, -105.345615264635 39.94108360484331, -105.3455381459786 39.94104387979846, -105.3454334287735 39.9410140239936, -105.3453117618755 39.94100848106682, -105.3450852114466 39.94102997251904, -105.3448614030582 39.94115051238641, -105.3446456843429 39.94134535515964, -105.3445461638083 39.94154136582213, -105.3445315828068 39.94172656519589, -105.3445047050119 39.94184048084426, -105.3444750322293 39.94189565912026, -105.3444167376543 39.94194527050977, -105.3443649776773 39.94197293540188, -105.3443022889449 39.94198370270044, -105.344249041942 39.94197639575263, -105.3442083965542 39.94193895905808, -105.3441408110076 39.94183801666134, -105.3441087282511 39.94165209942394, -105.3440588417544 39.94157217882472, -105.3440180360536 39.9414596316175, -105.3441504891605 39.94123572850936, -105.3444201768378 39.94090922146732, -105.3446045737641 39.94074602105159, -105.3448738103961 39.94061565635842, -105.3452125109515 39.94050206995038, -105.3455340356399 39.94031737702138, -105.3458940131122 39.94017027039276, -105.3462908554426 39.93994198794666, -105.3465605025822 39.93965010336079, -105.3466027453232 39.93944998874962, -105.3466367324471 39.93921113490654, -105.3467565528364 39.93909550958383, -105.3470468203971 39.93901336640935, -105.3473049946615 39.93897551567823, -105.3476625902587 39.93895811649597, -105.3480247199548 39.93897680428015, -105.3483566129954 39.93906216994667, -105.3491629100225 39.93940835371188, -105.3498018128802 39.9396293548314, -105.3502194413498 39.93976572926093, -105.3503294207818 39.93976661884747, -105.350400661343 39.93971234687233, -105.3503915615324 39.93962654754644, -105.3501228431005 39.93934738838904, -105.3499051285607 39.93910404030952, -105.3497608354034 39.93903131515625, -105.3489173950713 39.93849151148685, -105.3485663290427 39.93847499271768, -105.3482955902814 39.93838219132165, -105.3481168738894 39.93835503070434, -105.3479497636173 39.93835181827158, -105.3478098587675 39.93834864154184, -105.3477165832549 39.93834851827387, -105.3476427485254 39.93834542866371, -105.3475339681682 39.93832733465823, -105.3474407528604 39.93830028702409, -105.3473708908066 39.93825831035578, -105.3472699713123 39.9382013334698, -105.3472311803472 39.93816837384888, -105.3471458595813 39.93808748619713, -105.347083770364 39.9380455196671, -105.3469867370542 39.93798854768993, -105.346881985164 39.93790763402901, -105.346796571137 39.93786862831799, -105.3466761661568 39.93783555903681, -105.3465673868684 39.93781746411783, -105.3464624809674 39.93780535822026, -105.346357547 39.93780521831134, -105.3462526142029 39.93780507830835, -105.3461399078266 39.93780492782732, -105.3460427137029 39.93781975607154, -105.3459610115226 39.93785853899554, -105.3458169574422 39.93797202983635, -105.345774126217 39.93800787266722, -105.3457078670991 39.93809155129362, -105.3456999526396 39.93815436688384, -105.3456336662278 39.93825001155182, -105.3455869479147 39.93828584910379, -105.3455324096934 39.93834261821461, -105.3454701315971 39.93838441881511, -105.3453961873443 39.93842919480537, -105.3453141688943 39.93859363192674, -105.3453174834947 39.93873308230828, -105.3453324758724 39.93894757124433, -105.3453478192813 39.93900716756229, -105.3452854454025 39.93920963782646, -105.3451764562121 39.93935034054514, -105.3450992150013 39.93942385726057, -105.3448396699272 39.93948645664532, -105.3446657570558 39.93944710316149, -105.344384129159 39.93940398872251, -105.3442635820429 39.93932741052702, -105.3440806476839 39.93926808631675, -105.3439079255175 39.93917203517659, -105.3437689444899 39.93902886666783, -105.3437227820638 39.93890965441344, -105.343645771096 39.93874274023654, -105.3434795630392 39.93860290917354, -105.3433831552227 39.93851599989166, -105.3431822898061 39.93836083262784, -105.3430840868266 39.93827947499772, -105.3428732685956 39.93812211134178, -105.3427297277895 39.93806265947011, -105.3424400931839 39.93802619959498, -105.3422698308905 39.93802596659072, -105.3420222592663 39.93798988298423, -105.3418208462812 39.93807301188947, -105.3417123320203 39.93814435154387, -105.3416192681011 39.93822762982641, -105.341515849407 39.93836323363961, -105.3414020988481 39.93842988418462, -105.3412781318281 39.93848928917005, -105.3411230970743 39.93859630941661, -105.3410336766268 39.93871870956254, -105.3410450662076 39.93887024632174, -105.3410447332516 39.93901322507722, -105.3410443447997 39.93918003422367, -105.3410282836238 39.93943022612975, -105.34099674378 39.93968039576468, -105.340980932132 39.93982335404601, -105.3409897233237 39.94002551761, -105.3409808920442 39.94028805576299, -105.3410412926193 39.94049067422415, -105.3409326348646 39.94062158865495, -105.3408703853 39.94076448278047, -105.3406533181873 39.94091907671124, -105.3404674572864 39.940966480408, -105.3401886114176 39.94106141307962, -105.3401421178431 39.94108517813758, -105.3399406107836 39.94120404886886, -105.339832060449 39.94128730237721, -105.339630748214 39.94132276755802, -105.3393828295825 39.94142965521113, -105.3393363074271 39.94146533648792, -105.3393233416274 39.94161898118039, -105.3392428151568 39.94172733397711, -105.3392114080417 39.9419179302638, -105.3390715885114 39.94213220471062, -105.3389010628894 39.9422392012124, -105.338513937799 39.94229823311669, -105.3382505347019 39.94240509842705, -105.3380491323672 39.94247630506577, -105.3377548544015 39.94254738149012, -105.3375226061463 39.94257088373504, -105.3372129605016 39.94259427617204, -105.3369187084585 39.94265343391514, -105.3367018532639 39.94271270244277, -105.3363922364222 39.94272417883428, -105.3360516872704 39.94272369469476, -105.3358194951483 39.94272336402315, -105.3355252712221 39.94277060346691, -105.3352777722196 39.94269876025473, -105.3350612033855 39.94263887467899, -105.3348139071973 39.94248362637954, -105.3346597191067 39.94223319204949, -105.3345673052172 39.94204242014799, -105.3345957688523 39.9417773393035, -105.3346303196934 39.94158974164895, -105.3346773338235 39.94135150985174, -105.3346157633717 39.94120844226929, -105.3344961789176 39.94099717557393, -105.3342914539426 39.94089818733744, -105.33424524894 39.94080279988832, -105.3342300595007 39.940683629287, -105.3342187703895 39.94049634854602, -105.3344784168929 39.94039802796743, -105.3347416450673 39.94036266062547, -105.3349893366625 39.94035110089884, -105.3353456676618 39.9402205463219, -105.3355624587094 39.94018510982277, -105.3356713555442 39.93995888250201, -105.3356098428274 39.93979198504802, -105.3355636642642 39.93968468337358, -105.3353162913976 39.93956518034897, -105.3350997900354 39.9394814671437, -105.3349760472421 39.93944554468823, -105.3347906766642 39.93929038497647, -105.334605279229 39.93914713971061, -105.3345127252388 39.93901594144148, -105.3344355343734 39.93893242522267, -105.3342964869261 39.9388249913192, -105.3341728325842 39.9387533228644, -105.3339407409348 39.93871724417198, -105.3338326803261 39.93859793868223, -105.3337554338947 39.93853825329758, -105.3337092010423 39.93845478035888, -105.3334821172266 39.93789782489326, -105.3327829133291 39.93746449862973, -105.3325662183295 39.93746418386972, -105.3323184782625 39.93749956787977, -105.332163519595 39.93757083274084, -105.3319930238681 39.93766590340954, -105.3317141785255 39.9377608164918, -105.331559101029 39.9378797395179, -105.3314351864608 39.9379153035246, -105.3312028634002 39.93797453727169, -105.3310941896124 39.93810544244619, -105.3310164730188 39.9382363938341, -105.3309541765365 39.93839119647253, -105.3308299347333 39.93855782381141, -105.3306129394301 39.93867665461612, -105.3304578579342 39.93879557615114, -105.3303646313504 39.93893841725295, -105.3303333191918 39.93908135218683, -105.3303173668751 39.93927196798317, -105.3302550370624 39.93943868497224, -105.3301771394815 39.93964112423741, -105.330037503932 39.939771983658, -105.3298048465427 39.93996227854622, -105.3296652107925 39.94009313751392, -105.3295720093546 39.94022406411649, -105.3294013842727 39.94036679079821, -105.3292308777148 39.9404618573578, -105.3289675567365 39.94053295723312, -105.328363397086 39.94072269795484, -105.3280464391735 39.94068518217745, -105.3277290582858 39.94060260054161, -105.3275436118999 39.94048317340886, -105.3273737955304 39.94030419546518, -105.3272230655047 39.94017627980257, -105.3270338333477 39.94007730187811, -105.326848479111 39.93992212849384, -105.3267233057162 39.93972059487754, -105.3264008665194 39.93942102655195, -105.326510155908 39.93905182646767, -105.3266788045178 39.93861631287486, -105.3269504474838 39.93818943437444, -105.3269152288096 39.93801583390401, -105.3268536776333 39.93787276303662, -105.3268076059926 39.93772971450777, -105.3266840208323 39.93763420851904, -105.3266223796962 39.9375268817555, -105.3264369133073 39.93741936755629, -105.326332444717 39.93736300821741, -105.3260812174063 39.93729968138211, -105.3258956297566 39.93723982618449, -105.3256479783452 39.93723945161755, -105.3253848794217 39.9372271383133, -105.3251372891076 39.93720293135949, -105.3248586806939 39.93720250809899, -105.3246419865635 39.93720217843251, -105.3243941513812 39.93727329143306, -105.3242700796447 39.93736842144941, -105.3241615174665 39.9374516611181, -105.3238359511774 39.93765371783137, -105.3231420733671 39.93807305242971, -105.3227684117605 39.93860002799841, -105.3229032642183 39.93918931809423, -105.3227789715475 39.93936785058116, -105.3225929785905 39.9394628853095, -105.3222368443683 39.93950999545962, -105.3220975354618 39.93950978040615, -105.3218807395759 39.93954518976606, -105.3213232553279 39.93963964654615, -105.3212456742569 39.93971101672305, -105.3211522710472 39.93991342586091, -105.3211365426721 39.94000872155141, -105.3210277850324 39.94016344578863, -105.3209655879741 39.94027058403997, -105.3207332478084 39.94032979846212, -105.3204701065221 39.94032938867544, -105.3198388293764 39.9404390245125, -105.3191692463489 39.94056565340757, -105.3189680191451 39.94056533736213, -105.3186740765611 39.9405053002228, -105.3183802624779 39.94039760247852, -105.3179781597508 39.94026590245163, -105.3175447179208 39.94027713156014, -105.3172351396482 39.94027664082628, -105.3169565199088 39.94027619845558, -105.3166467816132 39.94033528163523, -105.316476321442 39.94040649983918, -105.3163519765155 39.9405969410111, -105.3163205701327 39.94076369979045, -105.3162423730982 39.94106144931301, -105.316195455252 39.94124009899878, -105.3159009337462 39.94139452276405, -105.3156220829817 39.94147748302713, -105.315393589911 39.94149240574951, -105.3149875012233 39.94145263516127, -105.3148020101678 39.94135701700087, -105.3146322573936 39.94116610555177, -105.3143695989769 39.94098695806902, -105.3142307086453 39.9408318392145, -105.3142470304991 39.9405220764947, -105.3141701546706 39.94033131316758, -105.3141398137156 39.9401048796018, -105.3140940256521 39.93986650720636, -105.3140018023195 39.93962805802159, -105.3139564708813 39.93922287561901, -105.3139259350723 39.9390679331113, -105.3136326539993 39.93876958471586, -105.3135248903767 39.93855494046591, -105.3135409870585 39.938328582769, -105.313541572907 39.93811411295194, -105.3135728884073 39.93798309911708, -105.3135886919486 39.93786397586513, -105.3135582226762 39.93768520106113, -105.3135586131968 39.93754222327778, -105.3135281127685 39.93737536320363, -105.3135443067977 39.93711326126337, -105.313668360496 39.93703005663828, -105.3138543255822 39.93694695284194, -105.3140710200188 39.93694730280319, -105.3142952267474 39.93694088522145, -105.3144116361982 39.93691210769416, -105.3146129496925 39.93687668567372, -105.3147370974993 39.93675773567037, -105.3149541789319 39.93661510617261, -105.3151556836821 39.93650819475129, -105.3151716143362 39.93634141140234, -105.3152646112064 39.93629390050486, -105.3152959536364 39.93615097053843, -105.3153426458871 39.93605572614626, -105.3153428715063 39.93597232205011, -105.3151730015705 39.93582906938609, -105.3151269546172 39.93568601616223, -105.3150107817862 39.93562102376601, -105.3152947463766 39.93560825239187, -105.3189277387964 39.93544482213235, -105.3191391063055 39.9317901419817, -105.3205148429798 39.9317151039824, -105.3239541807884 39.93152857193745, -105.3240442233703 39.93038144497817, -105.3242555787687 39.92783278270667, -105.3240379379819 39.92434240818668, -105.3238539754728 39.92139180765506, -105.3238336179889 39.92104928059182, -105.3238185156393 39.92104925748924, -105.3236539993554 39.92104899939051, -105.3232179993169 39.92095999891312, -105.3230946808704 39.92091515582619, -105.3230754639435 39.92090816782166, -105.322810999039 39.92081199876494, -105.3228091235898 39.92081034046993, -105.314962656992 39.91387604616386, -105.3186637285294 39.91384134022072, -105.3212698069163 39.91381682948519, -105.3215006511357 39.91381465579448, -105.3227129433033 39.91380322945029, -105.323354140306 39.91379718248584, -105.3279073637289 39.9138067691513, -105.3323281555307 39.91381591637837, -105.3325418885809 39.91381635798417, -105.3328397048168 39.91381390137353, -105.334524796101 39.91379991975911, -105.3357223963508 39.91378996644013, -105.3360327017027 39.91378738519001, -105.3409074326082 39.91374673320104, -105.3419491615664 39.91373801818488, -105.3426961315184 39.91373050995593, -105.3464788027438 39.91369240329173, -105.3513537524865 39.91364310980608, -105.3528087207196 39.91361749517808, -105.3535508659689 39.913604419963, -105.3570569970404 39.91354257768043, -105.3575647191606 39.91353361299981, -105.3577143168157 39.91353096987616, -105.3578080288027 39.9135293149364, -105.3579479405976 39.91352684688559, -105.360726387632 39.91347774057059, -105.3626713467703 39.91344411322467, -105.3630360175505 39.91343780431702, -105.364028600592 39.91342062611375, -105.3654597559985 39.91339584487707, -105.3658523373689 39.91338904538176, -105.3665939284883 39.91337619259116, -105.3667161394004 39.91337407345735, -105.3668283884871 39.91337212820923, -105.3681499654785 39.9133492123433, -105.3687455638757 39.91333888041709, -105.3700998449686 39.91331537600603, -105.3701987914307 39.91331435275244, -105.3702803654887 39.91331351699651, -105.3713686533495 39.91330235646162, -105.3715726433937 39.91330026315164, -105.3723180191877 39.91329261324411, -105.3727062091699 39.91328862708968, -105.3728444536078 39.91328720727761, -105.3729372325635 39.91328625411846, -105.3730265786787 39.91328533762903, -105.3741243196769 39.91327405429676, -105.3746287719808 39.91326886562454, -105.3750805012749 39.91326421559691, -105.375528444443 39.91325960653901, -105.3759644480829 39.91325511617619, -105.3764989569724 39.91324961123397, -105.3770298750515 39.91324413780398, -105.3775644726632 39.91323862530895, -105.3781002538376 39.91323310077718, -105.3786426970783 39.91322750061524, -105.3791513838786 39.9132222497599, -105.379874445467 39.91321461308471, -105.3805848188801 39.91320710461893, -105.3814863544534 39.91319756945008, -105.382202498405 39.91318998939478, -105.3829076244009 39.91318252337764, -105.3837367354787 39.91317373903913, -105.3845278911197 39.91316534929708, -105.3850657205366 39.91315964310123, -105.3857696657633 39.91315217189074, -105.3863071920433 39.91314646229795, -105.3868507323952 39.91314068765575, -105.3874265259714 39.91313456821035, -105.3881273864053 39.91312711559791, -105.3888784839925 39.91311912178179, -105.3895167349293 39.91310925226507, -105.3900743869313 39.9131006235636, -105.3913934750771 39.91308020089357, -105.3917814950745 39.91307419044647, -105.3921958186435 39.91306777010362, -105.3926274455239 39.91306108069853, -105.3930632080981 39.91305432866896, -105.3934766670766 39.91304791642477, -105.3935153909127 39.9130473154753, -105.394319146609 39.9130348477802, -105.3952755188074 39.91302000864341, -105.3958087301344 39.91301172983554, -105.3964937997429 39.91300134792505, -105.3965903464187 39.91299959372266, -105.3966978356719 39.91299792220955, -105.3968488757159 39.91299557539469, -105.3983183962212 39.9129727357535, -105.3983210341569 39.91298417823263, -105.3983219324942 39.91301396556613, -105.3983223459219 39.91302772707497, -105.398333431356 39.91339613543983, -105.398333844787 39.91340989784895, -105.3983522526618 39.91402148383398, -105.3983526672674 39.9140352480448, -105.3983778425658 39.91487183135766, -105.3983782571737 39.91488560097144, -105.3983798343123 39.91493793235012, -105.3983802489236 39.91495170016253, -105.3983820599438 39.9150119224053, -105.3983824745547 39.91502569111829, -105.3984018106093 39.91566807851793, -105.3984022252254 39.91568184903149, -105.3984202050643 39.91627928250205, -105.3984208825517 39.91629325949732, -105.3984243463552 39.91635977428161, -105.3984245531202 39.91637331764547, -105.3984245542349 39.91637335457343, -105.3984250501899 39.9164385995149, -105.3984254133924 39.91645234206192, -105.3984493646693 39.91724802529494, -105.3984496473764 39.91726163177085, -105.398449648455 39.91726169301648, -105.3984507589101 39.91732038081131, -105.3984512786714 39.91733424868674, -105.39845370355 39.9173931285796, -105.3984541450573 39.91740692073075, -105.3984665193604 39.91781805006798, -105.398466933988 39.91783183048639, -105.3984798536997 39.91826093109985, -105.3984803290957 39.91827475210088, -105.3984828140969 39.91834515684929, -105.3984831785016 39.91835889218999, -105.3984848565185 39.91842687435983, -105.3984852594673 39.91844064756203, -105.3984990197162 39.91889776022787, -105.3984994355225 39.91891154334807, -105.3985162065597 39.91946874595399, -105.3985166959705 39.91948259218443, -105.3985205360901 39.91958806339631, -105.3985208900887 39.91960172667393, -105.3985208911554 39.91960179602547, -105.3985233411816 39.91970523863268, -105.3985237406861 39.9197189785061, -105.3985237406312 39.919719015433, -105.3985355249807 39.92011052426341, -105.3985359396254 39.92012431188453, -105.3985367254955 39.92015040730921, -105.3985371413104 39.9201641949313, -105.3985453221885 39.92043585466617, -105.3985457368344 39.92044964408826, -105.398546602953 39.92047841723579, -105.3985470187679 39.92049220755951, -105.3985604243746 39.92093742396103, -105.3985608390226 39.9209512160845, -105.3985652321848 39.92109710564678, -105.398565646836 39.92111089686941, -105.3985675196082 39.92117307806518, -105.3985679354288 39.92118687018941, -105.3985696120286 39.92124252415203, -105.398570026679 39.92125631717582, -105.3985772446762 39.92149599281457, -105.3985776593297 39.92150978583809, -105.3985781866026 39.92152729777273, -105.3985786012565 39.9215410907962, -105.398586678742 39.92180934142345, -105.3985870945678 39.92182313534828, -105.398594726368 39.92207647430345, -105.3985951410246 39.92209027002828, -105.3986023824908 39.92233080219584, -105.398602611461 39.92234439510914, -105.3986026125611 39.92234444194428, -105.3986027046735 39.92235094386645, -105.3986030959543 39.92236472876249, -105.3986114287511 39.92263132959327, -105.3986118213059 39.92264425886626, -105.3986118469183 39.92264512892318, -105.3986201020632 39.92291916730255, -105.398620516726 39.92293296572834, -105.3986229603509 39.92301411614823, -105.398623328441 39.92302776862658, -105.3986233306174 39.92302787850861, -105.3986247646202 39.92308232446863, -105.398625211001 39.92309603375719, -105.398625214331 39.9230961544481, -105.3986271203261 39.92315257776472, -105.3986275443485 39.92316637709919, -105.3986363458028 39.92345860470918, -105.3986367616392 39.92347240493673, -105.398640059122 39.92358199884207, -105.3986404340673 39.92359576570926, -105.3986593239096 39.92430639952359, -105.3986596895086 39.92432016367973, -105.3986610423362 39.92437101684337, -105.3986614091043 39.92438478190112, -105.398661938663 39.92440472380518, -105.3986623593045 39.92441844657942, -105.3986623615104 39.92441853664702, -105.3986642149489 39.9244773133269, -105.3986646506542 39.92449113338527, -105.3986653789949 39.92451428450352, -105.3986658147006 39.92452810456187, -105.3986735254079 39.92477281614058, -105.3986739611156 39.92478663709926, -105.39867628483 39.92486039120937, -105.3986767205375 39.92487421306861, -105.3986809267899 39.92500765354416, -105.3986813624992 39.92502147540325, -105.3986843521299 39.92511632167318, -105.398684787838 39.92513014533341, -105.3986860592404 39.92517046344225, -105.398686493782 39.92518428530008, -105.3986874544791 39.92521483371372, -105.3986878901898 39.9252286564732, -105.3986946649734 39.92544356989327, -105.3986950995171 39.92545739265146, -105.3986961730707 39.92549151406815, -105.3986966087809 39.92550533952928, -105.3986987962665 39.92557475415193, -105.398699587186 39.92558885822826, -105.3987008331634 39.92560926820119, -105.3987008308551 39.92562265015393, -105.3987008308083 39.92562268167683, -105.3987007035779 39.92563195472458, -105.3987010318213 39.92564567651554, -105.3987010329363 39.92564571344339, -105.3987025021679 39.925692263367, -105.3987029378834 39.92570608702656, -105.3987088054537 39.92589230022041, -105.3987092411689 39.92590612568109, -105.3987157668427 39.92611320315834, -105.3987162025581 39.92612703042011, -105.3987165086773 39.9261367442696, -105.398716944397 39.92615056882935, -105.3987174180642 39.92616562461984, -105.3987178537816 39.92617945098084, -105.3987232153443 39.92634959330871, -105.3987236510628 39.9263634205702, -105.3987268664642 39.92646544706136, -105.3987272813745 39.92647910768292, -105.3987272858266 39.92647926079844, -105.3987277296268 39.92649394999507, -105.3987281781977 39.92650778897621, -105.3987286203391 39.92652123076214, -105.3987290595639 39.92653506162907, -105.3987454149852 39.92705399372688, -105.3987453775411 39.92706740897156, -105.3987094196417 39.9305860929671, -105.3987092828172 39.93059946128667, -105.398687214628 39.93275895406263, -105.3986870777828</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>21</v>
-      </c>
-      <c r="E16" t="n">
-        <v>21</v>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Nederland HS</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>597 Co Hwy 130, Nederland, CO 80466</t>
+        </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Nederland HS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>597 Co Hwy 130, Nederland, CO 80466</t>
+          <t>https://neh.bvsd.org/</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
+          <t>Nederland Middle/Senior High School</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>39.95383849383303</v>
+      </c>
+      <c r="K16" t="n">
+        <v>-105.5233421126253</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
           <t>https://neh.bvsd.org/</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>Nederland Middle/Senior High School</t>
-        </is>
-      </c>
-      <c r="L16" t="n">
-        <v>39.95383849383303</v>
-      </c>
-      <c r="M16" t="n">
-        <v>-105.5233421126253</v>
-      </c>
       <c r="N16" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>https://neh.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr">
         <is>
           <t>POINT (-105.5233421126253 39.95383849383303)</t>
         </is>
@@ -1600,19 +1500,49 @@
           <t>POLYGON ((-105.2665028856773 40.00008302921293, -105.2677639960641 40.0000800858277, -105.2687848652311 40.00008103962393, -105.2700220559592 40.00007912146844, -105.2712538896729 40.0000780026072, -105.2724860869347 40.00007495020975, -105.2737168453467 40.00007490171039, -105.2749419062467 40.00007098586583, -105.2749439353011 40.00183587613848, -105.2749439861859 40.0018452979681, -105.2749541445287 40.00371800203029, -105.2761939054203 40.00371410054612, -105.277421161032 40.00371400557973, -105.2774251347819 40.00413704801434, -105.2774248286698 40.00433991763281, -105.2774230429322 40.00488703093239, -105.2774240231571 40.00546187703087, -105.2778681120404 40.00545888939006, -105.2786630827622 40.00546398736055, -105.2798871783135 40.00545699704956, -105.2799030378844 40.0072899927621, -105.2811321477586 40.00728794062378, -105.2819328809913 40.00728396638529, -105.2819728960741 40.00727388539485, -105.2820611343066 40.00725401178327, -105.2831478234024 40.00724700172137, -105.284303060725 40.00723708977463, -105.2855649684075 40.00724905147178, -105.2864738555099 40.00724909075706, -105.2869468595005 40.00724996565361, -105.2872299698913 40.0072430760162, -105.2876390732287 40.00724410484807, -105.2884758772812 40.00723493682361, -105.2890631285643 40.007231894771, -105.2890970445134 40.00723113361098, -105.2891459174028 40.00724192903881, -105.2891968309264 40.00728594512627, -105.289223168539 40.00742709573112, -105.2892639375149 40.00751913492665, -105.2893250772793 40.0076040727572, -105.289405168331 40.00767888851305, -105.2895010031458 40.00774192810649, -105.2896179351386 40.00779402536224, -105.2897431274692 40.00782994113508, -105.2898541047652 40.00784496816384, -105.2900128690378 40.00787600294159, -105.2901651591649 40.00792294834658, -105.2903059756377 40.00798607001173, -105.2904830588015 40.00809702258108, -105.290661065552 40.00825601822979, -105.2907819711598 40.00840996903745, -105.2908690869226 40.00844982779828, -105.2914292843717 40.00892559132514, -105.2914292099533 40.00893843358583, -105.2908119707734 40.00893655268581, -105.2900712087696 40.00893743474369, -105.2900702103074 40.00921343500197, -105.2903549358019 40.00921443393288, -105.2906932101914 40.00921443417534, -105.2906925531651 40.00929912848419, -105.2906912943824 40.00945966739491, -105.2906902700733 40.00962089482662, -105.2906892101524 40.00976243394203, -105.2906912103231 40.0098434340922, -105.2906906047592 40.01003956613808, -105.2906912104696 40.01034743433848, -105.290154209284 40.01034543526126, -105.2901552136538 40.0103924349007, -105.2900632101764 40.01038843427113, -105.29015521014 40.01039243489431, -105.2904481483452 40.01050448448408, -105.2907130561806 40.01063845205723, -105.2910521068837 40.01081245315488, -105.2913502088046 40.0109674357598, -105.2914002106621 40.01099343436549, -105.2915172102254 40.01104143452457, -105.2915192101345 40.01082443421697, -105.2916219709538 40.01082393365192, -105.2918546625634 40.01082371352069, -105.2921922106798 40.01082443486659, -105.2921912106079 40.01114143453822, -105.2921692110959 40.01143943493722, -105.2922312110156 40.01149543479373, -105.2922312110259 40.01162343450338, -105.2924722100788 40.01164043413667, -105.292480210274 40.01167843441603, -105.2926421528956 40.0116779178345, -105.2931072112711 40.01167643394096, -105.2931065501837 40.01189546581841, -105.293105976447 40.01208570852052, -105.293105211251 40.01233943420036, -105.2927022113221 40.01233843488738, -105.2926981092893 40.01260199958435, -105.292694211126 40.01285243494313, -105.2927912101938 40.01285643433663, -105.2931333503741 40.0128564352352, -105.2935512109194 40.0128564346988, -105.2936372113 40.01280243515163, -105.2938052106283 40.01277843517675, -105.2942141485911 40.01273466443779, -105.2948142108489 40.01267043461998, -105.2948072105055 40.01255543418904, -105.2948072112871 40.01214143441656, -105.2952052115695 40.01213443502252, -105.2953132109346 40.01212543471485, -105.2954662113391 40.01215043446568, -105.2957822123902 40.01218343415776, -105.2957852116624 40.012505434982, -105.295809211419 40.01257043426351, -105.2961832109625 40.01252843470885, -105.2969222108167 40.01264143451774, -105.2969212186651 40.01238543430799, -105.2969202114587 40.01211443461543, -105.2972624798172 40.01217012068312, -105.2974242114839 40.01219643372481, -105.2974275838077 40.01218258042406, -105.2974892276555 40.01192397025246, -105.2975392118156 40.01170843394527, -105.2976410500742 40.01171848383155, -105.2976912121973 40.01172343446013, -105.298122211411 40.01176843426795, -105.2984517355405 40.01181772238958, -105.2985718404069 40.01183568677898, -105.2986066136606 40.01177065292691, -105.2986916238546 40.01160627754996, -105.2992927086213 40.01167132375566, -105.2994896376608 40.01169225972444, -105.2993653365875 40.01249054937211, -105.2993753074033 40.01249150609813, -105.2993692121943 40.01253043425595, -105.299705267281 40.01255424261292, -105.3002518157827 40.01259380600695, -105.3004884530218 40.01261020130202, -105.3007216280422 40.01262778439228, -105.3007216232754 40.01262781230426, -105.3007216161107 40.01262785912573, -105.3007562324528 40.01263038942474, -105.3008117447473 40.01263456076815, -105.3009032128719 40.01264143397508, -105.3009735379753 40.01278267752139, -105.301023340076 40.01288285103966, -105.3010281067779 40.01289306454397, -105.3010292126056 40.01289543426423, -105.3011202771397 40.01296410208901, -105.3011419577046 40.01298029445854, -105.3011632841785 40.01299621061416, -105.3011729464176 40.01300340546396, -105.3011729942204 40.0130034812011, -105.3011764667329 40.01300603603117, -105.3011789468909 40.01300787493373, -105.301205212717 40.01302743462566, -105.3012592457636 40.01298185572877, -105.3013522126834 40.01290343407975, -105.3014602128255 40.01281143480046, -105.3014452129743 40.01287743392142, -105.3014437804599 40.01293093194339, -105.3014430498437 40.01295818709555, -105.3014422127245 40.01298943465143, -105.3013862127445 40.01335443432603, -105.3013157480595 40.01351102356379, -105.3012602122003 40.01363443507628, -105.3012511657355 40.01363978016212, -105.3010182134563 40.01377743388108, -105.3010158302282 40.01400687156732, -105.3010146521981 40.01412034528163, -105.3010143555852 40.01412043663623, -105.3010065439604 40.01412285491573, -105.3009841703811 40.01413088704314, -105.3008359183136 40.01416110284114, -105.300684149682 40.01417292017293, -105.3005359990144 40.01416799685423, -105.300254092653 40.01412001668933, -105.300067868143 40.0140719279547, -105.3000011606622 40.01405287069223, -105.2996880626172 40.01392796986438, -105.2994309509394 40.01382595114303, -105.2990971694855 40.01369387506902, -105.2989748438362 40.01364891574665, -105.2987091069599 40.01356691986554, -105.2984361789157 40.01350193131028, -105.2981560643021 40.0134531259425, -105.2978951689382 40.01342411927098, -105.2975649848486 40.01340487234885, -105.297280077546 40.01340711706504, -105.2972629400945 40.01340708693889, -105.2968701231647 40.01343988732408, -105.2966129379867 40.013483906396, -105.2959720191087 40.01362689650804, -105.2955889946644 40.01372696689724, -105.2951188286011 40.01383593998661, -105.2948950990359 40.01391405477982, -105.2948279437313 40.01392601395955, -105.2948850709373 40.01404306065437, -105.2949111667633 40.01415099338725, -105.2949149278989 40.01420590378106, -105.2949106525785 40.01428611088715, -105.2948669406371 40.01436130597801, -105.2948050566042 40.01443646962085, -105.2945651847544 40.01463397060598, -105.2942962425791 40.01484536492688, -105.2941799322994 40.01493717604964, -105.2940456558378 40.01498431869415, -105.2935522291935 40.01508380053187, -105.2932648974691 40.01514153813964, -105.2929311934506 40.01520907552712, -105.2924838834105 40.01529960385942, -105.2916482773999 40.01546871123976, -105.2904817987244 40.01572217487955, -105.2891551001181 40.01599098183944, -105.2885419939298 40.01611983770974, -105.2878670067061 40.0162528717229, -105.2866812529073 40.01650245354258, -105.2865308262578 40.01653288651573, -105.2852128642166 40.01680605680808, -105.2850088672696 40.01684712918449, -105.2841060700353 40.01702607643248, -105.2840110981352 40.01704713596685, -105.2838089245483 40.01709196535331, -105.2837991589066 40.01709413112621, -105.2838869444426 40.01755905605179, -105.2839600121989 40.01782410420856, -105.2840818920156 40.01812191122571, -105.280344103938 40.01889429097838, -105.2800122511694 40.01792531871845, -105.2797922499383 40.0173063188877, -105.2796422519211 40.01688331794094, -105.2795172500427 40.01656331893992, -105.2793182480616 40.01593431868323, -105.2792882488983 40.01584331888502, -105.279283131531 40.01582838979826, -105.2790212496877 40.01506431947683, -105.2789422504309 40.01484831880367, -105.2788752505237 40.01466131864607, -105.278851249496 40.01459531880194, -105.2786822492777 40.01411631803115, -105.2786769521653 40.01410055096331, -105.278663968713 40.01410393231048, -105.2782030961592 40.01419611210767, -105.278005899344 40.01423306829994, -105.2775250367717 40.01432794849211, -105.2773539185385 40.01436001199994, -105.2764250735946 40.01453802385365, -105.2760611408061 40.01457602595389, -105.2746458800721 40.01458095527774, -105.2736219240902 40.0145838908234, -105.2725519067238 40.01458809993736, -105.2716550449331 40.01459291590101, -105.270220141546 40.01459912551402, -105.2689819637891 40.01460406242605, -105.2678219770818 40.01460804739548, -105.2662260626349 40.01461196195721, -105.2657616256185 40.01461332253763, -105.2646558644589 40.01461288522881, -105.2638765422727 40.01460508854388, -105.2630753109644 40.01461633090538, -105.2630299591908 40.01461696725389, -105.258420544823 40.01462569237854, -105.2583967697713 40.01738897110558, -105.2583835533824 40.017841051784, -105.2583845465005 40.01820405441318, -105.2583845261048 40.01916806167687, -105.2583865082488 40.02003406862268, -105.2583999303681 40.02054880387701, -105.2584077255942 40.02163362987389, -105.2583830465151 40.0223399835016, -105.2583789356683 40.02339906985873, -105.2583811009352 40.02450099341501, -105.258382877582 40.02551095323694, -105.2585261275946 40.02549395801625, -105.2588440818718 40.02545097495982, -105.2603669897415 40.02515904067031, -105.2609680305519 40.02503593129295, -105.2619428416898 40.02483590064909, -105.2634068292216 40.02453694257784, -105.2637180536465 40.02447608769097, -105.2639678550197 40.02441702917763, -105.2652839000161 40.02414601860607, -105.2665938779832 40.02387086387858, -105.2679109587122 40.02360394413302, -105.2682411423188 40.02458107234318, -105.2684139123429 40.02522791115344, -105.2684711463209 40.02519810372616, -105.268499879351 40.02514902278204, -105.2685628779465 40.02510412746538, -105.2686079015087 40.02509488435066, -105.2687318382624 40.02508607416824, -105.2689580821212 40.02502311364085, -105.2695930218969 40.02490194833804, -105.2698180480713 40.02488208254371, -105.2701351511876 40.02487695076279, -105.2705571374207 40.02490112502463, -105.2711471268735 40.02497888759054, -105.2711960062075 40.02499106319144, -105.271283153701 40.02498492246853, -105.2714558843878 40.02490702710772, -105.2715121215238 40.02496094431037, -105.2716481672724 40.02506800120462, -105.2724079619951 40.02551696877548, -105.2725230499857 40.02559186516272, -105.2725799692758 40.02565593982267, -105.2726199882499 40.02575512003067, -105.2726178873861 40.02606394994715, -105.2726181274602 40.02620587677047, -105.2726248698914 40.02675410445867, -105.2726378711389 40.02799495559294, -105.2726431137961 40.02931402807485, -105.2726510020113 40.03005387211383, -105.2726558625326 40.03073798238746, -105.2726628596342 40.03142401880926, -105.2726661710148 40.03160905132167, -105.272671164566 40.03193189473561, -105.2726760357997 40.03272004799683, -105.2726760239568 40.0331518655748, -105.2726820898275 40.03390296023866, -105.2726840628362 40.03406108764794, -105.2726881734809 40.03464911391067, -105.2726940852457 40.03630310060525, -105.272693011895 40.03641098462665, -105.2722969317176 40.03641486978847, -105.270493035731 40.03641102135016, -105.2685051665427 40.03642104917662, -105.268183023931 40.03642204958091, -105.2647380295588 40.03643099813947, -105.263225170679 40.03643586385155, -105.2622890950964 40.03643997857341, -105.2612830205331 40.03644393997342, -105.2605001712293 40.03644396467524, -105.2590269395231 40.03645297536733, -105.2585008484345 40.03646011079696, -105.258446899267 40.03646603760756, -105.258455895004 40.03685010807402, -105.2584720435084 40.03753396766986, -105.2584653846817 40.03890912737619, -105.2584811444412 40.04010595201317, -105.2576250499565 40.04010196086148, -105.2572561306026 40.04009487076375, -105.2570050616881 40.04009104854779, -105.2564700565923 40.04008607648185, -105.2541156704493 40.04008547509496, -105.2541114189239 40.04008556330383, -105.2541130449594 40.0400350024811, -105.2541075664353 40.03908055851134, -105.2536959323025 40.03907688210359, -105.2536949545598 40.03812015275444, -105.2535405399283 40.03814509251686, -105.2533805946551 40.03816870800271, -105.2532201543185 40.03819018946845, -105.2530592634851 40.0382095298022, -105.2528979772607 40.03822672371619, -105.2527363390311 40.03824176679848, -105.252574399222 40.03825465195054, -105.2524122082365 40.03826537837855, -105.252087273247 40.03828033297279, -105.2519246265246 40.03828456224724, -105.2517619181192 40.03828706191138, -105.2515262941062 40.03828575038629, -105.2500216866296 40.03828440663961, -105.2489428716393 40.03828342936805, -105.2476788464136 40.03828923237084, -105.2463663111993 40.03830715832521, -105.2456601157548 40.03831973388306, -105.2446044735468 40.03855084401205, -105.2425780966287 40.03862463649937, -105.2427781086196 40.03829124483734, -105.2430111166943 40.0379132414562, -105.2432991274496 40.03743023787163, -105.2438753893139 40.0364924229959, -105.2440929793375 40.03610011054108, -105.2444588367812 40.03552861301022, -105.2453730542609 40.03402702879499, -105.2462652351348 40.03255119866444, -105.2466014210446 40.03199231009842, -105.2468743915512 40.03153389625475, -105.2470384585521 40.03125730147787, -105.2470527888195 40.03123232722809, -105.2472377688188 40.03090995649731, -105.2474157554355 40.03059976586545, -105.2475764919784 40.03031963966591, -105.2477685658453 40.02998489963429, -105.247983553166 40.0296102141241, -105.2481541927388 40.02931308733002, -105.2482195454966 40.02920455652909, -105.2475199805581 40.02920302743363, -105.2471535866196 40.02920497006868, -105.2470046722872 40.02920574144774, -105.2467879073245 40.02920691310877, -105.2459758332215 40.02921391257004, -105.2448980525407 40.02922690726311, -105.2447080626234 40.02923005531607, -105.2441955801484 40.02923144538298, -105.2431311238466 40.02922408398609, -105.2400198840386 40.02917511185208, -105.2395431210193 40.02918391916977, -105.2382999573494 40.02920828260488, -105.2375975186471 40.02922070455187, -105.2365361783417 40.02922211126447, -105.2346081604372 40.02922894693484, -105.2335989823584 40.02923101313294, -105.2329054947644 40.02923023263606, -105.2326919485125 40.02923001266877, -105.2317567030328 40.02922893947044, -105.2312381944585 40.02922828192708, -105.2308360988211 40.02922789375545, -105.2303165160975 40.02922777805944, -105.2300240500278 40.02922791711205, -105.2291319973156 40.02923104149665, -105.2286845476068 40.02923108871217, -105.2275989594909 40.02923100067746, -105.2260059682783 40.02922091333762, -105.2259449032419 40.029221042971, -105.2258520567489 40.02922109704281, -105.2253876759348 40.02922707245764, -105.2253838715813 40.02922712104237, -105.2250902606939 40.02922118797638, -105.2243452592167 40.02922218854747, -105.2242922587597 40.02922218887095, -105.2240485290634 40.0292221896779, -105.2240448012386 40.02921896182992, -105.2234171967727 40.02858844157902, -105.2231341967773 40.02873844263139, -105.2227491964695 40.02893444274527, -105.2221531959837 40.02913544191373, -105.2220471963629 40.0291604417221, -105.2217758048782 40.02920913506678, -105.2216681962193 40.02922844212854, -105.2215368541062 40.02924212396792, -105.221524196698 40.02924344258807, -105.2213741961431 40.02925244173912, -105.2209515721532 40.02925336013067, -105.22047383285 40.0292534418192, -105.2199463053364 40.02925557303384, -105.2191025662913 40.02925881640458, -105.2185102178733 40.02926210714222, -105.2184761957898 40.02926244201551, -105.2180831955133 40.02926644208032, -105.2178571961912 40.02928944246727, -105.2177341859115 40.02931463718165, -105.2176198784911 40.0293380499647, -105.2175251954509 40.02935744244781, -105.2173882346814 40.02940610874885, -105.2172628810816 40.02945581657214, -105.2171013733368 40.02953197961455, -105.2170861959579 40.02953944212074, -105.2169183296271 40.02964944212096, -105.216714195362 40.02978944179781, -105.216393195045 40.030018442685, -105.2163231954602 40.03000344222524, -105.2162281958708 40.02996544241743, -105.2161731957375 40.02993344293114, -105.2160821948466 40.029843442886, -105.2160431949233 40.02976544318457, -105.2160301953674 40.0296674427522, -105.2160241944471 40.02958644314366, -105.2160111955 40.02941744250101, -105.2159851951632 40.0292884429292, -105.2159541953328 40.02928944287671, -105.2158601952949 40.02929244290664, -105.2154397747579 40.02930063641094, -105.2142271952085 40.02931444306602, -105.2132951941631 40.02931044250712, -105.2121779687597 40.02931370359353, -105.2116561945448 40.0293154428859, -105.2115561934457 40.02929544246373, -105.2114661938733 40.02925644249451, -105.2113901939955 40.02920244289452, -105.2113691942612 40.02918144297956, -105.21132119374 40.02911044242671, -105.2112971941228 40.02903344233737, -105.2113005886311 40.02886265923356, -105.2113071938985 40.02853044222877, -105.2113161932457 40.02663444274262, -105.2112871930142 40.02556744269105, -105.2112831926451 40.02472144241093, -105.2112831927006 40.02414744200545, -105.2112661927701 40.02380644202619, -105.2112281926976 40.02354844225731, -105.2111681958693 40.02340961220849, -105.2111421929906 40.02334944202191, -105.2110908591813 40.02325882755933, -105.2110271929919 40.02314644131605, -105.2109292903985 40.02301884637291, -105.2109051937388 40.02298744145597, -105.2108295770383 40.02291528432966, -105.2107433476153 40.02283715262609, -105.2106593493525 40.0227561515699, -105.2104213509922 40.02261115079264, -105.210131353124 40.02246915041668, -105.2096453553682 40.02228714891598, -105.2092683557341 40.02218214859246, -105.2089568292927 40.02211259715015, -105.2085064200148 40.02197920421263, -105.2081351092813 40.0218317118302, -105.2077919256969 40.02163067272885, -105.2073173661939 40.02133714445619, -105.2072853658604 40.02131414432528, -105.2071853679822 40.02123014325992, -105.2069473712818 40.02099014246873, -105.2067823753913 40.02074214075176, -105.2066866789568 40.02047579851763, -105.2066508805403 40.02015162089645, -105.2066396306025 40.01988469898361, -105.2066282588804 40.01964637159548, -105.2066417223345 40.0193985748575, -105.2066873211797 40.01744464479255, -105.2067009491717 40.01715872104394, -105.2066918318187 40.01639614326426, -105.2067183070375 40.01600540075746, -105.2067098058444 40.0150998456722, -105.2067203549632 40.0147049988613, -105.2067196345875 40.01470499883064, -105.2066710004365 40.01470499853, -105.206367999478 40.01470099950867, -105.2059949767234 40.01469404358584, -105.2059949427587 40.01469404259862, -105.2055099991169 40.01468499841905, -105.2052452071275 40.01468054190908, -105.2052129998992 40.0146799993535, -105.2050079696713 40.01467855822093, -105.2048625378809 40.01467753585545, -105.2046439989874 40.01467599916017, -105.2045197317803 40.01467615277912, -105.2038309998592 40.01467699888822, -105.2036568942967 40.01467716858118, -105.2036567103979 40.01467716810863, -105.2028090273656 40.01467798954275, -105.2027581900902 40.01266844174256, -105.2038051899005 40.01281044069496, -105.2043981908388 40.01288544030034, -105.2045691898613 40.01294644116913, -105.2048331905392 40.01297844102542, -105.2050351910883 40.01296044132123, -105.2050398702081 40.01392145197964, -105.2050431900852 40.0146034419073, -105.2069742231526 40.01462497172324, -105.2078121909381 40.01462344028587, -105.2078361910397 40.01348944102689, -105.2075011914237 40.01348844053171, -105.2074681901274 40.01104044140051, -105.2098111911977 40.01104044022411, -105.2098286476958 40.01241859730428, -105.2098292659196 40.01246736656677, -105.2098311921049 40.01261944051893, -105.2101881770135 40.0126180919686, -105.2101880793582 40.01262205279892, -105.2121356176559 40.01262468172177, -105.2130646768166 40.01262642336378, -105.213064157268 40.01258789120162, -105.2130673059102 40.01280105946651, -105.2130736861623 40.01323274517098, -105.2130740693893 40.01339608598071, -105.2130777016322 40.01363575086111, -105.2130940324873 40.01467594647242, -105.2130969381798 40.01474897599216, -105.2130981903515 40.01474897460401, -105.2141074361257 40.0147478477099, -105.2148764361527 40.01473067926249, -105.2148910155936 40.01473046222324, -105.2157340623453 40.01471789690481, -105.215735902945 40.01471779606526, -105.2164723909476 40.01467739814613, -105.2164899016262 40.01467620189562, -105.217100941391 40.01463444043784, -105.2191844656205 40.01463953261158, -105.2239170504272 40.01464087196651, -105.2245834902002 40.0146398382582, -105.2254128747107 40.01466887521181, -105.2254145473955 40.01466887288986, -105.2258513852783 40.01466824594888, -105.2272090327501 40.01466628746812, -105.2281480626285 40.01466492383204, -105.22915700892 40.01466702306828, -105.230058133229 40.01466913584839, -105.2309519694455 40.01468609977, -105.2319659677214 40.01469691984863, -105.2338293506786 40.01473924403673, -105.234785953114 40.0147380290238, -105.2364884675618 40.01473462743368, -105.2379838714334 40.01472804370003, -105.239268545971 40.01470520202151, -105.2401101703597 40.01465348406194, -105.2407671682903 40.01461834492035, -105.2422256658095 40.01457244483336, -105.2432112087095 40.01457106881134, -105.2449033960308 40.01456052644195, -105.2460469422521 40.01457377343792, -105.2465954644375 40.01458212939171, -105.2477575533147 40.0146096980253, -105.2489568317006 40.01463733680855, -105.2501120279116 40.01463197668197, -105.2537731835135 40.0146261868912, -105.2537949903803 40.01406758669711, -105.2538081303951 40.01360465598484, -105.2538054741536 40.01274848195483, -105.2537806712891 40.01248002734037, -105.253715823358 40.01226403757396, -105.2536241596939 40.01204202995962, -105.2535630325855 40.01186593254538, -105.2535261719986 40.01169290685051, -105.2535019003321 40.01119789590327, -105.2535030853529 40.01100293505052, -105.2535039273517 40.01086430388367, -105.2535061296354 40.01032410969325, -105.2535068895725 40.00892900280688, -105.2535011689129 40.00823994697006, -105.2535111127166 40.00805686367984, -105.2535018757067 40.00784711067982, -105.2534788384062 40.0077021148444, -105.2534580881613 40.00761587168582, -105.253390440773 40.00738013872348, -105.2531470399376 40.00675897970751, -105.2531119710475 40.00658513352174, -105.2531028651088 40.00594493428408, -105.2531010238238 40.00517188259421, -105.2531039801196 40.00445402054249, -105.2531108838922 40.00373012711088, -105.2540440020844 40.00372910138983, -105.2583379493246 40.00373488608032, -105.258572133868 40.00373098416479, -105.2586434447849 40.0037284900354, -105.2586556382503 40.00290996136781, -105.2586436430115 40.00235946687246, -105.2586454140996 40.00185904416556, -105.2586142067626 40.00148365856045, -105.2585687794402 40.00118688281169, -105.2584680337078 40.00076130850472, -105.2583433547495 40.00053228127841, -105.2581675632618 40.00029957202448, -105.2589195861169 40.00036267320748, -105.2592544037049 40.00038408331039, -105.259251053428 40.00025364728025, -105.2593301393748 40.00027828043822, -105.2595041374749 40.0003192800807, -105.2597321375767 40.00033028045623, -105.2602051376428 40.00033828032775, -105.2606671387836 40.00031627988058, -105.2613031379176 40.00026628085262, -105.2614471376263 40.00025428044938, -105.262564137449 40.0001492804175, -105.2635226869538 40.00007661770653, -105.2635271382638 40.00007628008433, -105.2635316634515 40.00008266869302, -105.2635362436151 40.00008232142758, -105.263577605498 40.00014071094439, -105.2635825036177 40.00014762629726, -105.2636677621977 40.00013487760815, -105.2636851372977 40.00013227971019, -105.2637656435806 40.0000901112732, -105.2637600945748 40.00008210840647, -105.2643058348404 40.00009201025707, -105.2650550950247 40.00008502916437, -105.2665028856773 40.00008302921293), (-105.2782259265416 40.01288889235155, -105.2782434257579 40.01293071174543, -105.2782259988166 40.01288899876749, -105.2782259265416 40.01288889235155), (-105.2884699572886 40.0104089180808, -105.2887237568676 40.01041448734374, -105.2887551645736 40.01041517623894, -105.2884699572886 40.0104089180808), (-105.2899762105711 40.01037143456766, -105.2896527354309 40.01039073227599, -105.2892512100549 40.01041243440763, -105.2896527354281 40.01039073317661, -105.2899762105711 40.01037143456766))</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
-      <c r="J17" t="inlineStr"/>
-      <c r="K17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>New Vista</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>700 20th St, Boulder, CO 80302</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>BVSD</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>http://nvh.bvsd.org/</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/mVZ7Cv3jx5iSPW3u9</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>New Vista High School</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>40.0011978462681</v>
+      </c>
+      <c r="K17" t="n">
+        <v>-105.266504379284</v>
+      </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>POINT (-105.266504379284 40.0011978462681)</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1628,59 +1558,53 @@
           <t>POLYGON ((-105.178285099815 40.05095033556441, -105.1782909993724 40.05078899852872, -105.1783619916895 40.05013707172179, -105.1783619978893 40.05013699968696, -105.1783889994008 40.0494039987319, -105.1783889921711 40.04940279904402, -105.1783850000171 40.04872299868529, -105.1783823374743 40.04787297522466, -105.1783819997574 40.04776499876323, -105.1783700003943 40.04545199887659, -105.1783569989513 40.04397399911803, -105.1783593807407 40.04381992401295, -105.1783670002116 40.04332699857592, -105.1783709996006 40.04307199909479, -105.1783800001195 40.04215799916332, -105.1783800027096 40.04215794693271, -105.1783870000278 40.04106199875608, -105.1783899999625 40.04087199920473, -105.1783900004663 40.04081899851942, -105.1783920002899 40.04072099871122, -105.1784048433664 40.03966053615192, -105.1784199995207 40.03840899927504, -105.1784249996421 40.03670199816679, -105.1784399998176 40.03537799842891, -105.1784889999836 40.03472599927464, -105.178490000368 40.03469499888762, -105.178531999708 40.03353499925799, -105.1785369999334 40.03339099877271, -105.1785399991614 40.03279999949025, -105.1785309996551 40.03216499864769, -105.1784769999151 40.03169499900179, -105.1784589989599 40.03107899928678, -105.1784620001129 40.03036699889137, -105.1784680003464 40.02915899894963, -105.1785019999882 40.0272379988253, -105.1785159996695 40.0261089991069, -105.1785169994261 40.02605499869539, -105.1784799995173 40.02439999821404, -105.1784639995815 40.02391999874165, -105.1784449993586 40.02333599866598, -105.1784189992241 40.02213199938647, -105.1784120001571 40.02177899910858, -105.1783799991943 40.02048599914978, -105.1783460002359 40.01914399873556, -105.1783049994997 40.01838899907003, -105.1782029988481 40.01737399931093, -105.1781489999591 40.01684399893904, -105.1781320000762 40.01633599939375, -105.1781410003895 40.01595099914135, -105.1782570004259 40.01483999953051, -105.1782689995687 40.01463299858616, -105.179412999948 40.01461999874561, -105.1808354543097 40.01462562931187, -105.1827040007133 40.01463299831895, -105.1834549992717 40.0146349225061, -105.1838739999368 40.01463599886635, -105.1841701799736 40.01463570346134, -105.1858630004019 40.01463399899924, -105.1864974973728 40.01463462047163, -105.1868859994811 40.01463499863746, -105.1879306387029 40.01464043574966, -105.1880389993641 40.01464099911838, -105.1886723010191 40.01463892504425, -105.1895639999455 40.01463599872144, -105.1942429993284 40.01465399917136, -105.1943553939693 40.01465460062421, -105.1951779999087 40.01465899884218, -105.1966359998847 40.01466699895634, -105.1967699330014 40.01466790959612, -105.1967830001021 40.0146679988932, -105.1983059994697 40.01466299922393, -105.1988599995382 40.01467899903977, -105.2006159994158 40.01467999898198, -105.2009300000826 40.01468399931195, -105.201182717144 40.01468616479592, -105.2012799993588 40.01468699864344, -105.2020565681202 40.01468240032865, -105.2020579655673 40.01468239223043, -105.2027989994621 40.01467799882614, -105.2038309998592 40.01467699888822, -105.2045197317803 40.01467615277912, -105.2046439989874 40.01467599916017, -105.2048625378809 40.01467753585545, -105.2052129998992 40.0146799993535, -105.2052452071275 40.01468054190908, -105.2055099991169 40.01468499841905, -105.206367999478 40.01470099950867, -105.2066710004365 40.01470499853, -105.2067203549632 40.0147049988613, -105.2067098058444 40.0150998456722, -105.2067183070375 40.01600540075746, -105.2066918318187 40.01639614326426, -105.2067009491717 40.01715872104394, -105.2066873211797 40.01744464479255, -105.2066417223345 40.0193985748575, -105.2066282588804 40.01964637159548, -105.2066396306025 40.01988469898361, -105.2066508805403 40.02015162089645, -105.2066866789568 40.02047579851763, -105.2067823753913 40.02074214075176, -105.2069473712818 40.02099014246873, -105.2071853679822 40.02123014325992, -105.2072853658604 40.02131414432528, -105.2073173661939 40.02133714445619, -105.2077919256969 40.02163067272885, -105.2081351092813 40.0218317118302, -105.2085064200148 40.02197920421263, -105.2089568292927 40.02211259715015, -105.2092683557341 40.02218214859246, -105.2096453553682 40.02228714891598, -105.210131353124 40.02246915041668, -105.2104213509922 40.02261115079264, -105.2106593493525 40.0227561515699, -105.2107433476153 40.02283715262609, -105.2108295770383 40.02291528432966, -105.2109051937388 40.02298744145597, -105.2109292903985 40.02301884637291, -105.2110271929919 40.02314644131605, -105.2110908591813 40.02325882755933, -105.2111421929906 40.02334944202191, -105.2111681958693 40.02340961220849, -105.2112281926976 40.02354844225731, -105.2112661927701 40.02380644202619, -105.2112831927006 40.02414744200545, -105.2112831926451 40.02472144241093, -105.2112871930142 40.02556744269105, -105.2113161932457 40.02663444274262, -105.2113071938985 40.02853044222877, -105.2113005886311 40.02886265923356, -105.2112971941228 40.02903344233737, -105.21132119374 40.02911044242671, -105.2113691942612 40.02918144297956, -105.2113901939955 40.02920244289452, -105.2114661938733 40.02925644249451, -105.2115561934457 40.02929544246373, -105.2116561945448 40.0293154428859, -105.2121779687597 40.02931370359353, -105.2132951941631 40.02931044250712, -105.2142271952085 40.02931444306602, -105.2154397747579 40.02930063641094, -105.2158601952949 40.02929244290664, -105.2159541953328 40.02928944287671, -105.2159851951632 40.0292884429292, -105.2160111955 40.02941744250101, -105.2160241944471 40.02958644314366, -105.2160301953674 40.0296674427522, -105.2160431949233 40.02976544318457, -105.2160821948466 40.029843442886, -105.2161731957375 40.02993344293114, -105.2162281958708 40.02996544241743, -105.2163231954602 40.03000344222524, -105.216393195045 40.030018442685, -105.216714195362 40.02978944179781, -105.2169183296271 40.02964944212096, -105.2170861959579 40.02953944212074, -105.2171013733368 40.02953197961455, -105.2172628810816 40.02945581657214, -105.2173882346814 40.02940610874885, -105.2175251954509 40.02935744244781, -105.2176198784911 40.0293380499647, -105.2177341859115 40.02931463718165, -105.2178571961912 40.02928944246727, -105.2180831955133 40.02926644208032, -105.2184761957898 40.02926244201551, -105.2185102178733 40.02926210714222, -105.2191025662913 40.02925881640458, -105.2199463053364 40.02925557303384, -105.22047383285 40.0292534418192, -105.2209515721532 40.02925336013067, -105.2213741961431 40.02925244173912, -105.221524196698 40.02924344258807, -105.2215368541062 40.02924212396792, -105.2216681962193 40.02922844212854, -105.2217758048782 40.02920913506678, -105.2220471963629 40.0291604417221, -105.2221531959837 40.02913544191373, -105.2227491964695 40.02893444274527, -105.2231341967773 40.02873844263139, -105.2234171967727 40.02858844157902, -105.2240448012386 40.02921896182992, -105.2240485290634 40.0292221896779, -105.2242922587597 40.02922218887095, -105.2243452592167 40.02922218854747, -105.2250902606939 40.02922118797638, -105.2253838715813 40.02922712104237, -105.2253876759348 40.02922707245764, -105.2253944375382 40.02922698588036, -105.2258520567489 40.02922109704281, -105.2259449032419 40.029221042971, -105.2260059682783 40.02922091333762, -105.2275989594909 40.02923100067746, -105.2286845476068 40.02923108871217, -105.2291319973156 40.02923104149665, -105.2300240500278 40.02922791711205, -105.2303165160975 40.02922777805944, -105.2308360988211 40.02922789375545, -105.2312381944585 40.02922828192708, -105.2317567030328 40.02922893947044, -105.2326919485125 40.02923001266877, -105.2329054947644 40.02923023263606, -105.2335989823584 40.02923101313294, -105.2346081604372 40.02922894693484, -105.2365361783417 40.02922211126447, -105.2375975186471 40.02922070455187, -105.2382999573494 40.02920828260488, -105.2395431210193 40.02918391916977, -105.2400198840386 40.02917511185208, -105.2431311238466 40.02922408398609, -105.2441955801484 40.02923144538298, -105.2447080626234 40.02923005531607, -105.2448980525407 40.02922690726311, -105.2459758332215 40.02921391257004, -105.2467879073245 40.02920691310877, -105.2470046722872 40.02920574144774, -105.2471535866196 40.02920497006868, -105.2475199805581 40.02920302743363, -105.2482195454966 40.02920455652909, -105.2481541927388 40.02931308733002, -105.247983553166 40.0296102141241, -105.2477685658453 40.02998489963429, -105.2475764919784 40.03031963966591, -105.2474157554355 40.03059976586545, -105.2472377688188 40.03090995649731, -105.2470527888195 40.03123232722809, -105.2470384585521 40.03125730147787, -105.2468743915512 40.03153389625475, -105.2466014210446 40.03199231009842, -105.2462652351348 40.03255119866444, -105.2453730542609 40.03402702879499, -105.2444588367812 40.03552861301022, -105.2440929793375 40.03610011054108, -105.2438753893139 40.0364924229959, -105.2432991274496 40.03743023787163, -105.2430111166943 40.0379132414562, -105.2427781086196 40.03829124483734, -105.2425780966287 40.03862463649937, -105.2437996973181 40.03858015455958, -105.2446044735468 40.03855084401205, -105.2456601157548 40.03831973388306, -105.2463663111993 40.03830715832521, -105.2476788464136 40.03828923237084, -105.2489428716393 40.03828342936805, -105.2500216866296 40.03828440663961, -105.2515262941062 40.03828575038629, -105.2517619181192 40.03828706191138, -105.2519246265246 40.03828456224724, -105.252087273247 40.03828033297279, -105.2524122082365 40.03826537837855, -105.252574399222 40.03825465195054, -105.2527363390311 40.03824176679848, -105.2528979772607 40.03822672371619, -105.2530592634851 40.0382095298022, -105.2532201543185 40.03819018946845, -105.2533805946551 40.03816870800271, -105.2535405399283 40.03814509251686, -105.2536949545598 40.03812015275444, -105.2536959323025 40.03907688210359, -105.2541075664353 40.03908055851134, -105.2541130449594 40.0400350024811, -105.2541114189239 40.04008556330383, -105.2541156704493 40.04008547509496, -105.2564700565923 40.04008607648185, -105.2570050616881 40.04009104854779, -105.2572561306026 40.04009487076375, -105.2576250499565 40.04010196086148, -105.2584811444412 40.04010595201317, -105.2585019067495 40.04140309591936, -105.2585200529217 40.0428339247763, -105.2585328883272 40.04344502971864, -105.258535903728 40.04360206066097, -105.2585405106698 40.04557391508014, -105.2585412801613 40.04583500499989, -105.2585431409786 40.0466000914717, -105.2585491366171 40.04702505910149, -105.2585801436604 40.04744788236328, -105.2586361577098 40.04786993381616, -105.2587031080589 40.04822996778709, -105.2587330305727 40.04835411276961, -105.2588011065953 40.04859802744705, -105.2588770324828 40.04884497745633, -105.2589520194323 40.04905404325294, -105.2590968835464 40.04940298337421, -105.2592908491195 40.04980693019196, -105.2594790114012 40.05013509748598, -105.2595461504909 40.05024092674891, -105.2597039348822 40.05047294914017, -105.2598909228966 40.05073001337415, -105.2600729289857 40.05098212507661, -105.2601188264747 40.05103410417082, -105.2602141708121 40.05114493352249, -105.2603760318205 40.0513360595755, -105.2605749425811 40.05155608753633, -105.2606671334609 40.05164988950381, -105.2607870983266 40.05176900406456, -105.2609530191591 40.05192390191151, -105.2610698287841 40.05202599008051, -105.2612450666888 40.0521729459601, -105.2614929991048 40.05237111141436, -105.2617659165283 40.0525759170593, -105.2620028794537 40.05274495970432, -105.2621960311828 40.05287795048658, -105.2623361003706 40.0529699277751, -105.2624829531093 40.05306301764614, -105.2628900215765 40.05331696043408, -105.2636688880578 40.05380006284676, -105.2643711340155 40.05423304186316, -105.2651129178647 40.0547020581333, -105.2656519227221 40.05503202749767, -105.2668749737009 40.05580013493221, -105.2682239553873 40.05662805383557, -105.269613922533 40.05749501959285, -105.2704799468352 40.05801009468256, -105.2708018933556 40.05820399463217, -105.2713911776679 40.05857795867715, -105.2730720982822 40.05964009195046, -105.2764060265012 40.06171701384444, -105.2766818087143 40.0618889301708, -105.2794570843467 40.06360607635985, -105.2799809979885 40.06393952401127, -105.2802739685094 40.06411686471955, -105.280571421083 40.06429735375461, -105.2809515658617 40.06431108663833, -105.2814222747994 40.06419864439965, -105.2818065024136 40.0636562328228, -105.282127928685 40.06372330059435, -105.282319982506 40.06372626586732, -105.2832962374926 40.06372837690664, -105.2835079480766 40.06372864274691, -105.283919471611 40.06372879883411, -105.2844681111398 40.06372971757044, -105.2844693643109 40.06404057361777, -105.2844743893111 40.06528829290035, -105.2844750682011 40.06545646919614, -105.2844696482367 40.06556530130753, -105.2844419581037 40.06556495868456, -105.2844392150506 40.0657224424132, -105.2843132151617 40.06563044283727, -105.2842552150438 40.06560344292603, -105.2842092152591 40.06558744250346, -105.2841555199931 40.0655765955805, -105.2841102147732 40.06556744313233, -105.2840422155819 40.0655634422325, -105.2840396611971 40.06556052476189, -105.2826421053623 40.06555460571782, -105.2823076520964 40.06555737709394, -105.2818205276817 40.06556514578249, -105.2821777644898 40.06610051550977, -105.2824690223394 40.06665264506963, -105.2826287480644 40.0671032160873, -105.282708682352 40.06730598772923, -105.2827667487974 40.0674749475167, -105.2828103083754 40.06759885395986, -105.2828828825465 40.06781286879525, -105.2830899236575 40.06843101948598, -105.283447132496 40.06958603676775, -105.2839564523263 40.07122915445703, -105.2841258539786 40.07178289850857, -105.2844119360205 40.07272887084649, -105.2844238046166 40.07276114874126, -105.2845098877672 40.0730540823975, -105.284634842972 40.07354103535643, -105.2846740115247 40.07381095898337, -105.2846799442029 40.07408191848048, -105.2846558254534 40.07436407727556, -105.2846140488599 40.07458004438773, -105.2844881096322 40.07496797674111, -105.2843430443443 40.07530206774775, -105.2841729060126 40.07565395617164, -105.284061438017 40.07587059340077, -105.2839819795333 40.07602502070181, -105.2839320007679 40.07612210589992, -105.2838018419132 40.0763738690773, -105.2826709107073 40.07859011936667, -105.2825129694785 40.07892198794374, -105.2823438719979 40.07938999478642, -105.2823048577945 40.07952086600779, -105.2822690597651 40.07965201797717, -105.2822223466844 40.07989150774977, -105.2821342160606 40.0791254445771, -105.2821112161553 40.07666744386643, -105.2782532143109 40.07666244408787, -105.278372214492 40.07653744417692, -105.2783742148064 40.07579144511136, -105.2780202147794 40.07579044515734, -105.2779022152453 40.07603844420503, -105.2777612150901 40.07620044483633, -105.2776022148752 40.07633644500343, -105.2774795717141 40.0764360956394, -105.277414215237 40.07647944379102, -105.2774182151642 40.07662844439344, -105.2774232152314 40.07679644423713, -105.277462333618 40.07819218232893, -105.277486220627 40.07914765992864, -105.2775032146846 40.07989444554472, -105.2774442150245 40.07989344467622, -105.2774492150437 40.079994445459, -105.2760592152198 40.07997644544199, -105.275236925473 40.07998199934345, -105.2741904007602 40.07997698391911, -105.2738472151207 40.07997344533944, -105.2732488422515 40.07998423568615, -105.2722111865081 40.08000293913378, -105.271602868858 40.08001390036796, -105.270773469619 40.08002883906712, -105.269120467453 40.08006436083225, -105.2678107184368 40.08009626548748, -105.265906623877 40.08014227963445, -105.2635022120304 40.08020744623987, -105.263475212196 40.07824944591677, -105.2552788447606 40.07829042246069, -105.2509901360431 40.07831039649412, -105.2479762077927 40.07832544680577, -105.2467352086361 40.07833144715077, -105.245048207299 40.07833944731037, -105.2446880583013 40.07833920790986, -105.2446880588089 40.07833844686491, -105.2435522068469 40.07833844725607, -105.2423652076105 40.07833744689923, -105.2403432064991 40.07833344770941, -105.2384812068036 40.07833244791702, -105.2378132062725 40.07833444783447, -105.2352892054144 40.07873844737262, -105.2334432055741 40.07899144749057, -105.2299052044168 40.08008044876753, -105.2350032064051 40.08016044862552, -105.2350497203358 40.08268589163298, -105.2350776389745 40.08420165278985, -105.2350852057845 40.0846124484227, -105.2351382054217 40.08551144874158, -105.2351162069385 40.08560644881669, -105.2349272055709 40.08608544943124, -105.2347532059639 40.0863524487831, -105.2346296381483 40.08650825210744, -105.2344113616564 40.08671008020809, -105.2342874907976 40.08682176614175, -105.2342102060382 40.08689144861766, -105.2341886118381 40.08690464559623, -105.2341742062996 40.08691344866173, -105.234116919408 40.08694927681879, -105.2340547143473 40.08698818193187, -105.2340141176357 40.08701357127359, -105.2338752055783 40.08710044895112, -105.2337498879304 40.08716518662143, -105.2336642062275 40.0872094484582, -105.233557508418 40.08725212883198, -105.2334842065225 40.08728144947539, -105.2335198087354 40.08730061994037, -105.2335350154684 40.08731185997121, -105.2335182680553 40.08731887517195, -105.2334670391323 40.08733945284803, -105.2334153508784 40.08735934044687, -105.2333632162177 40.08737853169327, -105.2333106562827 40.0873970203308, -105.2332572252643 40.08741486387087, -105.2332115864704 40.0874290192368, -105.233160289808 40.08744409547717, -105.2331195646996 40.08745541432238, -105.2331086089517 40.08745846109794, -105.2330565603615 40.08747210532881, -105.2330041639691 40.08748502911613, -105.2329514268327 40.08749722707182, -105.232898377103 40.08750869745924, -105.2328450159892 40.08751943127434, -105.2327913728077 40.08752942858451, -105.232737453437 40.08753868580036, -105.2326832836757 40.08754720298132, -105.2326288764451 40.08755497475301, -105.2325748982646 40.08756217648359, -105.2325209052109 40.08756868375681, -105.2324667696581 40.08757444944327, -105.2324125138727 40.08757947719696, -105.2323581460858 40.0875837616329, -105.2323036897474 40.08758730370593, -105.2322491612788 40.08759010255342, -105.2321945759326 40.08759215640933, -105.232139950141 40.08759346170912, -105.2320852944376 40.08759402388102, -105.2320306369806 40.0875938393878, -105.2319759906559 40.08759291186197, -105.2319213672231 40.08759123322496, -105.2318667865754 40.08758881433079, -105.2318122651521 40.08758564981383, -105.2317578193674 40.08758174061293, -105.2317034632943 40.08757708676092, -105.2316492191852 40.08757169551478, -105.2315951034686 40.08756556421094, -105.2315411374752 40.08755923148525, -105.2283729549368 40.08717092525384, -105.2272444844378 40.08716355701311, -105.2272236163383 40.08716344466387, -105.2271977580158 40.08717057341977, -105.2271717266588 40.08717815928905, -105.2271459834793 40.08718610609185, -105.2271204311677 40.08719440999577, -105.2270950662131 40.08720306919137, -105.227069908556 40.08721208192462, -105.2270449570381 40.08722144459034, -105.2270202222304 40.08723115271041, -105.226995713506 40.08724120810847, -105.2269713781346 40.08725160165343, -105.2269462956309 40.08726233387031, -105.2269214580284 40.08727339899931, -105.226896880574 40.08728479617606, -105.2268725621166 40.08729651999401, -105.2268485155578 40.08730856958332, -105.2268247444441 40.08732093774738, -105.2268012569799 40.08733362540633, -105.226778067272 40.08734662358735, -105.2267551729715 40.08735993318564, -105.2267325834878 40.08737354701852, -105.2267103070542 40.08738745880117, -105.2266883530404 40.08740167125784, -105.2266667226549 40.08741617538511, -105.2266454253037 40.08743096490092, -105.2266244715363 40.08744604073107, -105.2266038602236 40.08746139206541, -105.22658359957 40.0874770198241, -105.2265637001611 40.08749291592657, -105.2265441631842 40.08750907677334, -105.226524998038 40.0875254978835, -105.2265062070929 40.08754217295839, -105.2264878009205 40.08755909752002, -105.2264697795498 40.08757626436348, -105.2264521500162 40.08759367350561, -105.226434455812 40.08761141663134, -105.2264158800905 40.08762967283475, -105.2263977138776 40.0876481506639, -105.2263825065714 40.08766855838156, -105.2263789361496 40.08767231912204, -105.2263767305145 40.08767464926904, -105.2263745307277 40.0876769830324, -105.2263723344585 40.0876793168041, -105.2263701416961 40.08768165328597, -105.2263679524405 40.08768399247809, -105.2263657702201 40.0876863316868, -105.2263635879888 40.08768867359738, -105.2263614080953 40.08769101731477, -105.2263592363989 40.0876933637535, -105.2263570647023 40.08769571019219, -105.226354900023 40.08769806115065, -105.2263527353471 40.08770041120849, -105.2263505776958 40.08770276398484, -105.2263484247239 40.08770511947421, -105.2263462740824 40.08770747857164, -105.2263441269622 40.08770983677667, -105.2263419810035 40.08771219768641, -105.2263398455944 40.08771455952174, -105.2263377078255 40.08771692495404, -105.2263355759121 40.08771929220145, -105.226333448689 40.08772165945994, -105.2263313249726 40.08772402942868, -105.2263292047701 40.08772640030627, -105.2263270845495 40.0877287756871, -105.2263249737094 40.08773115109006, -105.226322866376 40.08773352920324, -105.2263207637256 40.08773590912882, -105.2263186598953 40.08773829085281, -105.2263165619241 40.08774067349134, -105.226314467456 40.08774305974064, -105.2263123800232 40.08774544600666, -105.2263102972735 40.08774783408501, -105.2263082145056 40.08775022666651, -105.2263061352625 40.08775261745505, -105.2263040642092 40.08775501276614, -105.2263019919905 40.08775740627321, -105.2262999267926 40.08775980339941, -105.2262978662741 40.08776220323865, -105.2262958045756 40.08776460487633, -105.2262937499053 40.08776700833194, -105.226291699918 40.08776941359987, -105.2262896569624 40.08777181978507, -105.2262876128304 40.08777422686813, -105.2262855745432 40.08777663846826, -105.2262835374175 40.08777905277302, -105.2262815085034 40.08778146619655, -105.2262794831069 40.0877838796284, -105.2262774576886 40.08778629846402, -105.2262754393057 40.08778871731626, -105.2262734244331 40.08779113797818, -105.2262714142507 40.0877935586511, -105.2262694052227 40.08779598382996, -105.2262674008741 40.08779841172184, -105.2262654059096 40.08780083873525, -105.2262634085889 40.08780326844501, -105.2262614183 40.08780569907206, -105.2262594326977 40.0878081306108, -105.226257445901 40.08781056755058, -105.2262554673158 40.08781300360911, -105.2262534898923 40.08781544237237, -105.2262515195077 40.08781788025156, -105.2262495549714 40.08782032174722, -105.2262475892516 40.08782276594194, -105.2262456270494 40.08782521014498, -105.2262436742169 40.08782765707216, -105.2262417237222 40.08783010580613, -105.2262397767451 40.08783255454839, -105.2262378332675 40.08783500780219, -105.2262358933076 40.08783746106425, -105.2262339568581 40.08783991613592, -105.226232023919 40.08784237301715, -105.2262300991841 40.08784483081848, -105.2262281732657 40.08784729131887, -105.2262262543791 40.08784975273657, -105.2262243401755 40.08785221596659, -105.226222428306 40.08785468190413, -105.2262205211268 40.08785714785272, -105.2262186162781 40.08785961740938, -105.2262167161233 40.08786208607652, -105.2262148218203 40.0878645574594, -105.2262129298625 40.08786702884783, -105.2262110437421 40.0878695065546, -105.2262091611538 40.08787198066713, -105.2262072808852 40.08787446108968, -105.2262054064867 40.08787693972477, -105.226203534426 40.08787942016669, -105.2262016682208 40.08788190242377, -105.2261998043462 40.08788438828893, -105.226197947507 40.08788687417072, -105.226196091833 40.08788936185654, -105.2261942361589 40.08789184954237, -105.2261923945412 40.08789434086405, -105.2261905517435 40.08789683398418, -105.2261887112837 40.08789932891115, -105.2261868778629 40.08790182295415, -105.2261850455965 40.08790432150305, -105.2261832203618 40.08790682096924, -105.2261813974722 40.08790932044101, -105.2261795792655 40.08791182172511, -105.2261777645729 40.08791432391816, -105.2261759557322 40.08791682882699, -105.2261741480568 40.08791933553987, -105.226172348582 40.08792184407345, -105.2261705502725 40.0879243544111, -105.2261687566533 40.08792686475982, -105.2261669688859 40.08792937782427, -105.2261651799496 40.08793188998534, -105.2261634015482 40.08793440667458, -105.2261616231395 40.08793692516508, -105.2261598505936 40.08793944366944, -105.2261580815545 40.08794196488402, -105.2261563172056 40.08794448610973, -105.2261545551981 40.08794700824161, -105.2261528013842 40.08794953399544, -105.2261510475738 40.08795205884863, -105.226149300777 40.08795458912228, -105.2261475563434 40.08795711489833, -105.2261458165711 40.08795964789051, -105.2261440803236 40.08796217908979, -105.2261423475865 40.08796471209865, -105.2261406218776 40.08796724692545, -105.2261388996683 40.08796978626372, -105.2261371809875 40.08797232290842, -105.2261354658207 40.08797486046209, -105.2261337541534 40.08797740252725, -105.2261320460038 40.0879799446007, -105.2261303460513 40.08798248939556, -105.2261286460914 40.08798503599166, -105.226126950829 40.08798758079754, -105.2261252602387 40.08799013011774, -105.2261235755077 40.08799268035245, -105.2261218943052 40.08799522789362, -105.2261202165914 40.08799778264812, -105.226118542406 40.08800033470907, -105.2261168764069 40.08800289219328, -105.2261152092496 40.08800544607216, -105.2261135491024 40.08800800627216, -105.2261118948289 40.0880105637841, -105.2261102405372 40.08801312579922, -105.2261085932736 40.08801568963229, -105.2261069495313 40.08801825257306, -105.2261053092994 40.08802081732343, -105.2261036725816 40.08802338298269, -105.2261020440572 40.08802595226398, -105.2261004178852 40.08802851974954, -105.2260987916986 40.08803109083762, -105.2260971760652 40.08803366195077, -105.2260955615934 40.08803623576855, -105.2260939506355 40.08803881049528, -105.2260923455334 40.08804138703718, -105.2260907451214 40.08804396359018, -105.2260891482163 40.08804654285341, -105.2260875536562 40.08804912212216, -105.2260859637863 40.08805170140207, -105.2260843809301 40.08805428610243, -105.2260827980811 40.08805686900151, -105.2260812222603 40.08805945371852, -105.2260796499462 40.0880620411458, -105.226078084664 40.08806462949036, -105.2260765193853 40.08806721693423, -105.2260749611275 40.0880698079974, -105.2260734087289 40.088072399975, -105.2260718574956 40.08807499375673, -105.2260703097799 40.08807758754672, -105.2260687690924 40.08808018315465, -105.2260672295774 40.08808277876541, -105.2260656970834 40.08808537799534, -105.2260641669416 40.08808797542954, -105.2260626414721 40.08809057737804, -105.2260611230379 40.08809317934323, -105.2260596034202 40.08809578400751, -105.2260580920141 40.08809838779062, -105.2260565841257 40.08810099158206, -105.2260550832546 40.0881035998933, -105.2260535823798 40.08810620910523, -105.2260520885404 40.08810881833376, -105.2260505993841 40.08811142937476, -105.2260491125655 40.08811404222255, -105.2260476280957 40.08811665417521, -105.226046152992 40.08811926975269, -105.2260446767192 40.08812188442674, -105.2260432086508 40.08812450002085, -105.2260417429166 40.08812711832244, -105.2260402865523 40.08812973934819, -105.2260388290152 40.08813236037112, -105.2260373773409 40.08813498140795, -105.226035930357 40.08813760245592, -105.2260344868726 40.08814022801536, -105.2260330445643 40.08814285267693, -105.2260316128055 40.08814547826421, -105.2260301833774 40.08814810745953, -105.2260289772142 40.08815032829153, -105.2260799511012 40.08815043483378, -105.2260951784236 40.08815046645809, -105.2259971464311 40.08825128178296, -105.2258660776002 40.08846675183878, -105.2258442047025 40.08817345056035, -105.225847257111 40.08702564690289, -105.2258422045073 40.08612344890279, -105.2246712037403 40.08611344976358, -105.2246852045713 40.08554044892636, -105.2230462031982 40.08603244956893, -105.2219812039535 40.08618344991433, -105.2211162029895 40.08627444986659, -105.2211262032423 40.08639345027048, -105.2182432027494 40.08641344971119, -105.2182532019159 40.08714945059754, -105.2163692023297 40.08714545077098, -105.216360202134 40.08892145040806, -105.2163292022599 40.08892045018143, -105.2159742024865 40.08892045011142, -105.2148588360544 40.08892679371123, -105.2148042021617 40.08892745043244, -105.2143002021996 40.08892245043239, -105.213437201397 40.08892445097817, -105.2114362013246 40.08891745132185, -105.2102848781286 40.08891722303895, -105.2093902465011 40.08891684883024, -105.208456199712 40.08891645102268, -105.2075245971012 40.08890693460845, -105.2069481319076 40.08890527106102, -105.2069438732727 40.0889052926268, -105.2069747075104 40.09435044215074, -105.2067688747363 40.09435139755085, -105.2067696857456 40.09448197611559, -105.206084292794 40.09448027846468, -105.204067954345 40.09447526321931, -105.2020925487541 40.09447072187066, -105.2004028346573 40.09447194731246, -105.2000942419318 40.09447216840297, -105.20004901646 40.0944713051883, -105.1999431444402 40.09446928464906, -105.1961591443175 40.09444728514715, -105.1941921454042 40.0944432846204, -105.1914201445046 40.09443828540665, -105.1878551441828 40.09443028595678, -105.1878554742897 40.09442402015232, -105.1878581437286 40.09437328585741, -105.1878579783739 40.09437328631103, -105.1878583084638 40.09436702410904, -105.1878489982433 40.09436703406432, -105.1869333094328 40.09436802324625, -105.1869288298045 40.09436799308698, -105.1864923089405 40.09436502536359, -105.1851823083869 40.09435602463465, -105.1851806430128 40.0943560507158, -105.1847691909817 40.09436254127205, -105.1842981568986 40.09474644455597, -105.1842254973132 40.09480566330672, -105.1770289540793 40.10167497796913, -105.1763019499671 40.1023029683946, -105.1688417643584 40.10884061707407, -105.1685799278165 40.10901976085416, -105.1674439177613 40.11003576716704, -105.1614528663692 40.11528080007928, -105.1594641412873 40.11689641328065, -105.1594566443818 40.11609286922273, -105.159467921669 40.11419687283805, -105.1594718259507 40.11205812132699, -105.1594520114176 40.10922888777313, -105.1594495599439 40.10886022285561, -105.1594219558605 40.10315811995677, -105.1594259842159 40.10399044520795, -105.1594259918098 40.10399197542836, -105.1590781918603 40.10400245670831, -105.1588411915942 40.10426645671227, -105.1588201907179 40.10434845704976, -105.1589061910858 40.10450845692532, -105.1588991905787 40.10458445709242, -105.1587201908592 40.10476045668218, -105.1584981900914 40.10477145654381, -105.1581892413284 40.10490396872007, -105.1580761909817 40.10495245717316, -105.1576681914213 40.10507845747404, -105.1572321903226 40.10529845652795, -105.1571241898577 40.1053754563856, -105.1571241900853 40.10546345672344, -105.157253190884 40.10562845707536, -105.157239191129 40.10571045628147, -105.157138190582 40.10579245659894, -105.1569951900118 40.10582045723518, -105.1565797245652 40.10604856929712, -105.1564161904518 40.10613345690832, -105.1557151895679 40.10621545706669, -105.155372190027 40.10630845692795, -105.1551781906975 40.10638545677693, -105.1551071895624 40.106484457227, -105.1549851905804 40.10658345749179, -105.1546631906193 40.10667645674386, -105.1543781900811 40.10669245702027, -105.1538481902248 40.10664345777509, -105.1536831893247 40.10669845729011, -105.153533190452 40.10679645699769, -105.1534041890178 40.10683545695765, -105.1532181895994 40.10680245729557, -105.1529611896807 40.10678045703483, -105.1528251894787 40.1068184572149, -105.1528251898034 40.10689545706076, -105.1527461895664 40.10708745705721, -105.1527891896304 40.10716445739909, -105.1530821895656 40.10724745707277, -105.1531971895655 40.10730745767818, -105.1532041904084 40.10742245698562, -105.1531681905297 40.10752745787505, -105.1530101897713 40.1076424577811, -105.1526961899649 40.10774645807478, -105.1522381891769 40.1078014575306, -105.1521161891182 40.10785645730169, -105.1520521905081 40.10809245803009, -105.1518081899357 40.10844445794176, -105.1518011892207 40.10854845784844, -105.1519151896514 40.1086254581982, -105.1522161898024 40.10867445774499, -105.1522521895131 40.10872445833751, -105.1522441899349 40.10883445806299, -105.1521871900507 40.10886745719991, -105.1521720437602 40.10888555509551, -105.152168642065 40.10888557367066, -105.152058189739 40.10899345806407, -105.1516361903776 40.10915845863114, -105.1515425217955 40.10915797339747, -105.151443190266 40.10915745838717, -105.1512721889252 40.10905345792743, -105.1511498943537 40.108892914989, -105.1510291895926 40.10873445721234, -105.1509501898016 40.10867945738578, -105.1507351896093 40.10865745754312, -105.1505561895843 40.10874045817922, -105.1503701892914 40.10874045812216, -105.1502991895659 40.10876745797281, -105.1502271897408 40.1088934573679, -105.150216358927 40.10890001008798, -105.1501990355049 40.1089104906731, -105.1501829687099 40.10892021131422, -105.1501628272604 40.1089323972873, -105.1501361731898 40.10894852276716, -105.1500271894042 40.10901445758356, -105.1499411886424 40.10911345803316, -1</t>
         </is>
       </c>
-      <c r="D18" t="n">
-        <v>22</v>
-      </c>
-      <c r="E18" t="n">
-        <v>22</v>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Niwot HS</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>8989 Niwot Rd, Niwot, CO 80503</t>
+        </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Niwot HS</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>8989 Niwot Rd, Niwot, CO 80503</t>
+          <t>https://nhs.svvsd.org/</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
+          <t>Niwot High School</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>40.10369506217272</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-105.1442414652976</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
           <t>https://nhs.svvsd.org/</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>Niwot High School</t>
-        </is>
-      </c>
-      <c r="L18" t="n">
-        <v>40.10369506217272</v>
-      </c>
-      <c r="M18" t="n">
-        <v>-105.1442414652976</v>
-      </c>
       <c r="N18" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>https://nhs.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="P18" t="inlineStr">
         <is>
           <t>POINT (-105.1442414652976 40.10369506217272)</t>
         </is>
@@ -1700,59 +1624,53 @@
           <t>POLYGON ((-105.2331971337308 39.985840282157, -105.2330351331852 39.98576428266011, -105.2327191338569 39.98561728215761, -105.2325671332445 39.98554728283532, -105.2324551331664 39.98549528298939, -105.2323551334779 39.9854482825155, -105.2319832192942 39.98527649380193, -105.2319351336893 39.9852542826066, -105.2311531345965 39.98489128325956, -105.2309501326586 39.98479628222291, -105.2302491328946 39.98447128245876, -105.2293111332321 39.98403928262311, -105.228734132372 39.98377128349869, -105.2276381336663 39.98326528294741, -105.2268921334482 39.98292028334055, -105.2259871327598 39.98250228293273, -105.2259021321316 39.9824632823856, -105.2233041316678 39.98126628283385, -105.221716133175 39.98053428301674, -105.2212240428698 39.98030670587036, -105.2212231314078 39.9803062839601, -105.221164278762 39.98041401321424, -105.2211641313148 39.98041428305446, -105.2208531327514 39.98027028363045, -105.2205529411696 39.98013265378606, -105.2205521325287 39.98013228345715, -105.2205507460672 39.98013349868391, -105.220540062076 39.98012857681351, -105.2205416976377 39.98012714153003, -105.2205429995072 39.98012599905148, -105.2198569987801 39.97980999936001, -105.217670999848 39.9788049982916, -105.2175789989619 39.97876299865521, -105.216200462426 39.97812263862686, -105.214956998355 39.97754499902697, -105.2135299983809 39.97688599922395, -105.2133739976538 39.97681299863746, -105.2131699989533 39.97671799874688, -105.2128311259303 39.97656205643337, -105.21283099974 39.97656199847693, -105.2101649988539 39.97532799912825, -105.2096699996618 39.9751049989255, -105.2093549990471 39.97496399882614, -105.2090049985782 39.97480699849135, -105.2087029993851 39.97467099834954, -105.2070459994989 39.9739889990676, -105.2048370000834 39.97313299845037, -105.2041369988925 39.97286199893107, -105.2034419994515 39.97259099900295, -105.2027290000227 39.97231199833313, -105.2014580003957 39.9718209988399, -105.1994079998071 39.97102099847267, -105.1989119987643 39.97083099883623, -105.1983979997043 39.9706339986794, -105.194591998727 39.96914999847615, -105.1918849995989 39.96810099902086, -105.1911419992523 39.96781299893013, -105.1901129992968 39.96740799898152, -105.1892829988523 39.96708899899218, -105.1886569997244 39.96684799823526, -105.1878959996133 39.96655099935374, -105.1847509988542 39.96532799810699, -105.1845030591753 39.96523090136483, -105.1845014339616 39.96523026465304, -105.1836529999933 39.96489799860698, -105.1823289247008 39.96438302700813, -105.1823765858315 39.96435856048586, -105.1829501799709 39.96406143557106, -105.1831431795536 39.96390943620628, -105.183359179438 39.96390543564833, -105.1846811801298 39.96359143505422, -105.1846831809932 39.96346543564761, -105.1850871806001 39.96337543512138, -105.1852101802556 39.96334743554963, -105.1859091799674 39.96319543556243, -105.1867561809799 39.96303243590308, -105.1875491802892 39.96290443543483, -105.1882881813402 39.96279743543808, -105.1892731804752 39.96267043497246, -105.1892811813567 39.96148043493095, -105.1891011772413 39.96160943265309, -105.1889071811083 39.96174843466853, -105.1882603172043 39.9619761564318, -105.1877131813326 39.96209643507789, -105.1876121808403 39.9621674358669, -105.1872551801046 39.96227843565087, -105.187073180655 39.96230143525784, -105.1867361810641 39.96239743503643, -105.1862821800566 39.96244943611252, -105.1852781797714 39.96245943558378, -105.185250937121 39.96248567933362, -105.1851691808371 39.96256443568562, -105.1846881802595 39.96256443553224, -105.1846878292357 39.9626284939408, -105.1845921801246 39.96264443594031, -105.1842001793857 39.96258943629537, -105.1841021800759 39.96259043491916, -105.183756179454 39.96352043583736, -105.183681180111 39.96353243572506, -105.1835581803465 39.96355343554686, -105.1834961799503 39.96356143605633, -105.1833721791185 39.96357743607462, -105.1832471796654 39.96358943518963, -105.1831221800468 39.96359843587509, -105.1829971802545 39.96360343569754, -105.1828711795887 39.96360543613775, -105.182745178819 39.96360443634497, -105.1826201798852 39.9636004354759, -105.1824941789573 39.96359343521812, -105.1823521786804 39.96357643573872, -105.1822441795616 39.96356843645984, -105.1821201788212 39.96355143678812, -105.1820251788167 39.96353643541125, -105.1818761791532 39.9635074363657, -105.1815991793696 39.96344043598965, -105.1815181794293 39.96341743539393, -105.1814281797796 39.9633894364229, -105.1813451795762 39.96336143602115, -105.1812645225385 39.96333271971175, -105.1811751798336 39.96329843665993, -105.1811201784924 39.96327643628931, -105.1810651795186 39.96325343616735, -105.1810111789803 39.96322943544858, -105.1809571796388 39.96320443587675, -105.1809041787385 39.96317943634221, -105.1808511790458 39.96315343615423, -105.180799178964 39.96312643537638, -105.1807481784856 39.96309843581128, -105.1806971792238 39.96307043532614, -105.1806471783964 39.96304143605229, -105.1805491783552 39.96298243605077, -105.1805011791406 39.96295143559319, -105.1804541783631 39.96292043608274, -105.1804071788043 39.96288743619242, -105.1803891795854 39.96287543542729, -105.1800231788606 39.96283243551652, -105.1791101784401 39.96248843618227, -105.1790331792207 39.9626014355022, -105.1780361786519 39.96221443573692, -105.1780248042583 39.96220476780362, -105.1780795667658 39.96212243842648, -105.1780617120378 39.96101742820876, -105.1780563504867 39.96064057285627, -105.1780562582363 39.96063407794388, -105.1760332411225 39.96066191903108, -105.1753197877496 39.96067107019252, -105.1752660781159 39.9606704126778, -105.1751530130947 39.96066902761821, -105.1751515536733 39.96066900909348, -105.1751673978478 39.95941085853762, -105.1752731802447 39.95941238698667, -105.1756586725545 39.95941795615956, -105.1767015637337 39.95943301604639, -105.1770275234974 39.95943772098945, -105.1770358705875 39.9584045834283, -105.1770363078439 39.95835052526509, -105.1770375221035 39.95820029775011, -105.1770375790401 39.9581932133214, -105.1753811772785 39.95817043580769, -105.1753791767883 39.95758643523679, -105.1786071510341 39.95766248213681, -105.178782063112 39.95766574209604, -105.1789897484092 39.957669611876, -105.1789848485213 39.95766031512748, -105.177648397834 39.95512435329022, -105.1776144429687 39.95506001242811, -105.1775799624868 39.95499299062175, -105.1775470406094 39.95492554265083, -105.1775156877714 39.95485768836055, -105.1774859155525 39.95478945300295, -105.1774577273785 39.95472085370143, -105.1774311360077 39.95465191391003, -105.1774061518873 39.95458265077165, -105.1773827784174 39.95451308681337, -105.1773610213213 39.95444324817128, -105.1773575396614 39.95443111644111, -105.1773408910587 39.95437314928622, -105.177322394536 39.95430281359553, -105.1773055304672 39.95423226451359, -105.177290313959 39.95416152369918, -105.1772767414146 39.95409060825552, -105.1772648208975 39.95401954432493, -105.1772552845585 39.95394743780206, -105.1772475047739 39.95387510202673, -105.1772414131593 39.9538026430856, -105.1772370166073 39.95373008711738, -105.1772416938306 39.95365372245707, -105.1772507335152 39.95357595507921, -105.1772613072263 39.95349823162613, -105.1772734159885 39.95342058182205, -105.177290609483 39.95332415578926, -105.1774078670555 39.95259250878293, -105.1774296504487 39.95249004043743, -105.1774426914856 39.95247925641739, -105.1776474059061 39.95230996035514, -105.1776425915952 39.95225318368962, -105.1776494915453 39.95224847092626, -105.1776503630244 39.95222278293825, -105.1776527450811 39.9521525489294, -105.1776542787933 39.95210731667019, -105.1777091771583 39.95048843468322, -105.1765421764602 39.95049343511674, -105.1765441762881 39.95029543509211, -105.1737901766914 39.9502784352506, -105.1732691751886 39.95049443510379, -105.171721175293 39.95049343486586, -105.171721175489 39.95026543539605, -105.1713521750109 39.95026343503369, -105.1710701754516 39.9496574351276, -105.1709821753827 39.94931543455208, -105.1708731754645 39.94899843388744, -105.1706751750825 39.94883443513947, -105.1705001743236 39.94877043461553, -105.1702541750417 39.94875143479771, -105.1703601751532 39.94872843443577, -105.1699691748952 39.94766043485847, -105.1696509264492 39.94772961758919, -105.1696508514793 39.94772963358609, -105.1685594742733 39.94796687370324, -105.1663871736281 39.94844043457117, -105.1657381741117 39.9485814352014, -105.1657421736359 39.94800016035729, -105.1657468007817 39.94732775484253, -105.165775173689 39.94320443381061, -105.1664695916308 39.9432063625764, -105.1683021747413 39.94321143381614, -105.1693041740566 39.94127343310699, -105.1693161728545 39.9392404329576, -105.1676961733447 39.939242433397, -105.1669986961005 39.93946070845881, -105.1664371723441 39.93963643311929, -105.1657621735393 39.94010243415755, -105.1657314686955 39.9377869994332, -105.1657411728798 39.93778699967167, -105.1687795281632 39.93778699271773, -105.1705111261316 39.93778695271561, -105.1705041256043 39.93953147032551, -105.1705041235479 39.93953189633235, -105.170503856046 39.93959870391294, -105.1706001480141 39.93959920896221, -105.1706007611061 39.93959921251663, -105.1752061254244 39.93962327452727, -105.1752117639349 39.94144391979933, -105.1752117838299 39.94145375507232, -105.1752147521367 39.9424101139557, -105.1752173188591 39.9432381770126, -105.1761254808051 39.94324195231821, -105.1789957423668 39.94325383880542, -105.1795291232214 39.94325604071027, -105.1795857546609 39.94325627388761, -105.179680680969 39.9432566666597, -105.1799269123049 39.9432576806739, -105.1799269771434 39.9431864638202, -105.1799270111662 39.94314876676573, -105.1799270269173 39.94313068604808, -105.1799271965382 39.94293307347776, -105.1799284928579 39.94143895759951, -105.1799300690526 39.93962613628113, -105.1819970768541 39.93962050076085, -105.1825172429311 39.93962242816511, -105.1825172620205 39.9396190786604, -105.1846548192044 39.93961336109664, -105.1894029282757 39.93957558427936, -105.1893867343792 39.93594894951613, -105.1914911317678 39.93594133715856, -105.1923511717818 39.93593821445231, -105.1933688742004 39.93593450898793, -105.1933702477947 39.93593450363773, -105.1941599816869 39.93593162428242, -105.1945942211984 39.93592965200351, -105.1951635483 39.93592706564407, -105.1952762078992 39.93592655313077, -105.1972458768153 39.93591757849988, -105.1989481266646 39.93590979541442, -105.2002993179784 39.93590013495036, -105.2004456872241 39.93589909443324, -105.2005289440003 39.93589930820974, -105.2005695998748 39.93589960573908, -105.2005767561356 39.93597682174268, -105.2007855838866 39.93595828117817, -105.2016135821577 39.93571128289184, -105.2017205818092 39.93570628394144, -105.2019415807419 39.93585928284536, -105.2020485805162 39.93587628311925, -105.2022345798063 39.93581028363036, -105.2022817052154 39.93578010452304, -105.2022817218954 39.9357827182824, -105.2022819718508 39.93582278570346, -105.2022823369061 39.93589360196512, -105.203430843309 39.93588732563549, -105.2047070368473 39.93587606396571, -105.2046882733971 39.93394651148376, -105.2046864363509 39.93375887309851, -105.2046865622196 39.93375357663749, -105.2046865938261 39.93375222032397, -105.2046872617554 39.93372412053174, -105.2047298796838 39.93225646940934, -105.2047394578092 39.92861052434253, -105.20815190367 39.92859781286307, -105.2127497371948 39.92855694032826, -105.21745002281 39.92854504863909, -105.2182946341396 39.92854109387441, -105.2189537516798 39.92853800621756, -105.2189574099148 39.92853798902473, -105.2192246119665 39.92853673580493, -105.2193899800826 39.92853595984494, -105.2194595415266 39.92853648685829, -105.2221224251364 39.92852872241523, -105.2225585730252 39.92852772662706, -105.2269942832364 39.92851750262659, -105.231838615029 39.92851118067422, -105.2320906879295 39.92850933729788, -105.232244880529 39.92825937905761, -105.2322470002203 39.92825999913596, -105.2323239999907 39.92827499846799, -105.2325869997246 39.92832599949908, -105.2328459990954 39.92836499926473, -105.233193999894 39.92839699846957, -105.2333020002307 39.92840299930947, -105.2335169999823 39.92840799934192, -105.2338429992942 39.9284019990797, -105.2339589999796 39.92840599941181, -105.2342460000307 39.92840799944923, -105.2345579999572 39.92840399945201, -105.2346220868783 39.92839808298703, -105.235008498219 39.92954535037926, -105.2357094840183 39.93165934189567, -105.2360154780325 39.93263533803334, -105.236281472281 39.93344833402639, -105.2362914736262 39.93347633500713, -105.2363204718143 39.93355633311082, -105.2364244699075 39.93388233241797, -105.2365124675654 39.934211332045, -105.2365834657741 39.93454233001258, -105.2366494631262 39.9349403282457, -105.2367214605929 39.93554832524025, -105.2367244595431 39.93564532498768, -105.2367184583478 39.93593632327084, -105.2366914560335 39.93622632334893, -105.2365934533178 39.93682131971666, -105.2362604460931 39.93836731278099, -105.2361144443316 39.93896730909405, -105.2359764419444 39.93959030654941, -105.2358854385444 39.94007630426844, -105.2357694354685 39.94059430261459, -105.2356634342481 39.94112030001217, -105.2356304332279 39.94131729835097, -105.2356114323706 39.94151029746016, -105.2356014320325 39.94161229663906, -105.2355924294382 39.94190829551381, -105.2356074283079 39.94235429384504, -105.2356354249494 39.94272929243355, -105.235684424172 39.94310129046235, -105.2357704201069 39.94349128922146, -105.2358764195226 39.94388028719909, -105.2360184168766 39.9442792856082, -105.2362374114519 39.94482928352224, -105.2362994105811 39.94501728301593, -105.2363644094841 39.94521428241291, -105.2365134060399 39.94563127962134, -105.2365574053572 39.94586827954905, -105.2365854034608 39.94610727835873, -105.2365894029548 39.94626527741081, -105.2365814017142 39.9465022772988, -105.2365614007355 39.94666427533257, -105.2365313996723 39.94682527598022, -105.2364683993308 39.94706327408439, -105.2364103991369 39.94722027296941, -105.2363433979527 39.94737627311073, -105.2362663973395 39.94752527202102, -105.2361803968036 39.94767327125486, -105.2360353964538 39.94788527024479, -105.2358123949861 39.94815426851239, -105.2353373949938 39.94864726599771, -105.2349013944894 39.94908826348983, -105.2345443929722 39.94947226127717, -105.2341583927248 39.94993525893874, -105.2339843922855 39.95015925813851, -105.2338933927668 39.95028225714832, -105.2337133911016 39.95055025544299, -105.2332173879164 39.95142925195454, -105.2329263859335 39.95198824857948, -105.2328813846094 39.95204324832668, -105.2327903849929 39.95215824771139, -105.2327193862173 39.95224424719736, -105.232524383524 39.95259824508297, -105.2323133847181 39.95296324303607, -105.2320883826542 39.95329924107202, -105.2318913807338 39.95362223977587, -105.2318323814242 39.95370923934254, -105.2316703806363 39.95397423748284, -105.2314753793715 39.95433623591635, -105.2314223789011 39.95446223513391, -105.2313453770757 39.95467723363021, -105.2313003767481 39.9548462335438, -105.231253376375 39.95506123258171, -105.2312233748296 39.95522923168615, -105.2311983738348 39.95548223033251, -105.2311963731234 39.95565322998704, -105.2312023733035 39.9557382300675, -105.2312363718279 39.95601922818315, -105.2312903702832 39.95625422768943, -105.2313363694249 39.95640222747937, -105.2313723684942 39.95650822697466, -105.2313993672773 39.95657122608427, -105.2314743674655 39.95674822524581, -105.2315163654634 39.9568392256063, -105.2316053645577 39.95700022378365, -105.2317183627099 39.95718222346612, -105.2318093614744 39.95731022333126, -105.2319253601265 39.9574562223896, -105.2321203576787 39.9576752222892, -105.2321207867455 39.95767563668858, -105.2323323583044 39.95788022189713, -105.2323339852215 39.95788198466088, -105.2324863593553 39.95804721921932, -105.2334443494492 39.95875021940091, -105.233571348484 39.95868821912516, -105.233714348323 39.95861822001959, -105.2338239520144 39.95857110046063, -105.2338049737405 39.95855745128576, -105.2337782867351 39.95853826416749, -105.2336986413383 39.95848099104538, -105.2336468045691 39.95844371280378, -105.2336171748539 39.95842344796374, -105.2341725434769 39.9580392688392, -105.2347950472625 39.95760869288404, -105.2342243926122 39.95691524152589, -105.2341524978376 39.95682786948809, -105.2349909423702 39.95628870009567, -105.2376695730872 39.95553943080883, -105.237869403808 39.95544896598811, -105.2380925487423 39.95534793956568, -105.2381381075876 39.95533712804144, -105.2384707501498 39.9552581735205, -105.2387606413787 39.95522995514532, -105.2391404503259 39.95508480189946, -105.2392353862244 39.95517125116451, -105.2392371589414 39.95517286555238, -105.239258389572 39.9551921984806, -105.23927647946 39.95520867371651, -105.2394538794511 39.95516317297034, -105.2394675768633 39.95518923114921, -105.2396736377063 39.955581234407, -105.2406711572687 39.95439742475489, -105.240024053321 39.95392266004539, -105.2398894907311 39.95382393336795, -105.2398824476685 39.95381877110944, -105.2398473876931 39.95379304572359, -105.2398453407215 39.95379154330794, -105.2398296126404 39.95378000279207, -105.2399006156666 39.95375236339038, -105.2399205402457 39.95374460686801, -105.2399483505752 39.95372724911473, -105.2400416944829 39.9536974417265, -105.2400878385559 39.95367947772901, -105.240487048047 39.95352406659201, -105.2404916539113 39.95352201806195, -105.2408652368515 39.95346000915787, -105.240933089732 39.95344874590243, -105.2409499829143 39.95344750044689, -105.2409629638922 39.95344654341077, -105.2411807314999 39.95343048229564, -105.2412136382214 39.95342633392487, -105.2412244358653 39.95342464512465, -105.2412358248517 39.95342286488371, -105.2412578671857 39.95341887043079, -105.2412797394526 39.95341435681286, -105.2413014182228 39.95340933028208, -105.2413228882888 39.95340378900303, -105.2413441273671 39.95339774553509, -105.2413651120586 39.95339119802451, -105.2413858282717 39.95338415904898, -105.2414062525904 39.95337663125811, -105.2414263685928 39.95336862452243, -105.2414461540193 39.95336014509677, -105.2414655936254 39.95335120105296, -105.2414846663152 39.95334180044981, -105.2415033556772 39.9533319504559, -105.2415216464464 39.95332166454715, -105.2415395163498 39.95331095258089, -105.2415569548413 39.95329981813632, -105.2415739384536 39.9532882773729, -105.2415904554602 39.9532763365691, -105.2416064894054 39.95326401460206, -105.2416220297466 39.95325131415024, -105.24163705301 39.95323825317441, -105.241651550963 39.95322484246419, -105.2416655106915 39.95321109279873, -105.2416789145904 39.95319701764863, -105.2416924969039 39.95318372827051, -105.2417926015235 39.95306197295623, -105.2420940138068 39.95269873993102, -105.2423550234888 39.95238460880659, -105.242400847213 39.95232958199797, -105.2424229928676 39.95230461213298, -105.2424350975266 39.95228989182103, -105.2424467138614 39.95227494525179, -105.2424578289587 39.95225978320441, -105.2424684416042 39.95224441738487, -105.2424785412352 39.95222885587566, -105.2424881208034 39.95221310586636, -105.2424971779208 39.95219717996105, -105.2425056985141 39.95218108623425, -105.2425136860365 39.95216484000501, -105.2425211357905 39.95214844576619, -105.242528036016 39.9521319188029, -105.2425343843559 39.95211526361316, -105.242540178402 39.95209849820491, -105.242545419308 39.95208162708401, -105.2425500906432 39.9520646628231, -105.2425542040459 39.95204762256071, -105.2425577466438 39.95203050626817, -105.2425604849985 39.95201470223844, -105.2425631226928 39.95199611044753, -105.2425649537362 39.95197884892725, -105.2425662114527 39.95196156000681, -105.2425668899367 39.9519442580837, -105.2425669973535 39.95192695038124, -105.242566527808 39.95190964859498, -105.2425654812633 39.95189236263193, -105.2425638623396 39.95187510871434, -105.2425616698536 39.95185789044219, -105.2425589060715 39.95184072763487, -105.2425555709869 39.95182362209368, -105.2425516692268 39.95180658823951, -105.2425471983968 39.9517896404774, -105.2425469995326 39.95178899876466, -105.2425421690058 39.95177278513545, -105.2425365751554 39.9517560348095, -105.242530432015 39.95173940124199, -105.2425237313593 39.95172289342101, -105.2425164848536 39.95170652127981, -105.2425086947983 39.95169029563127, -105.2425003742863 39.95167477851509, -105.2424059484562 39.95151136733212, -105.2421494028326 39.95106741309232, -105.2421263742837 39.95102756327953, -105.2421244396496 39.95102421300519, -105.2421117923814 39.95100232933174, -105.2421532349839 39.9508776521355, -105.2422356511012 39.95062967915599, -105.2423203763545 39.95053644972544, -105.2423583595049 39.95045226550373, -105.2424326983841 39.95038139681725, -105.2424193456011 39.95036537308143, -105.2424164774736 39.95036192975837, -105.2424288673095 39.95035465582276, -105.2424902617059 39.95031861002217, -105.2428650690549 39.95009855353451, -105.2428848292195 39.95012039805992, -105.2428864176305 39.95012215428513, -105.2429218079034 39.95016127407835, -105.2432539182085 39.94997577837081, -105.2436207472383 39.94976943938573, -105.2436116776633 39.94976111333539, -105.2436098898687 39.94975947286139, -105.2435487854324 39.94970338529077, -105.2435552591411 39.94969465971476, -105.2437521608587 39.94942704577121, -105.2437723123789 39.94941200006306, -105.243901119003 39.94931583227635, -105.2439133601279 39.94929227305281, -105.2439907943965 39.94920904960991, -105.2438902370072 39.94913250436197, -105.243843496383 39.9490969244327, -105.2443336805456 39.94899766010215, -105.2450769997713 39.94893541989843, -105.2450769622432 39.94898556845416, -105.2450769407175 39.94901326183933, -105.2450769015449 39.94906353738384, -105.2450768554042 39.94912445058453, -105.2450768545068 39.94912625730254, -105.2450768068025 39.94918915554966, -105.2459288147174 39.9491932396644, -105.2459273019017 39.94880149693439, -105.2459270969151 39.94874811268062, -105.2459271138438 39.9487184180232, -105.2459271149365 39.94871560977393, -105.2459271527736 39.94865357973831, -105.2459280088195 39.94859022934073, -105.2464013539658 39.94842233398014, -105.2467081124108 39.948313522097, -105.2470891135391 39.94809851549275, -105.2472302242334 39.94801888546431, -105.2476083139154 39.94780552076305, -105.2476846981875 39.94776122618649, -105.2478094284176 39.94735633375443, -105.2478469404037 39.94723456492972, -105.2478433560362 39.94713228736064, -105.2478890047047 39.94705597092624, -105.2479304177987 39.9468527631968, -105.2479367866069 39.94684940326579, -105.2480295986053 39.94680042405117, -105.2485796528338 39.94651128238812, -105.2486454636441 39.94641330739307, -105.2487568057952 39.94624753735123, -105.248831466112 39.94598356233421, -105.249021310299 39.94563334264168, -105.249080831418 39.94552353705695, -105.2495449506102 39.94530671557963, -105.2503360267622 39.94525208564679, -105.2506537737573 39.9452363809138, -105.2509883201429 39.94522203648467, -105.2510883945363 39.94521343349978, -105.2511768961192 39.94520772446678, -105.2511800028379 39.94524977930156, -105.2511838734138 39.94530217534098, -105.2515099428432 39.94523367793365, -105.2518436376838 39.94515417827923, -105.2518477719972 39.94515670272256, -105.2518512447883 39.94515611576839, -105.2518547164191 39.94515552610967, -105.2518581857455 39.94515492653865, -105.251861651591 39.94515431885415, -105.2518651127853 39.94515370305352, -105.2518685751693 39.94515308185147, -105.2518720329022 39.94515245253334, -105.2518754918346 39.94515181511175, -105.2518789425989 39.94515117136789, -105.2518823933992 39.94515051771672, -105.2518858465593 39.94514985866664, -105.251889289211 39.9451491932892, -105.2518927354026 39.94514851981333, -105.251896174606 39.94514783731576, -105.2518996161757 39.9451471476179, -105.2519030495741 39.94514645249836, -105.2519064841721 39.94514574927545, -105.2519099141221 39.9451450370358, -105.2519133441015 39.9451443166902, -105.2519159145514 39.94514377282392, -105.2519167670797 39.94514359092548, -105.2519201889171 39.94514285705226, -105.2519236084339 39.94514211777003, -105.2519256753871 39.94514166558714, -105.2519270256396 39.94514137037679, -105.2519304405346 39.94514061487251, -105.2519338496082 39.9451398512497, -105.2519372587047 39.94513908132221, -105.2519406643201 39.94513830328125, -105.2519440664447 39.9451375198287, -105.2519474674253 39.94513672916829, -105.2519508625911 39.94513592858804, -105.2519542542693 39.94513512169561, -105.2519576448035 39.94513430759532, -105.2519610330267 39.94513348538403, -105.2519644165857 39.94513265865931, -105.2519677966735 39.94513182111915, -105.2519711744374 39.94513097907053, -105.2519745475565 39.94513012710465, -105.2519779218621 39.94512927063791, -105.2519812880159 39.94512840334556, -105.2519846541827 39.94512753245058, -105.2519880133548 39.94512665433513, -105.2519913737362 39.94512576541436, -105.2519947294501 39.94512487288078, -105.2519980781757 39.94512397132544, -105.2520014269308 39.94512306166417, -105.2520047721983 39.94512214569071, -105.2520081139781 39.94512122340501, -105.2520114487632 39.94512029389892, -105.2520147835744 39.94511935718746, -105.2520181149079 39.94511841146189, -105.2520214427504 39.94511746032477, -105.2520247647684 39.94511650196974, -105.2520280821318 39.94511553639932, -105.2520313995214 39.94511456362362, -105.2520347134299 39.94511358273439, -105.2520380226774 39.94511259643108, -105.2520413261068 39.9451116011086, -105.2520446283922 39.94511059857827, -105.2520479236795 39.94510958972817, -105.2520512201533 39.94510857637726, -105.2520545073116 39.94510755039697, -105.2520577933096 39.94510652171215, -105.2520610793434 39.94510548312004, -105.2520643572058 39.94510443910632, -105.2520676304072 39.94510338967851, -105.2520708989607 39.94510233123408, -105.2520741651999 39.94510126557928, -105.2520774291217 39.9451001936148, -105.252080686052 39.9450991135292, -105.2520839394946 39.94509802713147, -105.2520871917932 39.94509693352585, -105.2520904382705 39.94509583180172, -105.2520936765796 39.94509472375534, -105.2520969160751 39.94509361120816, -105.2521001520927 39.94509248964676, -105.2521033799521 39.94509135906114, -105.2521066054841 39.9450902248678, -105.2521098263649 39.94508908255848, -105.2521130414211 39.94508793303122, -105.2521162541663 39.94508677539298, -105.2521194610771 39.94508561323882, -105.2521226656769 39.94508444297368, -105.2521258656191 39.94508326639381, -105.2521290573995 39.9450820816904, -105.2521322515365 39.94508089248868, -105.2521354363483 39.9450796933595, -105.2521386153256 39.94507848971444, -105.2521417943322 39.94507727796344, -105.2521449663408 39.94507605989268, -105.2521481336949 39.94507483460657, -105.2521512975614 39.94507360300824, -105.2521544556032 39.945072364192, -105.2521576089873 39.9450711190611, -105.2521607588903 39.94506986581668, -105.2521639029653 39.94506860625501, -105.2521670423859 39.945067339478, -105.2521701783156 39.9450660672895, -105.2521733084173 39.9450647887837, -105.2521764326977 39.94506350215937, -105.2521795546639 39.94506220832474, -105.252182669632 39.94506090817035, -105.2521857811092 39.94505960260445, -105.2521888891053 39.94505828892499, -105.2521919901034 39.94505696892586, -105.2521950864469 39.94505564171133, -105.2521981757891 39.94505430907772, -105.2522012628204 39.94505296833312, -105.2522043451939 39.94505162127381, -105.2522074217362 39.94505026879794, -105.252210493624 39.94504890910668, -105.2522135585137 39.94504754309576, -105.2522166199256 39.94504616807063, -105.2522196755064 39.94504478762895, -105.2522227252527 39.94504340267135, -105.2522257738581 39.94504200960528, -105.2522288131219 39.94504061111508, -105.2522318465677 39.94503920360577, -105.2522348753491 39.945037791583, -105.2522379029864 39.94503637235244, -105.2522409212886 39.94503494589646, -105.2522439360999 39.94503351402893, -105.2522469450801 39.94503207674485, -105.2522499470686 39.94503063133973, -105.2522529443995 39.94502917961992, -105.2522559382492 39.94502771978662, -105.2522589250976 39.94502625453423, -105.2522619096219 39.9450247847735, -105.2522648848177 39.94502330598599, -105.2522678541855 39.94502182088132, -105.252270820056 39.94502033216641, -105.2522737789414 39.94501883352913, -105.2522767331494 39.94501733398111, -105.2522796815557 39.94501582091064, -105.2522826229475 39.94501430602371, -105.2522855596848 39.94501278392142, -105.2522884929345 39.94501125550695, -105.2522914203628 39.94500971897397, -105.2522943396065 39.94500818062199, -105.2522972530451 39.94500662964825, -105.2523001606396 39.94500507686057, -105.2523030659263 39.94500351506126, -105.2523059606881 39.94500195143796, -105.2523088519786 39.94500037699914, -105.2523117397717 39.94499879895016, -105.2523146170629 39.94499721277261, -105.252317489693 39.94499562118102, -105.2523203600023 39.94499402418045, -105.2523232186395 39.9449924190487, -105.2523260772863 39.94499081121498, -105.2523289266047 39.94498919435458, -105.2523317712685 39.94498757027878, -105.2523346100946 39.94498594258777, -105.2523374395856 39.94498430767137, -105.2523402632486 39.94498266643776, -105.2523430834208 39.9449810197926, -105.2523458965916 39.94497936772839, -105.2523487051111 39.94497770754813, -105.252351504289 39.94497604194386, -105.2523542988092 39.94497437002488, -105.2523570886649 39.94497269359248, -105.2523598726928 39.94497101084288, -105.2523626462154 39.9449693208654, -105.2523654162504 39.94496762457575, -105.252368179284 39.94496592286701, -105.2523709399968 39.9449642157493, -105.2523736890245 39.94496250410312, -105.2523764345645 39.94496078614474, -105.2523791719461 39.94495905916219, -105.2523819034965 39.94495732676307, -105.2523846303825 39.9449555898506, -105.2523873479302 39.94495384661338, -105.2523900608136 39.94495209886276, -105.2523927666989 39.94495034479245, -105.2523954667595 39.94494858350431, -105.2523981598155 39.94494681769777, -105.2524008458767 39.9449450446708, -105.2524035249366 39.94494326622485, -105.2524061993255 39.94494148506679, -105.2524088667262 39.94493969488705, -105.252411525962 39.94493789748446, -105.25241417936 39.9449360964666, -105.2524168245865 39.9449342900272, -105.2524194639786 39.94493247907191, -105.2524220987194 39.94493066000064, -105.2524247229484 39.94492883550277, -105.2524273448566 39.94492700559591, -105.2524299550862 39.94492516935929, -105.2524325618152 39.94492333041308, -105.252435161559 39.94492148154463, -105.252437754295 39.94491962905835, -105.2524403388627 39.94491777024991, -105.2524429175862 39.94491590962748, -105.2524454893214 39.94491403998344, -105.2524480563956 39.94491216492536, -105.2524506141249 39.9449102853439, -105.2524531636891 39.94490839853952, -105.2524557062489 39.94490650721674, -105.2524582453176 39.94490461048248, -105.2524607738779 39.94490270742096, -105.2524632989439 39.94490079984861, -105.2524658123281 39.94489888684717, -105.2524683198811 39.94489696842913, -105.2524708239463 39.94489504369899, -105.2524733163298 39.94489311353974, -105.2524758063826 39.94489118067343, -105.2524782847633 39.94488923967614, -105.2524807596564 39.94488729236664, -105.2524832240246 39.94488534323313, -105.2524856814013 39.94488338597866, -105.252488135287 39.94488142331268, -105.2524905786512 39.94487945792206, -105.2524930138569 39.94487748350729, -105.2524954432185 39.94487550727858, -105.2524978655852 39.94487352382955, -105.2525002797738 39.94487153676027, -105.2525026881378 39.94486954247318, -105.2525050883238 39.9448675445658, -105.252507481515 39.94486553943809, -105.2525098665282 39.94486353069011, -105.2525122433633 39.94486151832191, -105.2525146155505 39.9448594969371, -105.2525169772161 39.94485747282765, -105.2525193342173 39.94485544420483, -105.2525216818835 39.94485340835668, -105.2525240213717 39.94485136888823, -105.2525263538618 39.94484932310012, -105.2525286805207 39.94484727189551, -105.252530998995 39.94484521887192, -105.2525333069609 39.94484315952113, -105.2525356102689 39.94484109385569, -105.2525379651215 39.94483901208904, -105.252540327011 39.94483692583418, -105.2525426772219 39.94483483324961, -105.2525450250989 39.94483273885861, -105.2525473613071 39.94483063543593, -105.2525496916743 39.94482852929868, -105.25255201387 39.94482641773995, -105.2525543255507 39.94482430165525, -105.2525566337372 39.94482218105967, -105.2525589314087 39.94482005593821, -105.252561220912 39.94481792449454, -105.2525635045808 39.944815788535, -105.2525657812514 39.94481364625581, -105.2525680497376 39.94481150215764, -105.2525703088854 39.94480935173479, -105.2525725598618 39.94480719589041, -105.2525748026569 39.94480503732641, -105.2525770407876 39.94480287424906, -105.2525792695832 39.94480070394635, -105.2525814902041 39.94479852912275, -105.2525837014737 39.94479635157708, -105.2525859057418 39.94479416861237, -105.252588104182 39.94479197933045, -105.2525902920974 39.94478978822466, -105.252</t>
         </is>
       </c>
-      <c r="D19" t="n">
-        <v>24</v>
-      </c>
-      <c r="E19" t="n">
-        <v>24</v>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Southern Hills MS</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>1500 Knox Dr, Boulder, CO 80305</t>
+        </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>1500 Knox Dr, Boulder, CO 80305</t>
+          <t>http://shm.bvsd.org/</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
+          <t>Southern Hills Middle School</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>39.97413389369987</v>
+      </c>
+      <c r="K19" t="n">
+        <v>-105.2452260530946</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
           <t>http://shm.bvsd.org/</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>Southern Hills Middle School</t>
-        </is>
-      </c>
-      <c r="L19" t="n">
-        <v>39.97413389369987</v>
-      </c>
-      <c r="M19" t="n">
-        <v>-105.2452260530946</v>
-      </c>
       <c r="N19" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
-        </is>
-      </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>http://shm.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="P19" t="inlineStr">
         <is>
           <t>POINT (-105.2452260530946 39.97413389369987)</t>
         </is>
@@ -1772,59 +1690,53 @@
           <t>POLYGON ((-105.0551956991301 40.18184398208187, -105.0551970626169 40.18167032751156, -105.0551970875692 40.18166723030277, -105.05523025625 40.17744353616711, -105.0552302810579 40.17744046057113, -105.0552414762126 40.17601476607788, -105.0552513829568 40.17475301109806, -105.0552514076745 40.17474994901017, -105.0552519959952 40.1746750538799, -105.0552520195328 40.17467199268808, -105.0552526354381 40.17459269892721, -105.0552526542794 40.17458963771727, -105.0552531367156 40.17451028580081, -105.0552531555569 40.17450722459085, -105.0552583571967 40.17365096448745, -105.0552583760022 40.17364790868083, -105.0552600120969 40.17337863736143, -105.0552600297223 40.17337558245075, -105.0552661709637 40.17236480711001, -105.0552661885532 40.1723617576026, -105.0552760273123 40.17074210973164, -105.0552963083236 40.16740327517449, -105.0552966362117 40.16734916580195, -105.0553334854068 40.16102383273662, -105.0553368567356 40.16044496943694, -105.0553372380196 40.16037944725436, -105.0553376788475 40.16030391644374, -105.0553377713311 40.16028796999728, -105.0580710513005 40.16025799056519, -105.0606010313516 40.16022699272562, -105.062539016009 40.16009099355082, -105.0634333444827 40.15986251985857, -105.064296309749 40.15959008850385, -105.064919505624 40.15935175545492, -105.0662970046367 40.1588843247345, -105.066765552507 40.15964313063317, -105.067322977026 40.16013699897744, -105.0678959694674 40.1604240008717, -105.0687409608614 40.16070000328342, -105.0694111630307 40.16090422372054, -105.0694629539653 40.16092000499503, -105.0705369421375 40.16129000865394, -105.0719189271613 40.16175401236442, -105.0730759142553 40.16213901527696, -105.0739259058449 40.16241901849396, -105.0744968993014 40.16262302002178, -105.0756918859996 40.16302902328239, -105.0775498655427 40.16357702807103, -105.0787978532788 40.16380003091128, -105.0795948459216 40.16388103180415, -105.0802848402826 40.16392203294821, -105.0807888352324 40.1639220337433, -105.0813998304982 40.16392203444205, -105.0829128177578 40.16392203457659, -105.083609519032 40.16392308127849, -105.0836161082395 40.16399500687811, -105.0836141587786 40.16413802271901, -105.0836030415373 40.16460987586909, -105.0836106635436 40.16484891209912, -105.0836300593452 40.16545713053579, -105.0836269525403 40.16549692411329, -105.0836220561698 40.16553698593949, -105.083613938554 40.16557703616078, -105.0835959221352 40.16565603140108, -105.0835711141966 40.16573390518737, -105.0835558587693 40.16577090983481, -105.0835398631979 40.16581202954788, -105.0835210296103 40.16584902129782, -105.0835000500647 40.16588600531175, -105.0834769351456 40.1659210605575, -105.0834260412004 40.16599307439358, -105.0833268254032 40.1661261315451, -105.0832439014171 40.16622795275293, -105.0832150677106 40.16626188854235, -105.0831919525168 40.16629694372924, -105.0831681144781 40.16633309328626, -105.0831478259643 40.16637392366613, -105.0831339771326 40.16641505106289, -105.0831190490881 40.16645699775201, -105.0831080505025 40.16650005739481, -105.0830950003841 40.16658593425269, -105.0830878765151 40.16693097503487, -105.0830959771383 40.16724395293009, -105.0830960976557 40.16792502758191, -105.0830930531922 40.16830494684462, -105.0830910643746 40.16868788974446, -105.0830899607455 40.16886796812796, -105.0830891382825 40.16941095828075, -105.0830898739331 40.16975794923593, -105.0830908276374 40.17077009335227, -105.0830780316235 40.17151508279193, -105.083075148123 40.17192712109441, -105.083080876397 40.17274410150467, -105.0830810478255 40.17329999660924, -105.0830759771914 40.17348500237775, -105.0830749017534 40.17371888591792, -105.0830771760332 40.1739901157939, -105.0830668337051 40.17410098249666, -105.0830771458684 40.17399043991578, -105.088302814376 40.1739809907825, -105.0883029993709 40.17397700160376, -105.0883031426125 40.17397700121329, -105.0883123178483 40.17397704920117, -105.0888742073944 40.17397999371771, -105.0892635502055 40.17397922794395, -105.0898870002667 40.17397799833534, -105.0899358508228 40.17397797709733, -105.0920959995587 40.17397699788575, -105.0920961416262 40.17397699748644, -105.0920962144237 40.17397699684266, -105.0928349994319 40.17396899906539, -105.0928751701174 40.17396600181887, -105.093035412355 40.17395404356559, -105.0930355022931 40.17396373747397, -105.0930905495083 40.1739629603663, -105.0933063695626 40.17394767675843, -105.0947811388498 40.17392604651604, -105.0950699350661 40.17392596063161, -105.0955101015059 40.1739269531794, -105.0957541527641 40.17392890476933, -105.0963270854283 40.17393008282001, -105.0964931512326 40.17392709427654, -105.0974990948966 40.17392895400177, -105.0977370735687 40.17392895919532, -105.0979528772734 40.17392696481058, -105.0981518434555 40.1739279313386, -105.0989699184054 40.17392802714794, -105.0998391512321 40.17393103942207, -105.1001161310761 40.17393199790583, -105.101211927436 40.17392892050625, -105.1023799809039 40.17393102219533, -105.1024508498185 40.17392907018132, -105.1024948495252 40.17393196664215, -105.1024928436826 40.1739690192746, -105.1024659300747 40.1745939986924, -105.1024538771325 40.17579907983215, -105.1024459726393 40.17647792955385, -105.102446985836 40.17691688312216, -105.1024359298053 40.17764513457093, -105.1024348285392 40.17795588288692, -105.1024151073728 40.17943188442915, -105.102413175028 40.18019091209275, -105.1023970324222 40.18093204823994, -105.1023829530066 40.18125894705506, -105.1023831548078 40.18140800978896, -105.102370035092 40.18248900592155, -105.1023460249624 40.18414699542499, -105.1023359709285 40.18488705328424, -105.102324014524 40.18558510414968, -105.102314050903 40.18661587375054, -105.1022961545613 40.18759500754209, -105.1022951231635 40.18764908370499, -105.1022919348154 40.18813304226678, -105.1022929712663 40.18856787832284, -105.1022938744325 40.18859697923833, -105.102305841591 40.18899891023079, -105.1023129456827 40.18974287047573, -105.1023359238445 40.19064912338679, -105.1023450792598 40.19183807835071, -105.1023480324539 40.19219001707661, -105.1023401095519 40.19238187512373, -105.1023501276933 40.19385193690373, -105.1023748592168 40.19451991641212, -105.1023850650994 40.1948559566662, -105.1023868541003 40.19503988820251, -105.1023809230087 40.19574811518007, -105.1023788304601 40.19586093436818, -105.1024139175533 40.19696213301737, -105.1024319782109 40.19815907813807, -105.1024859020631 40.19952909100861, -105.1024847271985 40.20065462381238, -105.1024006556609 40.20088934679336, -105.1024054437498 40.2013562575215, -105.102421336487 40.20328529873123, -105.1024213646525 40.20328751259089, -105.1024214449243 40.20329367141449, -105.1024151901731 40.20329347428748, -105.1018971891388 40.2032814736801, -105.1018961897053 40.20421247454206, -105.1025107003073 40.20422330641446, -105.1025237619839 40.20539370203086, -105.1025237636843 40.20571670054039, -105.1025437709455 40.20634669622018, -105.1025137811899 40.20727069089985, -105.1025047847938 40.20772268878633, -105.102465788828 40.20820268604596, -105.102494799139 40.20914168066236, -105.1024778062865 40.2099546758207, -105.1024751480868 40.2103992398415, -105.1020764826853 40.210400971623, -105.0978221643321 40.21038836945402, -105.0978192865362 40.20995801171471, -105.0978192638643 40.20995469549757, -105.0977981545344 40.20679786929404, -105.0976247893968 40.20679703029651, -105.0976247948587 40.20679491652393, -105.0971607119664 40.20679337303581, -105.0971599989639 40.20679337055231, -105.0954331146536 40.20678761374383, -105.0932545485407 40.20678031284936, -105.0932022136999 40.20678056108493, -105.0932041876712 40.206406475457, -105.0932105779957 40.2051159902964, -105.0932147345931 40.20427675894129, -105.0932201875574 40.20317547481145, -105.0930820960962 40.20317412349315, -105.093005727191 40.20317337651804, -105.09300572348 40.20317301534985, -105.0928657727666 40.20317203549725, -105.0926146724067 40.20317027581347, -105.0921975370513 40.20316735111282, -105.0919455217571 40.20316558314721, -105.0917522278974 40.20316422728517, -105.0914944937617 40.2031624183343, -105.0912832223234 40.20316093513956, -105.0908696894077 40.20316115529705, -105.0904716416836 40.20316441081984, -105.0897408380691 40.20317038385568, -105.088853254461 40.20317763139809, -105.0877735888691 40.20318643920209, -105.0856447171413 40.20320449486757, -105.0837211863008 40.203227474651, -105.0835981069327 40.20321967515504, -105.0835791856489 40.20321847582563, -105.0830682814023 40.2032196909061, -105.0822069163204 40.20323024316917, -105.0816501847357 40.20324047561559, -105.0806879610338 40.20324837306046, -105.0798893828385 40.20325404710055, -105.0790784538952 40.20326612103604, -105.0787342713654 40.20327551513552, -105.0783671987761 40.20327647585538, -105.0779601843807 40.2032754757722, -105.0776037795553 40.20327547689448, -105.0765138064435 40.20327584437361, -105.0747471835121 40.20329593233741, -105.0741741031875 40.20330244293366, -105.0741613829337 40.20330267867917, -105.0740449135742 40.20330506064477, -105.074014699015 40.20330567887017, -105.0690749998827 40.2033999992119, -105.067296999437 40.20343799958135, -105.0662489993874 40.20346199884766, -105.0650095092602 40.20349053724983, -105.0649459997082 40.20349199875547, -105.0647999996946 40.20349499884104, -105.0647763071737 40.20349548788953, -105.0647501006766 40.20349602781442, -105.0647029999319 40.20349699885044, -105.0625290002004 40.20354499890966, -105.0605809999359 40.20358599860956, -105.0604691803914 40.20358828730515, -105.0594589803057 40.20360895889921, -105.0594569996611 40.2036089990881, -105.0594407995711 40.20360935166872, -105.058538999233 40.20362899881254, -105.056911999972 40.20367299893432, -105.0557639998678 40.20367599809817, -105.0557612194496 40.20367601713887, -105.0551933208667 40.20367993430043, -105.0551658094086 40.20367990683798, -105.0551658058408 40.20367704099404, -105.0551658037605 40.20367628174822, -105.0551657962894 40.20366431764384, -105.0551658011341 40.20366106365725, -105.055165939419 40.20355375046467, -105.0551659441694 40.2035505108879, -105.055166559143 40.20308397822347, -105.0551673600189 40.20247699891858, -105.0551687234147 40.20144399367533, -105.0551698371555 40.20059995386577, -105.055169869857 40.20057520624766, -105.0551698743182 40.20057201079945, -105.0551708702638 40.19981742814952, -105.0551708746955 40.19981423720408, -105.0551741094728 40.19736226693898, -105.0551741138158 40.19735908950151, -105.0551753876223 40.19639540436918, -105.0551753942906 40.19639223054278, -105.0551776862514 40.19523231880929, -105.0551776917097 40.19522915038146, -105.0551857428336 40.19115277071814, -105.0551895198951 40.1892402250088, -105.0551895204548 40.18923708718096, -105.0551895524011 40.1891528441331, -105.0551895553035 40.18914970721488, -105.0551896237061 40.18907048357343, -105.0551896265968 40.18906734845638, -105.0551907707022 40.18769647581839, -105.0551953437782 40.18224286923797, -105.0551953462757 40.18223997368663, -105.0551956753519 40.18184707929512, -105.0551956991301 40.18184398208187), (-105.0682879304474 40.17423889546031, -105.0679761762959 40.1742478872944, -105.0682879316216 40.17423889546469, -105.0705337647592 40.17417980111477, -105.0682879304474 40.17423889546031), (-105.0741833857628 40.19582695548362, -105.0741934852469 40.19582692062273, -105.0860866501783 40.19578522125577, -105.0741833857628 40.19582695548362), (-105.0741833528738 40.19582695582105, -105.0741833528728 40.19582695626313, -105.0741833857628 40.19582695548362, -105.0741833528738 40.19582695582105))</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>27</v>
-      </c>
-      <c r="E20" t="n">
-        <v>27</v>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Trail Ridge MS</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>1000 Button Rock Dr, Longmont, CO 80504</t>
+        </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>1000 Button Rock Dr, Longmont, CO 80504</t>
+          <t>https://trms.svvsd.org/</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
+          <t>Trail Ridge Middle School</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>40.17693117783666</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-105.0576162268638</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
           <t>https://trms.svvsd.org/</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>Trail Ridge Middle School</t>
-        </is>
-      </c>
-      <c r="L20" t="n">
-        <v>40.17693117783666</v>
-      </c>
-      <c r="M20" t="n">
-        <v>-105.0576162268638</v>
-      </c>
       <c r="N20" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>https://trms.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="P20" t="inlineStr">
         <is>
           <t>POINT (-105.0576162268638 40.17693117783666)</t>
         </is>
@@ -1844,35 +1756,29 @@
           <t>POLYGON ((-105.4661484313311 40.16510540791135, -105.46628891067 40.16510477709761, -105.470815740543 40.16518143398583, -105.4708146541582 40.16519354991458, -105.4707617910061 40.16578360363307, -105.4707617862852 40.16578366217297, -105.4705125686798 40.16856524699041, -105.4704672528061 40.1690710003927, -105.4704561694049 40.16919470380456, -105.4704014266738 40.1698729832864, -105.4703235422809 40.17083798352486, -105.4701471120568 40.17302390050776, -105.470147089627 40.17302417969756, -105.4701398981323 40.17311326375602, -105.4701498775658 40.17311351851009, -105.470200732758 40.17311482223527, -105.470709432716 40.1731278654992, -105.4711861857428 40.17314008889846, -105.471439289043 40.1731465768118, -105.4727391684574 40.17317988978623, -105.4749708600473 40.17323704782745, -105.4750032321987 40.1726821562563, -105.4750206722191 40.17238323337168, -105.4750210361202 40.17237698847438, -105.4752042504024 40.16923656802826, -105.479787691759 40.16935887360058, -105.4797873653326 40.16937091048318, -105.4797734359278 40.16988387259018, -105.4797733872597 40.16988566754004, -105.4796805373642 40.17330482726621, -105.4796240684069 40.17656529689094, -105.4796152483834 40.17796396985926, -105.4796026937846 40.17995501780022, -105.479611783183 40.17995483837693, -105.4809046495147 40.17992930563622, -105.4809104417855 40.17992919131213, -105.4821456944617 40.17990478346833, -105.4842904768209 40.17986236891954, -105.4842904845098 40.17987483273979, -105.4842905938626 40.18005209836011, -105.484290852698 40.18047691385383, -105.4842909836418 40.18069288673419, -105.4842919357208 40.18225457717938, -105.4842923359611 40.18291119120383, -105.4842927315417 40.18355750826427, -105.4843017355777 40.18355781209871, -105.4858596675139 40.18361035232417, -105.4887108236855 40.18370645233315, -105.4890342964373 40.18371735136233, -105.4913673103303 40.18380308278645, -105.4916169415424 40.18381225335324, -105.493803003558 40.18389564358236, -105.4938093397902 40.1838958852905, -105.4938123200268 40.18389599982997, -105.4938523169958 40.18035330559622, -105.4938523205461 40.18035299938223, -105.4942081234937 40.18036470973328, -105.4942254027887 40.18036558420872, -105.4988689323545 40.18060051532034, -105.5037971648563 40.18084965648772, -105.5066788071574 40.18091382279687, -105.5115988430433 40.18102320894966, -105.5138093385616 40.18107228813918, -105.5207705453987 40.18122672640443, -105.5208006874244 40.18122739465633, -105.522236754261 40.18127360796668, -105.5222435283211 40.18127382641728, -105.5222435741154 40.18127382730909, -105.522435320304 40.18127999739902, -105.5224377955276 40.18127643582816, -105.5224378823772 40.18127630972313, -105.523680357985 40.181292988343, -105.523688178229 40.1812930930153, -105.5236896753479 40.18129311342297, -105.5237041709683 40.18072051517435, -105.5237197330747 40.18010577977868, -105.5237413580885 40.17925150068127, -105.5237454789506 40.17908870192743, -105.5237510683669 40.17886786445666, -105.5237651645466 40.17831101269118, -105.5237857437776 40.17749800315436, -105.5238776530766 40.17387231186575, -105.5258247721261 40.17387231837259, -105.5258340931253 40.17387231809113, -105.5332652858553 40.17387203873018, -105.5332746068535 40.17387203604751, -105.5332742031089 40.1738843189681, -105.5331893193217 40.17646799626176, -105.5331568626344 40.17752450998029, -105.5331662580995 40.17752449827886, -105.5332269975165 40.17752442499798, -105.5332266806333 40.17753671869425, -105.5331269808046 40.18141083850799, -105.5330262556054 40.1837602446121, -105.532976230018 40.18492700366666, -105.5328963810823 40.18678931519381, -105.5328252778692 40.18844755645122, -105.5328252743849 40.18844763660821, -105.5328144473783 40.1887670954498, -105.5328026033848 40.18959315645375, -105.5327760272405 40.19144611821562, -105.5327628767569 40.19236313910528, -105.5327720701403 40.19236356970227, -105.5328092241853 40.19236530368316, -105.5328090737093 40.1923771568957, -105.5328019262174 40.19293933922767, -105.5328018956497 40.19294170518686, -105.5328006690869 40.1930380970772, -105.5328098787648 40.19303559882346, -105.5328294254024 40.19303029578, -105.5328935660998 40.19301413198865, -105.5329570730651 40.19299410915016, -105.5330083598834 40.19297567307023, -105.5330790606768 40.1929545853694, -105.5331549173888 40.1929269242624, -105.5332445784334 40.19289053114875, -105.5333357318797 40.19285139332066, -105.5334323856855 40.19282329373202, -105.5335304733625 40.19279520175227, -105.5336091149603 40.19277140683688, -105.5336459058447 40.19275785969391, -105.5336515583924 40.19275577849825, -105.533684251341 40.19274374108799, -105.5337565232855 40.19271606081569, -105.5338179414305 40.19269327228345, -105.533890165039 40.19266779307718, -105.5339501238616 40.19264610006633, -105.5340122329798 40.19262441809995, -105.5341047369489 40.19258913845898, -105.5341957862916 40.19255495433799, -105.5342200411473 40.19254790514945, -105.5342198678148 40.19256285923371, -105.5342193376537 40.19260852935302, -105.5342183473157 40.19269425235101, -105.5342183360385 40.19269518000148, -105.5342180715312 40.19271798939261, -105.5342271532779 40.19272517011618, -105.5343393829121 40.19281390637015, -105.5346356497051 40.19259680260618, -105.5348823209668 40.19251699672893, -105.5349371865247 40.19249180670148, -105.5349909777208 40.19246710871604, -105.537495561658 40.19258391871914, -105.5375025897888 40.19185229996346, -105.5375101454505 40.19106602720946, -105.5375433224156 40.1910399954814, -105.5375224677095 40.18937951494874, -105.5375223216064 40.1893679950532, -105.5372715249519 40.18934647278628, -105.537254321171 40.18934499589563, -105.5375677880135 40.18893092853408, -105.5375946466315 40.18889544853639, -105.541762862168 40.1891617345586, -105.5422569890588 40.18918897106952, -105.5422571009006 40.18920076026023, -105.5422758519701 40.1911640951709, -105.5422833975333 40.19195391480071, -105.5422833975938 40.19195401206859, -105.542297092536 40.19338773536003, -105.5422970925746 40.19338779750338, -105.5423024628827 40.19394992984792, -105.5423929265994 40.20341858732859, -105.542401834668 40.20341858226157, -105.5424019515685 40.20343087127191, -105.5471617411033 40.203428251832, -105.5471710649767 40.20342824622806, -105.5471762500321 40.20702449927905, -105.5471669256137 40.20702443013139, -105.5469038813974 40.20702247197197, -105.5423441045886 40.20698842150102, -105.5423441034594 40.20698849445215, -105.5422953313193 40.21055420708196, -105.5422860075863 40.21055412132916, -105.5404398525206 40.21053711938241, -105.5326909158406 40.21046358966055, -105.5326905760758 40.21136204136256, -105.5326905761208 40.21136213502758, -105.5326902668153 40.21217981128849, -105.5326894995797 40.21419262998702, -105.5326895026425 40.21419411331591, -105.5326985284376 40.21419413237972, -105.5422526119581 40.21421377049138, -105.5422524668593 40.21422603345813, -105.5422084115658 40.21794388539156, -105.5411373910101 40.21826779544625, -105.5398831425591 40.21944693342513, -105.5379809748795 40.21961963612427, -105.5379291219123 40.21962350240685, -105.5378566567431 40.21962890467403, -105.5364658151693 40.21975515971221, -105.5364659849748 40.21975632326548, -105.536469145231 40.2197779543675, -105.5364610049816 40.21977874858243, -105.5360297782496 40.21982080776719, -105.5360049453737 40.2214518136923, -105.5348769137664 40.22144872610919, -105.5338911592008 40.22144602273305, -105.5333207578963 40.22144445293673, -105.5326849358092 40.22144269979285, -105.5326849473221 40.2214446523428, -105.5326967674883 40.2233561262393, -105.5326825303639 40.22418840574673, -105.5326820404199 40.22504857987344, -105.5326910735317 40.22504859983672, -105.5344553890728 40.22505242161549, -105.5353538558136 40.22505402382836, -105.5360637775385 40.22505528352068, -105.5364251454815 40.22505592322528, -105.5364318357178 40.22505593462795, -105.536760204845 40.22505651522585, -105.5373800222655 40.2250576054056, -105.5374809703504 40.2250577834895, -105.5385255461858 40.22505961624928, -105.5405764553367 40.22506318763808, -105.5419484417806 40.22506555326001, -105.5419590751946 40.22506557191936, -105.5420808495041 40.22506765406047, -105.5420823229212 40.22506767874194, -105.5420822364319 40.22507980477056, -105.5420562713165 40.22872637531357, -105.542057627296 40.22872637662191, -105.5420429039838 40.2322667322377, -105.5418212665354 40.24069807142973, -105.5417703294095 40.24320999597101, -105.5417913293522 40.24484599488542, -105.5418693303538 40.25068399588682, -105.5419533310875 40.25691899504218, -105.5420123310872 40.26132699564431, -105.5420510583876 40.26143505394957, -105.5420511054112 40.26143505393247, -105.5420601092523 40.26143504165487, -105.546896776124 40.26142835486699, -105.5469164731246 40.26142832707124, -105.5488073098715 40.26142565841789, -105.5516765188264 40.26142154904153, -105.5516962275788 40.26142152042718, -105.5564490412647 40.26141455566594, -105.5564687629445 40.26141452623263, -105.5591675481954 40.26141048439985, -105.559187278102 40.26141045449919, -105.5591940095238 40.26141044475258, -105.5610087103939 40.26140744097114, -105.5795558249904 40.26109930837292, -105.5795753264785 40.2610990572043, -105.5951059878192 40.26090826365041, -105.5951255644495 40.26090802240864, -105.5978803250462 40.26087396174936, -105.5978999087103 40.26087372003241, -105.5990498899888 40.26085948275252, -105.5990694865891 40.26085924983279, -105.5995397909104 40.26085370200565, -105.5995593945634 40.26085347079817, -105.6024803232683 40.26081898919289, -105.6142594281275 40.26067918769429, -105.6159287966142 40.26065927760523, -105.6159484448253 40.26065904267666, -105.6183738399164 40.26063000678786, -105.6183934869193 40.2606297624392, -105.6213214042607 40.26059298525797, -105.6213410559414 40.26059273860285, -105.6230240548107 40.26057156630034, -105.6230437100057 40.26057131935239, -105.6277277549875 40.26051225854213, -105.627747425429 40.26051200987794, -105.632275471989 40.26045473382353, -105.6322951553285 40.26045448437176, -105.6333595672079 40.26044099555356, -105.6333792540661 40.26044074591335, -105.6336239250111 40.26043764207176, -105.6336436106918 40.26043739238794, -105.6344099544128 40.26042767444419, -105.6344296424389 40.26042742462398, -105.6344533637605 40.26042712418371, -105.6344730517862 40.26042687435609, -105.6370401114326 40.26039427547199, -105.6370598053172 40.2603940251974, -105.641661457955 40.26033544727563, -105.6416811682616 40.26033519529398, -105.6421922091127 40.26032867946999, -105.6422119170661 40.2603284283015, -105.6463212330816 40.26027594287727, -105.6463409574624 40.26027569098492, -105.6510511032203 40.26021535336445, -105.6510708369704 40.26021510065377, -105.653220247745 40.26018750197031, -105.6534108731882 40.2601810802276, -105.6533823627512 40.26010275780921, -105.6532830172156 40.25994882313275, -105.6532015168119 40.259833817446, -105.6530755380744 40.25970888806435, -105.653056450447 40.25969061631895, -105.6528639596007 40.25950741268624, -105.6526889307466 40.2593871624231, -105.652642514434 40.25935601447338, -105.6524271025182 40.25918859577206, -105.652112632482 40.25892918790828, -105.6518414912158 40.25866632340869, -105.6518412163808 40.2586659058817, -105.6518402220181 40.25866439414499, -105.6518249196642 40.25864111788805, -105.651683174363 40.25842552064559, -105.6516722710576 40.25840806831427, -105.6515514218632 40.25817243805065, -105.6515429003808 40.25815503662493, -105.6514243241588 40.25786656297638, -105.6514187228448 40.25784972511072, -105.6514055789766 40.25757162818682, -105.6513344204328 40.25729383767664, -105.6513306212376 40.25727751710651, -105.6512928566423 40.25697723763877, -105.6512494136496 40.25670131742907, -105.6512475526345 40.25668592286098, -105.6512481806062 40.25659521519253, -105.6512491443465 40.25645626717135, -105.6512492414307 40.25644232184331, -105.651250394949 40.25627562546527, -105.6512238153397 40.25580599850561, -105.6512233117349 40.25579151809188, -105.6512386810696 40.2554038107325, -105.6512392740317 40.25539031326282, -105.6512547967072 40.25511750050543, -105.651254798984 40.25511746717952, -105.6512556523308 40.25510424315733, -105.6512679930778 40.25496298995328, -105.651283544426 40.25478497372899, -105.6512465313483 40.25451425149574, -105.6510657606499 40.25415446368373, -105.651056843717 40.25413708614312, -105.6508969847668 40.25382258276831, -105.6505310873636 40.2534957431415, -105.6505198035114 40.25348589422141, -105.650277580469 40.25334159185142, -105.6502158172845 40.25330586876338, -105.6497508549943 40.25305330688136, -105.6493031225032 40.25278747457062, -105.6489024621259 40.25250204640531, -105.6485320184643 40.25224942820618, -105.648122926153 40.25197372674319, -105.6478519627375 40.25176733123399, -105.647595323896 40.2516000866161, -105.6474810359026 40.2515261922803, -105.6473040944805 40.25143101667013, -105.6471837932539 40.25136724816764, -105.6468534777815 40.25120486346038, -105.6466993803544 40.25114202354365, -105.6465010494459 40.25106199343578, -105.6463131316636 40.25101511518552, -105.6461854347542 40.25098444290174, -105.6459617149985 40.25091212623183, -105.645862718699 40.25086625543839, -105.6439109359637 40.24997257845546, -105.6439113906358 40.24997248152362, -105.6440326178304 40.24994670984607, -105.6460486209198 40.24951810932338, -105.6461040002026 40.24950599091284, -105.6461040377955 40.24950598185919, -105.6461837138841 40.24948586944218, -105.6461837538199 40.24948585678304, -105.6462761693258 40.24945621494909, -105.6462878338384 40.24945293635419, -105.6465034720074 40.2493933900957, -105.6465165544287 40.24939030511742, -105.6468338582291 40.24931722103709, -105.6468479730201 40.24931432744434, -105.6473447774411 40.24921444122509, -105.6473620074362 40.24921285670883, -105.6478251640483 40.24917729760249, -105.6478451563986 40.24917744047953, -105.6483876106674 40.24918924142482, -105.6484084764347 40.24918997028969, -105.6490580710522 40.24921440685837, -105.6490793598224 40.24921560338041, -105.6496621472309 40.24925061573745, -105.649857509743 40.24926235109255, -105.6498792923866 40.24926416375346, -105.6504807419691 40.24931712691847, -105.6505029278615 40.24931949642218, -105.6510873439726 40.249384258711, -105.6510876331863 40.24938428985514, -105.6517955093473 40.24946011446387, -105.6524384646635 40.24946103545784, -105.6532240381383 40.24939543248849, -105.6532429858952 40.24939464187201, -105.6540359245012 40.24936764317474, -105.6540561108867 40.24936779732936, -105.6547920954059 40.24937937171175, -105.6548135707898 40.24938089655689, -105.6553635528423 40.24942562557963, -105.6560772134397 40.2494691280667, -105.6560990989358 40.2494710970272, -105.6566697271875 40.24952454693272, -105.6572882420254 40.24953298344785, -105.6572884124538 40.2495329823156, -105.6577466825842 40.24952787256891, -105.6577468823637 40.24952785698604, -105.658364554839 40.24947889500469, -105.6583837733506 40.24947829771016, -105.658383836817 40.24947829582203, -105.6588610698823 40.24946552024045, -105.6593578213218 40.24936558880857, -105.6596740517714 40.24922577817019, -105.6598284918649 40.24908374683517, -105.6600357955445 40.24885510058633, -105.6601709350914 40.24869839282666, -105.6602180098776 40.24847606239258, -105.6602904669786 40.24808708989965, -105.6603197434563 40.24775706340495, -105.6603209213945 40.24774420990298, -105.6603381955352 40.24758479666077, -105.6603395938818 40.24757220763556, -105.6603473707779 40.24750678741342, -105.6603488540162 40.24749431264927, -105.6603658886433 40.24735099924052, -105.6603676534624 40.2473388122845, -105.6604413607002 40.24701574268065, -105.6604416576382 40.2466576694766, -105.660406673147 40.24625862093598, -105.6604060936211 40.24624414514405, -105.6604638791043 40.2458376972433, -105.6604423228038 40.24554413969873, -105.6604183656476 40.24532331789342, -105.6604176166594 40.24530874776879, -105.6604654929911 40.24502852130396, -105.6604680799253 40.24501810382434, -105.6606031082612 40.24480953958241, -105.6608380761308 40.24465551037683, -105.661090919282 40.24451736259382, -105.6614394345306 40.24425372862866, -105.6617972409519 40.24400229844849, -105.661993737268 40.24379598909656, -105.6622515148447 40.24354079687833, -105.6623638976777 40.24339320647818, -105.6623412545372 40.243148140186, -105.6622271542483 40.24289913312061, -105.6622212185086 40.24288262853066, -105.662246928383 40.24270330468485, -105.6622493009619 40.24269235519348, -105.6624203867668 40.24238932411787, -105.6626383198902 40.24217056212871, -105.6627478603099 40.2420858297572, -105.6628966257281 40.24188143849485, -105.6630035083658 40.2416272908031, -105.6630070175849 40.24161941982204, -105.6631343254574 40.24137469705771, -105.6632915945943 40.24121971764026, -105.6634577117512 40.24103557054804, -105.6636414775772 40.24080598165017, -105.6638605888681 40.24047958579609, -105.6641361334141 40.24008308784516, -105.6643937880334 40.23986345373206, -105.6646430665669 40.23956239662796, -105.6647837931359 40.23929073503575, -105.6649769754472 40.23895438237981, -105.6651788634559 40.23861149463966, -105.665323466031 40.23835513830205, -105.6653962474659 40.23809944644505, -105.665431211319 40.23766674878126, -105.6654329294115 40.23765467076841, -105.6655795293855 40.23730339632174, -105.6656516849346 40.23700392224806, -105.6655733758443 40.23677124300807, -105.6654192999047 40.23653663304073, -105.6652664880635 40.23634685679159, -105.6651081521364 40.23616363214872, -105.6650945635468 40.23614659102824, -105.6649503217293 40.23588669668948, -105.6649408301455 40.23586931017438, -105.6648173713558 40.23562903403352, -105.6648096253163 40.23561180533154, -105.6647862204469 40.23550442489909, -105.6647251887129 40.23522442147496, -105.6647251756337 40.23522435844993, -105.6646582848182 40.23494468934514, -105.6646546756029 40.23492852738642, -105.6645951132258 40.23457015220544, -105.6645927169959 40.23455456581809, -105.6645619404331 40.23428038048088, -105.6645609881937 40.23426566023956, -105.6646107631039 40.23381407701542, -105.6646123901615 40.23380175146494, -105.6646686018296 40.23352436399449, -105.6646712989217 40.23351378322931, -105.6648220164282 40.23318151580031, -105.6648255241641 40.23317475342208, -105.6650047084142 40.2329491006681, -105.6651964929561 40.2327528359099, -105.6654011529644 40.23258888212007, -105.6657063539013 40.23236997563181, -105.6659413331565 40.23217075944036, -105.6661675652812 40.23202312776482, -105.6663889616327 40.23191128709515, -105.6666810970455 40.23171510873143, -105.6666926686825 40.23171249465987, -105.6670132530934 40.23164008776747, -105.6670310503309 40.23163893539422, -105.6670310985044 40.23163893352346, -105.6671542201482 40.23163200282799, -105.6671543176415 40.23163198737654, -105.6673891053773 40.23159393428879, -105.6675672799185 40.23153819341664, -105.6677025916841 40.23133320802084, -105.6677681890939 40.23097816878754, -105.6677631503988 40.23075299479768, -105.6677483196333 40.23044769834121, -105.6677481743348 40.23043358126473, -105.6677741899327 40.2302316910987, -105.6677764100459 40.23022044448404, -105.6678022827057 40.23016966127873, -105.6679082388013 40.22996248731734, -105.6680695015121 40.2297791769222, -105.6682133000139 40.22966333765718, -105.6684010177816 40.22951487491294, -105.6685625454325 40.22935359900887, -105.6687415781404 40.22916824706451, -105.6688267008086 40.22894056836384, -105.6688429479812 40.22873624245703, -105.6688205696722 40.22852339716228, -105.6687613011443 40.22838176133099, -105.6686730393414 40.22821884274862, -105.6685174411165 40.22801933434805, -105.6683511792286 40.22783588408025, -105.6683375401028 40.22781896947912, -105.6682470624096 40.22761127111529, -105.6682416637716 40.22759486778096, -105.6682721112314 40.22737017614368, -105.6682739650483 40.22735817442233, -105.6683029921154 40.22722332576805, -105.6683058044111 40.2272130959819, -105.6683934966554 40.22704599071793, -105.6685196675831 40.22692074262096, -105.6687379630553 40.22675606758625, -105.6689083831121 40.22657508868081, -105.6690438599216 40.22640284891151, -105.6690758537972 40.22632072549793, -105.6690792556187 40.22631231949595, -105.6691903428408 40.22606427355334, -105.6692787329387 40.22583821434375, -105.6693278820078 40.22567399448331, -105.6693861052922 40.22544429847117, -105.669440759808 40.22514343033741, -105.66945233353 40.2249046090048, -105.6694532890332 40.22489151701731, -105.6694919852029 40.22466959399863, -105.6694915482502 40.22436290200361, -105.6693372707889 40.22410474212811, -105.6691337832986 40.22385606282835, -105.6689801460077 40.22368898447323, -105.6688367933033 40.22358134839062, -105.668820995009 40.22356996322452, -105.6686399339946 40.22346121020597, -105.66857070503 40.22342023718163, -105.6684063343704 40.22334358118142, -105.6683101888107 40.22329963458959, -105.6680685904649 40.22318068359311, -105.6678529537799 40.22304919374229, -105.6676002381706 40.22290378130718, -105.6674823272445 40.22284463958258, -105.6673437859818 40.22277593321919, -105.6672358734293 40.22272320634443, -105.6669856426672 40.22260732588539, -105.6667614982625 40.22246269083642, -105.6664857475077 40.222278601177, -105.6662919082906 40.22213095583463, -105.6661158510701 40.22201122023689, -105.6660285158423 40.22195229519745, -105.6659311617552 40.22189506412996, -105.6658563941644 40.22185175849506, -105.6656409412277 40.2217135933068, -105.6654520699702 40.22157582560256, -105.6653094536946 40.22148618217604, -105.6652393815789 40.22144276315675, -105.665179073635 40.2214088029338, -105.6650717714665 40.22134893480318, -105.6648732975747 40.22122908068761, -105.664797561422 40.22118791743397, -105.6646748951959 40.22112196728029, -105.6644591962295 40.22100981930868, -105.6642219518465 40.22087489948009, -105.6640011588874 40.22075494675638, -105.6639699494858 40.22073950563956, -105.6638033782239 40.22065749648416, -105.663644079153 40.22058103005954, -105.6635385751952 40.22048613622436, -105.6635385995102 40.22048598758672, -105.6635388206752 40.22048464173911, -105.6635459583738 40.22044129623704, -105.6635476333263 40.22043232723859, -105.663673564368 40.22034839813178, -105.6636823712486 40.22034252890084, -105.6636991629626 40.22034265464351, -105.6638131673268 40.22034350736083, -105.6638342814396 40.22034461134673, -105.66407395674 40.22035701730299, -105.6643249631576 40.22033462269664, -105.6643434378263 40.22033350759454, -105.6644807467734 40.22032595522565, -105.6644996202503 40.22032505838363, -105.664784009688 40.22031195569402, -105.6648041558022 40.22031213053535, -105.6650694737762 40.22031713167482, -105.665091824547 40.22032044650427, -105.665285107907 40.22035381967699, -105.6653082109339 40.22036160950015, -105.665453274059 40.22041584313852, -105.665476017825 40.22042613357929, -105.6656793835069 40.22052078736321, -105.666025019436 40.22065934213276, -105.6662109684469 40.22072644191363, -105.6665026809634 40.22079240572894, -105.6667602715467 40.22079269933909, -105.6670897912757 40.22075811984187, -105.6671100524527 40.2207586849872, -105.6675771648658 40.22078108328294, -105.6679161754167 40.22078667180477, -105.6679372613319 40.22078769222535, -105.6683273153827 40.22080907895852, -105.668349755364 40.22081223091617, -105.6686076023389 40.22085048682219, -105.6689434412469 40.22085470710499, -105.6689437513543 40.22085468143454, -105.6692620187301 40.22082685426683, -105.6692621514361 40.22082683155698, -105.6694877544554 40.22078559660721, -105.6697167316999 40.22070633274292, -105.670025529971 40.2205818739025, -105.6702602768931 40.22048289117972, -105.6704487179681 40.22038269732911, -105.6705318160145 40.22031142090378, -105.6706279297542 40.22020806563764, -105.6707634219981 40.22005296253833, -105.6709557580282 40.2198097498957, -105.6710802586927 40.2195102805907, -105.6711688587618 40.21926150827178, -105.6712223812788 40.21908071032284, -105.6712253346044 40.21907080716942, -105.6712666943526 40.21893789998065, -105.6712699602049 40.21892894021936, -105.6714498496281 40.21861495681172, -105.6715202551233 40.21847299480071, -105.671677961364 40.21823353650302, -105.6717915822289 40.21803192563492, -105.6718254444284 40.21785519677312, -105.6717553058992 40.21764151836187, -105.6717134573279 40.21753417629488, -105.6717077086626 40.21751735122088, -105.6716852102138 40.21736043335561, -105.6716834977097 40.21734524052872, -105.6716820255947 40.21698238032493, -105.6716342371114 40.21666497320453, -105.6716330510765 40.21665029385176, -105.6716974302847 40.21638855819683, -105.6716844886336 40.21617089596663, -105.6716031140915 40.21590230216545, -105.6715988975821 40.21588596024648, -105.6715868140986 40.21564834423229, -105.6715866363083 40.21563422447139, -105.671620006545 40.21537038231266, -105.6714720476905 40.21507356785254, -105.6713067369528 40.21484232290414, -105.6711008389497 40.21459721857093, -105.6708955791502 40.21438856038766, -105.6708818677844 40.2143719965027, -105.6707985907888 40.21404450838158, -105.6707963908123 40.21403062936756, -105.6710172976288 40.21375003597582, -105.6711798523966 40.21360484501722, -105.6713683785321 40.21343511289258, -105.6714650322431 40.21323580950317, -105.6715368673237 40.21305180125874, -105.6716108388324 40.21274444621527, -105.6716288543036 40.2124036293946, -105.6715814682046 40.21200177952105, -105.6714895341933 40.21156533862437, -105.671486455078 40.21154944621814, -105.6714344058856 40.21113793040745, -105.6714332596219 40.21112312849539, -105.6714547991578 40.21092602580006, -105.6714563055534 40.21091361022041, -105.6714980512335 40.21065270683239, -105.6715004847314 40.2106417939246, -105.6716179011028 40.21040545184155, -105.671664020672 40.21016743042685, -105.6716005492482 40.20992461097636, -105.6714341043355 40.20968414709365, -105.6714230068125 40.20966684897819, -105.6713526988938 40.20947998468864, -105.6712415442038 40.20922611109982, -105.6712343401312 40.20920897381667, -105.6711858342907 40.20906879448798, -105.671180227529 40.20905200698229, -105.6711120121573 40.20881812486911, -105.6711076268386 40.2088016985051, -105.6710679500579 40.20858059997141, -105.6710660945438 40.20856538390952, -105.6710951345212 40.20828515027478, -105.6710971069037 40.20827352295509, -105.6712490761915 40.20794918102887, -105.671252188425 40.20794333224706, -105.6714572507412 40.20776888574395, -105.671692983331 40.20760782260579, -105.671946837003 40.20746655576141, -105.6721096169302 40.20735484743265, -105.6723544287556 40.20722381706818, -105.6726600896722 40.20703938899105, -105.6728621527235 40.20688668559855, -105.6729976289071 40.20669015514054, -105.6730647160993 40.20644451025514, -105.6730678105499 40.20643499409206, -105.673206630464 40.20617431563913, -105.6733991767576 40.20599920259642, -105.6736513100163 40.20574410144964, -105.673799651054 40.20551870087024, -105.6739011514344 40.20534961296253, -105.6740954712419 40.20501136167052, -105.6742218988902 40.20476981641871, -105.674327059758 40.20462555292173, -105.6743913490012 40.20458955425074, -105.674406410934 40.20458814547064, -105.674457882481 40.20458362323701, -105.6744758279328 40.20458215786167, -105.6745819942282 40.20457132159748, -105.6747229798607 40.20452271252111, -105.6748448176996 40.20443287443803, -105.674994499918 40.20430770117226, -105.6751955721305 40.20415308938585, -105.6753971589113 40.20402163432263, -105.6756075566028 40.20390695053762, -105.6758225187993 40.20378210304028, -105.6760931932345 40.20362448291268, -105.6763292401676 40.20353687486897, -105.6763395737016 40.2035335024706, -105.6763396335542 40.2035334825655, -105.6766524176939 40.20343302824362, -105.6766648130916 40.20342984450046, -105.6769356120544 40.20336198784395, -105.6771745118465 40.20329083899474, -105.6774120088294 40.20319948890239, -105.6775459069634 40.20313382843321, -105.6778039324744 40.20302953190082, -105.6778152165018 40.20302631461814, -105.6780621159669 40.20295850286715, -105.6781938470535 40.20289104192163, -105.6782686189575 40.20277966302427, -105.6782330253896 40.20256177745768, -105.678146814832 40.20234917729157, -105.6780636463431 40.20218882324744, -105.6779048632146 40.20200063177179, -105.6778913430041 40.20198365230154, -105.6777848579481 40.20178683232973, -105.6777760633732 40.201769519553, -105.6776790023688 40.20151917503038, -105.6775820109331 40.20131543154896, -105.6774806636888 40.20113149318991, -105.677471925699 40.20111419741364, -105.6774135739281 40.20093048570482, -105.6774087103606 40.2009139179919, -105.6773746711299 40.20074969189098, -105.6773025737169 40.20067296439435, -105.6772870750698 40.20065833402217, -105.6772867405361 40.20065796437652, -105.6772855154855 40.20065661170868, -105.6772124247469 40.20057588058088, -105.6771303299135 40.20050091461442, -105.677110930098 40.20048379905398, -105.6769837093085 40.20036940590301, -105.6769828743263 40.20036854708027, -105.6769820711433 40.20036772153204, -105.6768967181972 40.20027993903021, -105.6768820765282 40.20026326826825, -105.6768159285832 40.20014339393698, -105.6768091210255 40.20012714709139, -105.6768556014762 40.19994812733729, -105.6768585909085 40.19993829059837, -105.67695172948 40.19973998451265, -105.676955236575 40.19973274799546, -105.6770774666019 40.19950071915762, -105.677191466394 40.19929860908254, -105.677309877271 40.19910291361013, -105.6774321865941 40.19887741471136, -105.6775502241474 40.19865534192194, -105.6776388836061 40.19850001203584, -105.6777664012934 40.19833084362219, -105.677859358288 40.19817902390867, -105.6779915239622 40.19802619180775, -105.6780673977488 40.19789303763628, -105.6780974597292 40.19781217787021, -105.678093610375 40.19765681352559, -105.6780492504934 40.19744129817882, -105.677985354926 40.19729188755628, -105.6779247261666 40.19718164024333, -105.6779174020624 40.19716501868773, -105.6779351602477 40.19701107739367, -105.6779372746921 40.1970000027021, -105.678004741952 40.19688982213197, -105.6780596499286 40.19671669514958, -105.678071926527 40.19656638369481, -105.6780735871556 40.19634390762809, -105.678074154487 40.19633047746711, -105.67810410177 40.19616573681866, -105.678122920101 40.19591730248069, -105.6781240986365 40.19590451082409, -105.6781697967753 40.19562028816761, -105.6781797409691 40.19534197737302, -105.6781803389271 40.19532859309427, -105.6781977556393 40.19513170030768, -105.6782070388807 40.19484594049832, -105.6782075650279 40.19483249508618, -105.6782244408778 40.19458256772621, -105.6782341424972 40.19434313834616, -105.6782347793217 40.19432980353974, -105.6782519002093 40.19410310032079, -105.6782529398048 40.19409019359268, -105.6782742489293 40.19386989909211, -105.6782875275536 40.19356417239761, -105.6782485732217 40.19336613348817, -105.6781494802977 40.19314990804275, -105.6781414339438 40.1931326985922, -105.6780370489998 40.19289911524799, -105.6780297956547 40.1928819919292, -105.6779584459529 40.19267161911222, -105.6779532208666 40.19265495198785, -105.6778824219966 40.19233396648192, -105.677879096605 40.19231799622053, -105.6778530901214 40.19216014855787, -105.6778259574849 40.19203372650452, -105.6778234235607 40.1920181666116, -105.6778331188409 40.19186483292374, -105.6778347578226 40.19185297810984, -105.6779274774696 40.19168121408297, -105.6780466278303 40.19153206643568, -105.6781600304808 40.19136463031327, -105.6781519689368 40.19109901984651, -105.6780483550102 40.19096721548783, -105.6780341644516 40.19095039284954, -105.6779374023908 40.19082985643251, -105.6779258125981 40.19081283344089, -105.6778831211533 40.19062535816793, -105.6778806803566 40.19060991791348, -105.6779063544293 40.19041914381376, -105.6779083317913 40.19040736953217, -105.677971367463 40.1901881086194, -105.6780090548469 40.18971784405401, -105.6779019323254 40.18925666184236, -105.677765546384 40.18893325343011, -105.6777584028516 40.18891617134472, -105.6776926608927 40.18874264792856, -105.6775924744353 40.18855230766899, -105.6774687696009 40.18834147264181, -105.6773329173417 40.18814377739658, -105.6773211596643 40.18812653754374, -105.6772256809055 40.18797639568763, -105.6770380712492 40.18774144196102, -105.6770246010461 40.1877244559753, -105.6768426188331 40.18747682323465, -105.6766742782837 40.18730812405553, -105.6765065596637 40.18717919733659, -105.6764839112511 40.18716219017327, -105.6764829605575 40.18716147652353, -105.6763959415487 40.18710202448237, -105.6763308014061 40.18705804967441, -105.6760992185649 40.18689566223739, -105.6759303858499 40.18679373368499, -105.6758363636698 40.18673768635443, -105.6755581622642 40.18657711774318, -105.6754319340273 40.18652047142681, -105.6753559905684 40.18648750826154, -105.6751336758973 40.18639575841871, -105.</t>
         </is>
       </c>
-      <c r="D21" t="n">
-        <v>28</v>
-      </c>
-      <c r="E21" t="n">
-        <v>28</v>
-      </c>
-      <c r="F21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Ward Private Home</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>Ward private home</t>
         </is>
       </c>
-      <c r="L21" t="n">
+      <c r="J21" t="n">
         <v>40.0733984409928</v>
       </c>
-      <c r="M21" t="n">
+      <c r="K21" t="n">
         <v>-105.506518983446</v>
       </c>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr">
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
         <is>
           <t>POINT (-105.506518983446 40.0733984409928)</t>
         </is>

</xml_diff>

<commit_message>
Update supersite changes 1-20-2024
</commit_message>
<xml_diff>
--- a/data/supersites_geom_2024.xlsx
+++ b/data/supersites_geom_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,55 +446,60 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Venue</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>address</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>organization</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>website</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>google_map_link</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>google_map_name</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>lat</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>lon</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>google_map_url</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>website_url</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>location_geom</t>
         </is>
@@ -514,49 +519,52 @@
           <t>POLYGON ((-105.3383475896821 40.25279579827692, -105.3382794314722 40.25524525249802, -105.3381412199228 40.25881617856658, -105.3381829609955 40.26243240924209, -105.3381828979697 40.26243567209774, -105.3478002549402 40.26237901406024, -105.3479202448766 40.26237941764173, -105.3480531934493 40.2623798651291, -105.3480609959063 40.26237989068174, -105.3483753054478 40.26238094047059, -105.3483831137831 40.26238096600925, -105.3502716880137 40.26238727182132, -105.3502795316186 40.26238729727766, -105.3574027486471 40.26241077828855, -105.3620853399815 40.26241822105709, -105.3620933905265 40.26241823335076, -105.3672010594676 40.26242613784095, -105.3672092063966 40.26242615889559, -105.3719103561596 40.26243791500907, -105.3719185889108 40.26243793582719, -105.3766294256697 40.26244652003982, -105.3766298418329 40.26244652138401, -105.3768931198172 40.26244699532722, -105.3769018181211 40.26244701088236, -105.3814089843745 40.26106398454443, -105.3814148842667 40.26106217584215, -105.3856822884296 40.25975451154127, -105.389306418282 40.25868505833365, -105.3893126034273 40.25868324139569, -105.3920579591849 40.25787665318066, -105.3920641982831 40.25787481993468, -105.3924852901653 40.25775109572469, -105.3924896028312 40.25774982805633, -105.392492463916 40.25774917956623, -105.3924926331846 40.25774918422654, -105.3925017878451 40.25774940437503, -105.3942308924439 40.25779098039329, -105.3942396415731 40.25779119102752, -105.3962976245635 40.25784063924261, -105.3963064113209 40.25784085065493, -105.3969000271832 40.25785510728947, -105.3969088233486 40.25785531866444, -105.4015359961488 40.25796628527932, -105.4015360784346 40.25796628624992, -105.404327806051 40.25801654858331, -105.4043367140068 40.25801670905149, -105.4059574231582 40.25804585556789, -105.4059663605099 40.2580460159345, -105.4107477294264 40.25813203184654, -105.4155198889819 40.25829770498576, -105.4155290636505 40.25829802329604, -105.4203330852328 40.25846415434641, -105.4251861794957 40.25840726140195, -105.4251953382348 40.25840715384359, -105.4294812217399 40.2583567394641, -105.4294904615783 40.25835663071469, -105.4295536757102 40.25835588566847, -105.4295629143729 40.25835577691257, -105.4298646896997 40.25835280079793, -105.4299225583033 40.25835581509605, -105.4299320479088 40.25835630897658, -105.4305133050051 40.25838657975033, -105.4305228051982 40.25838707448938, -105.4306757416342 40.25839503849969, -105.4306852441799 40.2583955341274, -105.4307426027005 40.25839852069145, -105.430752107599 40.25839901541449, -105.4308077781424 40.25840191357626, -105.4308172818664 40.25840240829324, -105.4322794064476 40.25847853230823, -105.4322889360531 40.25847902872076, -105.4323419078253 40.25848178857227, -105.4323514409584 40.25848228498171, -105.4324151589678 40.25848560045744, -105.4324246932774 40.2584860968615, -105.4345929559632 40.25859894893045, -105.4346025279193 40.25859944787823, -105.4369612784415 40.25872217258483, -105.4369708915756 40.25872267225978, -105.4393363255669 40.25884516486855, -105.4409258012767 40.25883700876198, -105.4409352809209 40.25883695956276, -105.4434546744453 40.25882398712621, -105.4434642011069 40.25882393864347, -105.4443764377183 40.25881922909699, -105.4443859820117 40.25881918054682, -105.4462974984619 40.25880928571338, -105.4463070780196 40.25880923612055, -105.4476086573605 40.25880271230612, -105.4522696778767 40.25889905814066, -105.4522794676884 40.2588992603134, -105.457320490272 40.25900313029224, -105.4620166225517 40.2590381363858, -105.4620265441448 40.25903821079019, -105.4638404081088 40.25905168042018, -105.4638503614461 40.25905175377748, -105.4671613666072 40.25907632231434, -105.4714882186452 40.25913474836782, -105.4714983353781 40.25913488415101, -105.4763999511735 40.25920087241619, -105.4764101572673 40.2592010095895, -105.4808091579479 40.25926021774424, -105.4808194451724 40.25926035544283, -105.4856590016976 40.25932525952785, -105.4900841554215 40.25936213161643, -105.4900945931585 40.25936221806891, -105.4914674244207 40.25937362026658, -105.4914778868478 40.25937370749673, -105.4949090741289 40.25940296772085, -105.4993103492368 40.25992138523038, -105.4993210915308 40.25992265066251, -105.5029085134606 40.26034512851926, -105.502931935669 40.26034788652174, -105.5041307628281 40.26048828783482, -105.5088612768845 40.26059839940055, -105.5088719511472 40.26059864715346, -105.5136047435574 40.26070861601637, -105.5136154296108 40.26070886513165, -105.5183519417781 40.26081923745897, -105.5183626384468 40.26081948703492, -105.5231001382505 40.26092971894171, -105.5246476950239 40.2609710938596, -105.525269431533 40.26098771039094, -105.5273444115898 40.26104314285998, -105.5273551400827 40.26104342942336, -105.5274352605084 40.26104556924201, -105.5274459878262 40.26104585489666, -105.5321867141913 40.2611723584543, -105.5321974533053 40.26117264456591, -105.5325643454667 40.2611824271107, -105.5325750857591 40.26118271228633, -105.5358139134438 40.2612686678133, -105.5374657135926 40.26131247066026, -105.5374700080801 40.26131258454924, -105.5374807589939 40.26131286926624, -105.5376060021513 40.26131618794863, -105.5376167542434 40.26131647535446, -105.5377707903809 40.26132060406002, -105.5377815436505 40.2613208923508, -105.5420407296155 40.26143500096256, -105.5420510583876 40.26143505394957, -105.5420123310872 40.26132699564431, -105.5419533310875 40.25691899504218, -105.5418693303538 40.25068399588682, -105.5417913293522 40.24484599488542, -105.5417703294095 40.24320999597101, -105.5418212665354 40.24069807142973, -105.5420429039838 40.2322667322377, -105.542057627296 40.22872637662191, -105.5420562713165 40.22872637531357, -105.5420822364319 40.22507980477056, -105.5420823229212 40.22506767874194, -105.5420808495041 40.22506765406047, -105.5419590751946 40.22506557191936, -105.5419484417806 40.22506555326001, -105.5405764553367 40.22506318763808, -105.5385255461858 40.22505961624928, -105.5374809703504 40.2250577834895, -105.5373800222655 40.2250576054056, -105.536760204845 40.22505651522585, -105.5364318357178 40.22505593462795, -105.5364251454815 40.22505592322528, -105.5360637775385 40.22505528352068, -105.5353538558136 40.22505402382836, -105.5344553890728 40.22505242161549, -105.5326910735317 40.22504859983672, -105.5326820404199 40.22504857987344, -105.5326825303639 40.22418840574673, -105.5326967674883 40.2233561262393, -105.5326849473221 40.2214446523428, -105.5326849358092 40.22144269979285, -105.5333207578963 40.22144445293673, -105.5338911592008 40.22144602273305, -105.5348769137664 40.22144872610919, -105.5360049453737 40.2214518136923, -105.5360297782496 40.21982080776719, -105.5364610049816 40.21977874858243, -105.536469145231 40.2197779543675, -105.5364659849748 40.21975632326548, -105.5364658151693 40.21975515971221, -105.5378566567431 40.21962890467403, -105.5379291219123 40.21962350240685, -105.5379809748795 40.21961963612427, -105.5398831425591 40.21944693342513, -105.5411373910101 40.21826779544625, -105.5422084115658 40.21794388539156, -105.5422524668593 40.21422603345813, -105.5422526119581 40.21421377049138, -105.5326985284376 40.21419413237972, -105.5326895026425 40.21419411331591, -105.5326894995797 40.21419262998702, -105.5326902668153 40.21217981128849, -105.5326905761208 40.21136213502758, -105.5326905760758 40.21136204136256, -105.5326909158406 40.21046358966055, -105.5404398525206 40.21053711938241, -105.5422860075863 40.21055412132916, -105.5422953313193 40.21055420708196, -105.5423441034594 40.20698849445215, -105.5423441045886 40.20698842150102, -105.5469038813974 40.20702247197197, -105.5471669256137 40.20702443013139, -105.5471762500321 40.20702449927905, -105.5471710649767 40.20342824622806, -105.5471617411033 40.203428251832, -105.5424019515685 40.20343087127191, -105.542401834668 40.20341858226157, -105.5423929265994 40.20341858732859, -105.5423024628827 40.19394992984792, -105.5422970925746 40.19338779750338, -105.542297092536 40.19338773536003, -105.5422833975938 40.19195401206859, -105.5422833975333 40.19195391480071, -105.5422758519701 40.1911640951709, -105.5422571009006 40.18920076026023, -105.5422569890588 40.18918897106952, -105.541762862168 40.1891617345586, -105.5375946466315 40.18889544853639, -105.5375677880135 40.18893092853408, -105.537254321171 40.18934499589563, -105.5372715249519 40.18934647278628, -105.5375223216064 40.1893679950532, -105.5375224677095 40.18937951494874, -105.5375433224156 40.1910399954814, -105.5375101454505 40.19106602720946, -105.5375025897888 40.19185229996346, -105.537495561658 40.19258391871914, -105.5349909777208 40.19246710871604, -105.5349371865247 40.19249180670148, -105.5348823209668 40.19251699672893, -105.5346356497051 40.19259680260618, -105.5343393829121 40.19281390637015, -105.5342271532779 40.19272517011618, -105.5342180715312 40.19271798939261, -105.5342183360385 40.19269518000148, -105.5342183473157 40.19269425235101, -105.5342193376537 40.19260852935302, -105.5342198678148 40.19256285923371, -105.5342200411473 40.19254790514945, -105.5341957862916 40.19255495433799, -105.5341047369489 40.19258913845898, -105.5340122329798 40.19262441809995, -105.5339501238616 40.19264610006633, -105.533890165039 40.19266779307718, -105.5338179414305 40.19269327228345, -105.5337565232855 40.19271606081569, -105.533684251341 40.19274374108799, -105.5336515583924 40.19275577849825, -105.5336459058447 40.19275785969391, -105.5336091149603 40.19277140683688, -105.5335304733625 40.19279520175227, -105.5334323856855 40.19282329373202, -105.5333357318797 40.19285139332066, -105.5332445784334 40.19289053114875, -105.5331549173888 40.1929269242624, -105.5330790606768 40.1929545853694, -105.5330083598834 40.19297567307023, -105.5329570730651 40.19299410915016, -105.5328935660998 40.19301413198865, -105.5328294254024 40.19303029578, -105.5328098787648 40.19303559882346, -105.5328006690869 40.1930380970772, -105.5328018956497 40.19294170518686, -105.5328019262174 40.19293933922767, -105.5328090737093 40.1923771568957, -105.5328092241853 40.19236530368316, -105.5327720701403 40.19236356970227, -105.5327628767569 40.19236313910528, -105.5327760272405 40.19144611821562, -105.5328026033848 40.18959315645375, -105.5328144473783 40.1887670954498, -105.5328252743849 40.18844763660821, -105.5328252778692 40.18844755645122, -105.5328963810823 40.18678931519381, -105.532976230018 40.18492700366666, -105.5330262556054 40.1837602446121, -105.5331269808046 40.18141083850799, -105.5332266806333 40.17753671869425, -105.5332269975165 40.17752442499798, -105.5331662580995 40.17752449827886, -105.5331568626344 40.17752450998029, -105.5331893193217 40.17646799626176, -105.5332742031089 40.1738843189681, -105.5332746068535 40.17387203604751, -105.5332652858553 40.17387203873018, -105.5258340931253 40.17387231809113, -105.5258247721261 40.17387231837259, -105.5238776530766 40.17387231186575, -105.5237857437776 40.17749800315436, -105.5237651645466 40.17831101269118, -105.5237510683669 40.17886786445666, -105.5237454789506 40.17908870192743, -105.5237413580885 40.17925150068127, -105.5237197330747 40.18010577977868, -105.5237041709683 40.18072051517435, -105.5236896753479 40.18129311342297, -105.523688178229 40.1812930930153, -105.523680357985 40.181292988343, -105.5224378823772 40.18127630972313, -105.5224377955276 40.18127643582816, -105.522435320304 40.18127999739902, -105.5222435741154 40.18127382730909, -105.5222435283211 40.18127382641728, -105.522236754261 40.18127360796668, -105.5208006874244 40.18122739465633, -105.5207705453987 40.18122672640443, -105.5138093385616 40.18107228813918, -105.5115988430433 40.18102320894966, -105.5066788071574 40.18091382279687, -105.5037971648563 40.18084965648772, -105.4988689323545 40.18060051532034, -105.4942254027887 40.18036558420872, -105.4942081234937 40.18036470973328, -105.4938523205461 40.18035299938223, -105.4938523169958 40.18035330559622, -105.4938123200268 40.18389599982997, -105.4938093397902 40.1838958852905, -105.493803003558 40.18389564358236, -105.4916169415424 40.18381225335324, -105.4913673103303 40.18380308278645, -105.4890342964373 40.18371735136233, -105.4887108236855 40.18370645233315, -105.4858596675139 40.18361035232417, -105.4843017355777 40.18355781209871, -105.4842927315417 40.18355750826427, -105.4842923359611 40.18291119120383, -105.4842919357208 40.18225457717938, -105.4842909836418 40.18069288673419, -105.484290852698 40.18047691385383, -105.4842905938626 40.18005209836011, -105.4842904845098 40.17987483273979, -105.4842904768209 40.17986236891954, -105.4821456944617 40.17990478346833, -105.4809104417855 40.17992919131213, -105.4809046495147 40.17992930563622, -105.479611783183 40.17995483837693, -105.4796026937846 40.17995501780022, -105.4796152483834 40.17796396985926, -105.4796240684069 40.17656529689094, -105.4796805373642 40.17330482726621, -105.4797733872597 40.16988566754004, -105.4797734359278 40.16988387259018, -105.4797873653326 40.16937091048318, -105.479787691759 40.16935887360058, -105.4752042504024 40.16923656802826, -105.4750210361202 40.17237698847438, -105.4750206722191 40.17238323337168, -105.4750032321987 40.1726821562563, -105.4749708600473 40.17323704782745, -105.4727391684574 40.17317988978623, -105.471439289043 40.1731465768118, -105.4711861857428 40.17314008889846, -105.470709432716 40.1731278654992, -105.470200732758 40.17311482223527, -105.4701498775658 40.17311351851009, -105.4701398981323 40.17311326375602, -105.470147089627 40.17302417969756, -105.4701471120568 40.17302390050776, -105.4703235422809 40.17083798352486, -105.4704014266738 40.1698729832864, -105.4704561694049 40.16919470380456, -105.4704672528061 40.1690710003927, -105.4705125686798 40.16856524699041, -105.4707617862852 40.16578366217297, -105.4707617910061 40.16578360363307, -105.4708146541582 40.16519354991458, -105.470815740543 40.16518143398583, -105.46628891067 40.16510477709761, -105.4661484313311 40.16510540791135, -105.4661390192035 40.16575318835307, -105.4661360291954 40.16575316856382, -105.4661360034201 40.16575542373876, -105.4661389863847 40.16575544352597, -105.4661041161459 40.16599498340007, -105.4659122147164 40.16731319895921, -105.4656564837945 40.16906980083949, -105.4654595827187 40.17042224296217, -105.4654156772836 40.17072380804591, -105.4653390047136 40.17125043193705, -105.4650859317025 40.17298856399155, -105.4650278923397 40.17298779802273, -105.465020799437 40.17303651100915, -105.4650205696819 40.17303809154707, -105.4639674508512 40.17302419196477, -105.4551151660433 40.17290698011092, -105.4548676764149 40.17289810889962, -105.4460938038541 40.17258326152695, -105.4460938893231 40.17258504211464, -105.4461030764639 40.17277599101477, -105.4464328855671 40.17963012402592, -105.4467706877612 40.18691469756227, -105.4467707570555 40.18691618453304, -105.4562018644992 40.18738200961488, -105.4654274239811 40.18748873382307, -105.4654337392727 40.18798117173748, -105.4660768702116 40.18800936007144, -105.4655238635754 40.19500728610073, -105.4649952892548 40.20169467125756, -105.4649758233132 40.20194092921771, -105.4474170601683 40.20137233213854, -105.4472734418836 40.20136766994612, -105.447226697916 40.22921312441949, -105.4391980447536 40.22936945487155, -105.4216202374492 40.22919080099819, -105.4200940059783 40.22911348585162, -105.4156150536366 40.22888699158656, -105.4156135450612 40.22912913839541, -105.415475085733 40.22912771340392, -105.4154249119026 40.22912767673616, -105.4154032237782 40.23260784691084, -105.4146656795209 40.23257685252141, -105.4110641024067 40.23242806717199, -105.4110586742406 40.23267442569232, -105.4109241110912 40.23266878334061, -105.4107917390044 40.23854881554955, -105.4106350047693 40.24360757533661, -105.4077967243588 40.24357879200166, -105.4078014258309 40.24362964482339, -105.4076809304183 40.24362842117775, -105.4061610915533 40.24361252845856, -105.4062353345834 40.2472014281798, -105.4061687067422 40.24720049697125, -105.3969333339457 40.24707105012143, -105.3966897457939 40.24346376519367, -105.3957980869377 40.24345499160201, -105.3920182790535 40.24341772408644, -105.3920307022783 40.24383753423813, -105.3920155279506 40.24341610220183, -105.3920154663501 40.24337721060778, -105.3772575504983 40.24783662782211, -105.3579966972145 40.24799691433613, -105.3385839153525 40.24791229438405, -105.3385811986579 40.24812077097913, -105.338448737321 40.25124619151066, -105.3384298201 40.25169256512352, -105.3384279523157 40.25173657136099, -105.3383900936446 40.25262978135259, -105.3383510062346 40.25260183093391, -105.3383475896821 40.25279579827692))</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Allenspark Fire Station</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>14861 CO-7, Allenspark, CO 80510</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
         <is>
           <t>http://www.allensparkfire.com/</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Allenspark Fire Protection</t>
         </is>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>40.19712777610975</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>-105.5279141785934</v>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>http://www.allensparkfire.com/</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>POINT (-105.5279141785934 40.19712777610975)</t>
         </is>
@@ -576,53 +584,56 @@
           <t>POLYGON ((-105.1462091902176 40.1287254615651, -105.1463811910671 40.1286814612758, -105.1465091905153 40.1286324608168, -105.1466521909948 40.12851646037345, -105.1467601907007 40.12837346040647, -105.1469681918037 40.12816546030267, -105.1471681902714 40.12801146050332, -105.1473611912454 40.12789646119431, -105.1474471915002 40.12785746102228, -105.1476831913874 40.12780346061299, -105.1478051914117 40.1277864601138, -105.1479051910319 40.12776446140642, -105.1480411907711 40.12775946117674, -105.148131047267 40.12775946111901, -105.1483701909708 40.12775946068273, -105.1484921909401 40.12776446038666, -105.1486281913429 40.12777546030672, -105.1488141912797 40.12775946127093, -105.1489711913174 40.12773246071522, -105.1490791919685 40.12769346043497, -105.1493501918869 40.12752346094415, -105.1498021911529 40.12714446046252, -105.1501191918396 40.1269784605735, -105.1503821911598 40.12695246089658, -105.1508891916811 40.12694046027134, -105.1513948839501 40.12694194872075, -105.1527758874465 40.12694600356159, -105.154300191837 40.12695046002028, -105.1548092204482 40.12693493214863, -105.1549821926101 40.12692646047514, -105.1550255475185 40.12692646026373, -105.1552101930545 40.12692646033931, -105.155437192927 40.12695445958236, -105.1555461931968 40.12695945989714, -105.1556001924722 40.12702245971152, -105.1555921921127 40.12707946011266, -105.15561919262 40.12719845979632, -105.1556931920723 40.12731245959085, -105.1557801926516 40.12740145928399, -105.1559481928024 40.12743746043777, -105.1563391925392 40.1276614597395, -105.1565141933392 40.12771445982453, -105.1565956562976 40.12772766228106, -105.1568041930755 40.12776145992218, -105.1571021940422 40.12773645947969, -105.1572911938164 40.12771146007818, -105.1574571934914 40.12767945991541, -105.1576939255081 40.12766480027194, -105.1578931932202 40.12765245913534, -105.1581221932529 40.12766346026724, -105.1583881937712 40.12771545958289, -105.1587271935286 40.12775946009889, -105.1590381943059 40.12775145938977, -105.1591931935459 40.12775345958096, -105.159295194393 40.12773946004652, -105.1593321942806 40.12776146020572, -105.1593099156614 40.12782736753463, -105.1593961945012 40.12792145999537, -105.1594101940028 40.12802046036595, -105.1593961948648 40.12808645966798, -105.1593311943713 40.12824045994564, -105.1593241941156 40.12833945963551, -105.1593311935832 40.1284274605238, -105.1594381937382 40.12879546005235, -105.1594881935436 40.12887746060884, -105.159567194188 40.1289214593066, -105.159667193892 40.12894945954594, -105.1598101948547 40.12896045970615, -105.1599321943844 40.1289494599988, -105.1601261845107 40.12889596708893, -105.1602477556501 40.1288630990707, -105.1603761943632 40.1288334601072, -105.1604831934606 40.12878445990846, -105.1620093210164 40.12797305594989, -105.1625441952281 40.1276864588521, -105.1627091942639 40.12764845894845, -105.1627731945469 40.12760446023837, -105.1628381942516 40.1275384598923, -105.1629311946616 40.12746646007216, -105.1633531947814 40.12731345908721, -105.1636321946816 40.12720345937235, -105.1644421950803 40.12692945902451, -105.1648051947436 40.12681345989837, -105.1653700089539 40.12664755526463, -105.1658119066372 40.12652845903283, -105.1665941954893 40.12633345884351, -105.1665751958297 40.1268584592293, -105.1665921947485 40.12690745915487, -105.166642195758 40.12696145922249, -105.1667081954379 40.12699345858284, -105.1667741949328 40.12700345879298, -105.1687057057889 40.12700441568506, -105.1687951961079 40.12700445884948, -105.1688701962396 40.1270274592329, -105.168898196283 40.12704245954604, -105.1689571957668 40.12709045909411, -105.1689921957212 40.12714645870656, -105.1690031954348 40.12720745836092, -105.1689281965424 40.13055845919673, -105.1689125986237 40.1306329048518, -105.1689124571838 40.13066294718519, -105.168948196977 40.1306634594016, -105.1763945382965 40.13068560471505, -105.1783901991411 40.13068445895293, -105.1784921990268 40.13071445866245, -105.1785511991025 40.13076045923802, -105.1785684592082 40.13078897836895, -105.1785641690483 40.13079204933064, -105.1785020389263 40.13084705429363, -105.1784840588681 40.13086786763377, -105.1784548908681 40.13091006260262, -105.178444049129 40.13093391475787, -105.1784339246554 40.13095694572148, -105.178427016947 40.13098108442205, -105.1784229738302 40.13100413231251, -105.1784189256439 40.1310280042764, -105.1784180942343 40.13105298307757, -105.1784131673081 40.13194404858856, -105.1783999480014 40.13330396605977, -105.1783991396833 40.1337020124477, -105.1784048791175 40.13377395099028, -105.1783991093832 40.13408688368758, -105.1783958547979 40.13492689429661, -105.1783961618531 40.13508913406532, -105.1783948972642 40.13528101768208, -105.1783940230415 40.13644990497878, -105.178390832764 40.13742799644631, -105.1783857569761 40.13792377194132, -105.1783856925215 40.13792375374909, -105.1783808185894 40.13938497043898, -105.178379409163 40.13975199673494, -105.1783763784656 40.14133788851696, -105.1783763779464 40.14133799839369, -105.1783713737261 40.14226699561438, -105.1783533903674 40.14336199241301, -105.1783493436875 40.14413299714823, -105.1783547608992 40.14414764583766, -105.178355161728 40.14414850346271, -105.1783513876863 40.14416088307052, -105.1783507230336 40.14416221146657, -105.1783483399981 40.14435999722787, -105.1783373495214 40.14522699350773, -105.178337307856 40.14535299840424, -105.1783402810778 40.14660499955411, -105.1783343699196 40.1478468345418, -105.1783342828933 40.1478649966097, -105.1783342685619 40.14786827670135, -105.1783322539086 40.14912099754154, -105.1783316896897 40.14922173345824, -105.1783252470594 40.15034799549664, -105.1783262111119 40.15130500003102, -105.1783232044195 40.15240999729076, -105.1783233146343 40.15242367651192, -105.1783301522852 40.15303800468062, -105.1783291792601 40.15375999780937, -105.1783012893748 40.15590656871396, -105.1783011802659 40.1559149983927, -105.1783005822134 40.15597644463524, -105.1782971626988 40.15633399335119, -105.1782960871354 40.15719749425114, -105.1782960854515 40.15719884340366, -105.1782960843966 40.15719956301125, -105.1782951121814 40.15799899804473, -105.178294217315 40.15818577184383, -105.1782870964684 40.15965399674796, -105.1782862950887 40.15989422276495, -105.1782860862953 40.15995699669625, -105.1782851194905 40.16030891223458, -105.1782850786808 40.16032399691657, -105.178284679339 40.16043600372073, -105.1782749234563 40.16315591889484, -105.178274033215 40.16340399540454, -105.1782655161564 40.1650051485672, -105.1782579902131 40.16641899487397, -105.1782538706628 40.16695343985297, -105.1735772011636 40.16694246349251, -105.1735112021403 40.16875746475598, -105.1735104074165 40.16876894654175, -105.1734888774345 40.16876895687698, -105.1734876717343 40.1687689579743, -105.1734854970979 40.16912908258862, -105.1734767013714 40.17058610997677, -105.1734766984293 40.17058819044085, -105.1734768239046 40.17088245964705, -105.1734768197971 40.17088453830642, -105.1733657812711 40.17083213172842, -105.1733576954174 40.17082828027013, -105.1729529231051 40.17063241614367, -105.1728205681745 40.1705683728318, -105.1728195198593 40.17056786550766, -105.1687255340658 40.16858670852341, -105.1687256438738 40.1685916425322, -105.1687231045455 40.16859477217606, -105.1677518350548 40.16979169341922, -105.1677465944088 40.16979815123889, -105.167035661948 40.17067421828263, -105.167026766362 40.17067109176306, -105.1670240178124 40.17067447924944, -105.1669332093008 40.17078637943621, -105.1669304607418 40.17078976692029, -105.1668896186171 40.17084009214113, -105.1668985520034 40.17084317464879, -105.1668943955052 40.17084829540469, -105.1668849048761 40.17085999075397, -105.1665201919034 40.17073175740313, -105.1665174951051 40.17073080935722, -105.1664129896231 40.17079382714124, -105.1650199693466 40.17032183177924, -105.1642709600386 40.17007883540592, -105.1642169582605 40.17006083511097, -105.1640679558686 40.16999983608142, -105.1638209526211 40.16989583642651, -105.1637179519749 40.16985083726004, -105.1635209475333 40.16973283788921, -105.1631259398792 40.16948983996239, -105.1622709235831 40.1688868436568, -105.161120902206 40.16807485153609, -105.1602088846895 40.16741385793949, -105.1599118790576 40.16721485751804, -105.1598118775726 40.1671618596847, -105.1596798760458 40.16712085952145, -105.1595208740774 40.16707385977891, -105.1593498721462 40.16705286010649, -105.1572978539927 40.16702986225165, -105.1562688454048 40.16703286263721, -105.1551078351645 40.16704986397507, -105.1546488300367 40.16705586518081, -105.1546488353165 40.16705898771062, -105.154647999395 40.16705899872255, -105.1546530002739 40.17018099915842, -105.1546569998319 40.17225799859407, -105.1546569996872 40.17249899848197, -105.1546589995688 40.17417299912417, -105.1546599342045 40.17417298750612, -105.1546620818144 40.17647724158829, -105.1546629131087 40.17736968103145, -105.1538534119111 40.17702152067658, -105.1538401553576 40.17416747340352, -105.1471472878128 40.17412208832916, -105.1308240275999 40.16707106507126, -105.1308251696132 40.16745401704761, -105.1308248690956 40.16770711920258, -105.1308339090772 40.16841512361963, -105.130829951995 40.16861687941822, -105.130829023898 40.16878789975995, -105.1308268264415 40.16899487857084, -105.130825096449 40.16911593337741, -105.130826950711 40.16923590355137, -105.1308328523583 40.16953294692157, -105.1308381211171 40.16968312372387, -105.1308380730325 40.1698239502182, -105.1308520529194 40.17054487184136, -105.130858089966 40.17094897815058, -105.1308571509205 40.17105603681589, -105.1308601753751 40.17135609075753, -105.1308610970434 40.17144997901022, -105.1308640602036 40.17169513068922, -105.1308731301453 40.17200206767621, -105.1308830569357 40.17234908671396, -105.1308980849702 40.1728770261307, -105.130890136097 40.17308892735598, -105.1308928515666 40.17318199632658, -105.1308981571233 40.1736550034996, -105.1308978484933 40.17384386824337, -105.1308928914898 40.17403189495574, -105.130896930049 40.17421089176275, -105.1308961355192 40.17475305743081, -105.1309030890619 40.17558211464502, -105.1309011192309 40.1758791343955, -105.1309108852502 40.17618991643079, -105.130907895079 40.17667497536176, -105.1309089894072 40.17686906099571, -105.1309088561322 40.17768491898182, -105.1309031473364 40.17900092566963, -105.1308910444444 40.1812969306925, -105.1308898627142 40.181442199769, -105.1309021056735 40.18314994122324, -105.1308979191687 40.1841851230857, -105.1309039419183 40.18465813085619, -105.1309051019469 40.18497190483541, -105.1309110183405 40.18513498587469, -105.1309118354979 40.18564393849361, -105.1309191252318 40.18634507253613, -105.1309188689071 40.186986063103, -105.1309220276749 40.18759110388334, -105.1309130611667 40.18812198620383, -105.1309169704838 40.1885889481708, -105.1288573477865 40.18857997484698, -105.1256918879809 40.18856611215961, -105.121360830748 40.18856299055086, -105.1194899230949 40.18855492662844, -105.1190850825382 40.1885568881324, -105.1186970917979 40.1885539619918, -105.1183019485997 40.18854991306068, -105.1179300587332 40.18854813537448, -105.1174969479037 40.18854890001953, -105.1172141737779 40.18854906207515, -105.1167671242837 40.18854593391976, -105.1158580022557 40.18853797614679, -105.1146671019506 40.18854389517986, -105.1145858430134 40.18854499691239, -105.1134489979368 40.18854998659783, -105.1133670179578 40.18855190824585, -105.1125820027335 40.18856108520247, -105.1125329666713 40.18856092088617, -105.1120540599835 40.18855794243968, -105.1120313601333 40.18760194311961, -105.112017894645 40.18707819066701, -105.112011570436 40.18673288206929, -105.1120085237062 40.186557607745, -105.1119319115066 40.18487960280919, -105.1119049061916 40.18402300359683, -105.1119118919206 40.18367686408679, -105.1119091664257 40.18315088404788, -105.1119081200098 40.18251894680662, -105.1118759946224 40.18181388411318, -105.1118629926047 40.18127002597253, -105.1115040224316 40.18126909494015, -105.1113569308159 40.18126805117004, -105.1112559916314 40.18126990755782, -105.1101640174649 40.18126520655875, -105.1089940736708 40.18126612354689, -105.1086240113595 40.18126487136174, -105.1084361110251 40.18126505829095, -105.1080911123929 40.18126196732355, -105.1072020949942 40.18126004898254, -105.106833109551 40.18125797063896, -105.106641973712 40.18126088969616, -105.1059451380013 40.18126098709274, -105.1052980584674 40.18125987759827, -105.1051319899099 40.18126013369076, -105.1047898365833 40.18126006333194, -105.1044011718303 40.18125708676741, -105.1036499481707 40.18125506224674, -105.1033940415842 40.18125610659184, -105.1027139937316 40.18126200709273, -105.1023829530066 40.18125894705506, -105.1023970324222 40.18093204823994, -105.102413175028 40.18019091209275, -105.1024151073728 40.17943188442915, -105.1024348285392 40.17795588288692, -105.1024359298053 40.17764513457093, -105.102446985836 40.17691688312216, -105.1024459726393 40.17647792955385, -105.1024538771325 40.17579907983215, -105.1024659300747 40.1745939986924, -105.1024928436826 40.1739690192746, -105.1024948495252 40.17393196664215, -105.1024508498185 40.17392907018132, -105.1023799809039 40.17393102219533, -105.101211927436 40.17392892050625, -105.1001161310761 40.17393199790583, -105.0998391512321 40.17393103942207, -105.0989699184054 40.17392802714794, -105.0981518434555 40.1739279313386, -105.0979528772734 40.17392696481058, -105.0977370735687 40.17392895919532, -105.0974990948966 40.17392895400177, -105.0964931512326 40.17392709427654, -105.0963270854283 40.17393008282001, -105.0957541527641 40.17392890476933, -105.0955101015059 40.1739269531794, -105.0950699350661 40.17392596063161, -105.0947811388498 40.17392604651604, -105.0933063695626 40.17394767675843, -105.0930905495083 40.1739629603663, -105.0930355022931 40.17396373747397, -105.093035412355 40.17395404356559, -105.093035999663 40.17395399970057, -105.0930759995535 40.17368299823816, -105.0931459999594 40.17231399916508, -105.0931330003842 40.17149199908522, -105.093151000261 40.17065999832266, -105.0931500001353 40.17054199825319, -105.0931479994263 40.17023599850143, -105.0931369991391 40.16900499892864, -105.0931339988095 40.16872599950739, -105.0931369998561 40.16781299868737, -105.0931289996238 40.16735399928291, -105.093122999789 40.1669069989264, -105.0931319995954 40.16601699884203, -105.0931289999454 40.16569099842605, -105.0931259993862 40.16516199880555, -105.0931569991541 40.16423199918421, -105.0931480029145 40.16392408767742, -105.0931479999207 40.16392399940396, -105.0931469291512 40.16390871444782, -105.0931039998199 40.16329599907725, -105.0931040000302 40.16325199822559, -105.0931050114934 40.1631399988786, -105.0931050119728 40.16313991872316, -105.0931070004038 40.1623779989626, -105.0931070011848 40.1623778683723, -105.0931070642517 40.16237164155648, -105.0931129997678 40.16178000016573, -105.0931149989175 40.16163199930823, -105.0931069993422 40.16131200006891, -105.0931069998108 40.1613119217147, -105.0930749990154 40.16110699945172, -105.0930749994591 40.16106100006206, -105.093074999123 40.16093800027746, -105.0930969990843 40.16066999982127, -105.0930949991611 40.1604880000312, -105.0931024819559 40.16045158549526, -105.0931099998072 40.16041499996014, -105.0931679955306 40.16027501197318, -105.0933151831979 40.16027514992445, -105.0941529994326 40.16027600012808, -105.0942474912358 40.16027599866759, -105.0943463028096 40.16027599968295, -105.0944589999225 40.16027599890212, -105.0946219991399 40.16027500002095, -105.0948714164467 40.16027221347903, -105.0951589994661 40.16026899899504, -105.095906860969 40.16024372245906, -105.0960168884854 40.16023999747829, -105.0960170000153 40.16023999516622, -105.0960982895062 40.16023918860394, -105.0967180002406 40.1602330001241, -105.0998739874729 40.16022399957189, -105.1010630001934 40.16022199906198, -105.1010699280626 40.16022203558438, -105.1010700959203 40.16022203616376, -105.101072318054 40.16022203122495, -105.1024143180025 40.16022903062637, -105.1025380465539 40.16023089182191, -105.1025414551247 40.16023094317227, -105.1037689994997 40.16021099846859, -105.1049759993214 40.16020199886749, -105.1051399994199 40.16020099938218, -105.1051399989076 40.16020108764328, -105.1051400004159 40.16025199911635, -105.1051410002289 40.16030099923575, -105.1051503173048 40.16030096622104, -105.1068299991866 40.16029499859334, -105.1073450001184 40.16022799895545, -105.1077819997477 40.16013699863746, -105.1082079998631 40.16001999929222, -105.108461998888 40.15992999885013, -105.1086199994601 40.15987499865997, -105.1090149994251 40.15970599910182, -105.1093910002993 40.15951199882478, -105.1097429994652 40.15929699888233, -105.1100720003185 40.15905999866217, -105.1103729990311 40.15880299892639, -105.1104429993529 40.15873099894289, -105.1106439998662 40.15852399914743, -105.113046069445 40.15615724048531, -105.1131817329908 40.15603004308861, -105.1131833166732 40.1560310309896, -105.1132350662543 40.15598003692975, -105.1171083166701 40.15216303071296, -105.1174373163797 40.15206603050657, -105.1176343172161 40.15199203009031, -105.1178293167799 40.15191002952171, -105.1180609815329 40.15179809088321, -105.1180673167806 40.15179502982453, -105.1181203168223 40.15176802990709, -105.1182913165957 40.15165502930292, -105.1183783160733 40.15159102880732, -105.1185163167286 40.15147502962919, -105.1186593166722 40.15133602907218, -105.1187093166785 40.15128002911514, -105.1191113168914 40.1508870293791, -105.1196193162772 40.15040603050766, -105.1198893170867 40.15014302898289, -105.1201383165571 40.14990102921602, -105.1208303159887 40.14919902937343, -105.1212533161005 40.14879703059298, -105.1214593168065 40.1485880297608, -105.1214633158546 40.14837802926677, -105.1214643159671 40.14822102985509, -105.1214713155419 40.14797502969255, -105.1219613160375 40.14750802952513, -105.1243203153778 40.14526002966053, -105.1247883151495 40.14478902902466, -105.1303313154118 40.13922902808567, -105.1303923142009 40.13916902875051, -105.1308769439179 40.13869433055886, -105.1308803144594 40.13869102876136, -105.1308803139455 40.13859202915448, -105.1308793142346 40.13849702881259, -105.1308863138307 40.13833002958336, -105.1308973153534 40.13793402935524, -105.1308973195819 40.13793389877544, -105.1309083153879 40.13760103000428, -105.1309613147293 40.13428302934808, -105.1309633151163 40.13416902954575, -105.1309663158803 40.13407590265542, -105.131264018241 40.13407590214059, -105.1351949880881 40.13406190558131, -105.1355969920545 40.13406290499365, -105.136218990986 40.13406390604963, -105.1383481339877 40.1340678960071, -105.1387142130814 40.13405542457127, -105.1387601569389 40.13397838399309, -105.1388641599894 40.13379438525001, -105.1394061770989 40.13283739637802, -105.1396172542842 40.13246945491051, -105.1399113154917 40.13199350715775, -105.1400313152862 40.13181050557099, -105.1402873438578 40.13141953294432, -105.1404134075242 40.13123259600766, -105.1404134914445 40.13123248008579, -105.1405674928146 40.13101869438201, -105.1409685953441 40.13051183984713, -105.1410715897065 40.13039683245281, -105.1412255205253 40.13022372772332, -105.1414536901801 40.12994403235987, -105.1416416731433 40.12976299450775, -105.1433827002903 40.12803805788978, -105.1443716376531 40.12710336772473, -105.1446938377278 40.12679883459163, -105.1447137065043 40.12678007314066, -105.1448846966432 40.12662004649052, -105.1451267445326 40.1263892194086, -105.1456327957312 40.12596286157071, -105.1456423360221 40.12643537867292, -105.1456487281823 40.12675200170747, -105.1456168014993 40.12884799589443, -105.1456167647361 40.12885442637872, -105.1456271903526 40.12885446106298, -105.1457651912196 40.12883446131615, -105.1459941909125 40.12876946043333, -105.1462091902176 40.1287254615651))</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Altona MS</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>4600 Clover Basin Dr, Longmont, CO 80503</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>https://ams.svvsd.org/</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Altona Middle School</t>
         </is>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>40.14448266991539</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>-105.1626179175455</v>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>https://ams.svvsd.org/</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>POINT (-105.1626179175455 40.14448266991539)</t>
         </is>
@@ -642,53 +653,56 @@
           <t>POLYGON ((-105.1295199780874 40.13072688132058, -105.129739962766 40.13072788110647, -105.1308018207651 40.13073588184478, -105.131019817435 40.13074388165322, -105.1310098430939 40.13155699817882, -105.1310003956401 40.13199844572109, -105.130988858237 40.13253599608295, -105.1309879188726 40.13259022536034, -105.1309708325789 40.13358999631841, -105.1309568622919 40.13407299670184, -105.1309663158803 40.13407590265542, -105.1309633151163 40.13416902954575, -105.1309613147293 40.13428302934808, -105.1309083153879 40.13760103000428, -105.1308973195819 40.13793389877544, -105.1308973153534 40.13793402935524, -105.1308863138307 40.13833002958336, -105.1308793142346 40.13849702881259, -105.1308803139455 40.13859202915448, -105.1308803144594 40.13869102876136, -105.1308769439179 40.13869433055886, -105.1303923142009 40.13916902875051, -105.1303313154118 40.13922902808567, -105.1247883151495 40.14478902902466, -105.1243203153778 40.14526002966053, -105.1219613160375 40.14750802952513, -105.1214713155419 40.14797502969255, -105.1214643159671 40.14822102985509, -105.1214633158546 40.14837802926677, -105.1214593168065 40.1485880297608, -105.1212533161005 40.14879703059298, -105.1208303159887 40.14919902937343, -105.1201383165571 40.14990102921602, -105.1198893170867 40.15014302898289, -105.1196193162772 40.15040603050766, -105.1191113168914 40.1508870293791, -105.1187093166785 40.15128002911514, -105.1186593166722 40.15133602907218, -105.1185163167286 40.15147502962919, -105.1183783160733 40.15159102880732, -105.1182913165957 40.15165502930292, -105.1181203168223 40.15176802990709, -105.1180673167806 40.15179502982453, -105.1180609815329 40.15179809088321, -105.1178293167799 40.15191002952171, -105.1176343172161 40.15199203009031, -105.1174373163797 40.15206603050657, -105.1171083166701 40.15216303071296, -105.1131833166732 40.1560310309896, -105.1131817329908 40.15603004308861, -105.1130460729817 40.15615723779523, -105.1106439998662 40.15852399914743, -105.1104429993529 40.15873099894289, -105.1103729990311 40.15880299892639, -105.1100720003185 40.15905999866217, -105.1097429994652 40.15929699888233, -105.1093910002993 40.15951199882478, -105.1090149994251 40.15970599910182, -105.1086199994601 40.15987499865997, -105.108461998888 40.15992999885013, -105.1082079998631 40.16001999929222, -105.1077819997477 40.16013699863746, -105.1073450001184 40.16022799895545, -105.1068299991866 40.16029499859334, -105.1051503173048 40.16030096622104, -105.1051410002289 40.16030099923575, -105.1051400004159 40.16025199911635, -105.1051399989076 40.16020108764328, -105.1051399994199 40.16020099938218, -105.1049759993214 40.16020199886749, -105.1037689994997 40.16021099846859, -105.1025414551247 40.16023094317227, -105.1025380465539 40.16023089182191, -105.1024143180025 40.16022903062637, -105.101072318054 40.16022203122495, -105.1010700959203 40.16022203616376, -105.1010699280626 40.16022203558438, -105.1010630001934 40.16022199906198, -105.0998739874729 40.16022399957189, -105.0967180002406 40.1602330001241, -105.0960982895062 40.16023918860394, -105.0960170000153 40.16023999516622, -105.0960168884854 40.16023999747829, -105.095906860969 40.16024372245906, -105.0951589994661 40.16026899899504, -105.0948714164467 40.16027221347903, -105.0946219991399 40.16027500002095, -105.0944589999225 40.16027599890212, -105.0943463028096 40.16027599968295, -105.0942474912358 40.16027599866759, -105.0941529994326 40.16027600012808, -105.0933151831979 40.16027514992445, -105.0931679955306 40.16027501197318, -105.0931099998072 40.16041499996014, -105.0931024819559 40.16045158549526, -105.0930949991611 40.1604880000312, -105.0930969990843 40.16066999982127, -105.093074999123 40.16093800027746, -105.0930749994591 40.16106100006206, -105.0930749990154 40.16110699945172, -105.0931069998108 40.1613119217147, -105.0931069993422 40.16131200006891, -105.0931149989175 40.16163199930823, -105.0931129997678 40.16178000016573, -105.0931070642517 40.16237164155648, -105.0931070011848 40.1623778683723, -105.0925199158311 40.16237689791628, -105.0917190936679 40.16238697525812, -105.0909838252546 40.16238410086513, -105.089468094328 40.16239711982808, -105.0886809584908 40.16239212456986, -105.0881623938254 40.1623954782369, -105.0881598089886 40.16280928973737, -105.0881648387267 40.16306998948579, -105.0881668740553 40.16350208512876, -105.0881650625537 40.16356494168014, -105.0881693626968 40.16382478228903, -105.0881761464068 40.16392102833853, -105.083609519032 40.16392308127849, -105.0829128177578 40.16392203457659, -105.0813998304982 40.16392203444205, -105.0807888352324 40.1639220337433, -105.0802848402826 40.16392203294821, -105.0795948459216 40.16388103180415, -105.0787978532788 40.16380003091128, -105.0775498655427 40.16357702807103, -105.0756918859996 40.16302902328239, -105.0744968993014 40.16262302002178, -105.0739259058449 40.16241901849396, -105.0730759142553 40.16213901527696, -105.0719189271613 40.16175401236442, -105.0705369421375 40.16129000865394, -105.0694629539653 40.16092000499503, -105.0694111630307 40.16090422372054, -105.0687409608614 40.16070000328342, -105.0678959694674 40.1604240008717, -105.067322977026 40.16013699897744, -105.066765552507 40.15964313063317, -105.0662970046367 40.1588843247345, -105.064919505624 40.15935175545492, -105.064296309749 40.15959008850385, -105.0634333444827 40.15986251985857, -105.062539016009 40.16009099355082, -105.0606010313516 40.16022699272562, -105.0580710513005 40.16025799056519, -105.0553377713311 40.16028796999728, -105.0553382965441 40.16019791122213, -105.0553387559006 40.1601157733564, -105.0553383718875 40.15647913976149, -105.0553382920939 40.15571473362403, -105.0553382659259 40.15546513428482, -105.0553379947871 40.15282923958088, -105.0553386499967 40.15257631307534, -105.055340783666 40.15175194196998, -105.0553462127781 40.14965381974552, -105.055348545721 40.14875222591935, -105.0553554845123 40.14607040548283, -105.0553568117257 40.14555727121959, -105.0553581629 40.14497257258469, -105.0553735349496 40.13831543018563, -105.0553734627153 40.13826344007112, -105.055393108424 40.1382658753683, -105.0570841697421 40.13820687462603, -105.0623920537045 40.13814787912667, -105.0630970281733 40.13814387787887, -105.0644970736709 40.13812287925889, -105.0646163718572 40.1381387740668, -105.0647026837377 40.13816640688852, -105.0647902892207 40.13821288423826, -105.0648822428967 40.13829711858007, -105.0649247890964 40.13837338792121, -105.0649496601588 40.13851303311695, -105.0649012584268 40.13969700518675, -105.0649223983107 40.13978009284535, -105.0649318121612 40.13979936609553, -105.064944699213 40.13982145163131, -105.0650172912994 40.139897965545, -105.0651172543858 40.13995483397098, -105.0652349113323 40.13998458559128, -105.0728341139191 40.13987189343821, -105.0737770801883 40.13984989482434, -105.0742440761428 40.13984499868648, -105.0742413915201 40.13481684621029, -105.0745131984398 40.13479486487819, -105.0762711360049 40.13472286783558, -105.077656234461 40.13468386293215, -105.0799831751011 40.13457186759719, -105.0831630652203 40.13445687173049, -105.0832755753651 40.13446682896835, -105.0846750309919 40.13445787330612, -105.0879403055598 40.13442385884984, -105.0887041365292 40.13437587163286, -105.0899250393446 40.13434187663415, -105.0905391301851 40.13433687298826, -105.0920430472559 40.13429687652557, -105.0927490541487 40.13428987731798, -105.0930212415033 40.13428686643668, -105.0932020045514 40.13427787787717, -105.0940880142722 40.13427987836944, -105.0944050049201 40.13427896522876, -105.0944350199997 40.134278878763, -105.094924071347 40.13427687757695, -105.0960260840791 40.13426087793793, -105.100395113552 40.13418487869186, -105.1024960005596 40.13413300172339, -105.1025130341002 40.13316287731691, -105.1025130798614 40.13316287747433, -105.1041803847008 40.13315484466681, -105.1044939964566 40.13312987928641, -105.1055759631424 40.13312799972009, -105.1055759857053 40.13312511863367, -105.1055770144187 40.13300287849541, -105.1085152097078 40.13299386796137, -105.1086315304633 40.13298881317525, -105.1087220040101 40.13297863883014, -105.1088964020049 40.13293936322003, -105.1089796055062 40.13291013523579, -105.1090587413161 40.13287489693305, -105.1091328252846 40.13283461228306, -105.1092018368701 40.13278836166751, -105.1092647735506 40.13273806278027, -105.1093205768746 40.13268270513078, -105.1093585944797 40.13263279385802, -105.1093701834689 40.13263246468068, -105.1096519310758 40.13263086368207, -105.1098582235746 40.1326323161728, -105.1103350195741 40.13263517546018, -105.110591834876 40.13263671418122, -105.1109074261621 40.13263860431368, -105.111021497991 40.13263928746463, -105.1115905511339 40.13264209640875, -105.1119701840193 40.13263846362696, -105.1119769681384 40.13240697386129, -105.1119826842302 40.13221195301501, -105.1119871837674 40.13205846401782, -105.1121931826917 40.1319974642461, -105.1122250359624 40.13198450641528, -105.1122248807698 40.13196726034626, -105.1123102126654 40.13194232418207, -105.1126460873139 40.13184417366759, -105.1130752163228 40.13171876581113, -105.1134884683498 40.13159766957149, -105.1138787565874 40.13160434794801, -105.1142691989206 40.13161076343259, -105.1146592764502 40.13161717097666, -105.1150500767831 40.13162358771766, -105.1152464520673 40.13162554514241, -105.1155191846595 40.13164146329787, -105.1167491843696 40.13166446387874, -105.1167582823744 40.13069277850736, -105.1190737172402 40.13069586675535, -105.1190789667365 40.13069587415787, -105.1190837455796 40.13069590702754, -105.1196690057948 40.13069987439082, -105.1214287020073 40.13069788718315, -105.1214388421045 40.13069787537972, -105.1214389852497 40.1306978758488, -105.125637981124 40.13071087844324, -105.1295199780874 40.13072688132058))</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>Burlington Elementary</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>1051 S Pratt Pkwy, Longmont, CO 80501</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>http://bes.svvsd.org/</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>Burlington Elementary School</t>
         </is>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>40.1466539913149</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>-105.108633248163</v>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>http://bes.svvsd.org/</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>POINT (-105.108633248163 40.1466539913149)</t>
         </is>
@@ -705,56 +719,59 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2583845261048 40.01916806167687, -105.2583845465005 40.01820405441318, -105.2583835533824 40.017841051784, -105.2583967697713 40.01738897110558, -105.258420544823 40.01462569237854, -105.2630299591908 40.01461696725389, -105.2630753109644 40.01461633090538, -105.2638765422727 40.01460508854388, -105.2646558644589 40.01461288522881, -105.2657616256185 40.01461332253763, -105.2662260626349 40.01461196195721, -105.2678219770818 40.01460804739548, -105.2689819637891 40.01460406242605, -105.270220141546 40.01459912551402, -105.2716550449331 40.01459291590101, -105.2725519067238 40.01458809993736, -105.2736219240902 40.0145838908234, -105.2746458800721 40.01458095527774, -105.2760611408061 40.01457602595389, -105.2764250735946 40.01453802385365, -105.2773539185385 40.01436001199994, -105.2775250367717 40.01432794849211, -105.278005899344 40.01423306829994, -105.2782030961592 40.01419611210767, -105.278663968713 40.01410393231048, -105.2786769521653 40.01410055096331, -105.2786822492777 40.01411631803115, -105.278851249496 40.01459531880194, -105.2788752505237 40.01466131864607, -105.2789422504309 40.01484831880367, -105.2790212496877 40.01506431947683, -105.279283131531 40.01582838979826, -105.2792882488983 40.01584331888502, -105.2793182480616 40.01593431868323, -105.2795172500427 40.01656331893992, -105.2796422519211 40.01688331794094, -105.2797922499383 40.0173063188877, -105.2800122511694 40.01792531871845, -105.280344103938 40.01889429097838, -105.2840818920156 40.01812191122571, -105.2839600121989 40.01782410420856, -105.2838869444426 40.01755905605179, -105.2837991589066 40.01709413112621, -105.2840110981352 40.01704713596685, -105.2841060700353 40.01702607643248, -105.2850088672696 40.01684712918449, -105.2852128642166 40.01680605680808, -105.2865308262578 40.01653288651573, -105.2866812529073 40.01650245354258, -105.2878670067061 40.0162528717229, -105.2885419939298 40.01611983770974, -105.2891551001181 40.01599098183944, -105.2904817987244 40.01572217487955, -105.2916482773999 40.01546871123976, -105.2924838834105 40.01529960385942, -105.2929311934506 40.01520907552712, -105.2932648974691 40.01514153813964, -105.2935522291935 40.01508380053187, -105.2940456558378 40.01498431869415, -105.2941799322994 40.01493717604964, -105.2942962425791 40.01484536492688, -105.2945651847544 40.01463397060598, -105.2948050566042 40.01443646962085, -105.2948669406371 40.01436130597801, -105.2949106525785 40.01428611088715, -105.2949149278989 40.01420590378106, -105.2949111667633 40.01415099338725, -105.2948850709373 40.01404306065437, -105.2948279437313 40.01392601395955, -105.2948950990359 40.01391405477982, -105.2951188286011 40.01383593998661, -105.2955889946644 40.01372696689724, -105.2959720191087 40.01362689650804, -105.2966129379867 40.013483906396, -105.2968701231647 40.01343988732408, -105.2972629400945 40.01340708693889, -105.297280077546 40.01340711706504, -105.2975649848486 40.01340487234885, -105.2978951689382 40.01342411927098, -105.2981560643021 40.0134531259425, -105.2984361789157 40.01350193131028, -105.2987091069599 40.01356691986554, -105.2989748438362 40.01364891574665, -105.2990971694855 40.01369387506902, -105.2994309509394 40.01382595114303, -105.2996880626172 40.01392796986438, -105.3000011606622 40.01405287069223, -105.300067868143 40.0140719279547, -105.300254092653 40.01412001668933, -105.3005359990144 40.01416799685423, -105.300684149682 40.01417292017293, -105.3008359183136 40.01416110284114, -105.3009841703811 40.01413088704314, -105.3010065439604 40.01412285491573, -105.3010146521981 40.01412034528163, -105.3010158302282 40.01400687156732, -105.3010182134563 40.01377743388108, -105.3012170449381 40.01365994277487, -105.3012511657355 40.01363978016212, -105.3012602122003 40.01363443507628, -105.3013157480595 40.01351102356379, -105.3013862127445 40.01335443432603, -105.3014422127245 40.01298943465143, -105.3014430498437 40.01295818709555, -105.3014855972748 40.01291567214673, -105.3016445781594 40.01279315270759, -105.301669611214 40.01277386057978, -105.3018438953327 40.01265106276252, -105.3018840442789 40.01258892735918, -105.3019098151939 40.01254904485556, -105.3019510380944 40.012454651744, -105.3020538088907 40.01231838041662, -105.3021905057177 40.01225039243434, -105.3023609783213 40.0122379765276, -105.3024963718175 40.01215354095651, -105.3025641030316 40.01212000680025, -105.3028339352925 40.01201999358893, -105.302871088117 40.01201209624642, -105.3030868287403 40.01197513103055, -105.3032639351221 40.01196500016254, -105.3034049259969 40.01197512435276, -105.3035260492263 40.01198695187986, -105.3036140681767 40.01199799158061, -105.3039102543303 40.01202602940209, -105.305557109506 40.01218191783366, -105.3057609542073 40.0121850065404, -105.3059319946257 40.01217403816238, -105.3061630807291 40.01213901500693, -105.3063570745538 40.01209102548007, -105.3065429044971 40.01202600142455, -105.3076141292119 40.01157813163452, -105.3077088271884 40.01154589495262, -105.3079238782443 40.01149903669649, -105.3080870674058 40.01148613185906, -105.308331942269 40.01149806925132, -105.3085360305202 40.01154095864429, -105.3087150704405 40.01160411941821, -105.3088508945874 40.01167407305289, -105.3089869755116 40.01177998905509, -105.3091108765658 40.01190098145004, -105.3091959108223 40.0120048916048, -105.3093011218043 40.01217087461801, -105.3095111066217 40.01265986544916, -105.3095949315841 40.01281400891951, -105.309699132441 40.01295912720237, -105.3098229913196 40.01309604135331, -105.3099480980261 40.01320694391978, -105.3102739955811 40.01344789402713, -105.3118234160897 40.01453544148655, -105.3120567925063 40.01470010708103, -105.312361933919 40.01489993781325, -105.3125289085233 40.0149733016851, -105.3127352332546 40.01504169007535, -105.3129480200329 40.0150804391507, -105.3130960043414 40.01509110681246, -105.3132370369799 40.01508886480606, -105.3133744223811 40.01507836676347, -105.3135317804734 40.01504298074446, -105.3136827254333 40.01498525341332, -105.3138217195852 40.01490369158279, -105.3139311537581 40.01480613317056, -105.3140840267508 40.01465100213418, -105.3141580699373 40.01454765470404, -105.314161100045 40.01453610243495, -105.3142523826783 40.01432569713389, -105.3144299782174 40.0138658864271, -105.3145150378233 40.01370213541934, -105.3146211428467 40.01354500553955, -105.3147468556418 40.01339806550179, -105.3152511428208 40.01293713504057, -105.3153959888806 40.01284293193758, -105.3155440900743 40.01275764490002, -105.3157016044707 40.01269236446624, -105.3158787245793 40.01264979891742, -105.3161049520235 40.01262999701227, -105.3162930090429 40.01263710205752, -105.3164618248755 40.012656038649, -105.3166248808208 40.01269308423035, -105.3170811216146 40.01283491108664, -105.3185478949735 40.0133129701069, -105.318734015863 40.01340412766929, -105.3188769358608 40.01349604118355, -105.3190030450923 40.01360000856643, -105.3190590450488 40.01365991406973, -105.319111985134 40.01371602570779, -105.3192538759621 40.01392707882941, -105.3194131462352 40.01418208192421, -105.3196241265045 40.01445912624737, -105.3197259873269 40.0145528964566, -105.3197746679137 40.01458662986119, -105.3198439456211 40.01463488779377, -105.3200051121442 40.01471392747337, -105.3201231738931 40.01475693671951, -105.3202769540203 40.01479396174955, -105.3205160984978 40.01481794203936, -105.3206771327974 40.01481187808569, -105.3207571317286 40.01480212051062, -105.3210079447452 40.01473305728056, -105.3215281528368 40.01458809318348, -105.3215913105161 40.01457452082933, -105.3216871073137 40.01455786734842, -105.3218510178522 40.0145441209512, -105.3219609779378 40.01454511395445, -105.3221377392204 40.01457308621488, -105.3221690399934 40.01457700548138, -105.3223699117416 40.01462810094041, -105.3225621678807 40.01469702558393, -105.3228649500641 40.01482486826393, -105.3233328044708 40.01505322987001, -105.323660104682 40.01519062698569, -105.3238888151895 40.01526805234592, -105.3241205694507 40.01532592516624, -105.3241648728118 40.01538111073737, -105.3242303884762 40.01548755042216, -105.3244247008065 40.01574628088172, -105.3245436788014 40.01591887528656, -105.3245492477389 40.0159269544882, -105.3246059212577 40.01602909790676, -105.3247017555202 40.01622526479302, -105.3247730382696 40.01643244347468, -105.3248041000856 40.01657168709549, -105.3248219629255 40.01670913457539, -105.3248553573099 40.01687431775166, -105.3249133701591 40.01707073862386, -105.3249952481318 40.0172958282551, -105.3250760460801 40.01745401497376, -105.3252098556754 40.0176254206745, -105.3253212573837 40.01774829766252, -105.3255659482411 40.01799501028366, -105.3257195021807 40.01817081069291, -105.3258066509846 40.01828485840267, -105.3258460155857 40.01835697437657, -105.3259681394613 40.01858573655364, -105.3260399610972 40.01874900580488, -105.3261540656113 40.01894792884458, -105.3262193760422 40.01910160164122, -105.3263929273057 40.0195099539127, -105.3264250268082 40.01966400709756, -105.3264778781707 40.01980107190855, -105.3265102510802 40.01985978085294, -105.3265528701127 40.01993707119846, -105.326870866398 40.0204130156731, -105.3269570457379 40.02050291279555, -105.3270988940789 40.02060497193763, -105.3274174830837 40.02081711266219, -105.3275899041758 40.02100756890201, -105.3276826272177 40.02115700281578, -105.3277198721696 40.02124929852239, -105.3277770989521 40.02139110936605, -105.3278828940231 40.021773946245, -105.3279280546751 40.02198896183513, -105.3279869488215 40.0221389376397, -105.3281110299227 40.02235105094308, -105.3281758228844 40.02243234016946, -105.3283149827645 40.02260693121875, -105.3284389778593 40.02271198198343, -105.3287591164508 40.02291395380421, -105.3288938247745 40.02301901997969, -105.3290120195943 40.02315892566909, -105.3290941141536 40.02331387534033, -105.3291661187661 40.02350587084195, -105.329187860145 40.02366402561023, -105.3291856108905 40.0237299462356, -105.3291851632656 40.02374308334997, -105.3292105083722 40.02393861410442, -105.3292580015209 40.02409411493859, -105.3293400314355 40.02426807343316, -105.3293850744826 40.02433971920112, -105.329517076826 40.0245221086009, -105.3296581319994 40.02466094949524, -105.3297101574987 40.0247041251023, -105.3298849343158 40.02478097424918, -105.330075850617 40.02482902161795, -105.3301448347398 40.02483905198635, -105.3303063677034 40.02486253821598, -105.3305089314445 40.02490174321267, -105.3307188932055 40.02497976589941, -105.3311201805862 40.02514192076426, -105.3313211016588 40.02521297880104, -105.3315614094424 40.02528981493634, -105.3316864080329 40.02530226875604, -105.3318593114162 40.02530661078252, -105.3320268883447 40.02527797201461, -105.3322212954186 40.02522737817259, -105.3323144391407 40.0251865241619, -105.3324583090925 40.02512342117116, -105.3326207608531 40.02505003162955, -105.3327166037238 40.02501949364788, -105.3328488509051 40.02500107885299, -105.3329530767121 40.0250179756226, -105.3330761532333 40.02506509655677, -105.3334181797729 40.02523387018027, -105.3336921200928 40.0253378996183, -105.3338808648359 40.02539134594898, -105.3341307947925 40.02544487907239, -105.3342930478431 40.0254532928835, -105.3344340886531 40.02543304437418, -105.3345139544222 40.02540861718986, -105.3346764107789 40.02533318028983, -105.3348588869171 40.02521323380916, -105.3349301769176 40.02516213123148, -105.334942439392 40.0251533413287, -105.3351340153575 40.02508456072082, -105.3352794641085 40.02507572510495, -105.3354306917962 40.02509896697647, -105.3355180506154 40.02513393951381, -105.3358146694223 40.02529351858141, -105.3360870116539 40.02543283740193, -105.3366797666057 40.02573373858232, -105.3368153907778 40.02580180617613, -105.3369393034369 40.0258639947272, -105.3370898293551 40.02596861159827, -105.337211444122 40.02608962972621, -105.3372945325549 40.02622374646779, -105.3373147386148 40.02627063395128, -105.337421175453 40.02647877096612, -105.3374981735376 40.026582085771, -105.3376050923685 40.02666898418729, -105.3377398955795 40.02674301993157, -105.3378653071847 40.02677945552124, -105.3379240857469 40.02679433669536, -105.3381088963428 40.02683907028913, -105.3381922987373 40.02687609862392, -105.3382659791816 40.02691977176665, -105.3383043922788 40.02695517610391, -105.3383708887366 40.02703599359061, -105.3383777622052 40.02713038225339, -105.338366843368 40.02723611127646, -105.3383566309992 40.0272642467565, -105.3382529574146 40.02752611738724, -105.338225780298 40.02763739410864, -105.3382170012274 40.02773192113717, -105.3382338601833 40.02783799351767, -105.3383062021897 40.02799593461113, -105.338404047229 40.02811187719205, -105.3384651416272 40.02816304037792, -105.3385772570687 40.02823389648423, -105.3387027374635 40.02828469390063, -105.3388570775456 40.02831510567995, -105.3390817408703 40.0283388001672, -105.339237772709 40.02837330724666, -105.3393408026778 40.02842274061585, -105.339427070937 40.0284871535725, -105.3395271463893 40.02860730522766, -105.3395743309235 40.02869523638033, -105.3395908092224 40.02880027047129, -105.3395907679906 40.02884567393286, -105.3395316310671 40.02907021534642, -105.3395313939624 40.0291709390978, -105.3395785284584 40.029280301116, -105.3396758483765 40.02938759113305, -105.3398070717007 40.02948011247911, -105.34001105511 40.02959898763005, -105.34015883881 40.02966944762828, -105.3403328781856 40.02971994667367, -105.3404849920475 40.02972509898724, -105.3406360896496 40.02970691478322, -105.3410469038371 40.02961451122763, -105.341183063898 40.02960005782608, -105.3413729948086 40.02962008481045, -105.3415028859989 40.02966089163202, -105.3416609109556 40.02973495466169, -105.3418081666057 40.02983288521217, -105.3419061589185 40.02992388512177, -105.3420809641687 40.03015389630465, -105.342137060486 40.03029507504125, -105.3421488596493 40.03044031811095, -105.3421403156747 40.03055896510004, -105.3421095060823 40.0306210722046, -105.3420716051278 40.03069511489726, -105.3419991759212 40.03077501854443, -105.341919419521 40.03083712699294, -105.3418300778567 40.03089928889136, -105.3415005965306 40.03112171569501, -105.3410174858492 40.03147037200236, -105.3408471369649 40.03159443563352, -105.340665615881 40.03172705505519, -105.3405288206844 40.03180830358372, -105.3403725243837 40.03188309433408, -105.3402050811774 40.03195572768927, -105.3399985277202 40.03206259515791, -105.3398923459022 40.03216531452311, -105.3398401151529 40.03228710789242, -105.339815900834 40.03266454513719, -105.3397910481914 40.03276958840173, -105.3397623867686 40.03289592220633, -105.3397648869638 40.0330180815536, -105.3398021263316 40.03310402182879, -105.3398648639367 40.03318323722127, -105.3399094257732 40.03320258646184, -105.3399874379754 40.03322412473215, -105.3400861009968 40.03322904669189, -105.3404129451709 40.03319600779776, -105.340606091903 40.03321988353994, -105.3407891693523 40.03327394200747, -105.3409739123984 40.03337906294917, -105.3411214760025 40.03350214896666, -105.3414135867008 40.03377043530846, -105.3416446218389 40.03392719713566, -105.3418169530248 40.03404894816423, -105.3419979269082 40.03425771521409, -105.3420729438595 40.03436925697198, -105.3421506900844 40.03450652043009, -105.3422027158252 40.03456991529723, -105.3422675171242 40.0346224063464, -105.3423343685873 40.03464821394812, -105.3424653436751 40.03467410999632, -105.3429150731083 40.03468705674727, -105.3431410697753 40.03471591391834, -105.3433656111949 40.03478463226877, -105.3435020608055 40.03485553907074, -105.3438695438839 40.03508748923305, -105.3440168467119 40.03514205613806, -105.3440255978391 40.03514317666856, -105.3441489464593 40.03515897953323, -105.3442811158003 40.03514598153194, -105.3445051287401 40.03510592924802, -105.3447008653332 40.03509301643103, -105.3448968898014 40.03511112379889, -105.3450871457833 40.0351531064796, -105.3453108748094 40.03523795776137, -105.3454389324795 40.03530511152007, -105.3455861725568 40.0354181365134, -105.3457001544155 40.0355508806632, -105.3457428449966 40.03562395961514, -105.3458831215092 40.03597388322648, -105.345896628054 40.03615305911401, -105.3458797746984 40.03628602631347, -105.3457491322696 40.03663309661266, -105.3457611032644 40.03670887964498, -105.3458098776353 40.03677702573989, -105.3458869092818 40.03682599243626, -105.3459829278598 40.03684890616413, -105.3461322249344 40.0368457054413, -105.3466198830052 40.03677206577161, -105.3467530710819 40.03678294877792, -105.3468751210049 40.03682401467811, -105.3469760397207 40.03689195387994, -105.3471355108481 40.03703348689576, -105.3472691705876 40.0371086708003, -105.3472744176314 40.03710968647263, -105.3474308076592 40.03714103151144, -105.3475785708468 40.03714336947589, -105.3481836375957 40.03712059375427, -105.348392981334 40.03713896938038, -105.3485029214573 40.03716601706564, -105.348603897788 40.03720897453926, -105.3486919822502 40.03726701348017, -105.3487650432671 40.0373360133605, -105.3488319497072 40.03744288818694, -105.3488511085128 40.03750001347461, -105.348856789205 40.03820800949617, -105.3487067298522 40.03821232955207, -105.3477914050935 40.03821638893005, -105.3474817926258 40.03821722291953, -105.3468614299469 40.03822512838605, -105.3450104181683 40.03829153532944, -105.3450179171597 40.03868015700185, -105.3460405482716 40.0386437539853, -105.3461031168401 40.03898908284479, -105.3453268746833 40.03901948006025, -105.3452802180325 40.03911018389644, -105.345271517239 40.03912433761808, -105.3452452833364 40.03915814157467, -105.3452130574343 40.03918918870853, -105.3451781010895 40.03921517142847, -105.3451448277192 40.03923480953083, -105.3451089087152 40.03925177274996, -105.3450576487383 40.03926988529709, -105.3450069768098 40.03928187960952, -105.344961760615 40.03928819273935, -105.3449089508063 40.03929064807553, -105.3448494533033 40.03928712489946, -105.3447950264157 40.03927776511058, -105.3447425347318 40.03926247803446, -105.3446092328436 40.03929490292018, -105.3445765512982 40.03930516501039, -105.344539877266 40.03932120387111, -105.3444846960346 40.03935795158987, -105.3444426165169 40.03940586426801, -105.344423128196 40.03944725428348, -105.3444160073502 40.03949552391189, -105.3444275517575 40.03955601888752, -105.3444731759986 40.03968833424123, -105.3444965572211 40.03975520013649, -105.3445205624492 40.03981616221999, -105.3445578084813 40.03989778498795, -105.3446376646379 40.04003968424905, -105.3447276531524 40.04016680845205, -105.344795157412 40.04024733253993, -105.3448549167217 40.04031071675156, -105.3448484541613 40.04055274004725, -105.3448541691076 40.0406499600528, -105.3448674149786 40.04072253855343, -105.3448882399842 40.04079357632659, -105.3449216829459 40.04087332410908, -105.3449704426995 40.04095811087339, -105.3446364322639 40.04102959990085, -105.3446007162516 40.04104340376086, -105.3445703711054 40.04106466860651, -105.3445493695219 40.04108914063158, -105.3445380231417 40.04111119661664, -105.3445343361066 40.04112275146215, -105.3445311011553 40.04114724832418, -105.3445392814093 40.04121096396332, -105.3419896303343 40.04121709476975, -105.3422755387781 40.04337513429397, -105.3465131388534 40.04343423722576, -105.3501117189857 40.04341854173573, -105.3509604583964 40.04341720319611, -105.351061685705 40.04341728708226, -105.3544519058515 40.04524596662837, -105.355091416096 40.04556889885021, -105.3559880623356 40.04583041298836, -105.3567595372542 40.04599519383382, -105.3579301381531 40.04606086270712, -105.3600970053326 40.04564174739976, -105.3606742433043 40.0468628855719, -105.3621557651074 40.04965424089358, -105.3639920692559 40.05282887853546, -105.3641080684391 40.05289587827868, -105.3797250233372 40.06069585746808, -105.3900870057658 40.06584284178945, -105.3912861257657 40.07092499987773, -105.3914749402041 40.07083101793872, -105.3920811145549 40.07050298994405, -105.3925910222121 40.07026600808574, -105.3937980289077 40.06981087854467, -105.3940840170989 40.06972192263695, -105.3946001680771 40.06959803960483, -105.3947989293112 40.06953590537677, -105.3948919023455 40.06948987079981, -105.394964868722 40.06944107368035, -105.395060070696 40.06933903984681, -105.3952621280964 40.06899113614033, -105.3955138612367 40.0686358647477, -105.3957139250865 40.06842109885081, -105.3959568633348 40.06820609746421, -105.3961321294408 40.06808409464642, -105.3965509251752 40.06782505281563, -105.3967590498075 40.06770994229892, -105.3970411697905 40.06757211203932, -105.3973890575354 40.06741704540752, -105.3979349933502 40.06719105257222, -105.3989681210101 40.0668320704148, -105.3993949116376 40.0667119298152, -105.4001279456997 40.06656295502956, -105.400853036919 40.06646804795456, -105.401574842874 40.0664209000962, -105.4031081030495 40.06634588138125, -105.4033760986539 40.06632908658128, -105.4036001268962 40.06632597936235, -105.4039354886404 40.06629270998662, -105.4039684530764 40.06628998415017, -105.4041299199174 40.06627663574243, -105.4042548603106 40.06623819278212, -105.4043540234276 40.06619888982722, -105.4044344048956 40.06614050729836, -105.4045148499365 40.06603666564356, -105.4047389400583 40.06573287074457, -105.4047829657393 40.06567608181868, -105.4049212700939 40.06553693910522, -105.4051253441126 40.06542981958253, -105.4053520055905 40.06532884620861, -105.4056105037759 40.06528097971057, -105.4058260373516 40.06528440260607, -105.4060288655031 40.0653072983951, -105.4061852130406 40.0653236615075, -105.4063458769007 40.0652750842445, -105.4065446697525 40.06515834714913, -105.406676242775 40.06503075664818, -105.4068038590952 40.06490576206056, -105.4069109925564 40.06477432561354, -105.4072568691801 40.06434998263192, -105.4075520798087 40.0638858471748, -105.4076144271041 40.06375352486941, -105.4076986539011 40.06358322723908, -105.4077424376704 40.06351872295893, -105.4078528920384 40.06344490160728, -105.407979736912 40.06339954278057, -105.4081488124669 40.06337694790046, -105.4081993022081 40.06354259319305, -105.4082583191018 40.06365304293325, -105.4083384376527 40.06378623987003, -105.4086252315054 40.0642215866695, -105.4087813728473 40.06439056211295, -105.4089458907069 40.06461799217212, -105.4091018907903 40.06489412393282, -105.4092368182365 40.06512802479963, -105.4093225643208 40.06526853688391, -105.409504095397 40.06548498442051, -105.4098262734777 40.06579167091841, -105.4100664892069 40.06598563197285, -105.4102657157319 40.06612999100079, -105.4104355939177 40.0662923524043, -105.4104999331161 40.06642759351949, -105.4105231868886 40.06658533416806, -105.4111090704269 40.0668027547869, -105.4113230710384 40.06683775452498, -105.4123600762381 40.06670774877939, -105.4126030773382 40.06671874798173, -105.4127710765582 40.06675374711786, -105.4135470770253 40.06717174623984, -105.4143210780151 40.06733974415099, -105.4147190788605 40.06742674212688, -105.4148260788204 40.06747274227973, -105.4149630792546 40.06748474171021, -105.4150690789331 40.06755474126348, -105.4153730784282 40.06789174239631, -105.4157380779817 40.06803174076535, -105.4159660790526 40.06803073976152, -105.417218086706 40.06765573284537, -105.4192990814895 40.06934373178217, -105.4204860820148 40.06988972973171, -105.4213540837626 40.07010972666475, -105.4217650863564 40.07012072544669, -105.4219790865552 40.07007372430561, -105.4224070903935 40.06972272033761, -105.4231560979392 40.06916171416628, -105.4234760999032 40.06905671176163, -105.4241311017381 40.06905570945187, -105.4263101075327 40.06940170123508, -105.4276811134631 40.06938769518695, -105.4296940698257 40.06907550496865, -105.429696726161 40.06942996754758, -105.429694386054 40.06959605113096, -105.4296933119867 40.06967240975321, -105.429641808105 40.06967550540362, -105.4292166920104 40.06972721171748, -105.4288950002293 40.06976633789137, -105.4286274367091 40.0698159315109, -105.428326045251 40.06989903627482, -105.4279288266033 40.07006320863681, -105.427767388902 40.07014234364784, -105.4274301435079 40.07031168907899, -105.427187862742 40.07041321736073, -105.4265850469876 40.07060213368924, -105.4264385616445 40.0706539625285, -105.4262836121072 40.07072092919811, -105.4261582347105 40.07078358879082, -105.4259539328541 40.0709165081871, -105.4258003383412 40.07103107048781, -105.4253944374446 40.07137217887671, -105.4252350299228 40.07147595325737, -105.4243155617368 40.07219115576593, -105.4231393098885 40.07308417705716, -105.4226100060591 40.07339089775018, -105.4222132276659 40.07363857455535, -105.4217252471861 40.07398674410683, -105.4215431642913 40.07408511303873, -105.4211965898197 40.07427234585262, -105.4210308105794 40.07434951045089, -105.4206584442087 40.07448493070384, -105.4202083996824 40.07461261810035, -105.4195352042127 40.07476456033439, -105.4191247017771 40.07482938094511, -105.4189980306713 40.07484611794027, -105.4186447055464 40.07487513225324, -105.4180009566014 40.07488857546316, -105.4177762251645 40.07488622163074, -105.4174610348563 40.0748779494316, -105.4172705764785 40.07488147149702, -105.4170810759536 40.07488206684572, -105.4170306009453 40.07488568808787, -105.4169286974435 40.07489512468741, -105.4167905896386 40.07491916695444, -105.4166333942057 40.07497684600628, -105.4162312907294 40.07517846289863, -105.4159997512771 40.07528949075067, -105.4156196132907 40.07543625610639, -105.4153350203652 40.07550396612029, -105.4151395682494 40.07551491221498, -105.4149634135315 40.07550234559449, -105.4148358409656 40.07547591583315, -105.4146111929816 40.07540552041137, -105.4143570994708 40.07527584758753, -105.4142381667132 40.07519455728776, -105.4139032823823 40.07494558003621, -105.4136444687195 40.07478517666688, -105.413329475767 40.07462253567618, -105.4130705753038 40.0745330917355, -105.4129058764918 40.07449931594424, -105.4127516241002 40.07448895733638, -105.4125773454127 40.07450053023379, -105.4124096976944 40.0745384436123, -105.4122829936822 40.0745807785052, -105.4116113120437 40.07483923530526, -105.4112998081208 40.07492678295778, -105.4111312145296 40.07495957269411, -105.4109493026843 40.07498064805032, -105.4104369611586 40.07499780879358, -105.4099465988038 40.07495572838605, -105.4096666239786 40.07496136200007, -105.4094075828542 40.07497944835027, -105.4087209130649 40.07504255224723, -105.4072133339139 40.07514450001526, -105.4064926228099 40.07519135351045, -105.4058410165122 40.0752136172959, -105.4054705638814 40.0752272141406, -105.40520487196 40.07523357995193, -105.4049353748692 40.07523628450529, -105.4047392325432 40.07521783433648, -105.4045848509388 40.0751897922855, -105.4041947147465 40.07508862949976, -105.403705422345 40.0749653223569, -105.4035454821902 40.07493738955924, -105.4033969451357 40.07492482835819, -105.4031503024901 40.07492901141337, -105.4028950470262 40.07496317992302, -105.4025169204411 40.07501553263012, -105.4023550157805 40.07502929541273, -105.4021645541007 40.07503425519602, -105.4019389002541 40.07501138551396, -105.40168661591 40.074965083188, -105.4015019436022 40.07491810670258, -105.40096224968 40.07475231378992, -105.4007728206619 40.07470313718637, -105.4006128875573 40.0746708105926, -105.4003900881106 40.07465013520603, -105.4001936699258 40.07464511287059, -105.3999920191408 40.0746658845997, -105.3997996016553 40.07470668529642, -105.3996328800538 40.07475774923518, -105.3994223224821 40.0748299894019, -105.3992936939425 40.07487962339136, -105.3991136328338 40.07493506377642, -105.3989345365082 40.07498245837664, -105.3987192795767 40.0750122629322, -105.3984012230241 40.07501125209868, -105.3982545679028 40.07501551265776, -105.3981326490511 40.07503442581616, -105.3980545259296 40.07505922901456, -105.3979649460374 40.07510377494535, -105.3978486566331 40.0751790217227, -105.3973899365647 40.07562852046983, -105.3972817002089 40.0757136836102, -105.397169427459 40.07578848025003, -105.3968792179321 40.0759179797459, -105.3959609054664 40.07622318892043, -105.3953231254621 40.07647233550051, -105.3947619214149 40.07666278952232, -105.3941305833764 40.07686297010658, -105.3939136913895 40.07697539101873, -105.3934575621836 40.07722224613386, -105.3931865114511 40.07731992618486, -105.3929282780375 40.07737354901404, -105.3926318413482 40.07740020380218, -105.3923466903028 40.0774207953173, -105.3919433258007 40.07747300969441, -105.3915512466445 40.07751915932716, -105.3910859383422 40.07751872123406, -105.390588819259 40.07748152648809, -105.3899547533051 40.07738544205882, -105.3895851208953 40.07734591650613, -105.3890560983312 40.07733071977488, -105.3886608422517 40.07736951179238, -105.3882208880001 40.07745722445686, -105.3878287902893 40.07751315322446, -105.3875386890442 40.07756183623066, -105.3871751517061 40.07769123986255, -105.386958188724 40.07783792342001, -105.3868401010417 40.07793818621354, -105.3866996581514 40.07806535888105, -105.386575220841 40.07815092657836, -105.3864348761523 40.07821933925117, -105.3862435609229 40.07827301294386, -105.3861064964615 40.0782851193332, -105.3859439556369 40.07828495884738, -105.3854915187126 40.07820861461854, -105.3852495670619 40.07817436606354, -105.3849689629014 40.07813464671029, -105.384647065656 40.07813677433686, -105.3843346505428 40.07818542609105, -105.3841911614831 40.07822690365325, -105.3838658088119 40.07838571414805, -105.3835116873142 40.07859345906748, -105.3832533311892 40.07871071489546, -105.3828706781617 40.07882784409028, -105.3824975639514 40.07895722236837, -105.3821530389425 40.07914049159699, -105.3818913601033 40.079333636382, -105.3816040092101 40.07962713452685, -105.381316880753 40.07979087291746, -105.3809245713487 40.07995695099259, -105.3802294146402 40.08015943763821, -105.379588467187 40.08034483921757, -105.3792504093654 40.08046689970899, -105.3786411661966 40.08074291496696, -105.3780797871333 40.08098470179396, -105.3777130575363 40.08109693300169, -105.3774866867055 40.08114076234569, -105.3770053036764 40.08120390520853, -105.3766993091122 40.08121582032145, -105.3761925603991 40.08120548435789, -105.3760268068356 40.08121510006245, -105.3757111712446 40.08127107066737, -105.3751786731141 40.08139780561959, -105.3744967961343 40.08157402736211, -105.3735477428702 40.0818006048877, -105.3730416668277 40.08192675278983, -105.3726786466126 40.08199815224141, -105.3724146658471 40.08203164841389, -105.3720517316847 40.08205658721963, -105.3715667481044 40.08210790769671, -105.3712911926056 40.08211536164035, -105.3710047166085 40.08208494329329, -105.3706571489542 40.0819848523058, -105.3701603136584 40.08182251295334, -105.3693330902472 40.08154316557858, -105.3691740018331 40.08149407507, -105.3689732329173 40.08146939130329, -105.3687454792302 40.08146913257269, -105.3682581015067 40.08148550858736, -105.3674792688943 40.08151471573545, -105.3669855945874 40.08156515588454, -105.3666338417142 40.08163741303427, -105.3665354783196 40.08168099405719, -105.3664748780766 40.08172531938194, -105.3664584034446 40.08159014621046, -105.3664654543084 40.08151024750345, -105.3665410705586 40.0813216177777, -105.3666249026477 40.08104341501357, -105.3665924458401 40.08081366575016, -105.3664632649919 40.08064976953737, -105.3662886091598 40.08052481296188, -105.3660390097108 40.08039337010403, -105.3659304079325 40.08034970692742, -105.3658929678842 40.08033465331701, -105.3657461992619 40.08003983094896, -105.3657423068642 40.08003200973842, -105.3656923072547 40.07998801008782, -105.365564750368 40.07986337558394, -105.3655613064671 40.07986000947152, -105.36547830664 40.07972600962538, -105.3654660928458 40.0796893671258, -105.3654633071831 40.0796810104118, -105.365430306542 40.07966001037191, -105.365182305831 40.0795810101703, -105.3650123076826 40.07954700945725, -105.3646413071265 40.07954001023455, -105.3646409597663 40.07954016834047, -105.3644273067806 40.07963700967829, -105.3641503065364 40.07968800899322, -105.3640113064601 40.07968900896079, -105.3640110721188 40.07968893393132, -105.3638723068514 40.07964401110103, -105.3637572863339 40.079587932841, -105.3637380311503 40.07957854522331, -105.3652410674733 40.07915339564261, -105.3652857427266 40.07914075772138, -105.3650620067686 40.07914218420888, -105.364451609022 40.07932611178899, -105.3644452352826 40.0793280334828, -105.3644119629354 40.07914632201314, -105.3643715348942 40.07889535434658, -105.3643097355887 40.07858571793681, -105.3642741451352 40.07840741532311, -105.3642283755162 40.07817809457496, -105.3642159208946 40.0781157013513, -105.3641896030986 40.07800118147891, -105.3641331627319 40.07770186991803, -105.364130402719 40.07768724201821, -105.3639345284794 40.07776073618592, -105.3638318920551 40.07763710989789, -105.3637768699827 40.07764845253151, -105.3628899389825 40.07783129497066, -105.3627564852363 40.07785880595277, -105.362</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+          <t>POLYGON ((-105.2716550449331 40.01459291590101, -105.2725519067238 40.01458809993736, -105.2736219240902 40.0145838908234, -105.2746458800721 40.01458095527774, -105.2760611408061 40.01457602595389, -105.2764250735946 40.01453802385365, -105.2773539185385 40.01436001199994, -105.2775250367717 40.01432794849211, -105.278005899344 40.01423306829994, -105.2782030961592 40.01419611210767, -105.278663968713 40.01410393231048, -105.2786769521653 40.01410055096331, -105.2786822492777 40.01411631803115, -105.278851249496 40.01459531880194, -105.2788752505237 40.01466131864607, -105.2789422504309 40.01484831880367, -105.2790212496877 40.01506431947683, -105.279283131531 40.01582838979826, -105.2792882488983 40.01584331888502, -105.2793182480616 40.01593431868323, -105.2795172500427 40.01656331893992, -105.2796422519211 40.01688331794094, -105.2797922499383 40.0173063188877, -105.2800122511694 40.01792531871845, -105.280344103938 40.01889429097838, -105.2840818920156 40.01812191122571, -105.2839600121989 40.01782410420856, -105.2838869444426 40.01755905605179, -105.2837991589066 40.01709413112621, -105.2840110981352 40.01704713596685, -105.2841060700353 40.01702607643248, -105.2850088672696 40.01684712918449, -105.2852128642166 40.01680605680808, -105.2865308262578 40.01653288651573, -105.2866812529073 40.01650245354258, -105.2878670067061 40.0162528717229, -105.2885419939298 40.01611983770974, -105.2891551001181 40.01599098183944, -105.2904817987244 40.01572217487955, -105.2916482773999 40.01546871123976, -105.2924838834105 40.01529960385942, -105.2929311934506 40.01520907552712, -105.2932648974691 40.01514153813964, -105.2935522291935 40.01508380053187, -105.2940456558378 40.01498431869415, -105.2941799322994 40.01493717604964, -105.2942962425791 40.01484536492688, -105.2945651847544 40.01463397060598, -105.2948050566042 40.01443646962085, -105.2948669406371 40.01436130597801, -105.2949106525785 40.01428611088715, -105.2949149278989 40.01420590378106, -105.2949111667633 40.01415099338725, -105.2948850709373 40.01404306065437, -105.2948279437313 40.01392601395955, -105.2948950990359 40.01391405477982, -105.2951188286011 40.01383593998661, -105.2955889946644 40.01372696689724, -105.2959720191087 40.01362689650804, -105.2966129379867 40.013483906396, -105.2968701231647 40.01343988732408, -105.2972629400945 40.01340708693889, -105.297280077546 40.01340711706504, -105.2975649848486 40.01340487234885, -105.2978951689382 40.01342411927098, -105.2981560643021 40.0134531259425, -105.2984361789157 40.01350193131028, -105.2987091069599 40.01356691986554, -105.2989748438362 40.01364891574665, -105.2990971694855 40.01369387506902, -105.2994309509394 40.01382595114303, -105.2996880626172 40.01392796986438, -105.3000011606622 40.01405287069223, -105.300067868143 40.0140719279547, -105.300254092653 40.01412001668933, -105.3005359990144 40.01416799685423, -105.300684149682 40.01417292017293, -105.3008359183136 40.01416110284114, -105.3009841703811 40.01413088704314, -105.3010065439604 40.01412285491573, -105.3010146521981 40.01412034528163, -105.3010158302282 40.01400687156732, -105.3010182134563 40.01377743388108, -105.3012170449381 40.01365994277487, -105.3012511657355 40.01363978016212, -105.3012602122003 40.01363443507628, -105.3013157480595 40.01351102356379, -105.3013862127445 40.01335443432603, -105.3014422127245 40.01298943465143, -105.3014430498437 40.01295818709555, -105.3014855972748 40.01291567214673, -105.3016445781594 40.01279315270759, -105.301669611214 40.01277386057978, -105.3018438953327 40.01265106276252, -105.3018840442789 40.01258892735918, -105.3019098151939 40.01254904485556, -105.3019510380944 40.012454651744, -105.3020538088907 40.01231838041662, -105.3021905057177 40.01225039243434, -105.3023609783213 40.0122379765276, -105.3024963718175 40.01215354095651, -105.3025641030316 40.01212000680025, -105.3028339352925 40.01201999358893, -105.302871088117 40.01201209624642, -105.3030868287403 40.01197513103055, -105.3032639351221 40.01196500016254, -105.3034049259969 40.01197512435276, -105.3035260492263 40.01198695187986, -105.3036140681767 40.01199799158061, -105.3039102543303 40.01202602940209, -105.305557109506 40.01218191783366, -105.3057609542073 40.0121850065404, -105.3059319946257 40.01217403816238, -105.3061630807291 40.01213901500693, -105.3063570745538 40.01209102548007, -105.3065429044971 40.01202600142455, -105.3076141292119 40.01157813163452, -105.3077088271884 40.01154589495262, -105.3079238782443 40.01149903669649, -105.3080870674058 40.01148613185906, -105.308331942269 40.01149806925132, -105.3085360305202 40.01154095864429, -105.3087150704405 40.01160411941821, -105.3088508945874 40.01167407305289, -105.3089869755116 40.01177998905509, -105.3091108765658 40.01190098145004, -105.3091959108223 40.0120048916048, -105.3093011218043 40.01217087461801, -105.3095111066217 40.01265986544916, -105.3095949315841 40.01281400891951, -105.309699132441 40.01295912720237, -105.3098229913196 40.01309604135331, -105.3099480980261 40.01320694391978, -105.3102739955811 40.01344789402713, -105.3118234160897 40.01453544148655, -105.3120567925063 40.01470010708103, -105.312361933919 40.01489993781325, -105.3125289085233 40.0149733016851, -105.3127352332546 40.01504169007535, -105.3129480200329 40.0150804391507, -105.3130960043414 40.01509110681246, -105.3132370369799 40.01508886480606, -105.3133744223811 40.01507836676347, -105.3135317804734 40.01504298074446, -105.3136827254333 40.01498525341332, -105.3138217195852 40.01490369158279, -105.3139311537581 40.01480613317056, -105.3140840267508 40.01465100213418, -105.3141580699373 40.01454765470404, -105.314161100045 40.01453610243495, -105.3142523826783 40.01432569713389, -105.3144299782174 40.0138658864271, -105.3145150378233 40.01370213541934, -105.3146211428467 40.01354500553955, -105.3147468556418 40.01339806550179, -105.3152511428208 40.01293713504057, -105.3153959888806 40.01284293193758, -105.3155440900743 40.01275764490002, -105.3157016044707 40.01269236446624, -105.3158787245793 40.01264979891742, -105.3161049520235 40.01262999701227, -105.3162930090429 40.01263710205752, -105.3164618248755 40.012656038649, -105.3166248808208 40.01269308423035, -105.3170811216146 40.01283491108664, -105.3185478949735 40.0133129701069, -105.318734015863 40.01340412766929, -105.3188769358608 40.01349604118355, -105.3190030450923 40.01360000856643, -105.3190590450488 40.01365991406973, -105.319111985134 40.01371602570779, -105.3192538759621 40.01392707882941, -105.3194131462352 40.01418208192421, -105.3196241265045 40.01445912624737, -105.3197259873269 40.0145528964566, -105.3197746679137 40.01458662986119, -105.3198439456211 40.01463488779377, -105.3200051121442 40.01471392747337, -105.3201231738931 40.01475693671951, -105.3202769540203 40.01479396174955, -105.3205160984978 40.01481794203936, -105.3206771327974 40.01481187808569, -105.3207571317286 40.01480212051062, -105.3210079447452 40.01473305728056, -105.3215281528368 40.01458809318348, -105.3215913105161 40.01457452082933, -105.3216871073137 40.01455786734842, -105.3218510178522 40.0145441209512, -105.3219609779378 40.01454511395445, -105.3221377392204 40.01457308621488, -105.3221690399934 40.01457700548138, -105.3223699117416 40.01462810094041, -105.3225621678807 40.01469702558393, -105.3228649500641 40.01482486826393, -105.3233328044708 40.01505322987001, -105.323660104682 40.01519062698569, -105.3238888151895 40.01526805234592, -105.3241205694507 40.01532592516624, -105.3241648728118 40.01538111073737, -105.3242303884762 40.01548755042216, -105.3244247008065 40.01574628088172, -105.3245436788014 40.01591887528656, -105.3245492477389 40.0159269544882, -105.3246059212577 40.01602909790676, -105.3247017555202 40.01622526479302, -105.3247730382696 40.01643244347468, -105.3248041000856 40.01657168709549, -105.3248219629255 40.01670913457539, -105.3248553573099 40.01687431775166, -105.3249133701591 40.01707073862386, -105.3249952481318 40.0172958282551, -105.3250760460801 40.01745401497376, -105.3252098556754 40.0176254206745, -105.3253212573837 40.01774829766252, -105.3255659482411 40.01799501028366, -105.3257195021807 40.01817081069291, -105.3258066509846 40.01828485840267, -105.3258460155857 40.01835697437657, -105.3259681394613 40.01858573655364, -105.3260399610972 40.01874900580488, -105.3261540656113 40.01894792884458, -105.3262193760422 40.01910160164122, -105.3263929273057 40.0195099539127, -105.3264250268082 40.01966400709756, -105.3264778781707 40.01980107190855, -105.3265102510802 40.01985978085294, -105.3265528701127 40.01993707119846, -105.326870866398 40.0204130156731, -105.3269570457379 40.02050291279555, -105.3270988940789 40.02060497193763, -105.3274174830837 40.02081711266219, -105.3275899041758 40.02100756890201, -105.3276826272177 40.02115700281578, -105.3277198721696 40.02124929852239, -105.3277770989521 40.02139110936605, -105.3278828940231 40.021773946245, -105.3279280546751 40.02198896183513, -105.3279869488215 40.0221389376397, -105.3281110299227 40.02235105094308, -105.3281758228844 40.02243234016946, -105.3283149827645 40.02260693121875, -105.3284389778593 40.02271198198343, -105.3287591164508 40.02291395380421, -105.3288938247745 40.02301901997969, -105.3290120195943 40.02315892566909, -105.3290941141536 40.02331387534033, -105.3291661187661 40.02350587084195, -105.329187860145 40.02366402561023, -105.3291856108905 40.0237299462356, -105.3291851632656 40.02374308334997, -105.3292105083722 40.02393861410442, -105.3292580015209 40.02409411493859, -105.3293400314355 40.02426807343316, -105.3293850744826 40.02433971920112, -105.329517076826 40.0245221086009, -105.3296581319994 40.02466094949524, -105.3297101574987 40.0247041251023, -105.3298849343158 40.02478097424918, -105.330075850617 40.02482902161795, -105.3301448347398 40.02483905198635, -105.3303063677034 40.02486253821598, -105.3305089314445 40.02490174321267, -105.3307188932055 40.02497976589941, -105.3311201805862 40.02514192076426, -105.3313211016588 40.02521297880104, -105.3315614094424 40.02528981493634, -105.3316864080329 40.02530226875604, -105.3318593114162 40.02530661078252, -105.3320268883447 40.02527797201461, -105.3322212954186 40.02522737817259, -105.3323144391407 40.0251865241619, -105.3324583090925 40.02512342117116, -105.3326207608531 40.02505003162955, -105.3327166037238 40.02501949364788, -105.3328488509051 40.02500107885299, -105.3329530767121 40.0250179756226, -105.3330761532333 40.02506509655677, -105.3334181797729 40.02523387018027, -105.3336921200928 40.0253378996183, -105.3338808648359 40.02539134594898, -105.3341307947925 40.02544487907239, -105.3342930478431 40.0254532928835, -105.3344340886531 40.02543304437418, -105.3345139544222 40.02540861718986, -105.3346764107789 40.02533318028983, -105.3348588869171 40.02521323380916, -105.3349301769176 40.02516213123148, -105.334942439392 40.0251533413287, -105.3351340153575 40.02508456072082, -105.3352794641085 40.02507572510495, -105.3354306917962 40.02509896697647, -105.3355180506154 40.02513393951381, -105.3358146694223 40.02529351858141, -105.3360870116539 40.02543283740193, -105.3366797666057 40.02573373858232, -105.3368153907778 40.02580180617613, -105.3369393034369 40.0258639947272, -105.3370898293551 40.02596861159827, -105.337211444122 40.02608962972621, -105.3372945325549 40.02622374646779, -105.3373147386148 40.02627063395128, -105.337421175453 40.02647877096612, -105.3374981735376 40.026582085771, -105.3376050923685 40.02666898418729, -105.3377398955795 40.02674301993157, -105.3378653071847 40.02677945552124, -105.3379240857469 40.02679433669536, -105.3381088963428 40.02683907028913, -105.3381922987373 40.02687609862392, -105.3382659791816 40.02691977176665, -105.3383043922788 40.02695517610391, -105.3383708887366 40.02703599359061, -105.3383777622052 40.02713038225339, -105.338366843368 40.02723611127646, -105.3383566309992 40.0272642467565, -105.3382529574146 40.02752611738724, -105.338225780298 40.02763739410864, -105.3382170012274 40.02773192113717, -105.3382338601833 40.02783799351767, -105.3383062021897 40.02799593461113, -105.338404047229 40.02811187719205, -105.3384651416272 40.02816304037792, -105.3385772570687 40.02823389648423, -105.3387027374635 40.02828469390063, -105.3388570775456 40.02831510567995, -105.3390817408703 40.0283388001672, -105.339237772709 40.02837330724666, -105.3393408026778 40.02842274061585, -105.339427070937 40.0284871535725, -105.3395271463893 40.02860730522766, -105.3395743309235 40.02869523638033, -105.3395908092224 40.02880027047129, -105.3395907679906 40.02884567393286, -105.3395316310671 40.02907021534642, -105.3395313939624 40.0291709390978, -105.3395785284584 40.029280301116, -105.3396758483765 40.02938759113305, -105.3398070717007 40.02948011247911, -105.34001105511 40.02959898763005, -105.34015883881 40.02966944762828, -105.3403328781856 40.02971994667367, -105.3404849920475 40.02972509898724, -105.3406360896496 40.02970691478322, -105.3410469038371 40.02961451122763, -105.341183063898 40.02960005782608, -105.3413729948086 40.02962008481045, -105.3415028859989 40.02966089163202, -105.3416609109556 40.02973495466169, -105.3418081666057 40.02983288521217, -105.3419061589185 40.02992388512177, -105.3420809641687 40.03015389630465, -105.342137060486 40.03029507504125, -105.3421488596493 40.03044031811095, -105.3421403156747 40.03055896510004, -105.3421095060823 40.0306210722046, -105.3420716051278 40.03069511489726, -105.3419991759212 40.03077501854443, -105.341919419521 40.03083712699294, -105.3418300778567 40.03089928889136, -105.3415005965306 40.03112171569501, -105.3410174858492 40.03147037200236, -105.3408471369649 40.03159443563352, -105.340665615881 40.03172705505519, -105.3405288206844 40.03180830358372, -105.3403725243837 40.03188309433408, -105.3402050811774 40.03195572768927, -105.3399985277202 40.03206259515791, -105.3398923459022 40.03216531452311, -105.3398401151529 40.03228710789242, -105.339815900834 40.03266454513719, -105.3397910481914 40.03276958840173, -105.3397623867686 40.03289592220633, -105.3397648869638 40.0330180815536, -105.3398021263316 40.03310402182879, -105.3398648639367 40.03318323722127, -105.3399094257732 40.03320258646184, -105.3399874379754 40.03322412473215, -105.3400861009968 40.03322904669189, -105.3404129451709 40.03319600779776, -105.340606091903 40.03321988353994, -105.3407891693523 40.03327394200747, -105.3409739123984 40.03337906294917, -105.3411214760025 40.03350214896666, -105.3414135867008 40.03377043530846, -105.3416446218389 40.03392719713566, -105.3418169530248 40.03404894816423, -105.3419979269082 40.03425771521409, -105.3420729438595 40.03436925697198, -105.3421506900844 40.03450652043009, -105.3422027158252 40.03456991529723, -105.3422675171242 40.0346224063464, -105.3423343685873 40.03464821394812, -105.3424653436751 40.03467410999632, -105.3429150731083 40.03468705674727, -105.3431410697753 40.03471591391834, -105.3433656111949 40.03478463226877, -105.3435020608055 40.03485553907074, -105.3438695438839 40.03508748923305, -105.3440168467119 40.03514205613806, -105.3440255978391 40.03514317666856, -105.3441489464593 40.03515897953323, -105.3442811158003 40.03514598153194, -105.3445051287401 40.03510592924802, -105.3447008653332 40.03509301643103, -105.3448968898014 40.03511112379889, -105.3450871457833 40.0351531064796, -105.3453108748094 40.03523795776137, -105.3454389324795 40.03530511152007, -105.3455861725568 40.0354181365134, -105.3457001544155 40.0355508806632, -105.3457428449966 40.03562395961514, -105.3458831215092 40.03597388322648, -105.345896628054 40.03615305911401, -105.3458797746984 40.03628602631347, -105.3457491322696 40.03663309661266, -105.3457611032644 40.03670887964498, -105.3458098776353 40.03677702573989, -105.3458869092818 40.03682599243626, -105.3459829278598 40.03684890616413, -105.3461322249344 40.0368457054413, -105.3466198830052 40.03677206577161, -105.3467530710819 40.03678294877792, -105.3468751210049 40.03682401467811, -105.3469760397207 40.03689195387994, -105.3471355108481 40.03703348689576, -105.3472691705876 40.0371086708003, -105.3472744176314 40.03710968647263, -105.3474308076592 40.03714103151144, -105.3475785708468 40.03714336947589, -105.3481836375957 40.03712059375427, -105.348392981334 40.03713896938038, -105.3485029214573 40.03716601706564, -105.348603897788 40.03720897453926, -105.3486919822502 40.03726701348017, -105.3487650432671 40.0373360133605, -105.3488319497072 40.03744288818694, -105.3488511085128 40.03750001347461, -105.348856789205 40.03820800949617, -105.3487067298522 40.03821232955207, -105.3477914050935 40.03821638893005, -105.3474817926258 40.03821722291953, -105.3468614299469 40.03822512838605, -105.3450104181683 40.03829153532944, -105.3450179171597 40.03868015700185, -105.3460405482716 40.0386437539853, -105.3461031168401 40.03898908284479, -105.3453268746833 40.03901948006025, -105.3452802180325 40.03911018389644, -105.345271517239 40.03912433761808, -105.3452452833364 40.03915814157467, -105.3452130574343 40.03918918870853, -105.3451781010895 40.03921517142847, -105.3451448277192 40.03923480953083, -105.3451089087152 40.03925177274996, -105.3450576487383 40.03926988529709, -105.3450069768098 40.03928187960952, -105.344961760615 40.03928819273935, -105.3449089508063 40.03929064807553, -105.3448494533033 40.03928712489946, -105.3447950264157 40.03927776511058, -105.3447425347318 40.03926247803446, -105.3446092328436 40.03929490292018, -105.3445765512982 40.03930516501039, -105.344539877266 40.03932120387111, -105.3444846960346 40.03935795158987, -105.3444426165169 40.03940586426801, -105.344423128196 40.03944725428348, -105.3444160073502 40.03949552391189, -105.3444275517575 40.03955601888752, -105.3444731759986 40.03968833424123, -105.3444965572211 40.03975520013649, -105.3445205624492 40.03981616221999, -105.3445578084813 40.03989778498795, -105.3446376646379 40.04003968424905, -105.3447276531524 40.04016680845205, -105.344795157412 40.04024733253993, -105.3448549167217 40.04031071675156, -105.3448484541613 40.04055274004725, -105.3448541691076 40.0406499600528, -105.3448674149786 40.04072253855343, -105.3448882399842 40.04079357632659, -105.3449216829459 40.04087332410908, -105.3449704426995 40.04095811087339, -105.3446364322639 40.04102959990085, -105.3446007162516 40.04104340376086, -105.3445703711054 40.04106466860651, -105.3445493695219 40.04108914063158, -105.3445380231417 40.04111119661664, -105.3445343361066 40.04112275146215, -105.3445311011553 40.04114724832418, -105.3445392814093 40.04121096396332, -105.3419896303343 40.04121709476975, -105.3422755387781 40.04337513429397, -105.3465131388534 40.04343423722576, -105.3501117189857 40.04341854173573, -105.3509604583964 40.04341720319611, -105.351061685705 40.04341728708226, -105.3544519058515 40.04524596662837, -105.355091416096 40.04556889885021, -105.3559880623356 40.04583041298836, -105.3567595372542 40.04599519383382, -105.3579301381531 40.04606086270712, -105.3600970053326 40.04564174739976, -105.3606742433043 40.0468628855719, -105.3621557651074 40.04965424089358, -105.3639920692559 40.05282887853546, -105.3641080684391 40.05289587827868, -105.3797250233372 40.06069585746808, -105.3900870057658 40.06584284178945, -105.3912861257657 40.07092499987773, -105.3914749402041 40.07083101793872, -105.3920811145549 40.07050298994405, -105.3925910222121 40.07026600808574, -105.3937980289077 40.06981087854467, -105.3940840170989 40.06972192263695, -105.3946001680771 40.06959803960483, -105.3947989293112 40.06953590537677, -105.3948919023455 40.06948987079981, -105.394964868722 40.06944107368035, -105.395060070696 40.06933903984681, -105.3952621280964 40.06899113614033, -105.3955138612367 40.0686358647477, -105.3957139250865 40.06842109885081, -105.3959568633348 40.06820609746421, -105.3961321294408 40.06808409464642, -105.3965509251752 40.06782505281563, -105.3967590498075 40.06770994229892, -105.3970411697905 40.06757211203932, -105.3973890575354 40.06741704540752, -105.3979349933502 40.06719105257222, -105.3989681210101 40.0668320704148, -105.3993949116376 40.0667119298152, -105.4001279456997 40.06656295502956, -105.400853036919 40.06646804795456, -105.401574842874 40.0664209000962, -105.4031081030495 40.06634588138125, -105.4033760986539 40.06632908658128, -105.4036001268962 40.06632597936235, -105.4039354886404 40.06629270998662, -105.4039684530764 40.06628998415017, -105.4041299199174 40.06627663574243, -105.4042548603106 40.06623819278212, -105.4043540234276 40.06619888982722, -105.4044344048956 40.06614050729836, -105.4045148499365 40.06603666564356, -105.4047389400583 40.06573287074457, -105.4047829657393 40.06567608181868, -105.4049212700939 40.06553693910522, -105.4051253441126 40.06542981958253, -105.4053520055905 40.06532884620861, -105.4056105037759 40.06528097971057, -105.4058260373516 40.06528440260607, -105.4060288655031 40.0653072983951, -105.4061852130406 40.0653236615075, -105.4063458769007 40.0652750842445, -105.4065446697525 40.06515834714913, -105.406676242775 40.06503075664818, -105.4068038590952 40.06490576206056, -105.4069109925564 40.06477432561354, -105.4072568691801 40.06434998263192, -105.4075520798087 40.0638858471748, -105.4076144271041 40.06375352486941, -105.4076986539011 40.06358322723908, -105.4077424376704 40.06351872295893, -105.4078528920384 40.06344490160728, -105.407979736912 40.06339954278057, -105.4081488124669 40.06337694790046, -105.4081993022081 40.06354259319305, -105.4082583191018 40.06365304293325, -105.4083384376527 40.06378623987003, -105.4086252315054 40.0642215866695, -105.4087813728473 40.06439056211295, -105.4089458907069 40.06461799217212, -105.4091018907903 40.06489412393282, -105.4092368182365 40.06512802479963, -105.4093225643208 40.06526853688391, -105.409504095397 40.06548498442051, -105.4098262734777 40.06579167091841, -105.4100664892069 40.06598563197285, -105.4102657157319 40.06612999100079, -105.4104355939177 40.0662923524043, -105.4104999331161 40.06642759351949, -105.4105231868886 40.06658533416806, -105.4111090704269 40.0668027547869, -105.4113230710384 40.06683775452498, -105.4123600762381 40.06670774877939, -105.4126030773382 40.06671874798173, -105.4127710765582 40.06675374711786, -105.4135470770253 40.06717174623984, -105.4143210780151 40.06733974415099, -105.4147190788605 40.06742674212688, -105.4148260788204 40.06747274227973, -105.4149630792546 40.06748474171021, -105.4150690789331 40.06755474126348, -105.4153730784282 40.06789174239631, -105.4157380779817 40.06803174076535, -105.4159660790526 40.06803073976152, -105.417218086706 40.06765573284537, -105.4192990814895 40.06934373178217, -105.4204860820148 40.06988972973171, -105.4213540837626 40.07010972666475, -105.4217650863564 40.07012072544669, -105.4219790865552 40.07007372430561, -105.4224070903935 40.06972272033761, -105.4231560979392 40.06916171416628, -105.4234760999032 40.06905671176163, -105.4241311017381 40.06905570945187, -105.4263101075327 40.06940170123508, -105.4276811134631 40.06938769518695, -105.4296940698257 40.06907550496865, -105.429696726161 40.06942996754758, -105.429694386054 40.06959605113096, -105.4296933119867 40.06967240975321, -105.429641808105 40.06967550540362, -105.4292166920104 40.06972721171748, -105.4288950002293 40.06976633789137, -105.4286274367091 40.0698159315109, -105.428326045251 40.06989903627482, -105.4279288266033 40.07006320863681, -105.427767388902 40.07014234364784, -105.4274301435079 40.07031168907899, -105.427187862742 40.07041321736073, -105.4265850469876 40.07060213368924, -105.4264385616445 40.0706539625285, -105.4262836121072 40.07072092919811, -105.4261582347105 40.07078358879082, -105.4259539328541 40.0709165081871, -105.4258003383412 40.07103107048781, -105.4253944374446 40.07137217887671, -105.4252350299228 40.07147595325737, -105.4243155617368 40.07219115576593, -105.4231393098885 40.07308417705716, -105.4226100060591 40.07339089775018, -105.4222132276659 40.07363857455535, -105.4217252471861 40.07398674410683, -105.4215431642913 40.07408511303873, -105.4211965898197 40.07427234585262, -105.4210308105794 40.07434951045089, -105.4206584442087 40.07448493070384, -105.4202083996824 40.07461261810035, -105.4195352042127 40.07476456033439, -105.4191247017771 40.07482938094511, -105.4189980306713 40.07484611794027, -105.4186447055464 40.07487513225324, -105.4180009566014 40.07488857546316, -105.4177762251645 40.07488622163074, -105.4174610348563 40.0748779494316, -105.4172705764785 40.07488147149702, -105.4170810759536 40.07488206684572, -105.4170306009453 40.07488568808787, -105.4169286974435 40.07489512468741, -105.4167905896386 40.07491916695444, -105.4166333942057 40.07497684600628, -105.4162312907294 40.07517846289863, -105.4159997512771 40.07528949075067, -105.4156196132907 40.07543625610639, -105.4153350203652 40.07550396612029, -105.4151395682494 40.07551491221498, -105.4149634135315 40.07550234559449, -105.4148358409656 40.07547591583315, -105.4146111929816 40.07540552041137, -105.4143570994708 40.07527584758753, -105.4142381667132 40.07519455728776, -105.4139032823823 40.07494558003621, -105.4136444687195 40.07478517666688, -105.413329475767 40.07462253567618, -105.4130705753038 40.0745330917355, -105.4129058764918 40.07449931594424, -105.4127516241002 40.07448895733638, -105.4125773454127 40.07450053023379, -105.4124096976944 40.0745384436123, -105.4122829936822 40.0745807785052, -105.4116113120437 40.07483923530526, -105.4112998081208 40.07492678295778, -105.4111312145296 40.07495957269411, -105.4109493026843 40.07498064805032, -105.4104369611586 40.07499780879358, -105.4099465988038 40.07495572838605, -105.4096666239786 40.07496136200007, -105.4094075828542 40.07497944835027, -105.4087209130649 40.07504255224723, -105.4072133339139 40.07514450001526, -105.4064926228099 40.07519135351045, -105.4058410165122 40.0752136172959, -105.4054705638814 40.0752272141406, -105.40520487196 40.07523357995193, -105.4049353748692 40.07523628450529, -105.4047392325432 40.07521783433648, -105.4045848509388 40.0751897922855, -105.4041947147465 40.07508862949976, -105.403705422345 40.0749653223569, -105.4035454821902 40.07493738955924, -105.4033969451357 40.07492482835819, -105.4031503024901 40.07492901141337, -105.4028950470262 40.07496317992302, -105.4025169204411 40.07501553263012, -105.4023550157805 40.07502929541273, -105.4021645541007 40.07503425519602, -105.4019389002541 40.07501138551396, -105.40168661591 40.074965083188, -105.4015019436022 40.07491810670258, -105.40096224968 40.07475231378992, -105.4007728206619 40.07470313718637, -105.4006128875573 40.0746708105926, -105.4003900881106 40.07465013520603, -105.4001936699258 40.07464511287059, -105.3999920191408 40.0746658845997, -105.3997996016553 40.07470668529642, -105.3996328800538 40.07475774923518, -105.3994223224821 40.0748299894019, -105.3992936939425 40.07487962339136, -105.3991136328338 40.07493506377642, -105.3989345365082 40.07498245837664, -105.3987192795767 40.0750122629322, -105.3984012230241 40.07501125209868, -105.3982545679028 40.07501551265776, -105.3981326490511 40.07503442581616, -105.3980545259296 40.07505922901456, -105.3979649460374 40.07510377494535, -105.3978486566331 40.0751790217227, -105.3973899365647 40.07562852046983, -105.3972817002089 40.0757136836102, -105.397169427459 40.07578848025003, -105.3968792179321 40.0759179797459, -105.3959609054664 40.07622318892043, -105.3953231254621 40.07647233550051, -105.3947619214149 40.07666278952232, -105.3941305833764 40.07686297010658, -105.3939136913895 40.07697539101873, -105.3934575621836 40.07722224613386, -105.3931865114511 40.07731992618486, -105.3929282780375 40.07737354901404, -105.3926318413482 40.07740020380218, -105.3923466903028 40.0774207953173, -105.3919433258007 40.07747300969441, -105.3915512466445 40.07751915932716, -105.3910859383422 40.07751872123406, -105.390588819259 40.07748152648809, -105.3899547533051 40.07738544205882, -105.3895851208953 40.07734591650613, -105.3890560983312 40.07733071977488, -105.3886608422517 40.07736951179238, -105.3882208880001 40.07745722445686, -105.3878287902893 40.07751315322446, -105.3875386890442 40.07756183623066, -105.3871751517061 40.07769123986255, -105.386958188724 40.07783792342001, -105.3868401010417 40.07793818621354, -105.3866996581514 40.07806535888105, -105.386575220841 40.07815092657836, -105.3864348761523 40.07821933925117, -105.3862435609229 40.07827301294386, -105.3861064964615 40.0782851193332, -105.3859439556369 40.07828495884738, -105.3854915187126 40.07820861461854, -105.3852495670619 40.07817436606354, -105.3849689629014 40.07813464671029, -105.384647065656 40.07813677433686, -105.3843346505428 40.07818542609105, -105.3841911614831 40.07822690365325, -105.3838658088119 40.07838571414805, -105.3835116873142 40.07859345906748, -105.3832533311892 40.07871071489546, -105.3828706781617 40.07882784409028, -105.3824975639514 40.07895722236837, -105.3821530389425 40.07914049159699, -105.3818913601033 40.079333636382, -105.3816040092101 40.07962713452685, -105.381316880753 40.07979087291746, -105.3809245713487 40.07995695099259, -105.3802294146402 40.08015943763821, -105.379588467187 40.08034483921757, -105.3792504093654 40.08046689970899, -105.3786411661966 40.08074291496696, -105.3780797871333 40.08098470179396, -105.3777130575363 40.08109693300169, -105.3774866867055 40.08114076234569, -105.3770053036764 40.08120390520853, -105.3766993091122 40.08121582032145, -105.3761925603991 40.08120548435789, -105.3760268068356 40.08121510006245, -105.3757111712446 40.08127107066737, -105.3751786731141 40.08139780561959, -105.3744967961343 40.08157402736211, -105.3735477428702 40.0818006048877, -105.3730416668277 40.08192675278983, -105.3726786466126 40.08199815224141, -105.3724146658471 40.08203164841389, -105.3720517316847 40.08205658721963, -105.3715667481044 40.08210790769671, -105.3712911926056 40.08211536164035, -105.3710047166085 40.08208494329329, -105.3706571489542 40.0819848523058, -105.3701603136584 40.08182251295334, -105.3693330902472 40.08154316557858, -105.3691740018331 40.08149407507, -105.3689732329173 40.08146939130329, -105.3687454792302 40.08146913257269, -105.3682581015067 40.08148550858736, -105.3674792688943 40.08151471573545, -105.3669855945874 40.08156515588454, -105.3666338417142 40.08163741303427, -105.3665354783196 40.08168099405719, -105.3664748780766 40.08172531938194, -105.3664584034446 40.08159014621046, -105.3664654543084 40.08151024750345, -105.3665410705586 40.0813216177777, -105.3666249026477 40.08104341501357, -105.3665924458401 40.08081366575016, -105.3664632649919 40.08064976953737, -105.3662886091598 40.08052481296188, -105.3660390097108 40.08039337010403, -105.3659304079325 40.08034970692742, -105.3658929678842 40.08033465331701, -105.3657461992619 40.08003983094896, -105.3657423068642 40.08003200973842, -105.3656923072547 40.07998801008782, -105.365564750368 40.07986337558394, -105.3655613064671 40.07986000947152, -105.36547830664 40.07972600962538, -105.3654660928458 40.0796893671258, -105.3654633071831 40.0796810104118, -105.365430306542 40.07966001037191, -105.365182305831 40.0795810101703, -105.3650123076826 40.07954700945725, -105.3646413071265 40.07954001023455, -105.3646409597663 40.07954016834047, -105.3644273067806 40.07963700967829, -105.3641503065364 40.07968800899322, -105.3640113064601 40.07968900896079, -105.3640110721188 40.07968893393132, -105.3638723068514 40.07964401110103, -105.3637572863339 40.079587932841, -105.3637380311503 40.07957854522331, -105.3652410674733 40.07915339564261, -105.3652857427266 40.07914075772138, -105.3650620067686 40.07914218420888, -105.364451609022 40.07932611178899, -105.3644452352826 40.0793280334828, -105.3644119629354 40.07914632201314, -105.3643715348942 40.07889535434658, -105.3643097355887 40.07858571793681, -105.3642741451352 40.07840741532311, -105.3642283755162 40.07817809457496, -105.3642159208946 40.0781157013513, -105.3641896030986 40.07800118147891, -105.3641331627319 40.07770186991803, -105.364130402719 40.07768724201821, -105.3639345284794 40.07776073618592, -105.3638318920551 40.07763710989789, -105.3637768699827 40.07764845253151, -105.3628899389825 40.07783129497066, -105.3627564852363 40.07785880595277, -105.362650306177 40.07779700989174, -105.3621513056302 40.07752001023393, -105.3617303055701 40.07727800991306, -105.3612283062352 40.07688201049471, -105.3606163062426 40.0762420105657, -105.3600943059392 40.07558800966181, -105.3600823364097 40.07558033697835, -105.3600733286092 40.07558051699573, -105.3597576897657 40.07558682392172, -105.3580379658965 40.07561815271803, -105.3571651961045 40.07563123686058, -105.3571567757665 40.07563136333869, -105.3571387269635 40.07522658799327, -105.3581805956881 40.07496615732713, -105.3</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>Casey MS</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>1301 High St, Boulder, CO 80304</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>http://cam.bvsd.org/</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>Casey Middle School</t>
         </is>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>40.0228711759357</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>-105.2791579470394</v>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>http://cam.bvsd.org/</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>POINT (-105.2791579470394 40.0228711759357)</t>
         </is>
@@ -774,53 +791,56 @@
           <t>MULTIPOLYGON (((-105.0528254173539 39.97775321191219, -105.0623973749708 39.97372063584294, -105.0649011917563 39.97266558612067, -105.0651118917171 39.97257307983785, -105.0655694045389 39.9723662368725, -105.065843589435 39.97223613527462, -105.0658811416601 39.97221831119657, -105.0661894751648 39.97206622071226, -105.0664943064096 39.97191000920827, -105.0667955519143 39.97174972953768, -105.0669332243926 39.97167371577209, -105.0670931060007 39.97158542816613, -105.0673868899058 39.97141715346223, -105.0676768084355 39.97124496093888, -105.0679627769857 39.97106889804302, -105.0682344853294 39.97089555776282, -105.0682447038632 39.97088902300355, -105.0685225067772 39.97070538868115, -105.068796101087 39.97051804972923, -105.0690654009565 39.9703270653004, -105.0693303228938 39.97013249455646, -105.0695907916381 39.96993439128609, -105.0698467248178 39.9697328236623, -105.0700980436669 39.96952784546108, -105.0703446716672 39.96931952577825, -105.0705865334178 39.96910794272046, -105.0707451313361 39.96896671059965, -105.0710392581784 39.96869541182943, -105.0717161300403 39.96807106305508, -105.0721451917206 39.96767528499866, -105.0748030386571 39.96522348552804, -105.0755271326264 39.96455551191475, -105.0756795819458 39.96441977864863, -105.0760226022435 39.9641223622555, -105.0762591021639 39.96392605437885, -105.0765000134104 39.96373295238015, -105.0765121122001 39.96372358851206, -105.076745267736 39.96354311362378, -105.0769947863516 39.96335659723671, -105.0772484951806 39.96317345786009, -105.0775063177919 39.96299375282862, -105.0777681754329 39.96281753676679, -105.078033987013 39.96264486429067, -105.0782188195883 39.96252897618582, -105.078303672632 39.96247578731922, -105.0785771512385 39.96231035506532, -105.078790249033 39.96218600590304, -105.0788543347446 39.96214861941868, -105.0791351467864 39.96199062961024, -105.0792737237913 39.96191547900955, -105.0794194922649 39.96183643660421, -105.0797072960419 39.96168608153102, -105.0797096277661 39.96168490746428, -105.0799981319371 39.96153978167267, -105.0804681708858 39.96137839815337, -105.0807716778314 39.96128039372289, -105.0810773181376 39.96118649517031, -105.0811351954348 39.96116960736901, -105.0813850402922 39.96109671219882, -105.0816947493415 39.9610110768708, -105.0820063527403 39.96092961045033, -105.0823197567362 39.96085234050275, -105.0826348617594 39.9607792891692, -105.0829515752528 39.9607104804185, -105.0832698046996 39.96064593191601, -105.0834149319631 39.96061856582238, -105.0835894458524 39.96058566578888, -105.0835950222725 39.96058461865386, -105.0835984859981 39.9605839691827, -105.0836019532348 39.96058331972419, -105.0836054181252 39.96058267115772, -105.0836088841913 39.96058202169477, -105.083612350252 39.96058137313233, -105.0836158186588 39.96058072367757, -105.083619282362 39.96058007780842, -105.0836227484114 39.96057943104697, -105.0836262144553 39.96057878518599, -105.0836296828453 39.9605781384328, -105.0836331500594 39.96057749257591, -105.0836366160866 39.96057684941663, -105.08364008446 39.96057620536502, -105.0836435540202 39.96057555861563, -105.0836470188713 39.96057491635244, -105.0836504848872 39.96057427499397, -105.0836539556066 39.96057363004976, -105.0836574192707 39.96057299048394, -105.0836608911548 39.96057234644444, -105.0836643559891 39.9605717068826, -105.0836678278567 39.96057106554482, -105.0836712938558 39.96057042688767, -105.0836747633769 39.96056978644184, -105.0836782317166 39.96056914779295, -105.0836817000507 39.96056851004457, -105.0836851707256 39.96056787230461, -105.0836886390596 39.96056723455608, -105.0836921109103 39.96056659591945, -105.0836955792277 39.96056596087259, -105.0836990510781 39.9605653222358, -105.0837025182251 39.9605646871845, -105.0837059912293 39.96056405125364, -105.0837094583596 39.96056341890407, -105.0837129290119 39.96056278476582, -105.0837163996588 39.96056215152812, -105.0837198714869 39.96056151649324, -105.0837233409632 39.96056088325109, -105.0837268127747 39.96056025091792, -105.0837302810585 39.96055962127388, -105.0837337552162 39.96055898804835, -105.083737227011 39.9605583584168, -105.0837406988058 39.96055772878519, -105.0837441694246 39.96055710004981, -105.0837476412248 39.96055646951731, -105.0837511153602 39.96055583989384, -105.0837545847974 39.96055521295525, -105.0837580589381 39.9605545824309, -105.0837615307161 39.96055395550054, -105.0837650024939 39.96055332857008, -105.0837684742552 39.96055270434148, -105.0837719518849 39.96055207743193, -105.0837754213053 39.96055145319465, -105.0837788989348 39.96055082628491, -105.0837823671848 39.96055020204319, -105.0837858412865 39.96054957782249, -105.0837893153773 39.96054895540301, -105.0837927918197 39.96054833119056, -105.0837962647344 39.96054770966726, -105.0837997388194 39.96054708814808, -105.0838032140748 39.96054646663302, -105.083806690506 39.96054584422146, -105.0838101634205 39.96054522269775, -105.0838136363184 39.96054460387581, -105.0838171092107 39.96054398595449, -105.0838205879769 39.96054336445156, -105.083824057347 39.96054274831861, -105.0838275360967 39.96054212951744, -105.0838310148517 39.96054150981553, -105.0838344865624 39.96054089369068, -105.0838379606137 39.96054027757422, -105.0838414393467 39.96053966147456, -105.0838449145684 39.96053904536213, -105.0838483921307 39.960538429258, -105.083851864995 39.9605378158388, -105.0838553460684 39.9605371997472, -105.0838588212679 39.96053658723688, -105.0838622964727 39.96053597382583, -105.0838657751887 39.96053536042736, -105.0838692503714 39.96053475061868, -105.0838727314336 39.9605341363278, -105.0838762042755 39.96053352651045, -105.0838796818043 39.96053291580925, -105.0838831605036 39.9605323051122, -105.0838866392027 39.96053169441505, -105.0838901143741 39.96053108640699, -105.0838935954139 39.96053047571807, -105.0838970717556 39.96052986771409, -105.083900550438 39.96052925971836, -105.0839040314611 39.96052865173108, -105.0839075066102 39.96052804732509, -105.0839109888036 39.96052743934182, -105.0839144651286 39.96052683403919, -105.0839179461349 39.96052622875342, -105.0839214248005 39.96052562345907, -105.0839249022901 39.96052501906101, -105.0839283844667 39.9605244137791, -105.0839318607694 39.96052381207851, -105.083935341759 39.96052320949416, -105.0839388215782 39.96052260690542, -105.0839423025677 39.96052200432079, -105.0839457847275 39.96052140174031, -105.083949259843 39.96052080273695, -105.0839527443434 39.96052020016469, -105.0839562241459 39.96051960027736, -105.083959706289 39.96051900039836, -105.0839631860858 39.96051840141151, -105.0839666670419 39.96051780423004, -105.0839701480144 39.96051720434649, -105.0839736266242 39.96051660805698, -105.0839771099209 39.96051601088363, -105.0839805943879 39.9605154137144, -105.0839840753383 39.96051481743307, -105.0839875551072 39.96051422294863, -105.0839910407444 39.96051362578331, -105.0839945181669 39.96051303219087, -105.0839980014469 39.96051243771883, -105.0840014870674 39.96051184325513, -105.0840049680009 39.96051124967506, -105.084008447753 39.96051065789194, -105.0840119357142 39.96051006343639, -105.0840154131144 39.96050947344588, -105.0840189010645 39.9605088807914, -105.084022379624 39.96050829260622, -105.0840258663927 39.96050770174858, -105.0840293519908 39.9605071108866, -105.084032831726 39.9605065218047, -105.0840363161426 39.96050593273956, -105.0840398029001 39.96050534368276, -105.0840432861352 39.96050475641453, -105.0840467670241 39.96050417003831, -105.0840502514186 39.96050358457534, -105.0840537405165 39.96050299552659, -105.0840572225701 39.96050241005499, -105.0840607081403 39.96050182369524, -105.0840641913476 39.96050124092958, -105.0840676792585 39.96050065457812, -105.0840711612954 39.96050007180799, -105.0840746480192 39.96049948815401, -105.0840781347376 39.96049890540058, -105.0840816214558 39.96049832264705, -105.0840851046519 39.96049774168201, -105.0840885925404 39.96049715893248, -105.0840920780771 39.96049657797571, -105.0840955624379 39.96049599791521, -105.084099047969 39.96049541785884, -105.0841025381871 39.96049483691866, -105.0841060213608 39.96049425955555, -105.0841095115733 39.96049367951577, -105.0841129982635 39.96049310126449, -105.0841164849483 39.96049252391376, -105.084119971633 39.96049194656296, -105.0841234583011 39.9604913719139, -105.084126947332 39.96049079367064, -105.0841304328296 39.96049021901722, -105.0841339218383 39.96048964437633, -105.084137410847 39.96048906973534, -105.0841409010315 39.96048849419781, -105.0841443830013 39.96048792223324, -105.0841478731802 39.96048734759611, -105.0841513598314 39.96048677564822, -105.0841548488288 39.96048620280799, -105.0841583413319 39.96048563088095, -105.0841618303292 39.96048505804052, -105.0841653157933 39.96048448878988, -105.0841688047685 39.96048391955179, -105.084172296101 39.96048334762011, -105.084175786252 39.96048277748539, -105.0841792728698 39.96048221094053, -105.0841827641856 39.96048164171044, -105.084186253144 39.96048107517378, -105.0841897444597 39.96048050594352, -105.0841932345885 39.96047993941084, -105.0841967235468 39.96047937287384, -105.084200213659 39.9604788090429, -105.0842037049579 39.96047824251414, -105.0842071938996 39.96047767867879, -105.0842106840116 39.96047711484754, -105.0842141752939 39.96047655102036, -105.0842176677466 39.96047598719733, -105.0842211601992 39.96047542337421, -105.0842246467834 39.96047486223177, -105.0842281427526 39.96047429752046, -105.0842316316773 39.96047373638628, -105.0842351229429 39.96047317526042, -105.0842386165491 39.96047261414292, -105.0842421054573 39.96047205571033, -105.0842456002338 39.96047149459685, -105.0842490903123 39.96047093616829, -105.0842525827315 39.96047037774804, -105.0842560774913 39.96046981933619, -105.0842595687235 39.96046926361346, -105.0842630623074 39.96046870609777, -105.084266553545 39.96046814947415, -105.0842700471124 39.96046759466021, -105.0842735418555 39.96046703894973, -105.0842770330929 39.96046648232583, -105.0842805290064 39.96046592661936, -105.0842840190458 39.96046537449425, -105.0842875137723 39.96046482148525, -105.084291009691 39.96046426487781, -105.0842944985435 39.96046371545011, -105.0842979956051 39.9604631633499, -105.0843014903368 39.96046260943984, -105.0843049838761 39.96046205912804, -105.0843084762395 39.96046150971257, -105.084311972114 39.96046096030963, -105.0843154691753 39.9604604082089, -105.0843189638848 39.96045985790089, -105.0843224562315 39.96045931118692, -105.084325955617 39.96045876179622, -105.0843294456338 39.9604582132723, -105.084332941497 39.96045766567005, -105.084336433827 39.96045712165759, -105.0843399355421 39.9604565740762, -105.0843434325701 39.96045602737846, -105.0843469248999 39.9604554833657, -105.0843504219278 39.96045493666776, -105.0843539166038 39.96045439176255, -105.0843574100874 39.9604538504556, -105.0843609117802 39.96045330647613, -105.0843644052637 39.96045276516899, -105.0843679010934 39.9604522229695, -105.0843714004397 39.96045167988194, -105.0843748950935 39.9604511385787, -105.0843783956046 39.96045059639577, -105.0843818890714 39.96045005779001, -105.0843853907528 39.96044951561112, -105.0843888830491 39.96044897700094, -105.0843923823731 39.96044843751532, -105.0843958758232 39.96044790161103, -105.084399377488 39.96044736213367, -105.0844028744492 39.96044682624184, -105.0844063749324 39.9604462885613, -105.084409871899 39.96044575176866, -105.08441336886 39.96044521587651, -105.0844168669913 39.96044467998852, -105.0844203651116 39.96044414590168, -105.0844238655837 39.96044361002188, -105.0844273637038 39.96044307593485, -105.0844308618186 39.96044254274836, -105.0844343622794 39.96044200866955, -105.0844378592126 39.96044147727986, -105.0844413596679 39.96044094410149, -105.0844448577714 39.96044041271587, -105.0844483605509 39.96043988224761, -105.0844518598192 39.96043935176664, -105.0844553579115 39.96043882218198, -105.0844588583501 39.96043829170497, -105.0844623576018 39.9604377639256, -105.0844658615568 39.96043723256042, -105.0844693537751 39.9604367065568, -105.0844728588786 39.96043617879819, -105.0844763604763 39.96043565012621, -105.0844798585408 39.96043512504401, -105.0844833613033 39.96043459727665, -105.0844868605436 39.96043407129777, -105.08449036446 39.96043354623639, -105.084493861343 39.9604330229508, -105.0844973664296 39.9604324978934, -105.0845008668181 39.96043197552092, -105.0845043707397 39.96043144955845, -105.0845078687929 39.96043092627666, -105.0845113679944 39.96043040660159, -105.0845148742347 39.9604298842498, -105.0845183769638 39.96042936188523, -105.084521877341 39.96042884131344, -105.0845253812295 39.96042832075415, -105.0845288827715 39.96042780108701, -105.084532385484 39.96042728142393, -105.084535885839 39.96042676445424, -105.0845393908921 39.96042624479943, -105.0845428912471 39.96042572782954, -105.0845463951242 39.96042520907093, -105.0845498989903 39.9604246921135, -105.0845534028563 39.96042417515598, -105.0845569031947 39.96042366088757, -105.0845604058738 39.96042314662753, -105.0845639132453 39.96042263058297, -105.0845674159353 39.96042211452143, -105.0845709185977 39.96042160296298, -105.0845744247878 39.96042108871516, -105.0845779274502 39.96042057715649, -105.0845814336346 39.96042006380912, -105.0845849386486 39.96041955045742, -105.0845884389701 39.96041903889005, -105.0845919427861 39.96041853003707, -105.0845954524706 39.96041801850324, -105.0845989527754 39.96041750963744, -105.0846024612894 39.96041699809916, -105.0846059651107 39.96041648834515, -105.0846094677397 39.96041598218939, -105.0846129774075 39.96041547335694, -105.0846164765197 39.96041496808895, -105.0846199861873 39.96041445925627, -105.0846234911624 39.96041395220792, -105.0846269961319 39.96041344606006, -105.0846305022718 39.9604129399163, -105.0846340072247 39.9604124364702, -105.0846375180461 39.96041193034313, -105.0846410230044 39.96041142599616, -105.0846445279518 39.96041092345035, -105.0846480352453 39.96041042001222, -105.0846515390111 39.96040991926331, -105.0846550486509 39.96040941493276, -105.084658553587 39.96040891418785, -105.0846620596881 39.96040841434764, -105.0846655681353 39.96040791361514, -105.0846690754121 39.9604074128783, -105.0846725838647 39.96040691124497, -105.0846760887787 39.96040641410207, -105.0846795960389 39.96040591606685, -105.0846831091674 39.96040541535069, -105.0846866093832 39.96040492089254, -105.0846901236711 39.96040442198164, -105.0846936321015 39.96040392395023, -105.0846971358338 39.96040342860376, -105.0847006442421 39.96040293417474, -105.0847041550022 39.96040243795269, -105.0847076657566 39.96040194263121, -105.0847111706537 39.96040144818916, -105.0847146790509 39.96040095556098, -105.084718187448 39.96040046293266, -105.0847217017135 39.96039996762343, -105.0847252042421 39.96039947767574, -105.0847287173152 39.96039898596462, -105.0847322268825 39.96039849334009, -105.0847357340925 39.96039800340896, -105.0847392436433 39.96039751348618, -105.0847427531886 39.96039702446389, -105.0850096380202 39.96035979868915, -105.0850658527888 39.96035196090204, -105.0854661723567 39.96029612401237, -105.0857839598441 39.9602517994901, -105.08581766119 39.96024710027866, -105.0859393187197 39.96023012947124, -105.0863498292124 39.96017287246411, -105.0870446975825 39.96009434918611, -105.0871191644284 39.96008593633609, -105.0872096218029 39.96007571814968, -105.0874111940689 39.96005124220132, -105.08747407241 39.95978207714827, -105.0879262449088 39.95978400035138, -105.0880333812514 39.95978094919757, -105.0880380735751 39.95888622819314, -105.0880382211008 39.95885810821171, -105.088040376847 39.95844732158841, -105.0881544918518 39.95844611011514, -105.088625575105 39.95844758571651, -105.0886640890448 39.95844581560196, -105.0886662517168 39.95824081254283, -105.0886676791558 39.95810768699305, -105.0886681074652 39.95803876706348, -105.088667006154 39.95803876493348, -105.0886669710434 39.95803876480815, -105.0886139490879 39.95803863676791, -105.0886136635223 39.95803863574837, -105.0886129648172 39.95803863415455, -105.0886128489525 39.9580386337409, -105.088156924958 39.9580375355978, -105.0881558248172 39.95803753346706, -105.0880454746665 39.95803347060461, -105.0880445006021 39.9580195635822, -105.0880433829552 39.95801955328184, -105.0879369926213 39.95801852529694, -105.0879358702931 39.9580185149788, -105.0879130844023 39.95801829479073, -105.0879119632444 39.95801828447654, -105.087644656805 39.95801569800683, -105.0876435368176 39.95801568769421, -105.0864090392693 39.95800374277388, -105.0864089196698 39.95800377927178, -105.085944272825 39.95814719484354, -105.085944214198 39.95814721264614, -105.0858422212814 39.95817869446593, -105.0858421626544 39.95817871226845, -105.0853102002613 39.95834290120607, -105.0853101451451 39.95834291902096, -105.0852568616573 39.95835978581623, -105.0852568276513 39.95835979650178, -105.0852142572362 39.95837252275794, -105.0852141728226 39.95837254677202, -105.0851744799152 39.95838380628351, -105.0851743486054 39.95838384363866, -105.0851713683735 39.95838468583803, -105.0851712382503 39.95838472049549, -105.0851282032845 39.95839627148312, -105.0851280286276 39.95839631588745, -105.0850847889214 39.95840727438583, -105.0850845674009 39.95840732672732, -105.0850411288291 39.95841768915476, -105.0850408592745 39.95841774942916, -105.0849972405584 39.95842751675351, -105.0849969218048 39.95842758405593, -105.0849531323029 39.95843675721125, -105.0849527690538 39.95843682795595, -105.0849088216957 39.95844539798203, -105.0849084092641 39.95844547305273, -105.08486432509 39.95845344452852, -105.084863865833 39.95845352123168, -105.0848196530585 39.9584608905839, -105.0848191434705 39.95846096800619, -105.0847748173279 39.95846773258756, -105.0847742609255 39.95846780984096, -105.0847298330974 39.95847397329614, -105.0847292287157 39.95847404947573, -105.0847027555357 39.95847736217756, -105.084702105477 39.95847744359641, -105.0846847144455 39.95847960735617, -105.0846840621009 39.95847967976002, -105.0846394730714 39.95848463571034, -105.0846387715935 39.95848470433415, -105.0845941253996 39.95848905211304, -105.0845933771403 39.95848911516397, -105.0845486842725 39.95849286201446, -105.0845478892426 39.95849291769114, -105.0845031673014 39.95849605647136, -105.0845023278417 39.95849610478225, -105.0844575826417 39.95849864181768, -105.0844566952575 39.95849868004812, -105.084411946718 39.95850061180795, -105.0844110125797 39.95850063996208, -105.0843662724055 39.95850196648848, -105.0843652950352 39.95850198277773, -105.0843205760685 39.95850270952104, -105.0843195519606 39.95850271303195, -105.0842768016851 39.9585028461176, -105.0842748694392 39.95850283644447, -105.0842738021159 39.95850282538841, -105.0842291677117 39.95850235091626, -105.0842290811161 39.95850234880245, -105.084228056008 39.95850232438844, -105.0841834837884 39.95850124847972, -105.0841823300452 39.95850120648842, -105.0841378188191 39.95849953274163, -105.0841366382675 39.95849947263985, -105.0840922289767 39.9584972048054, -105.0840921470791 39.95849720000647, -105.0840909911929 39.95849712558269, -105.084046681476 39.95849426725479, -105.0840454063616 39.95849416808221, -105.0840012149839 39.9584907130241, -105.0840011529878 39.95849070739629, -105.0839998978684 39.95849059208348, -105.0839558329632 39.95848655023193, -105.0839557534282 39.95848654183878, -105.0839544773578 39.95848640753589, -105.0839105506463 39.95848177623136, -105.0839091600622 39.95848161179256, -105.0838653855513 39.95847639739046, -105.0838639576698 39.95847620759785, -105.0838390743395 39.95847291137007, -105.083837605523 39.958472716926, -105.0838203494051 39.95847041014899, -105.083820295618 39.9584704018488, -105.0838188865613 39.95847019591163, -105.0837754562364 39.95846381725983, -105.0837739607767 39.95846357768551, -105.0837307130412 39.95845662325169, -105.0837291908175 39.95845635836152, -105.0836861584315 39.9584488300656, -105.0836861011444 39.95844881995132, -105.0836845965917 39.95844853621046, -105.0836417643307 39.95844043579893, -105.0836401827601 39.95844011485198, -105.0835975938788 39.95843145058738, -105.083597505047 39.95843143135245, -105.0835959715385 39.95843109796932, -105.0835536225104 39.95842187254114, -105.0835535208322 39.95842184875641, -105.0835519734337 39.95842149010389, -105.0835098782986 39.95841170446378, -105.0835097976648 39.95841168435775, -105.0835082013262 39.95841129040186, -105.0834663694259 39.95840094818657, -105.0834663110015 39.95840093266411, -105.0834646692338 39.95840050341751, -105.0834231134047 39.95838961097829, -105.0834230736785 39.95838960002673, -105.0834213876632 39.95838913369234, -105.0833801172471 39.95837769466598, -105.0833783706378 39.95837718488006, -105.0833374008502 39.95836519932185, -105.083335634549 39.95836465613951, -105.0832949770394 39.95835213309849, -105.0832931933815 39.95835155742886, -105.0832528481451 39.9583384978061, -105.0832510541473 39.95833789057515, -105.0832110480427 39.95832430437537, -105.0832092320398 39.95832365923636, -105.0831695767604 39.9583095483035, -105.0831677422527 39.95830886707035, -105.0831284436178 39.95829423682988, -105.0831265976219 39.95829352042862, -105.083089599058 39.95827597494203, -105.0830896020937 39.9582756696281, -105.0830905175779 39.95814383200661, -105.0830917470141 39.95796309669239, -105.0830914379236 39.95791388241516, -105.0830912914456 39.9578828783425, -105.0830916557268 39.9578012227973, -105.0830905532878 39.95780121430522, -105.0827441915763 39.95779842227282, -105.0827430961593 39.95779841380289, -105.0811926774133 39.95778589991825, -105.0811915867279 39.95778588334476, -105.0797086205163 39.95776348378201, -105.079707513408 39.95776347343922, -105.0796278873055 39.95776268671114, -105.0796267977524 39.9577626764316, -105.0765567090186 39.95773230338303, -105.0765556299548 39.95773230031829, -105.0753803964513 39.95772928419706, -105.0753793466463 39.95772928122915, -105.07420410847 39.95772626840448, -105.0742030621761 39.95772626543882, -105.0719823361877 39.95771661303881, -105.0719822955386 39.95771376408718, -105.0719811965841 39.95763613716662, -105.0718814336875 39.95058499173008, -105.071880156866 39.95049172946248, -105.0718823803634 39.9502020119051, -105.0720227034047 39.95021855966071, -105.074243983681 39.95048048858849, -105.0745735205932 39.95052068211166, -105.0753572740584 39.95053202794011, -105.076103921084 39.95054268882134, -105.076548242864 39.95054710934591, -105.0765585879308 39.94919947316338, -105.076573762168 39.94765414067553, -105.0765867743723 39.9464964353545, -105.0766014550372 39.94499877740917, -105.076617719676 39.94333941431218, -105.0767360412157 39.94334022196765, -105.0812630425988 39.9433621325146, -105.0821871148648 39.94335411398962, -105.0860388355787 39.94332055103774, -105.089837629017 39.94329425448934, -105.0905070988288 39.94329150589123, -105.0905381523252 39.94329137849177, -105.0906429394402 39.94329094929207, -105.0908401727396 39.94329100598443, -105.0910515015407 39.94328985775073, -105.0910588121924 39.94240422444584, -105.0910630538564 39.94143533357321, -105.0910619951027 39.94143530369561, -105.0910619178891 39.94143530162019, -105.0909044712291 39.9414271563125, -105.0909043710449 39.94131892761472, -105.0909032136222 39.94006601094053, -105.0909447678353 39.94006555055373, -105.0909399203652 39.93925547113504, -105.0909388888204 39.93925539722021, -105.0909386654367 39.93925538111568, -105.0908988896852 39.93924889918723, -105.0908992109706 39.93920895855562, -105.0909009129949 39.93899798932196, -105.0909023057667 39.93869844672675, -105.0909012831155 39.93869845210159, -105.0908424959132 39.93869504775551, -105.090845184441 39.93815985715184, -105.0908493310474 39.93733416590344, -105.0908557345987 39.93605890767786, -105.0910157459438 39.93605931468678, -105.0918615391184 39.93606134993986, -105.0924035059316 39.93606276275314, -105.0933812509434 39.93606530861484, -105.0936100881903 39.93606736899439, -105.0938741497766 39.9360664242047, -105.0940532611034 39.93606746625473, -105.0941950319923 39.93606829722803, -105.0942317090223 39.936068511994, -105.0944119399563 39.93606956913881, -105.0945908398346 39.93607115000719, -105.09476502367 39.93607269419247, -105.0950355885139 39.93607365200723, -105.0951422560202 39.93606933899665, -105.099991742204 39.93605491013817, -105.1046341365572 39.93611220688962, -105.1081492163309 39.93614206184396, -105.1086808361625 39.93614327640896, -105.109037945844 39.93614408640219, -105.1091476096643 39.93614433425925, -105.1092309617087 39.93614452157765, -105.109237555661 39.93614271109521, -105.109236684834 39.93553881744052, -105.1092370249853 39.93540888430044, -105.1097777212305 39.93505856392756, -105.1108825455564 39.93434273300105, -105.1122097787322 39.93350518891695, -105.1122542835765 39.93347639049676, -105.112298162726 39.93344754492023, -105.1123413922496 39.93341812792112, -105.1123839627366 39.93338814847505, -105.1124258612613 39.93335761644661, -105.1124670725634 39.93332654079186, -105.1125075872323 39.93329493048649, -105.1125473923425 39.93326279539504, -105.1125864726237 39.93323014627482, -105.1126248198305 39.93319699300623, -105.1126624222279 39.93316334185509, -105.112699266845 39.93312921079185, -105.1127353419725 39.93309460157923, -105.1127706323048 39.93305953127903, -105.1128051389664 39.93302400800174, -105.1128388431675 39.93298804429421, -105.1128717343385 39.93295164732695, -105.1129038065386 39.93291483329256, -105.112935043359 39.93287760754068, -105.1129654411784 39.93283998987437, -105.1129949918083 39.93280198026674, -105.113023677573 39.93276360117568, -105.1130514984277 39.93272486070767, -105.113078446138 39.93268576694161, -105.1131045065741 39.93264633604267, -105.1131296761662 39.93260657880734, -105.1131539431397 39.93256650870666, -105.1131773051049 39.93252613473981, -105.1131997491178 39.9324854703738, -105.1132212762678 39.9324445300235, -105.1132418736157 39.9324033262552, -105.1132615340774 39.93236187075425, -105.1132802564333 39.93232017252367, -105.1132980335634 39.93227824955331, -105.1133148583837 39.93223611352849, -105.1133307273246 39.93219377524553, -105.1133456344566 39.93215124909558, -105.113359577355 39.93210855038208, -105.1133725489611 39.9320656862871, -105.1133845491696 39.93202267572452, -105.1133955662373 39.93197952676115, -105.1134056070834 39.93193625743383, -105.113414662279 39.93189288032042, -105.1134227329501 39.9318494035309, -105.113429811982 39.93180584415427, -105.1134359028049 39.93176221661275, -105.1134409983348 39.93171853259142, -105.1134451020171 39.93167480381061, -105.1134482067322 39.93163104825973, -105.113450314771 39.93158727495323, -105.1134514272185 39.93154349920609, -105.1134515416603 39.9314997345202, -105.1134506592019 39.93145599260789, -105.1134487762438 39.931412289669, -105.1134459032609 39.93136863564597, -105.113442030799 39.93132504761954, -105.113437162339 39.9312815310053, -105.1134313012498 39.93123811103305, -105.1134244521873 39.93119479222157, -105.113416610382 39.93115159076657, -105.1134077827836 39.93110851930052, -105.1133979751567 39.93106559315386, -105.1133871804378 39.93102282040854, -105.1133754137557 39.93098021552567, -105.1133626703306 39.93093779650227, -105.113348960637 39.93089557328036, -105.113334278771 39.93085355574722, -105.1133186421806 39.93081176197423, -105.1133020484817 39.93077020005903, -105.1132844999339 39.93072888441935, -105.1132659917676 39.93068783125076, -105.113233333253 39.93062041135646, -105.1131118570121 39.93037915497996, -105.1122051443685 39.9286176515559, -105.112204645089 39.92861698878723, -105.1122038636647 39.92861595039223, -105.1121075772735 39.92848730040697, -105.112107214614 39.92848647687905, -105.1120967981585 39.92846279035226, -105.1120837940408 39.92843332545336, -105.1120587550635 39.92837964708677, -105.1120324811199 39.92832631491299, -105.1120049849938 39.9282733442855, -105.1119762689248 39.92822075322429, -105.1119463480464 39.92816855528933, -105.1119452737562 39.92816676565235, -105.1119152257527 39.92811677120648, -105.1119151561972 39.92811665928968, -105.1119141116025 39.92811499674616, -105.1118829195319 39.92806541184156, -105.1118817643469 39.92806365345461, -105.1118494304382 39.92801449791246, -105.111848236553 39.92801275650742, -105.1118147748001 39.92796403847989, -105.1118135410398 39.92796231495335, -105.1117789525426 39.92791404705239, -105.1117776870397 39.92791235133907, -105.1117419938938 39.92786455705546, -105.1117406873717 39.92786287471342, -105.1117038953714 39.92781556397286, -105.1117025524685 39.92781390222298, -105.111664672062 39.92776708947031, -105.111663293943 39.92776544921718, -105.1116243367531 39.92771914800042, -105.1116229245829 39.92771753014858, -105.1115828952545 39.92767174678695, -105.1115814571705 39.92767016037045, -105.1115403777728 39.9276249228577, -105.1115389009839 39.92762335432344, -105.1114967808562 39.92757866629268, -105.1114967564333 39.92757864099171, -105.1114952746698 39.92757712467863, -105.1114521207296 39.9275330041653, -105.1114505828162 39.92753148766221, -105.1114063367063 39.92748791105097, -105.1114047705602 39.92748642237255, -105.1113594310861 39.92744339416132, -105.1113578471896 39.927441941449, -105.1113115286313 39.92739952596935, -105.1113099106939 39.9273980938567, -105.1112626165257 39.92735629742379, -105.1112609750245 39.92735489495286, -105.1112127180535 39.92731372841661, -105.111212659834 39.92731368048491, -105.1112110529834 39.92731235648804, -105.1111618506854 39.92727183251554, -105.111160165556 39.92727049114104, -105.1111100307173 39.9272306241849, -105.1111100062535 39.92723060608901, -105.1111083231939 39.92722931245594, -105.1110572686417 39.92719010976344, -105.1110572395243 39.92719008714854, -105.1110555422339 39.92718882769187, -105.1110035830733 39.92715030732615, -105.11100184127 39.92714905852634, -105.1109489916877 39.92711119441476, -105.1109472591628 39.92710996005612, -105.1108928284495 39.92707140337049, -105.1108909641212 39.9270703063674, -105.1093961302332 39.92618804064294, -105.1093961314852 39.9261876173348, -105.1093963927524 39.92610719247062, -105.1093970325059 39.92591051920145, -105.1093983533093 39.92550463644266, -105.1097181218421 39.92570515554632, -105.1102888127801 39.92606301804486, -105.110533010465 39.92620741090535, -105.1109611901158 39.92646588786492, -105.1117548190385 39.92701045155007, -105.1118443320229 39.92708224169476, -105.1127892552828 39.92784224790676, -105.1134254430625 39.92836563900499, -105.113704554754 39.92859527303179, -105.1137050251862 39.92859566099454, -105.1137255080341 39.92864659560585, -105.1137262203602 39.92864847858181, -105.1140585185026 39.92932809442664, -105.1142666296578 39.9297534484365, -105.1142675329075 39.92975529512095, -105.1144409722058 39.93010978460534, -105.1144411075297 39.93011005976095, -105.1144418766246 39.9301116330937, -105.1186305278242 39.93297156507604, -105.1186310511322 39.93297192257087, -105.1187423547122 39.93370473330269, -105.1187426310094 39.93370658508118, -105.1187496800574 39.93377277206956, -105.1187554050253 39.93382717399349, -105.1187555828143 39.93382885792241, -105.1187358911118 39.93399247936708, -105.1187356803395 39.93399418722844, -105.1187155377534 39.93415766216859, -105.1187153808925 39.93415893428716, -105.118673946249 39.93423753404684, -105.1186732794773 39.93423877115278, -105.1182594976906 39.93500675201376, -105.1182587942474 39.93500805834684, -105.1186175723289 39.93567414007994, -105.1186184037774 39.93567568026551, -105.1186179894219 39.93603778437812, -105.1186179804826 39.93603959378159, -105.1185991792267 39.93884273667501, -105.1185991667161 39.93884455687426, -105.1185988645399 39.93887769668284, -105.1185988473492 39.93887951686656, -105.1185965575348 39.9391274519986, -105.1185965403389 39.93912927308293, -105.1185957855938 39.93921094994099, -105.1185957683928 39.93921277192599, -105.1185948788888 39.93930872385114, -105.1185948615821 39.93931056474968, -105.1185970663537 39.93942461764238, -105.1185971028635 39.93942645961974, -105.1186016797191 39.93965792092657, -105.1186017162192 39.93965976470523, -105.1186032568698 39.9397377195128, -105.1186032935058 39.93973953897395, -105.1186017200063 39.93990283122475, -105.1186017016353 39.93990465320577, -105.1185787173852 39.94163370729682, -105.1185786931275 39.94163553556272, -105.1185577375591 39.9432111717849, -105.1185561841228 39.94332791779106, -105.1139808884187 39.94334427863482, -105.1139797592105 39.94334428565912, -105.1117289010016 39.94335835641672, -105.1117277916897 39.94335836258531, -105.1115097327091 39.94335971429, -105.1115086222681 39.94335971324735, -105.1113693752345 39.94335951289126, -105.111368241391</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>Centaurus HS</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>10300 W South Boulder Rd, Lafayette, CO 80026</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>http://ceh.bvsd.org/</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>Centaurus High School</t>
         </is>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>39.98635981263706</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>-105.1125276640655</v>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>http://ceh.bvsd.org/</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>POINT (-105.1125276640655 39.98635981263706)</t>
         </is>
@@ -840,53 +860,56 @@
           <t>POLYGON ((-105.2726881734809 40.03464911391067, -105.2726840628362 40.03406108764794, -105.2726820898275 40.03390296023866, -105.2726760239568 40.0331518655748, -105.2726760357997 40.03272004799683, -105.272671164566 40.03193189473561, -105.2726661710148 40.03160905132167, -105.2726628596342 40.03142401880926, -105.2726558625326 40.03073798238746, -105.2726510020113 40.03005387211383, -105.273645871071 40.030061869293, -105.2741701059328 40.03006097391676, -105.2751321551345 40.03005901118281, -105.276498044355 40.03007099921356, -105.277470066055 40.03007699534945, -105.2781960300691 40.03008690379698, -105.2784088644469 40.03008703905117, -105.2791998402836 40.03009102538928, -105.2793758908887 40.03009191253876, -105.2803029427175 40.03009011263436, -105.2804018518184 40.030093047055, -105.2805939720805 40.03009396023452, -105.2820898563745 40.03010393344913, -105.2820900004695 40.03010393732394, -105.2821084505153 40.03010442340204, -105.28212225549 40.02926831736175, -105.2821221918683 40.02925559915963, -105.2832689344744 40.02923208823412, -105.2844270167391 40.02923096285564, -105.2854201124465 40.02923199133771, -105.2855761122275 40.02924902721826, -105.2855863693432 40.02924869918922, -105.2855862117171 40.02922543814994, -105.2855754584629 40.02732638721953, -105.2855712105374 40.02672743692585, -105.2855692118289 40.02663843724292, -105.2855892107703 40.02642143748587, -105.2856742107215 40.02601043682525, -105.2856822111836 40.02592843665887, -105.2856812109885 40.02583443661324, -105.2856660543705 40.0255160131922, -105.2867490705732 40.02551994347327, -105.2887301598848 40.02552001896971, -105.290043906236 40.02550594671673, -105.2902481507636 40.02550796560364, -105.2915040127181 40.02550612476494, -105.2920939363481 40.025498130862, -105.2925031180585 40.02550902431486, -105.2926069291672 40.02543973575167, -105.2936339345848 40.02541515269726, -105.2962396867081 40.02535273730569, -105.2962396415504 40.02215067912587, -105.2965063930992 40.02212077652984, -105.3009340316972 40.02443523818599, -105.3015129345043 40.02495411241519, -105.3019768726209 40.02523547047512, -105.3036913518517 40.02668039861787, -105.3158896760477 40.03657502954008, -105.3192074195506 40.03913430974992, -105.3199463280383 40.03974204931587, -105.3213194875436 40.04086764115979, -105.3218374986145 40.04129224587619, -105.3223361207968 40.04169918639315, -105.3228326493725 40.0421032961798, -105.3234564439344 40.04261022835578, -105.3235650157017 40.04270601443687, -105.3236279789155 40.04277070698105, -105.3236391294289 40.04281891589837, -105.3237254066363 40.04321419443117, -105.3237860406652 40.04349198382817, -105.3237843665057 40.04387571131006, -105.3237828875122 40.04421431571672, -105.3237823449867 40.0443384818003, -105.3237809310199 40.04466280651826, -105.3237793817299 40.04501725408277, -105.3237789988946 40.04510503603166, -105.3237783998165 40.04528551141335, -105.3237739562574 40.045350713323, -105.3237755669408 40.04610054821104, -105.3237764999897 40.04656136329066, -105.3237777433405 40.04717500970264, -105.3232106563202 40.04719455446896, -105.323221528834 40.04849852044671, -105.3232344307103 40.05085237381964, -105.3237807104702 40.05084289607972, -105.3237746785025 40.05174426081269, -105.323768510175 40.05268741436502, -105.3237595236597 40.05413331629786, -105.3237456249731 40.05636891728329, -105.3237422288764 40.05691517045657, -105.3236649981389 40.05690199939841, -105.3234309988263 40.05688399882967, -105.3232779999172 40.05690299883362, -105.323172998984 40.05698399884937, -105.3231529996911 40.05707399863253, -105.3231499993645 40.05709199885952, -105.3231619998333 40.05718199904416, -105.3232919997439 40.05737999907437, -105.3234339985885 40.05755099881815, -105.3235629988358 40.05765899900364, -105.3235989988297 40.05778499864036, -105.3235999997156 40.05792899912804, -105.3235059990182 40.05802799856036, -105.3233419994831 40.05810999915607, -105.3231779991147 40.05811899852135, -105.3227089981302 40.05811199963112, -105.3222399987181 40.05809499805878, -105.3220289988635 40.05805999885644, -105.321676998539 40.05804299884692, -105.3214079998949 40.05808799885816, -105.3211850003847 40.05818799905649, -105.3210514373444 40.0582376509077, -105.32106095721 40.05823758461141, -105.3221724264569 40.05822988914631, -105.3225816832363 40.05822705158369, -105.3237332159603 40.05821906132902, -105.3244526418999 40.05821394350896, -105.3282194852361 40.05818707363856, -105.3283319969811 40.05818626656585, -105.3292573137716 40.05818135374078, -105.3292665417278 40.05818130434862, -105.3292919364783 40.05818116989376, -105.3319541386962 40.05816256206004, -105.3339319600427 40.05815113377263, -105.3363688276225 40.05813097199744, -105.3372943533713 40.05812628053155, -105.3373097910866 40.05812620232494, -105.3425993028118 40.05804701136856, -105.3442073023861 40.05802301073521, -105.3446489917473 40.05801662437516, -105.3446489909119 40.05801647666802, -105.3446488464446 40.0580006719369, -105.3472232555888 40.05794871736776, -105.3472232182339 40.05796119576863, -105.3472322260892 40.05796101405485, -105.3472271551965 40.05966073692544, -105.3472224896003 40.06133066754241, -105.3486782908329 40.061357989212, -105.3486782404571 40.06137011633922, -105.3486742154388 40.06233587690733, -105.3473107204354 40.06232116573092, -105.3472109110526 40.06235733955729, -105.3470235657521 40.06242702740272, -105.346800850027 40.0625838279675, -105.3467783723339 40.06259127168354, -105.3467801571126 40.06283435827675, -105.3472076899097 40.06342523965154, -105.3472079425455 40.06342548676287, -105.3486885970446 40.06487342811074, -105.3486849106566 40.06487334582209, -105.3486975687233 40.06488572377337, -105.3471897519431 40.06485211464241, -105.3473133623905 40.06933911891326, -105.3473207934553 40.06961740186438, -105.3473209038137 40.06962151345378, -105.3473428026947 40.07044154251917, -105.3473863264873 40.07207482178335, -105.3521890440063 40.07206474065865, -105.3527429298888 40.0720635653864, -105.3527521643292 40.07206354564473, -105.3566839075929 40.0720551235077, -105.3566879098085 40.07206743037823, -105.3569141002044 40.07276297868636, -105.3569186609197 40.07276170632576, -105.3570182822697 40.07273390079512, -105.3570189338859 40.07274851995955, -105.3570658145457 40.07380002971021, -105.3570743376764 40.07380220901534, -105.357075228185 40.07380243798097, -105.357075334534 40.07380483292546, -105.3570756794207 40.07381255367425, -105.3571196919032 40.07479969608959, -105.3571280259499 40.07479762231507, -105.35803786981 40.07457117646017, -105.358117034332 40.07453663682637, -105.3581232652609 40.07453391823564, -105.358847711203 40.0742178328324, -105.3587794465179 40.07430909535827, -105.3588135101471 40.07430030621352, -105.3588112717716 40.07430329631586, -105.3590849558513 40.07423267261267, -105.3592610081719 40.07404768796147, -105.3594411968741 40.07396265795662, -105.3594470525279 40.07397642512769, -105.3594917021376 40.07408138741301, -105.3596075059446 40.0743536065922, -105.359597384184 40.07435795069615, -105.3595915406397 40.07436046088824, -105.3584869030154 40.074834666367, -105.3584826247326 40.07483650293884, -105.3581805956881 40.07496615732713, -105.3571387269635 40.07522658799327, -105.3571567757665 40.07563136333869, -105.3571651961045 40.07563123686058, -105.3580379658965 40.07561815271803, -105.3597576897657 40.07558682392172, -105.3600733286092 40.07558051699573, -105.3600823364097 40.07558033697835, -105.3600943059392 40.07558800966181, -105.3606163062426 40.0762420105657, -105.3612283062352 40.07688201049471, -105.3617303055701 40.07727800991306, -105.3621513056302 40.07752001023393, -105.362650306177 40.07779700989174, -105.3627564852363 40.07785880595277, -105.3628899389825 40.07783129497066, -105.3637768699827 40.07764845253151, -105.3638318920551 40.07763710989789, -105.3639345284794 40.07776073618592, -105.364130402719 40.07768724201821, -105.3641331627319 40.07770186991803, -105.3641896030986 40.07800118147891, -105.3642159208946 40.0781157013513, -105.3642283755162 40.07817809457496, -105.3642741451352 40.07840741532311, -105.3643097355887 40.07858571793681, -105.3643715348942 40.07889535434658, -105.3644119629354 40.07914632201314, -105.3644452352826 40.0793280334828, -105.364451609022 40.07932611178899, -105.3650620067686 40.07914218420888, -105.3652857427266 40.07914075772138, -105.3652410674733 40.07915339564261, -105.3637380311503 40.07957854522331, -105.3637572863339 40.079587932841, -105.3638723068514 40.07964401110103, -105.3640110721188 40.07968893393132, -105.3640113064601 40.07968900896079, -105.3641503065364 40.07968800899322, -105.3644273067806 40.07963700967829, -105.3646409597663 40.07954016834047, -105.3646413071265 40.07954001023455, -105.3650123076826 40.07954700945725, -105.365182305831 40.0795810101703, -105.365430306542 40.07966001037191, -105.3654633071831 40.0796810104118, -105.3654660928458 40.0796893671258, -105.36547830664 40.07972600962538, -105.3655613064671 40.07986000947152, -105.365564750368 40.07986337558394, -105.3656923072547 40.07998801008782, -105.3657423068642 40.08003200973842, -105.3657461992619 40.08003983094896, -105.3658929678842 40.08033465331701, -105.3659703076023 40.08049001044129, -105.3660033070792 40.08058400926235, -105.3651603062312 40.08079800940757, -105.36386330684 40.08112600999898, -105.3614307179702 40.08181077296624, -105.3614136449111 40.08208931510966, -105.361373970351 40.08273668039418, -105.3613838696417 40.08273389398298, -105.3616833691065 40.08264960897541, -105.3616895744276 40.08266268384122, -105.3618231569629 40.08294413896749, -105.3618343745151 40.08296777085793, -105.3618626507548 40.08302734621064, -105.3612294649398 40.08322514258172, -105.3582044235136 40.08420073402425, -105.3580926092154 40.08423693487651, -105.3581270614178 40.08459850432136, -105.3581348601366 40.08459842924469, -105.3591926002434 40.08458815364854, -105.3591925371214 40.08460053741205, -105.3591905319785 40.0849959100054, -105.3573681646263 40.08502614465402, -105.3569189380437 40.08526239120709, -105.3568395193715 40.08711423232176, -105.3556791226172 40.08712097800886, -105.3556774246944 40.08712098849529, -105.354242246951 40.08712931769688, -105.3542328567851 40.08712937248871, -105.3527096423569 40.08713819019081, -105.3527001841789 40.08713824477123, -105.3519880447198 40.08755429373965, -105.3510273451841 40.08805364431768, -105.3510314240971 40.08805658117283, -105.3510339691511 40.08805849111732, -105.3510364707778 40.08806041991922, -105.3510389277868 40.0880623756828, -105.3510405793695 40.08806372697654, -105.3510413472218 40.08806435481455, -105.3510437197018 40.08806635730237, -105.3510460487584 40.0880683768463, -105.3510483355446 40.08807042245434, -105.3510505753798 40.08807248961713, -105.3510527729524 40.08807457924146, -105.3510549200622 40.08807668771413, -105.3510570237446 40.08807881504423, -105.351059080476 40.08808096392912, -105.351061091431 40.08808313346974, -105.3510630566174 40.08808532006347, -105.3510649713371 40.08808752730682, -105.3510668391175 40.08808975070119, -105.351068656435 40.0880919929439, -105.3510704291584 40.08809425134065, -105.3510721502444 40.0880965294849, -105.3510738208755 40.08809882287498, -105.3510754457399 40.08810113241754, -105.3510770166333 40.08810345630074, -105.3510772620555 40.08810383308597, -105.3510785405837 40.08810579813619, -105.3510800410192 40.08810816876191, -105.3510817287355 40.08811069273843, -105.3510833753659 40.08811323737671, -105.3510849820807 40.08811580357887, -105.351086548892 40.08811838594115, -105.3510880757858 40.08812099076799, -105.3510895604248 40.08812361445374, -105.3510910063348 40.08812625340051, -105.3510924076469 40.08812891030255, -105.3510937713965 40.08813158516899, -105.3510950928933 40.08813427799377, -105.3510963697981 40.08813698607194, -105.3510976021068 40.08813971120482, -105.3510987945178 40.08814244979585, -105.3510999482036 40.08814520184658, -105.3511010526129 40.0881479664427, -105.3511021147673 40.08815074989782, -105.3511031346887 40.08815354230494, -105.3511041123671 40.08815634816715, -105.3511050454592 40.08815916658087, -105.351105933969 40.08816199574477, -105.351106776724 40.08816483565742, -105.3511075737242 40.08816768631873, -105.3511083343561 40.08817054503891, -105.3511090421975 40.08817341449873, -105.3511097078077 40.08817629200986, -105.3511103311927 40.08817917487041, -105.3511109029578 40.08818206937269, -105.3511114371899 40.08818496832981, -105.351111919806 40.08818787712743, -105.3511123602068 40.08819078677125, -105.3511127548545 40.08819370626314, -105.3511131061122 40.08819662750032, -105.3511134057638 40.08819955407481, -105.3511136655411 40.08820248329983, -105.3511138760653 40.08820541426265, -105.3511140443603 40.08820835237604, -105.351114163412 40.08821128772411, -105.351114241413 40.08821422752239, -105.3511142701628 40.08821716815781, -105.3511142520106 40.08822010783207, -105.3511141893056 40.08822304474702, -105.3511140808613 40.08822598520552, -105.3511139243503 40.08822892109879, -105.3511137267983 40.08823185693918, -105.3511134800089 40.08823478731219, -105.351113191008 40.08823771673009, -105.3511128527656 40.08824064248196, -105.3511124723156 40.08824356547749, -105.3511120426341 40.08824648030368, -105.3511115695742 40.08824939147138, -105.3511110496261 40.08825229537347, -105.3511104874762 40.08825519381728, -105.3511098760888 40.08825808679372, -105.3511092248507 40.08826097161301, -105.3511085279028 40.08826384646623, -105.3511077805547 40.08826671134739, -105.3511069968658 40.08826957167852, -105.3511061604374 40.08827241933256, -105.3511052865074 40.08827525703119, -105.3511043656989 40.08827808296099, -105.3511034015258 40.0882808989278, -105.3511023951647 40.08828370313181, -105.3511013407563 40.08828649376421, -105.3511002453384 40.08828926993341, -105.3510991053852 40.08829203523749, -105.3510979279441 40.08829478428164, -105.3510967024539 40.08829752065474, -105.3510954347834 40.08830024166259, -105.3510941284525 40.08830294640897, -105.3510927799473 40.08830563308802, -105.3510913869165 40.08830830439874, -105.3510899505349 40.088310959442, -105.3510884766733 40.0883135946227, -105.3510869629747 40.08831621534176, -105.3510854047624 40.08831881528859, -105.3510838090661 40.0883213971742, -105.3510821712054 40.0883239564893, -105.3510804970312 40.08832649864536, -105.3510787818711 40.08832901553052, -105.3510770257072 40.08833151525054, -105.3510752332379 40.08833399420897, -105.3510734009512 40.08833644969923, -105.3510715288491 40.08833888082079, -105.3510696239633 40.08834128938393, -105.3510676816053 40.088343674482, -105.351065699426 40.0883460379133, -105.3510636821256 40.08834837518056, -105.3510616261805 40.08835068898124, -105.3510595374595 40.08835297662093, -105.3510574124448 40.08835523809517, -105.351055252313 40.08835747160411, -105.3510530570523 40.08835968255164, -105.3510508290275 40.08836186193435, -105.3510485693955 40.08836401695893, -105.3510462734738 40.08836614401667, -105.3510439459587 40.08836824041177, -105.3510415833244 40.08837030974222, -105.3509560258479 40.08843761152456, -105.3507798770322 40.08857084662024, -105.3507538096081 40.08863307525191, -105.3507519531502 40.08863799036086, -105.3507511319305 40.08864084523704, -105.3507504935722 40.08864373007083, -105.3507500357499 40.08864663585278, -105.3507497561281 40.08864955807664, -105.3507496605839 40.08865249044558, -105.3507497479682 40.08865542215029, -105.3507500159438 40.08865834958532, -105.3507504680483 40.0886612637487, -105.3507511019483 40.08866415923357, -105.350751910624 40.08866702882577, -105.3507528976031 40.08866986802661, -105.3507540605621 40.08867266692603, -105.3507553959971 40.08867541921492, -105.350756900396 40.08867812218688, -105.3507585679157 40.08868076682799, -105.350760398576 40.0886833441317, -105.3507623876923 40.08868585139007, -105.3507645258996 40.08868828138591, -105.3507648979519 40.08868866373927, -105.3507668167196 40.08869063232233, -105.3507692461027 40.08869289427427, -105.3507718140629 40.08869506093713, -105.3507745112231 40.08869713049755, -105.3507773305537 40.08869910024445, -105.3507802720763 40.08870096027083, -105.350783320557 40.08870270605373, -105.3507864724758 40.08870433848928, -105.3507897254995 40.0887058521706, -105.3507930608822 40.08870723986828, -105.3507965301085 40.0887090870666, -105.3508980689437 40.08877062856219, -105.3509009761502 40.08877209766227, -105.3509038776238 40.08877350731244, -105.3509068038209 40.08877487196231, -105.3509097547317 40.08877619611515, -105.350912730362 40.08877747706896, -105.3509157295431 40.08877871302094, -105.3509187499201 40.08877990847136, -105.3509217926772 40.08878105801779, -105.3509248566341 40.08878216526129, -105.35092793711 40.08878322569265, -105.350931043486 40.08878423932394, -105.3509341651927 40.08878521334669, -105.3509373034264 40.08878613695467, -105.3509404581733 40.0887870164524, -105.3509436294314 40.08878785274052, -105.3509468183891 40.08878863861543, -105.3509500215108 40.08878938217835, -105.3509532376397 40.0887900762226, -105.3509564620774 40.08879072434474, -105.3509596995144 40.08879132655078, -105.3509629511253 40.0887918819416, -105.3509662087037 40.08879238960599, -105.3509694781146 40.08879284865083, -105.3509727546598 40.0887932626727, -105.3509760383511 40.08879362626768, -105.3509793291805 40.08879394303838, -105.3509826283206 40.08879421298629, -105.3509859299085 40.08879443610383, -105.3509892327773 40.08879460968762, -105.3509925416098 40.08879473734624, -105.3509958505506 40.08879481546952, -105.3509991642883 40.08879484496426, -105.351002473436 40.08879482852016, -105.3510057838647 40.0887947625423, -105.3510090932251 40.08879464882887, -105.3510124038607 40.08879448828358, -105.3510157063963 40.08879427819243, -105.3510190055145 40.08879402216397, -105.3510223012154 40.0887937201983, -105.3510255911674 40.08879336598777, -105.3510288730156 40.08879296403265, -105.3510321479246 40.08879251793702, -105.3510354123884 40.08879202229245, -105.3510386675698 40.08879148160367, -105.3510419158218 40.08879089227121, -105.3510451512775 40.08879025608872, -105.3510483774528 40.08878957396133, -105.3510515873119 40.08878884588005, -105.3510547843766 40.08878807004817, -105.3510579662997 40.08878724736322, -105.3510611354167 40.08878638233142, -105.3510642882273 40.08878546684256, -105.3510674200216 40.08878450989691, -105.3510705378526 40.08878350339787, -105.351073635838 40.08878245634416, -105.351076711646 40.08878136242842, -105.3510797711359 40.08878022345936, -105.3510828072641 40.08877904303054, -105.3510858235602 40.08877781574264, -105.3510888164907 40.08877654879628, -105.3510917860694 40.08877523588691, -105.3510947287704 40.08877388061261, -105.3512448646096 40.08871567828783, -105.3512486912542 40.08871387742979, -105.351251635128 40.08871251945109, -105.3512545906727 40.08871118670531, -105.3512575602452 40.0887098737917, -105.3512605403221 40.08870858340758, -105.3512635344228 40.08870731465686, -105.3512665378591 40.08870606663291, -105.3512695517975 40.08870484203913, -105.3512725785854 40.08870363997784, -105.3512756147108 40.08870245774266, -105.3512786625149 40.08870129713789, -105.3512817208154 40.08870016266518, -105.3512847896299 40.08869904621879, -105.3512878689408 40.08869795590442, -105.3512909599343 40.08869688541922, -105.3512940579142 40.088695837459, -105.3512971652179 40.08869481562927, -105.3513002865475 40.08869381453241, -105.3513034125184 40.08869283595745, -105.3513065466482 40.08869187990894, -105.3513096901057 40.08869094818974, -105.3513128440714 40.08869003719879, -105.3513160014997 40.08868915143022, -105.3513191753012 40.08868828549675, -105.3513223490436 40.08868744658238, -105.3513255344688 40.08868662749714, -105.3513287268686 40.08868583634074, -105.3513319239214 40.08868506230241, -105.3513351302921 40.08868431709655, -105.3513383424805 40.0886835926129, -105.3513415639967 40.08868289245849, -105.3513447889775 40.08868221662582, -105.3513480174328 40.08868156061168, -105.3513512563826 40.08868093163021, -105.3513544999716 40.08868032607136, -105.3513577481959 40.08867974573641, -105.3513610010635 40.08867918702274, -105.3513642573977 40.08867865173011, -105.3513675218851 40.08867814166592, -105.3513707898391 40.08867765502278, -105.351374061254 40.08867719450269, -105.3513773396651 40.0886767520043, -105.3513806180192 40.08867633562443, -105.3513839045245 40.08867594537359, -105.3513871886334 40.08867557853625, -105.3513904773837 40.08867523422086, -105.3513937731164 40.08867491423175, -105.3513970699648 40.08867462036259, -105.3514003655933 40.08867434810722, -105.3514036693692 40.08867410378213, -105.3514069719272 40.08867388017016, -105.3514102744283 40.08867368267664, -105.3514135815726 40.08867350680448, -105.3514168910031 40.08867335795441, -105.3514201968706 40.08867322981446, -105.3514235061931 40.08867313049941, -105.3514268213333 40.08867305190653, -105.3514301305556 40.08867299852394, -105.351433442068 40.0886729703622, -105.3514367535353 40.08867296291506, -105.3514400661123 40.08867298428987, -105.3514433751263 40.08867302637476, -105.3514466852559 40.08867309457963, -105.3514499941619 40.08867318619949, -105.3514533041913 40.08867330033678, -105.3514566094714 40.08867344148718, -105.3514599147025 40.08867360515348, -105.3514632187059 40.0886737940361, -105.3514665238309 40.08867400633676, -105.3514698206927 40.08867424384466, -105.3514731186721 40.08867450657194, -105.3514764154318 40.088674790913, -105.3514797051029 40.08867509956215, -105.3514829958916 40.08867543343067, -105.3514862807701 40.08867578890692, -105.3514895644133 40.088676173202, -105.351492839807 40.08867657639993, -105.351496113975 40.0886770039135, -105.3514993869117 40.08867745844471, -105.351502651593 40.08867793458061, -105.3515059103563 40.08867843592677, -105.351509167896 40.08867896068803, -105.3515124206924 40.0886795097604, -105.351515666404 40.08868008133964, -105.3515189050231 40.08868067902834, -105.3515221377321 40.08868129832474, -105.3515253680449 40.08868194103469, -105.3515285912691 40.08868260805275, -105.3515318050615 40.08868329847537, -105.3515350152831 40.08868401321057, -105.351538218422 40.08868474955204, -105.3515414121252 40.08868551109929, -105.351544601087 40.08868629605706, -105.3515477841348 40.08868710442384, -105.351550956584 40.08868793349171, -105.3515541207701 40.08868878776683, -105.3515572778715 40.0886896645488, -105.3517668144786 40.08874223138561, -105.3517712897696 40.08874356918196, -105.3517744433507 40.08874444955605, -105.3517776193232 40.08874527862216, -105.3517808059531 40.08874605996785, -105.3517840102742 40.08874679450269, -105.3517872311274 40.08874747592078, -105.3517904591143 40.08874811231585, -105.3517937024629 40.08874869469192, -105.3517969588061 40.08874923295311, -105.3518002199575 40.08874971718186, -105.3518034929369 40.08875015459225, -105.3518067765795 40.08875054158026, -105.3518100650282 40.08875087543642, -105.3518133582732 40.08875116066397, -105.3518166574911 40.0887513954631, -105.3518199626836 40.08875157893316, -105.3518232679801 40.08875171466919, -105.3518265780846 40.08875179637275, -105.3518298906361 40.08875183124597, -105.3518331997874 40.08875181207614, -105.351836513733 40.08875174517834, -105.3518398242724 40.08875162693941, -105.351843130231 40.08875145825852, -105.3518464339581 40.08875123733741, -105.3518497284121 40.08875096686898, -105.351853025319 40.08875064686825, -105.3518563106055 40.0887502782178, -105.3518595901426 40.08874985732261, -105.3518628604085 40.08874938597948, -105.3518661213993 40.0887488659896, -105.3518693707716 40.08874829644942, -105.3518726108767 40.08874767465998, -105.3518758393555 40.08874700692275, -105.3518790550472 40.08874628783244, -105.3518822532574 40.08874551918425, -105.3518854386629 40.08874470728863, -105.351889048104 40.08874410218412, -105.3518929562721 40.08874362985717, -105.3518968528061 40.08874311518499, -105.3519007388787 40.08874255816904, -105.3519046109777 40.0887419561029, -105.3519084726114 40.08874131349427, -105.3519123167499 40.08874062763223, -105.3519161433971 40.08873989671551, -105.3519199560572 40.08873912705313, -105.3519237430216 40.08873831052417, -105.3519268312332 40.0887368977742, -105.3521297321906 40.08870965310233, -105.3521353584751 40.08870744742942, -105.3521389316516 40.0887062604555, -105.35214258898 40.0887052005799, -105.352146323415 40.08870427229673, -105.3521501244089 40.08870347289052, -105.3521539755295 40.0887028095455, -105.352157868561 40.08870228585356, -105.3521617941243 40.08870190090214, -105.3521657357991 40.08870165647144, -105.3521696806946 40.08870154894242, -105.3521736287951 40.08870158552017, -105.3521775519679 40.0887017616655, -105.3521814513797 40.08870208008177, -105.3521853059354 40.08870253533819, -105.3521891109386 40.08870313013065, -105.3521928558477 40.08870385904178, -105.352196519546 40.08870472654777, -105.3522001044021 40.08870572184397, -105.3522035893053 40.08870684670466, -105.3522069672316 40.08870809571696, -105.3522102276295 40.08870946796671, -105.3522133623026 40.0887109580397, -105.3522163618855 40.08871255871862, -105.352219215825 40.08871426999018, -105.3522219182773 40.08871608284031, -105.3522244551869 40.08871799004599, -105.3522268277186 40.08871999521124, -105.3522290230108 40.08872208120746, -105.3522310328513 40.08872424982536, -105.3522328549184 40.08872649025432, -105.3522344833588 40.08872879798358, -105.352235912325 40.08873116580063, -105.3522371173096 40.08873353963548, -105.3522371383208 40.08873358379383, -105.3522381554927 40.08873604745254, -105.3522389661979 40.08873855137593, -105.3522395610806 40.08874108384367, -105.352239944849 40.08874363675592, -105.352240111642 40.08874620920469, -105.3522400626633 40.08874878678113, -105.3522397955776 40.08875136497907, -105.3522393150947 40.08875393479811, -105.3522386212323 40.08875648813249, -105.3522377175237 40.08875901778155, -105.3522366039846 40.08876151654021, -105.3522352829679 40.08876398080893, -105.3522337603739 40.088766393483, -105.3522320455755 40.08876875817698, -105.3522301350824 40.08877106227742, -105.3522280394693 40.08877329589072, -105.3522257645975 40.08877545992507, -105.3522233151827 40.08877754267818, -105.3522207041373 40.08877953786197, -105.3520968124044 40.08889266474071, -105.3520116371138 40.08897043866074, -105.3520098123099 40.08897269603393, -105.3505603079781 40.0901770108341, -105.3504353074468 40.09028001126072, -105.3501143193342 40.09054518814754, -105.3501030044008 40.09054683514306, -105.3488602740463 40.09072766624689, -105.3477420438011 40.0911531132065, -105.3477390155334 40.0912676727278, -105.3474905654169 40.09126545526282, -105.3473647716007 40.09190101374886, -105.3473760618604 40.09190161138967, -105.3477358623749 40.09192063968359, -105.3480775784211 40.09193222086797, -105.3480752065149 40.09194413324476, -105.3480493301681 40.09207408349272, -105.3480266875468 40.09218004037569, -105.3480266804584 40.09218321693172, -105.3480375101837 40.09218369231485, -105.3481173225404 40.09218719725872, -105.3481261729915 40.09218758627011, -105.3489303591214 40.092222907135, -105.3489536535213 40.09211378066907, -105.3489559026821 40.09210480060535, -105.3514657513061 40.0921898080533, -105.3517804351884 40.0920302926229, -105.351787338956 40.09204363909638, -105.3517906752359 40.09205008747434, -105.3517977978255 40.09205880042371, -105.3517996510527 40.09206238375607, -105.3518824545005 40.0921636816697, -105.351910777043 40.0921732918272, -105.3519259366955 40.09217843592464, -105.3515570003769 40.09260513227046, -105.3497571221252 40.09339322755047, -105.3493959159767 40.09370220408351, -105.3486197191432 40.0943661447682, -105.3485938374456 40.09439569602217, -105.348069812973 40.09441758316737, -105.3477279376078 40.09443076942602, -105.3454396442972 40.09442644731377, -105.3454145566375 40.09442639841708, -105.345406450746 40.09442645331113, -105.3428267490629 40.0944438410692, -105.3409616965941 40.09446173446745, -105.3385806165806 40.09448453710624, -105.338038240879 40.09448972631531, -105.3380597264658 40.09816320496651, -105.3380679597995 40.0999829026921, -105.3380680672347 40.10000677074521, -105.3380762485868 40.10181497668572, -105.333785237299 40.10179680139225, -105.3337278521754 40.10179655756251, -105.3333790260725 40.10179507305974, -105.3286884549565 40.10177504586694, -105.3286846007798 40.10277183683161, -105.3286845468612 40.10278580930287, -105.3286746087921 40.10535684263111, -105.3284493757341 40.1053164531441, -105.3279727853101 40.10523011210574, -105.3276491086925 40.105171102215, -105.3276308985215 40.10516778229127, -105.3241715938379 40.10453703921772, -105.3234060627616 40.10495320304896, -105.3230735027185 40.10513227377913, -105.3227056071184 40.10533036849009, -105.3219837186156 40.10571906357421, -105.319637666022 40.10559853352776, -105.3196340094476 40.10608717073401, -105.319633491415 40.10615609689889, -105.3196328620638 40.10624003657848, -105.3196324203565 40.10629918820222, -105.3196321462285 40.10633581324939, -105.3196164950359 40.10877483107916, -105.3196168898822 40.10882458490146, -105.31961907359 40.10910010517093, -105.3196088120404 40.11007871015286, -105.3195981387719 40.11109660301321, -105.3195867291031 40.1121868781655, -105.3195919018123 40.11259425855098, -105.3196073099071 40.11368319199543, -105.3196427185068 40.11618538426401, -105.3196367383125 40.11705363330758, -105.3196284268623 40.1182610946904, -105.3196215022174 40.11926648962921, -105.3196127185051 40.12054217426306, -105.3196075600112 40.12129130371403, -105.3196046445937 40.12171457176227, -105.3196039198489 40.12181983195664, -105.3195907343885 40.12373976980507, -105.3195996402118 40.1271990756839, -105.3196040280096 40.12890583323124, -105.3196047145051 40.12917274842658, -105.3196092372073 40.13093185442296, -105.3196129903288 40.13171254519044, -105.3196132716022 40.13177111142701, -105.3196444735669 40.13826003807267, -105.3196579593377 40.14029878475719, -105.3196943576456 40.14580098361585, -105.3197968729787 40.15181213863595, -105.3198011602762 40.15206351632045, -105.3198251871729 40.15347217831872, -105.3198628279538 40.15498735145348, -105.3198628290226 40.15498739108313, -105.3199164563804 40.15714591594258, -105.319937660156 40.15871453421283, -105.3199658798908 40.16081322516637, -105.319965912186 40.1608156596316, -105.3199470384802 40.16081628319009, -105.3102029758523 40.16093165450556, -105.3038011272576 40.16070799014367, -105.3005885640191 40.16059547665297, -105.2974028537698 40.16033230682975, -105.2914146194853 40.15983716419294, -105.2823830523645 40.1598017510487, -105.2801049068414 40.15978890188411, -105.2797491442513 40.15978689060664, -105.279438147905 40.15965574319318, -105.2789691635483 40.1595966967908, -105.2786951569143 40.15951033105921, -105.2783387574589 40.15923550989657, -105.2778164113579 40.15894098523002, -105.2776541607318 40.15889359876963, -105.2773907774724 40.1588709397186, -105.2764745864344 40.15871964151842, -105.2759892007606 40.15864821436704, -105.2754891981546 40.15864307329331, -105.2749458418215 40.15860031614835, -105.2738102982743 40.15848967626626, -105.2735568724613 40.15844106713092, -105.2738358838627 40.15824286475723, -105.2741450220795 40.15802193630074, -105.2742468856654 40.15794499676178, -105.2744588801126 40.15777987830076, -105.2746357770759 40.15761080747117, -105.2747344479813 40.15752711641187, -105.2748632858387 40.15741202752761, -105.2750305123632 40.15725926668, -105.2754225917291 40.15688255289814, -105.2758929495494 40.15644495979728, -105.2763959191594 40.15594704292194, -105.2766783327523 40.15567077309503, -105.2781341188324 40.15428111162556, -105.2785179368782 40.15391275991212, -105.2793160425854 40.15314803978234, -105.2794728569717 40.15300092477589, -105.280206041469 40.15228913282684, -105.280836947521 40.15167212428224, -105.2809808922424 40.1515200419104, -105.2811198405698 40.15136410597679, -105.2812509272502 40.15120513605844, -105.2813741570252 40.1510420334142, -105.2814298541274 40.15096500015037, -105.2815369705137 40.15080598366004, -105.2815880233071 40.15072702048, -105.281682976191 40.15056798085986, -105.2817290364374 40.15048406638984, -105.2817718698596 40.1504020677656, -105.2818528863331 40.15023806078776, -105.2819260558769 40.15006690229658, -105.2820759337992 40.1496241186037, -105.2821258875183 40.14944111154255, -105.2821458605589 40.14934808820088, -105.2822096587099 40.14892990318661, -105.2822448240156 40.14826998094643, -105.2822451208162 40.14784201323412, -105.2822360982994 40.14719606295897, -105.28224793464 40.14573292184287, -105.2822446240266 40.14535916374291, -105.2822411001326 40.1</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" t="n">
+        <v>7</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>Centennial MS</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>2205 Norwood Ave, Boulder, CO 80304</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>http://cem.bvsd.org/</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>Centennial Middle School</t>
         </is>
       </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
         <v>40.04506796264024</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>-105.2671472290834</v>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>http://cem.bvsd.org/</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>POINT (-105.2671472290834 40.04506796264024)</t>
         </is>
@@ -906,53 +929,56 @@
           <t>POLYGON ((-105.1470238512916 39.92761587682738, -105.1470244855684 39.92746831055086, -105.1470393599495 39.92524137222502, -105.147038645905 39.92502944310596, -105.147046321183 39.92186965993315, -105.1470470425149 39.92145044388781, -105.1470531994023 39.91775944655548, -105.1471032891195 39.91405210433869, -105.1473391472332 39.91405215140002, -105.147676653323 39.91405221810871, -105.1511818705786 39.9140528369392, -105.1532334610398 39.91405315098152, -105.1550121913589 39.91405339401757, -105.1560293437166 39.91405351953847, -105.156420131756 39.91405356845262, -105.1597894853714 39.91405668205347, -105.1653843869967 39.91413671650596, -105.1656197775234 39.91414007793439, -105.1657674166974 39.91414214035058, -105.1660335028282 39.91414237825769, -105.1660414667389 39.91414238424149, -105.1660433311038 39.91414238604561, -105.1660586296656 39.91414239888842, -105.1667719578876 39.91414299090538, -105.1672381230998 39.91414337611825, -105.1698987794962 39.91414553623513, -105.1703876457997 39.91414592693626, -105.1750099583544 39.91414955744559, -105.1797462276226 39.91415918540865, -105.183940205586 39.91416757726816, -105.184478826679 39.91416864003449, -105.1907538888507 39.91416762414558, -105.1921136011874 39.91416735873496, -105.1926978672329 39.91416724236024, -105.1933546555779 39.91416710270681, -105.1938763305775 39.91416699469512, -105.1953160550247 39.91416702303262, -105.1971047644128 39.91416703407202, -105.1985745597549 39.91416702150446, -105.1991893697619 39.91416701068361, -105.2006351177575 39.91416696934041, -105.2032744790532 39.91416684927634, -105.2062749820281 39.91414793981343, -105.2062611795562 39.91424142750945, -105.206223179592 39.91428442723124, -105.2055840142236 39.91454527467528, -105.2051264319463 39.91473201341331, -105.2047771484222 39.9148745542603, -105.2046181793619 39.91493942746109, -105.2044351788381 39.9150464284585, -105.2039238798093 39.91526835479848, -105.2036994329652 39.91536577400033, -105.2034951787843 39.91545442818257, -105.2032861789647 39.91558342752357, -105.2029610455153 39.91570919533338, -105.2026927027816 39.91582616438962, -105.2019980528428 39.91613227988852, -105.2013773094024 39.91640582131284, -105.2005472795797 39.91677157902036, -105.199981771958 39.9170207684681, -105.1988809443973 39.91750583145522, -105.1980761776685 39.9178604287125, -105.1977971773725 39.91800542846681, -105.1975931774295 39.91818342841723, -105.1971382584971 39.91865717884937, -105.1969171547176 39.91888743134161, -105.1963542841982 39.91947358440687, -105.1960461779453 39.91979442941913, -105.1960031773458 39.91985842861604, -105.1958741782275 39.91996042930643, -105.1957021779222 39.92016442965017, -105.1956491770346 39.92026642822356, -105.1956271775804 39.92046542890528, -105.1956074363542 39.92104863795893, -105.1955832718303 39.92176253388807, -105.1955539541311 39.92260363188283, -105.1955126848871 39.9235025188834, -105.1954828953945 39.92415135493398, -105.1954701680578 39.92442856826072, -105.1954277266185 39.92535293082255, -105.1953454862046 39.92714404290943, -105.1952731788288 39.9286614295662, -105.1921605878346 39.92866908889513, -105.1912021775201 39.92867143016532, -105.1900135071195 39.92868142556227, -105.1891882146993 39.92868835848437, -105.188280750955 39.92869597460466, -105.1874398749427 39.92870302575108, -105.1862427122102 39.92871305375947, -105.1860781767717 39.92871443107489, -105.1857881765031 39.92869343037078, -105.185584175611 39.92863943112477, -105.1853591757001 39.92871443082796, -105.1851551757211 39.92870443083596, -105.1848971762652 39.92868243096175, -105.1846711757492 39.92865043161049, -105.1843711756133 39.92868243090511, -105.1841991763519 39.92873643054561, -105.1838441764116 39.92869343178848, -105.1818511117197 39.92869648384348, -105.1784019212843 39.92870168376908, -105.1754136393685 39.92870368858787, -105.1754132357649 39.92870368835112, -105.1720714920114 39.92870144219746, -105.1691971726547 39.92869943197082, -105.1689792892025 39.92870089102008, -105.1684020970337 39.92870328012041, -105.1674080147692 39.92870738861864, -105.1666546602336 39.92871548911919, -105.1662549995615 39.92871799924519, -105.1662549969533 39.928718054178, -105.1662548834643 39.92871805655115, -105.1658309152665 39.92871792608083, -105.1660201718075 39.92872443199441, -105.1660261074718 39.92941559118069, -105.166031494597 39.93004289540448, -105.1660381193122 39.93081421993796, -105.1660467016499 39.93181341576487, -105.166056515896 39.93295616617159, -105.1660647969186 39.93392020542746, -105.1660503453821 39.93509378069637, -105.1660326082687 39.93546115149928, -105.166003329776 39.93598570561753, -105.1660033259753 39.93598576505014, -105.1659873030505 39.93626023394562, -105.1659872391716 39.93626133344856, -105.1659871764604 39.93626243299418, -105.1659749417947 39.93647953441914, -105.1659674910183 39.93676935921954, -105.1659572086535 39.93679429393993, -105.1659335404815 39.93685168841169, -105.1658977131763 39.93693353750162, -105.1658600197634 39.93701487859802, -105.1658204732303 39.93709568651817, -105.1657790841984 39.93717594147653, -105.1657358633377 39.93725561378023, -105.1657309930949 39.93726410639616, -105.1657314686866 39.93778700123453, -105.1657621735393 39.94010243415755, -105.1664371723441 39.93963643311929, -105.1669986961005 39.93946070845881, -105.1676961733447 39.939242433397, -105.1693161728545 39.9392404329576, -105.1693041740566 39.94127343310699, -105.1683021747413 39.94321143381614, -105.1664695916308 39.9432063625764, -105.165775173689 39.94320443381061, -105.1657468007817 39.94732775484253, -105.1657421736448 39.94800015855595, -105.1657381741117 39.9485814352014, -105.1663871736281 39.94844043457117, -105.1685594742733 39.94796687370324, -105.1696508514793 39.94772963358609, -105.1696509264492 39.94772961758919, -105.1699691748952 39.94766043485847, -105.1703601751532 39.94872843443577, -105.1702541750417 39.94875143479771, -105.1705001743236 39.94877043461553, -105.1706751750825 39.94883443513947, -105.1708731754645 39.94899843388744, -105.1709821753827 39.94931543455208, -105.1710701754516 39.9496574351276, -105.1713521750109 39.95026343503369, -105.171721175489 39.95026543539605, -105.171721175293 39.95049343486586, -105.1732691751886 39.95049443510379, -105.1737901766914 39.9502784352506, -105.1765441762881 39.95029543509211, -105.1765421764602 39.95049343511674, -105.1777091771583 39.95048843468322, -105.1776542787933 39.95210731667019, -105.1776527450811 39.9521525489294, -105.1776503630244 39.95222278293825, -105.1776494915453 39.95224847092626, -105.1776425915952 39.95225318368962, -105.1776474058934 39.95230996305708, -105.1774426914856 39.95247925641739, -105.1774296504487 39.95249004043743, -105.1774078670555 39.95259250878293, -105.177290609483 39.95332415578926, -105.1772734159885 39.95342058182205, -105.1772613072263 39.95349823162613, -105.1772507335152 39.95357595507921, -105.1772416938306 39.95365372245707, -105.1772370166073 39.95373008711738, -105.1772414131593 39.9538026430856, -105.1772475047739 39.95387510202673, -105.1772552845585 39.95394743780206, -105.1772648208975 39.95401954432493, -105.1772767414146 39.95409060825552, -105.177290313959 39.95416152369918, -105.1773055304672 39.95423226451359, -105.177322394536 39.95430281359553, -105.1773408910587 39.95437314928622, -105.1773575396614 39.95443111644111, -105.1773610213213 39.95444324817128, -105.1773827784174 39.95451308681337, -105.1774061518873 39.95458265077165, -105.1774311360077 39.95465191391003, -105.1774577273785 39.95472085370143, -105.1774859155525 39.95478945300295, -105.1775156877714 39.95485768836055, -105.1775470406094 39.95492554265083, -105.1775799624868 39.95499299062175, -105.1776144429687 39.95506001242811, -105.177648397834 39.95512435329022, -105.1789848485213 39.95766031512748, -105.1789897484092 39.957669611876, -105.178782063112 39.95766574209604, -105.1786071533748 39.95766248214333, -105.1753791767883 39.95758643523679, -105.1753811772785 39.95817043580769, -105.1770375813809 39.95819321332797, -105.1770375221035 39.95820029775011, -105.1770363078439 39.95835052526509, -105.1770358705875 39.9584045834283, -105.1770275234974 39.95943772098945, -105.1767015637337 39.95943301604639, -105.1756586713841 39.95941795615627, -105.1752731802447 39.95941238698667, -105.1751673978478 39.95941085853762, -105.1751515536733 39.96066900909348, -105.1751530130947 39.96066902761821, -105.1752660781159 39.9606704126778, -105.1753197877496 39.96067107019252, -105.1760332411225 39.96066191903108, -105.1780562582363 39.96063407794388, -105.1780563504867 39.96064057285627, -105.1780617120378 39.96101742820876, -105.1780795667658 39.96212243842648, -105.1779603294206 39.96230169761951, -105.1777988506388 39.9622247658564, -105.1777786369145 39.96221513532904, -105.1777779996259 39.96221599908061, -105.1777729991336 39.96222499799526, -105.175195000182 39.96134899884276, -105.1750629987647 39.96129699910314, -105.1718929991997 39.96004699882172, -105.16867899997 39.95862899864169, -105.1677549991503 39.95786999907147, -105.1672029990481 39.95741599921722, -105.1668249995467 39.95710599849211, -105.1661219997786 39.95695499897838, -105.1660599995567 39.9569419984156, -105.1660659997773 39.95698699837227, -105.1661089994848 39.95726499912967, -105.1661250002072 39.95739999859541, -105.1663429988309 39.95789999829524, -105.1663939993887 39.95801599875833, -105.1663729998672 39.95804199855646, -105.1663260779203 39.95809453148716, -105.166280999977 39.95814499912188, -105.1658829843055 39.95798883313223, -105.1657049993032 39.95791899851163, -105.1655459994386 39.95785699862255, -105.1640439992191 39.95727199887524, -105.1635449998441 39.95706699912397, -105.163260000118 39.95693999941128, -105.1629539988249 39.95680199904174, -105.1626729999983 39.95667199866357, -105.1623139998591 39.95649799874107, -105.162090999951 39.95638499933245, -105.1615179991773 39.95607999946219, -105.1612710001578 39.9559439989421, -105.1611820283237 39.95589271854974, -105.1609239990875 39.95574399904351, -105.1605739993225 39.95553199876508, -105.1605070003541 39.955487998663, -105.160507601197 39.95548743481859, -105.160553485336 39.95544433019448, -105.1605729992732 39.95542599889634, -105.1605708372656 39.95542490543037, -105.1604879993213 39.95538299862599, -105.1603829998639 39.95530799832515, -105.1594730000078 39.95466099895394, -105.1568089995898 39.95264699943566, -105.1564621234448 39.95235626096443, -105.155603998905 39.95163699829544, -105.154634999516 39.95082499893148, -105.1545469991415 39.95082499900798, -105.1543240000297 39.95082499846626, -105.1538259995572 39.95043899936822, -105.1526479997484 39.94953399844792, -105.1520270002295 39.94907999894239, -105.1510029999227 39.9483689989986, -105.1505859991704 39.94808599920534, -105.1502339997436 39.94785999905235, -105.1493769991665 39.94730899849206, -105.1487869967502 39.94692837327946, -105.1483709999483 39.94665999878806, -105.1479109994562 39.94636399921564, -105.1470224473384 39.94578389403245, -105.1469689981003 39.94574899894534, -105.1465979998178 39.94550799907834, -105.1444109992605 39.94408999827592, -105.1438049994702 39.94369699936311, -105.1436849993157 39.94361699895295, -105.1435829995349 39.94355199879121, -105.1429179998172 39.94312999953807, -105.1415170000054 39.9422179981579, -105.141208999877 39.9420169995477, -105.1409599991531 39.94185799904378, -105.1405889992587 39.94161999863454, -105.1400129996827 39.94124299866457, -105.1380069982713 39.93995099908016, -105.1376659994644 39.93973899908963, -105.1376101742235 39.93970626003536, -105.1376101662146 39.93970556469871, -105.1376101533659 39.93970445864476, -105.1376092642489 39.9396308257882, -105.1376082126364 39.93954372301226, -105.1376032162488 39.9391298924964, -105.1376002640181 39.93888552805745, -105.1376000835919 39.93887058729946, -105.1375934532797 39.93832156847123, -105.1375901359232 39.9380468199151, -105.137587250081 39.93780781910959, -105.13758090158 39.93728200849577, -105.1375804232843 39.93724229677402, -105.1375796290724 39.93717680439059, -105.1375669599118 39.93612418884327, -105.1375702679211 39.93577373335888, -105.137586602701 39.93404371593252, -105.1375954953071 39.9331018756593, -105.1375976976845 39.93286861358298, -105.1376017361011 39.93244089603266, -105.1376081834016 39.93175509745066, -105.137605376672 39.93128768051638, -105.1376034417805 39.93096545410189, -105.1376029272597 39.93086976333272, -105.1376238948989 39.93013023535828, -105.1376321063676 39.92984063493733, -105.1376407559584 39.92953592366019, -105.1376599462519 39.92897351444855, -105.1376612209119 39.92893150972372, -105.1376618506932 39.92891071719205, -105.138619806365 39.92890769866385, -105.1386248219273 39.92890763964525, -105.1391145604889 39.92890607867842, -105.1423066729647 39.92889593602464, -105.1435950820782 39.92889181774414, -105.1435958776075 39.92889181480177, -105.1436712912503 39.92889157348318, -105.1470184689167 39.92887114754381, -105.1470187184292 39.92881293486509, -105.1470188937999 39.92877200297731, -105.1470238512916 39.92761587682738), (-105.169197172132 39.92863411235809, -105.1691864470017 39.92863672319584, -105.1691971726547 39.92869943197082, -105.169197172132 39.92863411235809))</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>Eldorado K8</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>3351 S Indiana St, Superior, CO 80027</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>http://el8.bvsd.org/</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>Eldorado K-8 School</t>
         </is>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>39.921698179021</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>-105.161197194222</v>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>http://el8.bvsd.org/</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>POINT (-105.161197194222 39.921698179021)</t>
         </is>
@@ -972,53 +998,56 @@
           <t>POLYGON ((-105.0553096519419 40.02197149228508, -105.0553161721816 40.02152862889884, -105.0553212996101 40.02118039422834, -105.0554144707321 40.01485168306485, -105.0554156695371 40.01476968888103, -105.055416567316 40.01468733327196, -105.0554222037575 40.01418812084223, -105.0554725655142 40.00972422301597, -105.0554720783693 40.0096054501175, -105.0554763115184 40.00921806165778, -105.0554777210193 40.00908880877136, -105.0554783834164 40.00902816353494, -105.055478575345 40.00901219736176, -105.0554871758176 40.00854380587615, -105.0554879813757 40.00814947087598, -105.055488010625 40.00814642135131, -105.0554881852632 40.00812897442378, -105.0554887295674 40.00808087222916, -105.0554920362152 40.00777826834898, -105.0554948489156 40.00752250682681, -105.055531007058 40.00563956685976, -105.0555401553612 40.00564045054492, -105.0555902120115 40.00566690495083, -105.0556471557209 40.00567245091049, -105.0557201558533 40.00567145055776, -105.0558361548308 40.00567645117783, -105.0559061543596 40.00567545085779, -105.0559701557746 40.00568045011807, -105.0561221547891 40.00567145049642, -105.0561661556522 40.00563345075564, -105.0561531550697 40.0055424501676, -105.056107155146 40.00544945007372, -105.0571341561924 40.00545445010541, -105.0604611556923 40.00038144912251, -105.0640551537651 40.00037580618888, -105.0678619251848 40.00037085969463, -105.0744775635209 40.00036260693889, -105.074477999321 40.00046599897158, -105.0744799997885 40.0007489983894, -105.0744820000614 40.00248399837474, -105.074475000093 40.00379499887224, -105.0744809997915 40.00389299933561, -105.0744759999931 40.00412799915949, -105.0744768152457 40.00418672611349, -105.0744770006211 40.00419999892615, -105.074476815134 40.00421095567354, -105.0744759988608 40.00425899837897, -105.0744770000379 40.00485699808893, -105.0744799998352 40.00548099818882, -105.0744800693377 40.00549913954058, -105.0744829989317 40.00626690809695, -105.0744829995353 40.0062669990658, -105.0744834354184 40.00666768629058, -105.0744840001084 40.00718699899353, -105.0744840001105 40.00754717649394, -105.0744840004529 40.00754899853014, -105.0744840014802 40.00754920928831, -105.0744959994806 40.00913899920532, -105.0744850002892 40.01025499937742, -105.0744939996588 40.01117199953493, -105.0744939994117 40.01312199935634, -105.0744879997328 40.01486699832747, -105.0750330000281 40.01486599880874, -105.0776729999707 40.01487699919728, -105.0778080003735 40.01487099884424, -105.0780740000252 40.01483699883885, -105.0785220001667 40.0147389989032, -105.0787519998548 40.01470499815898, -105.0790640003765 40.0146869983785, -105.0798880004663 40.01470099918091, -105.0827519996697 40.0147379995101, -105.083827279062 40.01474776707985, -105.0838636006166 40.01474809629242, -105.0838678605798 40.01474813508104, -105.0839630017275 40.01474899892437, -105.084275999784 40.01475199921421, -105.084343261355 40.01475098794224, -105.0844090000323 40.01474999906352, -105.0863749999974 40.01472599885857, -105.0865649991523 40.01472399889266, -105.0905288819658 40.01468199225995, -105.0905289991035 40.0146819917752, -105.0905557415763 40.01468189398261, -105.0924409249201 40.01467444931598, -105.0932924249816 40.01467107691634, -105.0933119998438 40.01467099914053, -105.0940020010792 40.01467199918716, -105.0968210984977 40.01464899904126, -105.0968081659261 40.01339944902477, -105.0977161660674 40.01340144824596, -105.097693165477 40.01108044794793, -105.1029281665798 40.01109144817353, -105.1029321674492 40.01426744896852, -105.1029350211734 40.01499712229778, -105.1029381666813 40.01697244858164, -105.1029531677396 40.0182424491116, -105.1029258020212 40.01922928731726, -105.1028801685531 40.02039944897465, -105.1028411684982 40.02101744933578, -105.1027191685341 40.0229774492492, -105.1026901679704 40.02391744893649, -105.102681714784 40.02523098211869, -105.1026813585937 40.02624327690542, -105.1026851686352 40.02731645051675, -105.1026703866881 40.0282598185744, -105.1026821685567 40.02903745095252, -105.1027065698951 40.02953569354239, -105.1025462936187 40.0295350594423, -105.1025509999655 40.02982099987915, -105.1026589993872 40.0325789998223, -105.1028159251721 40.03659410284713, -105.1028159996535 40.03659599988478, -105.1028159808093 40.03659641862485, -105.1026950932294 40.03923308897296, -105.1026695167741 40.03979091557985, -105.102684106142 40.03979099374556, -105.1026843791355 40.04070640471347, -105.1026843795041 40.04070875362413, -105.1026844241735 40.04085566869285, -105.1026853227765 40.04386122510869, -105.1026792879808 40.04699933304118, -105.1026468422424 40.04711176082813, -105.1026515547724 40.04751510558266, -105.1026531716483 40.0476534526228, -105.1026544039104 40.04765355413717, -105.1030171704752 40.04768345267631, -105.1033391709822 40.04790545288033, -105.1037471714223 40.0480454529342, -105.1041869090785 40.04810254797782, -105.1051951720775 40.0482334531068, -105.1056231709406 40.0481744531596, -105.1064479966728 40.0482222769794, -105.1072881721325 40.04830245271919, -105.1075741724027 40.04816445209948, -105.1084266880845 40.04775137397073, -105.109125173029 40.04741245282467, -105.1096111728036 40.0474164516294, -105.1100331727537 40.04752645257917, -105.1103231729248 40.04751845193728, -105.1107256413342 40.047267544397, -105.1111171727025 40.04702345167325, -105.1111851729639 40.04692845194887, -105.1112241729621 40.04694545172396, -105.111576173255 40.04658445258669, -105.1116441732981 40.04653845179544, -105.1117501733669 40.04650145208792, -105.1118461736203 40.04649345213979, -105.1123371190536 40.04651893042601, -105.1123366900865 40.04658012665188, -105.1123366731379 40.04658248811084, -105.1123354147434 40.04676250668771, -105.1123309979452 40.04739433331647, -105.112330888596 40.04741005387065, -105.1123302681899 40.04749872120584, -105.1123296974318 40.0475803086633, -105.1123229001954 40.04855248897933, -105.1123218382726 40.04870461756659, -105.112392173119 40.04869545288748, -105.1127817580233 40.04864540026167, -105.1141782671779 40.04846883077132, -105.1151371742824 40.04834545259219, -105.1159511368379 40.04820936852636, -105.1180384926233 40.04779473006271, -105.1220411513055 40.04703446196407, -105.1244748378258 40.0465721293676, -105.1281644085359 40.04587100599928, -105.1311570490046 40.04532707446116, -105.1311558744463 40.04547805719804, -105.1311661736642 40.04661103317486, -105.1311759744774 40.04744011431053, -105.1311790599092 40.04779398012801, -105.1311841143478 40.04824612972813, -105.1311891001171 40.04930496819956, -105.1311931055019 40.05054498601775, -105.131205846102 40.05096312075745, -105.1312107819624 40.05257722664825, -105.131211005441 40.05265005956795, -105.1312209170923 40.05372291390245, -105.131216169747 40.05413797270889, -105.1312141679244 40.05437597462971, -105.1312034302793 40.05463055486094, -105.1312059997651 40.05463199871355, -105.1312151333568 40.05463829014283, -105.1312051341252 40.0549272902714, -105.1312061330529 40.05519229072108, -105.131207134803 40.05564929051275, -105.1312051349296 40.05727829088557, -105.1312131325501 40.05874928993782, -105.1312141338369 40.05887029037866, -105.131228134939 40.05974929071716, -105.1312201340746 40.06002129004976, -105.1312141343774 40.06023929086055, -105.1312251347958 40.06072029049393, -105.1312291345053 40.06187129073018, -105.131234134076 40.06223529081105, -105.131220135557 40.06361729016729, -105.1312161352539 40.06423529025914, -105.1312261348082 40.06486429056906, -105.1312181355008 40.06555429029728, -105.1312311345578 40.06758328902276, -105.1312421349654 40.06840629078298, -105.1312471352586 40.06877329065517, -105.1312571353166 40.07052429035368, -105.1312561355187 40.07114629121654, -105.131250135106 40.07142728958371, -105.1312471358889 40.07157529118987, -105.1312769801043 40.07280485163446, -105.1312771363536 40.07281128908546, -105.1313291354456 40.07367829108345, -105.1313121353605 40.07453929131646, -105.1313161362929 40.07558629064913, -105.131364137045 40.08008229048873, -105.1314061367591 40.0827892910741, -105.1314141381591 40.08325728973681, -105.1314231385745 40.08373028926654, -105.1314680581192 40.08735891798165, -105.1314681373808 40.08736529032833, -105.1314686920482 40.08736528489368, -105.1315023083889 40.0879120286511, -105.1315123076631 40.08860202899108, -105.1315573093293 40.09073602900505, -105.131565308569 40.09121302826923, -105.1315713090677 40.09267102844738, -105.1315353089882 40.09441602918015, -105.1315413093822 40.09489902827075, -105.1315033084531 40.09835802848521, -105.13149630911 40.09849502893818, -105.1314753089459 40.09960702888224, -105.1314743099729 40.09982802847355, -105.1314613102898 40.1017110280084, -105.1314603103063 40.10285102851227, -105.1313783109039 40.10663902806576, -105.1313063115642 40.10894602876141, -105.1312713110947 40.10989302815075, -105.1312733098291 40.11046202797889, -105.1312403110973 40.11140002800153, -105.1312113114617 40.11250802867715, -105.1311973097867 40.11310902852121, -105.1311303117171 40.114313029054, -105.1310553120431 40.11535402919674, -105.1310183122412 40.11621802952327, -105.1310173486831 40.11641334503174, -105.1310173105552 40.11642102922118, -105.1310173108496 40.11649802904655, -105.1310243109556 40.11903302886184, -105.131030312504 40.11993502837323, -105.1310413121898 40.12134002807184, -105.1310483121341 40.12350602835088, -105.1310553132711 40.12555802887955, -105.1310573131 40.12712102857881, -105.1310483145869 40.12882902900039, -105.131019817435 40.13074388165322, -105.1308018207651 40.13073588184478, -105.129739962766 40.13072788110647, -105.1295199780874 40.13072688132058, -105.125637981124 40.13071087844324, -105.1214389852497 40.1306978758488, -105.1214388421045 40.13069787537972, -105.1214287020073 40.13069788718315, -105.1196690057948 40.13069987439082, -105.1190837455796 40.13069590702754, -105.1190789667365 40.13069587415787, -105.1190737172402 40.13069586675535, -105.1167582823744 40.13069277850736, -105.1167491843696 40.13166446387874, -105.1155191846595 40.13164146329787, -105.1152464520673 40.13162554514241, -105.1150500767831 40.13162358771766, -105.1146592764502 40.13161717097666, -105.1142691989206 40.13161076343259, -105.1138787565874 40.13160434794801, -105.1134884683498 40.13159766957149, -105.1130752163228 40.13171876581113, -105.1126460873139 40.13184417366759, -105.1122248807698 40.13196726034626, -105.1122250359624 40.13198450641528, -105.1121931826917 40.1319974642461, -105.1119871837674 40.13205846401782, -105.1119826842302 40.13221195301501, -105.1119769681384 40.13240697386129, -105.1119701840193 40.13263846362696, -105.1115905511339 40.13264209640875, -105.111021497991 40.13263928746463, -105.1109074261621 40.13263860431368, -105.110591834876 40.13263671418122, -105.1103350195741 40.13263517546018, -105.1098582235746 40.1326323161728, -105.1096519310758 40.13263086368207, -105.1093701834689 40.13263246468068, -105.1093585944797 40.13263279385802, -105.1093205768746 40.13268270513078, -105.1092647735506 40.13273806278027, -105.1092018368701 40.13278836166751, -105.1091328252846 40.13283461228306, -105.1090587413161 40.13287489693305, -105.1089796055062 40.13291013523579, -105.1088964020049 40.13293936322003, -105.1087220040101 40.13297863883014, -105.1086315304633 40.13298881317525, -105.1085152097078 40.13299386796137, -105.1055770144187 40.13300287849541, -105.1055759857053 40.13312511863367, -105.1055759631424 40.13312799972009, -105.1044939964566 40.13312987928641, -105.1041803847008 40.13315484466681, -105.1025130798614 40.13316287747433, -105.1025130341002 40.13316287731691, -105.1024960005596 40.13413300172339, -105.100395113552 40.13418487869186, -105.0960260840791 40.13426087793793, -105.094924071347 40.13427687757695, -105.0944350199997 40.134278878763, -105.0944050049201 40.13427896522876, -105.0940880142722 40.13427987836944, -105.0932020045514 40.13427787787717, -105.0930212415033 40.13428686643668, -105.0927490541487 40.13428987731798, -105.0920430472559 40.13429687652557, -105.0905391301851 40.13433687298826, -105.0899250393446 40.13434187663415, -105.0887041365292 40.13437587163286, -105.0879403055598 40.13442385884984, -105.0846750309919 40.13445787330612, -105.0832755753651 40.13446682896835, -105.0831630652203 40.13445687173049, -105.0799831751011 40.13457186759719, -105.077656234461 40.13468386293215, -105.0762711360049 40.13472286783558, -105.0745131984398 40.13479486487819, -105.0742413915201 40.13481684621029, -105.0742440761428 40.13984499868648, -105.0737770801883 40.13984989482434, -105.0728341139191 40.13987189343821, -105.0652349113323 40.13998458559128, -105.0651172543858 40.13995483397098, -105.0650172912994 40.139897965545, -105.064944699213 40.13982145163131, -105.0649318121612 40.13979936609553, -105.0649223983107 40.13978009284535, -105.0649012584268 40.13969700518675, -105.0649496601588 40.13851303311695, -105.0649247890964 40.13837338792121, -105.0648822428967 40.13829711858007, -105.0647902892207 40.13821288423826, -105.0647026837377 40.13816640688852, -105.0646163718572 40.1381387740668, -105.0644970736709 40.13812287925889, -105.0630970281733 40.13814387787887, -105.0623920537045 40.13814787912667, -105.0570841697421 40.13820687462603, -105.055393108424 40.1382658753683, -105.0553734627153 40.13826344007112, -105.055373432471 40.13824238373312, -105.0553733597693 40.13819028553863, -105.0553632754563 40.13104290372788, -105.055364943468 40.13045509249489, -105.0553838251001 40.1238012151376, -105.0554011703724 40.12074599216336, -105.0554021173245 40.12057908303889, -105.0554247936661 40.11658455689023, -105.0554252479113 40.11650224198018, -105.0554253132042 40.11642002734557, -105.0554270937738 40.11409009148291, -105.0554307971221 40.10923987562791, -105.0554303061645 40.10813983466713, -105.0554291707098 40.1055942872819, -105.0554283485588 40.10374754276933, -105.0554275913097 40.10204463836374, -105.0554275553799 40.10196193683294, -105.0554275083234 40.10188004134116, -105.0554258013926 40.0987667225997, -105.0554241217421 40.09570511636053, -105.0554235981428 40.09475507605646, -105.0554115838102 40.0876056618749, -105.0554116626656 40.08751615800497, -105.0554120967009 40.08737439782387, -105.0554338942331 40.0802760293785, -105.0554359155676 40.07955726421665, -105.0554393436516 40.07833891985845, -105.0554454483656 40.07616858804563, -105.0554543197811 40.07301208584704, -105.0554524783247 40.07097781636424, -105.0554510471109 40.06937851290341, -105.0554511248211 40.06936354972414, -105.0554693891445 40.06582907619643, -105.0554580642362 40.05842399669204, -105.0554542737668 40.05209778695296, -105.0554563122968 40.05151114401765, -105.0554564529153 40.05147054475928, -105.0554575802229 40.05114448977547, -105.0554617276261 40.04898736880429, -105.0554635752588 40.04802681178261, -105.0554639797832 40.04781621901886, -105.0554654855536 40.04674097808282, -105.0554656988988 40.04658897680252, -105.0554665087686 40.04601063733477, -105.0554691137273 40.04415188527337, -105.0554694939043 40.04386956126768, -105.0554628576467 40.04251422452845, -105.0554558612454 40.04108497102352, -105.0554471109753 40.03929767112174, -105.0554415609123 40.03816398170832, -105.0554342598844 40.03667252329386, -105.0554338426251 40.03658900636015, -105.0554331606792 40.03650690784292, -105.0554302318307 40.03615562906905, -105.0554208607084 40.03503174441796, -105.0554056000837 40.03320149646342, -105.0553923068964 40.03160700942662, -105.0553916639802 40.0315298997633, -105.0553898967095 40.03131800400271, -105.0553734970732 40.02935099038166, -105.0553731474197 40.02930921737802, -105.0553704800526 40.02900128894915, -105.0553096519419 40.02197149228508))</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>Erie MS</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>650 Main St, Erie, CO 80516</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>https://ems.svvsd.org/</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>Erie Middle School</t>
         </is>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>40.05101707648438</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>-105.0529688258069</v>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>https://ems.svvsd.org/</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>POINT (-105.0529688258069 40.05101707648438)</t>
         </is>
@@ -1038,53 +1067,56 @@
           <t xml:space="preserve">POLYGON ((-105.348856789205 40.03820800949617, -105.3487067298522 40.03821232955207, -105.3477914050935 40.03821638893005, -105.3474817926258 40.03821722291953, -105.3468614299469 40.03822512838605, -105.3450104181683 40.03829153532944, -105.3450179171597 40.03868015700185, -105.3460405482716 40.0386437539853, -105.3461031168401 40.03898908284479, -105.3453268746833 40.03901948006025, -105.3452802180325 40.03911018389644, -105.345271517239 40.03912433761808, -105.3452452833364 40.03915814157467, -105.3452130574343 40.03918918870853, -105.3451781010895 40.03921517142847, -105.3451448277192 40.03923480953083, -105.3451089087152 40.03925177274996, -105.3450576487383 40.03926988529709, -105.3450069768098 40.03928187960952, -105.344961760615 40.03928819273935, -105.3449089508063 40.03929064807553, -105.3448494533033 40.03928712489946, -105.3447950264157 40.03927776511058, -105.3447425347318 40.03926247803446, -105.3446092328436 40.03929490292018, -105.3445765512982 40.03930516501039, -105.344539877266 40.03932120387111, -105.3444846960346 40.03935795158987, -105.3444426165169 40.03940586426801, -105.344423128196 40.03944725428348, -105.3444160073502 40.03949552391189, -105.3444275517575 40.03955601888752, -105.3444731759986 40.03968833424123, -105.3444965572211 40.03975520013649, -105.3445205624492 40.03981616221999, -105.3445578084813 40.03989778498795, -105.3446376646379 40.04003968424905, -105.3447276531524 40.04016680845205, -105.344795157412 40.04024733253993, -105.3448549167217 40.04031071675156, -105.3448484541613 40.04055274004725, -105.3448541691076 40.0406499600528, -105.3448674149786 40.04072253855343, -105.3448882399842 40.04079357632659, -105.3449216829459 40.04087332410908, -105.3449704426995 40.04095811087339, -105.3446364322639 40.04102959990085, -105.3446007162516 40.04104340376086, -105.3445703711054 40.04106466860651, -105.3445493695219 40.04108914063158, -105.3445380231417 40.04111119661664, -105.3445343361066 40.04112275146215, -105.3445311011553 40.04114724832418, -105.3445392814093 40.04121096396332, -105.3419896303343 40.04121709476975, -105.3422755387781 40.04337513429397, -105.3465131388534 40.04343423722576, -105.3501117189857 40.04341854173573, -105.3509604583964 40.04341720319611, -105.351061685705 40.04341728708226, -105.3544519058515 40.04524596662837, -105.355091416096 40.04556889885021, -105.3559880623356 40.04583041298836, -105.3567595372542 40.04599519383382, -105.3579301381531 40.04606086270712, -105.3600970053326 40.04564174739976, -105.3606742433043 40.0468628855719, -105.3621557651074 40.04965424089358, -105.3639920692559 40.05282887853546, -105.3641080684391 40.05289587827868, -105.3797250233372 40.06069585746808, -105.3900870057658 40.06584284178945, -105.3912861257657 40.07092499987773, -105.3914749402041 40.07083101793872, -105.3920811145549 40.07050298994405, -105.3925910222121 40.07026600808574, -105.3937980289077 40.06981087854467, -105.3940840170989 40.06972192263695, -105.3946001680771 40.06959803960483, -105.3947989293112 40.06953590537677, -105.3948919023455 40.06948987079981, -105.394964868722 40.06944107368035, -105.395060070696 40.06933903984681, -105.3952621280964 40.06899113614033, -105.3955138612367 40.0686358647477, -105.3957139250865 40.06842109885081, -105.3959568633348 40.06820609746421, -105.3961321294408 40.06808409464642, -105.3965509251752 40.06782505281563, -105.3967590498075 40.06770994229892, -105.3970411697905 40.06757211203932, -105.3973890575354 40.06741704540752, -105.3979349933502 40.06719105257222, -105.3989681210101 40.0668320704148, -105.3993949116376 40.0667119298152, -105.4001279456997 40.06656295502956, -105.400853036919 40.06646804795456, -105.401574842874 40.0664209000962, -105.4031081030495 40.06634588138125, -105.4033760986539 40.06632908658128, -105.4036001268962 40.06632597936235, -105.4039354886404 40.06629270998662, -105.4039684530764 40.06628998415017, -105.4041299199174 40.06627663574243, -105.4042548603106 40.06623819278212, -105.4043540234276 40.06619888982722, -105.4044344048956 40.06614050729836, -105.4045148499365 40.06603666564356, -105.4047389400583 40.06573287074457, -105.4047829657393 40.06567608181868, -105.4049212700939 40.06553693910522, -105.4051253441126 40.06542981958253, -105.4053520055905 40.06532884620861, -105.4056105037759 40.06528097971057, -105.4058260373516 40.06528440260607, -105.4060288655031 40.0653072983951, -105.4061852130406 40.0653236615075, -105.4063458769007 40.0652750842445, -105.4065446697525 40.06515834714913, -105.406676242775 40.06503075664818, -105.4068038590952 40.06490576206056, -105.4069109925564 40.06477432561354, -105.4072568691801 40.06434998263192, -105.4075520798087 40.0638858471748, -105.4076144271041 40.06375352486941, -105.4076986539011 40.06358322723908, -105.4077424376704 40.06351872295893, -105.4078528920384 40.06344490160728, -105.407979736912 40.06339954278057, -105.4081488124669 40.06337694790046, -105.4081993022081 40.06354259319305, -105.4082583191018 40.06365304293325, -105.4083384376527 40.06378623987003, -105.4086252315054 40.0642215866695, -105.4087813728473 40.06439056211295, -105.4089458907069 40.06461799217212, -105.4091018907903 40.06489412393282, -105.4092368182365 40.06512802479963, -105.4093225643208 40.06526853688391, -105.409504095397 40.06548498442051, -105.4098262734777 40.06579167091841, -105.4100664892069 40.06598563197285, -105.4102657157319 40.06612999100079, -105.4104355939177 40.0662923524043, -105.4104999331161 40.06642759351949, -105.4105231868886 40.06658533416806, -105.4111090704269 40.0668027547869, -105.4113230710384 40.06683775452498, -105.4123600762381 40.06670774877939, -105.4126030773382 40.06671874798173, -105.4127710765582 40.06675374711786, -105.4135470770253 40.06717174623984, -105.4143210780151 40.06733974415099, -105.4147190788605 40.06742674212688, -105.4148260788204 40.06747274227973, -105.4149630792546 40.06748474171021, -105.4150690789331 40.06755474126348, -105.4153730784282 40.06789174239631, -105.4157380779817 40.06803174076535, -105.4159660790526 40.06803073976152, -105.417218086706 40.06765573284537, -105.4192990814895 40.06934373178217, -105.4204860820148 40.06988972973171, -105.4213540837626 40.07010972666475, -105.4217650863564 40.07012072544669, -105.4219790865552 40.07007372430561, -105.4224070903935 40.06972272033761, -105.4231560979392 40.06916171416628, -105.4234760999032 40.06905671176163, -105.4241311017381 40.06905570945187, -105.4263101075327 40.06940170123508, -105.4276811134631 40.06938769518695, -105.4296940698257 40.06907550496865, -105.4296848584402 40.06784624750029, -105.429671773314 40.0661001537952, -105.4296579769224 40.06425909176156, -105.4296368548572 40.06155809847662, -105.4296177827629 40.05856372052644, -105.4298099905968 40.05861586964885, -105.430018256796 40.0586642013499, -105.4304940701495 40.0588180812849, -105.4308276096539 40.05895208149089, -105.4313349350903 40.05921427306927, -105.4316590735046 40.0594648528358, -105.4318892343097 40.0596640133864, -105.4322990968159 40.05986651955405, -105.4329873576576 40.06004930992891, -105.4335605933063 40.06004038995119, -105.434434235593 40.0599712445611, -105.4354783925689 40.05975633761448, -105.435996631219 40.05945534342511, -105.4366632696116 40.0590005622899, -105.4374423829502 40.0583688561975, -105.4380710690886 40.05782633790203, -105.4387283869856 40.0573751360412, -105.439546349493 40.0571235327649, -105.4398747066513 40.05698872465391, -105.4406386271914 40.05675863519146, -105.4417548336166 40.05638679447648, -105.442567773736 40.05613305341807, -105.4442686974679 40.05566339315051, -105.445343246227 40.05543155148678, -105.4460872580018 40.05530049376619, -105.4475361795096 40.05506323819086, -105.4484647042474 40.05492359728375, -105.4497124891264 40.05482749056537, -105.4509974746667 40.054709341968, -105.4519105410676 40.05459009159843, -105.4529452414847 40.05436689697932, -105.4539354331393 40.05422779377801, -105.4543838348087 40.05421363093428, -105.4550889579488 40.05414451371335, -105.4556747016011 40.05404522521154, -105.4556195417862 40.05389977953413, -105.4555785994819 40.05312561237029, -105.4555800785149 40.05277505477387, -105.4556423342693 40.05229494829926, -105.455604087428 40.05216777687549, -105.455363854523 40.05189813544341, -105.4549647203148 40.05156158659062, -105.4547531376207 40.05138317782109, -105.4544031511611 40.05106908044412, -105.4542784159924 40.05074735203495, -105.4542974585342 40.05030084833979, -105.4543602124875 40.0498831708682, -105.4544043076297 40.04934065378175, -105.4543482479448 40.04909096993268, -105.4542109292466 40.04890847082154, -105.4540922782555 40.04883640624273, -105.453598796094 40.04875458782777, -105.4530865461581 40.04871117041102, -105.4526367273778 40.04873019111304, -105.4522869920531 40.04882560463331, -105.4518609877183 40.04893312059847, -105.4515392148404 40.04900042535454, -105.4512371760301 40.04894566223346, -105.4510311076975 40.04881594232108, -105.4506189061122 40.04864772506455, -105.450381521998 40.04862841875691, -105.4500442086895 40.04865036424795, -105.449748527079 40.04863651001132, -105.4494197230372 40.04853976397921, -105.4491713770628 40.0484220791417, -105.4488324815664 40.04824364741962, -105.4484976187861 40.04824101085237, -105.4483742062581 40.04828836479434, -105.4481527085251 40.04847342744434, -105.4480825457048 40.04858899738371, -105.4479574354427 40.04880499423177, -105.4477557093762 40.04894803549239, -105.4475449876894 40.04896804860563, -105.447285091094 40.0489087685434, -105.4470577998178 40.04883339300962, -105.4467455619172 40.04867000817741, -105.4466253298221 40.04859381923382, -105.4463159689591 40.04821745074411, -105.4462490902482 40.04814167709562, -105.4460691639663 40.04793781841308, -105.4459530422406 40.04787097758558, -105.4456060940407 40.04782908762505, -105.4452030334892 40.04782752432455, -105.4447533455736 40.04783846618427, -105.4441126313704 40.0478088560095, -105.4436975850779 40.04781395002598, -105.4430717601619 40.04784941480156, -105.4428542106095 40.04781353540704, -105.4426133763108 40.04766957101944, -105.4424314041075 40.04752003349248, -105.4423133012629 40.04740912390634, -105.4421861847308 40.04730907867685, -105.4419926239673 40.04718895154178, -105.4418061612007 40.04717136530205, -105.4417081954194 40.047182415411, -105.4416026797826 40.04721179966809, -105.4415072036721 40.04724939290262, -105.4414255327156 40.04729616164285, -105.4411577224697 40.04751082582863, -105.4409777288979 40.04763690177953, -105.4407871880504 40.04777450210482, -105.4404879006635 40.04801117476408, -105.4403389720799 40.04814775195113, -105.4401721086119 40.04840903387786, -105.4401067707136 40.04857846009677, -105.4399833163249 40.04911181062739, -105.4398729838371 40.04928598490994, -105.4397192008006 40.04939319049351, -105.4394855114924 40.04943941990325, -105.4392044056712 40.04941046497871, -105.4388636524953 40.04931851093392, -105.438546327513 40.04918193415831, -105.4380767786613 40.04891900617424, -105.437743143361 40.04872791764675, -105.4373933085161 40.04859639978524, -105.4370453058392 40.04845061923234, -105.436850100213 40.04838174734803, -105.4366416043731 40.04822077949636, -105.4364623815374 40.04804718592201, -105.4362633499358 40.04785329407545, -105.4359270011547 40.04771609612432, -105.4356638386845 40.04761770272381, -105.4353588193232 40.04759065426665, -105.4351715745744 40.04763071171844, -105.4349968999914 40.0476738768727, -105.4347454162208 40.04770360844505, -105.4345268098148 40.04765547297004, -105.434388492245 40.04755708258775, -105.4343273663388 40.04749335953326, -105.4342501879127 40.04733242057809, -105.434314678797 40.04709269363552, -105.4345204999711 40.04693740685487, -105.4347929737008 40.04689355559919, -105.434987328464 40.04692391707396, -105.4353581394735 40.04718062489702, -105.4356328975705 40.04730560893702, -105.4361277795634 40.04738267032662, -105.4367424163266 40.04755614551331, -105.4373232663294 40.04777462146167, -105.4378965827389 40.04799394153435, -105.4384082122526 40.04818466005356, -105.4385869413177 40.04827225757087, -105.4387181248332 40.04828192910482, -105.4387681853788 40.04819073376519, -105.4387698323472 40.04798677707445, -105.4388164240695 40.04785346836961, -105.4388570582708 40.04770509858814, -105.4388749958935 40.04751382260495, -105.4389056636208 40.04744816914924, -105.438936292543 40.04738259762316, -105.4390135085617 40.0472337121499, -105.4391753715978 40.04694264036142, -105.4393494826775 40.04675592722637, -105.4394709162605 40.04664744693813, -105.4397443071152 40.0464388139819, -105.4398818573897 40.04630925394687, -105.4400319946386 40.04607407341846, -105.4401119276108 40.04575211954744, -105.4401573906037 40.04555561044507, -105.4401888235684 40.04532997165521, -105.4403184492711 40.04515190537982, -105.4404637006837 40.04504664805176, -105.4410062310046 40.04487488619607, -105.441351219543 40.04480243757087, -105.4416959411179 40.04480147386886, -105.4420395016487 40.04485806074565, -105.4423881029662 40.04493259178905, -105.4426691968809 40.04495673762963, -105.4429191074365 40.04491845168188, -105.4432654711716 40.04476847759636, -105.4434739426463 40.04461030486147, -105.443662898663 40.04442909629897, -105.4437817103438 40.04428511840506, -105.4439256132001 40.04410673258661, -105.4441404970957 40.04401270487976, -105.444329416994 40.04400206228913, -105.444606475449 40.0440694640092, -105.4447865945989 40.04423422180232, -105.4449203593976 40.04436476415748, -105.4451131401293 40.04456520837888, -105.4451744249196 40.0447130948, -105.445220507406 40.04488588584199, -105.4452409774836 40.04505930867118, -105.445308555714 40.04528334672855, -105.4454035915627 40.04552010855499, -105.4454710483879 40.04576237462368, -105.4455283401477 40.04598646261165, -105.4456105755037 40.04613445233301, -105.4458916514732 40.04618739837201, -105.446129018222 40.04621631660641, -105.4463039778235 40.04616358427998, -105.446407424162 40.04602195805321, -105.446667215597 40.0458187188582, -105.4468895653487 40.0456291768839, -105.4471443524481 40.04551644473226, -105.4475418471934 40.04542649938936, -105.4478799981491 40.04537433230562, -105.4482973977438 40.04536749866653, -105.4488277934268 40.04536792065857, -105.4493054526135 40.04542072925156, -105.4496841719427 40.04544973101621, -105.4499403346239 40.04540183080188, -105.4501028615711 40.04525786537818, -105.450179275188 40.04507186814531, -105.4502155530288 40.0449218307571, -105.4502282296804 40.04467217531494, -105.4502221263177 40.04447532385408, -105.4501223199638 40.04427843101776, -105.44994131148 40.04407190199892, -105.449822712307 40.0439470200139, -105.4496354242496 40.04378849942575, -105.4494168828578 40.04365397065786, -105.4492077275886 40.04355080971189, -105.4490446942465 40.04343302515638, -105.4488765011509 40.04324751308347, -105.4486865345227 40.04294787288507, -105.4485806074133 40.04259253785128, -105.448517087676 40.04241607109771, -105.4484560132822 40.04214117014943, -105.4484216352835 40.04183236545518, -105.4484403420923 40.04165558502374, -105.4484503267856 40.04140178460691, -105.4484771618931 40.0411400570128, -105.4484394873438 40.04089571999755, -105.4483385338129 40.04054712281781, -105.4484261968361 40.04026869292268, -105.4485450117775 40.04009590378584, -105.4488563328945 40.03998217976847, -105.4492260106934 40.03992336241087, -105.4493999185044 40.03990184221139, -105.4498007028263 40.03990440851381, -105.4501284912924 40.03993647409516, -105.4505348695174 40.03993307438179, -105.4508376767798 40.03982803620941, -105.4510314426461 40.03965527552067, -105.4512557276107 40.03936568470912, -105.4515151705002 40.0391549643555, -105.4518251986846 40.03901225076601, -105.4522750253273 40.03889240763946, -105.4526248871359 40.03880132893642, -105.4529747678841 40.03868144289466, -105.453237146107 40.0386383383169, -105.4534620325642 40.03861442341547, -105.4537868411229 40.03861935533121, -105.4540054406916 40.03865305122331, -105.4542052675649 40.03873955137311, -105.4542940217177 40.03884616820108, -105.454366795153 40.03897296933693, -105.4544554621322 40.03918807970334, -105.4545109151869 40.03937823169469, -105.4545295258558 40.03957028571636, -105.454487349659 40.0397120164544, -105.4544054341493 40.03994098882126, -105.4542949264418 40.04016001026518, -105.4542279658648 40.04041583399074, -105.4542476615172 40.04072245971157, -105.4542663008047 40.04087130524294, -105.4543486699077 40.04097342704688, -105.4544643931002 40.040968531833, -105.4545805139184 40.04090324200731, -105.4547373974696 40.04076906500305, -105.4548604161138 40.0406947188977, -105.4551222424858 40.04065080284435, -105.4553784604135 40.04046363889831, -105.455659724781 40.04020448362071, -105.4559284862173 40.03995492466868, -105.4562574718578 40.03965648192272, -105.4564090054578 40.03950116242441, -105.456544441536 40.03938317116771, -105.4566409306176 40.03929220433345, -105.4567330166988 40.03921855880425, -105.4568672587436 40.03918028655645, -105.4570091920068 40.03917737460529, -105.4571970735713 40.03920399012449, -105.4574727919017 40.0392091978561, -105.4576742374468 40.03919142832632, -105.4579028156498 40.03916299208306, -105.4580965338489 40.03912512646967, -105.4583214307786 40.03908199761207, -105.4585054251747 40.03903662811377, -105.4586676194872 40.0389573510736, -105.4587712987346 40.03887570672356, -105.4589205871877 40.0387839462538, -105.4589924053408 40.03873263674406, -105.4591488750491 40.03866982801697, -105.459281754371 40.03863528565626, -105.4594378452955 40.03860761423366, -105.4596225164181 40.03856567735592, -105.4598300573352 40.03850206237642, -105.4599893871282 40.03843129178706, -105.4601258643819 40.03835200377073, -105.4602619808966 40.03827793021264, -105.4604027375314 40.03820934932943, -105.4605223438437 40.03817541162056, -105.4606932532367 40.03813578027771, -105.4608392966388 40.0381130381778, -105.4610267088864 40.0380746926612, -105.4612703428166 40.03802676213171, -105.4614515026273 40.03799801562068, -105.4616514018601 40.0379692750558, -105.4617950968508 40.03791650970663, -105.4619726054274 40.03783872995795, -105.4620915575303 40.03779868942447, -105.4623023201674 40.03771283408327, -105.4624873757552 40.037614068235, -105.462680990125 40.03753699153216, -105.4628770812229 40.03750054437869, -105.4631042408409 40.03747206674869, -105.4633246112622 40.03744797986833, -105.4635589055868 40.03743185778323, -105.4636235490246 40.03743105409266, -105.4637816937117 40.03741302606748, -105.4639503426529 40.03741307889101, -105.4640814886207 40.03746113147709, -105.4642376044186 40.03753799884461, -105.4644186940067 40.03763888044522, -105.4644748512307 40.03775412559912, -105.4644935320498 40.03786455874874, -105.464507907916 40.03797734576097, -105.4645360958713 40.03802786540076, -105.4645957267993 40.03805259025746, -105.4647120461754 40.03807107744546, -105.4647745202732 40.03805189114709, -105.4648182696122 40.03800389282083, -105.4648550685247 40.03794835304665, -105.4648811532233 40.0379220071657, -105.4649476205288 40.03784790775509, -105.4650122987282 40.03778012129685, -105.465078759705 40.03771782568425, -105.4652080980914 40.03761629342243, -105.4653431327449 40.0375499005596, -105.4654888673151 40.03750904137418, -105.4656178024517 40.03749645190426, -105.4658131584533 40.03749952982961, -105.4660088678796 40.0375105683452, -105.4661702981009 40.03750814532204, -105.4663217330367 40.03749473846992, -105.4664925413939 40.03748106235036, -105.4666674604658 40.03743310044315, -105.4668236445499 40.03737553198952, -105.467013123584 40.03729241699619, -105.4670695855542 40.03724375496851, -105.4671485419023 40.03718837779355, -105.4672235362509 40.03710677890788, -105.4673192818278 40.0370246661799, -105.4674984575032 40.03692441086024, -105.4676921375748 40.0368236405516, -105.4679095874308 40.03674822793891, -105.4680732248038 40.03673756825309, -105.4682168562857 40.03674696743575, -105.4683792638509 40.03673260892104, -105.4685229377228 40.0367086414703, -105.4686916125601 40.03665107389151, -105.4687915756962 40.03659828794598, -105.4688728038787 40.03653589416309, -105.4688978201256 40.03646868383298, -105.46890064363 40.03636922615923, -105.4688683094032 40.03608649176768, -105.4688294375998 40.03588523171646, -105.4688453914475 40.03575198531156, -105.4689044311294 40.0356668865015, -105.4689419428456 40.03559007772576, -105.4689169763039 40.03555166201114, -105.4688687105725 40.03552112246808, -105.4688380044873 40.03550464314591, -105.4687795777049 40.0355180163664, -105.4687296018647 40.0355324059768, -105.4686733742518 40.03556119791493, -105.4686108936511 40.03560439217124, -105.4684359628538 40.03569076511911, -105.4682860068023 40.03579635096558, -105.4681547858792 40.0359067413368, -105.4679898241449 40.03601471206911, -105.4678578285873 40.03608621465351, -105.4676237554177 40.03613705106031, -105.467331920507 40.03621440190616, -105.4670365504225 40.03627611937569, -105.4667993245486 40.03628512626556, -105.4664259061041 40.03627563525414, -105.4659622339207 40.03622779481458, -105.4657686241495 40.03618452719056, -105.4655562815755 40.03613165095232, -105.4653189563666 40.03607396546633, -105.4651072879263 40.03602165240844, -105.4648750882777 40.03598032150571, -105.4646506937304 40.03592972757208, -105.4644258726802 40.03585283868239, -105.4641948044623 40.0357807496646, -105.463994948226 40.03574227847106, -105.4636166427366 40.03564888337526, -105.4634112977461 40.03563673985305, -105.4631798796471 40.03562788131242, -105.4627395533892 40.03560744655459, -105.4624397267235 40.035631355169, -105.4621398918474 40.03566966614794, -105.4619150074207 40.03571280336544, -105.4616719714894 40.03578798273691, -105.4614169324756 40.03586668451568, -105.4612479840717 40.0359075307685, -105.4609737105466 40.03589837960226, -105.4607032034072 40.03581322166796, -105.4606220451006 40.03574117646026, -105.4605471650208 40.03561631940264, -105.4604515209555 40.03538155913075, -105.4605411771969 40.03516980628697, -105.460745325164 40.03496219663339, -105.4611847842231 40.03470911039988, -105.4615213042833 40.03444444280142, -105.4617724253972 40.03433691517333, -105.4620627975974 40.03428677473638, -105.4621856634314 40.03426018654425, -105.4624639281927 40.03414607807002, -105.4626064878654 40.03402615997216, -105.4626558295333 40.03391856483394, -105.4626843287107 40.03379737847219, -105.4629445889004 40.03354610975452, -105.4631298230737 40.03329166422314, -105.4632530713163 40.03312539363773, -105.4631723676173 40.03300656352572, -105.4630145229104 40.03300203861048, -105.4628089278983 40.0330699704752, -105.462622870385 40.03313041401965, -105.462382416347 40.03320324775477, -105.4622308653884 40.03324942665533, -105.4621123091782 40.03323456402543, -105.4619137414415 40.03324987178478, -105.4615197640719 40.03337876415366, -105.4611247327144 40.03347334016239, -105.4609518658094 40.03350869522491, -105.4605078941259 40.03362493922769, -105.4602885655572 40.03372039648056, -105.4601135314883 40.03379527894455, -105.4598056262865 40.03390250849921, -105.4594550870504 40.03394992648856, -105.4592302812619 40.03386822790948, -105.4590304952082 40.03372892247928, -105.4589306386476 40.03359925412024, -105.4588994919795 40.03346000837385, -105.4589271012316 40.03330786827071, -105.4589510975607 40.03319367744554, -105.4589993853942 40.03306631878111, -105.4590991911509 40.03278360050758, -105.4591199652827 40.03268258496826, -105.4591150188724 40.03259226720602, -105.4590904327338 40.0325011183871, -105.459025065846 40.03237018159784, -105.4588191192251 40.03234372289711, -105.4585877890754 40.0324852542631, -105.4584940642501 40.03254763633696, -105.4582941296471 40.03265799168989, -105.4581254393853 40.03274435218859, -105.4578592433275 40.03283393990661, -105.4575384963822 40.03292249191365, -105.4573638484304 40.03294795724295, -105.4570363191193 40.03302854362433, -105.4568385346368 40.03315678050264, -105.4567821974185 40.03335360847299, -105.456810316454 40.0335063948916, -105.4568163017309 40.03364255787771, -105.4568147670809 40.03380864114875, -105.4567836160767 40.03393792729251, -105.4566574104255 40.03415831783961, -105.4565391460978 40.03424556947021, -105.4564459062538 40.03429220223725, -105.4563455251661 40.03433663644886, -105.4560561887739 40.03443617689543, -105.4558820640041 40.03447194538261, -105.4557134367721 40.03444787492125, -105.4555069673559 40.03437282740676, -105.4553591579345 40.03431072922503, -105.4552213537833 40.03423957512793, -105.4549828448176 40.0341595210442, -105.4547518082643 40.03406340635529, -105.4545894553672 40.03400092681017, -105.4544048394762 40.03389006898158, -105.4542148135177 40.03382793642425, -105.4539275651147 40.03373179865706, -105.4537152263285 40.03369810510524, -105.4535757331263 40.03368906599719, -105.4534339224975 40.03373649996782, -105.4532404333301 40.03384675008265, -105.4530966444898 40.03403873941181, -105.4528996095487 40.03433390838572, -105.4528367976827 40.03440445563236, -105.4527409866604 40.03449518904446, -105.4525621631257 40.03462637055709, -105.4522822055471 40.03474707870705, -105.4520285899935 40.03482274046059, -105.4517953516685 40.03486876177074, -105.4514831856922 40.03491859340362, -105.4511863413582 40.03494227858606, -105.450978883285 40.03494341729687, -105.45071074166 40.03487928414413, -105.4505560733715 40.03482792970555, -105.4503783085403 40.03480474727579, -105.4501840342861 40.0347983500095, -105.4498454715085 40.03480396835326, -105.4493036907586 40.03482404562962, -105.4491090456025 40.03483741109122, -105.4488319062706 40.03484689660222, -105.4486097899218 40.03482264071118, -105.4484766115696 40.03478112902216, -105.4482506454887 40.03465337735646, -105.4481422809494 40.03446165746902, -105.4481362684162 40.03443481097717, -105.4481329205014 40.03422597370815, -105.4481470076392 40.03414109764547, -105.4481260795742 40.03400366028069, -105.4480701046018 40.03385408082433, -105.4479668218472 40.03368427038595, -105.4477793721983 40.03355888403479, -105.4475619122258 40.03350832662646, -105.4472766183654 40.03355603716927, -105.4470286594717 40.03362738453134, -105.4467532642444 40.03366443105853, -105.4464040673902 40.03357560062572, -105.4462047509766 40.03342034703974, -105.4460304452506 40.03321525848548, -105.4458930090361 40.03289636765589, -105.4457851194213 40.03274544416081, -105.4456660007642 40.03260247699643, -105.4453974909924 40.03253882935554, -105.4446410104286 40.03254153280623, -105.4443343926845 40.0324079993765, -105.4441504963008 40.03223680009287, -105.4440493814973 40.03200426787598, -105.4441734651061 40.03145424855277, -105.4443124284151 40.03109085401899, -105.4444913236292 40.03071718412532, -105.4446928182208 40.03043460997001, -105.4447325990232 40.03008338367997, -105.4446249435774 40.02990234691063, -105.4444081617735 40.02975138055803, -105.4440156551388 40.02976707094705, -105.4432925149635 40.02991757979642, -105.4428953339191 40.02995247669094, -105.4423222079109 40.03004926154301, -105.4417223648292 40.03014946061934, -105.4411541727373 40.03024205234754, -105.440751507376 40.03005922461082, -105.4405693242223 40.02980844642548, -105.4405247569878 40.02950330023305, -105.4408239584615 40.02917871927851, -105.4411421879788 40.02891412948831, -105.441529024559 40.02852970729988, -105.4421143146823 40.02801533542056, -105.4424566530376 40.02772811448784, -105.4427645731155 40.02748946811337, -105.4428733963731 40.02729685366441, -105.442856035971 40.02709878718856, -105.442753379335 40.02694066987466, -105.4424740740986 40.02667581247531, -105.4422361561291 40.02641171725879, -105.4421627354118 40.02633215234981, -105.4419899014615 40.02608653720438, -105.4418746425845 40.02586809995525, -105.4417586206913 40.02558237748611, -105.4415278888112 40.02530001926016, -105.4411748071398 40.0251914071028, -105.4409601991724 40.0251496406772, -105.4405059529632 40.02491765159761, -105.4402623567944 40.02491513807523, -105.4400030944076 40.02498272684421, -105.4397966454858 40.02508904976244, -105.4395597793163 40.02530826612527, -105.4393847531026 40.02549418783097, -105.4388881862617 40.02578392638166, -105.4383964394073 40.02608161988581, -105.4381236062599 40.02620263262403, -105.4378150629437 40.02627055208302, -105.4374616035033 40.02636780929908, -105.4371070967812 40.02648420993519, -105.436882284474 40.02647389089999, -105.4365096676688 40.02643308879092, -105.4359709061833 40.02638233037293, -105.4353397279123 40.02626338634593, -105.434560662546 40.02605373725178, -105.4342120425081 40.02594238635933, -105.4339840279204 40.02588647444495, -105.4338078295614 40.0258265830417, -105.4336360797591 40.0257101710548, -105.4334659702456 40.02555939012371, -105.4333209616463 40.02541186218291, -105.4331701377172 40.02536766024828, -105.4329232416404 40.02530635391786, -105.4327884855952 40.02530015376797, -105.4323855395824 40.02538971378622, -105.4321131539127 40.0254310601623, -105.431864312664 40.02545883262779, -105.431596830892 40.02545181137284, -105.4312362792186 40.02535266078985, -105.4309884373621 40.02531084067979, -105.4308018192828 40.0253187176223, -105.4306240087566 40.02533914468896, -105.4304440918217 40.02535833452203, -105.4302921227901 40.02531887724997, -105.4300035208585 40.02531027780987, -105.4291686127435 40.02527695480858, -105.4288489351101 40.0252641769005, -105.4286467628336 40.02526405201116, -105.4284398918819 40.02526030865064, -105.4282505399818 40.02526532921783, -105.4280928649176 40.02528905947762, -105.4279403393489 40.02533865214975, -105.4278456463248 40.02536769199481, -105.427565462158 40.02545363275944, -105.4273723149777 40.02548955524393, -105.4272992408456 40.02550315312805, -105.4271607401996 40.02553472983659, -105.4269397331792 40.02553620222038, -105.4268080952425 40.02553707795469, -105.4266553884723 40.025530481876, -105.4264506883495 40.02552826112606, -105.4262204100254 40.02551554731503, -105.4258348759512 40.02550807146258, -105.4255253832655 40.02549189094529, -105.425336537817 40.02546798904408, -105.425231865712 40.02542433437173, -105.4250448922275 40.02530065309304, -105.4248890756269 40.02500178419848, -105.4244829277462 40.02529516184836, -105.4242888337048 40.02538617480473, -105.4241702737477 40.0253943819846, -105.4241055263623 40.02546890946908, -105.4241320967277 40.02580448864965, -105.4240306161858 40.02596997449884, -105.4238353616644 40.02612328375539, -105.4235583844979 40.0262484968697, -105.4232855239439 40.02628862962832, -105.4228380888603 40.02643746950258, -105.4225416650763 40.02647455585658, -105.4219594939403 40.02663572980704, -105.4205957282032 40.02702669446086, -105.4197519470123 40.02744890804984, -105.4194212648639 40.02804059421167, -105.4184673673066 40.02854728053241, -105.416944467668 40.0296031872475, -105.4101147222736 40.03337543824303, -105.3968760313684 40.03572857755817, -105.394174734267 40.03570604764993, -105.3892469026911 40.03526736561258, -105.3858182204366 40.03487996422837, -105.3839568393852 40.03435439097252, -105.3783727923253 40.03162968231719, -105.3782848636422 40.03160427235456, -105.3780233455173 40.03110744717045, -105.3779293998402 40.030962511854, -105.377849027609 40.03075552266019, -105.3776743587331 40.03060018019208, -105.3776073031798 40.03047597181467, -105.377439515432 40.03024819084041, -105.377318552172 40.03015497304926, -105.3772364880586 40.03010182404736, -105.3758836857723 40.03131424309618, -105.3741650995925 40.03020252129752, -105.3749849405123 40.02941898313524, -105.3759045695671 40.02852069220432, -105.3759343080993 40.02849147923748, -105.3763925710351 40.02793364120749, -105.3755117821475 40.02776524000981, -105.3711961630059 40.02695645121048, -105.3546712500328 40.03672381851344, -105.3538108379241 40.03696897306946, -105.3534381461273 40.03724483790737, -105.3532612450637 40.03799366841366, -105.3532354600683 40.03808060757868, -105.3529609690354 40.03773591963947, -105.3527190080583 40.03748607386943, -105.3525869533672 40.0372800170782, -105.3523828838969 40.03685013532778, -105.3523540487777 40.0368069988163, -105.3522848114288 40.03672236455037, -105.35217505533 40.0366652138417, -105.3520679691729 40.03664396178009, -105.3519211633894 40.03665710662899, -105.3512350652558 40.03690471542134, -105.350752066814 40.0370649058794, -105.3506308648587 40.03712486907259, -105.3505725782028 40.03717210823402, -105.3505319465621 40.03720512829423, -105.3504601218263 40.03730088848148, -105.3503969068409 40.03746386974544, -105.3503780571488 40.03759094744733, -105.3503898767918 40.03773810433935, -105.3504460158685 40.03786994552974, -105.3505489509703 40.03799800425764, -105.3506721684706 40.03816013003582, -105.3507470909403 40.03831630026858, -105.3509839656849 40.03881004263459, </t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" t="n">
+        <v>12</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>Gold Hill School</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>890 Main St, Boulder, CO 80302</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>http://ghe.bvsd.org/</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>Gold Hill Elementary School</t>
         </is>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>40.063366273762</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>-105.412472825461</v>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>http://ghe.bvsd.org/</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>POINT (-105.412472825461 40.063366273762)</t>
         </is>
@@ -1104,53 +1136,56 @@
           <t>POLYGON ((-105.3286746087921 40.10535684263111, -105.3285829759231 40.10933249677196, -105.3284764287342 40.12320395037586, -105.338666880128 40.12287074752498, -105.3570154846513 40.1222005135923, -105.3572191082018 40.13342581422324, -105.3574479985069 40.14350680276687, -105.3620470526125 40.14373967239412, -105.3653863238086 40.14390863896946, -105.3724445532802 40.14426314701497, -105.3756249977702 40.14442229898955, -105.3802069307475 40.14393475996678, -105.3846142384698 40.1434086231454, -105.3862709652701 40.14324061297724, -105.3884044813609 40.14302421617785, -105.3910227813257 40.14275859159998, -105.3938559354602 40.14264260717856, -105.3978471903133 40.1426810170485, -105.4016158940963 40.1426539946228, -105.4066619382064 40.14222189343135, -105.4120613755037 40.14185679013661, -105.4179731644263 40.14225905162373, -105.4289403298768 40.14271447214097, -105.4395878986195 40.14311825474861, -105.4401727770837 40.14261598846758, -105.4403537810245 40.14238998659867, -105.4402237421184 40.14213030229881, -105.4398852818033 40.14202560438268, -105.4391855920727 40.14174264501145, -105.4393165432695 40.14129639233892, -105.4395625963222 40.14089103276203, -105.4398186194974 40.14076761273627, -105.4401414380125 40.14074512764935, -105.4405929261264 40.14068677884232, -105.4409967632386 40.14032264183017, -105.4408534704239 40.13999095099267, -105.4408490334069 40.1397371658542, -105.4409085075205 40.13945272425534, -105.441627017672 40.13887924774726, -105.4422207242613 40.13851520124469, -105.4423573790931 40.13831032625852, -105.4423578766834 40.13772282112337, -105.4420495241894 40.13747673476857, -105.4415508498067 40.13774518734458, -105.4412480293186 40.13796819417399, -105.4409217230848 40.13789971366144, -105.4402577275296 40.13721622648192, -105.4398547178956 40.13666039171091, -105.4398429826147 40.13651009378682, -105.4400806386873 40.13616409029089, -105.440282517764 40.13601390299153, -105.4407039510041 40.13585471919701, -105.4410720982984 40.13555887751171, -105.4412266339091 40.13525837165508, -105.4411750208083 40.13502962615528, -105.4405388181168 40.13469784026258, -105.4400879145676 40.13463840129412, -105.4398744863336 40.13443334705769, -105.4401657041598 40.13389608953084, -105.4405278974666 40.13361390997284, -105.4407654448196 40.13337720790327, -105.4407125232153 40.1328261093088, -105.4403627730081 40.13245703042931, -105.4402728914216 40.13220656203799, -105.4400644616442 40.13193095930646, -105.4400899194859 40.13145686664786, -105.4403538378005 40.13138993460992, -105.4406096397451 40.13120850977839, -105.4409832887742 40.13115620496019, -105.4415594082608 40.13093225824515, -105.441792766598 40.13083022495606, -105.4419769745805 40.13066338102513, -105.442261322216 40.13000361890706, -105.4427208929108 40.12940160451431, -105.4427095572324 40.12913991797465, -105.4427675703991 40.12897916774902, -105.4424877633457 40.12872236349825, -105.4418814652586 40.1289485387039, -105.4410267929101 40.12911244475854, -105.44062622681 40.12903535671395, -105.4403426310507 40.12882378520813, -105.4401681268348 40.12794595764182, -105.4401434427004 40.1275423135798, -105.4403271348666 40.12745911950469, -105.4404194428449 40.12688895761845, -105.4407201871724 40.12656877013251, -105.4410708990064 40.1263703374706, -105.4412380885365 40.12606289377323, -105.4414134233512 40.12598610083815, -105.4414711420068 40.12577942124896, -105.441420042683 40.12563999291525, -105.4412759346113 40.12536469040398, -105.4410619516994 40.12512509566417, -105.4410137480186 40.12490314051508, -105.441097430001 40.12464690956161, -105.4414813607216 40.12462788419529, -105.4421071991706 40.1247563359244, -105.442947647063 40.12445436328711, -105.4436769171171 40.12394344283241, -105.4439275358654 40.1236488491693, -105.4445202014138 40.12351459181477, -105.4451130029283 40.12320734603828, -105.4452216943186 40.12296393819889, -105.4455611269561 40.12272303852475, -105.445739396922 40.12263102590813, -105.446039955218 40.12249021602141, -105.4464489749707 40.12238789669911, -105.4469749932546 40.12208061124908, -105.4471671525513 40.12181161128712, -105.4477683125735 40.12145310125752, -105.4479437114356 40.12126738157929, -105.448185771842 40.12121623602334, -105.4483776567044 40.12129961021427, -105.4487616002662 40.12123571340185, -105.4491705174989 40.1212551145804, -105.4495626968083 40.12133857566865, -105.4498965579845 40.12128746567679, -105.4500717861507 40.12132598257076, -105.4503472639266 40.12122359163366, -105.4505059458994 40.1210634885219, -105.4511987403007 40.12090361208407, -105.4518080037448 40.12084620635756, -105.4523171416668 40.12075672224367, -105.4526509209928 40.12081452108134, -105.4530014589959 40.12077622322268, -105.4534186065663 40.12096219016633, -105.4539860841122 40.12098804526939, -105.4543114739603 40.12111631176514, -105.4548953690357 40.12155861384782, -105.4551289863891 40.12164840024029, -105.4553375129245 40.12182146652683, -105.4556211845854 40.12194330604206, -105.4567476952424 40.12218078657261, -105.4571148602626 40.12225139836272, -105.4574820900696 40.12221950024355, -105.4577658308258 40.12223882484343, -105.4579744528898 40.12227093481082, -105.4586420805521 40.12231602393006, -105.4591427629213 40.12241230464112, -105.459426540493 40.12237396365717, -105.4596351523571 40.12242529202669, -105.4598603799639 40.12260476219456, -105.4601857548838 40.12279067271524, -105.4604945657169 40.12275874486985, -105.4606280161351 40.12289974109881, -105.4611287323885 40.12295116506065, -105.4613456231521 40.12312422327806, -105.4615375910474 40.12309865972016, -105.4617545600843 40.12313717276883, -105.4619130583798 40.12326536242697, -105.4622383982413 40.12352815004496, -105.4624136462316 40.12355383483845, -105.4626138907714 40.12365640856648, -105.4626722522616 40.12376534421811, -105.4634983443994 40.12404110236733, -105.4637237036221 40.1240027323586, -105.4640575672274 40.12395158235574, -105.4641327441804 40.12382987558185, -105.4642913426707 40.12377866944794, -105.4644582960157 40.12370824606593, -105.464775458548 40.12366990221442, -105.4649006295363 40.12370197418591, -105.4652261281958 40.12368285213142, -105.4653263239067 40.12359318687636, -105.4654765552431 40.12358041760589, -105.465534927737 40.12367653754603, -105.4657352353888 40.12366378377023, -105.4660107054588 40.12354854214486, -105.4662193640389 40.12352297571797, -105.4664447117113 40.12350382089762, -105.4665866247402 40.12343338716104, -105.4668203139106 40.12342064025405, -105.467245981875 40.12335669309825, -105.4675131398364 40.12316456351811, -105.4677718743203 40.12313260212488, -105.4680472876695 40.12312627150369, -105.4683310322217 40.12315197728206, -105.4684896408024 40.12306873151195, -105.4689653473825 40.12307526653493, -105.4696414409102 40.12288324117313, -105.4703897895339 40.12268154313838, -105.4716698357625 40.12198039095991, -105.4719954824268 40.1215768388424, -105.4722709491116 40.12142314124566, -105.4725463847205 40.12134632501065, -105.4728551832017 40.12131436321324, -105.4730555092523 40.12123112095186, -105.4732224711366 40.12110302336163, -105.4734121622826 40.12123371277409, -105.4737473731746 40.12100852646682, -105.4740469092332 40.12082102645913, -105.4745189206885 40.12052595655688, -105.4754638457052 40.11996697409248, -105.4760371636699 40.11961489194562, -105.4767299243416 40.1192079281799, -105.4772510215974 40.11886296609708, -105.4776018882412 40.118590990685, -105.4790361330383 40.11731092193791, -105.4796448686728 40.11676090215462, -105.4798029604164 40.11659100560805, -105.4799828931568 40.11631707090588, -105.4800680420141 40.11614304270354, -105.4801081295797 40.11600304720499, -105.4801271615554 40.11572194687562, -105.4801321518591 40.11565345599552, -105.480126854251 40.11554900265974, -105.4800709291615 40.11483195882938, -105.4799571387577 40.11392000040892, -105.47994689984 40.11347995026318, -105.4799831084339 40.11315108747889, -105.4800228351893 40.11301603279571, -105.4800750724082 40.11289196174184, -105.4803280011827 40.11237701453049, -105.4807411547071 40.11166993238112, -105.4810369668682 40.11119699196959, -105.481141719745 40.11102902557507, -105.481172888273 40.11097904880864, -105.4816951330304 40.1100400158963, -105.4818546629206 40.10977445435542, -105.4823589838911 40.10893492078437, -105.482582135903 40.10869502801032, -105.4828170706975 40.10851196147547, -105.4830648709474 40.10834509253929, -105.4836849112431 40.10788811373511, -105.484198027461 40.10752006052201, -105.4845709709276 40.10725602731577, -105.4853990868868 40.10667498578111, -105.4858270889044 40.10635687564845, -105.486026963706 40.10620893576657, -105.486304682836 40.10598285091034, -105.4863931105853 40.10589493374012, -105.4865518733471 40.10573710627398, -105.4866348289009 40.10565503613041, -105.4869580787954 40.10529600615231, -105.4870421135721 40.1051768763199, -105.4871983867236 40.10493120199538, -105.487371107932 40.10466301956749, -105.4875799550242 40.10427789721646, -105.4877459068544 40.10386586691835, -105.4877981448226 40.10361990686008, -105.4878260717741 40.10337806193478, -105.4878189785318 40.10306209335884, -105.4877879352173 40.10273596572463, -105.4877500744142 40.10255999741634, -105.4876560960379 40.10233598297891, -105.487465982088 40.10197003253423, -105.4872232530914 40.10196231987193, -105.4870658759538 40.10185095894693, -105.4868196809375 40.10165327938159, -105.4866314968063 40.10150845106372, -105.4864409512302 40.10137037515732, -105.4862588024056 40.101262715445, -105.4860921845815 40.10116130415413, -105.485836424144 40.1010056361766, -105.4849920033265 40.1006347135134, -105.4839093249891 40.10031426319865, -105.4830191331509 40.10007645950926, -105.4820120665893 40.09979723467995, -105.4810633072941 40.09953297116691, -105.4804127682046 40.09934531424202, -105.4798790898619 40.09915212792707, -105.4796824446445 40.09903871820308, -105.479522623448 40.09891664061265, -105.47930842218 40.09870538968306, -105.4791915455861 40.09854274547259, -105.4791229733392 40.09834346283061, -105.4790505879534 40.09799448492377, -105.479052359013 40.09769652549827, -105.4791607602249 40.09740045238264, -105.4794961388154 40.09700293191574, -105.479797634012 40.0967043939273, -105.4801272805915 40.09645000218192, -105.4804192775763 40.09622379676028, -105.4807603604884 40.0959618559625, -105.4810373636038 40.09577718040623, -105.4815054397459 40.09552895692337, -105.4828849789354 40.0947965137981, -105.4834266856064 40.09449934716857, -105.4839563409643 40.09420958858656, -105.4843160786468 40.09401001008721, -105.4849600779124 40.09369009269385, -105.4853886269958 40.09344662435053, -105.4855847413489 40.0933274545906, -105.4857615504926 40.09322955615455, -105.4858563001833 40.09318953431386, -105.4859493892815 40.09312657467158, -105.4860073291051 40.0930647932408, -105.4861085231208 40.09283111166538, -105.4862261265858 40.09261623463396, -105.4862796494349 40.09253696028742, -105.4863440427661 40.09244053089211, -105.4864980044573 40.09217910013354, -105.4865441300771 40.09209076614776, -105.4865734608415 40.09198365362728, -105.4865740605829 40.09184425428345, -105.4865353522169 40.09178458501036, -105.4864553790939 40.09173698668518, -105.4862821973595 40.09160110904213, -105.4861073632745 40.09172768854545, -105.4859915724628 40.09188118251183, -105.4859399173889 40.09224669687541, -105.4855569227272 40.09245426085091, -105.4853991721848 40.09275577199028, -105.4851288304584 40.09284965722114, -105.4848585210306 40.0928001904127, -105.4845881940973 40.09282981365086, -105.484388652141 40.09291629160026, -105.4842631327652 40.09297312031171, -105.4841569490116 40.09291131642115, -105.4838834046625 40.09293599485009, -105.4834812175096 40.09261957708101, -105.4829727683574 40.09258243013446, -105.4827860975529 40.09266890721459, -105.4827313666256 40.09276034651839, -105.482319451568 40.09275534145816, -105.4819042578073 40.09297524606438, -105.4814987763503 40.09297765406125, -105.4813056759049 40.09302705373208, -105.4810578863604 40.09300724067585, -105.4808809131605 40.09292812172586, -105.4800635134075 40.09293045483656, -105.4794326933343 40.09316514307063, -105.4792073022026 40.09326798560966, -105.4790400326163 40.09332819563044, -105.4788469508883 40.09330838774851, -105.4786957308279 40.09320949749731, -105.4783771380855 40.09320449555493, -105.4780746382073 40.09319207991353, -105.4776658860475 40.09334771066776, -105.4775306528645 40.09356765334825, -105.4772474503477 40.09358737055681, -105.4771798253259 40.09371835001559, -105.4770510914053 40.09374303988567, -105.4768934234911 40.09368121997633, -105.4765330558175 40.09349330784084, -105.4760471484061 40.09340423194784, -105.4759119562152 40.0934931799337, -105.47569635047 40.09346841936511, -105.475580499466 40.09346097994491, -105.4754786601035 40.09343640599089, -105.4753745308298 40.0934856524864, -105.474866935992 40.09328879541138, -105.4746087047842 40.09324327275854, -105.4745636236239 40.09331740989728, -105.47428364008 40.09333464918728, -105.4742160376812 40.09339147986027, -105.4741162532533 40.09345077464172, -105.4739263878601 40.09344084558703, -105.473807349652 40.09335431389002, -105.4733664608556 40.09336904298313, -105.4731444341594 40.09330720218613, -105.4729916792803 40.0932286162595, -105.4728645084006 40.0931786152824, -105.4726553723939 40.09307723213188, -105.4724719569328 40.09303517184765, -105.4721758977621 40.0930177995692, -105.4718701942519 40.09297570969477, -105.4716835380748 40.09299049312087, -105.471474831456 40.09294463514954, -105.4710559544133 40.09296597786506, -105.4707674328991 40.0928908421586, -105.4705300663141 40.09290865323496, -105.4703206714044 40.09281923890566, -105.4697115083137 40.09283601095878, -105.4697155590948 40.09300137780273, -105.469580518479 40.09316219136713, -105.4692547133936 40.09320142434954, -105.4689847098194 40.09316435921112, -105.4687893378856 40.09312623647281, -105.468551822928 40.09315517446294, -105.4684076755523 40.09317974872646, -105.4680772432944 40.09316178552184, -105.4678259063069 40.09319388575036, -105.4675976897138 40.09313492541786, -105.4674769094881 40.09306510889996, -105.4673382935705 40.09303567465224, -105.4670449195582 40.09282043987553, -105.466830142165 40.0927503751534, -105.4665508752498 40.09279676225574, -105.466175368936 40.09283502917013, -105.4660133546789 40.09291547457706, -105.4658247582281 40.09295739868286, -105.4654896758057 40.09293227830818, -105.4653501000844 40.09283930116639, -105.4643976530924 40.09280481316541, -105.4631414548872 40.09316059275267, -105.4626582682873 40.09335336468543, -105.4624649122545 40.09357591069848, -105.4617286574722 40.09384614586697, -105.4615178994789 40.09387241055427, -105.4611654802694 40.09384973690847, -105.4610315535357 40.09376359322027, -105.4608583491733 40.0938136841182, -105.460658211982 40.09382791377131, -105.460243147953 40.09372063406089, -105.4599415660822 40.09367039294574, -105.4598018508458 40.09382404415791, -105.459650247651 40.09392369492305, -105.4594387633614 40.0939311501803, -105.4590250747669 40.09403479846681, -105.4585034035345 40.09393072863794, -105.4583682293032 40.09378227417517, -105.457595301498 40.09376715213234, -105.4571117811182 40.09377660859597, -105.4565999711225 40.0935476545582, -105.4562231144058 40.09334734393994, -105.4555297114199 40.09325414451478, -105.455083043723 40.09306095254485, -105.454748087056 40.09285350500218, -105.4544735196476 40.09281765242407, -105.4542315415061 40.09276751534037, -105.4539848272495 40.09283890565887, -105.4537427462525 40.09293889265795, -105.4537315827848 40.09234097421643, -105.4539008079947 40.09109986475135, -105.4544090914951 40.09054553456455, -105.454911908807 40.08989274726373, -105.4542163050892 40.08989247351533, -105.4535787792297 40.08972897229278, -105.4527672945866 40.08965444022031, -105.4525356967895 40.08926849065042, -105.4516859108819 40.08871903688248, -105.4512031061514 40.08837750060519, -105.4507010271719 40.08797659187697, -105.4501216663902 40.08757564758034, -105.4487837599722 40.08707073310003, -105.4486953969671 40.08646003986499, -105.4482595350263 40.08540252877995, -105.4478127204892 40.08505892551648, -105.4479228999761 40.08487798226903, -105.4478072669787 40.08469779895818, -105.4476238579465 40.0846890219965, -105.4475036345719 40.08450405928904, -105.4475897214318 40.08435881224172, -105.4470531159785 40.08438867944763, -105.4469366294201 40.08394907302981, -105.447177440526 40.08384352104201, -105.4471899505661 40.08355873923949, -105.4472465702956 40.0830880661421, -105.4461800763135 40.08279278918044, -105.4450593525014 40.08230016385585, -105.4443783256202 40.08273042306977, -105.4436178451164 40.08239173691055, -105.442816765798 40.08272966012455, -105.4425360960861 40.08319086210443, -105.4420155464476 40.08322135784578, -105.4416144854269 40.08399005819694, -105.4408534971651 40.08423571992876, -105.4391716431737 40.08438862612866, -105.438571195249 40.08420377113308, -105.4377308990862 40.08358819949705, -105.4374515200174 40.08260385368555, -105.4361713659957 40.08140366490991, -105.4352912053459 40.08066502816462, -105.434250820534 40.08001856161342, -105.4332097920201 40.08004872002739, -105.4323160686941 40.07981172585485, -105.4316887331096 40.07964800046999, -105.431048340433 40.07943232741334, -105.4287271625604 40.07844672135369, -105.4285285568764 40.07693954925447, -105.424953062166 40.07568973903737, -105.4238530554861 40.07588974495376, -105.4224688082221 40.07553496080854, -105.4210854863552 40.07510219739299, -105.4210690908914 40.07502410942288, -105.4210379038569 40.07498123368718, -105.4206329695366 40.0749038455992, -105.4204181933324 40.07484263681267, -105.4202083996824 40.07461261810035, -105.4195352042127 40.07476456033439, -105.4191247017771 40.07482938094511, -105.4189980306713 40.07484611794027, -105.4186447055464 40.07487513225324, -105.4180009566014 40.07488857546316, -105.4177762251645 40.07488622163074, -105.4174610348563 40.0748779494316, -105.4172705764785 40.07488147149702, -105.4170810759536 40.07488206684572, -105.4170306009453 40.07488568808787, -105.4169286974435 40.07489512468741, -105.4167905896386 40.07491916695444, -105.4166333942057 40.07497684600628, -105.4162312907294 40.07517846289863, -105.4159997512771 40.07528949075067, -105.4156196132907 40.07543625610639, -105.4153350203652 40.07550396612029, -105.4151395682494 40.07551491221498, -105.4149634135315 40.07550234559449, -105.4148358409656 40.07547591583315, -105.4146111929816 40.07540552041137, -105.4143570994708 40.07527584758753, -105.4142381667132 40.07519455728776, -105.4139032823823 40.07494558003621, -105.4136444687195 40.07478517666688, -105.413329475767 40.07462253567618, -105.4130705753038 40.0745330917355, -105.4129058764918 40.07449931594424, -105.4127516241002 40.07448895733638, -105.4125773454127 40.07450053023379, -105.4124096976944 40.0745384436123, -105.4122829936822 40.0745807785052, -105.4116113120437 40.07483923530526, -105.4112998081208 40.07492678295778, -105.4111312145296 40.07495957269411, -105.4109493026843 40.07498064805032, -105.4104369611586 40.07499780879358, -105.4099465988038 40.07495572838605, -105.4096666239786 40.07496136200007, -105.4094075828542 40.07497944835027, -105.4087209130649 40.07504255224723, -105.4072133339139 40.07514450001526, -105.4064926228099 40.07519135351045, -105.4058410165122 40.0752136172959, -105.4054705638814 40.0752272141406, -105.40520487196 40.07523357995193, -105.4049353748692 40.07523628450529, -105.4047392325432 40.07521783433648, -105.4045848509388 40.0751897922855, -105.4041947147465 40.07508862949976, -105.403705422345 40.0749653223569, -105.4035454821902 40.07493738955924, -105.4033969451357 40.07492482835819, -105.4031503024901 40.07492901141337, -105.4028950470262 40.07496317992302, -105.4025169204411 40.07501553263012, -105.4023550157805 40.07502929541273, -105.4021645541007 40.07503425519602, -105.4019389002541 40.07501138551396, -105.40168661591 40.074965083188, -105.4015019436022 40.07491810670258, -105.40096224968 40.07475231378992, -105.4007728206619 40.07470313718637, -105.4006128875573 40.0746708105926, -105.4003900881106 40.07465013520603, -105.4001936699258 40.07464511287059, -105.3999920191408 40.0746658845997, -105.3997996016553 40.07470668529642, -105.3996328800538 40.07475774923518, -105.3994223224821 40.0748299894019, -105.3992936939425 40.07487962339136, -105.3991136328338 40.07493506377642, -105.3989345365082 40.07498245837664, -105.3987192795767 40.0750122629322, -105.3984012230241 40.07501125209868, -105.3982545679028 40.07501551265776, -105.3981326490511 40.07503442581616, -105.3980545259296 40.07505922901456, -105.3979649460374 40.07510377494535, -105.3978486566331 40.0751790217227, -105.3973899365647 40.07562852046983, -105.3972817002089 40.0757136836102, -105.397169427459 40.07578848025003, -105.3968792179321 40.0759179797459, -105.3959609054664 40.07622318892043, -105.3953231254621 40.07647233550051, -105.3947619214149 40.07666278952232, -105.3941305833764 40.07686297010658, -105.3939136913895 40.07697539101873, -105.3934575621836 40.07722224613386, -105.3931865114511 40.07731992618486, -105.3929282780375 40.07737354901404, -105.3926318413482 40.07740020380218, -105.3923466903028 40.0774207953173, -105.3919433258007 40.07747300969441, -105.3915512466445 40.07751915932716, -105.3910859383422 40.07751872123406, -105.390588819259 40.07748152648809, -105.3899547533051 40.07738544205882, -105.3895851208953 40.07734591650613, -105.3890560983312 40.07733071977488, -105.3886608422517 40.07736951179238, -105.3882208880001 40.07745722445686, -105.3878287902893 40.07751315322446, -105.3875386890442 40.07756183623066, -105.3871751517061 40.07769123986255, -105.386958188724 40.07783792342001, -105.3868401010417 40.07793818621354, -105.3866996581514 40.07806535888105, -105.386575220841 40.07815092657836, -105.3864348761523 40.07821933925117, -105.3862435609229 40.07827301294386, -105.3861064964615 40.0782851193332, -105.3859439556369 40.07828495884738, -105.3854915187126 40.07820861461854, -105.3852495670619 40.07817436606354, -105.3849689629014 40.07813464671029, -105.384647065656 40.07813677433686, -105.3843346505428 40.07818542609105, -105.3841911614831 40.07822690365325, -105.3838658088119 40.07838571414805, -105.3835116873142 40.07859345906748, -105.3832533311892 40.07871071489546, -105.3828706781617 40.07882784409028, -105.3824975639514 40.07895722236837, -105.3821530389425 40.07914049159699, -105.3818913601033 40.079333636382, -105.3816040092101 40.07962713452685, -105.381316880753 40.07979087291746, -105.3809245713487 40.07995695099259, -105.3802294146402 40.08015943763821, -105.379588467187 40.08034483921757, -105.3792504093654 40.08046689970899, -105.3786411661966 40.08074291496696, -105.3780797871333 40.08098470179396, -105.3777130575363 40.08109693300169, -105.3774866867055 40.08114076234569, -105.3770053036764 40.08120390520853, -105.3766993091122 40.08121582032145, -105.3761925603991 40.08120548435789, -105.3760268068356 40.08121510006245, -105.3757111712446 40.08127107066737, -105.3751786731141 40.08139780561959, -105.3744967961343 40.08157402736211, -105.3735477428702 40.0818006048877, -105.3730416668277 40.08192675278983, -105.3726786466126 40.08199815224141, -105.3724146658471 40.08203164841389, -105.3720517316847 40.08205658721963, -105.3715667481044 40.08210790769671, -105.3712911926056 40.08211536164035, -105.3710047166085 40.08208494329329, -105.3706571489542 40.0819848523058, -105.3701603136584 40.08182251295334, -105.3693330902472 40.08154316557858, -105.3691740018331 40.08149407507, -105.3689732329173 40.08146939130329, -105.3687454792302 40.08146913257269, -105.3682581015067 40.08148550858736, -105.3674792688943 40.08151471573545, -105.3669855945874 40.08156515588454, -105.3666338417142 40.08163741303427, -105.3665354783196 40.08168099405719, -105.3664748780766 40.08172531938194, -105.3664584034446 40.08159014621046, -105.3664654543084 40.08151024750345, -105.3665410705586 40.0813216177777, -105.3666249026477 40.08104341501357, -105.3665924458401 40.08081366575016, -105.3664632649919 40.08064976953737, -105.3662886091598 40.08052481296188, -105.3660390097108 40.08039337010403, -105.3659304079325 40.08034970692742, -105.3658929678842 40.08033465331701, -105.3659703076023 40.08049001044129, -105.3660033070792 40.08058400926235, -105.3651603062312 40.08079800940757, -105.36386330684 40.08112600999898, -105.3614307179702 40.08181077296624, -105.3614136449111 40.08208931510966, -105.361373970351 40.08273668039418, -105.3613838696417 40.08273389398298, -105.3616833691065 40.08264960897541, -105.3616895744276 40.08266268384122, -105.3618231569629 40.08294413896749, -105.3618343745151 40.08296777085793, -105.3618626507548 40.08302734621064, -105.3612294649398 40.08322514258172, -105.3582044235136 40.08420073402425, -105.3580926092154 40.08423693487651, -105.3581270614178 40.08459850432136, -105.3581348601366 40.08459842924469, -105.3591926002434 40.08458815364854, -105.3591925371214 40.08460053741205, -105.3591905319785 40.0849959100054, -105.3573681646263 40.08502614465402, -105.3569189380437 40.08526239120709, -105.3568395193715 40.08711423232176, -105.3556791226172 40.08712097800886, -105.3556774246944 40.08712098849529, -105.354242246951 40.08712931769688, -105.3542328567851 40.08712937248871, -105.3527096423569 40.08713819019081, -105.3527001841789 40.08713824477123, -105.3519880447198 40.08755429373965, -105.3510273451841 40.08805364431768, -105.3510314240971 40.08805658117283, -105.3510339691511 40.08805849111732, -105.3510364707778 40.08806041991922, -105.3510389277868 40.0880623756828, -105.3510405793695 40.08806372697654, -105.3510413472218 40.08806435481455, -105.3510437197018 40.08806635730237, -105.3510460487584 40.0880683768463, -105.3510483355446 40.08807042245434, -105.3510505753798 40.08807248961713, -105.3510527729524 40.08807457924146, -105.3510549200622 40.08807668771413, -105.3510570237446 40.08807881504423, -105.351059080476 40.08808096392912, -105.351061091431 40.08808313346974, -105.3510630566174 40.08808532006347, -105.3510649713371 40.08808752730682, -105.3510668391175 40.08808975070119, -105.351068656435 40.0880919929439, -105.3510704291584 40.08809425134065, -105.3510721502444 40.0880965294849, -105.3510738208755 40.08809882287498, -105.3510754457399 40.08810113241754, -105.3510770166333 40.08810345630074, -105.3510772620555 40.08810383308597, -105.3510785405837 40.08810579813619, -105.3510800410192 40.08810816876191, -105.3510817287355 40.08811069273843, -105.3510833753659 40.08811323737671, -105.3510849820807 40.08811580357887, -105.351086548892 40.08811838594115, -105.3510880757858 40.08812099076799, -105.3510895604248 40.08812361445374, -105.3510910063348 40.08812625340051, -105.3510924076469 40.08812891030255, -105.3510937713965 40.08813158516899, -105.3510950928933 40.08813427799377, -105.3510963697981 40.08813698607194, -105.3510976021068 40.08813971120482, -105.3510987945178 40.08814244979585, -105.3510999482036 40.08814520184658, -105.3511010526129 40.0881479664427, -105.3511021147673 40.08815074989782, -105.3511031346887 40.08815354230494, -105.3511041123671 40.08815634816715, -105.3511050454592 40.08815916658087, -105.351105933969 40.08816199574477, -105.351106776724 40.08816483565742, -105.3511075737242 40.08816768631873, -105.3511083343561 40.08817054503891, -105.3511090421975 40.08817341449873, -105.3511097078077 40.08817629200986, -105.3511103311927 40.08817917487041, -105.3511109029578 40.08818206937269, -105.3511114371899 40.08818496832981, -105.351111919806 40.08818787712743, -105.3511123602068 40.08819078677125, -105.3511127548545 40.08819370626314, -105.3511131061122 40.08819662750032, -105.3511134057638 40.08819955407481, -105.3511136655411 40.08820248329983, -105.3511138760653 40.08820541426265, -105.3511140443603 40.08820835237604, -105.351114163412 40.08821128772411, -105.351114241413 40.08821422752239, -105.3511142701628 40.08821716815781, -105.3511142520106 40.08822010783207, -105.3511141893056 40.08822304474702, -105.3511140808613 40.08822598520552, -105.3511139243503 40.08822892109879, -105.3511137267983 40.08823185693918, -105.3511134800089 40.08823478731219, -105.351113191008 40.08823771673009, -105.3511128527656 40.08824064248196, -105.3511124723156 40.08824356547749, -105.3511120426341 40.08824648030368, -105.3511115695742 40.08824939147138, -105.3511110496261 40.08825229537347, -105.3511104874762 40.08825519381728, -105.3511098760888 40.08825808679372, -105.3511092248507 40.08826097161301, -105.3511085279028 40.08826384646623, -105.3511077805547 40.08826671134739, -105.3511069968658 40.08826957167852, -105.3511061604374 40.08827241933256, -105.3511052865074 40.08827525703119, -105.3511043656989 40.08827808296099, -105.3511034015258 40.0882808989278, -105.3511023951647 40.08828370313181, -105.3511013407563 40.08828649376421, -105.3511002453384 40.08828926993341, -105.3510991053852 40.08829203523749, -105.3510979279441 40.08829478428164, -105.3510967024539 40.08829752065474, -105.3510954347834 40.08830024166259, -105.3510941284525 40.08830294640897, -105.3510927799473 40.08830563308802, -105.3510913869165 40.08830830439874, -105.3510899505349 40.088310959442, -105.3510884766733 40.0883135946227, -105.3510869629747 40.08831621534176, -105.3510854047624 40.08831881528859, -105.3510838090661 40.0883213971742, -105.3510821712054 40.0883239564893, -105.3510804970312 40.08832649864536, -105.3510787818711 40.08832901553052, -105.3510770257072 40.08833151525054, -105.3510752332379 40.08833399420897, -105.3510734009512 40.08833644969923, -105.3510715288491 40.08833888082079, -105.3510696239633 40.08834128938393, -105.3510676816053 40.088343674482, -105.351065699426 40.0883460379133, -105.3510636821256 40.08834837518056, -105.3510616261805 40.08835068898124, -105.3510595374595 40.08835297662093, -105.3510574124448 40.08835523809517, -105.351055252313 40.08835747160411, -105.3510530570523 40.08835968255164, -105.3510508290275 40.08836186193435, -105.3510485693955 40.08836401695893, -105.3510462734738 40.08836614401667, -105.3510439459587 40.08836824041177, -105.3510415833244 40.08837030974222, -105.3509560258479 40.08843761152456, -105.3507798770322 40.08857084662024, -105.3507538096081 40.08863307525191, -105.3507519531502 40.08863799036086, -105.3507511319305 40.08864084523704, -105.3507504935722 40.08864373007083, -105.3507500357499 40.08864663585278, -105.3507497561281 40.08864955807664, -105.3507496605839 40.08865249044558, -105.3507497479682 40.08865542215029, -105.3507500159438 40.08865834958532, -105.3507504680483 40.0886612637487, -105.3507511019483 40.08866415923357, -105.350751910624 40.08866702882577, -105.3507528976031 40.08866986802661, -105.3507540605621 40.08867266692603, -105.3507553959971 40.08867541921492, -105.350756900396 40.08867812218688, -105.3507585679157 40.08868076682799, -105.350760398576 40.0886833441317, -105.3507623876923 40.08868585139007, -105.3507645258996 40.08868828138591, -105.3507648979519 40.08868866373927, -105.3507668167196 40.08869063232233, -105.3507692461027 40.08869289427427, -105.3507718140629 40.08869506093713, -105.3507745112231 40.08869713049755, -105.3507773305537 40.08869910024445, -105.3507802720763 40.08870096027083, -105.350783320557 40.08870270605373, -105.3507864724758 40.08870433848928, -105.3507897254995 40.0887058521706, -105.3507930608822 40.08870723986828, -105.3507965301085 40.0887090870666, -105.3508980689437 40.08877062856219, -105.3509009761502 40.08877209766227, -105.3509038776238 40.08877350731244, -105.3509068038209 40.08877487196231, -105.3509097547317 40.08877619611515, -105.350912730362 40.08877747706896, -105.3509157295431 40.08877871302094, -105.3509187499201 40.08877990847136, -105.3509217926772 40.08878105801779, -105.3509248566341 40.08878216526129, -105.35092793711 40.08878322569265, -105.350931043486 40.08878423932394, -105.3509341651927 40.08878521334669, -105.3509373034264 40.08878613695467, -105.3509404581733 40.0887870164524, -105.3509436294314 40.08878785274052, -105.3509468183891 40.08878863861543, -105.3509500215108 40.08878938217835, -105.3509532376397 40.0887900762226, -105.3509564620774 40.08879072434474, -105.3509596995144 40.08879132655078, -105.3509629511253 40.0887918819416, -105.3509662087037 40.08879238960599, -105.3509694781146 40.08879284865083, -105.3509727546598 40.0887932626727, -105.3509760383511 40.08879362626768, -105.3509793291805 40.08879394303838, -105.3509826283206 40.08879421298629, -105.3509859299085 40.08879443610383, -105.3509892327773 40.08879460968762, -105.3509925416098 40.08879473734624, -105.3509958505506 40.08879481546952, -105.3509991642883 40.08879484496426, -105</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" t="n">
+        <v>14</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>Jamestown School</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>111 Mesa St, Jamestown, CO 80455</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>http://jae.bvsd.org/</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>Jamestown Elementary School</t>
         </is>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>40.1164318137431</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>-105.387802261192</v>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>http://jae.bvsd.org/</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>POINT (-105.387802261192 40.1164318137431)</t>
         </is>
@@ -1170,53 +1205,56 @@
           <t>MULTIPOLYGON (((-105.130907895079 40.17667497536176, -105.1309108852502 40.17618991643079, -105.1309011192309 40.1758791343955, -105.1309030890619 40.17558211464502, -105.1308961355192 40.17475305743081, -105.130896930049 40.17421089176275, -105.1308928914898 40.17403189495574, -105.1308978484933 40.17384386824337, -105.1308981571233 40.1736550034996, -105.1308928515666 40.17318199632658, -105.130890136097 40.17308892735598, -105.1308980849702 40.1728770261307, -105.1308830569357 40.17234908671396, -105.1308731301453 40.17200206767621, -105.1308640602036 40.17169513068922, -105.1308610970434 40.17144997901022, -105.1308601753751 40.17135609075753, -105.1308571509205 40.17105603681589, -105.130858089966 40.17094897815058, -105.1308520529194 40.17054487184136, -105.1308380730325 40.1698239502182, -105.1308381211171 40.16968312372387, -105.1308328523583 40.16953294692157, -105.130826950711 40.16923590355137, -105.130825096449 40.16911593337741, -105.1308268264415 40.16899487857084, -105.130829023898 40.16878789975995, -105.130829951995 40.16861687941822, -105.1308339090772 40.16841512361963, -105.1308248690956 40.16770711920258, -105.1308251696132 40.16745401704761, -105.1308240275999 40.16707106507126, -105.1471472878128 40.17412208832916, -105.1538401553576 40.17416747340352, -105.1538534119111 40.17702152067658, -105.1546629131087 40.17736968103145, -105.1546620818144 40.17647724158829, -105.1546599342045 40.17417298750612, -105.1546589995688 40.17417299912417, -105.1546569996872 40.17249899848197, -105.1546569998319 40.17225799859407, -105.1546530002739 40.17018099915842, -105.154647999395 40.16705899872255, -105.1546488353165 40.16705898771062, -105.1546488300367 40.16705586518081, -105.1551078351645 40.16704986397507, -105.1562688454048 40.16703286263721, -105.1572978539927 40.16702986225165, -105.1593498721462 40.16705286010649, -105.1595208740774 40.16707385977891, -105.1596798760458 40.16712085952145, -105.1598118775726 40.1671618596847, -105.1599118790576 40.16721485751804, -105.1602088846895 40.16741385793949, -105.161120902206 40.16807485153609, -105.1622709235831 40.1688868436568, -105.1631259398792 40.16948983996239, -105.1635209475333 40.16973283788921, -105.1637179519749 40.16985083726004, -105.1638209526211 40.16989583642651, -105.1640679558686 40.16999983608142, -105.1642169582605 40.17006083511097, -105.1642709600386 40.17007883540592, -105.1650199693466 40.17032183177924, -105.1664129896231 40.17079382714124, -105.1665174951051 40.17073080935722, -105.1665201919034 40.17073175740313, -105.1668849048761 40.17085999075397, -105.1668943955052 40.17084829540469, -105.1668985520034 40.17084317464879, -105.1668896186171 40.17084009214113, -105.1669304607418 40.17078976692029, -105.1669332093008 40.17078637943621, -105.1670240178124 40.17067447924944, -105.167026766362 40.17067109176306, -105.167035661948 40.17067421828263, -105.1677465944088 40.16979815123889, -105.1677518350548 40.16979169341922, -105.1687231045455 40.16859477217606, -105.1687256438738 40.1685916425322, -105.1687255340658 40.16858670852341, -105.1728195198593 40.17056786550766, -105.1728205681745 40.1705683728318, -105.1729529231051 40.17063241614367, -105.1733576954174 40.17082828027013, -105.1733657812711 40.17083213172842, -105.1734768197971 40.17088453830642, -105.1734768239046 40.17088245964705, -105.1734766984293 40.17058819044085, -105.1734767013714 40.17058610997677, -105.1734876717343 40.1687689579743, -105.1734888774345 40.16876895687698, -105.1735104074165 40.16876894654175, -105.1735112021403 40.16875746475598, -105.1735772011636 40.16694246349251, -105.1782538706628 40.16695343985297, -105.1782449702689 40.1681079937859, -105.178239767373 40.1687701694254, -105.1782249819881 40.17185948877151, -105.1781973695228 40.17705081512157, -105.1781856753826 40.1794676433639, -105.1781825181676 40.17975001998585, -105.1781812588263 40.18010303695387, -105.1781793654503 40.18059104394589, -105.1781684523568 40.18168714946533, -105.1781684669265 40.18183643617814, -105.1781660473366 40.18316294860183, -105.1781498990898 40.18620289633849, -105.1781465206755 40.1865180200456, -105.1781438093425 40.18681401520618, -105.178140520294 40.18717302076964, -105.1781444987996 40.1872194370608, -105.1781439104042 40.18733011805361, -105.1781394025259 40.18737198322795, -105.1781394746657 40.18773489066125, -105.178139841851 40.18809600032777, -105.1781305791092 40.18957200588383, -105.1781304006922 40.18958464219161, -105.1781202084915 40.1900471212033, -105.1780948944239 40.19119569292697, -105.1780936532397 40.19125198092252, -105.1780785993141 40.19253098832572, -105.1780756714483 40.19337646219445, -105.17807555733 40.19340999518588, -105.1780755436376 40.19355999935622, -105.1780754437916 40.19356992676756, -105.1780551400565 40.19491920996467, -105.1780545724636 40.19495698637294, -105.1780511446152 40.19536670668712, -105.1780475346618 40.1958009894524, -105.1780295545943 40.19680784784939, -105.1780344485064 40.19725808820253, -105.1780344787037 40.19764486805438, -105.1780338448599 40.19770630300314, -105.1780338432419 40.19770639666449, -105.1780265031893 40.19837698788592, -105.1780244953112 40.19858399017504, -105.1780244611668 40.19870778033302, -105.1780244603029 40.19882999897617, -105.1780262933825 40.19946629969199, -105.1780294225022 40.20054600094512, -105.1780177912117 40.20209443943981, -105.1780154294347 40.20240789362089, -105.1780170937183 40.20279956093896, -105.1780170986384 40.20280075429105, -105.1780171024931 40.20280167654974, -105.1780171035354 40.20280170447224, -105.1780193743578 40.20332300422022, -105.1780125892502 40.20344194989982, -105.1779985287708 40.20376896198804, -105.1779793391662 40.20578677022317, -105.1779733735186 40.20641786448409, -105.1779725180975 40.20704933316319, -105.1779724928907 40.20706829500229, -105.1779692945993 40.20951299755229, -105.1779642885702 40.21058099413643, -105.1779642880199 40.21058111031635, -105.1779548545939 40.21285325838544, -105.1779462410317 40.21411403975657, -105.1779402743808 40.21444507532357, -105.1779392003615 40.21541000119228, -105.1779391996817 40.21541064063836, -105.1779231113842 40.21602719206967, -105.1779222810411 40.216058878454, -105.1779061898209 40.21830724012914, -105.1779061013509 40.21831971271479, -105.1779001627716 40.21915299099524, -105.1778640906119 40.22388898961723, -105.177864540534 40.22467292051728, -105.1778669788484 40.22911209642017, -105.1778663526854 40.22919784805772, -105.177865003127 40.22937498989583, -105.1778569786166 40.23065399100331, -105.1778535241373 40.23095143561333, -105.1778529903291 40.23099711941484, -105.1778516407136 40.23142737115413, -105.1778499448728 40.23197999479415, -105.1778406387775 40.23204779070896, -105.1778184627386 40.23220092675904, -105.1777991760248 40.23223585886259, -105.1777990753533 40.2322360251985, -105.1777373000234 40.23228598032479, -105.1776563108877 40.23231160004515, -105.1776460005625 40.23231260073759, -105.1766870186988 40.23231559253281, -105.1762842567278 40.23231202562735, -105.1746699443099 40.2322976123188, -105.1733949514683 40.23228760767522, -105.1720667001548 40.23229148153948, -105.1720321683417 40.23229158269653, -105.1720320179274 40.2322915831708, -105.1715299999297 40.2322915883125, -105.1691109836499 40.23229392230051, -105.1684200036398 40.23229458111676, -105.1661308987598 40.2323106876401, -105.1660599158641 40.23231118707495, -105.1652950423296 40.23231656198064, -105.162829047121 40.2323355569361, -105.160993003236 40.23233656725746, -105.1596320574399 40.23234954749802, -105.159631111938 40.2326021603701, -105.159639287903 40.23489116429988, -105.1596411241535 40.23543000233618, -105.1596455377918 40.23602956648127, -105.1596490939906 40.23651103133323, -105.1596522712427 40.23722609101691, -105.1596540870133 40.23763600383838, -105.1596750332671 40.23923601341176, -105.1596793682309 40.23954562245473, -105.1596820218607 40.23973500530968, -105.1596852663667 40.24018047174287, -105.1596852684716 40.24018075544682, -105.1596864522177 40.24038181330056, -105.1597150691784 40.24686193224582, -105.1597140201794 40.24693386583294, -105.1597068877074 40.24714470682556, -105.1596630831104 40.24838283982047, -105.1596334362387 40.24898218808481, -105.1596333787975 40.24898333081097, -105.1596251227761 40.24914994405553, -105.1595390930119 40.25123381788716, -105.1595390876333 40.25123395296526, -105.159436146626 40.25319294047603, -105.1594315084507 40.25329819468507, -105.1594011116351 40.25399307586693, -105.1594193459625 40.25413204204748, -105.1594254824308 40.25417719946864, -105.1594376867242 40.25422352574407, -105.1594480492416 40.25426137441204, -105.1594480757986 40.2542614699565, -105.1595344547845 40.25439932079264, -105.1596523760393 40.25452303893846, -105.1597878147295 40.25460896776644, -105.1599382833191 40.25468036847293, -105.160341656995 40.25483557437291, -105.1603418083376 40.25483563335776, -105.1605874317561 40.25494246474813, -105.1608249922877 40.2550751577644, -105.1610305136834 40.25524053832483, -105.1610515290015 40.25526742410285, -105.1610813427591 40.25530659135412, -105.1611090626313 40.25537858837161, -105.1611188206494 40.25540469905818, -105.1611160671059 40.25552193081968, -105.1610980231822 40.25558792265264, -105.1610768827189 40.25562969209872, -105.16104190423 40.25569596936283, -105.1610295681123 40.25571325316199, -105.1609816117556 40.25576544534216, -105.160838322246 40.25591957105722, -105.1607775160145 40.25598497549689, -105.1607389143321 40.25602649736401, -105.1606064865818 40.25617027131609, -105.1605757980321 40.25620359452309, -105.1599924986764 40.25659730650925, -105.1599989720365 40.25673921994948, -105.1599547792698 40.25678485179284, -105.1598025509507 40.25693200702809, -105.1595811076893 40.2571367624378, -105.1594444833865 40.2572704528118, -105.1594442707474 40.25727066113117, -105.1593850046439 40.25732871936017, -105.1593135897142 40.25741741259193, -105.1592464000906 40.25751418241698, -105.1592073730529 40.25761787627735, -105.1592065780735 40.2576200489465, -105.1592065673312 40.25762008133739, -105.1591639582087 40.2577383241414, -105.1590671169694 40.25811957256996, -105.1588131688499 40.25926007653372, -105.1588050309629 40.25937747332689, -105.1588035176399 40.25938480355556, -105.1587867913851 40.25946585282338, -105.1587732062316 40.25970394070752, -105.1587867235447 40.25988310314099, -105.1588772703448 40.26029735125145, -105.1589371805952 40.26053541613221, -105.1589944087731 40.26086126506672, -105.1590273950741 40.26104527341096, -105.1590403258768 40.26112013450027, -105.1590548541795 40.26120439741041, -105.1590573513478 40.26121887960556, -105.157939095726 40.26123214999929, -105.1579317739117 40.26123219050455, -105.150072849193 40.26127578314014, -105.1500654098023 40.26127582459359, -105.1468465531939 40.26128064035046, -105.1467975327648 40.26128071323016, -105.1467900194693 40.26128072362639, -105.1429453634243 40.26128639073979, -105.1429377925196 40.26128640160884, -105.1406184806711 40.26128976910978, -105.1406108744983 40.26128977971715, -105.1379285346962 40.2612928022528, -105.1379208885625 40.2612928107571, -105.1342613927367 40.26129683485336, -105.1342536901744 40.26129684293716, -105.1314853591348 40.26129978664688, -105.1314776165972 40.2612997953193, -105.1311626635374 40.26130017098836, -105.1311533315791 40.26130018177933, -105.1310555398049 40.26130097878088, -105.1310552670561 40.26130098061338, -105.1310475630141 40.26130104431788, -105.1306819028509 40.26130423180297, -105.1306741940863 40.26130429907008, -105.1302260335092 40.26130820712956, -105.1302183188658 40.26130827434753, -105.1302173595303 40.26130828299087, -105.1302096472331 40.26130835111636, -105.1217148802063 40.26138175606975, -105.121707037398 40.26138182410287, -105.1177053612486 40.26141472727208, -105.115742714383 40.26143086470346, -105.1157347810537 40.26143093023018, -105.1157250642582 40.26143100964919, -105.1157171297533 40.26143107517082, -105.1142641668518 40.26144297225395, -105.114256210008 40.26144303760103, -105.1122949779269 40.26145914831125, -105.1122869928654 40.26145921342841, -105.1100575800509 40.26145729732243, -105.1100495048815 40.26145728993158, -105.108467570751 40.26145589258702, -105.1084594708947 40.26145588500171, -105.1057206751605 40.26145337069362, -105.1057125353351 40.26145336277992, -105.1055764423602 40.26145325215404, -105.1055683013489 40.26145324602741, -105.1029318436331 40.2614507919655, -105.1029236626631 40.26145078371452, -105.1026625533545 40.26145053973125, -105.1024478793076 40.26145187944849, -105.1024397379435 40.26145193344261, -105.1009687718798 40.26146179064328, -105.100960609353 40.26146184446047, -105.1005852751427 40.26146435504149, -105.1005771055564 40.26146440970788, -105.1000227844769 40.26146813525616, -105.1000146066554 40.261468190755, -105.0999062011835 40.26146891936003, -105.0998980221863 40.26146897484655, -105.0931208000076 40.26151409742457, -105.093112518724 40.26151415207208, -105.0880094105433 40.26154786605323, -105.0880010516577 40.26154792095951, -105.085095114039 40.2615670067869, -105.0835872226432 40.26157690882633, -105.0835787990881 40.26157696408129, -105.0835227733561 40.26157732810092, -105.0835143486308 40.2615773824463, -105.0834155232793 40.26157802110299, -105.0834070961972 40.26157807633273, -105.0828514814461 40.26158169068106, -105.0823658167984 40.26158485138247, -105.0740535654481 40.26163893567075, -105.0648359236269 40.26171750422144, -105.0645857591206 40.26171962647721, -105.0645770650161 40.26171970004614, -105.0550981174537 40.26181467832726, -105.0550882881114 40.26180786511199, -105.055089102158 40.2561198963567, -105.0550893227732 40.25454176871278, -105.0550893173981 40.25453828145123, -105.0550786320396 40.24742874159061, -105.0550786266126 40.24742526243025, -105.0550781606866 40.24716273015109, -105.0549125264558 40.23982547279036, -105.0549124708876 40.2398219348914, -105.0549113570069 40.23974294872203, -105.0549114469985 40.23973943660069, -105.0550890166748 40.23277390435145, -105.0550845739097 40.2318966321016, -105.055084557513 40.2318932132323, -105.0550521333209 40.22547414490511, -105.0550521966061 40.22547075966209, -105.0551545759616 40.22001725305361, -105.055154576327 40.22001719721558, -105.0551656190208 40.21909135193408, -105.055165657996 40.21908808908051, -105.0551754353958 40.21826973689463, -105.0551754375666 40.2182695846955, -105.0551754907823 40.21826647950752, -105.0551768073136 40.21818594070018, -105.055175145165 40.21195627749737, -105.055175144372 40.21195298746794, -105.055174874339 40.21095185735524, -105.0551748699924 40.2109485718148, -105.0551659295546 40.20376782758404, -105.0551659250086 40.20376457266076, -105.0551658095187 40.20368024908086, -105.0551658094086 40.20367990683798, -105.0551933208667 40.20367993430043, -105.0557612194496 40.20367601713887, -105.0557639998678 40.20367599809817, -105.0558368854482 40.20367580791534, -105.056911999972 40.20367299893432, -105.0583553984353 40.20363396552585, -105.058538999233 40.20362899881254, -105.0594407995711 40.20360935166872, -105.0594569996611 40.2036089990881, -105.0594589803057 40.20360895889921, -105.0604691792169 40.20358828730067, -105.0605809999359 40.20358599860956, -105.0625290002004 40.20354499890966, -105.0647029999319 40.20349699885044, -105.0647501006766 40.20349602781442, -105.0647763071737 40.20349548788953, -105.0647999996946 40.20349499884104, -105.0649459997082 40.20349199875547, -105.0650095092602 40.20349053724983, -105.0662489993874 40.20346199884766, -105.067296999437 40.20343799958135, -105.0690749998827 40.2033999992119, -105.074014699015 40.20330567887017, -105.0740449135742 40.20330506064477, -105.0741578445987 40.20330274940949, -105.0741613829224 40.20330268048043, -105.074174153481 40.20330244200157, -105.0747471835121 40.20329593233741, -105.0765138346332 40.20327584447682, -105.0776037795497 40.20327547779507, -105.0779601843807 40.2032754757722, -105.0783671987761 40.20327647585538, -105.0783672903983 40.20327647528878, -105.0787342713654 40.20327551513552, -105.0788240199679 40.20327306536132, -105.0790784726884 40.20326612110446, -105.0798893828385 40.20325404710055, -105.0806879610338 40.20324837306046, -105.0816501847357 40.20324047561559, -105.0822069163204 40.20323024316917, -105.0830682814023 40.2032196909061, -105.0835791856489 40.20321847582563, -105.0835981069327 40.20321967515504, -105.0837211863008 40.203227474651, -105.0856447171358 40.20320449576815, -105.0856452363401 40.20320449042337, -105.0877735888691 40.20318643920209, -105.0888532544556 40.20317763229867, -105.0897408380637 40.20317038475633, -105.0904716416781 40.20316441172043, -105.0908696894022 40.20316115619768, -105.0912832223234 40.20316093513956, -105.0914944937617 40.2031624183343, -105.0917522278974 40.20316422728517, -105.0919455217571 40.20316558314721, -105.0921975370513 40.20316735111282, -105.0926146724067 40.20317027581347, -105.0928657727666 40.20317203549725, -105.0930057234746 40.2031730162505, -105.093005727191 40.20317337651804, -105.0930711835685 40.20317401664741, -105.0930820960962 40.20317412349315, -105.0932201875574 40.20317547481145, -105.0932147345931 40.20427675894129, -105.0932105779957 40.2051159902964, -105.0932041876712 40.206406475457, -105.0932022136999 40.20678056108493, -105.0932545485407 40.20678031284936, -105.0954331146536 40.20678761374383, -105.0971599989639 40.20679337055231, -105.0971607119664 40.20679337303581, -105.0976247948587 40.20679491652393, -105.0976247893968 40.20679703029651, -105.0977981545344 40.20679786929404, -105.0977981954315 40.20680406130543, -105.0978192166669 40.20994758211779, -105.0978192638643 40.20995469549757, -105.0978192865362 40.20995801171471, -105.0978221643321 40.21038836945402, -105.1020764826853 40.210400971623, -105.1023781912976 40.21039966129107, -105.1024751480868 40.2103992398415, -105.1024778062865 40.2099546758207, -105.102494799139 40.20914168066236, -105.102465788828 40.20820268604596, -105.1025047847938 40.20772268878633, -105.1025137811899 40.20727069089985, -105.1025437709455 40.20634669622018, -105.1025237636843 40.20571670054039, -105.1025237619839 40.20539370203086, -105.1025210625498 40.20515181087357, -105.1025107002389 40.20422331812248, -105.1022201967591 40.20421818627374, -105.1018961897053 40.20421247454206, -105.1018971891388 40.2032814736801, -105.1024151901731 40.20329347428748, -105.1024483477597 40.20329452110688, -105.1024214449243 40.20329367141449, -105.1024213646419 40.20328751439211, -105.102421336487 40.20328529873123, -105.1024054437498 40.2013562575215, -105.1024006556609 40.20088934679336, -105.1024847271985 40.20065462381238, -105.1024859020631 40.19952909100861, -105.1024319782109 40.19815907813807, -105.1024139175533 40.19696213301737, -105.1023788304601 40.19586093436818, -105.1023809230087 40.19574811518007, -105.1023868541003 40.19503988820251, -105.1023850650994 40.1948559566662, -105.1023748592168 40.19451991641212, -105.1023501276933 40.19385193690373, -105.1023401095519 40.19238187512373, -105.1023480324539 40.19219001707661, -105.1023450792598 40.19183807835071, -105.1023359238445 40.19064912338679, -105.1023129456827 40.18974287047573, -105.102305841591 40.18899891023079, -105.1022938744325 40.18859697923833, -105.1022929712663 40.18856787832284, -105.1022919348154 40.18813304226678, -105.1022951231635 40.18764908370499, -105.1022961545613 40.18759500754209, -105.102314050903 40.18661587375054, -105.102324014524 40.18558510414968, -105.1023359709285 40.18488705328424, -105.1023460249624 40.18414699542499, -105.102370035092 40.18248900592155, -105.1023831548078 40.18140800978896, -105.1023829530066 40.18125894705506, -105.1027139937316 40.18126200709273, -105.1033940415842 40.18125610659184, -105.1036499481707 40.18125506224674, -105.1044011718303 40.18125708676741, -105.1047898365833 40.18126006333194, -105.1051319899099 40.18126013369076, -105.1052980584674 40.18125987759827, -105.1059451380013 40.18126098709274, -105.106641973712 40.18126088969616, -105.106833109551 40.18125797063896, -105.1072020949942 40.18126004898254, -105.1080911123929 40.18126196732355, -105.1084361110251 40.18126505829095, -105.1086240113595 40.18126487136174, -105.1089940736708 40.18126612354689, -105.1101640174649 40.18126520655875, -105.1112559916314 40.18126990755782, -105.1113569308159 40.18126805117004, -105.1115040224316 40.18126909494015, -105.1118629926047 40.18127002597253, -105.1118759946224 40.18181388411318, -105.1119081200098 40.18251894680662, -105.1119091664257 40.18315088404788, -105.1119118919206 40.18367686408679, -105.1119049061916 40.18402300359683, -105.1119319115066 40.18487960280919, -105.1120085237062 40.186557607745, -105.112011570436 40.18673288206929, -105.112017894645 40.18707819066701, -105.1120313601333 40.18760194311961, -105.1120540599835 40.18855794243968, -105.1125329666713 40.18856092088617, -105.1125820027335 40.18856108520247, -105.1133670179578 40.18855190824585, -105.1134489979368 40.18854998659783, -105.1145858430134 40.18854499691239, -105.1146671019506 40.18854389517986, -105.1158580022557 40.18853797614679, -105.1167671242837 40.18854593391976, -105.1172141737779 40.18854906207515, -105.1174969479037 40.18854890001953, -105.1179300587332 40.18854813537448, -105.1183019485997 40.18854991306068, -105.1186970917979 40.1885539619918, -105.1190850825382 40.1885568881324, -105.1194899230949 40.18855492662844, -105.121360830748 40.18856299055086, -105.1256918879809 40.18856611215961, -105.1288573477865 40.18857997484698, -105.1309169704838 40.1885889481708, -105.1309130611667 40.18812198620383, -105.1309220276749 40.18759110388334, -105.1309188689071 40.186986063103, -105.1309191252318 40.18634507253613, -105.1309118354979 40.18564393849361, -105.1309110183405 40.18513498587469, -105.1309051019469 40.18497190483541, -105.1309039419183 40.18465813085619, -105.1308979191687 40.1841851230857, -105.1309021056735 40.18314994122324, -105.1308898627142 40.181442199769, -105.1308910444444 40.1812969306925, -105.1309031473364 40.17900092566963, -105.1309088561322 40.17768491898182, -105.1309089894072 40.17686906099571, -105.130907895079 40.17667497536176), (-105.1311514181201 40.2604706245238, -105.1311533230373 40.26129655853457, -105.1311533315791 40.26130018177933, -105.1311514181201 40.2604706245238), (-105.1263252377158 40.20680501554748, -105.1263252134739 40.20681968499972, -105.126325383258 40.20671719607243, -105.1263252377158 40.20680501554748), (-105.1155968517825 40.20318341103974, -105.1155968269777 40.20318946052415, -105.1155957253303 40.2034586936532, -105.1155968517825 40.20318341103974), (-105.1499563688645 40.20041626554917, -105.1499662706908 40.20210364514212, -105.1499562482724 40.20039565687276, -105.1499563688645 40.20041626554917), (-105.1499554011348 40.19980913608271, -105.1499554011414 40.19980913650229, -105.1499982009238 40.19982447013613, -105.1499554011348 40.19980913608271)), ((-105.083075148123 40.17192712109441, -105.0830780316235 40.17151508279193, -105.0830908276374 40.17077009335227, -105.0830898739331 40.16975794923593, -105.0830891382825 40.16941095828075, -105.0830899607455 40.16886796812796, -105.0830910643746 40.16868788974446, -105.0830930531922 40.16830494684462, -105.0830960976557 40.16792502758191, -105.0830959771383 40.16724395293009, -105.0830878765151 40.16693097503487, -105.0830950003841 40.16658593425269, -105.0831080505025 40.16650005739481, -105.0831190490881 40.16645699775201, -105.0831339771326 40.16641505106289, -105.0831478259643 40.16637392366613, -105.0831681144781 40.16633309328626, -105.0831919525168 40.16629694372924, -105.0832150677106 40.16626188854235, -105.0832439014171 40.16622795275293, -105.0833268254032 40.1661261315451, -105.0834260412004 40.16599307439358, -105.0834769351456 40.1659210605575, -105.0835000500647 40.16588600531175, -105.0835210296103 40.16584902129782, -105.0835398631979 40.16581202954788, -105.0835558587693 40.16577090983481, -105.0835711141966 40.16573390518737, -105.0835959221352 40.16565603140108, -105.083613938554 40.16557703616078, -105.0836220561698 40.16553698593949, -105.0836269525403 40.16549692411329, -105.0836300593452 40.16545713053579, -105.0836106635436 40.16484891209912, -105.0836030415373 40.16460987586909, -105.0836141587786 40.16413802271901, -105.0836161082395 40.16399500687811, -105.083609519032 40.16392308127849, -105.0881761464068 40.16392102833853, -105.0881693626968 40.16382478228903, -105.0881650625537 40.16356494168014, -105.0881668740553 40.16350208512876, -105.0881648387267 40.16306998948579, -105.0881598089886 40.16280928973737, -105.0881623938254 40.1623954782369, -105.0886809584908 40.16239212456986, -105.089468094328 40.16239711982808, -105.0909838252546 40.16238410086513, -105.0917190936679 40.16238697525812, -105.0925199158311 40.16237689791628, -105.0931070011848 40.1623778683723, -105.0931070004038 40.1623779989626, -105.0931050119728 40.16313991872316, -105.0931050114934 40.1631399988786, -105.0931040000302 40.16325199822559, -105.0931039998199 40.16329599907725, -105.0931469291512 40.16390871444782, -105.0931479999207 40.16392399940396, -105.0931480029145 40.16392408767742, -105.0931569991541 40.16423199918421, -105.0931259993862 40.16516199880555, -105.0931289999454 40.16569099842605, -105.0931319995954 40.16601699884203, -105.093122999789 40.1669069989264, -105.0931289996238 40.16735399928291, -105.0931369998561 40.16781299868737, -105.0931339988095 40.16872599950739, -105.0931369991391 40.16900499892864, -105.0931479994263 40.17023599850143, -105.0931500001353 40.17054199825319, -105.093151000261 40.17065999832266, -105.0931330003842 40.17149199908522, -105.0931459999594 40.17231399916508, -105.0930759995535 40.17368299823816, -105.093035999663 40.17395399970057, -105.093035412355 40.17395404356559, -105.0928751701174 40.17396600181887, -105.0928349994319 40.17396899906539, -105.0920962144237 40.17397699684266, -105.0920961416262 40.17397699748644, -105.0920959995587 40.17397699788575, -105.0899358508228 40.17397797709733, -105.0898870002667 40.17397799833534, -105.0892635502055 40.17397922794395, -105.0888742073944 40.17397999371771, -105.0883123178483 40.17397704920117, -105.0883031426125 40.17397700121329, -105.0883029993709 40.17397700160376, -105.088302814376 40.1739809907825, -105.0830771458684 40.17399043991578, -105.0830771760332 40.1739901157939, -105.0830749017534 40.17371888591792, -105.0830759771914 40.17348500237775, -105.0830810478255 40.17329999660924, -105.083080876397 40.17274410150467, -105.083075148123 40.17192712109441)))</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" t="n">
+        <v>15</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>Longs Peak MS</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>1500 14th Ave, Longmont, CO 80501</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>http://lpms.svvsd.org/</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>Longs Peak Middle School</t>
         </is>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>40.18399195721774</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>-105.117518880356</v>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>http://lpms.svvsd.org/</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>POINT (-105.117518880356 40.18399195721774)</t>
         </is>
@@ -1236,53 +1274,56 @@
           <t>POLYGON ((-105.1310483121341 40.12350602835088, -105.1310413121898 40.12134002807184, -105.131030312504 40.11993502837323, -105.1310243109556 40.11903302886184, -105.1310173108496 40.11649802904655, -105.1310173105552 40.11642102922118, -105.1310173486831 40.11641334503174, -105.131018259415 40.11641262021929, -105.1310181860247 40.11642745992815, -105.1311001857065 40.11641745990186, -105.1311361855693 40.11640146052148, -105.1311941855785 40.11632246004667, -105.1312731862733 40.11603745969056, -105.1313421735774 40.11588122329221, -105.1313536700491 40.11585518628547, -105.1314091855054 40.11572946035969, -105.1314881866388 40.11547746041233, -105.1315867964692 40.11541012927728, -105.1316741852191 40.11535046009578, -105.1317241867259 40.115191460073, -105.1318891858139 40.11515346003952, -105.1322901860955 40.11511545933612, -105.1322751860538 40.11537845966455, -105.1323321866405 40.11548845960182, -105.1323543636915 40.11550215156709, -105.1324471863394 40.11555946059213, -105.1326261859337 40.11553245951755, -105.1327901954493 40.11544179157702, -105.1330331862589 40.1153074606795, -105.1331191859966 40.11521445939096, -105.1331411856992 40.11488445961638, -105.133234186949 40.1147304599069, -105.1333340990247 40.11463557074746, -105.1334131856659 40.11456046023817, -105.1335362178282 40.11456046070084, -105.1336711859251 40.11456046016362, -105.1338501858913 40.11461045973502, -105.1342361863052 40.11481945914035, -105.134329186555 40.11493445989868, -105.1344361864871 40.11494046008041, -105.1346221871356 40.11477045999761, -105.1346861864186 40.1145994604477, -105.1347221866439 40.11440245982309, -105.1350148427649 40.11403187214655, -105.1350602254513 40.11397440482906, -105.1350801857764 40.1139464596064, -105.135182139388 40.11393135543081, -105.1352747246668 40.11399622867296, -105.1353697140693 40.11414098052226, -105.1354881867362 40.1143364596393, -105.1356101869878 40.11439745989412, -105.1357101866312 40.1143694590412, -105.1357961873731 40.11427645936892, -105.1357961869385 40.11416645986762, -105.1357461861792 40.11397446007563, -105.135839187088 40.11381545968592, -105.135989187307 40.11374945946562, -105.1360886500456 40.11374159503977, -105.1362041868162 40.11373245991339, -105.1363067782619 40.11374563253825, -105.1364611865636 40.11376545914218, -105.136647186488 40.11372745988353, -105.1367132737641 40.1136867910588, -105.1367901873759 40.11363945994061, -105.1368346130924 40.11357172155405, -105.1368911870444 40.11348545902928, -105.136926249788 40.11333338529389, -105.1369771870886 40.1131124602168, -105.1369701872679 40.11299745903131, -105.1369049964273 40.11285831592468, -105.1368341870956 40.11272245868071, -105.1367911864023 40.11260145944513, -105.1366771874476 40.11241445906841, -105.1367061863406 40.11229345931134, -105.1368491873511 40.11220045890114, -105.1369921868139 40.11221745873338, -105.1371491860115 40.11229945967833, -105.1373141862809 40.11240445921667, -105.1373815568126 40.11239409447652, -105.137381607722 40.11239400637307, -105.1374571875025 40.11238245959723, -105.1375501870297 40.11229945883865, -105.1375851861427 40.11219045989127, -105.1375783082322 40.11213281406475, -105.1375641863439 40.11201445996381, -105.1375291873222 40.1118764593884, -105.1375931871308 40.11181145885294, -105.1378641325305 40.11172992844479, -105.1379221864662 40.11171245960098, -105.1380043977404 40.11165544251909, -105.1381346354642 40.11156511596145, -105.1383520505958 40.11141634734895, -105.1385021871975 40.1113174589991, -105.1385885373203 40.11121663711587, -105.1386811865493 40.11110845948276, -105.1387881878956 40.11089445929716, -105.1388881875843 40.1108174596417, -105.1391321875739 40.11077945940796, -105.1392166376191 40.11076175266201, -105.1392452612604 40.11075575100678, -105.139318187819 40.11074045974925, -105.1393678994795 40.11072429438088, -105.1395584243935 40.11066233928282, -105.1396041866986 40.11064745841755, -105.139761662953 40.11061060263292, -105.139933186621 40.11057045894069, -105.1401831872421 40.11054845896744, -105.1402242919559 40.11052569800182, -105.1402249272183 40.11052579274737, -105.1403254691414 40.11047119351303, -105.1404621873911 40.11037345868738, -105.1406051874184 40.11035645826706, -105.1406771869243 40.11047245857907, -105.1407334051194 40.11062448513666, -105.1407481874379 40.11066445856965, -105.140834187162 40.11075245890581, -105.1409411875114 40.11075745877094, -105.1411311766261 40.1106291019769, -105.1413141878553 40.1105054587965, -105.1413481734702 40.11044279920952, -105.1413941070261 40.11035810907864, -105.1414421879518 40.11026945914983, -105.1414707361548 40.11017746660836, -105.1414781867133 40.11015345869473, -105.1415522170272 40.11016179340662, -105.1416291874734 40.11017045872525, -105.1416791872043 40.11020345863564, -105.1417791876447 40.11018145895183, -105.1418291878365 40.11010445836963, -105.1418291876094 40.11005455446081, -105.1418291868519 40.10988545812238, -105.1418336763905 40.10988134348353, -105.1419011880146 40.10981945778273, -105.1419941874593 40.10979745872118, -105.1420791878335 40.10989045903131, -105.1420893355731 40.10999193837458, -105.142101188436 40.11011045872333, -105.142126431106 40.11012005767923, -105.1421721882141 40.11013745854567, -105.1423603463296 40.11012042383983, -105.142415188456 40.11011545817529, -105.1424617281768 40.1101221067335, -105.1425371920236 40.11013288780438, -105.1425655734614 40.11013694209405, -105.1425889933667 40.11014028752435, -105.1426306946563 40.11014624465503, -105.142676579207 40.11015280013385, -105.142723188132 40.11015945870771, -105.1428108591608 40.11016490951189, -105.1429161884725 40.11017145869828, -105.1429648250731 40.11017641491812, -105.1429648182534 40.11017771543015, -105.1429664300369 40.11017657839365, -105.1430731876633 40.11018745855665, -105.1431521881496 40.11013245795137, -105.1431796482247 40.11002829750333, -105.1432101875002 40.10991245887465, -105.1433101881548 40.10983045861817, -105.1433261756351 40.10975684233937, -105.143353188753 40.10963245825586, -105.1433382934257 40.10957753407826, -105.143311550045 40.10947891718003, -105.1432891876009 40.10939645879092, -105.1432609860456 40.10935610828796, -105.1432241877329 40.10930345901374, -105.1432328627724 40.10926008276815, -105.143246187286 40.10919345809153, -105.1433391874849 40.10910545859052, -105.1434139958149 40.10909877173545, -105.1435181878683 40.10908945828713, -105.1436391882093 40.10914945901379, -105.1437251880138 40.10919945804216, -105.1438211598157 40.10919242101242, -105.1438751876574 40.10918845906782, -105.1439693495291 40.10914216706989, -105.1440541880079 40.10910045846919, -105.144096572717 40.10909719816408, -105.144123205141 40.10909515020784, -105.1441548387739 40.1090927168681, -105.1441971870977 40.10908945911586, -105.1442691886938 40.10915545782236, -105.144345777039 40.10927439618445, -105.1443541882314 40.10928745804113, -105.1444693672245 40.10929912209676, -105.1444797799127 40.10930245231871, -105.1444972586797 40.10930194682363, -105.1446208477053 40.10929837426536, -105.1447756584748 40.10929241273082, -105.1448795350452 40.10928805784319, -105.1450518589718 40.10928083304527, -105.145156188375 40.1092764585858, -105.1452858210533 40.10929371331622, -105.1454491885845 40.10931545852137, -105.1456711885987 40.10930945796668, -105.1457684551437 40.10927877952781, -105.1459173643046 40.10923181175473, -105.1459501886296 40.1092214585894, -105.14603607745 40.10920312262454, -105.1461281887017 40.10918345829599, -105.1462641887339 40.10909045812184, -105.1463979289381 40.10907882875447, -105.1465861886723 40.10906245846613, -105.1466952183154 40.10908102655211, -105.146815189195 40.10910145810936, -105.1469201518979 40.10911105121482, -105.1470011879937 40.10911845817668, -105.1470486443322 40.10911952728623, -105.1471561250959 40.10912194792165, -105.1472231888622 40.10912345873804, -105.1472670149087 40.10914467042698, -105.1473230421344 40.10917178706982, -105.1474308225596 40.10922395285124, -105.1474731885267 40.10924445749985, -105.1475425064825 40.10924445742264, -105.1476126056347 40.10924445788622, -105.1476639806363 40.10924445792431, -105.1477521893066 40.10924445771168, -105.1478568619915 40.10927209172333, -105.1480021884751 40.109310458268, -105.1481495371838 40.10931457831904, -105.1483626110154 40.10932053569708, -105.1484881807936 40.10932404681184, -105.1486101887807 40.10932745778867, -105.148681535631 40.10935141047885, -105.1486906073675 40.10935551079681, -105.1487742892276 40.10938470218268, -105.1488282710606 40.10942647438896, -105.1489321887245 40.1095144583186, -105.1489961900791 40.10967345746549, -105.1490951105112 40.10978119433448, -105.1491636738781 40.10981642606204, -105.1492181885192 40.10984345882783, -105.1493760472449 40.1098539470783, -105.1495327897234 40.10986436057436, -105.1498051887075 40.10988245858211, -105.1499037995298 40.10983605366251, -105.1500261889393 40.10977845814232, -105.1500616825502 40.10974049989558, -105.1500969366913 40.10970279759637, -105.1501310738441 40.10966628976156, -105.1501701894573 40.10962445796797, -105.150213190036 40.10948145755771, -105.150192927634 40.10942765734119, -105.1501841896918 40.10940445815319, -105.1501460270222 40.10937066109187, -105.150113914031 40.10934222227647, -105.150035810524 40.10927305377975, -105.1499481896146 40.10919545785707, -105.1499411886424 40.10911345803316, -105.1500271894042 40.10901445758356, -105.1501361731898 40.10894852276716, -105.1501628272604 40.1089323972873, -105.1501829687099 40.10892021131422, -105.1501990355049 40.1089104906731, -105.150216358927 40.10890001008798, -105.1502271897408 40.1088934573679, -105.1502991895659 40.10876745797281, -105.1503701892914 40.10874045812216, -105.1505561895843 40.10874045817922, -105.1507351896093 40.10865745754312, -105.1509501898016 40.10867945738578, -105.1510291895926 40.10873445721234, -105.1511498943537 40.108892914989, -105.1512721889252 40.10905345792743, -105.151443190266 40.10915745838717, -105.1515425217955 40.10915797339747, -105.1516361903776 40.10915845863114, -105.152058189739 40.10899345806407, -105.152168642065 40.10888557367066, -105.1521720437602 40.10888555509551, -105.1521871900507 40.10886745719991, -105.1522441899349 40.10883445806299, -105.1522521895131 40.10872445833751, -105.1522161898024 40.10867445774499, -105.1519151896514 40.1086254581982, -105.1518011892207 40.10854845784844, -105.1518081899357 40.10844445794176, -105.1520521905081 40.10809245803009, -105.1521161891182 40.10785645730169, -105.1522381891769 40.1078014575306, -105.1526961899649 40.10774645807478, -105.1530101897713 40.1076424577811, -105.1531681905297 40.10752745787505, -105.1532041904084 40.10742245698562, -105.1531971895655 40.10730745767818, -105.1530821895656 40.10724745707277, -105.1527891896304 40.10716445739909, -105.1527461895664 40.10708745705721, -105.1528251898034 40.10689545706076, -105.1528251894787 40.1068184572149, -105.1529611896807 40.10678045703483, -105.1532181895994 40.10680245729557, -105.1534041890178 40.10683545695765, -105.153533190452 40.10679645699769, -105.1536831893247 40.10669845729011, -105.1538481902248 40.10664345777509, -105.1543781900811 40.10669245702027, -105.1546631906193 40.10667645674386, -105.1549851905804 40.10658345749179, -105.1551071895624 40.106484457227, -105.1551781906975 40.10638545677693, -105.155372190027 40.10630845692795, -105.1557151895679 40.10621545706669, -105.1564161904518 40.10613345690832, -105.1565797245652 40.10604856929712, -105.1569951900118 40.10582045723518, -105.157138190582 40.10579245659894, -105.157239191129 40.10571045628147, -105.157253190884 40.10562845707536, -105.1571241900853 40.10546345672344, -105.1571241898577 40.1053754563856, -105.1572321903226 40.10529845652795, -105.1576681914213 40.10507845747404, -105.1580761909817 40.10495245717316, -105.1581892413284 40.10490396872007, -105.1584981900914 40.10477145654381, -105.1587201908592 40.10476045668218, -105.1588991905787 40.10458445709242, -105.1589061910858 40.10450845692532, -105.1588201907179 40.10434845704976, -105.1588411915942 40.10426645671227, -105.1590781918603 40.10400245670831, -105.1594259918098 40.10399197542836, -105.1594495599439 40.10886022285561, -105.1594520114176 40.10922888777313, -105.1594718259507 40.11205812132699, -105.159467921669 40.11419687283805, -105.1594566443818 40.11609286922273, -105.1594641412873 40.11689641328065, -105.1609821531084 40.11566321114483, -105.1614528663692 40.11528080007928, -105.1674439177613 40.11003576716704, -105.1685799278165 40.10901976085416, -105.1688417643584 40.10884061707407, -105.1763019499671 40.1023029683946, -105.1770289540793 40.10167497796913, -105.1842254973132 40.09480566330672, -105.1842981568986 40.09474644455597, -105.1847611298219 40.09436911199498, -105.1847691909817 40.09436254127205, -105.1851806430128 40.0943560507158, -105.1851823083869 40.09435602463465, -105.1864923089405 40.09436502536359, -105.1869288298045 40.09436799308698, -105.1869333094328 40.09436802324625, -105.1878489982433 40.09436703406432, -105.1878583084638 40.09436702410904, -105.1878579783739 40.09437328631103, -105.1878581437286 40.09437328585741, -105.1878581347478 40.09437345425398, -105.1878554742897 40.09442402015232, -105.1878551441828 40.09443028595678, -105.1914201445046 40.09443828540665, -105.1941921454042 40.0944432846204, -105.1961591443175 40.09444728514715, -105.1999431444402 40.09446928464906, -105.20004901646 40.0944713051883, -105.2000942419318 40.09447216840297, -105.2004028346573 40.09447194731246, -105.2020925487541 40.09447072187066, -105.204067954345 40.09447526321931, -105.206084292794 40.09448027846468, -105.2067696857456 40.09448197611559, -105.206769231588 40.09440878489543, -105.2067688747363 40.09435139755085, -105.2069082004758 40.09435075068787, -105.2069747075104 40.09435044215074, -105.2069438669998 40.08890529265857, -105.2069481319076 40.08890527106102, -105.2075245971012 40.08890693460845, -105.208456199712 40.08891645102268, -105.2093902465011 40.08891684883024, -105.2102848781325 40.08891722213826, -105.2102854292613 40.08891722262064, -105.2102871823232 40.08891722341717, -105.2102892648914 40.08891722413985, -105.2102906849293 40.08891722500127, -105.2114362013246 40.08891745132185, -105.213437201397 40.08892445097817, -105.2143002021996 40.08892245043239, -105.2148042021617 40.08892745043244, -105.2148588360544 40.08892679371123, -105.2159742024865 40.08892045011142, -105.2162802020392 40.08892045046189, -105.2163292022599 40.08892045018143, -105.216360202134 40.08892145040806, -105.2163692023297 40.08714545077098, -105.2182532019159 40.08714945059754, -105.2182432027494 40.08641344971119, -105.2191138039488 40.0864074176304, -105.2211262032423 40.08639345027048, -105.2211162029895 40.08627444986659, -105.2219812039535 40.08618344991433, -105.2230462031982 40.08603244956893, -105.2246852045713 40.08554044892636, -105.2246712037403 40.08611344976358, -105.2258422045073 40.08612344890279, -105.2258472562248 40.08702557574974, -105.2258472559384 40.08702564690012, -105.2258442047025 40.08817345056035, -105.2258660799562 40.08846674914248, -105.225866596984 40.08846589835929, -105.2259971464311 40.08825128178296, -105.2260951784236 40.08815046645809, -105.2260799511012 40.08815043483378, -105.2260289772142 40.08815032829153, -105.2260301833774 40.08814810745953, -105.2260316128055 40.08814547826421, -105.2260330445643 40.08814285267693, -105.2260344868726 40.08814022801536, -105.226035930357 40.08813760245592, -105.2260373773409 40.08813498140795, -105.2260388290152 40.08813236037112, -105.2260402865523 40.08812973934819, -105.2260417429166 40.08812711832244, -105.2260432086508 40.08812450002085, -105.2260446767192 40.08812188442674, -105.226046152992 40.08811926975269, -105.2260476280957 40.08811665417521, -105.2260491125655 40.08811404222255, -105.2260505993841 40.08811142937476, -105.2260520885404 40.08810881833376, -105.2260535823798 40.08810620910523, -105.2260550832546 40.0881035998933, -105.2260565841257 40.08810099158206, -105.2260580920141 40.08809838779062, -105.2260596034202 40.08809578400751, -105.2260611230379 40.08809317934323, -105.2260626414721 40.08809057737804, -105.2260641669416 40.08808797542954, -105.2260656970834 40.08808537799534, -105.2260672295774 40.08808277876541, -105.2260687690924 40.08808018315465, -105.2260703097799 40.08807758754672, -105.2260718574956 40.08807499375673, -105.2260734087289 40.088072399975, -105.2260749611275 40.0880698079974, -105.2260765193853 40.08806721693423, -105.226078084664 40.08806462949036, -105.2260796499462 40.0880620411458, -105.2260812222603 40.08805945371852, -105.2260827980811 40.08805686900151, -105.2260843809301 40.08805428610243, -105.2260859637863 40.08805170140207, -105.2260875536562 40.08804912212216, -105.2260891482163 40.08804654285341, -105.2260907451214 40.08804396359018, -105.2260923455334 40.08804138703718, -105.2260939506355 40.08803881049528, -105.2260955615934 40.08803623576855, -105.2260971760652 40.08803366195077, -105.2260987916986 40.08803109083762, -105.2261004178852 40.08802851974954, -105.2261020440572 40.08802595226398, -105.2261036725816 40.08802338298269, -105.2261053092994 40.08802081732343, -105.2261069495313 40.08801825257306, -105.2261085932736 40.08801568963229, -105.2261102405372 40.08801312579922, -105.2261118948289 40.0880105637841, -105.2261135491024 40.08800800627216, -105.2261152092496 40.08800544607216, -105.2261168764069 40.08800289219328, -105.226118542406 40.08800033470907, -105.2261202165914 40.08799778264812, -105.2261218943052 40.08799522789362, -105.2261235755077 40.08799268035245, -105.2261252602387 40.08799013011774, -105.226126950829 40.08798758079754, -105.2261286460914 40.08798503599166, -105.2261303460513 40.08798248939556, -105.2261320460038 40.0879799446007, -105.2261337541534 40.08797740252725, -105.2261354658207 40.08797486046209, -105.2261371809875 40.08797232290842, -105.2261388996683 40.08796978626372, -105.2261406218776 40.08796724692545, -105.2261423475865 40.08796471209865, -105.2261440803236 40.08796217908979, -105.2261458165711 40.08795964789051, -105.2261475563434 40.08795711489833, -105.226149300777 40.08795458912228, -105.2261510475738 40.08795205884863, -105.2261528013842 40.08794953399544, -105.2261545551981 40.08794700824161, -105.2261563172056 40.08794448610973, -105.2261580815545 40.08794196488402, -105.2261598505936 40.08793944366944, -105.2261616231395 40.08793692516508, -105.2261634015482 40.08793440667458, -105.2261651799496 40.08793188998534, -105.2261669688859 40.08792937782427, -105.2261687566533 40.08792686475982, -105.2261705502725 40.0879243544111, -105.226172348582 40.08792184407345, -105.2261741480568 40.08791933553987, -105.2261759557322 40.08791682882699, -105.2261777645729 40.08791432391816, -105.2261795792655 40.08791182172511, -105.2261813974722 40.08790932044101, -105.2261832203618 40.08790682096924, -105.2261850455965 40.08790432150305, -105.2261868778629 40.08790182295415, -105.2261887112837 40.08789932891115, -105.2261905517435 40.08789683398418, -105.2261923945412 40.08789434086405, -105.2261942361589 40.08789184954237, -105.226196091833 40.08788936185654, -105.226197947507 40.08788687417072, -105.2261998043462 40.08788438828893, -105.2262016682208 40.08788190242377, -105.226203534426 40.08787942016669, -105.2262054064867 40.08787693972477, -105.2262072808852 40.08787446108968, -105.2262091611538 40.08787198066713, -105.2262110437421 40.0878695065546, -105.2262129298625 40.08786702884783, -105.2262148218203 40.0878645574594, -105.2262167161233 40.08786208607652, -105.2262186162781 40.08785961740938, -105.2262205211268 40.08785714785272, -105.226222428306 40.08785468190413, -105.2262243401755 40.08785221596659, -105.2262262543791 40.08784975273657, -105.2262281732657 40.08784729131887, -105.2262300991841 40.08784483081848, -105.226232023919 40.08784237301715, -105.2262339568581 40.08783991613592, -105.2262358933076 40.08783746106425, -105.2262378332675 40.08783500780219, -105.2262397767451 40.08783255454839, -105.2262417237222 40.08783010580613, -105.2262436742169 40.08782765707216, -105.2262456270494 40.08782521014498, -105.2262475892516 40.08782276594194, -105.2262495549714 40.08782032174722, -105.2262515195077 40.08781788025156, -105.2262534898923 40.08781544237237, -105.2262554673158 40.08781300360911, -105.226257445901 40.08781056755058, -105.2262594326977 40.0878081306108, -105.2262614183 40.08780569907206, -105.2262634085889 40.08780326844501, -105.2262654059096 40.08780083873525, -105.2262674008741 40.08779841172184, -105.2262694052227 40.08779598382996, -105.2262714142507 40.0877935586511, -105.2262734244331 40.08779113797818, -105.2262754393057 40.08778871731626, -105.2262774576886 40.08778629846402, -105.2262794831069 40.0877838796284, -105.2262815085034 40.08778146619655, -105.2262835374175 40.08777905277302, -105.2262855745432 40.08777663846826, -105.2262876128304 40.08777422686813, -105.2262896569624 40.08777181978507, -105.226291699918 40.08776941359987, -105.2262937499053 40.08776700833194, -105.2262958045756 40.08776460487633, -105.2262978662741 40.08776220323865, -105.2262999267926 40.08775980339941, -105.2263019919905 40.08775740627321, -105.2263040642092 40.08775501276614, -105.2263061352625 40.08775261745505, -105.2263082145056 40.08775022666651, -105.2263102972735 40.08774783408501, -105.2263123800232 40.08774544600666, -105.226314467456 40.08774305974064, -105.2263165619241 40.08774067349134, -105.2263186598953 40.08773829085281, -105.2263207637256 40.08773590912882, -105.226322866376 40.08773352920324, -105.2263249737094 40.08773115109006, -105.2263270845495 40.0877287756871, -105.2263292047701 40.08772640030627, -105.2263313249726 40.08772402942868, -105.226333448689 40.08772165945994, -105.2263355759121 40.08771929220145, -105.2263377078255 40.08771692495404, -105.2263398455944 40.08771455952174, -105.2263419810035 40.08771219768641, -105.2263441269622 40.08770983677667, -105.2263462740824 40.08770747857164, -105.2263484247239 40.08770511947421, -105.2263505776958 40.08770276398484, -105.2263527353471 40.08770041120849, -105.226354900023 40.08769806115065, -105.2263570647023 40.08769571019219, -105.2263592363989 40.0876933637535, -105.2263614080953 40.08769101731477, -105.2263635879888 40.08768867359738, -105.2263657702201 40.0876863316868, -105.2263679524405 40.08768399247809, -105.2263701416961 40.08768165328597, -105.2263723344585 40.0876793168041, -105.2263745307277 40.0876769830324, -105.2263767305145 40.08767464926904, -105.2263789361496 40.08767231912204, -105.2263825065714 40.08766855838156, -105.2263977138776 40.0876481506639, -105.2264158800905 40.08762967283475, -105.226434455812 40.08761141663134, -105.2264521500162 40.08759367350561, -105.2264697795498 40.08757626436348, -105.2264878009205 40.08755909752002, -105.2265062070929 40.08754217295839, -105.226524998038 40.0875254978835, -105.2265441631842 40.08750907677334, -105.2265637001611 40.08749291592657, -105.22658359957 40.0874770198241, -105.2266038602236 40.08746139206541, -105.2266244715363 40.08744604073107, -105.2266454253037 40.08743096490092, -105.2266667226549 40.08741617538511, -105.2266883530404 40.08740167125784, -105.2267103070542 40.08738745880117, -105.2267325834878 40.08737354701852, -105.2267551729715 40.08735993318564, -105.226778067272 40.08734662358735, -105.2268012569799 40.08733362540633, -105.2268247444441 40.08732093774738, -105.2268485155578 40.08730856958332, -105.2268725621166 40.08729651999401, -105.226896880574 40.08728479617606, -105.2269214580284 40.08727339899931, -105.2269223132005 40.08727301824765, -105.2269462956309 40.08726233387031, -105.2269713781346 40.08725160165343, -105.226995713506 40.08724120810847, -105.2270202222304 40.08723115271041, -105.2270449570381 40.08722144459034, -105.227069908556 40.08721208192462, -105.2270950662131 40.08720306919137, -105.2271204311677 40.08719440999577, -105.2271459834793 40.08718610609185, -105.2271717266588 40.08717815928905, -105.2271977580158 40.08717057341977, -105.2272236163383 40.08716344466387, -105.2272444844378 40.08716355701311, -105.2272912108504 40.08716386193717, -105.2280258931392 40.08716865993154, -105.2283729549368 40.08717092525384, -105.229337317657 40.08728913118895, -105.2315411374752 40.08755923148525, -105.2315951034686 40.08756556421094, -105.2316492191852 40.08757169551478, -105.2317034632943 40.08757708676092, -105.2317578193674 40.08758174061293, -105.2318122651521 40.08758564981383, -105.2318667865754 40.08758881433079, -105.2319213672231 40.08759123322496, -105.2319759906559 40.08759291186197, -105.2320306369806 40.0875938393878, -105.2320852944376 40.08759402388102, -105.232139950141 40.08759346170912, -105.2321945759326 40.08759215640933, -105.2322491612788 40.08759010255342, -105.2323036897474 40.08758730370593, -105.2323581460858 40.0875837616329, -105.2324125138727 40.08757947719696, -105.2324667696581 40.08757444944327, -105.2325209052109 40.08756868375681, -105.2325748982646 40.08756217648359, -105.2326288764451 40.08755497475301, -105.2326832836757 40.08754720298132, -105.232737453437 40.08753868580036, -105.2327913728077 40.08752942858451, -105.2328450159892 40.08751943127434, -105.232898377103 40.08750869745924, -105.2329514268327 40.08749722707182, -105.2330041639691 40.08748502911613, -105.2330565603615 40.08747210532881, -105.2331086089517 40.08745846109794, -105.2331195646996 40.08745541432238, -105.233160289808 40.08744409547717, -105.2332115864704 40.0874290192368, -105.2332572252643 40.08741486387087, -105.2333106562827 40.0873970203308, -105.2333632162177 40.08737853169327, -105.2334153508784 40.08735934044687, -105.2334670391323 40.08733945284803, -105.2335182680553 40.08731887517195, -105.2335350154684 40.08731185997121, -105.2335198087319 40.087300620841, -105.2334842065225 40.08728144947539, -105.233557508418 40.08725212883198, -105.2336642062275 40.0872094484582, -105.2337498879304 40.08716518662143, -105.2338752055783 40.08710044895112, -105.2340141176357 40.08701357127359, -105.2340547143473 40.08698818193187, -105.234116919408 40.08694927681879, -105.2341742062996 40.08691344866173, -105.2342102060382 40.08689144861766, -105.2342874907976 40.08682176614175, -105.2344114016713 40.08671004247304, -105.2346296381483 40.08650825210744, -105.2347532059639 40.0863524487831, -105.2349272055709 40.08608544943124, -105.2351162069385 40.08560644881669, -105.2351382054217 40.08551144874158, -105.2350852057845 40.0846124484227, -105.2350776389745 40.08420165278985, -105.2350497203358 40.08268589163298, -105.2350032064051 40.08016044862552, -105.2299052044168 40.08008044876753, -105.2334432055741 40.07899144749057, -105.2352892054144 40.07873844737262, -105.2366591894632 40.0785191707074, -105.2370786377037 40.07845203165877, -105.2378132062725 40.07833444783447, -105.2384812068036 40.07833244791702, -105.2403432064991 40.07833344770941, -105.2422160069221 40.0783371534334, -105.2423652076105 40.07833744689923, -105.2435522068469 40.07833844725607, -105.2446880588089 40.07833844686491, -105.2446880583013 40.07833920790986, -105.245048207299 40.07833944731037, -105.2453581543005 40.07833797981056, -105.2453582656843 40.07833797915564, -105.2467352086361 40.07833144715077, -105.2479762077927 40.07832544680577, -105.2505104677892 40.07831279674013, -105.2509901360399 40.07831039739476, -105.2509912135285 40.07831039161324, -105.2528018115011 40.07830197852396, -105.2528020506824 40.07830197723486, -105.2552788447606 40.07829042246069, -105.2603639449122 40.0782650686866, -105.2610523420133 40.07826161962124, -105.2611378514393 40.07826119045901, -105.263475212196 40.07824944591677, -105.2635022120304 40.08020744623987, -105.265906623877 40.08014227963445, -105.2678107184368 40.08009626548748, -105.269120467453 40.08006436083225, -105.270773469619 40.08002883906712, -105.271602868858 40.08001390036796, -105.2722111865051 40.0800029400344, -105.2732488422515 40.07998423568615, -105.2738472151207 40.07997344533944, -105.2741904007602 40.07997698391911, -105.2752363556628 40.07998199733333, -105.2752365174616 40.07998199764835, -105.2752366651909 40.079981997936, -105.2752368011957 40.07998199820081, -105.275236925476 40.07998199844278, -105.2752370110651 40.07998199860944, -105.2760592152198 40.07997644544199, -105.2774492150437 40.079994445459, -105.2774442150245 40.07989344467622, -105.2775032146846 40.07989444554472, -105.277486220627 40.07914765992864, -105.277462332525 40.07819215800942, -105.2774232152314 40.07679644423713, -105.2774182151642 40.07662844439344, -105.277414215237 40.07647944379102, -105.2774795717141 40.0764360956394, -105.2776022148752 40.07633644500343, -105.2777612150901 40.07620044483633, -105.2779022152453 40.07603844420503, -105.2780202147794 40.07579044515734, -105.2783742148064 40.07579144511136, -105.278372214492 40.07653744417692, -105.2782532143109 40.07666244408787, -105.2821112161553 40.07666744386643, -105.2821342160606 40.0791254445771, -105.2822223466844 40.07989150774977, -105.2822036751846 40.07998723360745, -105.2822148038009 40.07998772474011, -105.2822150312255 40.07998773507623, -105.2823430660183 40.07999338222898, -105.2823919994679 40.07989699918794, -105.2823952780968 40.07991484894792, -105.2823021518433 40.08009827885829, -105.2822277607727 40.08031775722681, -105.2821622666328 40.08051098862354, -105.2821612415979 40.08051401375702, -105.2821593066155 40.08068901713151, -105.2821463073063 40.08169901632542, -105.2821403062932 40.0821320170198, -105.2821423070911 40.08263701682382, -105.2821423075853 40.08554501716329, -105.2821623079241 40.08608101577435, -105.2821621432272 40.08608704978086, -105.282162143671 40.08608727764472, -105.2821423153658 40.0868150166831, -105.2821421522846 40.08682127765446, -105.2821479765674 40.08702801532603, -105.2821481523551 40.0870342787379, -105.2821390907224 40.08703424902927, -105.2821441072337 40.08721088474018, -105.282137898842 40.0899340794033, -105.2821399488127 40.09152792746865, -105.2821341594649 40.09311407433201, -105.2821409624091 40.09422807602022, -105.2821221684136 40.09529810758003, -105.2821321056455 40.09710801302935, -105.2821051272783 40.09794304108583, -105.2820501495957 40.09926089139519, -105.282012830953 40.09975193069047, -105.2819761427939 40.10038105317948, -105.2819768350256 40.10072310238548, -105.2819774149438 40.10073831713714, -105.2819782232338 40.10075949547533, -105.2819900265868 40.10106901821791, -105.2819991328603 40.10135096358122, -105.2820498498076 40.10248206645011, -105.2821380164751 40.10397587712918, -105.2821500312105 40.10435500626381, -105.2821711087647 40.10503008189505, -105.2821721304822 40.10538091547843, -105.2821429877803 40.10588597033826, -105.2821100589534 40.10623289769167, -105.2820620998125 40.10658501047332, -105.2820240687228 40.10696212396728, -105.2818538952916 40.10852407589721, -105.28182207568 40.10885892394143, -105.2818161192508 40.10960202947805, -105.2818530515338 40.11001497049595, -105.281895999471 40.11033596102865, -105.282007019785 40.11112595402247, -105.2820288722131 40.11126901713702, -105.2820480529635 40.1114200377739, -105.2821319186914 40.11202687618564, -105.2822329804653 40.1128470466918, -105.2822851112858 40.11342801985863, -105.2822921703681 40.1144629590239, -105.2822860850855 40.11569497494339, -105.2822928240271 40.11638292419469, -105.2822928495963 40.11704588145643, -105.28230101788 40.11773410707254, -105.282302930207 40.11847804797252, -105.2823001360619 40.11979901308963, -105.2823039641844 40.12106206847565, -105.2822998880501 40.12211290531759, -105.2823098954699 40.12368013430066, -105.2823120718964 40.12389398635925, -105.2823138398862 40.12412403384995, -105.2823129161732 40.12418909163625, -105.2823108265935 40.12473098201075, -105.2823120082232 40.12503212758082, -105.2823139370068 40.12565912601642, -105.2823230762417 40.12615601536589, -105.2823149319752 40.12680193517511, -105.2823240983905 40.12807295927798, -105.2823100945402 40.12932087953102, -105.2823079566542 40.1295421346564, -105.2823048796789 40.12994511718988, -105.2823158253697 40.13054797525448, -105.2823018622755 40.13100007518779, -105.28227995875 40.13192213067715, -105.282278130057 40.13238193944374, -105.2822721443784 40.13369411122954, -105.2822869464721 40.13488086839918, -105.2822871155677 40.13605798978642, -105.2822808526307 40.13667399035533, -105.2822689487237 40.13804709279694, -105.2822731345116 40.13942187166376, -105.2822709455559 40.14021796128176, -105.2822679484925 40.14104287330215, -105.2822708529094 40.14181206938772, -105.2822551592731 40.14347505101375, -105.2822531667241 40.14398591947473, -105.2822421489368 40.14497003421873, -105.2822411001326 40.14507407386814, -105.2822446</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" t="n">
+        <v>17</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>Lyons Middle Senior</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>100 McConnell Dr, Lyons, CO 80540</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>https://lmshs.svvsd.org/</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>Lyons Middle/Senior High School</t>
         </is>
       </c>
-      <c r="J13" t="n">
+      <c r="K13" t="n">
         <v>40.2147599852984</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>-105.264461148759</v>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="N13" t="inlineStr">
         <is>
           <t>https://lmshs.svvsd.org/</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>POINT (-105.264461148759 40.2147599852984)</t>
         </is>
@@ -1299,56 +1340,59 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MULTIPOLYGON (((-105.1784019212843 39.92870168376908, -105.1818511117197 39.92869648384348, -105.1838441764116 39.92869343178848, -105.1841991763519 39.92873643054561, -105.1843711756133 39.92868243090511, -105.1846711757492 39.92865043161049, -105.1848971762652 39.92868243096175, -105.1851551757211 39.92870443083596, -105.1853591757001 39.92871443082796, -105.185584175611 39.92863943112477, -105.1857881765031 39.92869343037078, -105.1860781767717 39.92871443107489, -105.1862427122102 39.92871305375947, -105.1874398749427 39.92870302575108, -105.188280750955 39.92869597460466, -105.1891882146993 39.92868835848437, -105.1900135071195 39.92868142556227, -105.1912021775201 39.92867143016532, -105.1921605878346 39.92866908889513, -105.1952731788288 39.9286614295662, -105.1953454862046 39.92714404290943, -105.1954277266185 39.92535293082255, -105.1954701680578 39.92442856826072, -105.1954828953945 39.92415135493398, -105.1955126848871 39.9235025188834, -105.1955539541151 39.92260363548544, -105.1955832718303 39.92176253388807, -105.1956074363542 39.92104863795893, -105.1956271775804 39.92046542890528, -105.1956491770346 39.92026642822356, -105.1957021779222 39.92016442965017, -105.1958741782275 39.91996042930643, -105.1960031773458 39.91985842861604, -105.1960461779453 39.91979442941913, -105.1963542841982 39.91947358440687, -105.1969171547176 39.91888743134161, -105.1971382584971 39.91865717884937, -105.1975931774295 39.91818342841723, -105.1977971773725 39.91800542846681, -105.1980761776685 39.9178604287125, -105.1988809443973 39.91750583145522, -105.199981771958 39.9170207684681, -105.2005472795797 39.91677157902036, -105.2013773094024 39.91640582131284, -105.2019980528428 39.91613227988852, -105.2026927027816 39.91582616438962, -105.2029610455153 39.91570919533338, -105.2032861789647 39.91558342752357, -105.2034951787843 39.91545442818257, -105.2036994329652 39.91536577400033, -105.2039238798093 39.91526835479848, -105.2044351788381 39.9150464284585, -105.2046181793619 39.91493942746109, -105.2047771484222 39.9148745542603, -105.2051264319463 39.91473201341331, -105.2055840142236 39.91454527467528, -105.206223179592 39.91428442723124, -105.2062611795562 39.91424142750945, -105.2062749820281 39.91414793981343, -105.2080811675174 39.91413651982791, -105.2081010480463 39.91413639369402, -105.2082326020008 39.91413556073108, -105.2082437405714 39.91413548987958, -105.2127750952919 39.914106703786, -105.2128870458286 39.91410599043611, -105.213645040396 39.91410184790944, -105.2175004417789 39.91408067426644, -105.2189361314345 39.91407275709121, -105.2212525262855 39.91405994110492, -105.2221488638938 39.91405498129632, -105.2316342538218 39.91406393968015, -105.2328366111099 39.91406370115187, -105.2386024786223 39.91406237558283, -105.238920889073 39.91406229633754, -105.2392698990356 39.91406220443915, -105.239915923657 39.91406203514502, -105.2402281491856 39.91406195092515, -105.2405279089477 39.91406186839333, -105.2412789148089 39.91406166045791, -105.2459316121797 39.91403871789947, -105.2501535052445 39.91401773192297, -105.2598916796428 39.91397305810732, -105.2600457617387 39.91397082590954, -105.2654909078388 39.91389125974047, -105.2666177593649 39.91387476217126, -105.2692129079631 39.91383672570182, -105.2759740475008 39.91371767073185, -105.2763431408977 39.91371116039856, -105.2811042377732 39.91371047397082, -105.2816813633473 39.9137103780077, -105.2819189247833 39.91371033909354, -105.2826022004646 39.91371022423816, -105.2838975683199 39.91370999020454, -105.2841657430803 39.91370993925377, -105.2845492353484 39.91370986571884, -105.285848204384 39.91370961828155, -105.2953533084801 39.91370800138991, -105.3000747525567 39.91381446987435, -105.3040421127392 39.91390380243763, -105.3047891203881 39.91392060756144, -105.3067655027752 39.91391296285316, -105.307489992947 39.91391015846362, -105.3138618072536 39.91388526812848, -105.3138945250918 39.91388513907664, -105.3140600078973 39.91388448682844, -105.314962656992 39.91387604616386, -105.3149765887619 39.91388835983841, -105.3228091235898 39.92081034046993, -105.322810999039 39.92081199876494, -105.3230754639435 39.92090816782166, -105.3230946808704 39.92091515582619, -105.3232179993169 39.92095999891312, -105.3236539993554 39.92104899939051, -105.3238185156393 39.92104925748924, -105.3238336179889 39.92104928059182, -105.3238539754728 39.92139180765506, -105.3240379379819 39.92434240818668, -105.3242555787687 39.92783278270667, -105.3240442233703 39.93038144497817, -105.3239541807884 39.93152857193745, -105.3205148429798 39.9317151039824, -105.3191391063055 39.9317901419817, -105.3189277387964 39.93544482213235, -105.3152947463766 39.93560825239187, -105.3150107817862 39.93562102376601, -105.3143742582034 39.93564970797279, -105.3095358144376 39.93550462579071, -105.3071402630428 39.93542705711443, -105.3069899024326 39.93542112842958, -105.3069725184858 39.93542044362167, -105.3069620635541 39.93542003071309, -105.3069103940744 39.93541827429448, -105.3069092683438 39.93541834896335, -105.3069535269843 39.93561751436307, -105.3070365248101 39.93587851262632, -105.3070725234688 39.9360675137267, -105.3070965232637 39.93624851219369, -105.3071325228354 39.9364195118327, -105.3071215214023 39.9365905102257, -105.3070635204184 39.93681550897311, -105.30694751905 39.93696950805576, -105.306818518862 39.93700550812312, -105.3067365183501 39.93702350801441, -105.3065845176777 39.937024507514, -105.3064325177913 39.93698850691153, -105.306303518788 39.93693450642142, -105.3061745181336 39.93687250614514, -105.3060220519166 39.93676488394409, -105.3060215182982 39.93676450657076, -105.3058455198719 39.93655750740345, -105.3057515200265 39.93640450647627, -105.3056685207497 39.9362425084482, -105.3056205223492 39.93609850781798, -105.305585522285 39.9359185082124, -105.3055605239748 39.93568450944846, -105.3055245241444 39.9355225104711, -105.3054775255262 39.93536051092015, -105.3054185257825 39.9352255117001, -105.3053475260123 39.93510851162448, -105.3052649411208 39.93500105239805, -105.3051249998132 39.93487599901849, -105.3049609990574 39.9347679983106, -105.3047729999609 39.93465199848702, -105.3043750004235 39.93447299937178, -105.3041400002485 39.93438299901855, -105.3036249993473 39.9342399993314, -105.3033550004067 39.93418699885896, -105.3031559993366 39.93411499904182, -105.3030620004486 39.9340439989491, -105.3030613571231 39.93404313591987, -105.3030605270924 39.93404250944442, -105.3029665280378 39.93391650971581, -105.3028365281158 39.93377250899461, -105.3027425284081 39.93365550934977, -105.3026955304566 39.93353850908618, -105.3027175305075 39.9333315116956, -105.30274053066 39.93320551125296, -105.3027515328109 39.93302451231442, -105.3027395322691 39.93284451334089, -105.3027385331218 39.93272751349467, -105.3026555343237 39.93254751358649, -105.3025744395126 39.93245850672481, -105.3024929994625 39.93238699899254, -105.3023169997215 39.93232499931828, -105.3019069997756 39.93227199824996, -105.3018019998002 39.93225399901318, -105.3016729997055 39.93221799834335, -105.3015790000119 39.93216399873801, -105.3015777603272 39.93216264201322, -105.3015775337403 39.9321625119282, -105.301471534445 39.93204651279913, -105.3014125343503 39.93194751346691, -105.3013765351856 39.93182151241906, -105.3013755377297 39.93146951471951, -105.3013045384598 39.93132551488237, -105.3012215390554 39.93117251653352, -105.3011395392849 39.9310825154602, -105.300857545551 39.93070551454974, -105.3007179891391 39.93056299355572, -105.3007165416099 39.93056151667432, -105.3005405416353 39.93046251704081, -105.300258541759 39.93035551655753, -105.3000245404921 39.93036451610091, -105.2998255407144 39.93035651574085, -105.2996265409012 39.93035651468055, -105.2994985401073 39.93040251280053, -105.2993585393596 39.93050151340886, -105.2992295378499 39.93054751218898, -105.299124538251 39.93056551160236, -105.2989255374498 39.93058351168081, -105.2986565371699 39.93059350921907, -105.2979425358611 39.93053250925767, -105.2977785362033 39.93052350758106, -105.2976145345236 39.93055150739807, -105.2974745341685 39.93059650677375, -105.29729953411 39.93068750674149, -105.2971125337131 39.93079550503958, -105.2968435314715 39.93091350344232, -105.2967035312445 39.93093250348966, -105.2964925312223 39.93093250195601, -105.2962585312108 39.93088850094149, -105.2960563719337 39.93084592573341, -105.2958585855775 39.93080427208812, -105.295847148283 39.93079930450271, -105.2958119503042 39.93077165856035, -105.2957816844527 39.93075581006419, -105.2957414044352 39.93072857119356, -105.2957219621322 39.9307171523971, -105.2956935960834 39.93069431994228, -105.2956681569902 39.93066919149165, -105.2956372964884 39.93064254121168, -105.2956237638325 39.93062237308391, -105.2955785483912 39.93058333758654, -105.2955471287956 39.93054339167713, -105.2955092928667 39.9304939045054, -105.2954749140355 39.93045847282398, -105.2954526680995 39.9304390844845, -105.2954290224646 39.93041557494557, -105.2954147445271 39.93039897567736, -105.2954068553409 39.93038980647571, -105.2953777926859 39.93036449589522, -105.2953347401986 39.93032679351454, -105.2952763762496 39.93028128041745, -105.295274573325 39.93047988761785, -105.2952722289371 39.93073811110776, -105.2952668936788 39.93105153150454, -105.2952189307569 39.93289754368107, -105.295160662098 39.93513982394448, -105.2951595853357 39.93518128110463, -105.290629040115 39.93519372808762, -105.2860766755759 39.93520076136944, -105.2850264897052 39.93519797944938, -105.2839771732097 39.93519518868442, -105.2829408013373 39.93519241095223, -105.2819004552617 39.93518958664934, -105.2808121864995 39.93519349146156, -105.2800887155675 39.9351960772441, -105.2797114034442 39.93519741970312, -105.278656951618 39.93519510654447, -105.2776168693938 39.93519281778027, -105.2765200120783 39.93519044371492, -105.2764859620717 39.93515834754393, -105.2747866320536 39.93355640077568, -105.2747706478011 39.93361397472692, -105.2747423603218 39.93371587032925, -105.2746861686253 39.93391760425664, -105.274475989006 39.93468847254762, -105.2744480828891 39.93479082274935, -105.2736239195408 39.93479817386874, -105.2736102258134 39.93479829736632, -105.2734198916193 39.93444690778491, -105.2733207529988 39.93449712888253, -105.2732794633518 39.93451804827096, -105.2732929660188 39.9352475981247, -105.273205627434 39.93608284252236, -105.2732054606918 39.93608443275637, -105.2731873820246 39.93625731362162, -105.2723902507118 39.93621108668517, -105.2723284207845 39.93638767363275, -105.2722356958043 39.93638920518273, -105.2721475513831 39.93662031538015, -105.2717721351925 39.93717547281373, -105.2694582864074 39.93778338126474, -105.269458297737 39.93778522313335, -105.2694387046704 39.93779073737785, -105.2694348364191 39.93760893088588, -105.2689722975682 39.93761531931789, -105.2689648067507 39.93697763738977, -105.2689647839754 39.93697572434603, -105.2689642246452 39.93692803967598, -105.268962923301 39.9368175091889, -105.2689627153546 39.93679978651981, -105.2689617639647 39.93671860378159, -105.2691360682297 39.93671834980415, -105.2692993042267 39.93671810942311, -105.2693021532052 39.93671810251961, -105.2693057732006 39.93671809986206, -105.2693212793192 39.93671807597465, -105.2694158873298 39.93671793665199, -105.269415158357 39.93668366514719, -105.2694149432323 39.93667357464245, -105.2694131583252 39.93658960360316, -105.2694128787389 39.93657642911547, -105.2694038140611 39.93615028433254, -105.269402414808 39.93608446232579, -105.2693982096128 39.93584833463098, -105.2693961725226 39.9357908856665, -105.2693921113694 39.93566105214616, -105.2665075813326 39.93595690063123, -105.2665040068149 39.93595730138393, -105.2665004826126 39.93595770043715, -105.2664969572278 39.9359581030905, -105.266493433013 39.93595850574616, -105.2664899076251 39.93595890929992, -105.2664863833918 39.93595931735921, -105.2664828626622 39.93595972722687, -105.2664793372618 39.93596013438296, -105.2664758165229 39.93596054695234, -105.2664722946108 39.93596096041988, -105.2664687703433 39.93596137838583, -105.2664652484343 39.93596179095252, -105.2664617276643 39.93596221252799, -105.2664582069067 39.93596263050073, -105.2664546849667 39.93596305207362, -105.2664511665304 39.93596347545478, -105.2664476457418 39.93596390243377, -105.2664441249563 39.93596432851194, -105.2664406076683 39.93596475819975, -105.266437089201 39.93596519058704, -105.266433573086 39.93596561937634, -105.2664300511118 39.93596605085565, -105.2664265326259 39.93596648864649, -105.2664230188169 39.93596692734742, -105.2664195015009 39.93596736514042, -105.2664159841694 39.93596780743661, -105.2664124691871 39.93596824703551, -105.2664089518402 39.93596869383473, -105.2664054368363 39.93596913973796, -105.2664019241723 39.93596958564577, -105.266398405649 39.93597003424361, -105.2663948906264 39.93597048555044, -105.2663913779468 39.93597093596124, -105.2663878664156 39.93597139267883, -105.2663843513806 39.93597184758794, -105.2663808386793 39.93597230430299, -105.2663773271356 39.9359727646229, -105.2663738167588 39.9359732258457, -105.266370301705 39.93597368615828, -105.2663667913096 39.93597415278479, -105.2663632820903 39.93597461761227, -105.2663597693486 39.93597508603516, -105.2663562636176 39.93597555717412, -105.2663527532096 39.93597602740282, -105.2663492451323 39.93597650033816, -105.2663457347119 39.93597697416924, -105.2663422313052 39.93597744981572, -105.2663387196993 39.93597792814752, -105.2663352127703 39.93597840738936, -105.266331707005 39.93597888843473, -105.2663281988966 39.9359793703759, -105.2663246919396 39.93597985772328, -105.2663211849825 39.93598034507053, -105.2663176803685 39.93598083152179, -105.2663141769121 39.93598132157788, -105.2663106699487 39.93598181072613, -105.266307166483 39.93598230348399, -105.2663036618379 39.93598279894131, -105.2663001595173 39.93598329890657, -105.2662966595521 39.93598379437316, -105.2662931560676 39.93598429253451, -105.2662896514038 39.93598479339534, -105.2662861525683 39.93598530057253, -105.2662826525751 39.93598580414454, -105.2662791514057 39.93598630951543, -105.2662756513939 39.93598681849121, -105.266272150209 39.93598732836514, -105.266268650191 39.93598783914199, -105.2662651501605 39.93598835352134, -105.2662616536368 39.93598886880838, -105.2662581571069 39.93598938589656, -105.2662546570671 39.93598990297759, -105.2662511616978 39.93599042276991, -105.2662476651369 39.93599094886435, -105.2662441674276 39.9359914686517, -105.2662406755496 39.93599199385477, -105.2662371778124 39.93599252174779, -105.2662336847551 39.93599304965022, -105.2662301881878 39.9359935775454, -105.2662266951088 39.93599411175222, -105.2662232020297 39.9359946459589, -105.2662197089536 39.93599517926481, -105.2662162158652 39.93599571617321, -105.2662127227706 39.93599625488281, -105.2662092296635 39.93599679719492, -105.2662057388995 39.93599733861106, -105.2662022504722 39.93599788093246, -105.2661987608564 39.93599842865526, -105.2661952724198 39.93599897367843, -105.2661917816278 39.93599952319996, -105.2661882920026 39.93600007362445, -105.266184805878 39.93600062675795, -105.2661813162435 39.93600117988414, -105.2661778301157 39.93600173391802, -105.2661743416417 39.93600228974835, -105.2661708543161 39.93600285188555, -105.2661673693458 39.93600340952411, -105.2661638866907 39.93600397437252, -105.2661604005318 39.93600453741242, -105.2661569108568 39.93600510224636, -105.2661534352183 39.93600566800936, -105.2661499490345 39.93600623825417, -105.2661464663638 39.93600680760531, -105.2661429836744 39.93600738236026, -105.2661395010035 39.9360079517112, -105.2661360194654 39.93600853187225, -105.2661325367759 39.93600910662686, -105.2661290575778 39.93600968679246, -105.2661255795495 39.9360102669603, -105.2661220991689 39.93601085072593, -105.2661186234713 39.93601143360026, -105.2661151384013 39.93601202005809, -105.2661116626851 39.93601260833614, -105.2661081881356 39.93601319751714, -105.2661047089092 39.93601378578784, -105.2661012331743 39.9360143794695, -105.2660977574361 39.93601497405167, -105.266094281701 39.93601556773311, -105.2660908071143 39.93601616772138, -105.2660873313667 39.93601676500521, -105.2660838591105 39.93601736769999, -105.2660803798405 39.93601796857911, -105.2660769110941 39.93601857128082, -105.2660734399892 39.93601917938152, -105.2660699677142 39.9360197874798, -105.2660664954392 39.93602039557795, -105.2660630243279 39.93602100547969, -105.2660595555442 39.93602161898868, -105.2660560867604 39.93602223249754, -105.2660526156242 39.93602284960421, -105.2660491468249 39.93602346761613, -105.2660456780224 39.9360240865286, -105.266042212739 39.93602470274617, -105.2660387450786 39.93602532976669, -105.2660352797673 39.9360259540899, -105.266031810943 39.93602657930655, -105.2660283467954 39.93602720543321, -105.2660248826354 39.9360278351624, -105.2660214172961 39.93602846759107, -105.2660179554636 39.93602910092739, -105.2660144901242 39.93602973335587, -105.2660110294553 39.93603036849571, -105.2660075652672 39.93603100633023, -105.2660041034067 39.936031647772, -105.2660006415461 39.93603228921371, -105.2659971843715 39.93603292886351, -105.2659937224953 39.93603357480826, -105.2659902641352 39.93603421895872, -105.2659868034165 39.93603486850823, -105.2659833462108 39.93603551716411, -105.2659798866434 39.93603617211975, -105.2659764294376 39.9360368207754, -105.2659729757324 39.93603747214006, -105.2659695184955 39.93603812980206, -105.2659660636017 39.93603878656808, -105.2659626098653 39.93603944693898, -105.265959154959 39.93604010730738, -105.2659557012133 39.93604077038, -105.2659522462883 39.93604143615213, -105.265948794867 39.93604210373254, -105.2659453446218 39.93604276951394, -105.2659418908573 39.93604343799007, -105.2659384405965 39.93604410827455, -105.2659349879833 39.93604478215673, -105.26593154122 39.93604545605076, -105.2659280874274 39.93604613263231, -105.2659246441553 39.93604681193715, -105.2659211915295 39.93604748942159, -105.2659177459143 39.93604816962207, -105.2659143014597 39.93604885252684, -105.2659108546589 39.93604953722802, -105.265907407858 39.93605022192915, -105.2659039633878 39.93605090933685, -105.2659005189051 39.93605160034705, -105.2658970767685 39.93605228956062, -105.2658936322857 39.93605298057061, -105.2658901889604 39.93605367518549, -105.2658867491389 39.93605437160874, -105.265883305798 39.93605507072667, -105.2658798648002 39.93605576894862, -105.2658764249599 39.93605647077545, -105.2658729851226 39.9360571717015, -105.265869544106 39.93605787532707, -105.2658661077569 39.93605858256459, -105.2658626679009 39.93605928889429, -105.2658592303724 39.93605999883125, -105.2658557940076 39.93606071057177, -105.2658523576397 39.9360614232128, -105.2658489247817 39.93606213586093, -105.2658454883982 39.93606285300504, -105.2658420543607 39.93606356835247, -105.2658386214777 39.93606428820551, -105.2658351885885 39.93606500985974, -105.2658317556961 39.93606573241451, -105.2658283251405 39.93606645587457, -105.2658248957456 39.93606718203887, -105.2658214675236 39.9360679073048, -105.26581803694 39.9360686388704, -105.2658146075356 39.93606936773635, -105.2658111769426 39.93607010200375, -105.2658077486987 39.93607083357382, -105.2658043192662 39.93607157054531, -105.2658008933467 39.93607230662324, -105.2657974674086 39.93607304810493, -105.2657940403097 39.93607378688219, -105.2657906190483 39.9360745292739, -105.2657871919276 39.93607527435548, -105.2657837694868 39.93607601944651, -105.2657803470459 39.93607676453749, -105.2657769245864 39.93607751503225, -105.2657735021237 39.93607826642751, -105.2657700831709 39.93607901782988, -105.265766660705 39.9360797701256, -105.2657632417304 39.9360805278323, -105.265759822765 39.93608128283692, -105.265756400268 39.9360820441389, -105.2657529883069 39.93608280366088, -105.2657495704865 39.93608356587281, -105.2657461538298 39.93608432988832, -105.2657427383555 39.9360850903035, -105.2657393228439 39.93608586152641, -105.2657359085178 39.93608662824837, -105.2657324953399 39.93608740127714, -105.2657290810043 39.93608817070079, -105.2657256689838 39.93608894733435, -105.2657222569695 39.93608972216647, -105.2657188449551 39.93609049699854, -105.2657154364382 39.93609127544024, -105.265712027915 39.93609205568313, -105.2657086170456 39.93609283772245, -105.265705207343 39.93609362066471, -105.2657017987949 39.93609440811258, -105.2656983937628 39.9360951937661, -105.2656949863907 39.93609597941475, -105.2656915801607 39.93609677317161, -105.2656881762798 39.93609756423111, -105.2656847712289 39.93609835528819, -105.2656813696723 39.93609915085553, -105.2656779645996 39.93609994821697, -105.2656745642067 39.93610074558782, -105.2656711626345 39.93610154565809, -105.2656677610529 39.93610234843027, -105.2656643594682 39.93610315210301, -105.2656609625663 39.93610395488447, -105.2656575644759 39.93610476306737, -105.2656541640455 39.93610557124546, -105.2656507659549 39.93610637942817, -105.2656473713649 39.93610719031987, -105.2656439744225 39.93610800480935, -105.2656405798231 39.93610881840284, -105.2656371852112 39.9361096355988, -105.26563379059 39.9361104554966, -105.265630395981 39.93611127179175, -105.2656270025235 39.93611209349308, -105.2656236125726 39.93611291610208, -105.2656202226155 39.9361137405123, -105.2656168303091 39.93611456761963, -105.2656134438525 39.93611539473874, -105.2656100527098 39.93611622364953, -105.2656066627245 39.93611705616524, -105.2656032750854 39.9361178868843, -105.2655998885975 39.93611872300951, -105.2655965044526 39.93611955823877, -105.2655931179646 39.9361203943638, -105.2655897337918 39.93612123769871, -105.2655863496405 39.93612207472896, -105.2655829654675 39.93612291806367, -105.2655795824613 39.93612376230131, -105.2655762027855 39.93612465878385, -105.2655728252331 39.93612561831667, -105.2655694523606 39.9361265778589, -105.2655660759718 39.93612753919526, -105.2655627019199 39.93612850143685, -105.2655593290254 39.93612946728336, -105.2655559561215 39.93613043583178, -105.2655525855606 39.93613140348413, -105.2655492126535 39.93613237293297, -105.2655458420708 39.93613334688974, -105.2655424726641 39.93613431904748, -105.2655391020812 39.936135293004, -105.2655357361627 39.93613627147327, -105.2655323667433 39.9361372472333, -105.2655290008123 39.93613822930497, -105.2655256337141 39.93613921047346, -105.2655222712866 39.93614019435339, -105.265518905349 39.93614117822608, -105.2655155429089 39.93614216570838, -105.2655121793018 39.93614315228755, -105.2655088180252 39.93614414157337, -105.2655054543994 39.93614513355626, -105.2655020954503 39.93614612644924, -105.2654987353249 39.93614712114109, -105.265495376357 39.93614811943773, -105.2654920185621 39.93614911683608, -105.2654886584148 39.93615011783218, -105.2654853029473 39.93615111883766, -105.2654819474735 39.93615212164437, -105.2654785919965 39.93615312535166, -105.2654752329909 39.9361541344556, -105.2654718833544 39.93615514087652, -105.2654685278493 39.93615615268938, -105.265465175854 39.93615716450925, -105.2654618285416 39.93615817543794, -105.26545847654 39.93615918905895, -105.2654551233559 39.93616020628009, -105.2654517748516 39.93616122351064, -105.2654484251648 39.93616224434134, -105.2654450813217 39.93616326698513, -105.2654417327986 39.93616428961931, -105.265438387776 39.93616531496251, -105.2654350427533 39.93616634030555, -105.2654316977244 39.93616736744988, -105.2654283526798 39.93616839909735, -105.2654250111482 39.9361694298512, -105.2654216684465 39.9361704606026, -105.2654183280661 39.93617149676256, -105.2654149865156 39.93617253292003, -105.265411644962 39.93617356997804, -105.265408306915 39.93617460794378, -105.2654049700225 39.93617565041504, -105.2654016272738 39.93617669467564, -105.2653982973979 39.93617773806172, -105.2653949593197 39.93617878503358, -105.2653916247574 39.93617983021117, -105.2653882901734 39.93618088169328, -105.2653849555955 39.93618193137394, -105.2653816245151 39.93618298466431, -105.2653782934159 39.93618404335844, -105.2653749670152 39.93618509665813, -105.265371632409 39.93618615444431, -105.2653683013096 39.93618721313818, -105.2653649737138 39.93618827364041, -105.2653616461148 39.93618933504321, -105.2653583196703 39.93619040095154, -105.2653549920587 39.93619146595674, -105.2653516679446 39.93619253457162, -105.2653483449973 39.9361936040894, -105.265345024393 39.93619467271121, -105.2653416967531 39.93619574582191, -105.2653383761269 39.9361968207481, -105.2653350531606 39.93619789566948, -105.2653317336979 39.93619897239912, -105.2653284165597 39.93620005363675, -105.2653250947475 39.93620113306347, -105.2653217799491 39.93620221430564, -105.2653184616281 39.93620329914319, -105.2653151456501 39.93620438308478, -105.2653118296596 39.93620547062889, -105.2653085160059 39.93620655907829, -105.2653052035097 39.93620765113261, -105.2653018898465 39.93620874228376, -105.2652985773439 39.93620983613923, -105.2652952660112 39.93621092999692, -105.2652919570059 39.93621202746192, -105.2652886479943 39.93621312672814, -105.2652853378096 39.93621422689249, -105.2652820287885 39.93621532886046, -105.2652787221042 39.93621643173378, -105.2652754165836 39.93621753641067, -105.2652721110505 39.93621864469008, -105.265268807851 39.93621975477546, -105.2652655058277 39.93622086306181, -105.265262202628 39.93622197314698, -105.265258899419 39.93622308593407, -105.2652555973581 39.93622420502795, -105.2652522988257 39.936225318725, -105.2652490002776 39.93622643692521, -105.2652457005564 39.9362275560236, -105.2652424066789 39.93622867693512, -105.2652391069481 39.93622979873529, -105.2652358118756 39.93623092684947, -105.2652325156484 39.93623205045789, -105.2652292240794 39.9362331803803, -105.2652259278427 39.93623430669049, -105.265222636261 39.93623544021534, -105.2652193481923 39.93623657284661, -105.2652160554374 39.93623770726952, -105.2652127720361 39.93623884351279, -105.2652094757617 39.9362399806303, -105.2652061900108 39.93624111957054, -105.2652029030899 39.93624225850828, -105.2651996184902 39.93624340285459, -105.2651963292012 39.93624454989324, -105.2651930492875 39.93624569244763, -105.2651897635082 39.93624683949325, -105.2647621049353 39.9363846692419, -105.2601074640665 39.93777228649274, -105.2591736798439 39.93805987096734, -105.2588379020683 39.93822555703911, -105.2580742502519 39.93844907086968, -105.2580707972867 39.93845110811252, -105.2580673739306 39.93845205381953, -105.2580639505649 39.93845300222836, -105.2580605306933 39.93845395514767, -105.2580571107959 39.93845491527217, -105.2580536944054 39.93845587630452, -105.2580502779924 39.9384568436414, -105.2580468662467 39.93845781459057, -105.2580434521449 39.93845879003799, -105.2580400438867 39.93845976729891, -105.2580366379397 39.93846075267054, -105.2580332319894 39.93846173894266, -105.2580298295299 39.938462730626, -105.258026427048 39.93846372861379, -105.2580230292365 39.93846472931327, -105.2580196337585 39.93846573181887, -105.2580162382485 39.93846674333088, -105.2580128474185 39.93846775485262, -105.2580094553993 39.93846877177572, -105.2580060668709 39.93846979410996, -105.258002683016 39.93847081825532, -105.2579992991355 39.93847184960574, -105.2579959152486 39.93847288275735, -105.2579925360192 39.93847392222328, -105.2579891591138 39.93847496619729, -105.2579857821988 39.93847601287317, -105.257982407611 39.93847706315647, -105.2579790376903 39.93847811705206, -105.2579756665804 39.93847917634906, -105.2579723001377 39.93848023925836, -105.2579689371794 39.93848130938014, -105.2579655730478 39.93848238040005, -105.2579622147438 39.9384834577367, -105.2579588587702 39.93848453778014, -105.2579555027869 39.93848562052543, -105.2579521502944 39.93848670868189, -105.2579487977826 39.9384878022422, -105.2579454475981 39.9384888994099, -105.2579421032475 39.93849000109308, -105.257938756544 39.93849110637386, -105.2579354145046 39.9384922161676, -105.2579320759623 39.93849332957124, -105.257928738574 39.9384944474805, -105.2579254023428 39.93849556899472, -105.257922071952 39.93849669322312, -105.2579187403624 39.93849782555478, -105.2579154122859 39.93849895699314, -105.2579120888575 39.93850009744771, -105.2579087642589 39.93850123789974, -105.2579054431384 39.93850238736557, -105.257902126701 39.93850353594048, -105.2578988090615 39.93850469351932, -105.2578954949353 39.93850585020486, -105.2578921854698 39.938507012304, -105.257888874815 39.9385081798045, -105.2578855688274 39.93850935091735, -105.2578822663274 39.93851052834204, -105.2578789661674 39.93851170577157, -105.2578756659816 39.93851289040624, -105.2578723716331 39.93851407865567, -105.2578690749285 39.93851527140336, -105.2578657817275 39.93851646595966, -105.2578624943541 39.93851766683271, -105.2578592093078 39.93851887131318, -105.2578559230882 39.93852007669179, -105.2578526450235 39.93852129199465, -105.2578493634487 39.93852250729002, -105.257846088881 39.93852372620268, -105.2578428142877 39.93852495232048, -105.2578395431948 39.9385261811475, -105.2578362756022 39.93852741268378, -105.2578330079936 39.9385286487232, -105.2578297438725 39.9385298910745, -105.2578264832518 39.93853113613503, -105.2578232273047 39.9385323830066, -105.2578199689919 39.9385336370784, -105.2578167165194 39.93853489386431, -105.257813466371 39.93853615515832, -105.2578102197229 39.93853741916158, -105.2578069742255 39.93853868857114, -105.2578037310585 39.9385399606875, -105.2578004925491 39.93854123911814, -105.2577972540331 39.93854251934997, -105.2577940213544 39.93854380319665, -105.2577907886596 39.93854509154649, -105.2577875606224 39.9385463862106, -105.2577843325755 39.93854768357663, -105.2577811103722 39.93854898275616, -105.2577778893132 39.93855028914326, -105.257774671761 39.93855159643829, -105.2577714576964 39.93855291004524, -105.2577682424488 39.9385542272522, -105.2577650318652 39.93855554897218, -105.2577618247852 39.93855687250073, -105.2577586211864 39.93855820414242, -105.2577554210944 39.9385595366921, -105.2577522209926 39.93856087194365, -105.2577490243815 39.93856221260636, -105.2577458300945 39.93856355777719, -105.2577426428114 39.93856490746596, -105.2577394555219 39.93856625895595, -105.2577362693799 39.93856761675286, -105.2577330879082 39.93856897726144, -105.2577299075873 39.93857034317637, -105.2577267342864 39.93857170910593, -105.2577235621267 39.93857308314374, -105.2577203899572 39.93857445988341, -105.257717221288 39.93857583933234, -105.2577140572797 39.93857722419494, -105.2577108956017 39.93857861176435, -105.2577077385877 39.93858000384675, -105.2577045815576 39.9385814004323, -105.2577014303711 39.93858279883143, -105.2576982791653 39.9385842026343, -105.2576951326266 39.93858561004964, -105.2576919895787 39.93858702287611, -105.2576888500344 39.93858843751122, -105.2576857093071 39.93858985574636, -105.2576825732375 39.93859128029582, -105.2576794453418 39.93859270936571, -105.2576763151093 39.93859413752992, -105.257673190701 39.93859557291159, -105.2576700639367 39.93859701279147, -105.2576669465228 39.93859845539296, -105.2576638279292 39.93859990069383, -105.2576607163332 39.93860135231392, -105.2576576035575 39.93860280663348, -105.2576544966254 39.93860426276648, -105.2576513920108 39.93860572520894, -105.257648292057 39.93860719306509, -105.2576451909362 39.93860866001801, -105.2576420968036 39.93861013599214, -105.2576390038407 39.93861161196865, -105.2576359131986 39.93861309335391, -105.2576328272269 39.93861457745087, -105.2576297435759 39.93861606695663, -105.2576266645953 39.93861755917406, -105.2576235891118 39.93861905500142, -105.2576205159523 39.93862055533687, -105.2576174439499 39.93862205927732, -105.2576143777814 39.93862356773325, -105.2576113127733 39.93862507889351, -105.2576082559424 39.93862659367355, -105.2576051967522 39.93862811385245, -105.2576021422355 39.93862963584248, -105.2575990923764 39.93863116414679, -105.2575960436872 39.93863269245352, -105.2575929961391 39.93863422886844, -105.2575899567778 39.9386357662012, -105.2575869197437 39.93863730714142, -105.2575838826838 39.93863885528675, -105.2575808526472 39.93864040254618, -105.2575778237613 39.93864195521184, -105.2575747971961 39.93864351328624, -105.2575717741312 39.93864507406995, -105.2575687580735 39.93864663847096, -105.2575657443462 39.93864820557876, -105.2575627317728 39.93864977719219, -105.2575597238665 39.93865135241801, -105.2575567136041 39.93865293214206, -105.2575537126889 39.93865451548837, -105.2575507164441 39.93865610154639, -105.25754772018 39.93865769300825, -105.2575447262462 39.93865928717691, -105.257541740496 39.93866088316403, -105.2575387535534 39.9386624854532, -105.2575357724478 39.93866409135715, -105.2575327925058 39.93866569906486, -105.257</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
+          <t>MULTIPOLYGON (((-105.1842001793857 39.96258943629537, -105.1845921801246 39.96264443594031, -105.1846878292357 39.9626284939408, -105.184684179543 39.96329443567719, -105.183756179454 39.96352043583736, -105.1841021800759 39.96259043491916, -105.1842001793857 39.96258943629537)), ((-105.2128335385606 39.98575351525029, -105.2128209987258 39.98510499896647, -105.2128219705335 39.98490281397867, -105.2128239999816 39.98447999876575, -105.2128279999043 39.98376599906238, -105.2128298606279 39.98346834759489, -105.212830000377 39.98344599815635, -105.2128303968119 39.98311209701794, -105.21283300067 39.9809199993889, -105.2128330007686 39.98049724201171, -105.212833000599 39.98012599947322, -105.2128395034223 39.98012199063935, -105.2128301877808 39.97808843595108, -105.2149131886728 39.97773343595954, -105.2160471505688 39.97825984715396, -105.2161149998271 39.9782349994438, -105.216200462426 39.97812263862686, -105.2175789989619 39.97876299865521, -105.217670999848 39.9788049982916, -105.2198569987801 39.97980999936001, -105.2205429995072 39.98012599905148, -105.220540062076 39.98012857681351, -105.2205507460672 39.98013349868391, -105.2205521325287 39.98013228345715, -105.2208531327514 39.98027028363045, -105.2211641313148 39.98041428305446, -105.2212231314078 39.9803062839601, -105.221716133175 39.98053428301674, -105.2233041316678 39.98126628283385, -105.2259021321316 39.9824632823856, -105.2259871327598 39.98250228293273, -105.2268921334482 39.98292028334055, -105.2276381336663 39.98326528294741, -105.228734132372 39.98377128349869, -105.2293111332321 39.98403928262311, -105.2302491328946 39.98447128245876, -105.2309501326586 39.98479628222291, -105.2311531345965 39.98489128325956, -105.2319351336893 39.9852542826066, -105.2319832192942 39.98527649380193, -105.2323551334779 39.9854482825155, -105.2324551331664 39.98549528298939, -105.2325671332445 39.98554728283532, -105.2327191338569 39.98561728215761, -105.2330351331852 39.98576428266011, -105.2331971337308 39.985840282157, -105.2333186456079 39.98589620582294, -105.233549133973 39.98600228301675, -105.2345601331849 39.9864642829105, -105.2347186571129 39.98653701728261, -105.2347301344601 39.98654228280646, -105.2347290390252 39.98654275943437, -105.2401753609658 39.98955497449158, -105.2401816972446 39.98954904272472, -105.2410388945943 39.99004486718228, -105.2466227154164 39.99335930785364, -105.2483721362223 39.99436828224118, -105.2488871359441 39.99466728119395, -105.2519301367892 39.99643628146383, -105.252490135917 39.99676028120317, -105.2526451362952 39.9966972807593, -105.2529616488933 39.99687856120978, -105.2531881376958 39.99700828020997, -105.2551191376442 39.99812828080001, -105.2554151376702 39.99826728194028, -105.2569711373872 39.99907628081892, -105.2579881380721 39.9996242809139, -105.2581901380272 39.99973028114304, -105.2586371380042 39.99996628110418, -105.2588631378062 40.00007828100154, -105.2589691389426 40.00013528073883, -105.259208137926 40.00024028023068, -105.259251053428 40.00025364728025, -105.2592544037049 40.00038408331039, -105.2589195861169 40.00036267320748, -105.2581675632618 40.00029957202448, -105.2583433547495 40.00053228127841, -105.2584680337078 40.00076130850472, -105.2585687794402 40.00118688281169, -105.2586142067626 40.00148365856045, -105.2586454140996 40.00185904416556, -105.2586436430115 40.00235946687246, -105.2586556382503 40.00290996136781, -105.2586434447849 40.0037284900354, -105.258572133868 40.00373098416479, -105.2583379493246 40.00373488608032, -105.2540440020844 40.00372910138983, -105.2531108838922 40.00373012711088, -105.2531039801196 40.00445402054249, -105.2531010238238 40.00517188259421, -105.2531028651088 40.00594493428408, -105.2531119710475 40.00658513352174, -105.2531470399376 40.00675897970751, -105.253390440773 40.00738013872348, -105.2534580881613 40.00761587168582, -105.2534788384062 40.0077021148444, -105.2535018757067 40.00784711067982, -105.2535111127166 40.00805686367984, -105.2535011689129 40.00823994697006, -105.2535068895725 40.00892900280688, -105.2535061296354 40.01032410969325, -105.2535039273517 40.01086430388367, -105.2535030853529 40.01100293505052, -105.2535019003321 40.01119789590327, -105.2535261719986 40.01169290685051, -105.2535630325855 40.01186593254538, -105.2536241596939 40.01204202995962, -105.253715823358 40.01226403757396, -105.2537806712891 40.01248002734037, -105.2538054741536 40.01274848195483, -105.2538081303951 40.01360465598484, -105.2537949903803 40.01406758669711, -105.2537731835135 40.0146261868912, -105.2501120279116 40.01463197668197, -105.2489568317006 40.01463733680855, -105.2477575533147 40.0146096980253, -105.2465954644375 40.01458212939171, -105.2460469422521 40.01457377343792, -105.2449033960308 40.01456052644195, -105.2432112087095 40.01457106881134, -105.2422256658095 40.01457244483336, -105.2407671682903 40.01461834492035, -105.2401101703597 40.01465348406194, -105.239268545971 40.01470520202151, -105.2379838714334 40.01472804370003, -105.2364884675618 40.01473462743368, -105.234785953114 40.0147380290238, -105.2338293506786 40.01473924403673, -105.2319659677214 40.01469691984863, -105.2309519694455 40.01468609977, -105.230058133229 40.01466913584839, -105.22915700892 40.01466702306828, -105.2281480626285 40.01466492383204, -105.2272090327501 40.01466628746812, -105.2258513852783 40.01466824594888, -105.2254145473955 40.01466887288986, -105.2254128747107 40.01466887521181, -105.2245834902002 40.0146398382582, -105.2239170504272 40.01464087196651, -105.2191844656205 40.01463953261158, -105.217100941391 40.01463444043784, -105.2164899016262 40.01467620189562, -105.2164723909476 40.01467739814613, -105.215735902945 40.01471779606526, -105.2157340623453 40.01471789690481, -105.2148910155936 40.01473046222324, -105.2148764361527 40.01473067926249, -105.2141074361257 40.0147478477099, -105.2130981903515 40.01474897460401, -105.2130969381798 40.01474897599216, -105.2130940324873 40.01467594647242, -105.2130777016322 40.01363575086111, -105.2130740693893 40.01339608598071, -105.2130736861623 40.01323274517098, -105.2130673059102 40.01280105946651, -105.213064157268 40.01258789120162, -105.2130592574697 40.01222416348261, -105.2130589996108 40.01220499962974, -105.2130529986013 40.01186999911342, -105.2130460006044 40.01138699885649, -105.2130454473815 40.01133281594282, -105.2130440003177 40.01119099898076, -105.2130312388504 40.01016524665692, -105.2130280004494 40.00990499912331, -105.2130180708937 40.00983143781237, -105.2130060003659 40.00974199894547, -105.2129829999123 40.00961299956395, -105.2129829986977 40.0095865752715, -105.2129829998411 40.0095709993631, -105.2130219997471 40.00935599951865, -105.2130219996678 40.00906603303326, -105.2130219999797 40.00890899948654, -105.2130189997407 40.00870099855842, -105.2130112852478 40.00853642174128, -105.213003999585 40.0083809993364, -105.2129869521706 40.00829726722127, -105.2129700000606 40.00821399827627, -105.2129235378465 40.00809508272722, -105.2128859992807 40.00799899844429, -105.2126530118967 40.00758899420312, -105.2126529828366 40.00758894189271, -105.2125739999607 40.00741399830913, -105.2125429989301 40.00731899837689, -105.2125049987698 40.00709399945863, -105.2125054826385 40.00647891950867, -105.2125059976708 40.00582199879766, -105.2125107894076 40.00369755140002, -105.2110311909939 40.00371343942365, -105.21103119153 40.00352344002083, -105.2111551901976 40.00343643944229, -105.2111711906653 40.00325443919979, -105.2111441915764 40.00300243863417, -105.2117761908399 40.0030044389501, -105.2117791909032 40.00354043954807, -105.2125117588774 40.00352564947486, -105.2125161427577 40.00307331652181, -105.2125269999105 40.00195299848955, -105.212566988398 40.00156499793533, -105.2125669991999 40.00156493581707, -105.2125852425582 40.00147525356017, -105.2127399996955 40.00071399866724, -105.2127818519077 40.00052534458408, -105.2128050001144 40.00042099923211, -105.2128159972606 40.00024511251258, -105.2128159836817 40.00024499989686, -105.2127969995393 40.00008999943838, -105.2127928656112 40.00007553362977, -105.2127829993984 40.00004099865892, -105.2127459994442 39.99984399810055, -105.2127392146961 39.99881852246104, -105.2127389991961 39.99878599927126, -105.2127455277946 39.99746149416151, -105.2127469993367 39.99716299909484, -105.2127440001071 39.99692699925155, -105.2127449818323 39.99692495901152, -105.2126844006306 39.99661445128344, -105.2126006533221 39.99626870887596, -105.2125139076481 39.9958991302809, -105.2124961767938 39.99569533982743, -105.2124925687887 39.99544869177733, -105.2124983315102 39.99518419448454, -105.2124740351865 39.99470038739478, -105.2124601767598 39.99431311694229, -105.2124779991473 39.99348899860376, -105.2125093588739 39.99318486329975, -105.2126539990297 39.99178199891079, -105.2126889998817 39.99139699911375, -105.2127249983793 39.99099299884455, -105.2127899996551 39.99032999898677, -105.2128229998723 39.98972899884425, -105.2128209981865 39.98794399929118, -105.212820998313 39.98749399914585, -105.212819999065 39.9874409984555, -105.2128199983129 39.98714499875833, -105.2128409991863 39.98614399888426, -105.2128408265147 39.98613467486216, -105.2128393984281 39.98605755172515, -105.212838999747 39.98603599893198, -105.2128335385606 39.98575351525029)))</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>18</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>Manhattan MS</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>290 Manhattan Dr, Boulder, CO 80303</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>http://mam.bvsd.org/</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>Manhattan Middle School of Arts and Academics</t>
         </is>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>39.99410342530379</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>-105.2273572175253</v>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="N14" t="inlineStr">
         <is>
           <t>http://mam.bvsd.org/</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>POINT (-105.2273572175253 39.99410342530379)</t>
         </is>
@@ -1368,53 +1412,56 @@
           <t>POLYGON ((-105.1252489123642 39.97296264565752, -105.1251781675552 39.97293944155944, -105.1250681668962 39.972906441131, -105.1249497653521 39.97287524610411, -105.1249011680386 39.97286244087732, -105.1248531668425 39.97285044186012, -105.1247921674847 39.97283644067091, -105.1246601669836 39.97280844165002, -105.1245523833219 39.97278895695491, -105.1244201369517 39.97276780367894, -105.1242581672639 39.97274644167108, -105.1241911675568 39.97273944124998, -105.1229011674566 39.97270644080103, -105.1217242765111 39.97281619705816, -105.1214051667389 39.9728474415511, -105.1212921660192 39.9728514412086, -105.1211677547576 39.97285530417747, -105.1209041446044 39.97286348814555, -105.1206801658403 39.97287044195357, -105.1203420443671 39.97286990956984, -105.1194881869002 39.97287256612985, -105.1186181657589 39.97287744155079, -105.1186161666875 39.97368444138921, -105.1182721659632 39.97381044163679, -105.118018165306 39.97395344192811, -105.1171981652229 39.97420444199783, -105.1171265636503 39.97423590742287, -105.1158010195454 39.97481841383456, -105.114358165628 39.97545244199855, -105.1140021644149 39.97552144240487, -105.1135711643946 39.97554144292338, -105.113406165381 39.97567644266403, -105.1132631646667 39.97570744192655, -105.1133870040023 39.97608190631396, -105.1133790200561 39.97608188493721, -105.1123831027614 39.97608512830671, -105.1117668377299 39.9760899171973, -105.1108470594524 39.97608530949304, -105.1108412041789 39.97609179069381, -105.1092491642645 39.97610344217862, -105.1092964823203 39.97532071473902, -105.1092904101518 39.97530904500583, -105.1092758343959 39.97528099404412, -105.1092339554898 39.97511696238349, -105.1092260671889 39.97499889140114, -105.1092199916418 39.97462689328338, -105.1092231749659 39.97382200756769, -105.1092751638475 39.97241644265112, -105.1093741622733 39.95969644064292, -105.1093821626999 39.95928944047934, -105.1079021614665 39.95931444023918, -105.1078871611286 39.95851244033037, -105.1081481615724 39.95847244081943, -105.108159162151 39.95790844019832, -105.1081605804928 39.95790194404009, -105.1093269988958 39.95789799857891, -105.1093269879348 39.95789786884638, -105.1145961633331 39.95785343948453, -105.1145691634786 39.96033344011676, -105.1152741627195 39.96032944007523, -105.1152851635068 39.95784843935154, -105.1280631665933 39.95781743936814, -105.1279511266712 39.9541802399316, -105.1279522914871 39.95238450217838, -105.127953497769 39.95054658538529, -105.1279535055246 39.95053550276305, -105.1279608891086 39.94967093417858, -105.1279857222323 39.94676288303474, -105.1280107097569 39.9438364185598, -105.1280154169606 39.94328510754713, -105.1281202734379 39.94328281974127, -105.1281189566972 39.94321673837639, -105.128119170051 39.94275986892613, -105.1281188559567 39.9426128500413, -105.1281179815044 39.94209470227083, -105.1281166731066 39.94131881581806, -105.1281160435918 39.94095694729186, -105.1281027487722 39.93982376694078, -105.1280999834125 39.93958806354111, -105.1281533050244 39.93958961368488, -105.129260217686 39.93962179633774, -105.1305578104314 39.93965950845269, -105.1309208893939 39.93966636177272, -105.1364432759128 39.93974592316794, -105.1370090029643 39.93974203840741, -105.13757654182 39.9397486123599, -105.1376106683007 39.93974719309715, -105.1376101742235 39.93970626003536, -105.1376659994644 39.93973899908963, -105.1380069982713 39.93995099908016, -105.1400129996827 39.94124299866457, -105.1405889992587 39.94161999863454, -105.1409599991531 39.94185799904378, -105.141208999877 39.9420169995477, -105.1415170000054 39.9422179981579, -105.1429179998172 39.94312999953807, -105.1435829995349 39.94355199879121, -105.1436849993157 39.94361699895295, -105.1438049994702 39.94369699936311, -105.1444109992605 39.94408999827592, -105.1465979998178 39.94550799907834, -105.1469689981003 39.94574899894534, -105.1470224473384 39.94578389403245, -105.1479109994562 39.94636399921564, -105.1483709999483 39.94665999878806, -105.1487869967502 39.94692837327946, -105.1493769991665 39.94730899849206, -105.1502339997436 39.94785999905235, -105.1505859991704 39.94808599920534, -105.1510029999227 39.9483689989986, -105.1520270002295 39.94907999894239, -105.1526479997484 39.94953399844792, -105.1538259995572 39.95043899936822, -105.1543240000297 39.95082499846626, -105.1545469991415 39.95082499900798, -105.154634999516 39.95082499893148, -105.155603998905 39.95163699829544, -105.1564621234448 39.95235626096443, -105.1568089995898 39.95264699943566, -105.1594730000078 39.95466099895394, -105.1603829998639 39.95530799832515, -105.1604879993213 39.95538299862599, -105.1605708372656 39.95542490543037, -105.1605729992732 39.95542599889634, -105.160553485336 39.95544433019448, -105.160507601197 39.95548743481859, -105.1605070003541 39.955487998663, -105.1605739993225 39.95553199876508, -105.1609239990875 39.95574399904351, -105.1611820283237 39.95589271854974, -105.1612710001578 39.9559439989421, -105.1615179991773 39.95607999946219, -105.162090999951 39.95638499933245, -105.1623139998591 39.95649799874107, -105.1626729999983 39.95667199866357, -105.1629539988249 39.95680199904174, -105.163260000118 39.95693999941128, -105.1635449998441 39.95706699912397, -105.1640439992191 39.95727199887524, -105.1655459994386 39.95785699862255, -105.1657049993032 39.95791899851163, -105.1658829843055 39.95798883313223, -105.166280999977 39.95814499912188, -105.1663260779203 39.95809453148716, -105.1663729998672 39.95804199855646, -105.1663939993887 39.95801599875833, -105.1663429988309 39.95789999829524, -105.1661250002072 39.95739999859541, -105.1661089994848 39.95726499912967, -105.1660659997773 39.95698699837227, -105.1660599995567 39.9569419984156, -105.1661219997786 39.95695499897838, -105.1668249995467 39.95710599849211, -105.1672029990481 39.95741599921722, -105.1677549991503 39.95786999907147, -105.16867899997 39.95862899864169, -105.1718929991997 39.96004699882172, -105.1750629987647 39.96129699910314, -105.175195000182 39.96134899884276, -105.1777729991336 39.96222499799526, -105.1777779996259 39.96221599908061, -105.1777786369145 39.96221513532904, -105.1777988506388 39.9622247658564, -105.1779603294206 39.96230169761951, -105.1780248042583 39.96220476780362, -105.1780361786519 39.96221443573692, -105.1790331792207 39.9626014355022, -105.1791101784401 39.96248843618227, -105.1800231788606 39.96283243551652, -105.1803891795854 39.96287543542729, -105.1804071788043 39.96288743619242, -105.1804541783631 39.96292043608274, -105.1805011791406 39.96295143559319, -105.1805491783552 39.96298243605077, -105.1806471783964 39.96304143605229, -105.1806971792238 39.96307043532614, -105.1807481784856 39.96309843581128, -105.180799178964 39.96312643537638, -105.1808511790458 39.96315343615423, -105.1809041787385 39.96317943634221, -105.1809571796388 39.96320443587675, -105.1810111789803 39.96322943544858, -105.1810651795186 39.96325343616735, -105.1811201784924 39.96327643628931, -105.1811751798336 39.96329843665993, -105.1812645330557 39.96333272334351, -105.1813451795762 39.96336143602115, -105.1814281797796 39.9633894364229, -105.1815181794293 39.96341743539393, -105.1815991793696 39.96344043598965, -105.1818761791532 39.9635074363657, -105.1820251788167 39.96353643541125, -105.1821201788212 39.96355143678812, -105.1822441795616 39.96356843645984, -105.1823521786804 39.96357643573872, -105.1824941789573 39.96359343521812, -105.1826201798852 39.9636004354759, -105.182745178819 39.96360443634497, -105.1828711795887 39.96360543613775, -105.1829971802545 39.96360343569754, -105.1831221800468 39.96359843587509, -105.1832471796654 39.96358943518963, -105.1833721791185 39.96357743607462, -105.1835581803465 39.96355343554686, -105.183681180111 39.96353243572506, -105.183756179454 39.96352043583736, -105.184684179543 39.96329443567719, -105.1846881802595 39.96256443553224, -105.1851691808371 39.96256443568562, -105.1852781797714 39.96245943558378, -105.1862821800566 39.96244943611252, -105.1867361810641 39.96239743503643, -105.187073180655 39.96230143525784, -105.1872551801046 39.96227843565087, -105.1876121808403 39.9621674358669, -105.1877131813326 39.96209643507789, -105.188260316038 39.96197615552799, -105.1889071811083 39.96174843466853, -105.1892811813567 39.96148043493095, -105.1892731804752 39.96267043497246, -105.1882881813402 39.96279743543808, -105.1875491802892 39.96290443543483, -105.1867561809799 39.96303243590308, -105.1859091799674 39.96319543556243, -105.1852101802556 39.96334743554963, -105.1850871806001 39.96337543512138, -105.1846831809932 39.96346543564761, -105.1846811801298 39.96359143505422, -105.183359179438 39.96390543564833, -105.1831431795536 39.96390943620628, -105.1829501799709 39.96406143557106, -105.1823765858315 39.96435856048586, -105.182328924705 39.96438302610748, -105.1836529999933 39.96489799860698, -105.1845014339616 39.96523026465304, -105.184378790729 39.9663747723468, -105.1843769878934 39.96809980246061, -105.1834828991021 39.96810018023088, -105.1826965883272 39.96810050650755, -105.1827049815247 39.96884194995791, -105.1827443502702 39.97231958783131, -105.1826878500371 39.97232043832547, -105.1825779238971 39.97232006357458, -105.1824693614918 39.97231969607867, -105.1818888682263 39.97232118367459, -105.181313336771 39.97232225425414, -105.1807346165126 39.97232332753696, -105.1802034669848 39.97232431015902, -105.1797370086139 39.9723251692939, -105.1792927120879 39.97232533345959, -105.1782463742659 39.97232158132549, -105.1775629965025 39.97231860602722, -105.1761817574226 39.97231257916473, -105.1754036449972 39.97230917804725, -105.1753349979691 39.97230887841319, -105.1753040182588 39.97230874160383, -105.1753029543753 39.97233821445883, -105.1753000521294 39.97286562741104, -105.1752993592102 39.97299154292094, -105.1752986321791 39.97312339547399, -105.1752986400875 39.97327644619253, -105.1752986424906 39.97332390459598, -105.1752987049537 39.97441934769093, -105.1752970387502 39.97477164542337, -105.1752952276789 39.97514060311426, -105.1752932053162 39.97554706270822, -105.1752933364211 39.97554706487885, -105.1752921268262 39.97576430925468, -105.1752921682676 39.97579225049291, -105.1752957663743 39.97633889713853, -105.1752998415047 39.97695824622881, -105.1753039309026 39.97757977851963, -105.1753066251767 39.97798897490134, -105.1753071625874 39.97807062647465, -105.1753077055884 39.97815307154284, -105.1753102988506 39.97864007456597, -105.1749131590959 39.97863994859521, -105.1746315779191 39.97863985840293, -105.1737145515828 39.97863956374063, -105.1736004540525 39.97863952981174, -105.1713767703544 39.97863884954739, -105.1707601398161 39.97863865429652, -105.1705561331186 39.97863809480832, -105.1698279435228 39.97863609678081, -105.1688872339223 39.97863350366777, -105.1679504485915 39.97863091778471, -105.1660539287566 39.97862565398879, -105.1660529846982 39.97899093757391, -105.1660527537385 39.97906729471996, -105.1660524971388 39.97915319426635, -105.1660513282059 39.97953810432843, -105.1660546877398 39.97987039392753, -105.166056001947 39.98000036722793, -105.1660560052696 39.98000040596588, -105.166057391659 39.98000036044625, -105.1660575394011 39.98000748868384, -105.1660575821633 39.98001166786214, -105.1660576266512 39.98001166799104, -105.166065785029 39.98040377608608, -105.1659816707675 39.98040380617206, -105.165974894609 39.98681212206605, -105.1659751117827 39.98681224608544, -105.165974893996 39.98681224725572, -105.1654436915867 39.98681856417538, -105.165249938283 39.98682086759958, -105.1652483903585 39.98682087571383, -105.1652418264078 39.98717422250558, -105.16525834624 39.98830990071465, -105.1652600612412 39.9884278360004, -105.1652129168158 39.98840770990265, -105.164152903713 39.98795517594412, -105.1640557053296 39.98791588344694, -105.1639629797611 39.98801302742708, -105.1638820078671 39.98807702897645, -105.1636180300277 39.98827007062972, -105.1633738472757 39.98842912912709, -105.1632068468137 39.98856892148969, -105.1631318802227 39.98864501967785, -105.1630340843738 39.98879105290501, -105.1629701445979 39.98894706885007, -105.1629411450479 39.9891100499324, -105.1629369535138 39.98923604238151, -105.1629316619924 39.98939933324853, -105.1630484245457 39.98939258460942, -105.1652800904351 39.98963757722175, -105.165280121269 39.98963940654668, -105.165293913414 39.9904726547182, -105.1644396301791 39.99047469439939, -105.1603292951578 39.99048441784612, -105.1598894223283 39.99048544917379, -105.1582351763826 39.99048931494893, -105.1582367037443 39.99049132434087, -105.1585727934224 39.99093128003249, -105.158249423521 39.99149224398947, -105.1576955197453 39.99206442405352, -105.1570945121236 39.99246391068015, -105.156359603665 39.99274076059307, -105.1561716319405 39.99274373072714, -105.1560127966663 39.99270667940952, -105.1550702284904 39.99239786295302, -105.1548927785468 39.99227636637016, -105.1548910742555 39.99251738266482, -105.1548905001314 39.99259868061086, -105.1548904876865 39.99260044586263, -105.1548798542597 39.99410483914303, -105.1527289655441 39.99412802825835, -105.1527391763146 39.99397744204157, -105.1511885403603 39.99398043009678, -105.1489619720619 39.99399513205215, -105.1467891751321 39.99400744202379, -105.146790174619 39.9941694428106, -105.1466363980306 39.99416436382368, -105.1464615829938 39.99416230126948, -105.1459611770951 39.99455926085398, -105.145432872713 39.99479210016541, -105.1443011561806 39.99478265717581, -105.1442614765063 39.99492166747812, -105.1422639133758 39.99651569716553, -105.1418815666315 39.99705442482142, -105.1415483564617 39.99743752080339, -105.1412987486078 39.99773918448757, -105.1407003492131 39.99804212814589, -105.1405141950552 39.99813279982534, -105.1373344848354 39.99415560978961, -105.1373254730912 39.99414433762385, -105.130985314058 39.99412962806004, -105.1279510944342 39.99413186772644, -105.1277274031719 39.99403166429317, -105.1232577328613 39.99406674611331, -105.1232589140897 39.9941456611968, -105.122814800146 39.9941474397444, -105.1226719071595 39.99394172642054, -105.1225145804866 39.99383477964317, -105.1223849223714 39.99378832326342, -105.1223232452224 39.99378812123183, -105.1223389573864 39.99236704634767, -105.1223383484516 39.99236705245885, -105.1222303531299 39.99236784607286, -105.121007043891 39.9923704175954, -105.1204839651552 39.99237377836661, -105.1199496728335 39.99237720607682, -105.1189229397637 39.99238378801977, -105.1185472892864 39.99238619608135, -105.1185474045477 39.99235909652852, -105.118575976712 39.98710775588565, -105.1185703104926 39.98693549769058, -105.1173699922748 39.98694351032786, -105.1173718857854 39.98689901321579, -105.1173974168023 39.9851484639417, -105.1174133094992 39.98331547110325, -105.1186071665135 39.98330244358745, -105.1185851681232 39.98678444408168, -105.1211532829889 39.9867767735869, -105.1230647672254 39.98677086630205, -105.1252729795815 39.9867354607854, -105.1278491696747 39.98669844278966, -105.1278438505662 39.98611127501945, -105.127841169928 39.98581544210798, -105.1278368922283 39.98539987307798, -105.1278341691096 39.98513544239999, -105.1278081691162 39.98462244192449, -105.1278173436443 39.98417719271642, -105.1278251690041 39.98379744319919, -105.1278411686021 39.98365144210749, -105.1268601685777 39.98365144197767, -105.1268441685182 39.98313644257139, -105.1258921445311 39.98314315953377, -105.1249263230647 39.98314996424318, -105.1242251688294 39.98315444282675, -105.1240021678686 39.98305844296069, -105.1238561683382 39.98296444303244, -105.123744168235 39.98286744302084, -105.1236691677244 39.98278344313378, -105.1235781685477 39.98264044277064, -105.1235830349789 39.98201442443881, -105.123586168347 39.98161144252593, -105.1236411680837 39.98141344271861, -105.1237131684662 39.98127144197014, -105.123848168531 39.98109744278342, -105.1239481684561 39.98099044193104, -105.1239441684502 39.98063844197828, -105.12468924775 39.98064430008328, -105.1250891674626 39.98064744247992, -105.1253301685872 39.98066944203719, -105.1254741692224 39.98069944174981, -105.1256331685554 39.98073244235897, -105.1258431687578 39.98075244156166, -105.1259671694033 39.98075344203813, -105.1261481677718 39.9807394421338, -105.126331169116 39.98070644271509, -105.1264991677584 39.98067244239655, -105.1266091684414 39.98065844226225, -105.1266971688295 39.98065244248855, -105.1267971687024 39.98065044260115, -105.1268901681804 39.98065044284952, -105.1269711680979 39.98065844167844, -105.1270981684207 39.98067544186095, -105.127139392241 39.98068334791111, -105.1271711685487 39.98068944278467, -105.127214375739 39.98069969063391, -105.1273066551089 39.98072157695184, -105.1273271684002 39.98072644199087, -105.1274521692765 39.98074644262105, -105.1275471685854 39.9807554418902, -105.1277031693758 39.98076144258219, -105.1277022727454 39.98065050362139, -105.1277006654453 39.98045161563807, -105.1276992570783 39.98027720192252, -105.1276979486562 39.98011536714193, -105.12769489113 39.97973687298536, -105.1276880805791 39.97925149078886, -105.1276812036791 39.97880423869458, -105.1276742985784 39.97835509150174, -105.1276701687788 39.97808644191434, -105.1271081689285 39.97816144152506, -105.1262311691111 39.97870844220219, -105.1260051674357 39.97884844174765, -105.1255304415947 39.97914450912447, -105.1253541688852 39.97925444189506, -105.1255771679067 39.97947344233817, -105.1243405817918 39.98021614971381, -105.1235891680376 39.98066744275177, -105.1232421681502 39.98033144190374, -105.1225391670139 39.98073944211418, -105.1219081678686 39.98099644262695, -105.120230166672 39.98108244243971, -105.1201190479548 39.97979700902974, -105.1199982265585 39.97824241435777, -105.120213921188 39.9783408640164, -105.1204351430655 39.97840802722106, -105.1206690055671 39.97844805327635, -105.1209279925593 39.97846208286956, -105.1212738234645 39.9784519641494, -105.1218390971384 39.97837997317655, -105.1220440922178 39.97834907560969, -105.1251821045501 39.97776690536398, -105.1271320977502 39.97739411515896, -105.1273435143957 39.97735082326365, -105.1276466084615 39.97708321067033, -105.1276525381961 39.97673399347658, -105.1276644462961 39.97603262125949, -105.1275745938115 39.97544829877226, -105.1274121598896 39.97481223461234, -105.1269897690644 39.97410774900974, -105.1265094311803 39.97363524625856, -105.1259336601506 39.97325526013939, -105.125568498434 39.97308157000424, -105.1254721676893 39.97304244124539, -105.1254030021113 39.97301706732278, -105.1253031669845 39.97298044167606, -105.1252489123642 39.97296264565752), (-105.1278929800003 39.98688710210271, -105.1278667741885 39.9867742542211, -105.1278929788344 39.98688710119829, -105.1278529946731 39.98947786494407, -105.1278929800003 39.98688710210271))</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" t="n">
+        <v>19</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>Monarch HS</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>329 Campus Dr, Louisville, CO 80027</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>http://moh.bvsd.org/</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>Monarch High School</t>
         </is>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>39.9520220573069</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>-105.141776992356</v>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>http://moh.bvsd.org/</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>POINT (-105.141776992356 39.9520220573069)</t>
         </is>
@@ -1434,53 +1481,56 @@
           <t>POLYGON ((-105.3507120197024 39.96977708492175, -105.3502663555101 39.96962995325117, -105.3499738912252 39.96953306242339, -105.3497927648202 39.96950780452823, -105.349583788853 39.96947178771764, -105.3494212532477 39.96944297880439, -105.34924479809 39.96940700386404, -105.3490962626725 39.96934961793916, -105.3487714009241 39.96919906389083, -105.3486369377627 39.9690809296067, -105.3484932173364 39.96894848511075, -105.3483587404312 39.9688374998723, -105.3482335625351 39.96872295112451, -105.3480852136772 39.96858335152659, -105.347973974335 39.96846882176619, -105.3478347816061 39.96838999925331, -105.347653738839 39.9683289938379, -105.3473891086939 39.96825357959553, -105.3471476832231 39.96818891961232, -105.346920194601 39.96812427673464, -105.3467158863003 39.96808111151876, -105.3465302247974 39.96800937500215, -105.3464235532126 39.96793059408106, -105.3463448281598 39.96781967985631, -105.3463031951509 39.96774098641889, -105.3462013150994 39.96759787164284, -105.3460947908402 39.9674547496716, -105.3458116807017 39.96733641345445, -105.345677049642 39.96729691428796, -105.3454078122883 39.96720719142478, -105.3451943215452 39.96711754282754, -105.344799794762 39.96696688392825, -105.3445631686427 39.96683788403377, -105.3440530565571 39.96644757631712, -105.3438722349838 39.96629362851484, -105.3437703294546 39.96616480941587, -105.3437287659197 39.966057518448, -105.3436874645537 39.96583584560934, -105.3435903286542 39.96565341505423, -105.3434611855153 39.96524932320219, -105.3433549485055 39.96498466743203, -105.3432580364064 39.96470572634975, -105.3432596704031 39.96399440692426, -105.3432090325889 39.96379416665803, -105.3432139409706 39.9636797911035, -105.3433584770403 39.96344764579057, -105.3440104872482 39.96271576210818, -105.3441130822002 39.96254075062669, -105.3441646115461 39.96235137391512, -105.3441696243447 39.9621905291703, -105.3442119288581 39.96197254236927, -105.3443796023165 39.96177617221307, -105.3445844845748 39.96155840560913, -105.3447195684986 39.96139416148351, -105.3447756268418 39.96125483276604, -105.3447388797202 39.96107248443195, -105.3446230140441 39.96095794510541, -105.3444420997995 39.96085046636512, -105.3439919356307 39.96067113365707, -105.3435556196811 39.96053113787423, -105.343360798049 39.96041291535013, -105.3430825891228 39.96019806749968, -105.3428645192128 39.96009053566726, -105.342558426089 39.95988279881342, -105.342340474804 39.95972522305689, -105.3421550957813 39.95954267131271, -105.3419930516309 39.95931368197322, -105.3419145010556 39.95913485006723, -105.3417808581094 39.95867713300948, -105.3417254175696 39.95854837578747, -105.3416888387843 39.95829811186334, -105.3416286954819 39.95819436922678, -105.3415686602473 39.95804415830918, -105.3414855003038 39.95785102185104, -105.3414486570114 39.95771514066693, -105.34143978317 39.95753640426094, -105.3413796242992 39.9574398108651, -105.3411988658981 39.95727156089524, -105.340813971399 39.95700294350355, -105.3407585423853 39.95687061110937, -105.3407823576073 39.95661685560312, -105.3407644374192 39.9563344475167, -105.3407741612119 39.95614858733419, -105.3408163394168 39.95598779399175, -105.340737929226 39.9557517698098, -105.3404224215921 39.95560835426767, -105.339963064055 39.95540754654273, -105.3397169369457 39.9553893318278, -105.3395404716461 39.95537478831839, -105.3393595717931 39.95527087623741, -105.3391972860632 39.95515269194618, -105.3389332719973 39.95484134311943, -105.3387481361285 39.95456584840096, -105.3385674690961 39.95436542476165, -105.3383821243641 39.95417929127716, -105.3380613773924 39.95387922079283, -105.3381922100665 39.9539168925779, -105.3385208374587 39.95402999317365, -105.3389704612986 39.95410320173998, -105.3396355797279 39.95422398497384, -105.3401411453694 39.95431463685155, -105.3405915068032 39.9543867512165, -105.3410226063689 39.95442202475896, -105.3413251764538 39.95446640101372, -105.3415462146834 39.95453170278824, -105.341978907135 39.95476111029183, -105.342318205314 39.95497951658208, -105.3425857909343 39.95514264437324, -105.3431903754274 39.95531610814066, -105.3435986820116 39.95550253670501, -105.3438741990323 39.95558088547542, -105.3440186020231 39.95565550758867, -105.3441136976464 39.95574272423425, -105.3441389977332 39.95581652211911, -105.3441425364855 39.95588635109922, -105.3440711556896 39.95613686272678, -105.3440378720344 39.9564039015618, -105.3440884076289 39.95664703425503, -105.3441827960147 39.95684524841415, -105.3443946158489 39.95709611761605, -105.3446068353019 39.95717269309261, -105.3448191912631 39.95717297927444, -105.3451590792293 39.9571407418311, -105.3454434965831 39.95717430831029, -105.3456695563883 39.95726454891713, -105.3459817638437 39.95741094481667, -105.3462287436664 39.95746034235974, -105.3465296949049 39.95748316629089, -105.3467618157279 39.95753709210727, -105.3471456360077 39.95776202530593, -105.3478214840077 39.95814889463594, -105.3485363790411 39.95860993791083, -105.3487037748324 39.95867567956383, -105.3488962982591 39.95871689126606, -105.3490717285018 39.95871526312619, -105.3492283080394 39.95870384425507, -105.3494911127846 39.95865230559473, -105.3497176360485 39.9586526012469, -105.3499724607688 39.95866380511001, -105.3502291566699 39.95861756977649, -105.3503832841733 39.95857717838697, -105.3506098071917 39.95857747228528, -105.3510048124872 39.9586400226201, -105.351345777182 39.95870917935156, -105.3516733318363 39.95880173663877, -105.3518836686614 39.95878613315444, -105.3520178350116 39.95875210856961, -105.3520746957046 39.95872122336939, -105.3521102839133 39.95867938499769, -105.35212220401 39.95863842500425, -105.3521104398092 39.95860745169789, -105.3520702935195 39.95856915836187, -105.3519260940527 39.95849795111383, -105.3517903015078 39.95841226836524, -105.3516327162817 39.95825478871504, -105.3515030716467 39.95806517346453, -105.3514385408322 39.95783632304158, -105.3514614232365 39.95763062854918, -105.3516543984425 39.95738535951605, -105.3519882100022 39.95711141236313, -105.3522487218811 39.95692587313406, -105.3526579361303 39.95670835306336, -105.3530862636785 39.95657473750998, -105.3533690273359 39.95650551578468, -105.3536895321031 39.9564987737959, -105.3540065873437 39.95656501021908, -105.3544637367979 39.95665966283416, -105.3547191238183 39.95666362646298, -105.3549249516538 39.95662020943129, -105.3552374249272 39.95646773426095, -105.3554859298368 39.95637159505921, -105.3556823119012 39.95632088393366, -105.3558505676371 39.95630145846711, -105.3557992750611 39.95602245334246, -105.3557741141502 39.95576549921196, -105.3557386458138 39.95566937293702, -105.3557060233276 39.95561276915417, -105.3556469662596 39.95556472809908, -105.3555265701328 39.95553835283317, -105.35533130302 39.95549197808626, -105.3551509598883 39.955420341284, -105.354983454261 39.95532837636013, -105.3548194703378 39.95514520178909, -105.3547633005575 39.95493811633833, -105.354806468642 39.95460040077084, -105.3548830434188 39.95440920980376, -105.3549020387573 39.95421263782769, -105.3547589612953 39.95378709435537, -105.3544950960814 39.95337569701889, -105.354328387966 39.95314314435302, -105.3542544405529 39.95297147602072, -105.3544141255283 39.95269311604522, -105.3546227298896 39.95232853300234, -105.3546986643523 39.95203973189982, -105.3546976459791 39.951916725421, -105.354696493764 39.95184504081303, -105.3546691554396 39.95177685194528, -105.3545945513623 39.95167804960032, -105.3543318430792 39.95143562611569, -105.3540492663155 39.95118040016152, -105.3537479616793 39.95090835791643, -105.353706951089 39.95054013413743, -105.3535977264722 39.95029109927498, -105.3534278442595 39.95000483331427, -105.3532453961211 39.94974103325151, -105.3531911033443 39.94957306478888, -105.3531914570367 39.94940864067144, -105.353246801853 39.94908729334558, -105.3534345654886 39.94866188254792, -105.3535091801626 39.94851899837285, -105.3535095024001 39.94836886940653, -105.3533754572079 39.94807201753893, -105.3531236142911 39.94767376819163, -105.3528824496291 39.94735108971799, -105.3528263263688 39.94711130763148, -105.352854191666 39.94687038990777, -105.3528397428303 39.94667371057839, -105.3526547492991 39.94631602639261, -105.3524040429403 39.94599939878466, -105.3522201694978 39.94592290094791, -105.3520502790885 39.94594445355338, -105.3519560576344 39.94598776664162, -105.3518405762703 39.94601937441158, -105.3517208975748 39.94600567457899, -105.3516026725817 39.94597137759611, -105.3514444997917 39.94588811076953, -105.3513546245374 39.94579577849958, -105.3511027920363 39.94548997156586, -105.3509050233133 39.94529359798763, -105.3505838167 39.94513865452713, -105.3503982828856 39.9450347527661, -105.350300970492 39.94493811658024, -105.3502832029022 39.94481336976445, -105.3503120243307 39.94458459468469, -105.3503112624806 39.94448059585778, -105.3502143510659 39.94420166014947, -105.3500575626043 39.94379875040127, -105.3500026987519 39.94362534593829, -105.3498445102611 39.94343981278547, -105.3497053349327 39.9433752893389, -105.3495243107314 39.94333573399553, -105.3493059779342 39.94336762004309, -105.3491340108557 39.94343173423461, -105.3490129147341 39.94359242734798, -105.3487423315608 39.94414969374191, -105.3486259823145 39.94430691253987, -105.3484437905829 39.9444187019977, -105.3482453905888 39.94452739768072, -105.3481372522787 39.94476370979286, -105.3479977654047 39.94483858920728, -105.3478766414147 39.94483201306166, -105.3476077831022 39.94478806418913, -105.3473618750095 39.94468761993063, -105.3470789371956 39.94453354237368, -105.3468933634192 39.94445108312228, -105.3465051621862 39.94434773235889, -105.3463368710556 39.94425756130052, -105.3463274436908 39.94416437045862, -105.3463787208825 39.94407865046045, -105.3464923497525 39.94400257219984, -105.3466895263439 39.94394785691841, -105.3468249318228 39.94390409492455, -105.3469458653255 39.94381846726618, -105.3470014923789 39.94370856024724, -105.3469741140173 39.94364693072029, -105.3468813323513 39.9436039136981, -105.3466264719512 39.94357602811639, -105.3461619038107 39.94351265458335, -105.3458521496769 39.94348923147759, -105.3457354489024 39.94342004628592, -105.3457141629159 39.94332550653542, -105.3457536159009 39.94326998077975, -105.345841741395 39.9432602869895, -105.3459996916824 39.94329175730961, -105.3462238298761 39.94330439209571, -105.3464080083053 39.94323924565847, -105.3464764128338 39.94315766084034, -105.3465029621614 39.9431100037764, -105.3465102514326 39.94306756376609, -105.3464971988181 39.94302076089416, -105.3464276688434 39.94296347566614, -105.3461191802726 39.94278303907976, -105.3459129593672 39.94262678691265, -105.3455888314258 39.94217652562062, -105.3455008873075 39.94208291329695, -105.3453157028288 39.94183245170021, -105.345260220683 39.94172514236121, -105.3452994412459 39.94161807458997, -105.3454790206228 39.94148594525846, -105.3456232594566 39.94136103208576, -105.3456936576798 39.94124233435014, -105.3456794784697 39.94114306213983, -105.345615264635 39.94108360484331, -105.3455381459786 39.94104387979846, -105.3454334287735 39.9410140239936, -105.3453117618755 39.94100848106682, -105.3450852114466 39.94102997251904, -105.3448614030582 39.94115051238641, -105.3446456843429 39.94134535515964, -105.3445461638083 39.94154136582213, -105.3445315828068 39.94172656519589, -105.3445047050119 39.94184048084426, -105.3444750322293 39.94189565912026, -105.3444167376543 39.94194527050977, -105.3443649776773 39.94197293540188, -105.3443022889449 39.94198370270044, -105.344249041942 39.94197639575263, -105.3442083965542 39.94193895905808, -105.3441408110076 39.94183801666134, -105.3441087282511 39.94165209942394, -105.3440588417544 39.94157217882472, -105.3440180360536 39.9414596316175, -105.3441504891605 39.94123572850936, -105.3444201768378 39.94090922146732, -105.3446045737641 39.94074602105159, -105.3448738103961 39.94061565635842, -105.3452125109515 39.94050206995038, -105.3455340356399 39.94031737702138, -105.3458940131122 39.94017027039276, -105.3462908554426 39.93994198794666, -105.3465605025822 39.93965010336079, -105.3466027453232 39.93944998874962, -105.3466367324471 39.93921113490654, -105.3467565528364 39.93909550958383, -105.3470468203971 39.93901336640935, -105.3473049946615 39.93897551567823, -105.3476625902587 39.93895811649597, -105.3480247199548 39.93897680428015, -105.3483566129954 39.93906216994667, -105.3491629100225 39.93940835371188, -105.3498018128802 39.9396293548314, -105.3502194413498 39.93976572926093, -105.3503294207818 39.93976661884747, -105.350400661343 39.93971234687233, -105.3503915615324 39.93962654754644, -105.3501228431005 39.93934738838904, -105.3499051285607 39.93910404030952, -105.3497608354034 39.93903131515625, -105.3489173950713 39.93849151148685, -105.3485663290427 39.93847499271768, -105.3482955902814 39.93838219132165, -105.3481168738894 39.93835503070434, -105.3479497636173 39.93835181827158, -105.3478098587675 39.93834864154184, -105.3477165832549 39.93834851827387, -105.3476427485254 39.93834542866371, -105.3475339681682 39.93832733465823, -105.3474407528604 39.93830028702409, -105.3473708908066 39.93825831035578, -105.3472699713123 39.9382013334698, -105.3472311803472 39.93816837384888, -105.3471458595813 39.93808748619713, -105.347083770364 39.9380455196671, -105.3469867370542 39.93798854768993, -105.346881985164 39.93790763402901, -105.346796571137 39.93786862831799, -105.3466761661568 39.93783555903681, -105.3465673868684 39.93781746411783, -105.3464624809674 39.93780535822026, -105.346357547 39.93780521831134, -105.3462526142029 39.93780507830835, -105.3461399078266 39.93780492782732, -105.3460427137029 39.93781975607154, -105.3459610115226 39.93785853899554, -105.3458169574422 39.93797202983635, -105.345774126217 39.93800787266722, -105.3457078670991 39.93809155129362, -105.3456999526396 39.93815436688384, -105.3456336662278 39.93825001155182, -105.3455869479147 39.93828584910379, -105.3455324096934 39.93834261821461, -105.3454701315971 39.93838441881511, -105.3453961873443 39.93842919480537, -105.3453141688943 39.93859363192674, -105.3453174834947 39.93873308230828, -105.3453324758724 39.93894757124433, -105.3453478192813 39.93900716756229, -105.3452854454025 39.93920963782646, -105.3451764562121 39.93935034054514, -105.3450992150013 39.93942385726057, -105.3448396699272 39.93948645664532, -105.3446657570558 39.93944710316149, -105.344384129159 39.93940398872251, -105.3442635820429 39.93932741052702, -105.3440806476839 39.93926808631675, -105.3439079255175 39.93917203517659, -105.3437689444899 39.93902886666783, -105.3437227820638 39.93890965441344, -105.343645771096 39.93874274023654, -105.3434795630392 39.93860290917354, -105.3433831552227 39.93851599989166, -105.3431822898061 39.93836083262784, -105.3430840868266 39.93827947499772, -105.3428732685956 39.93812211134178, -105.3427297277895 39.93806265947011, -105.3424400931839 39.93802619959498, -105.3422698308905 39.93802596659072, -105.3420222592663 39.93798988298423, -105.3418208462812 39.93807301188947, -105.3417123320203 39.93814435154387, -105.3416192681011 39.93822762982641, -105.341515849407 39.93836323363961, -105.3414020988481 39.93842988418462, -105.3412781318281 39.93848928917005, -105.3411230970743 39.93859630941661, -105.3410336766268 39.93871870956254, -105.3410450662076 39.93887024632174, -105.3410447332516 39.93901322507722, -105.3410443447997 39.93918003422367, -105.3410282836238 39.93943022612975, -105.34099674378 39.93968039576468, -105.340980932132 39.93982335404601, -105.3409897233237 39.94002551761, -105.3409808920442 39.94028805576299, -105.3410412926193 39.94049067422415, -105.3409326348646 39.94062158865495, -105.3408703853 39.94076448278047, -105.3406533181873 39.94091907671124, -105.3404674572864 39.940966480408, -105.3401886114176 39.94106141307962, -105.3401421178431 39.94108517813758, -105.3399406107836 39.94120404886886, -105.339832060449 39.94128730237721, -105.339630748214 39.94132276755802, -105.3393828295825 39.94142965521113, -105.3393363074271 39.94146533648792, -105.3393233416274 39.94161898118039, -105.3392428151568 39.94172733397711, -105.3392114080417 39.9419179302638, -105.3390715885114 39.94213220471062, -105.3389010628894 39.9422392012124, -105.338513937799 39.94229823311669, -105.3382505347019 39.94240509842705, -105.3380491323672 39.94247630506577, -105.3377548544015 39.94254738149012, -105.3375226061463 39.94257088373504, -105.3372129605016 39.94259427617204, -105.3369187084585 39.94265343391514, -105.3367018532639 39.94271270244277, -105.3363922364222 39.94272417883428, -105.3360516872704 39.94272369469476, -105.3358194951483 39.94272336402315, -105.3355252712221 39.94277060346691, -105.3352777722196 39.94269876025473, -105.3350612033855 39.94263887467899, -105.3348139071973 39.94248362637954, -105.3346597191067 39.94223319204949, -105.3345673052172 39.94204242014799, -105.3345957688523 39.9417773393035, -105.3346303196934 39.94158974164895, -105.3346773338235 39.94135150985174, -105.3346157633717 39.94120844226929, -105.3344961789176 39.94099717557393, -105.3342914539426 39.94089818733744, -105.33424524894 39.94080279988832, -105.3342300595007 39.940683629287, -105.3342187703895 39.94049634854602, -105.3344784168929 39.94039802796743, -105.3347416450673 39.94036266062547, -105.3349893366625 39.94035110089884, -105.3353456676618 39.9402205463219, -105.3355624587094 39.94018510982277, -105.3356713555442 39.93995888250201, -105.3356098428274 39.93979198504802, -105.3355636642642 39.93968468337358, -105.3353162913976 39.93956518034897, -105.3350997900354 39.9394814671437, -105.3349760472421 39.93944554468823, -105.3347906766642 39.93929038497647, -105.334605279229 39.93914713971061, -105.3345127252388 39.93901594144148, -105.3344355343734 39.93893242522267, -105.3342964869261 39.9388249913192, -105.3341728325842 39.9387533228644, -105.3339407409348 39.93871724417198, -105.3338326803261 39.93859793868223, -105.3337554338947 39.93853825329758, -105.3337092010423 39.93845478035888, -105.3334821172266 39.93789782489326, -105.3327829133291 39.93746449862973, -105.3325662183295 39.93746418386972, -105.3323184782625 39.93749956787977, -105.332163519595 39.93757083274084, -105.3319930238681 39.93766590340954, -105.3317141785255 39.9377608164918, -105.331559101029 39.9378797395179, -105.3314351864608 39.9379153035246, -105.3312028634002 39.93797453727169, -105.3310941896124 39.93810544244619, -105.3310164730188 39.9382363938341, -105.3309541765365 39.93839119647253, -105.3308299347333 39.93855782381141, -105.3306129394301 39.93867665461612, -105.3304578579342 39.93879557615114, -105.3303646313504 39.93893841725295, -105.3303333191918 39.93908135218683, -105.3303173668751 39.93927196798317, -105.3302550370624 39.93943868497224, -105.3301771394815 39.93964112423741, -105.330037503932 39.939771983658, -105.3298048465427 39.93996227854622, -105.3296652107925 39.94009313751392, -105.3295720093546 39.94022406411649, -105.3294013842727 39.94036679079821, -105.3292308777148 39.9404618573578, -105.3289675567365 39.94053295723312, -105.328363397086 39.94072269795484, -105.3280464391735 39.94068518217745, -105.3277290582858 39.94060260054161, -105.3275436118999 39.94048317340886, -105.3273737955304 39.94030419546518, -105.3272230655047 39.94017627980257, -105.3270338333477 39.94007730187811, -105.326848479111 39.93992212849384, -105.3267233057162 39.93972059487754, -105.3264008665194 39.93942102655195, -105.326510155908 39.93905182646767, -105.3266788045178 39.93861631287486, -105.3269504474838 39.93818943437444, -105.3269152288096 39.93801583390401, -105.3268536776333 39.93787276303662, -105.3268076059926 39.93772971450777, -105.3266840208323 39.93763420851904, -105.3266223796962 39.9375268817555, -105.3264369133073 39.93741936755629, -105.326332444717 39.93736300821741, -105.3260812174063 39.93729968138211, -105.3258956297566 39.93723982618449, -105.3256479783452 39.93723945161755, -105.3253848794217 39.9372271383133, -105.3251372891076 39.93720293135949, -105.3248586806939 39.93720250809899, -105.3246419865635 39.93720217843251, -105.3243941513812 39.93727329143306, -105.3242700796447 39.93736842144941, -105.3241615174665 39.9374516611181, -105.3238359511774 39.93765371783137, -105.3231420733671 39.93807305242971, -105.3227684117605 39.93860002799841, -105.3229032642183 39.93918931809423, -105.3227789715475 39.93936785058116, -105.3225929785905 39.9394628853095, -105.3222368443683 39.93950999545962, -105.3220975354618 39.93950978040615, -105.3218807395759 39.93954518976606, -105.3213232553279 39.93963964654615, -105.3212456742569 39.93971101672305, -105.3211522710472 39.93991342586091, -105.3211365426721 39.94000872155141, -105.3210277850324 39.94016344578863, -105.3209655879741 39.94027058403997, -105.3207332478084 39.94032979846212, -105.3204701065221 39.94032938867544, -105.3198388293764 39.9404390245125, -105.3191692463489 39.94056565340757, -105.3189680191451 39.94056533736213, -105.3186740765611 39.9405053002228, -105.3183802624779 39.94039760247852, -105.3179781597508 39.94026590245163, -105.3175447179208 39.94027713156014, -105.3172351396482 39.94027664082628, -105.3169565199088 39.94027619845558, -105.3166467816132 39.94033528163523, -105.316476321442 39.94040649983918, -105.3163519765155 39.9405969410111, -105.3163205701327 39.94076369979045, -105.3162423730982 39.94106144931301, -105.316195455252 39.94124009899878, -105.3159009337462 39.94139452276405, -105.3156220829817 39.94147748302713, -105.315393589911 39.94149240574951, -105.3149875012233 39.94145263516127, -105.3148020101678 39.94135701700087, -105.3146322573936 39.94116610555177, -105.3143695989769 39.94098695806902, -105.3142307086453 39.9408318392145, -105.3142470304991 39.9405220764947, -105.3141701546706 39.94033131316758, -105.3141398137156 39.9401048796018, -105.3140940256521 39.93986650720636, -105.3140018023195 39.93962805802159, -105.3139564708813 39.93922287561901, -105.3139259350723 39.9390679331113, -105.3136326539993 39.93876958471586, -105.3135248903767 39.93855494046591, -105.3135409870585 39.938328582769, -105.313541572907 39.93811411295194, -105.3135728884073 39.93798309911708, -105.3135886919486 39.93786397586513, -105.3135582226762 39.93768520106113, -105.3135586131968 39.93754222327778, -105.3135281127685 39.93737536320363, -105.3135443067977 39.93711326126337, -105.313668360496 39.93703005663828, -105.3138543255822 39.93694695284194, -105.3140710200188 39.93694730280319, -105.3142952267474 39.93694088522145, -105.3144116361982 39.93691210769416, -105.3146129496925 39.93687668567372, -105.3147370974993 39.93675773567037, -105.3149541789319 39.93661510617261, -105.3151556836821 39.93650819475129, -105.3151716143362 39.93634141140234, -105.3152646112064 39.93629390050486, -105.3152959536364 39.93615097053843, -105.3153426458871 39.93605572614626, -105.3153428715063 39.93597232205011, -105.3151730015705 39.93582906938609, -105.3151269546172 39.93568601616223, -105.3150107817862 39.93562102376601, -105.3152947463766 39.93560825239187, -105.3189277387964 39.93544482213235, -105.3191391063055 39.9317901419817, -105.3205148429798 39.9317151039824, -105.3239541807884 39.93152857193745, -105.3240442233703 39.93038144497817, -105.3242555787687 39.92783278270667, -105.3240379379819 39.92434240818668, -105.3238539754728 39.92139180765506, -105.3238336179889 39.92104928059182, -105.3238185156393 39.92104925748924, -105.3236539993554 39.92104899939051, -105.3232179993169 39.92095999891312, -105.3230946808704 39.92091515582619, -105.3230754639435 39.92090816782166, -105.322810999039 39.92081199876494, -105.3228091235898 39.92081034046993, -105.314962656992 39.91387604616386, -105.3186637285294 39.91384134022072, -105.3212698069163 39.91381682948519, -105.3215006511357 39.91381465579448, -105.3227129433033 39.91380322945029, -105.323354140306 39.91379718248584, -105.3279073637289 39.9138067691513, -105.3323281555307 39.91381591637837, -105.3325418885809 39.91381635798417, -105.3328397048168 39.91381390137353, -105.334524796101 39.91379991975911, -105.3357223963508 39.91378996644013, -105.3360327017027 39.91378738519001, -105.3409074326082 39.91374673320104, -105.3419491615664 39.91373801818488, -105.3426961315184 39.91373050995593, -105.3464788027438 39.91369240329173, -105.3513537524865 39.91364310980608, -105.3528087207196 39.91361749517808, -105.3535508659689 39.913604419963, -105.3570569970404 39.91354257768043, -105.3575647191606 39.91353361299981, -105.3577143168157 39.91353096987616, -105.3578080288027 39.9135293149364, -105.3579479405976 39.91352684688559, -105.360726387632 39.91347774057059, -105.3626713467703 39.91344411322467, -105.3630360175505 39.91343780431702, -105.364028600592 39.91342062611375, -105.3654597559985 39.91339584487707, -105.3658523373689 39.91338904538176, -105.3665939284883 39.91337619259116, -105.3667161394004 39.91337407345735, -105.3668283884871 39.91337212820923, -105.3681499654785 39.9133492123433, -105.3687455638757 39.91333888041709, -105.3700998449686 39.91331537600603, -105.3701987914307 39.91331435275244, -105.3702803654887 39.91331351699651, -105.3713686533495 39.91330235646162, -105.3715726433937 39.91330026315164, -105.3723180191877 39.91329261324411, -105.3727062091699 39.91328862708968, -105.3728444536078 39.91328720727761, -105.3729372325635 39.91328625411846, -105.3730265786787 39.91328533762903, -105.3741243196769 39.91327405429676, -105.3746287719808 39.91326886562454, -105.3750805012749 39.91326421559691, -105.375528444443 39.91325960653901, -105.3759644480829 39.91325511617619, -105.3764989569724 39.91324961123397, -105.3770298750515 39.91324413780398, -105.3775644726632 39.91323862530895, -105.3781002538376 39.91323310077718, -105.3786426970783 39.91322750061524, -105.3791513838786 39.9132222497599, -105.379874445467 39.91321461308471, -105.3805848188801 39.91320710461893, -105.3814863544534 39.91319756945008, -105.382202498405 39.91318998939478, -105.3829076244009 39.91318252337764, -105.3837367354787 39.91317373903913, -105.3845278911197 39.91316534929708, -105.3850657205366 39.91315964310123, -105.3857696657633 39.91315217189074, -105.3863071920433 39.91314646229795, -105.3868507323952 39.91314068765575, -105.3874265259714 39.91313456821035, -105.3881273864053 39.91312711559791, -105.3888784839925 39.91311912178179, -105.3895167349293 39.91310925226507, -105.3900743869313 39.9131006235636, -105.3913934750771 39.91308020089357, -105.3917814950745 39.91307419044647, -105.3921958186435 39.91306777010362, -105.3926274455239 39.91306108069853, -105.3930632080981 39.91305432866896, -105.3934766670766 39.91304791642477, -105.3935153909127 39.9130473154753, -105.394319146609 39.9130348477802, -105.3952755188074 39.91302000864341, -105.3958087301344 39.91301172983554, -105.3964937997429 39.91300134792505, -105.3965903464187 39.91299959372266, -105.3966978356719 39.91299792220955, -105.3968488757159 39.91299557539469, -105.3983183962212 39.9129727357535, -105.3983210341569 39.91298417823263, -105.3983219324942 39.91301396556613, -105.3983223459219 39.91302772707497, -105.398333431356 39.91339613543983, -105.398333844787 39.91340989784895, -105.3983522526618 39.91402148383398, -105.3983526672674 39.9140352480448, -105.3983778425658 39.91487183135766, -105.3983782571737 39.91488560097144, -105.3983798343123 39.91493793235012, -105.3983802489236 39.91495170016253, -105.3983820599438 39.9150119224053, -105.3983824745547 39.91502569111829, -105.3984018106093 39.91566807851793, -105.3984022252254 39.91568184903149, -105.3984202050643 39.91627928250205, -105.3984208825517 39.91629325949732, -105.3984243463552 39.91635977428161, -105.3984245531202 39.91637331764547, -105.3984245542349 39.91637335457343, -105.3984250501899 39.9164385995149, -105.3984254133924 39.91645234206192, -105.3984493646693 39.91724802529494, -105.3984496473764 39.91726163177085, -105.398449648455 39.91726169301648, -105.3984507589101 39.91732038081131, -105.3984512786714 39.91733424868674, -105.39845370355 39.9173931285796, -105.3984541450573 39.91740692073075, -105.3984665193604 39.91781805006798, -105.398466933988 39.91783183048639, -105.3984798536997 39.91826093109985, -105.3984803290957 39.91827475210088, -105.3984828140969 39.91834515684929, -105.3984831785016 39.91835889218999, -105.3984848565185 39.91842687435983, -105.3984852594673 39.91844064756203, -105.3984990197162 39.91889776022787, -105.3984994355225 39.91891154334807, -105.3985162065597 39.91946874595399, -105.3985166959705 39.91948259218443, -105.3985205360901 39.91958806339631, -105.3985208900887 39.91960172667393, -105.3985208911554 39.91960179602547, -105.3985233411816 39.91970523863268, -105.3985237406861 39.9197189785061, -105.3985237406312 39.919719015433, -105.3985355249807 39.92011052426341, -105.3985359396254 39.92012431188453, -105.3985367254955 39.92015040730921, -105.3985371413104 39.9201641949313, -105.3985453221885 39.92043585466617, -105.3985457368344 39.92044964408826, -105.398546602953 39.92047841723579, -105.3985470187679 39.92049220755951, -105.3985604243746 39.92093742396103, -105.3985608390226 39.9209512160845, -105.3985652321848 39.92109710564678, -105.398565646836 39.92111089686941, -105.3985675196082 39.92117307806518, -105.3985679354288 39.92118687018941, -105.3985696120286 39.92124252415203, -105.398570026679 39.92125631717582, -105.3985772446762 39.92149599281457, -105.3985776593297 39.92150978583809, -105.3985781866026 39.92152729777273, -105.3985786012565 39.9215410907962, -105.398586678742 39.92180934142345, -105.3985870945678 39.92182313534828, -105.398594726368 39.92207647430345, -105.3985951410246 39.92209027002828, -105.3986023824908 39.92233080219584, -105.398602611461 39.92234439510914, -105.3986026125611 39.92234444194428, -105.3986027046735 39.92235094386645, -105.3986030959543 39.92236472876249, -105.3986114287511 39.92263132959327, -105.3986118213059 39.92264425886626, -105.3986118469183 39.92264512892318, -105.3986201020632 39.92291916730255, -105.398620516726 39.92293296572834, -105.3986229603509 39.92301411614823, -105.398623328441 39.92302776862658, -105.3986233306174 39.92302787850861, -105.3986247646202 39.92308232446863, -105.398625211001 39.92309603375719, -105.398625214331 39.9230961544481, -105.3986271203261 39.92315257776472, -105.3986275443485 39.92316637709919, -105.3986363458028 39.92345860470918, -105.3986367616392 39.92347240493673, -105.398640059122 39.92358199884207, -105.3986404340673 39.92359576570926, -105.3986593239096 39.92430639952359, -105.3986596895086 39.92432016367973, -105.3986610423362 39.92437101684337, -105.3986614091043 39.92438478190112, -105.398661938663 39.92440472380518, -105.3986623593045 39.92441844657942, -105.3986623615104 39.92441853664702, -105.3986642149489 39.9244773133269, -105.3986646506542 39.92449113338527, -105.3986653789949 39.92451428450352, -105.3986658147006 39.92452810456187, -105.3986735254079 39.92477281614058, -105.3986739611156 39.92478663709926, -105.39867628483 39.92486039120937, -105.3986767205375 39.92487421306861, -105.3986809267899 39.92500765354416, -105.3986813624992 39.92502147540325, -105.3986843521299 39.92511632167318, -105.398684787838 39.92513014533341, -105.3986860592404 39.92517046344225, -105.398686493782 39.92518428530008, -105.3986874544791 39.92521483371372, -105.3986878901898 39.9252286564732, -105.3986946649734 39.92544356989327, -105.3986950995171 39.92545739265146, -105.3986961730707 39.92549151406815, -105.3986966087809 39.92550533952928, -105.3986987962665 39.92557475415193, -105.398699587186 39.92558885822826, -105.3987008331634 39.92560926820119, -105.3987008308551 39.92562265015393, -105.3987008308083 39.92562268167683, -105.3987007035779 39.92563195472458, -105.3987010318213 39.92564567651554, -105.3987010329363 39.92564571344339, -105.3987025021679 39.925692263367, -105.3987029378834 39.92570608702656, -105.3987088054537 39.92589230022041, -105.3987092411689 39.92590612568109, -105.3987157668427 39.92611320315834, -105.3987162025581 39.92612703042011, -105.3987165086773 39.9261367442696, -105.398716944397 39.92615056882935, -105.3987174180642 39.92616562461984, -105.3987178537816 39.92617945098084, -105.3987232153443 39.92634959330871, -105.3987236510628 39.9263634205702, -105.3987268664642 39.92646544706136, -105.3987272813745 39.92647910768292, -105.3987272858266 39.92647926079844, -105.3987277296268 39.92649394999507, -105.3987281781977 39.92650778897621, -105.3987286203391 39.92652123076214, -105.3987290595639 39.92653506162907, -105.3987454149852 39.92705399372688, -105.3987453775411 39.92706740897156, -105.3987094196417 39.9305860929671, -105.3987092828172 39.93059946128667, -105.398687214628 39.93275895406263, -105.3986870777828</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" t="n">
+        <v>21</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>Nederland HS</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>597 Co Hwy 130, Nederland, CO 80466</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>https://neh.bvsd.org/</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>Nederland Middle/Senior High School</t>
         </is>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>39.95383849383303</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>-105.5233421126253</v>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>https://neh.bvsd.org/</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="O16" t="inlineStr">
         <is>
           <t>POINT (-105.5233421126253 39.95383849383303)</t>
         </is>
@@ -1497,48 +1547,51 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2665028856773 40.00008302921293, -105.2677639960641 40.0000800858277, -105.2687848652311 40.00008103962393, -105.2700220559592 40.00007912146844, -105.2712538896729 40.0000780026072, -105.2724860869347 40.00007495020975, -105.2737168453467 40.00007490171039, -105.2749419062467 40.00007098586583, -105.2749439353011 40.00183587613848, -105.2749439861859 40.0018452979681, -105.2749541445287 40.00371800203029, -105.2761939054203 40.00371410054612, -105.277421161032 40.00371400557973, -105.2774251347819 40.00413704801434, -105.2774248286698 40.00433991763281, -105.2774230429322 40.00488703093239, -105.2774240231571 40.00546187703087, -105.2778681120404 40.00545888939006, -105.2786630827622 40.00546398736055, -105.2798871783135 40.00545699704956, -105.2799030378844 40.0072899927621, -105.2811321477586 40.00728794062378, -105.2819328809913 40.00728396638529, -105.2819728960741 40.00727388539485, -105.2820611343066 40.00725401178327, -105.2831478234024 40.00724700172137, -105.284303060725 40.00723708977463, -105.2855649684075 40.00724905147178, -105.2864738555099 40.00724909075706, -105.2869468595005 40.00724996565361, -105.2872299698913 40.0072430760162, -105.2876390732287 40.00724410484807, -105.2884758772812 40.00723493682361, -105.2890631285643 40.007231894771, -105.2890970445134 40.00723113361098, -105.2891459174028 40.00724192903881, -105.2891968309264 40.00728594512627, -105.289223168539 40.00742709573112, -105.2892639375149 40.00751913492665, -105.2893250772793 40.0076040727572, -105.289405168331 40.00767888851305, -105.2895010031458 40.00774192810649, -105.2896179351386 40.00779402536224, -105.2897431274692 40.00782994113508, -105.2898541047652 40.00784496816384, -105.2900128690378 40.00787600294159, -105.2901651591649 40.00792294834658, -105.2903059756377 40.00798607001173, -105.2904830588015 40.00809702258108, -105.290661065552 40.00825601822979, -105.2907819711598 40.00840996903745, -105.2908690869226 40.00844982779828, -105.2914292843717 40.00892559132514, -105.2914292099533 40.00893843358583, -105.2908119707734 40.00893655268581, -105.2900712087696 40.00893743474369, -105.2900702103074 40.00921343500197, -105.2903549358019 40.00921443393288, -105.2906932101914 40.00921443417534, -105.2906925531651 40.00929912848419, -105.2906912943824 40.00945966739491, -105.2906902700733 40.00962089482662, -105.2906892101524 40.00976243394203, -105.2906912103231 40.0098434340922, -105.2906906047592 40.01003956613808, -105.2906912104696 40.01034743433848, -105.290154209284 40.01034543526126, -105.2901552136538 40.0103924349007, -105.2900632101764 40.01038843427113, -105.29015521014 40.01039243489431, -105.2904481483452 40.01050448448408, -105.2907130561806 40.01063845205723, -105.2910521068837 40.01081245315488, -105.2913502088046 40.0109674357598, -105.2914002106621 40.01099343436549, -105.2915172102254 40.01104143452457, -105.2915192101345 40.01082443421697, -105.2916219709538 40.01082393365192, -105.2918546625634 40.01082371352069, -105.2921922106798 40.01082443486659, -105.2921912106079 40.01114143453822, -105.2921692110959 40.01143943493722, -105.2922312110156 40.01149543479373, -105.2922312110259 40.01162343450338, -105.2924722100788 40.01164043413667, -105.292480210274 40.01167843441603, -105.2926421528956 40.0116779178345, -105.2931072112711 40.01167643394096, -105.2931065501837 40.01189546581841, -105.293105976447 40.01208570852052, -105.293105211251 40.01233943420036, -105.2927022113221 40.01233843488738, -105.2926981092893 40.01260199958435, -105.292694211126 40.01285243494313, -105.2927912101938 40.01285643433663, -105.2931333503741 40.0128564352352, -105.2935512109194 40.0128564346988, -105.2936372113 40.01280243515163, -105.2938052106283 40.01277843517675, -105.2942141485911 40.01273466443779, -105.2948142108489 40.01267043461998, -105.2948072105055 40.01255543418904, -105.2948072112871 40.01214143441656, -105.2952052115695 40.01213443502252, -105.2953132109346 40.01212543471485, -105.2954662113391 40.01215043446568, -105.2957822123902 40.01218343415776, -105.2957852116624 40.012505434982, -105.295809211419 40.01257043426351, -105.2961832109625 40.01252843470885, -105.2969222108167 40.01264143451774, -105.2969212186651 40.01238543430799, -105.2969202114587 40.01211443461543, -105.2972624798172 40.01217012068312, -105.2974242114839 40.01219643372481, -105.2974275838077 40.01218258042406, -105.2974892276555 40.01192397025246, -105.2975392118156 40.01170843394527, -105.2976410500742 40.01171848383155, -105.2976912121973 40.01172343446013, -105.298122211411 40.01176843426795, -105.2984517355405 40.01181772238958, -105.2985718404069 40.01183568677898, -105.2986066136606 40.01177065292691, -105.2986916238546 40.01160627754996, -105.2992927086213 40.01167132375566, -105.2994896376608 40.01169225972444, -105.2993653365875 40.01249054937211, -105.2993753074033 40.01249150609813, -105.2993692121943 40.01253043425595, -105.299705267281 40.01255424261292, -105.3002518157827 40.01259380600695, -105.3004884530218 40.01261020130202, -105.3007216280422 40.01262778439228, -105.3007216232754 40.01262781230426, -105.3007216161107 40.01262785912573, -105.3007562324528 40.01263038942474, -105.3008117447473 40.01263456076815, -105.3009032128719 40.01264143397508, -105.3009735379753 40.01278267752139, -105.301023340076 40.01288285103966, -105.3010281067779 40.01289306454397, -105.3010292126056 40.01289543426423, -105.3011202771397 40.01296410208901, -105.3011419577046 40.01298029445854, -105.3011632841785 40.01299621061416, -105.3011729464176 40.01300340546396, -105.3011729942204 40.0130034812011, -105.3011764667329 40.01300603603117, -105.3011789468909 40.01300787493373, -105.301205212717 40.01302743462566, -105.3012592457636 40.01298185572877, -105.3013522126834 40.01290343407975, -105.3014602128255 40.01281143480046, -105.3014452129743 40.01287743392142, -105.3014437804599 40.01293093194339, -105.3014430498437 40.01295818709555, -105.3014422127245 40.01298943465143, -105.3013862127445 40.01335443432603, -105.3013157480595 40.01351102356379, -105.3012602122003 40.01363443507628, -105.3012511657355 40.01363978016212, -105.3010182134563 40.01377743388108, -105.3010158302282 40.01400687156732, -105.3010146521981 40.01412034528163, -105.3010143555852 40.01412043663623, -105.3010065439604 40.01412285491573, -105.3009841703811 40.01413088704314, -105.3008359183136 40.01416110284114, -105.300684149682 40.01417292017293, -105.3005359990144 40.01416799685423, -105.300254092653 40.01412001668933, -105.300067868143 40.0140719279547, -105.3000011606622 40.01405287069223, -105.2996880626172 40.01392796986438, -105.2994309509394 40.01382595114303, -105.2990971694855 40.01369387506902, -105.2989748438362 40.01364891574665, -105.2987091069599 40.01356691986554, -105.2984361789157 40.01350193131028, -105.2981560643021 40.0134531259425, -105.2978951689382 40.01342411927098, -105.2975649848486 40.01340487234885, -105.297280077546 40.01340711706504, -105.2972629400945 40.01340708693889, -105.2968701231647 40.01343988732408, -105.2966129379867 40.013483906396, -105.2959720191087 40.01362689650804, -105.2955889946644 40.01372696689724, -105.2951188286011 40.01383593998661, -105.2948950990359 40.01391405477982, -105.2948279437313 40.01392601395955, -105.2948850709373 40.01404306065437, -105.2949111667633 40.01415099338725, -105.2949149278989 40.01420590378106, -105.2949106525785 40.01428611088715, -105.2948669406371 40.01436130597801, -105.2948050566042 40.01443646962085, -105.2945651847544 40.01463397060598, -105.2942962425791 40.01484536492688, -105.2941799322994 40.01493717604964, -105.2940456558378 40.01498431869415, -105.2935522291935 40.01508380053187, -105.2932648974691 40.01514153813964, -105.2929311934506 40.01520907552712, -105.2924838834105 40.01529960385942, -105.2916482773999 40.01546871123976, -105.2904817987244 40.01572217487955, -105.2891551001181 40.01599098183944, -105.2885419939298 40.01611983770974, -105.2878670067061 40.0162528717229, -105.2866812529073 40.01650245354258, -105.2865308262578 40.01653288651573, -105.2852128642166 40.01680605680808, -105.2850088672696 40.01684712918449, -105.2841060700353 40.01702607643248, -105.2840110981352 40.01704713596685, -105.2838089245483 40.01709196535331, -105.2837991589066 40.01709413112621, -105.2838869444426 40.01755905605179, -105.2839600121989 40.01782410420856, -105.2840818920156 40.01812191122571, -105.280344103938 40.01889429097838, -105.2800122511694 40.01792531871845, -105.2797922499383 40.0173063188877, -105.2796422519211 40.01688331794094, -105.2795172500427 40.01656331893992, -105.2793182480616 40.01593431868323, -105.2792882488983 40.01584331888502, -105.279283131531 40.01582838979826, -105.2790212496877 40.01506431947683, -105.2789422504309 40.01484831880367, -105.2788752505237 40.01466131864607, -105.278851249496 40.01459531880194, -105.2786822492777 40.01411631803115, -105.2786769521653 40.01410055096331, -105.278663968713 40.01410393231048, -105.2782030961592 40.01419611210767, -105.278005899344 40.01423306829994, -105.2775250367717 40.01432794849211, -105.2773539185385 40.01436001199994, -105.2764250735946 40.01453802385365, -105.2760611408061 40.01457602595389, -105.2746458800721 40.01458095527774, -105.2736219240902 40.0145838908234, -105.2725519067238 40.01458809993736, -105.2716550449331 40.01459291590101, -105.270220141546 40.01459912551402, -105.2689819637891 40.01460406242605, -105.2678219770818 40.01460804739548, -105.2662260626349 40.01461196195721, -105.2657616256185 40.01461332253763, -105.2646558644589 40.01461288522881, -105.2638765422727 40.01460508854388, -105.2630753109644 40.01461633090538, -105.2630299591908 40.01461696725389, -105.258420544823 40.01462569237854, -105.2583967697713 40.01738897110558, -105.2583835533824 40.017841051784, -105.2583845465005 40.01820405441318, -105.2583845261048 40.01916806167687, -105.2583865082488 40.02003406862268, -105.2583999303681 40.02054880387701, -105.2584077255942 40.02163362987389, -105.2583830465151 40.0223399835016, -105.2583789356683 40.02339906985873, -105.2583811009352 40.02450099341501, -105.258382877582 40.02551095323694, -105.2585261275946 40.02549395801625, -105.2588440818718 40.02545097495982, -105.2603669897415 40.02515904067031, -105.2609680305519 40.02503593129295, -105.2619428416898 40.02483590064909, -105.2634068292216 40.02453694257784, -105.2637180536465 40.02447608769097, -105.2639678550197 40.02441702917763, -105.2652839000161 40.02414601860607, -105.2665938779832 40.02387086387858, -105.2679109587122 40.02360394413302, -105.2682411423188 40.02458107234318, -105.2684139123429 40.02522791115344, -105.2684711463209 40.02519810372616, -105.268499879351 40.02514902278204, -105.2685628779465 40.02510412746538, -105.2686079015087 40.02509488435066, -105.2687318382624 40.02508607416824, -105.2689580821212 40.02502311364085, -105.2695930218969 40.02490194833804, -105.2698180480713 40.02488208254371, -105.2701351511876 40.02487695076279, -105.2705571374207 40.02490112502463, -105.2711471268735 40.02497888759054, -105.2711960062075 40.02499106319144, -105.271283153701 40.02498492246853, -105.2714558843878 40.02490702710772, -105.2715121215238 40.02496094431037, -105.2716481672724 40.02506800120462, -105.2724079619951 40.02551696877548, -105.2725230499857 40.02559186516272, -105.2725799692758 40.02565593982267, -105.2726199882499 40.02575512003067, -105.2726178873861 40.02606394994715, -105.2726181274602 40.02620587677047, -105.2726248698914 40.02675410445867, -105.2726378711389 40.02799495559294, -105.2726431137961 40.02931402807485, -105.2726510020113 40.03005387211383, -105.2726558625326 40.03073798238746, -105.2726628596342 40.03142401880926, -105.2726661710148 40.03160905132167, -105.272671164566 40.03193189473561, -105.2726760357997 40.03272004799683, -105.2726760239568 40.0331518655748, -105.2726820898275 40.03390296023866, -105.2726840628362 40.03406108764794, -105.2726881734809 40.03464911391067, -105.2726940852457 40.03630310060525, -105.272693011895 40.03641098462665, -105.2722969317176 40.03641486978847, -105.270493035731 40.03641102135016, -105.2685051665427 40.03642104917662, -105.268183023931 40.03642204958091, -105.2647380295588 40.03643099813947, -105.263225170679 40.03643586385155, -105.2622890950964 40.03643997857341, -105.2612830205331 40.03644393997342, -105.2605001712293 40.03644396467524, -105.2590269395231 40.03645297536733, -105.2585008484345 40.03646011079696, -105.258446899267 40.03646603760756, -105.258455895004 40.03685010807402, -105.2584720435084 40.03753396766986, -105.2584653846817 40.03890912737619, -105.2584811444412 40.04010595201317, -105.2576250499565 40.04010196086148, -105.2572561306026 40.04009487076375, -105.2570050616881 40.04009104854779, -105.2564700565923 40.04008607648185, -105.2541156704493 40.04008547509496, -105.2541114189239 40.04008556330383, -105.2541130449594 40.0400350024811, -105.2541075664353 40.03908055851134, -105.2536959323025 40.03907688210359, -105.2536949545598 40.03812015275444, -105.2535405399283 40.03814509251686, -105.2533805946551 40.03816870800271, -105.2532201543185 40.03819018946845, -105.2530592634851 40.0382095298022, -105.2528979772607 40.03822672371619, -105.2527363390311 40.03824176679848, -105.252574399222 40.03825465195054, -105.2524122082365 40.03826537837855, -105.252087273247 40.03828033297279, -105.2519246265246 40.03828456224724, -105.2517619181192 40.03828706191138, -105.2515262941062 40.03828575038629, -105.2500216866296 40.03828440663961, -105.2489428716393 40.03828342936805, -105.2476788464136 40.03828923237084, -105.2463663111993 40.03830715832521, -105.2456601157548 40.03831973388306, -105.2446044735468 40.03855084401205, -105.2425780966287 40.03862463649937, -105.2427781086196 40.03829124483734, -105.2430111166943 40.0379132414562, -105.2432991274496 40.03743023787163, -105.2438753893139 40.0364924229959, -105.2440929793375 40.03610011054108, -105.2444588367812 40.03552861301022, -105.2453730542609 40.03402702879499, -105.2462652351348 40.03255119866444, -105.2466014210446 40.03199231009842, -105.2468743915512 40.03153389625475, -105.2470384585521 40.03125730147787, -105.2470527888195 40.03123232722809, -105.2472377688188 40.03090995649731, -105.2474157554355 40.03059976586545, -105.2475764919784 40.03031963966591, -105.2477685658453 40.02998489963429, -105.247983553166 40.0296102141241, -105.2481541927388 40.02931308733002, -105.2482195454966 40.02920455652909, -105.2475199805581 40.02920302743363, -105.2471535866196 40.02920497006868, -105.2470046722872 40.02920574144774, -105.2467879073245 40.02920691310877, -105.2459758332215 40.02921391257004, -105.2448980525407 40.02922690726311, -105.2447080626234 40.02923005531607, -105.2441955801484 40.02923144538298, -105.2431311238466 40.02922408398609, -105.2400198840386 40.02917511185208, -105.2395431210193 40.02918391916977, -105.2382999573494 40.02920828260488, -105.2375975186471 40.02922070455187, -105.2365361783417 40.02922211126447, -105.2346081604372 40.02922894693484, -105.2335989823584 40.02923101313294, -105.2329054947644 40.02923023263606, -105.2326919485125 40.02923001266877, -105.2317567030328 40.02922893947044, -105.2312381944585 40.02922828192708, -105.2308360988211 40.02922789375545, -105.2303165160975 40.02922777805944, -105.2300240500278 40.02922791711205, -105.2291319973156 40.02923104149665, -105.2286845476068 40.02923108871217, -105.2275989594909 40.02923100067746, -105.2260059682783 40.02922091333762, -105.2259449032419 40.029221042971, -105.2258520567489 40.02922109704281, -105.2253876759348 40.02922707245764, -105.2253838715813 40.02922712104237, -105.2250902606939 40.02922118797638, -105.2243452592167 40.02922218854747, -105.2242922587597 40.02922218887095, -105.2240485290634 40.0292221896779, -105.2240448012386 40.02921896182992, -105.2234171967727 40.02858844157902, -105.2231341967773 40.02873844263139, -105.2227491964695 40.02893444274527, -105.2221531959837 40.02913544191373, -105.2220471963629 40.0291604417221, -105.2217758048782 40.02920913506678, -105.2216681962193 40.02922844212854, -105.2215368541062 40.02924212396792, -105.221524196698 40.02924344258807, -105.2213741961431 40.02925244173912, -105.2209515721532 40.02925336013067, -105.22047383285 40.0292534418192, -105.2199463053364 40.02925557303384, -105.2191025662913 40.02925881640458, -105.2185102178733 40.02926210714222, -105.2184761957898 40.02926244201551, -105.2180831955133 40.02926644208032, -105.2178571961912 40.02928944246727, -105.2177341859115 40.02931463718165, -105.2176198784911 40.0293380499647, -105.2175251954509 40.02935744244781, -105.2173882346814 40.02940610874885, -105.2172628810816 40.02945581657214, -105.2171013733368 40.02953197961455, -105.2170861959579 40.02953944212074, -105.2169183296271 40.02964944212096, -105.216714195362 40.02978944179781, -105.216393195045 40.030018442685, -105.2163231954602 40.03000344222524, -105.2162281958708 40.02996544241743, -105.2161731957375 40.02993344293114, -105.2160821948466 40.029843442886, -105.2160431949233 40.02976544318457, -105.2160301953674 40.0296674427522, -105.2160241944471 40.02958644314366, -105.2160111955 40.02941744250101, -105.2159851951632 40.0292884429292, -105.2159541953328 40.02928944287671, -105.2158601952949 40.02929244290664, -105.2154397747579 40.02930063641094, -105.2142271952085 40.02931444306602, -105.2132951941631 40.02931044250712, -105.2121779687597 40.02931370359353, -105.2116561945448 40.0293154428859, -105.2115561934457 40.02929544246373, -105.2114661938733 40.02925644249451, -105.2113901939955 40.02920244289452, -105.2113691942612 40.02918144297956, -105.21132119374 40.02911044242671, -105.2112971941228 40.02903344233737, -105.2113005886311 40.02886265923356, -105.2113071938985 40.02853044222877, -105.2113161932457 40.02663444274262, -105.2112871930142 40.02556744269105, -105.2112831926451 40.02472144241093, -105.2112831927006 40.02414744200545, -105.2112661927701 40.02380644202619, -105.2112281926976 40.02354844225731, -105.2111681958693 40.02340961220849, -105.2111421929906 40.02334944202191, -105.2110908591813 40.02325882755933, -105.2110271929919 40.02314644131605, -105.2109292903985 40.02301884637291, -105.2109051937388 40.02298744145597, -105.2108295770383 40.02291528432966, -105.2107433476153 40.02283715262609, -105.2106593493525 40.0227561515699, -105.2104213509922 40.02261115079264, -105.210131353124 40.02246915041668, -105.2096453553682 40.02228714891598, -105.2092683557341 40.02218214859246, -105.2089568292927 40.02211259715015, -105.2085064200148 40.02197920421263, -105.2081351092813 40.0218317118302, -105.2077919256969 40.02163067272885, -105.2073173661939 40.02133714445619, -105.2072853658604 40.02131414432528, -105.2071853679822 40.02123014325992, -105.2069473712818 40.02099014246873, -105.2067823753913 40.02074214075176, -105.2066866789568 40.02047579851763, -105.2066508805403 40.02015162089645, -105.2066396306025 40.01988469898361, -105.2066282588804 40.01964637159548, -105.2066417223345 40.0193985748575, -105.2066873211797 40.01744464479255, -105.2067009491717 40.01715872104394, -105.2066918318187 40.01639614326426, -105.2067183070375 40.01600540075746, -105.2067098058444 40.0150998456722, -105.2067203549632 40.0147049988613, -105.2067196345875 40.01470499883064, -105.2066710004365 40.01470499853, -105.206367999478 40.01470099950867, -105.2059949767234 40.01469404358584, -105.2059949427587 40.01469404259862, -105.2055099991169 40.01468499841905, -105.2052452071275 40.01468054190908, -105.2052129998992 40.0146799993535, -105.2050079696713 40.01467855822093, -105.2048625378809 40.01467753585545, -105.2046439989874 40.01467599916017, -105.2045197317803 40.01467615277912, -105.2038309998592 40.01467699888822, -105.2036568942967 40.01467716858118, -105.2036567103979 40.01467716810863, -105.2028090273656 40.01467798954275, -105.2027581900902 40.01266844174256, -105.2038051899005 40.01281044069496, -105.2043981908388 40.01288544030034, -105.2045691898613 40.01294644116913, -105.2048331905392 40.01297844102542, -105.2050351910883 40.01296044132123, -105.2050398702081 40.01392145197964, -105.2050431900852 40.0146034419073, -105.2069742231526 40.01462497172324, -105.2078121909381 40.01462344028587, -105.2078361910397 40.01348944102689, -105.2075011914237 40.01348844053171, -105.2074681901274 40.01104044140051, -105.2098111911977 40.01104044022411, -105.2098286476958 40.01241859730428, -105.2098292659196 40.01246736656677, -105.2098311921049 40.01261944051893, -105.2101881770135 40.0126180919686, -105.2101880793582 40.01262205279892, -105.2121356176559 40.01262468172177, -105.2130646768166 40.01262642336378, -105.213064157268 40.01258789120162, -105.2130673059102 40.01280105946651, -105.2130736861623 40.01323274517098, -105.2130740693893 40.01339608598071, -105.2130777016322 40.01363575086111, -105.2130940324873 40.01467594647242, -105.2130969381798 40.01474897599216, -105.2130981903515 40.01474897460401, -105.2141074361257 40.0147478477099, -105.2148764361527 40.01473067926249, -105.2148910155936 40.01473046222324, -105.2157340623453 40.01471789690481, -105.215735902945 40.01471779606526, -105.2164723909476 40.01467739814613, -105.2164899016262 40.01467620189562, -105.217100941391 40.01463444043784, -105.2191844656205 40.01463953261158, -105.2239170504272 40.01464087196651, -105.2245834902002 40.0146398382582, -105.2254128747107 40.01466887521181, -105.2254145473955 40.01466887288986, -105.2258513852783 40.01466824594888, -105.2272090327501 40.01466628746812, -105.2281480626285 40.01466492383204, -105.22915700892 40.01466702306828, -105.230058133229 40.01466913584839, -105.2309519694455 40.01468609977, -105.2319659677214 40.01469691984863, -105.2338293506786 40.01473924403673, -105.234785953114 40.0147380290238, -105.2364884675618 40.01473462743368, -105.2379838714334 40.01472804370003, -105.239268545971 40.01470520202151, -105.2401101703597 40.01465348406194, -105.2407671682903 40.01461834492035, -105.2422256658095 40.01457244483336, -105.2432112087095 40.01457106881134, -105.2449033960308 40.01456052644195, -105.2460469422521 40.01457377343792, -105.2465954644375 40.01458212939171, -105.2477575533147 40.0146096980253, -105.2489568317006 40.01463733680855, -105.2501120279116 40.01463197668197, -105.2537731835135 40.0146261868912, -105.2537949903803 40.01406758669711, -105.2538081303951 40.01360465598484, -105.2538054741536 40.01274848195483, -105.2537806712891 40.01248002734037, -105.253715823358 40.01226403757396, -105.2536241596939 40.01204202995962, -105.2535630325855 40.01186593254538, -105.2535261719986 40.01169290685051, -105.2535019003321 40.01119789590327, -105.2535030853529 40.01100293505052, -105.2535039273517 40.01086430388367, -105.2535061296354 40.01032410969325, -105.2535068895725 40.00892900280688, -105.2535011689129 40.00823994697006, -105.2535111127166 40.00805686367984, -105.2535018757067 40.00784711067982, -105.2534788384062 40.0077021148444, -105.2534580881613 40.00761587168582, -105.253390440773 40.00738013872348, -105.2531470399376 40.00675897970751, -105.2531119710475 40.00658513352174, -105.2531028651088 40.00594493428408, -105.2531010238238 40.00517188259421, -105.2531039801196 40.00445402054249, -105.2531108838922 40.00373012711088, -105.2540440020844 40.00372910138983, -105.2583379493246 40.00373488608032, -105.258572133868 40.00373098416479, -105.2586434447849 40.0037284900354, -105.2586556382503 40.00290996136781, -105.2586436430115 40.00235946687246, -105.2586454140996 40.00185904416556, -105.2586142067626 40.00148365856045, -105.2585687794402 40.00118688281169, -105.2584680337078 40.00076130850472, -105.2583433547495 40.00053228127841, -105.2581675632618 40.00029957202448, -105.2589195861169 40.00036267320748, -105.2592544037049 40.00038408331039, -105.259251053428 40.00025364728025, -105.2593301393748 40.00027828043822, -105.2595041374749 40.0003192800807, -105.2597321375767 40.00033028045623, -105.2602051376428 40.00033828032775, -105.2606671387836 40.00031627988058, -105.2613031379176 40.00026628085262, -105.2614471376263 40.00025428044938, -105.262564137449 40.0001492804175, -105.2635226869538 40.00007661770653, -105.2635271382638 40.00007628008433, -105.2635316634515 40.00008266869302, -105.2635362436151 40.00008232142758, -105.263577605498 40.00014071094439, -105.2635825036177 40.00014762629726, -105.2636677621977 40.00013487760815, -105.2636851372977 40.00013227971019, -105.2637656435806 40.0000901112732, -105.2637600945748 40.00008210840647, -105.2643058348404 40.00009201025707, -105.2650550950247 40.00008502916437, -105.2665028856773 40.00008302921293), (-105.2782259265416 40.01288889235155, -105.2782434257579 40.01293071174543, -105.2782259988166 40.01288899876749, -105.2782259265416 40.01288889235155), (-105.2884699572886 40.0104089180808, -105.2887237568676 40.01041448734374, -105.2887551645736 40.01041517623894, -105.2884699572886 40.0104089180808), (-105.2899762105711 40.01037143456766, -105.2896527354309 40.01039073227599, -105.2892512100549 40.01041243440763, -105.2896527354281 40.01039073317661, -105.2899762105711 40.01037143456766))</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
+          <t>POLYGON ((-105.2586436430115 40.00235946687246, -105.2586454140996 40.00185904416556, -105.2586142067626 40.00148365856045, -105.2585687794402 40.00118688281169, -105.2584680337078 40.00076130850472, -105.2583433547495 40.00053228127841, -105.2581675632618 40.00029957202448, -105.2589195861169 40.00036267320748, -105.2592544037049 40.00038408331039, -105.259251053428 40.00025364728025, -105.2593301393748 40.00027828043822, -105.2595041374749 40.0003192800807, -105.2597321375767 40.00033028045623, -105.2602051376428 40.00033828032775, -105.2606671387836 40.00031627988058, -105.2613031379176 40.00026628085262, -105.2614471376263 40.00025428044938, -105.262564137449 40.0001492804175, -105.2635226869538 40.00007661770653, -105.2635271382638 40.00007628008433, -105.2635316634515 40.00008266869302, -105.2635362436151 40.00008232142758, -105.263577605498 40.00014071094439, -105.2635825036177 40.00014762629726, -105.2636677621977 40.00013487760815, -105.2636851372977 40.00013227971019, -105.2637656435806 40.0000901112732, -105.2637600945748 40.00008210840647, -105.2643058348404 40.00009201025707, -105.2650550950247 40.00008502916437, -105.2665028856773 40.00008302921293, -105.2677639960641 40.0000800858277, -105.2687848652311 40.00008103962393, -105.2700220559592 40.00007912146844, -105.2712538896729 40.0000780026072, -105.2724860869347 40.00007495020975, -105.2737168453467 40.00007490171039, -105.2749419062467 40.00007098586583, -105.2749439353011 40.00183587613848, -105.2749439861859 40.0018452979681, -105.2749541445287 40.00371800203029, -105.2761939054203 40.00371410054612, -105.277421161032 40.00371400557973, -105.2774251347819 40.00413704801434, -105.2774248286698 40.00433991763281, -105.2774230429322 40.00488703093239, -105.2774240231571 40.00546187703087, -105.2778681120404 40.00545888939006, -105.2786630827622 40.00546398736055, -105.2798871783135 40.00545699704956, -105.2799030378844 40.0072899927621, -105.2811321477586 40.00728794062378, -105.2819328809913 40.00728396638529, -105.2819728960741 40.00727388539485, -105.2820611343066 40.00725401178327, -105.2831478234024 40.00724700172137, -105.284303060725 40.00723708977463, -105.2855649684075 40.00724905147178, -105.2864738555099 40.00724909075706, -105.2869468595005 40.00724996565361, -105.2872299698913 40.0072430760162, -105.2876390732287 40.00724410484807, -105.2884758772812 40.00723493682361, -105.2890631285643 40.007231894771, -105.2890970445134 40.00723113361098, -105.2891459174028 40.00724192903881, -105.2891968309264 40.00728594512627, -105.289223168539 40.00742709573112, -105.2892639375149 40.00751913492665, -105.2893250772793 40.0076040727572, -105.289405168331 40.00767888851305, -105.2895010031458 40.00774192810649, -105.2896179351386 40.00779402536224, -105.2897431274692 40.00782994113508, -105.2898541047652 40.00784496816384, -105.2900128690378 40.00787600294159, -105.2901651591649 40.00792294834658, -105.2903059756377 40.00798607001173, -105.2904830588015 40.00809702258108, -105.290661065552 40.00825601822979, -105.2907819711598 40.00840996903745, -105.2908690869226 40.00844982779828, -105.2914292843717 40.00892559132514, -105.2914292099533 40.00893843358583, -105.2908119707734 40.00893655268581, -105.2900712087696 40.00893743474369, -105.2900702103074 40.00921343500197, -105.2903549358019 40.00921443393288, -105.2906932101914 40.00921443417534, -105.2906925531651 40.00929912848419, -105.2906912943824 40.00945966739491, -105.2906902700733 40.00962089482662, -105.2906892101524 40.00976243394203, -105.2906912103231 40.0098434340922, -105.2906906047592 40.01003956613808, -105.2906912104696 40.01034743433848, -105.290154209284 40.01034543526126, -105.2901552136538 40.0103924349007, -105.2900632101764 40.01038843427113, -105.29015521014 40.01039243489431, -105.2904481483452 40.01050448448408, -105.2907130561806 40.01063845205723, -105.2910521068837 40.01081245315488, -105.2913502088046 40.0109674357598, -105.2914002106621 40.01099343436549, -105.2915172102254 40.01104143452457, -105.2915192101345 40.01082443421697, -105.2916219709538 40.01082393365192, -105.2918546625634 40.01082371352069, -105.2921922106798 40.01082443486659, -105.2921912106079 40.01114143453822, -105.2921692110959 40.01143943493722, -105.2922312110156 40.01149543479373, -105.2922312110259 40.01162343450338, -105.2924722100788 40.01164043413667, -105.292480210274 40.01167843441603, -105.2926421528956 40.0116779178345, -105.2931072112711 40.01167643394096, -105.2931065501837 40.01189546581841, -105.293105976447 40.01208570852052, -105.293105211251 40.01233943420036, -105.2927022113221 40.01233843488738, -105.2926981092893 40.01260199958435, -105.292694211126 40.01285243494313, -105.2927912101938 40.01285643433663, -105.2931333503741 40.0128564352352, -105.2935512109194 40.0128564346988, -105.2936372113 40.01280243515163, -105.2938052106283 40.01277843517675, -105.2942141485911 40.01273466443779, -105.2948142108489 40.01267043461998, -105.2948072105055 40.01255543418904, -105.2948072112871 40.01214143441656, -105.2952052115695 40.01213443502252, -105.2953132109346 40.01212543471485, -105.2954662113391 40.01215043446568, -105.2957822123902 40.01218343415776, -105.2957852116624 40.012505434982, -105.295809211419 40.01257043426351, -105.2961832109625 40.01252843470885, -105.2969222108167 40.01264143451774, -105.2969212186651 40.01238543430799, -105.2969202114587 40.01211443461543, -105.2972624798172 40.01217012068312, -105.2974242114839 40.01219643372481, -105.2974275838077 40.01218258042406, -105.2974892276555 40.01192397025246, -105.2975392118156 40.01170843394527, -105.2976410500742 40.01171848383155, -105.2976912121973 40.01172343446013, -105.298122211411 40.01176843426795, -105.2984517355405 40.01181772238958, -105.2985718404069 40.01183568677898, -105.2986066136606 40.01177065292691, -105.2986916238546 40.01160627754996, -105.2992927086213 40.01167132375566, -105.2994896376608 40.01169225972444, -105.2993653365875 40.01249054937211, -105.2993753074033 40.01249150609813, -105.2993692121943 40.01253043425595, -105.299705267281 40.01255424261292, -105.3002518157827 40.01259380600695, -105.3004884530218 40.01261020130202, -105.3007216280422 40.01262778439228, -105.3007216232754 40.01262781230426, -105.3007216161107 40.01262785912573, -105.3007562324528 40.01263038942474, -105.3008117447473 40.01263456076815, -105.3009032128719 40.01264143397508, -105.3009735379753 40.01278267752139, -105.301023340076 40.01288285103966, -105.3010281067779 40.01289306454397, -105.3010292126056 40.01289543426423, -105.3011202771397 40.01296410208901, -105.3011419577046 40.01298029445854, -105.3011632841785 40.01299621061416, -105.3011729464176 40.01300340546396, -105.3011729942204 40.0130034812011, -105.3011764667329 40.01300603603117, -105.3011789468909 40.01300787493373, -105.301205212717 40.01302743462566, -105.3012592457636 40.01298185572877, -105.3013522126834 40.01290343407975, -105.3014602128255 40.01281143480046, -105.3014452129743 40.01287743392142, -105.3014437804599 40.01293093194339, -105.3014430498437 40.01295818709555, -105.3014422127245 40.01298943465143, -105.3013862127445 40.01335443432603, -105.3013157480595 40.01351102356379, -105.3012602122003 40.01363443507628, -105.3012511657355 40.01363978016212, -105.3010182134563 40.01377743388108, -105.3010158302282 40.01400687156732, -105.3010146521981 40.01412034528163, -105.3010143555852 40.01412043663623, -105.3010065439604 40.01412285491573, -105.3009841703811 40.01413088704314, -105.3008359183136 40.01416110284114, -105.300684149682 40.01417292017293, -105.3005359990144 40.01416799685423, -105.300254092653 40.01412001668933, -105.300067868143 40.0140719279547, -105.3000011606622 40.01405287069223, -105.2996880626172 40.01392796986438, -105.2994309509394 40.01382595114303, -105.2990971694855 40.01369387506902, -105.2989748438362 40.01364891574665, -105.2987091069599 40.01356691986554, -105.2984361789157 40.01350193131028, -105.2981560643021 40.0134531259425, -105.2978951689382 40.01342411927098, -105.2975649848486 40.01340487234885, -105.297280077546 40.01340711706504, -105.2972629400945 40.01340708693889, -105.2968701231647 40.01343988732408, -105.2966129379867 40.013483906396, -105.2959720191087 40.01362689650804, -105.2955889946644 40.01372696689724, -105.2951188286011 40.01383593998661, -105.2948950990359 40.01391405477982, -105.2948279437313 40.01392601395955, -105.2948850709373 40.01404306065437, -105.2949111667633 40.01415099338725, -105.2949149278989 40.01420590378106, -105.2949106525785 40.01428611088715, -105.2948669406371 40.01436130597801, -105.2948050566042 40.01443646962085, -105.2945651847544 40.01463397060598, -105.2942962425791 40.01484536492688, -105.2941799322994 40.01493717604964, -105.2940456558378 40.01498431869415, -105.2935522291935 40.01508380053187, -105.2932648974691 40.01514153813964, -105.2929311934506 40.01520907552712, -105.2924838834105 40.01529960385942, -105.2916482773999 40.01546871123976, -105.2904817987244 40.01572217487955, -105.2891551001181 40.01599098183944, -105.2885419939298 40.01611983770974, -105.2878670067061 40.0162528717229, -105.2866812529073 40.01650245354258, -105.2865308262578 40.01653288651573, -105.2852128642166 40.01680605680808, -105.2850088672696 40.01684712918449, -105.2841060700353 40.01702607643248, -105.2840110981352 40.01704713596685, -105.2838089245483 40.01709196535331, -105.2837991589066 40.01709413112621, -105.2838869444426 40.01755905605179, -105.2839600121989 40.01782410420856, -105.2840818920156 40.01812191122571, -105.280344103938 40.01889429097838, -105.2800122511694 40.01792531871845, -105.2797922499383 40.0173063188877, -105.2796422519211 40.01688331794094, -105.2795172500427 40.01656331893992, -105.2793182480616 40.01593431868323, -105.2792882488983 40.01584331888502, -105.279283131531 40.01582838979826, -105.2790212496877 40.01506431947683, -105.2789422504309 40.01484831880367, -105.2788752505237 40.01466131864607, -105.278851249496 40.01459531880194, -105.2786822492777 40.01411631803115, -105.2786769521653 40.01410055096331, -105.278663968713 40.01410393231048, -105.2782030961592 40.01419611210767, -105.278005899344 40.01423306829994, -105.2775250367717 40.01432794849211, -105.2773539185385 40.01436001199994, -105.2764250735946 40.01453802385365, -105.2760611408061 40.01457602595389, -105.2746458800721 40.01458095527774, -105.2736219240902 40.0145838908234, -105.2725519067238 40.01458809993736, -105.2716550449331 40.01459291590101, -105.270220141546 40.01459912551402, -105.2689819637891 40.01460406242605, -105.2678219770818 40.01460804739548, -105.2662260626349 40.01461196195721, -105.2657616256185 40.01461332253763, -105.2646558644589 40.01461288522881, -105.2638765422727 40.01460508854388, -105.2630753109644 40.01461633090538, -105.2630299591908 40.01461696725389, -105.258420544823 40.01462569237854, -105.2537731835135 40.0146261868912, -105.2537949903803 40.01406758669711, -105.2538081303951 40.01360465598484, -105.2538054741536 40.01274848195483, -105.2537806712891 40.01248002734037, -105.253715823358 40.01226403757396, -105.2536241596939 40.01204202995962, -105.2535630325855 40.01186593254538, -105.2535261719986 40.01169290685051, -105.2535019003321 40.01119789590327, -105.2535030853529 40.01100293505052, -105.2535039273517 40.01086430388367, -105.2535061296354 40.01032410969325, -105.2535068895725 40.00892900280688, -105.2535011689129 40.00823994697006, -105.2535111127166 40.00805686367984, -105.2535018757067 40.00784711067982, -105.2534788384062 40.0077021148444, -105.2534580881613 40.00761587168582, -105.253390440773 40.00738013872348, -105.2531470399376 40.00675897970751, -105.2531119710475 40.00658513352174, -105.2531028651088 40.00594493428408, -105.2531010238238 40.00517188259421, -105.2531039801196 40.00445402054249, -105.2531108838922 40.00373012711088, -105.2540440020844 40.00372910138983, -105.2583379493246 40.00373488608032, -105.258572133868 40.00373098416479, -105.2586434447849 40.0037284900354, -105.2586556382503 40.00290996136781, -105.2586436430115 40.00235946687246), (-105.2782434257579 40.01293071174543, -105.2782259988166 40.01288899876749, -105.2782259265416 40.01288889235155, -105.2782434257579 40.01293071174543), (-105.2887551645736 40.01041517623894, -105.2884699572886 40.0104089180808, -105.2887237568676 40.01041448734374, -105.2887551645736 40.01041517623894), (-105.2896527354281 40.01039073317661, -105.2899762105711 40.01037143456766, -105.2896527354309 40.01039073227599, -105.2892512100549 40.01041243440763, -105.2896527354281 40.01039073317661))</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>22</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>New Vista</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>700 20th St, Boulder, CO 80302</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>http://nvh.bvsd.org/</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/mVZ7Cv3jx5iSPW3u9</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>New Vista High School</t>
         </is>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>40.0011978462681</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>-105.266504379284</v>
       </c>
-      <c r="L17" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr">
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr">
         <is>
           <t>POINT (-105.266504379284 40.0011978462681)</t>
         </is>
@@ -1558,53 +1611,56 @@
           <t>POLYGON ((-105.178285099815 40.05095033556441, -105.1782909993724 40.05078899852872, -105.1783619916895 40.05013707172179, -105.1783619978893 40.05013699968696, -105.1783889994008 40.0494039987319, -105.1783889921711 40.04940279904402, -105.1783850000171 40.04872299868529, -105.1783823374743 40.04787297522466, -105.1783819997574 40.04776499876323, -105.1783700003943 40.04545199887659, -105.1783569989513 40.04397399911803, -105.1783593807407 40.04381992401295, -105.1783670002116 40.04332699857592, -105.1783709996006 40.04307199909479, -105.1783800001195 40.04215799916332, -105.1783800027096 40.04215794693271, -105.1783870000278 40.04106199875608, -105.1783899999625 40.04087199920473, -105.1783900004663 40.04081899851942, -105.1783920002899 40.04072099871122, -105.1784048433664 40.03966053615192, -105.1784199995207 40.03840899927504, -105.1784249996421 40.03670199816679, -105.1784399998176 40.03537799842891, -105.1784889999836 40.03472599927464, -105.178490000368 40.03469499888762, -105.178531999708 40.03353499925799, -105.1785369999334 40.03339099877271, -105.1785399991614 40.03279999949025, -105.1785309996551 40.03216499864769, -105.1784769999151 40.03169499900179, -105.1784589989599 40.03107899928678, -105.1784620001129 40.03036699889137, -105.1784680003464 40.02915899894963, -105.1785019999882 40.0272379988253, -105.1785159996695 40.0261089991069, -105.1785169994261 40.02605499869539, -105.1784799995173 40.02439999821404, -105.1784639995815 40.02391999874165, -105.1784449993586 40.02333599866598, -105.1784189992241 40.02213199938647, -105.1784120001571 40.02177899910858, -105.1783799991943 40.02048599914978, -105.1783460002359 40.01914399873556, -105.1783049994997 40.01838899907003, -105.1782029988481 40.01737399931093, -105.1781489999591 40.01684399893904, -105.1781320000762 40.01633599939375, -105.1781410003895 40.01595099914135, -105.1782570004259 40.01483999953051, -105.1782689995687 40.01463299858616, -105.179412999948 40.01461999874561, -105.1808354543097 40.01462562931187, -105.1827040007133 40.01463299831895, -105.1834549992717 40.0146349225061, -105.1838739999368 40.01463599886635, -105.1841701799736 40.01463570346134, -105.1858630004019 40.01463399899924, -105.1864974973728 40.01463462047163, -105.1868859994811 40.01463499863746, -105.1879306387029 40.01464043574966, -105.1880389993641 40.01464099911838, -105.1886723010191 40.01463892504425, -105.1895639999455 40.01463599872144, -105.1942429993284 40.01465399917136, -105.1943553939693 40.01465460062421, -105.1951779999087 40.01465899884218, -105.1966359998847 40.01466699895634, -105.1967699330014 40.01466790959612, -105.1967830001021 40.0146679988932, -105.1983059994697 40.01466299922393, -105.1988599995382 40.01467899903977, -105.2006159994158 40.01467999898198, -105.2009300000826 40.01468399931195, -105.201182717144 40.01468616479592, -105.2012799993588 40.01468699864344, -105.2020565681202 40.01468240032865, -105.2020579655673 40.01468239223043, -105.2027989994621 40.01467799882614, -105.2038309998592 40.01467699888822, -105.2045197317803 40.01467615277912, -105.2046439989874 40.01467599916017, -105.2048625378809 40.01467753585545, -105.2052129998992 40.0146799993535, -105.2052452071275 40.01468054190908, -105.2055099991169 40.01468499841905, -105.206367999478 40.01470099950867, -105.2066710004365 40.01470499853, -105.2067203549632 40.0147049988613, -105.2067098058444 40.0150998456722, -105.2067183070375 40.01600540075746, -105.2066918318187 40.01639614326426, -105.2067009491717 40.01715872104394, -105.2066873211797 40.01744464479255, -105.2066417223345 40.0193985748575, -105.2066282588804 40.01964637159548, -105.2066396306025 40.01988469898361, -105.2066508805403 40.02015162089645, -105.2066866789568 40.02047579851763, -105.2067823753913 40.02074214075176, -105.2069473712818 40.02099014246873, -105.2071853679822 40.02123014325992, -105.2072853658604 40.02131414432528, -105.2073173661939 40.02133714445619, -105.2077919256969 40.02163067272885, -105.2081351092813 40.0218317118302, -105.2085064200148 40.02197920421263, -105.2089568292927 40.02211259715015, -105.2092683557341 40.02218214859246, -105.2096453553682 40.02228714891598, -105.210131353124 40.02246915041668, -105.2104213509922 40.02261115079264, -105.2106593493525 40.0227561515699, -105.2107433476153 40.02283715262609, -105.2108295770383 40.02291528432966, -105.2109051937388 40.02298744145597, -105.2109292903985 40.02301884637291, -105.2110271929919 40.02314644131605, -105.2110908591813 40.02325882755933, -105.2111421929906 40.02334944202191, -105.2111681958693 40.02340961220849, -105.2112281926976 40.02354844225731, -105.2112661927701 40.02380644202619, -105.2112831927006 40.02414744200545, -105.2112831926451 40.02472144241093, -105.2112871930142 40.02556744269105, -105.2113161932457 40.02663444274262, -105.2113071938985 40.02853044222877, -105.2113005886311 40.02886265923356, -105.2112971941228 40.02903344233737, -105.21132119374 40.02911044242671, -105.2113691942612 40.02918144297956, -105.2113901939955 40.02920244289452, -105.2114661938733 40.02925644249451, -105.2115561934457 40.02929544246373, -105.2116561945448 40.0293154428859, -105.2121779687597 40.02931370359353, -105.2132951941631 40.02931044250712, -105.2142271952085 40.02931444306602, -105.2154397747579 40.02930063641094, -105.2158601952949 40.02929244290664, -105.2159541953328 40.02928944287671, -105.2159851951632 40.0292884429292, -105.2160111955 40.02941744250101, -105.2160241944471 40.02958644314366, -105.2160301953674 40.0296674427522, -105.2160431949233 40.02976544318457, -105.2160821948466 40.029843442886, -105.2161731957375 40.02993344293114, -105.2162281958708 40.02996544241743, -105.2163231954602 40.03000344222524, -105.216393195045 40.030018442685, -105.216714195362 40.02978944179781, -105.2169183296271 40.02964944212096, -105.2170861959579 40.02953944212074, -105.2171013733368 40.02953197961455, -105.2172628810816 40.02945581657214, -105.2173882346814 40.02940610874885, -105.2175251954509 40.02935744244781, -105.2176198784911 40.0293380499647, -105.2177341859115 40.02931463718165, -105.2178571961912 40.02928944246727, -105.2180831955133 40.02926644208032, -105.2184761957898 40.02926244201551, -105.2185102178733 40.02926210714222, -105.2191025662913 40.02925881640458, -105.2199463053364 40.02925557303384, -105.22047383285 40.0292534418192, -105.2209515721532 40.02925336013067, -105.2213741961431 40.02925244173912, -105.221524196698 40.02924344258807, -105.2215368541062 40.02924212396792, -105.2216681962193 40.02922844212854, -105.2217758048782 40.02920913506678, -105.2220471963629 40.0291604417221, -105.2221531959837 40.02913544191373, -105.2227491964695 40.02893444274527, -105.2231341967773 40.02873844263139, -105.2234171967727 40.02858844157902, -105.2240448012386 40.02921896182992, -105.2240485290634 40.0292221896779, -105.2242922587597 40.02922218887095, -105.2243452592167 40.02922218854747, -105.2250902606939 40.02922118797638, -105.2253838715813 40.02922712104237, -105.2253876759348 40.02922707245764, -105.2253944375382 40.02922698588036, -105.2258520567489 40.02922109704281, -105.2259449032419 40.029221042971, -105.2260059682783 40.02922091333762, -105.2275989594909 40.02923100067746, -105.2286845476068 40.02923108871217, -105.2291319973156 40.02923104149665, -105.2300240500278 40.02922791711205, -105.2303165160975 40.02922777805944, -105.2308360988211 40.02922789375545, -105.2312381944585 40.02922828192708, -105.2317567030328 40.02922893947044, -105.2326919485125 40.02923001266877, -105.2329054947644 40.02923023263606, -105.2335989823584 40.02923101313294, -105.2346081604372 40.02922894693484, -105.2365361783417 40.02922211126447, -105.2375975186471 40.02922070455187, -105.2382999573494 40.02920828260488, -105.2395431210193 40.02918391916977, -105.2400198840386 40.02917511185208, -105.2431311238466 40.02922408398609, -105.2441955801484 40.02923144538298, -105.2447080626234 40.02923005531607, -105.2448980525407 40.02922690726311, -105.2459758332215 40.02921391257004, -105.2467879073245 40.02920691310877, -105.2470046722872 40.02920574144774, -105.2471535866196 40.02920497006868, -105.2475199805581 40.02920302743363, -105.2482195454966 40.02920455652909, -105.2481541927388 40.02931308733002, -105.247983553166 40.0296102141241, -105.2477685658453 40.02998489963429, -105.2475764919784 40.03031963966591, -105.2474157554355 40.03059976586545, -105.2472377688188 40.03090995649731, -105.2470527888195 40.03123232722809, -105.2470384585521 40.03125730147787, -105.2468743915512 40.03153389625475, -105.2466014210446 40.03199231009842, -105.2462652351348 40.03255119866444, -105.2453730542609 40.03402702879499, -105.2444588367812 40.03552861301022, -105.2440929793375 40.03610011054108, -105.2438753893139 40.0364924229959, -105.2432991274496 40.03743023787163, -105.2430111166943 40.0379132414562, -105.2427781086196 40.03829124483734, -105.2425780966287 40.03862463649937, -105.2437996973181 40.03858015455958, -105.2446044735468 40.03855084401205, -105.2456601157548 40.03831973388306, -105.2463663111993 40.03830715832521, -105.2476788464136 40.03828923237084, -105.2489428716393 40.03828342936805, -105.2500216866296 40.03828440663961, -105.2515262941062 40.03828575038629, -105.2517619181192 40.03828706191138, -105.2519246265246 40.03828456224724, -105.252087273247 40.03828033297279, -105.2524122082365 40.03826537837855, -105.252574399222 40.03825465195054, -105.2527363390311 40.03824176679848, -105.2528979772607 40.03822672371619, -105.2530592634851 40.0382095298022, -105.2532201543185 40.03819018946845, -105.2533805946551 40.03816870800271, -105.2535405399283 40.03814509251686, -105.2536949545598 40.03812015275444, -105.2536959323025 40.03907688210359, -105.2541075664353 40.03908055851134, -105.2541130449594 40.0400350024811, -105.2541114189239 40.04008556330383, -105.2541156704493 40.04008547509496, -105.2564700565923 40.04008607648185, -105.2570050616881 40.04009104854779, -105.2572561306026 40.04009487076375, -105.2576250499565 40.04010196086148, -105.2584811444412 40.04010595201317, -105.2585019067495 40.04140309591936, -105.2585200529217 40.0428339247763, -105.2585328883272 40.04344502971864, -105.258535903728 40.04360206066097, -105.2585405106698 40.04557391508014, -105.2585412801613 40.04583500499989, -105.2585431409786 40.0466000914717, -105.2585491366171 40.04702505910149, -105.2585801436604 40.04744788236328, -105.2586361577098 40.04786993381616, -105.2587031080589 40.04822996778709, -105.2587330305727 40.04835411276961, -105.2588011065953 40.04859802744705, -105.2588770324828 40.04884497745633, -105.2589520194323 40.04905404325294, -105.2590968835464 40.04940298337421, -105.2592908491195 40.04980693019196, -105.2594790114012 40.05013509748598, -105.2595461504909 40.05024092674891, -105.2597039348822 40.05047294914017, -105.2598909228966 40.05073001337415, -105.2600729289857 40.05098212507661, -105.2601188264747 40.05103410417082, -105.2602141708121 40.05114493352249, -105.2603760318205 40.0513360595755, -105.2605749425811 40.05155608753633, -105.2606671334609 40.05164988950381, -105.2607870983266 40.05176900406456, -105.2609530191591 40.05192390191151, -105.2610698287841 40.05202599008051, -105.2612450666888 40.0521729459601, -105.2614929991048 40.05237111141436, -105.2617659165283 40.0525759170593, -105.2620028794537 40.05274495970432, -105.2621960311828 40.05287795048658, -105.2623361003706 40.0529699277751, -105.2624829531093 40.05306301764614, -105.2628900215765 40.05331696043408, -105.2636688880578 40.05380006284676, -105.2643711340155 40.05423304186316, -105.2651129178647 40.0547020581333, -105.2656519227221 40.05503202749767, -105.2668749737009 40.05580013493221, -105.2682239553873 40.05662805383557, -105.269613922533 40.05749501959285, -105.2704799468352 40.05801009468256, -105.2708018933556 40.05820399463217, -105.2713911776679 40.05857795867715, -105.2730720982822 40.05964009195046, -105.2764060265012 40.06171701384444, -105.2766818087143 40.0618889301708, -105.2794570843467 40.06360607635985, -105.2799809979885 40.06393952401127, -105.2802739685094 40.06411686471955, -105.280571421083 40.06429735375461, -105.2809515658617 40.06431108663833, -105.2814222747994 40.06419864439965, -105.2818065024136 40.0636562328228, -105.282127928685 40.06372330059435, -105.282319982506 40.06372626586732, -105.2832962374926 40.06372837690664, -105.2835079480766 40.06372864274691, -105.283919471611 40.06372879883411, -105.2844681111398 40.06372971757044, -105.2844693643109 40.06404057361777, -105.2844743893111 40.06528829290035, -105.2844750682011 40.06545646919614, -105.2844696482367 40.06556530130753, -105.2844419581037 40.06556495868456, -105.2844392150506 40.0657224424132, -105.2843132151617 40.06563044283727, -105.2842552150438 40.06560344292603, -105.2842092152591 40.06558744250346, -105.2841555199931 40.0655765955805, -105.2841102147732 40.06556744313233, -105.2840422155819 40.0655634422325, -105.2840396611971 40.06556052476189, -105.2826421053623 40.06555460571782, -105.2823076520964 40.06555737709394, -105.2818205276817 40.06556514578249, -105.2821777644898 40.06610051550977, -105.2824690223394 40.06665264506963, -105.2826287480644 40.0671032160873, -105.282708682352 40.06730598772923, -105.2827667487974 40.0674749475167, -105.2828103083754 40.06759885395986, -105.2828828825465 40.06781286879525, -105.2830899236575 40.06843101948598, -105.283447132496 40.06958603676775, -105.2839564523263 40.07122915445703, -105.2841258539786 40.07178289850857, -105.2844119360205 40.07272887084649, -105.2844238046166 40.07276114874126, -105.2845098877672 40.0730540823975, -105.284634842972 40.07354103535643, -105.2846740115247 40.07381095898337, -105.2846799442029 40.07408191848048, -105.2846558254534 40.07436407727556, -105.2846140488599 40.07458004438773, -105.2844881096322 40.07496797674111, -105.2843430443443 40.07530206774775, -105.2841729060126 40.07565395617164, -105.284061438017 40.07587059340077, -105.2839819795333 40.07602502070181, -105.2839320007679 40.07612210589992, -105.2838018419132 40.0763738690773, -105.2826709107073 40.07859011936667, -105.2825129694785 40.07892198794374, -105.2823438719979 40.07938999478642, -105.2823048577945 40.07952086600779, -105.2822690597651 40.07965201797717, -105.2822223466844 40.07989150774977, -105.2821342160606 40.0791254445771, -105.2821112161553 40.07666744386643, -105.2782532143109 40.07666244408787, -105.278372214492 40.07653744417692, -105.2783742148064 40.07579144511136, -105.2780202147794 40.07579044515734, -105.2779022152453 40.07603844420503, -105.2777612150901 40.07620044483633, -105.2776022148752 40.07633644500343, -105.2774795717141 40.0764360956394, -105.277414215237 40.07647944379102, -105.2774182151642 40.07662844439344, -105.2774232152314 40.07679644423713, -105.277462333618 40.07819218232893, -105.277486220627 40.07914765992864, -105.2775032146846 40.07989444554472, -105.2774442150245 40.07989344467622, -105.2774492150437 40.079994445459, -105.2760592152198 40.07997644544199, -105.275236925473 40.07998199934345, -105.2741904007602 40.07997698391911, -105.2738472151207 40.07997344533944, -105.2732488422515 40.07998423568615, -105.2722111865081 40.08000293913378, -105.271602868858 40.08001390036796, -105.270773469619 40.08002883906712, -105.269120467453 40.08006436083225, -105.2678107184368 40.08009626548748, -105.265906623877 40.08014227963445, -105.2635022120304 40.08020744623987, -105.263475212196 40.07824944591677, -105.2552788447606 40.07829042246069, -105.2509901360431 40.07831039649412, -105.2479762077927 40.07832544680577, -105.2467352086361 40.07833144715077, -105.245048207299 40.07833944731037, -105.2446880583013 40.07833920790986, -105.2446880588089 40.07833844686491, -105.2435522068469 40.07833844725607, -105.2423652076105 40.07833744689923, -105.2403432064991 40.07833344770941, -105.2384812068036 40.07833244791702, -105.2378132062725 40.07833444783447, -105.2352892054144 40.07873844737262, -105.2334432055741 40.07899144749057, -105.2299052044168 40.08008044876753, -105.2350032064051 40.08016044862552, -105.2350497203358 40.08268589163298, -105.2350776389745 40.08420165278985, -105.2350852057845 40.0846124484227, -105.2351382054217 40.08551144874158, -105.2351162069385 40.08560644881669, -105.2349272055709 40.08608544943124, -105.2347532059639 40.0863524487831, -105.2346296381483 40.08650825210744, -105.2344113616564 40.08671008020809, -105.2342874907976 40.08682176614175, -105.2342102060382 40.08689144861766, -105.2341886118381 40.08690464559623, -105.2341742062996 40.08691344866173, -105.234116919408 40.08694927681879, -105.2340547143473 40.08698818193187, -105.2340141176357 40.08701357127359, -105.2338752055783 40.08710044895112, -105.2337498879304 40.08716518662143, -105.2336642062275 40.0872094484582, -105.233557508418 40.08725212883198, -105.2334842065225 40.08728144947539, -105.2335198087354 40.08730061994037, -105.2335350154684 40.08731185997121, -105.2335182680553 40.08731887517195, -105.2334670391323 40.08733945284803, -105.2334153508784 40.08735934044687, -105.2333632162177 40.08737853169327, -105.2333106562827 40.0873970203308, -105.2332572252643 40.08741486387087, -105.2332115864704 40.0874290192368, -105.233160289808 40.08744409547717, -105.2331195646996 40.08745541432238, -105.2331086089517 40.08745846109794, -105.2330565603615 40.08747210532881, -105.2330041639691 40.08748502911613, -105.2329514268327 40.08749722707182, -105.232898377103 40.08750869745924, -105.2328450159892 40.08751943127434, -105.2327913728077 40.08752942858451, -105.232737453437 40.08753868580036, -105.2326832836757 40.08754720298132, -105.2326288764451 40.08755497475301, -105.2325748982646 40.08756217648359, -105.2325209052109 40.08756868375681, -105.2324667696581 40.08757444944327, -105.2324125138727 40.08757947719696, -105.2323581460858 40.0875837616329, -105.2323036897474 40.08758730370593, -105.2322491612788 40.08759010255342, -105.2321945759326 40.08759215640933, -105.232139950141 40.08759346170912, -105.2320852944376 40.08759402388102, -105.2320306369806 40.0875938393878, -105.2319759906559 40.08759291186197, -105.2319213672231 40.08759123322496, -105.2318667865754 40.08758881433079, -105.2318122651521 40.08758564981383, -105.2317578193674 40.08758174061293, -105.2317034632943 40.08757708676092, -105.2316492191852 40.08757169551478, -105.2315951034686 40.08756556421094, -105.2315411374752 40.08755923148525, -105.2283729549368 40.08717092525384, -105.2272444844378 40.08716355701311, -105.2272236163383 40.08716344466387, -105.2271977580158 40.08717057341977, -105.2271717266588 40.08717815928905, -105.2271459834793 40.08718610609185, -105.2271204311677 40.08719440999577, -105.2270950662131 40.08720306919137, -105.227069908556 40.08721208192462, -105.2270449570381 40.08722144459034, -105.2270202222304 40.08723115271041, -105.226995713506 40.08724120810847, -105.2269713781346 40.08725160165343, -105.2269462956309 40.08726233387031, -105.2269214580284 40.08727339899931, -105.226896880574 40.08728479617606, -105.2268725621166 40.08729651999401, -105.2268485155578 40.08730856958332, -105.2268247444441 40.08732093774738, -105.2268012569799 40.08733362540633, -105.226778067272 40.08734662358735, -105.2267551729715 40.08735993318564, -105.2267325834878 40.08737354701852, -105.2267103070542 40.08738745880117, -105.2266883530404 40.08740167125784, -105.2266667226549 40.08741617538511, -105.2266454253037 40.08743096490092, -105.2266244715363 40.08744604073107, -105.2266038602236 40.08746139206541, -105.22658359957 40.0874770198241, -105.2265637001611 40.08749291592657, -105.2265441631842 40.08750907677334, -105.226524998038 40.0875254978835, -105.2265062070929 40.08754217295839, -105.2264878009205 40.08755909752002, -105.2264697795498 40.08757626436348, -105.2264521500162 40.08759367350561, -105.226434455812 40.08761141663134, -105.2264158800905 40.08762967283475, -105.2263977138776 40.0876481506639, -105.2263825065714 40.08766855838156, -105.2263789361496 40.08767231912204, -105.2263767305145 40.08767464926904, -105.2263745307277 40.0876769830324, -105.2263723344585 40.0876793168041, -105.2263701416961 40.08768165328597, -105.2263679524405 40.08768399247809, -105.2263657702201 40.0876863316868, -105.2263635879888 40.08768867359738, -105.2263614080953 40.08769101731477, -105.2263592363989 40.0876933637535, -105.2263570647023 40.08769571019219, -105.226354900023 40.08769806115065, -105.2263527353471 40.08770041120849, -105.2263505776958 40.08770276398484, -105.2263484247239 40.08770511947421, -105.2263462740824 40.08770747857164, -105.2263441269622 40.08770983677667, -105.2263419810035 40.08771219768641, -105.2263398455944 40.08771455952174, -105.2263377078255 40.08771692495404, -105.2263355759121 40.08771929220145, -105.226333448689 40.08772165945994, -105.2263313249726 40.08772402942868, -105.2263292047701 40.08772640030627, -105.2263270845495 40.0877287756871, -105.2263249737094 40.08773115109006, -105.226322866376 40.08773352920324, -105.2263207637256 40.08773590912882, -105.2263186598953 40.08773829085281, -105.2263165619241 40.08774067349134, -105.226314467456 40.08774305974064, -105.2263123800232 40.08774544600666, -105.2263102972735 40.08774783408501, -105.2263082145056 40.08775022666651, -105.2263061352625 40.08775261745505, -105.2263040642092 40.08775501276614, -105.2263019919905 40.08775740627321, -105.2262999267926 40.08775980339941, -105.2262978662741 40.08776220323865, -105.2262958045756 40.08776460487633, -105.2262937499053 40.08776700833194, -105.226291699918 40.08776941359987, -105.2262896569624 40.08777181978507, -105.2262876128304 40.08777422686813, -105.2262855745432 40.08777663846826, -105.2262835374175 40.08777905277302, -105.2262815085034 40.08778146619655, -105.2262794831069 40.0877838796284, -105.2262774576886 40.08778629846402, -105.2262754393057 40.08778871731626, -105.2262734244331 40.08779113797818, -105.2262714142507 40.0877935586511, -105.2262694052227 40.08779598382996, -105.2262674008741 40.08779841172184, -105.2262654059096 40.08780083873525, -105.2262634085889 40.08780326844501, -105.2262614183 40.08780569907206, -105.2262594326977 40.0878081306108, -105.226257445901 40.08781056755058, -105.2262554673158 40.08781300360911, -105.2262534898923 40.08781544237237, -105.2262515195077 40.08781788025156, -105.2262495549714 40.08782032174722, -105.2262475892516 40.08782276594194, -105.2262456270494 40.08782521014498, -105.2262436742169 40.08782765707216, -105.2262417237222 40.08783010580613, -105.2262397767451 40.08783255454839, -105.2262378332675 40.08783500780219, -105.2262358933076 40.08783746106425, -105.2262339568581 40.08783991613592, -105.226232023919 40.08784237301715, -105.2262300991841 40.08784483081848, -105.2262281732657 40.08784729131887, -105.2262262543791 40.08784975273657, -105.2262243401755 40.08785221596659, -105.226222428306 40.08785468190413, -105.2262205211268 40.08785714785272, -105.2262186162781 40.08785961740938, -105.2262167161233 40.08786208607652, -105.2262148218203 40.0878645574594, -105.2262129298625 40.08786702884783, -105.2262110437421 40.0878695065546, -105.2262091611538 40.08787198066713, -105.2262072808852 40.08787446108968, -105.2262054064867 40.08787693972477, -105.226203534426 40.08787942016669, -105.2262016682208 40.08788190242377, -105.2261998043462 40.08788438828893, -105.226197947507 40.08788687417072, -105.226196091833 40.08788936185654, -105.2261942361589 40.08789184954237, -105.2261923945412 40.08789434086405, -105.2261905517435 40.08789683398418, -105.2261887112837 40.08789932891115, -105.2261868778629 40.08790182295415, -105.2261850455965 40.08790432150305, -105.2261832203618 40.08790682096924, -105.2261813974722 40.08790932044101, -105.2261795792655 40.08791182172511, -105.2261777645729 40.08791432391816, -105.2261759557322 40.08791682882699, -105.2261741480568 40.08791933553987, -105.226172348582 40.08792184407345, -105.2261705502725 40.0879243544111, -105.2261687566533 40.08792686475982, -105.2261669688859 40.08792937782427, -105.2261651799496 40.08793188998534, -105.2261634015482 40.08793440667458, -105.2261616231395 40.08793692516508, -105.2261598505936 40.08793944366944, -105.2261580815545 40.08794196488402, -105.2261563172056 40.08794448610973, -105.2261545551981 40.08794700824161, -105.2261528013842 40.08794953399544, -105.2261510475738 40.08795205884863, -105.226149300777 40.08795458912228, -105.2261475563434 40.08795711489833, -105.2261458165711 40.08795964789051, -105.2261440803236 40.08796217908979, -105.2261423475865 40.08796471209865, -105.2261406218776 40.08796724692545, -105.2261388996683 40.08796978626372, -105.2261371809875 40.08797232290842, -105.2261354658207 40.08797486046209, -105.2261337541534 40.08797740252725, -105.2261320460038 40.0879799446007, -105.2261303460513 40.08798248939556, -105.2261286460914 40.08798503599166, -105.226126950829 40.08798758079754, -105.2261252602387 40.08799013011774, -105.2261235755077 40.08799268035245, -105.2261218943052 40.08799522789362, -105.2261202165914 40.08799778264812, -105.226118542406 40.08800033470907, -105.2261168764069 40.08800289219328, -105.2261152092496 40.08800544607216, -105.2261135491024 40.08800800627216, -105.2261118948289 40.0880105637841, -105.2261102405372 40.08801312579922, -105.2261085932736 40.08801568963229, -105.2261069495313 40.08801825257306, -105.2261053092994 40.08802081732343, -105.2261036725816 40.08802338298269, -105.2261020440572 40.08802595226398, -105.2261004178852 40.08802851974954, -105.2260987916986 40.08803109083762, -105.2260971760652 40.08803366195077, -105.2260955615934 40.08803623576855, -105.2260939506355 40.08803881049528, -105.2260923455334 40.08804138703718, -105.2260907451214 40.08804396359018, -105.2260891482163 40.08804654285341, -105.2260875536562 40.08804912212216, -105.2260859637863 40.08805170140207, -105.2260843809301 40.08805428610243, -105.2260827980811 40.08805686900151, -105.2260812222603 40.08805945371852, -105.2260796499462 40.0880620411458, -105.226078084664 40.08806462949036, -105.2260765193853 40.08806721693423, -105.2260749611275 40.0880698079974, -105.2260734087289 40.088072399975, -105.2260718574956 40.08807499375673, -105.2260703097799 40.08807758754672, -105.2260687690924 40.08808018315465, -105.2260672295774 40.08808277876541, -105.2260656970834 40.08808537799534, -105.2260641669416 40.08808797542954, -105.2260626414721 40.08809057737804, -105.2260611230379 40.08809317934323, -105.2260596034202 40.08809578400751, -105.2260580920141 40.08809838779062, -105.2260565841257 40.08810099158206, -105.2260550832546 40.0881035998933, -105.2260535823798 40.08810620910523, -105.2260520885404 40.08810881833376, -105.2260505993841 40.08811142937476, -105.2260491125655 40.08811404222255, -105.2260476280957 40.08811665417521, -105.226046152992 40.08811926975269, -105.2260446767192 40.08812188442674, -105.2260432086508 40.08812450002085, -105.2260417429166 40.08812711832244, -105.2260402865523 40.08812973934819, -105.2260388290152 40.08813236037112, -105.2260373773409 40.08813498140795, -105.226035930357 40.08813760245592, -105.2260344868726 40.08814022801536, -105.2260330445643 40.08814285267693, -105.2260316128055 40.08814547826421, -105.2260301833774 40.08814810745953, -105.2260289772142 40.08815032829153, -105.2260799511012 40.08815043483378, -105.2260951784236 40.08815046645809, -105.2259971464311 40.08825128178296, -105.2258660776002 40.08846675183878, -105.2258442047025 40.08817345056035, -105.225847257111 40.08702564690289, -105.2258422045073 40.08612344890279, -105.2246712037403 40.08611344976358, -105.2246852045713 40.08554044892636, -105.2230462031982 40.08603244956893, -105.2219812039535 40.08618344991433, -105.2211162029895 40.08627444986659, -105.2211262032423 40.08639345027048, -105.2182432027494 40.08641344971119, -105.2182532019159 40.08714945059754, -105.2163692023297 40.08714545077098, -105.216360202134 40.08892145040806, -105.2163292022599 40.08892045018143, -105.2159742024865 40.08892045011142, -105.2148588360544 40.08892679371123, -105.2148042021617 40.08892745043244, -105.2143002021996 40.08892245043239, -105.213437201397 40.08892445097817, -105.2114362013246 40.08891745132185, -105.2102848781286 40.08891722303895, -105.2093902465011 40.08891684883024, -105.208456199712 40.08891645102268, -105.2075245971012 40.08890693460845, -105.2069481319076 40.08890527106102, -105.2069438732727 40.0889052926268, -105.2069747075104 40.09435044215074, -105.2067688747363 40.09435139755085, -105.2067696857456 40.09448197611559, -105.206084292794 40.09448027846468, -105.204067954345 40.09447526321931, -105.2020925487541 40.09447072187066, -105.2004028346573 40.09447194731246, -105.2000942419318 40.09447216840297, -105.20004901646 40.0944713051883, -105.1999431444402 40.09446928464906, -105.1961591443175 40.09444728514715, -105.1941921454042 40.0944432846204, -105.1914201445046 40.09443828540665, -105.1878551441828 40.09443028595678, -105.1878554742897 40.09442402015232, -105.1878581437286 40.09437328585741, -105.1878579783739 40.09437328631103, -105.1878583084638 40.09436702410904, -105.1878489982433 40.09436703406432, -105.1869333094328 40.09436802324625, -105.1869288298045 40.09436799308698, -105.1864923089405 40.09436502536359, -105.1851823083869 40.09435602463465, -105.1851806430128 40.0943560507158, -105.1847691909817 40.09436254127205, -105.1842981568986 40.09474644455597, -105.1842254973132 40.09480566330672, -105.1770289540793 40.10167497796913, -105.1763019499671 40.1023029683946, -105.1688417643584 40.10884061707407, -105.1685799278165 40.10901976085416, -105.1674439177613 40.11003576716704, -105.1614528663692 40.11528080007928, -105.1594641412873 40.11689641328065, -105.1594566443818 40.11609286922273, -105.159467921669 40.11419687283805, -105.1594718259507 40.11205812132699, -105.1594520114176 40.10922888777313, -105.1594495599439 40.10886022285561, -105.1594219558605 40.10315811995677, -105.1594259842159 40.10399044520795, -105.1594259918098 40.10399197542836, -105.1590781918603 40.10400245670831, -105.1588411915942 40.10426645671227, -105.1588201907179 40.10434845704976, -105.1589061910858 40.10450845692532, -105.1588991905787 40.10458445709242, -105.1587201908592 40.10476045668218, -105.1584981900914 40.10477145654381, -105.1581892413284 40.10490396872007, -105.1580761909817 40.10495245717316, -105.1576681914213 40.10507845747404, -105.1572321903226 40.10529845652795, -105.1571241898577 40.1053754563856, -105.1571241900853 40.10546345672344, -105.157253190884 40.10562845707536, -105.157239191129 40.10571045628147, -105.157138190582 40.10579245659894, -105.1569951900118 40.10582045723518, -105.1565797245652 40.10604856929712, -105.1564161904518 40.10613345690832, -105.1557151895679 40.10621545706669, -105.155372190027 40.10630845692795, -105.1551781906975 40.10638545677693, -105.1551071895624 40.106484457227, -105.1549851905804 40.10658345749179, -105.1546631906193 40.10667645674386, -105.1543781900811 40.10669245702027, -105.1538481902248 40.10664345777509, -105.1536831893247 40.10669845729011, -105.153533190452 40.10679645699769, -105.1534041890178 40.10683545695765, -105.1532181895994 40.10680245729557, -105.1529611896807 40.10678045703483, -105.1528251894787 40.1068184572149, -105.1528251898034 40.10689545706076, -105.1527461895664 40.10708745705721, -105.1527891896304 40.10716445739909, -105.1530821895656 40.10724745707277, -105.1531971895655 40.10730745767818, -105.1532041904084 40.10742245698562, -105.1531681905297 40.10752745787505, -105.1530101897713 40.1076424577811, -105.1526961899649 40.10774645807478, -105.1522381891769 40.1078014575306, -105.1521161891182 40.10785645730169, -105.1520521905081 40.10809245803009, -105.1518081899357 40.10844445794176, -105.1518011892207 40.10854845784844, -105.1519151896514 40.1086254581982, -105.1522161898024 40.10867445774499, -105.1522521895131 40.10872445833751, -105.1522441899349 40.10883445806299, -105.1521871900507 40.10886745719991, -105.1521720437602 40.10888555509551, -105.152168642065 40.10888557367066, -105.152058189739 40.10899345806407, -105.1516361903776 40.10915845863114, -105.1515425217955 40.10915797339747, -105.151443190266 40.10915745838717, -105.1512721889252 40.10905345792743, -105.1511498943537 40.108892914989, -105.1510291895926 40.10873445721234, -105.1509501898016 40.10867945738578, -105.1507351896093 40.10865745754312, -105.1505561895843 40.10874045817922, -105.1503701892914 40.10874045812216, -105.1502991895659 40.10876745797281, -105.1502271897408 40.1088934573679, -105.150216358927 40.10890001008798, -105.1501990355049 40.1089104906731, -105.1501829687099 40.10892021131422, -105.1501628272604 40.1089323972873, -105.1501361731898 40.10894852276716, -105.1500271894042 40.10901445758356, -105.1499411886424 40.10911345803316, -1</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D18" t="n">
+        <v>23</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>Niwot HS</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>8989 Niwot Rd, Niwot, CO 80503</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>https://nhs.svvsd.org/</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>Niwot High School</t>
         </is>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>40.10369506217272</v>
       </c>
-      <c r="K18" t="n">
+      <c r="L18" t="n">
         <v>-105.1442414652976</v>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="M18" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="N18" t="inlineStr">
         <is>
           <t>https://nhs.svvsd.org/</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
+      <c r="O18" t="inlineStr">
         <is>
           <t>POINT (-105.1442414652976 40.10369506217272)</t>
         </is>
@@ -1621,56 +1677,59 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>POLYGON ((-105.2331971337308 39.985840282157, -105.2330351331852 39.98576428266011, -105.2327191338569 39.98561728215761, -105.2325671332445 39.98554728283532, -105.2324551331664 39.98549528298939, -105.2323551334779 39.9854482825155, -105.2319832192942 39.98527649380193, -105.2319351336893 39.9852542826066, -105.2311531345965 39.98489128325956, -105.2309501326586 39.98479628222291, -105.2302491328946 39.98447128245876, -105.2293111332321 39.98403928262311, -105.228734132372 39.98377128349869, -105.2276381336663 39.98326528294741, -105.2268921334482 39.98292028334055, -105.2259871327598 39.98250228293273, -105.2259021321316 39.9824632823856, -105.2233041316678 39.98126628283385, -105.221716133175 39.98053428301674, -105.2212240428698 39.98030670587036, -105.2212231314078 39.9803062839601, -105.221164278762 39.98041401321424, -105.2211641313148 39.98041428305446, -105.2208531327514 39.98027028363045, -105.2205529411696 39.98013265378606, -105.2205521325287 39.98013228345715, -105.2205507460672 39.98013349868391, -105.220540062076 39.98012857681351, -105.2205416976377 39.98012714153003, -105.2205429995072 39.98012599905148, -105.2198569987801 39.97980999936001, -105.217670999848 39.9788049982916, -105.2175789989619 39.97876299865521, -105.216200462426 39.97812263862686, -105.214956998355 39.97754499902697, -105.2135299983809 39.97688599922395, -105.2133739976538 39.97681299863746, -105.2131699989533 39.97671799874688, -105.2128311259303 39.97656205643337, -105.21283099974 39.97656199847693, -105.2101649988539 39.97532799912825, -105.2096699996618 39.9751049989255, -105.2093549990471 39.97496399882614, -105.2090049985782 39.97480699849135, -105.2087029993851 39.97467099834954, -105.2070459994989 39.9739889990676, -105.2048370000834 39.97313299845037, -105.2041369988925 39.97286199893107, -105.2034419994515 39.97259099900295, -105.2027290000227 39.97231199833313, -105.2014580003957 39.9718209988399, -105.1994079998071 39.97102099847267, -105.1989119987643 39.97083099883623, -105.1983979997043 39.9706339986794, -105.194591998727 39.96914999847615, -105.1918849995989 39.96810099902086, -105.1911419992523 39.96781299893013, -105.1901129992968 39.96740799898152, -105.1892829988523 39.96708899899218, -105.1886569997244 39.96684799823526, -105.1878959996133 39.96655099935374, -105.1847509988542 39.96532799810699, -105.1845030591753 39.96523090136483, -105.1845014339616 39.96523026465304, -105.1836529999933 39.96489799860698, -105.1823289247008 39.96438302700813, -105.1823765858315 39.96435856048586, -105.1829501799709 39.96406143557106, -105.1831431795536 39.96390943620628, -105.183359179438 39.96390543564833, -105.1846811801298 39.96359143505422, -105.1846831809932 39.96346543564761, -105.1850871806001 39.96337543512138, -105.1852101802556 39.96334743554963, -105.1859091799674 39.96319543556243, -105.1867561809799 39.96303243590308, -105.1875491802892 39.96290443543483, -105.1882881813402 39.96279743543808, -105.1892731804752 39.96267043497246, -105.1892811813567 39.96148043493095, -105.1891011772413 39.96160943265309, -105.1889071811083 39.96174843466853, -105.1882603172043 39.9619761564318, -105.1877131813326 39.96209643507789, -105.1876121808403 39.9621674358669, -105.1872551801046 39.96227843565087, -105.187073180655 39.96230143525784, -105.1867361810641 39.96239743503643, -105.1862821800566 39.96244943611252, -105.1852781797714 39.96245943558378, -105.185250937121 39.96248567933362, -105.1851691808371 39.96256443568562, -105.1846881802595 39.96256443553224, -105.1846878292357 39.9626284939408, -105.1845921801246 39.96264443594031, -105.1842001793857 39.96258943629537, -105.1841021800759 39.96259043491916, -105.183756179454 39.96352043583736, -105.183681180111 39.96353243572506, -105.1835581803465 39.96355343554686, -105.1834961799503 39.96356143605633, -105.1833721791185 39.96357743607462, -105.1832471796654 39.96358943518963, -105.1831221800468 39.96359843587509, -105.1829971802545 39.96360343569754, -105.1828711795887 39.96360543613775, -105.182745178819 39.96360443634497, -105.1826201798852 39.9636004354759, -105.1824941789573 39.96359343521812, -105.1823521786804 39.96357643573872, -105.1822441795616 39.96356843645984, -105.1821201788212 39.96355143678812, -105.1820251788167 39.96353643541125, -105.1818761791532 39.9635074363657, -105.1815991793696 39.96344043598965, -105.1815181794293 39.96341743539393, -105.1814281797796 39.9633894364229, -105.1813451795762 39.96336143602115, -105.1812645225385 39.96333271971175, -105.1811751798336 39.96329843665993, -105.1811201784924 39.96327643628931, -105.1810651795186 39.96325343616735, -105.1810111789803 39.96322943544858, -105.1809571796388 39.96320443587675, -105.1809041787385 39.96317943634221, -105.1808511790458 39.96315343615423, -105.180799178964 39.96312643537638, -105.1807481784856 39.96309843581128, -105.1806971792238 39.96307043532614, -105.1806471783964 39.96304143605229, -105.1805491783552 39.96298243605077, -105.1805011791406 39.96295143559319, -105.1804541783631 39.96292043608274, -105.1804071788043 39.96288743619242, -105.1803891795854 39.96287543542729, -105.1800231788606 39.96283243551652, -105.1791101784401 39.96248843618227, -105.1790331792207 39.9626014355022, -105.1780361786519 39.96221443573692, -105.1780248042583 39.96220476780362, -105.1780795667658 39.96212243842648, -105.1780617120378 39.96101742820876, -105.1780563504867 39.96064057285627, -105.1780562582363 39.96063407794388, -105.1760332411225 39.96066191903108, -105.1753197877496 39.96067107019252, -105.1752660781159 39.9606704126778, -105.1751530130947 39.96066902761821, -105.1751515536733 39.96066900909348, -105.1751673978478 39.95941085853762, -105.1752731802447 39.95941238698667, -105.1756586725545 39.95941795615956, -105.1767015637337 39.95943301604639, -105.1770275234974 39.95943772098945, -105.1770358705875 39.9584045834283, -105.1770363078439 39.95835052526509, -105.1770375221035 39.95820029775011, -105.1770375790401 39.9581932133214, -105.1753811772785 39.95817043580769, -105.1753791767883 39.95758643523679, -105.1786071510341 39.95766248213681, -105.178782063112 39.95766574209604, -105.1789897484092 39.957669611876, -105.1789848485213 39.95766031512748, -105.177648397834 39.95512435329022, -105.1776144429687 39.95506001242811, -105.1775799624868 39.95499299062175, -105.1775470406094 39.95492554265083, -105.1775156877714 39.95485768836055, -105.1774859155525 39.95478945300295, -105.1774577273785 39.95472085370143, -105.1774311360077 39.95465191391003, -105.1774061518873 39.95458265077165, -105.1773827784174 39.95451308681337, -105.1773610213213 39.95444324817128, -105.1773575396614 39.95443111644111, -105.1773408910587 39.95437314928622, -105.177322394536 39.95430281359553, -105.1773055304672 39.95423226451359, -105.177290313959 39.95416152369918, -105.1772767414146 39.95409060825552, -105.1772648208975 39.95401954432493, -105.1772552845585 39.95394743780206, -105.1772475047739 39.95387510202673, -105.1772414131593 39.9538026430856, -105.1772370166073 39.95373008711738, -105.1772416938306 39.95365372245707, -105.1772507335152 39.95357595507921, -105.1772613072263 39.95349823162613, -105.1772734159885 39.95342058182205, -105.177290609483 39.95332415578926, -105.1774078670555 39.95259250878293, -105.1774296504487 39.95249004043743, -105.1774426914856 39.95247925641739, -105.1776474059061 39.95230996035514, -105.1776425915952 39.95225318368962, -105.1776494915453 39.95224847092626, -105.1776503630244 39.95222278293825, -105.1776527450811 39.9521525489294, -105.1776542787933 39.95210731667019, -105.1777091771583 39.95048843468322, -105.1765421764602 39.95049343511674, -105.1765441762881 39.95029543509211, -105.1737901766914 39.9502784352506, -105.1732691751886 39.95049443510379, -105.171721175293 39.95049343486586, -105.171721175489 39.95026543539605, -105.1713521750109 39.95026343503369, -105.1710701754516 39.9496574351276, -105.1709821753827 39.94931543455208, -105.1708731754645 39.94899843388744, -105.1706751750825 39.94883443513947, -105.1705001743236 39.94877043461553, -105.1702541750417 39.94875143479771, -105.1703601751532 39.94872843443577, -105.1699691748952 39.94766043485847, -105.1696509264492 39.94772961758919, -105.1696508514793 39.94772963358609, -105.1685594742733 39.94796687370324, -105.1663871736281 39.94844043457117, -105.1657381741117 39.9485814352014, -105.1657421736359 39.94800016035729, -105.1657468007817 39.94732775484253, -105.165775173689 39.94320443381061, -105.1664695916308 39.9432063625764, -105.1683021747413 39.94321143381614, -105.1693041740566 39.94127343310699, -105.1693161728545 39.9392404329576, -105.1676961733447 39.939242433397, -105.1669986961005 39.93946070845881, -105.1664371723441 39.93963643311929, -105.1657621735393 39.94010243415755, -105.1657314686955 39.9377869994332, -105.1657411728798 39.93778699967167, -105.1687795281632 39.93778699271773, -105.1705111261316 39.93778695271561, -105.1705041256043 39.93953147032551, -105.1705041235479 39.93953189633235, -105.170503856046 39.93959870391294, -105.1706001480141 39.93959920896221, -105.1706007611061 39.93959921251663, -105.1752061254244 39.93962327452727, -105.1752117639349 39.94144391979933, -105.1752117838299 39.94145375507232, -105.1752147521367 39.9424101139557, -105.1752173188591 39.9432381770126, -105.1761254808051 39.94324195231821, -105.1789957423668 39.94325383880542, -105.1795291232214 39.94325604071027, -105.1795857546609 39.94325627388761, -105.179680680969 39.9432566666597, -105.1799269123049 39.9432576806739, -105.1799269771434 39.9431864638202, -105.1799270111662 39.94314876676573, -105.1799270269173 39.94313068604808, -105.1799271965382 39.94293307347776, -105.1799284928579 39.94143895759951, -105.1799300690526 39.93962613628113, -105.1819970768541 39.93962050076085, -105.1825172429311 39.93962242816511, -105.1825172620205 39.9396190786604, -105.1846548192044 39.93961336109664, -105.1894029282757 39.93957558427936, -105.1893867343792 39.93594894951613, -105.1914911317678 39.93594133715856, -105.1923511717818 39.93593821445231, -105.1933688742004 39.93593450898793, -105.1933702477947 39.93593450363773, -105.1941599816869 39.93593162428242, -105.1945942211984 39.93592965200351, -105.1951635483 39.93592706564407, -105.1952762078992 39.93592655313077, -105.1972458768153 39.93591757849988, -105.1989481266646 39.93590979541442, -105.2002993179784 39.93590013495036, -105.2004456872241 39.93589909443324, -105.2005289440003 39.93589930820974, -105.2005695998748 39.93589960573908, -105.2005767561356 39.93597682174268, -105.2007855838866 39.93595828117817, -105.2016135821577 39.93571128289184, -105.2017205818092 39.93570628394144, -105.2019415807419 39.93585928284536, -105.2020485805162 39.93587628311925, -105.2022345798063 39.93581028363036, -105.2022817052154 39.93578010452304, -105.2022817218954 39.9357827182824, -105.2022819718508 39.93582278570346, -105.2022823369061 39.93589360196512, -105.203430843309 39.93588732563549, -105.2047070368473 39.93587606396571, -105.2046882733971 39.93394651148376, -105.2046864363509 39.93375887309851, -105.2046865622196 39.93375357663749, -105.2046865938261 39.93375222032397, -105.2046872617554 39.93372412053174, -105.2047298796838 39.93225646940934, -105.2047394578092 39.92861052434253, -105.20815190367 39.92859781286307, -105.2127497371948 39.92855694032826, -105.21745002281 39.92854504863909, -105.2182946341396 39.92854109387441, -105.2189537516798 39.92853800621756, -105.2189574099148 39.92853798902473, -105.2192246119665 39.92853673580493, -105.2193899800826 39.92853595984494, -105.2194595415266 39.92853648685829, -105.2221224251364 39.92852872241523, -105.2225585730252 39.92852772662706, -105.2269942832364 39.92851750262659, -105.231838615029 39.92851118067422, -105.2320906879295 39.92850933729788, -105.232244880529 39.92825937905761, -105.2322470002203 39.92825999913596, -105.2323239999907 39.92827499846799, -105.2325869997246 39.92832599949908, -105.2328459990954 39.92836499926473, -105.233193999894 39.92839699846957, -105.2333020002307 39.92840299930947, -105.2335169999823 39.92840799934192, -105.2338429992942 39.9284019990797, -105.2339589999796 39.92840599941181, -105.2342460000307 39.92840799944923, -105.2345579999572 39.92840399945201, -105.2346220868783 39.92839808298703, -105.235008498219 39.92954535037926, -105.2357094840183 39.93165934189567, -105.2360154780325 39.93263533803334, -105.236281472281 39.93344833402639, -105.2362914736262 39.93347633500713, -105.2363204718143 39.93355633311082, -105.2364244699075 39.93388233241797, -105.2365124675654 39.934211332045, -105.2365834657741 39.93454233001258, -105.2366494631262 39.9349403282457, -105.2367214605929 39.93554832524025, -105.2367244595431 39.93564532498768, -105.2367184583478 39.93593632327084, -105.2366914560335 39.93622632334893, -105.2365934533178 39.93682131971666, -105.2362604460931 39.93836731278099, -105.2361144443316 39.93896730909405, -105.2359764419444 39.93959030654941, -105.2358854385444 39.94007630426844, -105.2357694354685 39.94059430261459, -105.2356634342481 39.94112030001217, -105.2356304332279 39.94131729835097, -105.2356114323706 39.94151029746016, -105.2356014320325 39.94161229663906, -105.2355924294382 39.94190829551381, -105.2356074283079 39.94235429384504, -105.2356354249494 39.94272929243355, -105.235684424172 39.94310129046235, -105.2357704201069 39.94349128922146, -105.2358764195226 39.94388028719909, -105.2360184168766 39.9442792856082, -105.2362374114519 39.94482928352224, -105.2362994105811 39.94501728301593, -105.2363644094841 39.94521428241291, -105.2365134060399 39.94563127962134, -105.2365574053572 39.94586827954905, -105.2365854034608 39.94610727835873, -105.2365894029548 39.94626527741081, -105.2365814017142 39.9465022772988, -105.2365614007355 39.94666427533257, -105.2365313996723 39.94682527598022, -105.2364683993308 39.94706327408439, -105.2364103991369 39.94722027296941, -105.2363433979527 39.94737627311073, -105.2362663973395 39.94752527202102, -105.2361803968036 39.94767327125486, -105.2360353964538 39.94788527024479, -105.2358123949861 39.94815426851239, -105.2353373949938 39.94864726599771, -105.2349013944894 39.94908826348983, -105.2345443929722 39.94947226127717, -105.2341583927248 39.94993525893874, -105.2339843922855 39.95015925813851, -105.2338933927668 39.95028225714832, -105.2337133911016 39.95055025544299, -105.2332173879164 39.95142925195454, -105.2329263859335 39.95198824857948, -105.2328813846094 39.95204324832668, -105.2327903849929 39.95215824771139, -105.2327193862173 39.95224424719736, -105.232524383524 39.95259824508297, -105.2323133847181 39.95296324303607, -105.2320883826542 39.95329924107202, -105.2318913807338 39.95362223977587, -105.2318323814242 39.95370923934254, -105.2316703806363 39.95397423748284, -105.2314753793715 39.95433623591635, -105.2314223789011 39.95446223513391, -105.2313453770757 39.95467723363021, -105.2313003767481 39.9548462335438, -105.231253376375 39.95506123258171, -105.2312233748296 39.95522923168615, -105.2311983738348 39.95548223033251, -105.2311963731234 39.95565322998704, -105.2312023733035 39.9557382300675, -105.2312363718279 39.95601922818315, -105.2312903702832 39.95625422768943, -105.2313363694249 39.95640222747937, -105.2313723684942 39.95650822697466, -105.2313993672773 39.95657122608427, -105.2314743674655 39.95674822524581, -105.2315163654634 39.9568392256063, -105.2316053645577 39.95700022378365, -105.2317183627099 39.95718222346612, -105.2318093614744 39.95731022333126, -105.2319253601265 39.9574562223896, -105.2321203576787 39.9576752222892, -105.2321207867455 39.95767563668858, -105.2323323583044 39.95788022189713, -105.2323339852215 39.95788198466088, -105.2324863593553 39.95804721921932, -105.2334443494492 39.95875021940091, -105.233571348484 39.95868821912516, -105.233714348323 39.95861822001959, -105.2338239520144 39.95857110046063, -105.2338049737405 39.95855745128576, -105.2337782867351 39.95853826416749, -105.2336986413383 39.95848099104538, -105.2336468045691 39.95844371280378, -105.2336171748539 39.95842344796374, -105.2341725434769 39.9580392688392, -105.2347950472625 39.95760869288404, -105.2342243926122 39.95691524152589, -105.2341524978376 39.95682786948809, -105.2349909423702 39.95628870009567, -105.2376695730872 39.95553943080883, -105.237869403808 39.95544896598811, -105.2380925487423 39.95534793956568, -105.2381381075876 39.95533712804144, -105.2384707501498 39.9552581735205, -105.2387606413787 39.95522995514532, -105.2391404503259 39.95508480189946, -105.2392353862244 39.95517125116451, -105.2392371589414 39.95517286555238, -105.239258389572 39.9551921984806, -105.23927647946 39.95520867371651, -105.2394538794511 39.95516317297034, -105.2394675768633 39.95518923114921, -105.2396736377063 39.955581234407, -105.2406711572687 39.95439742475489, -105.240024053321 39.95392266004539, -105.2398894907311 39.95382393336795, -105.2398824476685 39.95381877110944, -105.2398473876931 39.95379304572359, -105.2398453407215 39.95379154330794, -105.2398296126404 39.95378000279207, -105.2399006156666 39.95375236339038, -105.2399205402457 39.95374460686801, -105.2399483505752 39.95372724911473, -105.2400416944829 39.9536974417265, -105.2400878385559 39.95367947772901, -105.240487048047 39.95352406659201, -105.2404916539113 39.95352201806195, -105.2408652368515 39.95346000915787, -105.240933089732 39.95344874590243, -105.2409499829143 39.95344750044689, -105.2409629638922 39.95344654341077, -105.2411807314999 39.95343048229564, -105.2412136382214 39.95342633392487, -105.2412244358653 39.95342464512465, -105.2412358248517 39.95342286488371, -105.2412578671857 39.95341887043079, -105.2412797394526 39.95341435681286, -105.2413014182228 39.95340933028208, -105.2413228882888 39.95340378900303, -105.2413441273671 39.95339774553509, -105.2413651120586 39.95339119802451, -105.2413858282717 39.95338415904898, -105.2414062525904 39.95337663125811, -105.2414263685928 39.95336862452243, -105.2414461540193 39.95336014509677, -105.2414655936254 39.95335120105296, -105.2414846663152 39.95334180044981, -105.2415033556772 39.9533319504559, -105.2415216464464 39.95332166454715, -105.2415395163498 39.95331095258089, -105.2415569548413 39.95329981813632, -105.2415739384536 39.9532882773729, -105.2415904554602 39.9532763365691, -105.2416064894054 39.95326401460206, -105.2416220297466 39.95325131415024, -105.24163705301 39.95323825317441, -105.241651550963 39.95322484246419, -105.2416655106915 39.95321109279873, -105.2416789145904 39.95319701764863, -105.2416924969039 39.95318372827051, -105.2417926015235 39.95306197295623, -105.2420940138068 39.95269873993102, -105.2423550234888 39.95238460880659, -105.242400847213 39.95232958199797, -105.2424229928676 39.95230461213298, -105.2424350975266 39.95228989182103, -105.2424467138614 39.95227494525179, -105.2424578289587 39.95225978320441, -105.2424684416042 39.95224441738487, -105.2424785412352 39.95222885587566, -105.2424881208034 39.95221310586636, -105.2424971779208 39.95219717996105, -105.2425056985141 39.95218108623425, -105.2425136860365 39.95216484000501, -105.2425211357905 39.95214844576619, -105.242528036016 39.9521319188029, -105.2425343843559 39.95211526361316, -105.242540178402 39.95209849820491, -105.242545419308 39.95208162708401, -105.2425500906432 39.9520646628231, -105.2425542040459 39.95204762256071, -105.2425577466438 39.95203050626817, -105.2425604849985 39.95201470223844, -105.2425631226928 39.95199611044753, -105.2425649537362 39.95197884892725, -105.2425662114527 39.95196156000681, -105.2425668899367 39.9519442580837, -105.2425669973535 39.95192695038124, -105.242566527808 39.95190964859498, -105.2425654812633 39.95189236263193, -105.2425638623396 39.95187510871434, -105.2425616698536 39.95185789044219, -105.2425589060715 39.95184072763487, -105.2425555709869 39.95182362209368, -105.2425516692268 39.95180658823951, -105.2425471983968 39.9517896404774, -105.2425469995326 39.95178899876466, -105.2425421690058 39.95177278513545, -105.2425365751554 39.9517560348095, -105.242530432015 39.95173940124199, -105.2425237313593 39.95172289342101, -105.2425164848536 39.95170652127981, -105.2425086947983 39.95169029563127, -105.2425003742863 39.95167477851509, -105.2424059484562 39.95151136733212, -105.2421494028326 39.95106741309232, -105.2421263742837 39.95102756327953, -105.2421244396496 39.95102421300519, -105.2421117923814 39.95100232933174, -105.2421532349839 39.9508776521355, -105.2422356511012 39.95062967915599, -105.2423203763545 39.95053644972544, -105.2423583595049 39.95045226550373, -105.2424326983841 39.95038139681725, -105.2424193456011 39.95036537308143, -105.2424164774736 39.95036192975837, -105.2424288673095 39.95035465582276, -105.2424902617059 39.95031861002217, -105.2428650690549 39.95009855353451, -105.2428848292195 39.95012039805992, -105.2428864176305 39.95012215428513, -105.2429218079034 39.95016127407835, -105.2432539182085 39.94997577837081, -105.2436207472383 39.94976943938573, -105.2436116776633 39.94976111333539, -105.2436098898687 39.94975947286139, -105.2435487854324 39.94970338529077, -105.2435552591411 39.94969465971476, -105.2437521608587 39.94942704577121, -105.2437723123789 39.94941200006306, -105.243901119003 39.94931583227635, -105.2439133601279 39.94929227305281, -105.2439907943965 39.94920904960991, -105.2438902370072 39.94913250436197, -105.243843496383 39.9490969244327, -105.2443336805456 39.94899766010215, -105.2450769997713 39.94893541989843, -105.2450769622432 39.94898556845416, -105.2450769407175 39.94901326183933, -105.2450769015449 39.94906353738384, -105.2450768554042 39.94912445058453, -105.2450768545068 39.94912625730254, -105.2450768068025 39.94918915554966, -105.2459288147174 39.9491932396644, -105.2459273019017 39.94880149693439, -105.2459270969151 39.94874811268062, -105.2459271138438 39.9487184180232, -105.2459271149365 39.94871560977393, -105.2459271527736 39.94865357973831, -105.2459280088195 39.94859022934073, -105.2464013539658 39.94842233398014, -105.2467081124108 39.948313522097, -105.2470891135391 39.94809851549275, -105.2472302242334 39.94801888546431, -105.2476083139154 39.94780552076305, -105.2476846981875 39.94776122618649, -105.2478094284176 39.94735633375443, -105.2478469404037 39.94723456492972, -105.2478433560362 39.94713228736064, -105.2478890047047 39.94705597092624, -105.2479304177987 39.9468527631968, -105.2479367866069 39.94684940326579, -105.2480295986053 39.94680042405117, -105.2485796528338 39.94651128238812, -105.2486454636441 39.94641330739307, -105.2487568057952 39.94624753735123, -105.248831466112 39.94598356233421, -105.249021310299 39.94563334264168, -105.249080831418 39.94552353705695, -105.2495449506102 39.94530671557963, -105.2503360267622 39.94525208564679, -105.2506537737573 39.9452363809138, -105.2509883201429 39.94522203648467, -105.2510883945363 39.94521343349978, -105.2511768961192 39.94520772446678, -105.2511800028379 39.94524977930156, -105.2511838734138 39.94530217534098, -105.2515099428432 39.94523367793365, -105.2518436376838 39.94515417827923, -105.2518477719972 39.94515670272256, -105.2518512447883 39.94515611576839, -105.2518547164191 39.94515552610967, -105.2518581857455 39.94515492653865, -105.251861651591 39.94515431885415, -105.2518651127853 39.94515370305352, -105.2518685751693 39.94515308185147, -105.2518720329022 39.94515245253334, -105.2518754918346 39.94515181511175, -105.2518789425989 39.94515117136789, -105.2518823933992 39.94515051771672, -105.2518858465593 39.94514985866664, -105.251889289211 39.9451491932892, -105.2518927354026 39.94514851981333, -105.251896174606 39.94514783731576, -105.2518996161757 39.9451471476179, -105.2519030495741 39.94514645249836, -105.2519064841721 39.94514574927545, -105.2519099141221 39.9451450370358, -105.2519133441015 39.9451443166902, -105.2519159145514 39.94514377282392, -105.2519167670797 39.94514359092548, -105.2519201889171 39.94514285705226, -105.2519236084339 39.94514211777003, -105.2519256753871 39.94514166558714, -105.2519270256396 39.94514137037679, -105.2519304405346 39.94514061487251, -105.2519338496082 39.9451398512497, -105.2519372587047 39.94513908132221, -105.2519406643201 39.94513830328125, -105.2519440664447 39.9451375198287, -105.2519474674253 39.94513672916829, -105.2519508625911 39.94513592858804, -105.2519542542693 39.94513512169561, -105.2519576448035 39.94513430759532, -105.2519610330267 39.94513348538403, -105.2519644165857 39.94513265865931, -105.2519677966735 39.94513182111915, -105.2519711744374 39.94513097907053, -105.2519745475565 39.94513012710465, -105.2519779218621 39.94512927063791, -105.2519812880159 39.94512840334556, -105.2519846541827 39.94512753245058, -105.2519880133548 39.94512665433513, -105.2519913737362 39.94512576541436, -105.2519947294501 39.94512487288078, -105.2519980781757 39.94512397132544, -105.2520014269308 39.94512306166417, -105.2520047721983 39.94512214569071, -105.2520081139781 39.94512122340501, -105.2520114487632 39.94512029389892, -105.2520147835744 39.94511935718746, -105.2520181149079 39.94511841146189, -105.2520214427504 39.94511746032477, -105.2520247647684 39.94511650196974, -105.2520280821318 39.94511553639932, -105.2520313995214 39.94511456362362, -105.2520347134299 39.94511358273439, -105.2520380226774 39.94511259643108, -105.2520413261068 39.9451116011086, -105.2520446283922 39.94511059857827, -105.2520479236795 39.94510958972817, -105.2520512201533 39.94510857637726, -105.2520545073116 39.94510755039697, -105.2520577933096 39.94510652171215, -105.2520610793434 39.94510548312004, -105.2520643572058 39.94510443910632, -105.2520676304072 39.94510338967851, -105.2520708989607 39.94510233123408, -105.2520741651999 39.94510126557928, -105.2520774291217 39.9451001936148, -105.252080686052 39.9450991135292, -105.2520839394946 39.94509802713147, -105.2520871917932 39.94509693352585, -105.2520904382705 39.94509583180172, -105.2520936765796 39.94509472375534, -105.2520969160751 39.94509361120816, -105.2521001520927 39.94509248964676, -105.2521033799521 39.94509135906114, -105.2521066054841 39.9450902248678, -105.2521098263649 39.94508908255848, -105.2521130414211 39.94508793303122, -105.2521162541663 39.94508677539298, -105.2521194610771 39.94508561323882, -105.2521226656769 39.94508444297368, -105.2521258656191 39.94508326639381, -105.2521290573995 39.9450820816904, -105.2521322515365 39.94508089248868, -105.2521354363483 39.9450796933595, -105.2521386153256 39.94507848971444, -105.2521417943322 39.94507727796344, -105.2521449663408 39.94507605989268, -105.2521481336949 39.94507483460657, -105.2521512975614 39.94507360300824, -105.2521544556032 39.945072364192, -105.2521576089873 39.9450711190611, -105.2521607588903 39.94506986581668, -105.2521639029653 39.94506860625501, -105.2521670423859 39.945067339478, -105.2521701783156 39.9450660672895, -105.2521733084173 39.9450647887837, -105.2521764326977 39.94506350215937, -105.2521795546639 39.94506220832474, -105.252182669632 39.94506090817035, -105.2521857811092 39.94505960260445, -105.2521888891053 39.94505828892499, -105.2521919901034 39.94505696892586, -105.2521950864469 39.94505564171133, -105.2521981757891 39.94505430907772, -105.2522012628204 39.94505296833312, -105.2522043451939 39.94505162127381, -105.2522074217362 39.94505026879794, -105.252210493624 39.94504890910668, -105.2522135585137 39.94504754309576, -105.2522166199256 39.94504616807063, -105.2522196755064 39.94504478762895, -105.2522227252527 39.94504340267135, -105.2522257738581 39.94504200960528, -105.2522288131219 39.94504061111508, -105.2522318465677 39.94503920360577, -105.2522348753491 39.945037791583, -105.2522379029864 39.94503637235244, -105.2522409212886 39.94503494589646, -105.2522439360999 39.94503351402893, -105.2522469450801 39.94503207674485, -105.2522499470686 39.94503063133973, -105.2522529443995 39.94502917961992, -105.2522559382492 39.94502771978662, -105.2522589250976 39.94502625453423, -105.2522619096219 39.9450247847735, -105.2522648848177 39.94502330598599, -105.2522678541855 39.94502182088132, -105.252270820056 39.94502033216641, -105.2522737789414 39.94501883352913, -105.2522767331494 39.94501733398111, -105.2522796815557 39.94501582091064, -105.2522826229475 39.94501430602371, -105.2522855596848 39.94501278392142, -105.2522884929345 39.94501125550695, -105.2522914203628 39.94500971897397, -105.2522943396065 39.94500818062199, -105.2522972530451 39.94500662964825, -105.2523001606396 39.94500507686057, -105.2523030659263 39.94500351506126, -105.2523059606881 39.94500195143796, -105.2523088519786 39.94500037699914, -105.2523117397717 39.94499879895016, -105.2523146170629 39.94499721277261, -105.252317489693 39.94499562118102, -105.2523203600023 39.94499402418045, -105.2523232186395 39.9449924190487, -105.2523260772863 39.94499081121498, -105.2523289266047 39.94498919435458, -105.2523317712685 39.94498757027878, -105.2523346100946 39.94498594258777, -105.2523374395856 39.94498430767137, -105.2523402632486 39.94498266643776, -105.2523430834208 39.9449810197926, -105.2523458965916 39.94497936772839, -105.2523487051111 39.94497770754813, -105.252351504289 39.94497604194386, -105.2523542988092 39.94497437002488, -105.2523570886649 39.94497269359248, -105.2523598726928 39.94497101084288, -105.2523626462154 39.9449693208654, -105.2523654162504 39.94496762457575, -105.252368179284 39.94496592286701, -105.2523709399968 39.9449642157493, -105.2523736890245 39.94496250410312, -105.2523764345645 39.94496078614474, -105.2523791719461 39.94495905916219, -105.2523819034965 39.94495732676307, -105.2523846303825 39.9449555898506, -105.2523873479302 39.94495384661338, -105.2523900608136 39.94495209886276, -105.2523927666989 39.94495034479245, -105.2523954667595 39.94494858350431, -105.2523981598155 39.94494681769777, -105.2524008458767 39.9449450446708, -105.2524035249366 39.94494326622485, -105.2524061993255 39.94494148506679, -105.2524088667262 39.94493969488705, -105.252411525962 39.94493789748446, -105.25241417936 39.9449360964666, -105.2524168245865 39.9449342900272, -105.2524194639786 39.94493247907191, -105.2524220987194 39.94493066000064, -105.2524247229484 39.94492883550277, -105.2524273448566 39.94492700559591, -105.2524299550862 39.94492516935929, -105.2524325618152 39.94492333041308, -105.252435161559 39.94492148154463, -105.252437754295 39.94491962905835, -105.2524403388627 39.94491777024991, -105.2524429175862 39.94491590962748, -105.2524454893214 39.94491403998344, -105.2524480563956 39.94491216492536, -105.2524506141249 39.9449102853439, -105.2524531636891 39.94490839853952, -105.2524557062489 39.94490650721674, -105.2524582453176 39.94490461048248, -105.2524607738779 39.94490270742096, -105.2524632989439 39.94490079984861, -105.2524658123281 39.94489888684717, -105.2524683198811 39.94489696842913, -105.2524708239463 39.94489504369899, -105.2524733163298 39.94489311353974, -105.2524758063826 39.94489118067343, -105.2524782847633 39.94488923967614, -105.2524807596564 39.94488729236664, -105.2524832240246 39.94488534323313, -105.2524856814013 39.94488338597866, -105.252488135287 39.94488142331268, -105.2524905786512 39.94487945792206, -105.2524930138569 39.94487748350729, -105.2524954432185 39.94487550727858, -105.2524978655852 39.94487352382955, -105.2525002797738 39.94487153676027, -105.2525026881378 39.94486954247318, -105.2525050883238 39.9448675445658, -105.252507481515 39.94486553943809, -105.2525098665282 39.94486353069011, -105.2525122433633 39.94486151832191, -105.2525146155505 39.9448594969371, -105.2525169772161 39.94485747282765, -105.2525193342173 39.94485544420483, -105.2525216818835 39.94485340835668, -105.2525240213717 39.94485136888823, -105.2525263538618 39.94484932310012, -105.2525286805207 39.94484727189551, -105.252530998995 39.94484521887192, -105.2525333069609 39.94484315952113, -105.2525356102689 39.94484109385569, -105.2525379651215 39.94483901208904, -105.252540327011 39.94483692583418, -105.2525426772219 39.94483483324961, -105.2525450250989 39.94483273885861, -105.2525473613071 39.94483063543593, -105.2525496916743 39.94482852929868, -105.25255201387 39.94482641773995, -105.2525543255507 39.94482430165525, -105.2525566337372 39.94482218105967, -105.2525589314087 39.94482005593821, -105.252561220912 39.94481792449454, -105.2525635045808 39.944815788535, -105.2525657812514 39.94481364625581, -105.2525680497376 39.94481150215764, -105.2525703088854 39.94480935173479, -105.2525725598618 39.94480719589041, -105.2525748026569 39.94480503732641, -105.2525770407876 39.94480287424906, -105.2525792695832 39.94480070394635, -105.2525814902041 39.94479852912275, -105.2525837014737 39.94479635157708, -105.2525859057418 39.94479416861237, -105.252588104182 39.94479197933045, -105.2525902920974 39.94478978822466, -105.252</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
+          <t>MULTIPOLYGON (((-105.1691864470017 39.92863672319584, -105.169197172132 39.92863411235809, -105.1691971726547 39.92869943197082, -105.1691864470017 39.92863672319584)), ((-105.1784019212843 39.92870168376908, -105.1818511117197 39.92869648384348, -105.1838441764116 39.92869343178848, -105.1841991763519 39.92873643054561, -105.1843711756133 39.92868243090511, -105.1846711757492 39.92865043161049, -105.1848971762652 39.92868243096175, -105.1851551757211 39.92870443083596, -105.1853591757001 39.92871443082796, -105.185584175611 39.92863943112477, -105.1857881765031 39.92869343037078, -105.1860781767717 39.92871443107489, -105.1862427122102 39.92871305375947, -105.1874398749427 39.92870302575108, -105.188280750955 39.92869597460466, -105.1891882146993 39.92868835848437, -105.1900135071195 39.92868142556227, -105.1912021775201 39.92867143016532, -105.1921605878346 39.92866908889513, -105.1952731788288 39.9286614295662, -105.1953454862046 39.92714404290943, -105.1954277266185 39.92535293082255, -105.1954701680578 39.92442856826072, -105.1954828953945 39.92415135493398, -105.1955126848871 39.9235025188834, -105.1955539541151 39.92260363548544, -105.1955832718303 39.92176253388807, -105.1956074363542 39.92104863795893, -105.1956271775804 39.92046542890528, -105.1956491770346 39.92026642822356, -105.1957021779222 39.92016442965017, -105.1958741782275 39.91996042930643, -105.1960031773458 39.91985842861604, -105.1960461779453 39.91979442941913, -105.1963542841982 39.91947358440687, -105.1969171547176 39.91888743134161, -105.1971382584971 39.91865717884937, -105.1975931774295 39.91818342841723, -105.1977971773725 39.91800542846681, -105.1980761776685 39.9178604287125, -105.1988809443973 39.91750583145522, -105.199981771958 39.9170207684681, -105.2005472795797 39.91677157902036, -105.2013773094024 39.91640582131284, -105.2019980528428 39.91613227988852, -105.2026927027816 39.91582616438962, -105.2029610455153 39.91570919533338, -105.2032861789647 39.91558342752357, -105.2034951787843 39.91545442818257, -105.2036994329652 39.91536577400033, -105.2039238798093 39.91526835479848, -105.2044351788381 39.9150464284585, -105.2046181793619 39.91493942746109, -105.2047771484222 39.9148745542603, -105.2051264319463 39.91473201341331, -105.2055840142236 39.91454527467528, -105.206223179592 39.91428442723124, -105.2062611795562 39.91424142750945, -105.2062749820281 39.91414793981343, -105.2080811675174 39.91413651982791, -105.2081010480463 39.91413639369402, -105.2082326020008 39.91413556073108, -105.2082437405714 39.91413548987958, -105.2127750952919 39.914106703786, -105.2128870458286 39.91410599043611, -105.213645040396 39.91410184790944, -105.2175004417789 39.91408067426644, -105.2189361314345 39.91407275709121, -105.2212525262855 39.91405994110492, -105.2221488638938 39.91405498129632, -105.2316342538218 39.91406393968015, -105.2328366111099 39.91406370115187, -105.2386024786223 39.91406237558283, -105.238920889073 39.91406229633754, -105.2392698990356 39.91406220443915, -105.239915923657 39.91406203514502, -105.2402281491856 39.91406195092515, -105.2405279089477 39.91406186839333, -105.2412789148089 39.91406166045791, -105.2459316121797 39.91403871789947, -105.2501535052445 39.91401773192297, -105.2598916796428 39.91397305810732, -105.2600457617387 39.91397082590954, -105.2654909078388 39.91389125974047, -105.2666177593649 39.91387476217126, -105.2692129079631 39.91383672570182, -105.2759740475008 39.91371767073185, -105.2763431408977 39.91371116039856, -105.2811042377732 39.91371047397082, -105.2816813633473 39.9137103780077, -105.2819189247833 39.91371033909354, -105.2826022004646 39.91371022423816, -105.2838975683199 39.91370999020454, -105.2841657430803 39.91370993925377, -105.2845492353484 39.91370986571884, -105.285848204384 39.91370961828155, -105.2953533084801 39.91370800138991, -105.3000747525567 39.91381446987435, -105.3040421127392 39.91390380243763, -105.3047891203881 39.91392060756144, -105.3067655027752 39.91391296285316, -105.307489992947 39.91391015846362, -105.3138618072536 39.91388526812848, -105.3138945250918 39.91388513907664, -105.3140600078973 39.91388448682844, -105.314962656992 39.91387604616386, -105.3149765887619 39.91388835983841, -105.3228091235898 39.92081034046993, -105.322810999039 39.92081199876494, -105.3230754639435 39.92090816782166, -105.3230946808704 39.92091515582619, -105.3232179993169 39.92095999891312, -105.3236539993554 39.92104899939051, -105.3238185156393 39.92104925748924, -105.3238336179889 39.92104928059182, -105.3238539754728 39.92139180765506, -105.3240379379819 39.92434240818668, -105.3242555787687 39.92783278270667, -105.3240442233703 39.93038144497817, -105.3239541807884 39.93152857193745, -105.3205148429798 39.9317151039824, -105.3191391063055 39.9317901419817, -105.3189277387964 39.93544482213235, -105.3152947463766 39.93560825239187, -105.3150107817862 39.93562102376601, -105.3151269546172 39.93568601616223, -105.3151730015705 39.93582906938609, -105.3153428715063 39.93597232205011, -105.3153426458871 39.93605572614626, -105.3152959536364 39.93615097053843, -105.3152646112064 39.93629390050486, -105.3151716143362 39.93634141140234, -105.3151556836821 39.93650819475129, -105.3149541789319 39.93661510617261, -105.3147370974993 39.93675773567037, -105.3146129496925 39.93687668567372, -105.3144116361982 39.93691210769416, -105.3142952267474 39.93694088522145, -105.3140710200188 39.93694730280319, -105.3138543255822 39.93694695284194, -105.313668360496 39.93703005663828, -105.3135443067977 39.93711326126337, -105.3135281127685 39.93737536320363, -105.3135586131968 39.93754222327778, -105.3135582226762 39.93768520106113, -105.3135886919486 39.93786397586513, -105.3135728884073 39.93798309911708, -105.313541572907 39.93811411295194, -105.3135409870585 39.938328582769, -105.3135248903767 39.93855494046591, -105.3136326539993 39.93876958471586, -105.3139259350723 39.9390679331113, -105.3139564708813 39.93922287561901, -105.3140018023195 39.93962805802159, -105.3140940256521 39.93986650720636, -105.3141398137156 39.9401048796018, -105.3141701546706 39.94033131316758, -105.3142470304991 39.9405220764947, -105.3142307086453 39.9408318392145, -105.3143695989769 39.94098695806902, -105.3146322573936 39.94116610555177, -105.3148020101678 39.94135701700087, -105.3149875012233 39.94145263516127, -105.315393589911 39.94149240574951, -105.3156220829817 39.94147748302713, -105.3159009337462 39.94139452276405, -105.316195455252 39.94124009899878, -105.3162423730982 39.94106144931301, -105.3163205701327 39.94076369979045, -105.3163519765155 39.9405969410111, -105.316476321442 39.94040649983918, -105.3166467816132 39.94033528163523, -105.3169565199088 39.94027619845558, -105.3172351396482 39.94027664082628, -105.3175447179208 39.94027713156014, -105.3179781597508 39.94026590245163, -105.3183802624779 39.94039760247852, -105.3186740765611 39.9405053002228, -105.3189680191451 39.94056533736213, -105.3191692463489 39.94056565340757, -105.3198388293764 39.9404390245125, -105.3204701065221 39.94032938867544, -105.3207332478084 39.94032979846212, -105.3209655879741 39.94027058403997, -105.3210277850324 39.94016344578863, -105.3211365426721 39.94000872155141, -105.3211522710472 39.93991342586091, -105.3212456742569 39.93971101672305, -105.3213232553279 39.93963964654615, -105.3218807395759 39.93954518976606, -105.3220975354618 39.93950978040615, -105.3222368443683 39.93950999545962, -105.3225929785905 39.9394628853095, -105.3227789715475 39.93936785058116, -105.3229032642183 39.93918931809423, -105.3227684117605 39.93860002799841, -105.3231420733671 39.93807305242971, -105.3238359511774 39.93765371783137, -105.3241615174665 39.9374516611181, -105.3242700796447 39.93736842144941, -105.3243941513812 39.93727329143306, -105.3246419865635 39.93720217843251, -105.3248586806939 39.93720250809899, -105.3251372891076 39.93720293135949, -105.3253848794217 39.9372271383133, -105.3256479783452 39.93723945161755, -105.3258956297566 39.93723982618449, -105.3260812174063 39.93729968138211, -105.326332444717 39.93736300821741, -105.3264369133073 39.93741936755629, -105.3266223796962 39.9375268817555, -105.3266840208323 39.93763420851904, -105.3268076059926 39.93772971450777, -105.3268536776333 39.93787276303662, -105.3269152288096 39.93801583390401, -105.3269504474838 39.93818943437444, -105.3266788045178 39.93861631287486, -105.326510155908 39.93905182646767, -105.3264008665194 39.93942102655195, -105.3267233057162 39.93972059487754, -105.326848479111 39.93992212849384, -105.3270338333477 39.94007730187811, -105.3272230655047 39.94017627980257, -105.3273737955304 39.94030419546518, -105.3275436118999 39.94048317340886, -105.3277290582858 39.94060260054161, -105.3280464391735 39.94068518217745, -105.328363397086 39.94072269795484, -105.3289675567365 39.94053295723312, -105.3292308777148 39.9404618573578, -105.3294013842727 39.94036679079821, -105.3295720093546 39.94022406411649, -105.3296652107925 39.94009313751392, -105.3298048465427 39.93996227854622, -105.330037503932 39.939771983658, -105.3301771394815 39.93964112423741, -105.3302550370624 39.93943868497224, -105.3303173668751 39.93927196798317, -105.3303333191918 39.93908135218683, -105.3303646313504 39.93893841725295, -105.3304578579342 39.93879557615114, -105.3306129394301 39.93867665461612, -105.3308299347333 39.93855782381141, -105.3309541765365 39.93839119647253, -105.3310164730188 39.9382363938341, -105.3310941896124 39.93810544244619, -105.3312028634002 39.93797453727169, -105.3314351864608 39.9379153035246, -105.331559101029 39.9378797395179, -105.3317141785255 39.9377608164918, -105.3319930238681 39.93766590340954, -105.332163519595 39.93757083274084, -105.3323184782625 39.93749956787977, -105.3325662183295 39.93746418386972, -105.3327829133291 39.93746449862973, -105.3334821172266 39.93789782489326, -105.3337092010423 39.93845478035888, -105.3337554338947 39.93853825329758, -105.3338326803261 39.93859793868223, -105.3339407409348 39.93871724417198, -105.3341728325842 39.9387533228644, -105.3342964869261 39.9388249913192, -105.3344355343734 39.93893242522267, -105.3345127252388 39.93901594144148, -105.334605279229 39.93914713971061, -105.3347906766642 39.93929038497647, -105.3349760472421 39.93944554468823, -105.3350997900354 39.9394814671437, -105.3353162913976 39.93956518034897, -105.3355636642642 39.93968468337358, -105.3356098428274 39.93979198504802, -105.3356713555442 39.93995888250201, -105.3355624587094 39.94018510982277, -105.3353456676618 39.9402205463219, -105.3349893366625 39.94035110089884, -105.3347416450673 39.94036266062547, -105.3344784168929 39.94039802796743, -105.3342187703895 39.94049634854602, -105.3342300595007 39.940683629287, -105.33424524894 39.94080279988832, -105.3342914539426 39.94089818733744, -105.3344961789176 39.94099717557393, -105.3346157633717 39.94120844226929, -105.3346773338235 39.94135150985174, -105.3346303196934 39.94158974164895, -105.3345957688523 39.9417773393035, -105.3345673052172 39.94204242014799, -105.3346597191067 39.94223319204949, -105.3348139071973 39.94248362637954, -105.3350612033855 39.94263887467899, -105.3352777722196 39.94269876025473, -105.3355252712221 39.94277060346691, -105.3358194951483 39.94272336402315, -105.3360516872704 39.94272369469476, -105.3363922364222 39.94272417883428, -105.3367018532639 39.94271270244277, -105.3369187084585 39.94265343391514, -105.3372129605016 39.94259427617204, -105.3375226061463 39.94257088373504, -105.3377548544015 39.94254738149012, -105.3380491323672 39.94247630506577, -105.3382505347019 39.94240509842705, -105.338513937799 39.94229823311669, -105.3389010628894 39.9422392012124, -105.3390715885114 39.94213220471062, -105.3392114080417 39.9419179302638, -105.3392428151568 39.94172733397711, -105.3393233416274 39.94161898118039, -105.3393363074271 39.94146533648792, -105.3393828295825 39.94142965521113, -105.339630748214 39.94132276755802, -105.339832060449 39.94128730237721, -105.3399406107836 39.94120404886886, -105.3401421178431 39.94108517813758, -105.3401886114176 39.94106141307962, -105.3404674572864 39.940966480408, -105.3406533181873 39.94091907671124, -105.3408703853 39.94076448278047, -105.3409326348646 39.94062158865495, -105.3410412926193 39.94049067422415, -105.3409808920442 39.94028805576299, -105.3409897233237 39.94002551761, -105.340980932132 39.93982335404601, -105.34099674378 39.93968039576468, -105.3410282836238 39.93943022612975, -105.3410443447997 39.93918003422367, -105.3410447332516 39.93901322507722, -105.3410450662076 39.93887024632174, -105.3410336766268 39.93871870956254, -105.3411230970743 39.93859630941661, -105.3412781318281 39.93848928917005, -105.3414020988481 39.93842988418462, -105.341515849407 39.93836323363961, -105.3416192681011 39.93822762982641, -105.3417123320203 39.93814435154387, -105.3418208462812 39.93807301188947, -105.3420222592663 39.93798988298423, -105.3422698308905 39.93802596659072, -105.3424400931839 39.93802619959498, -105.3427297277895 39.93806265947011, -105.3428732685956 39.93812211134178, -105.3430840868266 39.93827947499772, -105.3431822898061 39.93836083262784, -105.3433831552227 39.93851599989166, -105.3434795630392 39.93860290917354, -105.343645771096 39.93874274023654, -105.3437227820638 39.93890965441344, -105.3437689444899 39.93902886666783, -105.3439079255175 39.93917203517659, -105.3440806476839 39.93926808631675, -105.3442635820429 39.93932741052702, -105.344384129159 39.93940398872251, -105.3446657570558 39.93944710316149, -105.3448396699272 39.93948645664532, -105.3450992150013 39.93942385726057, -105.3451764562121 39.93935034054514, -105.3452854454025 39.93920963782646, -105.3453478192813 39.93900716756229, -105.3453324758724 39.93894757124433, -105.3453174834947 39.93873308230828, -105.3453141688943 39.93859363192674, -105.3453961873443 39.93842919480537, -105.3454701315971 39.93838441881511, -105.3455324096934 39.93834261821461, -105.3455869479147 39.93828584910379, -105.3456336662278 39.93825001155182, -105.3456999526396 39.93815436688384, -105.3457078670991 39.93809155129362, -105.345774126217 39.93800787266722, -105.3458169574422 39.93797202983635, -105.3459610115226 39.93785853899554, -105.3460427137029 39.93781975607154, -105.3461399078266 39.93780492782732, -105.3462526142029 39.93780507830835, -105.346357547 39.93780521831134, -105.3464624809674 39.93780535822026, -105.3465673868684 39.93781746411783, -105.3466761661568 39.93783555903681, -105.346796571137 39.93786862831799, -105.346881985164 39.93790763402901, -105.3469867370542 39.93798854768993, -105.347083770364 39.9380455196671, -105.3471458595813 39.93808748619713, -105.3472311803472 39.93816837384888, -105.3472699713123 39.9382013334698, -105.3473708908066 39.93825831035578, -105.3474407528604 39.93830028702409, -105.3475339681682 39.93832733465823, -105.3476427485254 39.93834542866371, -105.3477165832549 39.93834851827387, -105.3478098587675 39.93834864154184, -105.3479497636173 39.93835181827158, -105.3481168738894 39.93835503070434, -105.3482955902814 39.93838219132165, -105.3485663290427 39.93847499271768, -105.3489173950713 39.93849151148685, -105.3497608354034 39.93903131515625, -105.3499051285607 39.93910404030952, -105.3501228431005 39.93934738838904, -105.3503915615324 39.93962654754644, -105.350400661343 39.93971234687233, -105.3503294207818 39.93976661884747, -105.3502194413498 39.93976572926093, -105.3498018128802 39.9396293548314, -105.3491629100225 39.93940835371188, -105.3483566129954 39.93906216994667, -105.3480247199548 39.93897680428015, -105.3476625902587 39.93895811649597, -105.3473049946615 39.93897551567823, -105.3470468203971 39.93901336640935, -105.3467565528364 39.93909550958383, -105.3466367324471 39.93921113490654, -105.3466027453232 39.93944998874962, -105.3465605025822 39.93965010336079, -105.3462908554426 39.93994198794666, -105.3458940131122 39.94017027039276, -105.3455340356399 39.94031737702138, -105.3452125109515 39.94050206995038, -105.3448738103961 39.94061565635842, -105.3446045737641 39.94074602105159, -105.3444201768378 39.94090922146732, -105.3441504891605 39.94123572850936, -105.3440180360536 39.9414596316175, -105.3440588417544 39.94157217882472, -105.3441087282511 39.94165209942394, -105.3441408110076 39.94183801666134, -105.3442083965542 39.94193895905808, -105.344249041942 39.94197639575263, -105.3443022889449 39.94198370270044, -105.3443649776773 39.94197293540188, -105.3444167376543 39.94194527050977, -105.3444750322293 39.94189565912026, -105.3445047050119 39.94184048084426, -105.3445315828068 39.94172656519589, -105.3445461638083 39.94154136582213, -105.3446456843429 39.94134535515964, -105.3448614030582 39.94115051238641, -105.3450852114466 39.94102997251904, -105.3453117618755 39.94100848106682, -105.3454334287735 39.9410140239936, -105.3455381459786 39.94104387979846, -105.345615264635 39.94108360484331, -105.3456794784697 39.94114306213983, -105.3456936576798 39.94124233435014, -105.3456232594566 39.94136103208576, -105.3454790206228 39.94148594525846, -105.3452994412459 39.94161807458997, -105.345260220683 39.94172514236121, -105.3453157028288 39.94183245170021, -105.3455008873075 39.94208291329695, -105.3455888314258 39.94217652562062, -105.3459129593672 39.94262678691265, -105.3461191802726 39.94278303907976, -105.3464276688434 39.94296347566614, -105.3464971988181 39.94302076089416, -105.3465102514326 39.94306756376609, -105.3465029621614 39.9431100037764, -105.3464764128338 39.94315766084034, -105.3464080083053 39.94323924565847, -105.3462238298761 39.94330439209571, -105.3459996916824 39.94329175730961, -105.345841741395 39.9432602869895, -105.3457536159009 39.94326998077975, -105.3457141629159 39.94332550653542, -105.3457354489024 39.94342004628592, -105.3458521496769 39.94348923147759, -105.3461619038107 39.94351265458335, -105.3466264719512 39.94357602811639, -105.3468813323513 39.9436039136981, -105.3469741140173 39.94364693072029, -105.3470014923789 39.94370856024724, -105.3469458653255 39.94381846726618, -105.3468249318228 39.94390409492455, -105.3466895263439 39.94394785691841, -105.3464923497525 39.94400257219984, -105.3463787208825 39.94407865046045, -105.3463274436908 39.94416437045862, -105.3463368710556 39.94425756130052, -105.3465051621862 39.94434773235889, -105.3468933634192 39.94445108312228, -105.3470789371956 39.94453354237368, -105.3473618750095 39.94468761993063, -105.3476077831022 39.94478806418913, -105.3478766414147 39.94483201306166, -105.3479977654047 39.94483858920728, -105.3481372522787 39.94476370979286, -105.3482453905888 39.94452739768072, -105.3484437905829 39.9444187019977, -105.3486259823145 39.94430691253987, -105.3487423315608 39.94414969374191, -105.3490129147341 39.94359242734798, -105.3491340108557 39.94343173423461, -105.3493059779342 39.94336762004309, -105.3495243107314 39.94333573399553, -105.3497053349327 39.9433752893389, -105.3498445102611 39.94343981278547, -105.3500026987519 39.94362534593829, -105.3500575626043 39.94379875040127, -105.3502143510659 39.94420166014947, -105.3503112624806 39.94448059585778, -105.3503120243307 39.94458459468469, -105.3502832029022 39.94481336976445, -105.350300970492 39.94493811658024, -105.3503982828856 39.9450347527661, -105.3505838167 39.94513865452713, -105.3509050233133 39.94529359798763, -105.3511027920363 39.94548997156586, -105.3513546245374 39.94579577849958, -105.3514444997917 39.94588811076953, -105.3516026725817 39.94597137759611, -105.3517208975748 39.94600567457899, -105.3518405762703 39.94601937441158, -105.3519560576344 39.94598776664162, -105.3520502790885 39.94594445355338, -105.3522201694978 39.94592290094791, -105.3524040429403 39.94599939878466, -105.3526547492991 39.94631602639261, -105.3528397428303 39.94667371057839, -105.352854191666 39.94687038990777, -105.3528263263688 39.94711130763148, -105.3528824496291 39.94735108971799, -105.3531236142911 39.94767376819163, -105.3533754572079 39.94807201753893, -105.3535095024001 39.94836886940653, -105.3535091801626 39.94851899837285, -105.3534345654886 39.94866188254792, -105.353246801853 39.94908729334558, -105.3531914570367 39.94940864067144, -105.3531911033443 39.94957306478888, -105.3532453961211 39.94974103325151, -105.3534278442595 39.95000483331427, -105.3535977264722 39.95029109927498, -105.353706951089 39.95054013413743, -105.3537479616793 39.95090835791643, -105.3540492663155 39.95118040016152, -105.3543318430792 39.95143562611569, -105.3545945513623 39.95167804960032, -105.3546691554396 39.95177685194528, -105.354696493764 39.95184504081303, -105.3546976459791 39.951916725421, -105.3546986643523 39.95203973189982, -105.3546227298896 39.95232853300234, -105.3544141255283 39.95269311604522, -105.3542544405529 39.95297147602072, -105.354328387966 39.95314314435302, -105.3544950960814 39.95337569701889, -105.3547589612953 39.95378709435537, -105.3549020387573 39.95421263782769, -105.3548830434188 39.95440920980376, -105.354806468642 39.95460040077084, -105.3547633005575 39.95493811633833, -105.3548194703378 39.95514520178909, -105.354983454261 39.95532837636013, -105.3551509598883 39.955420341284, -105.35533130302 39.95549197808626, -105.3555265701328 39.95553835283317, -105.3556469662596 39.95556472809908, -105.3557060233276 39.95561276915417, -105.3557386458138 39.95566937293702, -105.3557741141502 39.95576549921196, -105.3557992750611 39.95602245334246, -105.3558505676371 39.95630145846711, -105.3556823119012 39.95632088393366, -105.3554859298368 39.95637159505921, -105.3552374249272 39.95646773426095, -105.3549249516538 39.95662020943129, -105.3547191238183 39.95666362646298, -105.3544637367979 39.95665966283416, -105.3540065873437 39.95656501021908, -105.3536895321031 39.9564987737959, -105.3533690273359 39.95650551578468, -105.3530862636785 39.95657473750998, -105.3526579361303 39.95670835306336, -105.3522487218811 39.95692587313406, -105.3519882100022 39.95711141236313, -105.3516543984425 39.95738535951605, -105.3514614232365 39.95763062854918, -105.3514385408322 39.95783632304158, -105.3515030716467 39.95806517346453, -105.3516327162817 39.95825478871504, -105.3517903015078 39.95841226836524, -105.3519260940527 39.95849795111383, -105.3520702935195 39.95856915836187, -105.3521104398092 39.95860745169789, -105.35212220401 39.95863842500425, -105.3521102839133 39.95867938499769, -105.3520746957046 39.95872122336939, -105.3520178350116 39.95875210856961, -105.3518836686614 39.95878613315444, -105.3516733318363 39.95880173663877, -105.351345777182 39.95870917935156, -105.3510048124872 39.9586400226201, -105.3506098071917 39.95857747228528, -105.3503832841733 39.95857717838697, -105.3502291566699 39.95861756977649, -105.3499724607688 39.95866380511001, -105.3497176360485 39.9586526012469, -105.3494911127846 39.95865230559473, -105.3492283080394 39.95870384425507, -105.3490717285018 39.95871526312619, -105.3488962982591 39.95871689126606, -105.3487037748324 39.95867567956383, -105.3485363790411 39.95860993791083, -105.3478214840077 39.95814889463594, -105.3471456360077 39.95776202530593, -105.3467618157279 39.95753709210727, -105.3465296949049 39.95748316629089, -105.3462287436664 39.95746034235974, -105.3459817638437 39.95741094481667, -105.3456695563883 39.95726454891713, -105.3454434965831 39.95717430831029, -105.3451590792293 39.9571407418311, -105.3448191912631 39.95717297927444, -105.3446068353019 39.95717269309261, -105.3443946158489 39.95709611761605, -105.3441827960147 39.95684524841415, -105.3440884076289 39.95664703425503, -105.3440378720344 39.9564039015618, -105.3440711556896 39.95613686272678, -105.3441425364855 39.95588635109922, -105.3441389977332 39.95581652211911, -105.3441136976464 39.95574272423425, -105.3440186020231 39.95565550758867, -105.3438741990323 39.95558088547542, -105.3435986820116 39.95550253670501, -105.3431903754274 39.95531610814066, -105.3425857909343 39.95514264437324, -105.342318205314 39.95497951658208, -105.341978907135 39.95476111029183, -105.3415462146834 39.95453170278824, -105.3413251764538 39.95446640101372, -105.3410226063689 39.95442202475896, -105.3405915068032 39.9543867512165, -105.3401411453694 39.95431463685155, -105.3396355797279 39.95422398497384, -105.3389704612986 39.95410320173998, -105.3385208374587 39.95402999317365, -105.3381922100665 39.9539168925779, -105.3380613773924 39.95387922079283, -105.3383821243641 39.95417929127716, -105.3385674690961 39.95436542476165, -105.3387481361285 39.95456584840096, -105.3389332719973 39.95484134311943, -105.3391972860632 39.95515269194618, -105.3393595717931 39.95527087623741, -105.3395404716461 39.95537478831839, -105.3397169369457 39.9553893318278, -105.339963064055 39.95540754654273, -105.3404224215921 39.95560835426767, -105.340737929226 39.9557517698098, -105.3408163394168 39.95598779399175, -105.3407741612119 39.95614858733419, -105.3407644374192 39.9563344475167, -105.3407823576073 39.95661685560312, -105.3407585423853 39.95687061110937, -105.340813971399 39.95700294350355, -105.3411988658981 39.95727156089524, -105.3413796242992 39.9574398108651, -105.34143978317 39.95753640426094, -105.3414486570114 39.95771514066693, -105.3414855003038 39.95785102185104, -105.3415686602473 39.95804415830918, -105.3416286954819 39.95819436922678, -105.3416888387843 39.95829811186334, -105.3417254175696 39.95854837578747, -105.3417808581094 39.95867713300948, -105.3419145010556 39.95913485006723, -105.3419930516309 39.95931368197322, -105.3421550957813 39.95954267131271, -105.342340474804 39.95972522305689, -105.342558426089 39.95988279881342, -105.3428645192128 39.96009053566726, -105.3430825891228 39.96019806749968, -105.343360798049 39.96041291535013, -105.3435556196811 39.96053113787423, -105.3439919356307 39.96067113365707, -105.3444420997995 39.96085046636512, -105.3446230140441 39.96095794510541, -105.3447388797202 39.96107248443195, -105.3447756268418 39.96125483276604, -105.3447195684986 39.96139416148351, -105.3445844845748 39.96155840560913, -105.3443796023165 39.96177617221307, -105.3442119288581 39.96197254236927, -105.3441696243447 39.9621905291703, -105.3441646115461 39.96235137391512, -105.3441130822002 39.96254075062669, -105.3440104872482 39.96271576210818, -105.3433584770403 39.96344764579057, -105.3432139409706 39.9636797911035, -105.3432090325889 39.96379416665803, -105.3432596704031 39.96399440692426, -105.3432580364064 39.96470572634975, -105.3433549485055 39.96498466743203, -105.3434611855153 39.96524932320219, -105.3435903286542 39.96565341505423, -105.3436874645537 39.96583584560934, -105.3437287659197 39.966057518448, -105.3437703294546 39.96616480941587, -105.3438722349838 39.96629362851484, -105.3440530565571 39.96644757631712, -105.3445631686427 39.96683788403377, -105.344799794762 39.96696688392825, -105.3451943215452 39.96711754282754, -105.3454078122883 39.96720719142478, -105.345677049642 39.96729691428796, -105.3458116807017 39.96733641345445, -105.3460947908402 39.9674547496716, -105.3462013150994 39.96759787164284, -105.3463031951509 39.96774098641889, -105.3463448281598 39.96781967985631, -105.3464235532126 39.96793059408106, -105.3465302247974 39.96800937500215, -105.3467158863003 39.96808111151876, -105.346920194601 39.96812427673464, -105.3471476832231 39.96818891961232, -105.3473891086939 39.96825357959553, -105.347653738839 39.9683289938379, -105.3478347816061 39.96838999925331, -105.347973974335 39.96846882176619, -105.3480852136772 39.96858335152659, -105.3482335625351 39.96872295112451, -105.3483587404312 39.9688374998723, -105.3484932173364 39.96894848511075, -105.3486369377627 39.9690809296067, -105.3487714009241 39.96919906389083, -105.3490962626725 39.96934961793916, -105.34924479809 39.96940700386404, -105.3494212532477 39.96944297880439, -105.349583788853 39.96947178771764, -105.3497927648202 39.96950780452823, -105.3499738912252 39.96953306242339, -105.3502663555101 39.96962995325117, -105.3507120197024 39.96977708492175, -105.3508559102671 39.96983446364893, -105.3510144171056 39.96990402892676, -105.3507610907815 39.97224584708899, -105.3500652202326 39.97934719403165, -105.3418996623729 39.97937414849856, -105.3418721629839 39.98661936937633, -105.3419194826023 40.00001443725064, -105.3416399577307 40.00001575410552, -105.3418273290447 40.00360327366313, -105.3388374913609 40.0036448119106, -105.3388058949128 40.00530808243246, -105.338795726333 40.00584332251616, -105.3387934667453 40.00602183021768, -105.3387270035912 40.00601412317715, -105.3383982183178 40.00595568795652, -105.338151578013 40.00588208577564, -105.3377671040206 40.00570696236554, -105.3373285781182 40.00549910201315, -105.3369504362309 40.00532350205108, -105.3368431115566 40.00528007755263, -105.3367229895943 40.00523958266538, -105.3366450284994 40.00521783590182, -105.3365619458977 40.00519804704746, -105.3364175023756 40.0051673551794, -105.3361720663683 40.00513809942974, -105.3359278874195 40.00514186912645, -105.3357000601205 40.00517393845384, -105.3354821624764 40.00523292485326, -105.335277058553 40.00531608548594, -105.335055076946 40.00544012468988, -105.3348959384454 40.00555711760371, -105.3347421019816 40.00569607847567, -105.3340179982824 40.0063459228852, -105.3335919011093 40.00672798825328, -105.3334759135093 40.00684069852375, -105.3333473507778 40.00695992022458, -105.3331601474786 40.00708588568939, -105.3330295658755 40.00715674094787, -105.3328786508896 40.00721362901468, -105.3327277823436 40.00725148258998, -105.3326017095741 40.00727206505377, -105.3324666615118 40.00728225163382, -105.332346118196 40.00728175130358, -105.3322316470357 40.00727053562846, -105.3321223657283 40.00725068294549, -105.3319433704749 40.00719854380947, -105.3316156501056 40.00708357764866, -105.3314064550343 40.00701529443396, -105.3312693027479 40.00697573807232, -105.331129784745 40.00695227812372, -105.3309669722376 40.00694130651628, -105.3308157622544 40.00694287255563, -105.3306714891247 40.00696055042577, -105.3305364855549 40.00699255128497, -105.3304037790614 40.00703707891983, -105.3302803351907 40.00709772007642, -105.3301452063981 40.00717981001052, -105.3300472214122 40.00726222653275, -105.3299783669689 40.00734307646246, -105.3298798497388 40.00750110712818, -105.329809066238 40.00768410686648, -105.3297098708511 40.00795106653643, -105.3295979826967 40.00815404581825, -105.329499882572 40.00826810157434, -105.3293689386155 40.0083821068506, -105.329195923688 40.00847408909392, -105.3289869006922 40.00854707608948, -105.3288218496635 40.00859082710579, -105.3286158589629 40.00860108037538, -105.3284145150462 40.0085831831356, -105.3281219836957 40.00851696663079, -105.3279159694295 40.00844517470038, -105.3275821259779 40.00833556754117, -105.3273762606026 40.00829654415817, -105.3272108329855 40.00827704768114, -105.3270833797487 40.00827850662595, -105.3269506294364 40.00828534787819, -105.3267674613358 40.00832026850438, -105.3266071149637 40.00837986137141, -105.3264650321416 40.00845707842387, -105.3263229298923 40.00854133656269, -105.326249510518 40.00861513609797, -105.3261668917761 40.00870652224373, -105.3261255458378 40.00876629376748, -105.3260611355457 40.00889642177923, -105.3260196468901 40.00901250626066, -105.3260148170761 40.00911104821939, -105.3260327666925 40.00925185877676, -105.3260553014007 40.00938915920306, -105.3261052535136 40.0095440960903, -105.3263419692115 40.01005127617276, -105.3264465809688 40.01031188572199, -105.3264784225342 40.01038936440644, -105.3265010749391 40.01048090913334, -105.326505419393 40.0105724254117, -105.3265006092558 40.01066392701546, -105.3264866456551 40.01075541664722, -105.3264451565952 40.01087150035953, -105.3263256657921 40.01106138032973, -105.3262522167964 40.01114574084041, -105.3261604492859 40.0112335925341, -105.3260328565253 40.01132520617322, -105.3259401904095 40.01138908370987, -105.3257919662363 40.01147421727937, -105.3256159553481 40.01157353262292, -105.3254352718555 40.01169062397658, -105.3252082916487 40.0118254291365, -105.3250646454044 40.01192834935858, -105.3249255613895 40.01205617301965, -105.3247909537152 40.01224090823586, -105.3247397197977 40.01237953421825, -105.3247069966153 40.01251463164453, -105.3247112003153 40.01267823765443, -105.3247432951604 40.01278853780204, -105.3247984865576 40.01290954304061, -105.3248537615394 40.01299854105027, -105.3249275568867 40.01308045290926, -105.3250641494043 40.01318495554976, -105.3252415382173 40.0132907627538, -105.3254309559128 40.01337640611038, -105.3257083201453 40.01343728721716, -105.3258110662966 40.01344989845412, -105.3260961720675 40.01350907548051, -105.3262499582188 40.01354389677252, -105.3263658730266 40.01358991627712, -105.3265122528776 40.01367782032638, -105.3266246277955 40.0137544626723, -105.3267314842063 40.01385210429353, -105.3267894054645 40.0139</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>25</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>Southern Hills MS</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>1500 Knox Dr, Boulder, CO 80305</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>http://shm.bvsd.org/</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>Southern Hills Middle School</t>
         </is>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>39.97413389369987</v>
       </c>
-      <c r="K19" t="n">
+      <c r="L19" t="n">
         <v>-105.2452260530946</v>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="M19" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="N19" t="inlineStr">
         <is>
           <t>http://shm.bvsd.org/</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
+      <c r="O19" t="inlineStr">
         <is>
           <t>POINT (-105.2452260530946 39.97413389369987)</t>
         </is>
@@ -1690,53 +1749,56 @@
           <t>POLYGON ((-105.0551956991301 40.18184398208187, -105.0551970626169 40.18167032751156, -105.0551970875692 40.18166723030277, -105.05523025625 40.17744353616711, -105.0552302810579 40.17744046057113, -105.0552414762126 40.17601476607788, -105.0552513829568 40.17475301109806, -105.0552514076745 40.17474994901017, -105.0552519959952 40.1746750538799, -105.0552520195328 40.17467199268808, -105.0552526354381 40.17459269892721, -105.0552526542794 40.17458963771727, -105.0552531367156 40.17451028580081, -105.0552531555569 40.17450722459085, -105.0552583571967 40.17365096448745, -105.0552583760022 40.17364790868083, -105.0552600120969 40.17337863736143, -105.0552600297223 40.17337558245075, -105.0552661709637 40.17236480711001, -105.0552661885532 40.1723617576026, -105.0552760273123 40.17074210973164, -105.0552963083236 40.16740327517449, -105.0552966362117 40.16734916580195, -105.0553334854068 40.16102383273662, -105.0553368567356 40.16044496943694, -105.0553372380196 40.16037944725436, -105.0553376788475 40.16030391644374, -105.0553377713311 40.16028796999728, -105.0580710513005 40.16025799056519, -105.0606010313516 40.16022699272562, -105.062539016009 40.16009099355082, -105.0634333444827 40.15986251985857, -105.064296309749 40.15959008850385, -105.064919505624 40.15935175545492, -105.0662970046367 40.1588843247345, -105.066765552507 40.15964313063317, -105.067322977026 40.16013699897744, -105.0678959694674 40.1604240008717, -105.0687409608614 40.16070000328342, -105.0694111630307 40.16090422372054, -105.0694629539653 40.16092000499503, -105.0705369421375 40.16129000865394, -105.0719189271613 40.16175401236442, -105.0730759142553 40.16213901527696, -105.0739259058449 40.16241901849396, -105.0744968993014 40.16262302002178, -105.0756918859996 40.16302902328239, -105.0775498655427 40.16357702807103, -105.0787978532788 40.16380003091128, -105.0795948459216 40.16388103180415, -105.0802848402826 40.16392203294821, -105.0807888352324 40.1639220337433, -105.0813998304982 40.16392203444205, -105.0829128177578 40.16392203457659, -105.083609519032 40.16392308127849, -105.0836161082395 40.16399500687811, -105.0836141587786 40.16413802271901, -105.0836030415373 40.16460987586909, -105.0836106635436 40.16484891209912, -105.0836300593452 40.16545713053579, -105.0836269525403 40.16549692411329, -105.0836220561698 40.16553698593949, -105.083613938554 40.16557703616078, -105.0835959221352 40.16565603140108, -105.0835711141966 40.16573390518737, -105.0835558587693 40.16577090983481, -105.0835398631979 40.16581202954788, -105.0835210296103 40.16584902129782, -105.0835000500647 40.16588600531175, -105.0834769351456 40.1659210605575, -105.0834260412004 40.16599307439358, -105.0833268254032 40.1661261315451, -105.0832439014171 40.16622795275293, -105.0832150677106 40.16626188854235, -105.0831919525168 40.16629694372924, -105.0831681144781 40.16633309328626, -105.0831478259643 40.16637392366613, -105.0831339771326 40.16641505106289, -105.0831190490881 40.16645699775201, -105.0831080505025 40.16650005739481, -105.0830950003841 40.16658593425269, -105.0830878765151 40.16693097503487, -105.0830959771383 40.16724395293009, -105.0830960976557 40.16792502758191, -105.0830930531922 40.16830494684462, -105.0830910643746 40.16868788974446, -105.0830899607455 40.16886796812796, -105.0830891382825 40.16941095828075, -105.0830898739331 40.16975794923593, -105.0830908276374 40.17077009335227, -105.0830780316235 40.17151508279193, -105.083075148123 40.17192712109441, -105.083080876397 40.17274410150467, -105.0830810478255 40.17329999660924, -105.0830759771914 40.17348500237775, -105.0830749017534 40.17371888591792, -105.0830771760332 40.1739901157939, -105.0830668337051 40.17410098249666, -105.0830771458684 40.17399043991578, -105.088302814376 40.1739809907825, -105.0883029993709 40.17397700160376, -105.0883031426125 40.17397700121329, -105.0883123178483 40.17397704920117, -105.0888742073944 40.17397999371771, -105.0892635502055 40.17397922794395, -105.0898870002667 40.17397799833534, -105.0899358508228 40.17397797709733, -105.0920959995587 40.17397699788575, -105.0920961416262 40.17397699748644, -105.0920962144237 40.17397699684266, -105.0928349994319 40.17396899906539, -105.0928751701174 40.17396600181887, -105.093035412355 40.17395404356559, -105.0930355022931 40.17396373747397, -105.0930905495083 40.1739629603663, -105.0933063695626 40.17394767675843, -105.0947811388498 40.17392604651604, -105.0950699350661 40.17392596063161, -105.0955101015059 40.1739269531794, -105.0957541527641 40.17392890476933, -105.0963270854283 40.17393008282001, -105.0964931512326 40.17392709427654, -105.0974990948966 40.17392895400177, -105.0977370735687 40.17392895919532, -105.0979528772734 40.17392696481058, -105.0981518434555 40.1739279313386, -105.0989699184054 40.17392802714794, -105.0998391512321 40.17393103942207, -105.1001161310761 40.17393199790583, -105.101211927436 40.17392892050625, -105.1023799809039 40.17393102219533, -105.1024508498185 40.17392907018132, -105.1024948495252 40.17393196664215, -105.1024928436826 40.1739690192746, -105.1024659300747 40.1745939986924, -105.1024538771325 40.17579907983215, -105.1024459726393 40.17647792955385, -105.102446985836 40.17691688312216, -105.1024359298053 40.17764513457093, -105.1024348285392 40.17795588288692, -105.1024151073728 40.17943188442915, -105.102413175028 40.18019091209275, -105.1023970324222 40.18093204823994, -105.1023829530066 40.18125894705506, -105.1023831548078 40.18140800978896, -105.102370035092 40.18248900592155, -105.1023460249624 40.18414699542499, -105.1023359709285 40.18488705328424, -105.102324014524 40.18558510414968, -105.102314050903 40.18661587375054, -105.1022961545613 40.18759500754209, -105.1022951231635 40.18764908370499, -105.1022919348154 40.18813304226678, -105.1022929712663 40.18856787832284, -105.1022938744325 40.18859697923833, -105.102305841591 40.18899891023079, -105.1023129456827 40.18974287047573, -105.1023359238445 40.19064912338679, -105.1023450792598 40.19183807835071, -105.1023480324539 40.19219001707661, -105.1023401095519 40.19238187512373, -105.1023501276933 40.19385193690373, -105.1023748592168 40.19451991641212, -105.1023850650994 40.1948559566662, -105.1023868541003 40.19503988820251, -105.1023809230087 40.19574811518007, -105.1023788304601 40.19586093436818, -105.1024139175533 40.19696213301737, -105.1024319782109 40.19815907813807, -105.1024859020631 40.19952909100861, -105.1024847271985 40.20065462381238, -105.1024006556609 40.20088934679336, -105.1024054437498 40.2013562575215, -105.102421336487 40.20328529873123, -105.1024213646525 40.20328751259089, -105.1024214449243 40.20329367141449, -105.1024151901731 40.20329347428748, -105.1018971891388 40.2032814736801, -105.1018961897053 40.20421247454206, -105.1025107003073 40.20422330641446, -105.1025237619839 40.20539370203086, -105.1025237636843 40.20571670054039, -105.1025437709455 40.20634669622018, -105.1025137811899 40.20727069089985, -105.1025047847938 40.20772268878633, -105.102465788828 40.20820268604596, -105.102494799139 40.20914168066236, -105.1024778062865 40.2099546758207, -105.1024751480868 40.2103992398415, -105.1020764826853 40.210400971623, -105.0978221643321 40.21038836945402, -105.0978192865362 40.20995801171471, -105.0978192638643 40.20995469549757, -105.0977981545344 40.20679786929404, -105.0976247893968 40.20679703029651, -105.0976247948587 40.20679491652393, -105.0971607119664 40.20679337303581, -105.0971599989639 40.20679337055231, -105.0954331146536 40.20678761374383, -105.0932545485407 40.20678031284936, -105.0932022136999 40.20678056108493, -105.0932041876712 40.206406475457, -105.0932105779957 40.2051159902964, -105.0932147345931 40.20427675894129, -105.0932201875574 40.20317547481145, -105.0930820960962 40.20317412349315, -105.093005727191 40.20317337651804, -105.09300572348 40.20317301534985, -105.0928657727666 40.20317203549725, -105.0926146724067 40.20317027581347, -105.0921975370513 40.20316735111282, -105.0919455217571 40.20316558314721, -105.0917522278974 40.20316422728517, -105.0914944937617 40.2031624183343, -105.0912832223234 40.20316093513956, -105.0908696894077 40.20316115529705, -105.0904716416836 40.20316441081984, -105.0897408380691 40.20317038385568, -105.088853254461 40.20317763139809, -105.0877735888691 40.20318643920209, -105.0856447171413 40.20320449486757, -105.0837211863008 40.203227474651, -105.0835981069327 40.20321967515504, -105.0835791856489 40.20321847582563, -105.0830682814023 40.2032196909061, -105.0822069163204 40.20323024316917, -105.0816501847357 40.20324047561559, -105.0806879610338 40.20324837306046, -105.0798893828385 40.20325404710055, -105.0790784538952 40.20326612103604, -105.0787342713654 40.20327551513552, -105.0783671987761 40.20327647585538, -105.0779601843807 40.2032754757722, -105.0776037795553 40.20327547689448, -105.0765138064435 40.20327584437361, -105.0747471835121 40.20329593233741, -105.0741741031875 40.20330244293366, -105.0741613829337 40.20330267867917, -105.0740449135742 40.20330506064477, -105.074014699015 40.20330567887017, -105.0690749998827 40.2033999992119, -105.067296999437 40.20343799958135, -105.0662489993874 40.20346199884766, -105.0650095092602 40.20349053724983, -105.0649459997082 40.20349199875547, -105.0647999996946 40.20349499884104, -105.0647763071737 40.20349548788953, -105.0647501006766 40.20349602781442, -105.0647029999319 40.20349699885044, -105.0625290002004 40.20354499890966, -105.0605809999359 40.20358599860956, -105.0604691803914 40.20358828730515, -105.0594589803057 40.20360895889921, -105.0594569996611 40.2036089990881, -105.0594407995711 40.20360935166872, -105.058538999233 40.20362899881254, -105.056911999972 40.20367299893432, -105.0557639998678 40.20367599809817, -105.0557612194496 40.20367601713887, -105.0551933208667 40.20367993430043, -105.0551658094086 40.20367990683798, -105.0551658058408 40.20367704099404, -105.0551658037605 40.20367628174822, -105.0551657962894 40.20366431764384, -105.0551658011341 40.20366106365725, -105.055165939419 40.20355375046467, -105.0551659441694 40.2035505108879, -105.055166559143 40.20308397822347, -105.0551673600189 40.20247699891858, -105.0551687234147 40.20144399367533, -105.0551698371555 40.20059995386577, -105.055169869857 40.20057520624766, -105.0551698743182 40.20057201079945, -105.0551708702638 40.19981742814952, -105.0551708746955 40.19981423720408, -105.0551741094728 40.19736226693898, -105.0551741138158 40.19735908950151, -105.0551753876223 40.19639540436918, -105.0551753942906 40.19639223054278, -105.0551776862514 40.19523231880929, -105.0551776917097 40.19522915038146, -105.0551857428336 40.19115277071814, -105.0551895198951 40.1892402250088, -105.0551895204548 40.18923708718096, -105.0551895524011 40.1891528441331, -105.0551895553035 40.18914970721488, -105.0551896237061 40.18907048357343, -105.0551896265968 40.18906734845638, -105.0551907707022 40.18769647581839, -105.0551953437782 40.18224286923797, -105.0551953462757 40.18223997368663, -105.0551956753519 40.18184707929512, -105.0551956991301 40.18184398208187), (-105.0682879304474 40.17423889546031, -105.0679761762959 40.1742478872944, -105.0682879316216 40.17423889546469, -105.0705337647592 40.17417980111477, -105.0682879304474 40.17423889546031), (-105.0741833857628 40.19582695548362, -105.0741934852469 40.19582692062273, -105.0860866501783 40.19578522125577, -105.0741833857628 40.19582695548362), (-105.0741833528738 40.19582695582105, -105.0741833528728 40.19582695626313, -105.0741833857628 40.19582695548362, -105.0741833528738 40.19582695582105))</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D20" t="n">
+        <v>28</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>Trail Ridge MS</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>1000 Button Rock Dr, Longmont, CO 80504</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>https://trms.svvsd.org/</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>Trail Ridge Middle School</t>
         </is>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>40.17693117783666</v>
       </c>
-      <c r="K20" t="n">
+      <c r="L20" t="n">
         <v>-105.0576162268638</v>
       </c>
-      <c r="L20" t="inlineStr">
+      <c r="M20" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr">
+      <c r="N20" t="inlineStr">
         <is>
           <t>https://trms.svvsd.org/</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
+      <c r="O20" t="inlineStr">
         <is>
           <t>POINT (-105.0576162268638 40.17693117783666)</t>
         </is>
@@ -1756,29 +1818,32 @@
           <t>POLYGON ((-105.4661484313311 40.16510540791135, -105.46628891067 40.16510477709761, -105.470815740543 40.16518143398583, -105.4708146541582 40.16519354991458, -105.4707617910061 40.16578360363307, -105.4707617862852 40.16578366217297, -105.4705125686798 40.16856524699041, -105.4704672528061 40.1690710003927, -105.4704561694049 40.16919470380456, -105.4704014266738 40.1698729832864, -105.4703235422809 40.17083798352486, -105.4701471120568 40.17302390050776, -105.470147089627 40.17302417969756, -105.4701398981323 40.17311326375602, -105.4701498775658 40.17311351851009, -105.470200732758 40.17311482223527, -105.470709432716 40.1731278654992, -105.4711861857428 40.17314008889846, -105.471439289043 40.1731465768118, -105.4727391684574 40.17317988978623, -105.4749708600473 40.17323704782745, -105.4750032321987 40.1726821562563, -105.4750206722191 40.17238323337168, -105.4750210361202 40.17237698847438, -105.4752042504024 40.16923656802826, -105.479787691759 40.16935887360058, -105.4797873653326 40.16937091048318, -105.4797734359278 40.16988387259018, -105.4797733872597 40.16988566754004, -105.4796805373642 40.17330482726621, -105.4796240684069 40.17656529689094, -105.4796152483834 40.17796396985926, -105.4796026937846 40.17995501780022, -105.479611783183 40.17995483837693, -105.4809046495147 40.17992930563622, -105.4809104417855 40.17992919131213, -105.4821456944617 40.17990478346833, -105.4842904768209 40.17986236891954, -105.4842904845098 40.17987483273979, -105.4842905938626 40.18005209836011, -105.484290852698 40.18047691385383, -105.4842909836418 40.18069288673419, -105.4842919357208 40.18225457717938, -105.4842923359611 40.18291119120383, -105.4842927315417 40.18355750826427, -105.4843017355777 40.18355781209871, -105.4858596675139 40.18361035232417, -105.4887108236855 40.18370645233315, -105.4890342964373 40.18371735136233, -105.4913673103303 40.18380308278645, -105.4916169415424 40.18381225335324, -105.493803003558 40.18389564358236, -105.4938093397902 40.1838958852905, -105.4938123200268 40.18389599982997, -105.4938523169958 40.18035330559622, -105.4938523205461 40.18035299938223, -105.4942081234937 40.18036470973328, -105.4942254027887 40.18036558420872, -105.4988689323545 40.18060051532034, -105.5037971648563 40.18084965648772, -105.5066788071574 40.18091382279687, -105.5115988430433 40.18102320894966, -105.5138093385616 40.18107228813918, -105.5207705453987 40.18122672640443, -105.5208006874244 40.18122739465633, -105.522236754261 40.18127360796668, -105.5222435283211 40.18127382641728, -105.5222435741154 40.18127382730909, -105.522435320304 40.18127999739902, -105.5224377955276 40.18127643582816, -105.5224378823772 40.18127630972313, -105.523680357985 40.181292988343, -105.523688178229 40.1812930930153, -105.5236896753479 40.18129311342297, -105.5237041709683 40.18072051517435, -105.5237197330747 40.18010577977868, -105.5237413580885 40.17925150068127, -105.5237454789506 40.17908870192743, -105.5237510683669 40.17886786445666, -105.5237651645466 40.17831101269118, -105.5237857437776 40.17749800315436, -105.5238776530766 40.17387231186575, -105.5258247721261 40.17387231837259, -105.5258340931253 40.17387231809113, -105.5332652858553 40.17387203873018, -105.5332746068535 40.17387203604751, -105.5332742031089 40.1738843189681, -105.5331893193217 40.17646799626176, -105.5331568626344 40.17752450998029, -105.5331662580995 40.17752449827886, -105.5332269975165 40.17752442499798, -105.5332266806333 40.17753671869425, -105.5331269808046 40.18141083850799, -105.5330262556054 40.1837602446121, -105.532976230018 40.18492700366666, -105.5328963810823 40.18678931519381, -105.5328252778692 40.18844755645122, -105.5328252743849 40.18844763660821, -105.5328144473783 40.1887670954498, -105.5328026033848 40.18959315645375, -105.5327760272405 40.19144611821562, -105.5327628767569 40.19236313910528, -105.5327720701403 40.19236356970227, -105.5328092241853 40.19236530368316, -105.5328090737093 40.1923771568957, -105.5328019262174 40.19293933922767, -105.5328018956497 40.19294170518686, -105.5328006690869 40.1930380970772, -105.5328098787648 40.19303559882346, -105.5328294254024 40.19303029578, -105.5328935660998 40.19301413198865, -105.5329570730651 40.19299410915016, -105.5330083598834 40.19297567307023, -105.5330790606768 40.1929545853694, -105.5331549173888 40.1929269242624, -105.5332445784334 40.19289053114875, -105.5333357318797 40.19285139332066, -105.5334323856855 40.19282329373202, -105.5335304733625 40.19279520175227, -105.5336091149603 40.19277140683688, -105.5336459058447 40.19275785969391, -105.5336515583924 40.19275577849825, -105.533684251341 40.19274374108799, -105.5337565232855 40.19271606081569, -105.5338179414305 40.19269327228345, -105.533890165039 40.19266779307718, -105.5339501238616 40.19264610006633, -105.5340122329798 40.19262441809995, -105.5341047369489 40.19258913845898, -105.5341957862916 40.19255495433799, -105.5342200411473 40.19254790514945, -105.5342198678148 40.19256285923371, -105.5342193376537 40.19260852935302, -105.5342183473157 40.19269425235101, -105.5342183360385 40.19269518000148, -105.5342180715312 40.19271798939261, -105.5342271532779 40.19272517011618, -105.5343393829121 40.19281390637015, -105.5346356497051 40.19259680260618, -105.5348823209668 40.19251699672893, -105.5349371865247 40.19249180670148, -105.5349909777208 40.19246710871604, -105.537495561658 40.19258391871914, -105.5375025897888 40.19185229996346, -105.5375101454505 40.19106602720946, -105.5375433224156 40.1910399954814, -105.5375224677095 40.18937951494874, -105.5375223216064 40.1893679950532, -105.5372715249519 40.18934647278628, -105.537254321171 40.18934499589563, -105.5375677880135 40.18893092853408, -105.5375946466315 40.18889544853639, -105.541762862168 40.1891617345586, -105.5422569890588 40.18918897106952, -105.5422571009006 40.18920076026023, -105.5422758519701 40.1911640951709, -105.5422833975333 40.19195391480071, -105.5422833975938 40.19195401206859, -105.542297092536 40.19338773536003, -105.5422970925746 40.19338779750338, -105.5423024628827 40.19394992984792, -105.5423929265994 40.20341858732859, -105.542401834668 40.20341858226157, -105.5424019515685 40.20343087127191, -105.5471617411033 40.203428251832, -105.5471710649767 40.20342824622806, -105.5471762500321 40.20702449927905, -105.5471669256137 40.20702443013139, -105.5469038813974 40.20702247197197, -105.5423441045886 40.20698842150102, -105.5423441034594 40.20698849445215, -105.5422953313193 40.21055420708196, -105.5422860075863 40.21055412132916, -105.5404398525206 40.21053711938241, -105.5326909158406 40.21046358966055, -105.5326905760758 40.21136204136256, -105.5326905761208 40.21136213502758, -105.5326902668153 40.21217981128849, -105.5326894995797 40.21419262998702, -105.5326895026425 40.21419411331591, -105.5326985284376 40.21419413237972, -105.5422526119581 40.21421377049138, -105.5422524668593 40.21422603345813, -105.5422084115658 40.21794388539156, -105.5411373910101 40.21826779544625, -105.5398831425591 40.21944693342513, -105.5379809748795 40.21961963612427, -105.5379291219123 40.21962350240685, -105.5378566567431 40.21962890467403, -105.5364658151693 40.21975515971221, -105.5364659849748 40.21975632326548, -105.536469145231 40.2197779543675, -105.5364610049816 40.21977874858243, -105.5360297782496 40.21982080776719, -105.5360049453737 40.2214518136923, -105.5348769137664 40.22144872610919, -105.5338911592008 40.22144602273305, -105.5333207578963 40.22144445293673, -105.5326849358092 40.22144269979285, -105.5326849473221 40.2214446523428, -105.5326967674883 40.2233561262393, -105.5326825303639 40.22418840574673, -105.5326820404199 40.22504857987344, -105.5326910735317 40.22504859983672, -105.5344553890728 40.22505242161549, -105.5353538558136 40.22505402382836, -105.5360637775385 40.22505528352068, -105.5364251454815 40.22505592322528, -105.5364318357178 40.22505593462795, -105.536760204845 40.22505651522585, -105.5373800222655 40.2250576054056, -105.5374809703504 40.2250577834895, -105.5385255461858 40.22505961624928, -105.5405764553367 40.22506318763808, -105.5419484417806 40.22506555326001, -105.5419590751946 40.22506557191936, -105.5420808495041 40.22506765406047, -105.5420823229212 40.22506767874194, -105.5420822364319 40.22507980477056, -105.5420562713165 40.22872637531357, -105.542057627296 40.22872637662191, -105.5420429039838 40.2322667322377, -105.5418212665354 40.24069807142973, -105.5417703294095 40.24320999597101, -105.5417913293522 40.24484599488542, -105.5418693303538 40.25068399588682, -105.5419533310875 40.25691899504218, -105.5420123310872 40.26132699564431, -105.5420510583876 40.26143505394957, -105.5420511054112 40.26143505393247, -105.5420601092523 40.26143504165487, -105.546896776124 40.26142835486699, -105.5469164731246 40.26142832707124, -105.5488073098715 40.26142565841789, -105.5516765188264 40.26142154904153, -105.5516962275788 40.26142152042718, -105.5564490412647 40.26141455566594, -105.5564687629445 40.26141452623263, -105.5591675481954 40.26141048439985, -105.559187278102 40.26141045449919, -105.5591940095238 40.26141044475258, -105.5610087103939 40.26140744097114, -105.5795558249904 40.26109930837292, -105.5795753264785 40.2610990572043, -105.5951059878192 40.26090826365041, -105.5951255644495 40.26090802240864, -105.5978803250462 40.26087396174936, -105.5978999087103 40.26087372003241, -105.5990498899888 40.26085948275252, -105.5990694865891 40.26085924983279, -105.5995397909104 40.26085370200565, -105.5995593945634 40.26085347079817, -105.6024803232683 40.26081898919289, -105.6142594281275 40.26067918769429, -105.6159287966142 40.26065927760523, -105.6159484448253 40.26065904267666, -105.6183738399164 40.26063000678786, -105.6183934869193 40.2606297624392, -105.6213214042607 40.26059298525797, -105.6213410559414 40.26059273860285, -105.6230240548107 40.26057156630034, -105.6230437100057 40.26057131935239, -105.6277277549875 40.26051225854213, -105.627747425429 40.26051200987794, -105.632275471989 40.26045473382353, -105.6322951553285 40.26045448437176, -105.6333595672079 40.26044099555356, -105.6333792540661 40.26044074591335, -105.6336239250111 40.26043764207176, -105.6336436106918 40.26043739238794, -105.6344099544128 40.26042767444419, -105.6344296424389 40.26042742462398, -105.6344533637605 40.26042712418371, -105.6344730517862 40.26042687435609, -105.6370401114326 40.26039427547199, -105.6370598053172 40.2603940251974, -105.641661457955 40.26033544727563, -105.6416811682616 40.26033519529398, -105.6421922091127 40.26032867946999, -105.6422119170661 40.2603284283015, -105.6463212330816 40.26027594287727, -105.6463409574624 40.26027569098492, -105.6510511032203 40.26021535336445, -105.6510708369704 40.26021510065377, -105.653220247745 40.26018750197031, -105.6534108731882 40.2601810802276, -105.6533823627512 40.26010275780921, -105.6532830172156 40.25994882313275, -105.6532015168119 40.259833817446, -105.6530755380744 40.25970888806435, -105.653056450447 40.25969061631895, -105.6528639596007 40.25950741268624, -105.6526889307466 40.2593871624231, -105.652642514434 40.25935601447338, -105.6524271025182 40.25918859577206, -105.652112632482 40.25892918790828, -105.6518414912158 40.25866632340869, -105.6518412163808 40.2586659058817, -105.6518402220181 40.25866439414499, -105.6518249196642 40.25864111788805, -105.651683174363 40.25842552064559, -105.6516722710576 40.25840806831427, -105.6515514218632 40.25817243805065, -105.6515429003808 40.25815503662493, -105.6514243241588 40.25786656297638, -105.6514187228448 40.25784972511072, -105.6514055789766 40.25757162818682, -105.6513344204328 40.25729383767664, -105.6513306212376 40.25727751710651, -105.6512928566423 40.25697723763877, -105.6512494136496 40.25670131742907, -105.6512475526345 40.25668592286098, -105.6512481806062 40.25659521519253, -105.6512491443465 40.25645626717135, -105.6512492414307 40.25644232184331, -105.651250394949 40.25627562546527, -105.6512238153397 40.25580599850561, -105.6512233117349 40.25579151809188, -105.6512386810696 40.2554038107325, -105.6512392740317 40.25539031326282, -105.6512547967072 40.25511750050543, -105.651254798984 40.25511746717952, -105.6512556523308 40.25510424315733, -105.6512679930778 40.25496298995328, -105.651283544426 40.25478497372899, -105.6512465313483 40.25451425149574, -105.6510657606499 40.25415446368373, -105.651056843717 40.25413708614312, -105.6508969847668 40.25382258276831, -105.6505310873636 40.2534957431415, -105.6505198035114 40.25348589422141, -105.650277580469 40.25334159185142, -105.6502158172845 40.25330586876338, -105.6497508549943 40.25305330688136, -105.6493031225032 40.25278747457062, -105.6489024621259 40.25250204640531, -105.6485320184643 40.25224942820618, -105.648122926153 40.25197372674319, -105.6478519627375 40.25176733123399, -105.647595323896 40.2516000866161, -105.6474810359026 40.2515261922803, -105.6473040944805 40.25143101667013, -105.6471837932539 40.25136724816764, -105.6468534777815 40.25120486346038, -105.6466993803544 40.25114202354365, -105.6465010494459 40.25106199343578, -105.6463131316636 40.25101511518552, -105.6461854347542 40.25098444290174, -105.6459617149985 40.25091212623183, -105.645862718699 40.25086625543839, -105.6439109359637 40.24997257845546, -105.6439113906358 40.24997248152362, -105.6440326178304 40.24994670984607, -105.6460486209198 40.24951810932338, -105.6461040002026 40.24950599091284, -105.6461040377955 40.24950598185919, -105.6461837138841 40.24948586944218, -105.6461837538199 40.24948585678304, -105.6462761693258 40.24945621494909, -105.6462878338384 40.24945293635419, -105.6465034720074 40.2493933900957, -105.6465165544287 40.24939030511742, -105.6468338582291 40.24931722103709, -105.6468479730201 40.24931432744434, -105.6473447774411 40.24921444122509, -105.6473620074362 40.24921285670883, -105.6478251640483 40.24917729760249, -105.6478451563986 40.24917744047953, -105.6483876106674 40.24918924142482, -105.6484084764347 40.24918997028969, -105.6490580710522 40.24921440685837, -105.6490793598224 40.24921560338041, -105.6496621472309 40.24925061573745, -105.649857509743 40.24926235109255, -105.6498792923866 40.24926416375346, -105.6504807419691 40.24931712691847, -105.6505029278615 40.24931949642218, -105.6510873439726 40.249384258711, -105.6510876331863 40.24938428985514, -105.6517955093473 40.24946011446387, -105.6524384646635 40.24946103545784, -105.6532240381383 40.24939543248849, -105.6532429858952 40.24939464187201, -105.6540359245012 40.24936764317474, -105.6540561108867 40.24936779732936, -105.6547920954059 40.24937937171175, -105.6548135707898 40.24938089655689, -105.6553635528423 40.24942562557963, -105.6560772134397 40.2494691280667, -105.6560990989358 40.2494710970272, -105.6566697271875 40.24952454693272, -105.6572882420254 40.24953298344785, -105.6572884124538 40.2495329823156, -105.6577466825842 40.24952787256891, -105.6577468823637 40.24952785698604, -105.658364554839 40.24947889500469, -105.6583837733506 40.24947829771016, -105.658383836817 40.24947829582203, -105.6588610698823 40.24946552024045, -105.6593578213218 40.24936558880857, -105.6596740517714 40.24922577817019, -105.6598284918649 40.24908374683517, -105.6600357955445 40.24885510058633, -105.6601709350914 40.24869839282666, -105.6602180098776 40.24847606239258, -105.6602904669786 40.24808708989965, -105.6603197434563 40.24775706340495, -105.6603209213945 40.24774420990298, -105.6603381955352 40.24758479666077, -105.6603395938818 40.24757220763556, -105.6603473707779 40.24750678741342, -105.6603488540162 40.24749431264927, -105.6603658886433 40.24735099924052, -105.6603676534624 40.2473388122845, -105.6604413607002 40.24701574268065, -105.6604416576382 40.2466576694766, -105.660406673147 40.24625862093598, -105.6604060936211 40.24624414514405, -105.6604638791043 40.2458376972433, -105.6604423228038 40.24554413969873, -105.6604183656476 40.24532331789342, -105.6604176166594 40.24530874776879, -105.6604654929911 40.24502852130396, -105.6604680799253 40.24501810382434, -105.6606031082612 40.24480953958241, -105.6608380761308 40.24465551037683, -105.661090919282 40.24451736259382, -105.6614394345306 40.24425372862866, -105.6617972409519 40.24400229844849, -105.661993737268 40.24379598909656, -105.6622515148447 40.24354079687833, -105.6623638976777 40.24339320647818, -105.6623412545372 40.243148140186, -105.6622271542483 40.24289913312061, -105.6622212185086 40.24288262853066, -105.662246928383 40.24270330468485, -105.6622493009619 40.24269235519348, -105.6624203867668 40.24238932411787, -105.6626383198902 40.24217056212871, -105.6627478603099 40.2420858297572, -105.6628966257281 40.24188143849485, -105.6630035083658 40.2416272908031, -105.6630070175849 40.24161941982204, -105.6631343254574 40.24137469705771, -105.6632915945943 40.24121971764026, -105.6634577117512 40.24103557054804, -105.6636414775772 40.24080598165017, -105.6638605888681 40.24047958579609, -105.6641361334141 40.24008308784516, -105.6643937880334 40.23986345373206, -105.6646430665669 40.23956239662796, -105.6647837931359 40.23929073503575, -105.6649769754472 40.23895438237981, -105.6651788634559 40.23861149463966, -105.665323466031 40.23835513830205, -105.6653962474659 40.23809944644505, -105.665431211319 40.23766674878126, -105.6654329294115 40.23765467076841, -105.6655795293855 40.23730339632174, -105.6656516849346 40.23700392224806, -105.6655733758443 40.23677124300807, -105.6654192999047 40.23653663304073, -105.6652664880635 40.23634685679159, -105.6651081521364 40.23616363214872, -105.6650945635468 40.23614659102824, -105.6649503217293 40.23588669668948, -105.6649408301455 40.23586931017438, -105.6648173713558 40.23562903403352, -105.6648096253163 40.23561180533154, -105.6647862204469 40.23550442489909, -105.6647251887129 40.23522442147496, -105.6647251756337 40.23522435844993, -105.6646582848182 40.23494468934514, -105.6646546756029 40.23492852738642, -105.6645951132258 40.23457015220544, -105.6645927169959 40.23455456581809, -105.6645619404331 40.23428038048088, -105.6645609881937 40.23426566023956, -105.6646107631039 40.23381407701542, -105.6646123901615 40.23380175146494, -105.6646686018296 40.23352436399449, -105.6646712989217 40.23351378322931, -105.6648220164282 40.23318151580031, -105.6648255241641 40.23317475342208, -105.6650047084142 40.2329491006681, -105.6651964929561 40.2327528359099, -105.6654011529644 40.23258888212007, -105.6657063539013 40.23236997563181, -105.6659413331565 40.23217075944036, -105.6661675652812 40.23202312776482, -105.6663889616327 40.23191128709515, -105.6666810970455 40.23171510873143, -105.6666926686825 40.23171249465987, -105.6670132530934 40.23164008776747, -105.6670310503309 40.23163893539422, -105.6670310985044 40.23163893352346, -105.6671542201482 40.23163200282799, -105.6671543176415 40.23163198737654, -105.6673891053773 40.23159393428879, -105.6675672799185 40.23153819341664, -105.6677025916841 40.23133320802084, -105.6677681890939 40.23097816878754, -105.6677631503988 40.23075299479768, -105.6677483196333 40.23044769834121, -105.6677481743348 40.23043358126473, -105.6677741899327 40.2302316910987, -105.6677764100459 40.23022044448404, -105.6678022827057 40.23016966127873, -105.6679082388013 40.22996248731734, -105.6680695015121 40.2297791769222, -105.6682133000139 40.22966333765718, -105.6684010177816 40.22951487491294, -105.6685625454325 40.22935359900887, -105.6687415781404 40.22916824706451, -105.6688267008086 40.22894056836384, -105.6688429479812 40.22873624245703, -105.6688205696722 40.22852339716228, -105.6687613011443 40.22838176133099, -105.6686730393414 40.22821884274862, -105.6685174411165 40.22801933434805, -105.6683511792286 40.22783588408025, -105.6683375401028 40.22781896947912, -105.6682470624096 40.22761127111529, -105.6682416637716 40.22759486778096, -105.6682721112314 40.22737017614368, -105.6682739650483 40.22735817442233, -105.6683029921154 40.22722332576805, -105.6683058044111 40.2272130959819, -105.6683934966554 40.22704599071793, -105.6685196675831 40.22692074262096, -105.6687379630553 40.22675606758625, -105.6689083831121 40.22657508868081, -105.6690438599216 40.22640284891151, -105.6690758537972 40.22632072549793, -105.6690792556187 40.22631231949595, -105.6691903428408 40.22606427355334, -105.6692787329387 40.22583821434375, -105.6693278820078 40.22567399448331, -105.6693861052922 40.22544429847117, -105.669440759808 40.22514343033741, -105.66945233353 40.2249046090048, -105.6694532890332 40.22489151701731, -105.6694919852029 40.22466959399863, -105.6694915482502 40.22436290200361, -105.6693372707889 40.22410474212811, -105.6691337832986 40.22385606282835, -105.6689801460077 40.22368898447323, -105.6688367933033 40.22358134839062, -105.668820995009 40.22356996322452, -105.6686399339946 40.22346121020597, -105.66857070503 40.22342023718163, -105.6684063343704 40.22334358118142, -105.6683101888107 40.22329963458959, -105.6680685904649 40.22318068359311, -105.6678529537799 40.22304919374229, -105.6676002381706 40.22290378130718, -105.6674823272445 40.22284463958258, -105.6673437859818 40.22277593321919, -105.6672358734293 40.22272320634443, -105.6669856426672 40.22260732588539, -105.6667614982625 40.22246269083642, -105.6664857475077 40.222278601177, -105.6662919082906 40.22213095583463, -105.6661158510701 40.22201122023689, -105.6660285158423 40.22195229519745, -105.6659311617552 40.22189506412996, -105.6658563941644 40.22185175849506, -105.6656409412277 40.2217135933068, -105.6654520699702 40.22157582560256, -105.6653094536946 40.22148618217604, -105.6652393815789 40.22144276315675, -105.665179073635 40.2214088029338, -105.6650717714665 40.22134893480318, -105.6648732975747 40.22122908068761, -105.664797561422 40.22118791743397, -105.6646748951959 40.22112196728029, -105.6644591962295 40.22100981930868, -105.6642219518465 40.22087489948009, -105.6640011588874 40.22075494675638, -105.6639699494858 40.22073950563956, -105.6638033782239 40.22065749648416, -105.663644079153 40.22058103005954, -105.6635385751952 40.22048613622436, -105.6635385995102 40.22048598758672, -105.6635388206752 40.22048464173911, -105.6635459583738 40.22044129623704, -105.6635476333263 40.22043232723859, -105.663673564368 40.22034839813178, -105.6636823712486 40.22034252890084, -105.6636991629626 40.22034265464351, -105.6638131673268 40.22034350736083, -105.6638342814396 40.22034461134673, -105.66407395674 40.22035701730299, -105.6643249631576 40.22033462269664, -105.6643434378263 40.22033350759454, -105.6644807467734 40.22032595522565, -105.6644996202503 40.22032505838363, -105.664784009688 40.22031195569402, -105.6648041558022 40.22031213053535, -105.6650694737762 40.22031713167482, -105.665091824547 40.22032044650427, -105.665285107907 40.22035381967699, -105.6653082109339 40.22036160950015, -105.665453274059 40.22041584313852, -105.665476017825 40.22042613357929, -105.6656793835069 40.22052078736321, -105.666025019436 40.22065934213276, -105.6662109684469 40.22072644191363, -105.6665026809634 40.22079240572894, -105.6667602715467 40.22079269933909, -105.6670897912757 40.22075811984187, -105.6671100524527 40.2207586849872, -105.6675771648658 40.22078108328294, -105.6679161754167 40.22078667180477, -105.6679372613319 40.22078769222535, -105.6683273153827 40.22080907895852, -105.668349755364 40.22081223091617, -105.6686076023389 40.22085048682219, -105.6689434412469 40.22085470710499, -105.6689437513543 40.22085468143454, -105.6692620187301 40.22082685426683, -105.6692621514361 40.22082683155698, -105.6694877544554 40.22078559660721, -105.6697167316999 40.22070633274292, -105.670025529971 40.2205818739025, -105.6702602768931 40.22048289117972, -105.6704487179681 40.22038269732911, -105.6705318160145 40.22031142090378, -105.6706279297542 40.22020806563764, -105.6707634219981 40.22005296253833, -105.6709557580282 40.2198097498957, -105.6710802586927 40.2195102805907, -105.6711688587618 40.21926150827178, -105.6712223812788 40.21908071032284, -105.6712253346044 40.21907080716942, -105.6712666943526 40.21893789998065, -105.6712699602049 40.21892894021936, -105.6714498496281 40.21861495681172, -105.6715202551233 40.21847299480071, -105.671677961364 40.21823353650302, -105.6717915822289 40.21803192563492, -105.6718254444284 40.21785519677312, -105.6717553058992 40.21764151836187, -105.6717134573279 40.21753417629488, -105.6717077086626 40.21751735122088, -105.6716852102138 40.21736043335561, -105.6716834977097 40.21734524052872, -105.6716820255947 40.21698238032493, -105.6716342371114 40.21666497320453, -105.6716330510765 40.21665029385176, -105.6716974302847 40.21638855819683, -105.6716844886336 40.21617089596663, -105.6716031140915 40.21590230216545, -105.6715988975821 40.21588596024648, -105.6715868140986 40.21564834423229, -105.6715866363083 40.21563422447139, -105.671620006545 40.21537038231266, -105.6714720476905 40.21507356785254, -105.6713067369528 40.21484232290414, -105.6711008389497 40.21459721857093, -105.6708955791502 40.21438856038766, -105.6708818677844 40.2143719965027, -105.6707985907888 40.21404450838158, -105.6707963908123 40.21403062936756, -105.6710172976288 40.21375003597582, -105.6711798523966 40.21360484501722, -105.6713683785321 40.21343511289258, -105.6714650322431 40.21323580950317, -105.6715368673237 40.21305180125874, -105.6716108388324 40.21274444621527, -105.6716288543036 40.2124036293946, -105.6715814682046 40.21200177952105, -105.6714895341933 40.21156533862437, -105.671486455078 40.21154944621814, -105.6714344058856 40.21113793040745, -105.6714332596219 40.21112312849539, -105.6714547991578 40.21092602580006, -105.6714563055534 40.21091361022041, -105.6714980512335 40.21065270683239, -105.6715004847314 40.2106417939246, -105.6716179011028 40.21040545184155, -105.671664020672 40.21016743042685, -105.6716005492482 40.20992461097636, -105.6714341043355 40.20968414709365, -105.6714230068125 40.20966684897819, -105.6713526988938 40.20947998468864, -105.6712415442038 40.20922611109982, -105.6712343401312 40.20920897381667, -105.6711858342907 40.20906879448798, -105.671180227529 40.20905200698229, -105.6711120121573 40.20881812486911, -105.6711076268386 40.2088016985051, -105.6710679500579 40.20858059997141, -105.6710660945438 40.20856538390952, -105.6710951345212 40.20828515027478, -105.6710971069037 40.20827352295509, -105.6712490761915 40.20794918102887, -105.671252188425 40.20794333224706, -105.6714572507412 40.20776888574395, -105.671692983331 40.20760782260579, -105.671946837003 40.20746655576141, -105.6721096169302 40.20735484743265, -105.6723544287556 40.20722381706818, -105.6726600896722 40.20703938899105, -105.6728621527235 40.20688668559855, -105.6729976289071 40.20669015514054, -105.6730647160993 40.20644451025514, -105.6730678105499 40.20643499409206, -105.673206630464 40.20617431563913, -105.6733991767576 40.20599920259642, -105.6736513100163 40.20574410144964, -105.673799651054 40.20551870087024, -105.6739011514344 40.20534961296253, -105.6740954712419 40.20501136167052, -105.6742218988902 40.20476981641871, -105.674327059758 40.20462555292173, -105.6743913490012 40.20458955425074, -105.674406410934 40.20458814547064, -105.674457882481 40.20458362323701, -105.6744758279328 40.20458215786167, -105.6745819942282 40.20457132159748, -105.6747229798607 40.20452271252111, -105.6748448176996 40.20443287443803, -105.674994499918 40.20430770117226, -105.6751955721305 40.20415308938585, -105.6753971589113 40.20402163432263, -105.6756075566028 40.20390695053762, -105.6758225187993 40.20378210304028, -105.6760931932345 40.20362448291268, -105.6763292401676 40.20353687486897, -105.6763395737016 40.2035335024706, -105.6763396335542 40.2035334825655, -105.6766524176939 40.20343302824362, -105.6766648130916 40.20342984450046, -105.6769356120544 40.20336198784395, -105.6771745118465 40.20329083899474, -105.6774120088294 40.20319948890239, -105.6775459069634 40.20313382843321, -105.6778039324744 40.20302953190082, -105.6778152165018 40.20302631461814, -105.6780621159669 40.20295850286715, -105.6781938470535 40.20289104192163, -105.6782686189575 40.20277966302427, -105.6782330253896 40.20256177745768, -105.678146814832 40.20234917729157, -105.6780636463431 40.20218882324744, -105.6779048632146 40.20200063177179, -105.6778913430041 40.20198365230154, -105.6777848579481 40.20178683232973, -105.6777760633732 40.201769519553, -105.6776790023688 40.20151917503038, -105.6775820109331 40.20131543154896, -105.6774806636888 40.20113149318991, -105.677471925699 40.20111419741364, -105.6774135739281 40.20093048570482, -105.6774087103606 40.2009139179919, -105.6773746711299 40.20074969189098, -105.6773025737169 40.20067296439435, -105.6772870750698 40.20065833402217, -105.6772867405361 40.20065796437652, -105.6772855154855 40.20065661170868, -105.6772124247469 40.20057588058088, -105.6771303299135 40.20050091461442, -105.677110930098 40.20048379905398, -105.6769837093085 40.20036940590301, -105.6769828743263 40.20036854708027, -105.6769820711433 40.20036772153204, -105.6768967181972 40.20027993903021, -105.6768820765282 40.20026326826825, -105.6768159285832 40.20014339393698, -105.6768091210255 40.20012714709139, -105.6768556014762 40.19994812733729, -105.6768585909085 40.19993829059837, -105.67695172948 40.19973998451265, -105.676955236575 40.19973274799546, -105.6770774666019 40.19950071915762, -105.677191466394 40.19929860908254, -105.677309877271 40.19910291361013, -105.6774321865941 40.19887741471136, -105.6775502241474 40.19865534192194, -105.6776388836061 40.19850001203584, -105.6777664012934 40.19833084362219, -105.677859358288 40.19817902390867, -105.6779915239622 40.19802619180775, -105.6780673977488 40.19789303763628, -105.6780974597292 40.19781217787021, -105.678093610375 40.19765681352559, -105.6780492504934 40.19744129817882, -105.677985354926 40.19729188755628, -105.6779247261666 40.19718164024333, -105.6779174020624 40.19716501868773, -105.6779351602477 40.19701107739367, -105.6779372746921 40.1970000027021, -105.678004741952 40.19688982213197, -105.6780596499286 40.19671669514958, -105.678071926527 40.19656638369481, -105.6780735871556 40.19634390762809, -105.678074154487 40.19633047746711, -105.67810410177 40.19616573681866, -105.678122920101 40.19591730248069, -105.6781240986365 40.19590451082409, -105.6781697967753 40.19562028816761, -105.6781797409691 40.19534197737302, -105.6781803389271 40.19532859309427, -105.6781977556393 40.19513170030768, -105.6782070388807 40.19484594049832, -105.6782075650279 40.19483249508618, -105.6782244408778 40.19458256772621, -105.6782341424972 40.19434313834616, -105.6782347793217 40.19432980353974, -105.6782519002093 40.19410310032079, -105.6782529398048 40.19409019359268, -105.6782742489293 40.19386989909211, -105.6782875275536 40.19356417239761, -105.6782485732217 40.19336613348817, -105.6781494802977 40.19314990804275, -105.6781414339438 40.1931326985922, -105.6780370489998 40.19289911524799, -105.6780297956547 40.1928819919292, -105.6779584459529 40.19267161911222, -105.6779532208666 40.19265495198785, -105.6778824219966 40.19233396648192, -105.677879096605 40.19231799622053, -105.6778530901214 40.19216014855787, -105.6778259574849 40.19203372650452, -105.6778234235607 40.1920181666116, -105.6778331188409 40.19186483292374, -105.6778347578226 40.19185297810984, -105.6779274774696 40.19168121408297, -105.6780466278303 40.19153206643568, -105.6781600304808 40.19136463031327, -105.6781519689368 40.19109901984651, -105.6780483550102 40.19096721548783, -105.6780341644516 40.19095039284954, -105.6779374023908 40.19082985643251, -105.6779258125981 40.19081283344089, -105.6778831211533 40.19062535816793, -105.6778806803566 40.19060991791348, -105.6779063544293 40.19041914381376, -105.6779083317913 40.19040736953217, -105.677971367463 40.1901881086194, -105.6780090548469 40.18971784405401, -105.6779019323254 40.18925666184236, -105.677765546384 40.18893325343011, -105.6777584028516 40.18891617134472, -105.6776926608927 40.18874264792856, -105.6775924744353 40.18855230766899, -105.6774687696009 40.18834147264181, -105.6773329173417 40.18814377739658, -105.6773211596643 40.18812653754374, -105.6772256809055 40.18797639568763, -105.6770380712492 40.18774144196102, -105.6770246010461 40.1877244559753, -105.6768426188331 40.18747682323465, -105.6766742782837 40.18730812405553, -105.6765065596637 40.18717919733659, -105.6764839112511 40.18716219017327, -105.6764829605575 40.18716147652353, -105.6763959415487 40.18710202448237, -105.6763308014061 40.18705804967441, -105.6760992185649 40.18689566223739, -105.6759303858499 40.18679373368499, -105.6758363636698 40.18673768635443, -105.6755581622642 40.18657711774318, -105.6754319340273 40.18652047142681, -105.6753559905684 40.18648750826154, -105.6751336758973 40.18639575841871, -105.</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D21" t="n">
+        <v>29</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>Ward Private Home</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
         <is>
           <t>Ward private home</t>
         </is>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>40.0733984409928</v>
       </c>
-      <c r="K21" t="n">
+      <c r="L21" t="n">
         <v>-105.506518983446</v>
       </c>
-      <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr">
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr">
         <is>
           <t>POINT (-105.506518983446 40.0733984409928)</t>
         </is>

</xml_diff>

<commit_message>
Update from Judi's spreadsheet 1-21 noon
</commit_message>
<xml_diff>
--- a/data/supersites_geom_2024.xlsx
+++ b/data/supersites_geom_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,60 +446,70 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Venue</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>address</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>organization</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>website</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>google_map_link</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>google_map_name</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>lat</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>lon</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>google_map_url</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>website_url</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>location_geom</t>
         </is>
@@ -522,49 +532,55 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Allenspark Fire Station</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>14861 CO-7, Allenspark, CO 80510</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
         <is>
           <t>http://www.allensparkfire.com/</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Allenspark Fire Protection</t>
         </is>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>40.19712777610975</v>
       </c>
-      <c r="L2" t="n">
+      <c r="N2" t="n">
         <v>-105.5279141785934</v>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>http://www.allensparkfire.com/</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>POINT (-105.5279141785934 40.19712777610975)</t>
         </is>
@@ -587,53 +603,59 @@
       <c r="D3" t="n">
         <v>1</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>Altona MS</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>4600 Clover Basin Dr, Longmont, CO 80503</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>https://ams.svvsd.org/</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>Altona Middle School</t>
         </is>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>40.14448266991539</v>
       </c>
-      <c r="L3" t="n">
+      <c r="N3" t="n">
         <v>-105.1626179175455</v>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>https://ams.svvsd.org/</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>POINT (-105.1626179175455 40.14448266991539)</t>
         </is>
@@ -656,53 +678,59 @@
       <c r="D4" t="n">
         <v>4</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>Burlington Elementary</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>1051 S Pratt Pkwy, Longmont, CO 80501</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>http://bes.svvsd.org/</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Burlington Elementary School</t>
         </is>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>40.1466539913149</v>
       </c>
-      <c r="L4" t="n">
+      <c r="N4" t="n">
         <v>-105.108633248163</v>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>http://bes.svvsd.org/</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>POINT (-105.108633248163 40.1466539913149)</t>
         </is>
@@ -725,53 +753,59 @@
       <c r="D5" t="n">
         <v>5</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>Casey MS</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>1301 High St, Boulder, CO 80304</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>http://cam.bvsd.org/</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>Casey Middle School</t>
         </is>
       </c>
-      <c r="K5" t="n">
+      <c r="M5" t="n">
         <v>40.0228711759357</v>
       </c>
-      <c r="L5" t="n">
+      <c r="N5" t="n">
         <v>-105.2791579470394</v>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>http://cam.bvsd.org/</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>POINT (-105.2791579470394 40.0228711759357)</t>
         </is>
@@ -794,53 +828,59 @@
       <c r="D6" t="n">
         <v>6</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" t="n">
+        <v>6</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Centaurus HS</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>10300 W South Boulder Rd, Lafayette, CO 80026</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>http://ceh.bvsd.org/</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>Centaurus High School</t>
         </is>
       </c>
-      <c r="K6" t="n">
+      <c r="M6" t="n">
         <v>39.98635981263706</v>
       </c>
-      <c r="L6" t="n">
+      <c r="N6" t="n">
         <v>-105.1125276640655</v>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>http://ceh.bvsd.org/</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>POINT (-105.1125276640655 39.98635981263706)</t>
         </is>
@@ -863,53 +903,59 @@
       <c r="D7" t="n">
         <v>7</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" t="n">
+        <v>7</v>
+      </c>
+      <c r="F7" t="n">
+        <v>7</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>Centennial MS</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>2205 Norwood Ave, Boulder, CO 80304</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>http://cem.bvsd.org/</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>Centennial Middle School</t>
         </is>
       </c>
-      <c r="K7" t="n">
+      <c r="M7" t="n">
         <v>40.04506796264024</v>
       </c>
-      <c r="L7" t="n">
+      <c r="N7" t="n">
         <v>-105.2671472290834</v>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>http://cem.bvsd.org/</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>POINT (-105.2671472290834 40.04506796264024)</t>
         </is>
@@ -932,53 +978,59 @@
       <c r="D8" t="n">
         <v>8</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>Eldorado K8</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>3351 S Indiana St, Superior, CO 80027</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>http://el8.bvsd.org/</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>Eldorado K-8 School</t>
         </is>
       </c>
-      <c r="K8" t="n">
+      <c r="M8" t="n">
         <v>39.921698179021</v>
       </c>
-      <c r="L8" t="n">
+      <c r="N8" t="n">
         <v>-105.161197194222</v>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="O8" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>http://el8.bvsd.org/</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>POINT (-105.161197194222 39.921698179021)</t>
         </is>
@@ -1001,53 +1053,59 @@
       <c r="D9" t="n">
         <v>10</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>Erie MS</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>650 Main St, Erie, CO 80516</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>https://ems.svvsd.org/</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>Erie Middle School</t>
         </is>
       </c>
-      <c r="K9" t="n">
+      <c r="M9" t="n">
         <v>40.05101707648438</v>
       </c>
-      <c r="L9" t="n">
+      <c r="N9" t="n">
         <v>-105.0529688258069</v>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>https://ems.svvsd.org/</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>POINT (-105.0529688258069 40.05101707648438)</t>
         </is>
@@ -1070,53 +1128,59 @@
       <c r="D10" t="n">
         <v>12</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" t="n">
+        <v>12</v>
+      </c>
+      <c r="F10" t="n">
+        <v>12</v>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>Gold Hill School</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>890 Main St, Boulder, CO 80302</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>http://ghe.bvsd.org/</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>Gold Hill Elementary School</t>
         </is>
       </c>
-      <c r="K10" t="n">
+      <c r="M10" t="n">
         <v>40.063366273762</v>
       </c>
-      <c r="L10" t="n">
+      <c r="N10" t="n">
         <v>-105.412472825461</v>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="O10" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>http://ghe.bvsd.org/</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>POINT (-105.412472825461 40.063366273762)</t>
         </is>
@@ -1139,53 +1203,59 @@
       <c r="D11" t="n">
         <v>14</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" t="n">
+        <v>14</v>
+      </c>
+      <c r="F11" t="n">
+        <v>14</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>Jamestown School</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>111 Mesa St, Jamestown, CO 80455</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>http://jae.bvsd.org/</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>Jamestown Elementary School</t>
         </is>
       </c>
-      <c r="K11" t="n">
+      <c r="M11" t="n">
         <v>40.1164318137431</v>
       </c>
-      <c r="L11" t="n">
+      <c r="N11" t="n">
         <v>-105.387802261192</v>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>http://jae.bvsd.org/</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>POINT (-105.387802261192 40.1164318137431)</t>
         </is>
@@ -1208,53 +1278,59 @@
       <c r="D12" t="n">
         <v>15</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" t="n">
+        <v>15</v>
+      </c>
+      <c r="F12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>Longs Peak MS</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>1500 14th Ave, Longmont, CO 80501</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>http://lpms.svvsd.org/</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>Longs Peak Middle School</t>
         </is>
       </c>
-      <c r="K12" t="n">
+      <c r="M12" t="n">
         <v>40.18399195721774</v>
       </c>
-      <c r="L12" t="n">
+      <c r="N12" t="n">
         <v>-105.117518880356</v>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="O12" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>http://lpms.svvsd.org/</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>POINT (-105.117518880356 40.18399195721774)</t>
         </is>
@@ -1277,53 +1353,59 @@
       <c r="D13" t="n">
         <v>17</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" t="n">
+        <v>17</v>
+      </c>
+      <c r="F13" t="n">
+        <v>17</v>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>Lyons Middle Senior</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>100 McConnell Dr, Lyons, CO 80540</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>https://lmshs.svvsd.org/</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>Lyons Middle/Senior High School</t>
         </is>
       </c>
-      <c r="K13" t="n">
+      <c r="M13" t="n">
         <v>40.2147599852984</v>
       </c>
-      <c r="L13" t="n">
+      <c r="N13" t="n">
         <v>-105.264461148759</v>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="O13" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>https://lmshs.svvsd.org/</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>POINT (-105.264461148759 40.2147599852984)</t>
         </is>
@@ -1346,53 +1428,59 @@
       <c r="D14" t="n">
         <v>18</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" t="n">
+        <v>18</v>
+      </c>
+      <c r="F14" t="n">
+        <v>18</v>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>Manhattan MS</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>290 Manhattan Dr, Boulder, CO 80303</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>http://mam.bvsd.org/</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>Manhattan Middle School of Arts and Academics</t>
         </is>
       </c>
-      <c r="K14" t="n">
+      <c r="M14" t="n">
         <v>39.99410342530379</v>
       </c>
-      <c r="L14" t="n">
+      <c r="N14" t="n">
         <v>-105.2273572175253</v>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="O14" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
         </is>
       </c>
-      <c r="N14" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>http://mam.bvsd.org/</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>POINT (-105.2273572175253 39.99410342530379)</t>
         </is>
@@ -1415,53 +1503,59 @@
       <c r="D15" t="n">
         <v>19</v>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" t="n">
+        <v>19</v>
+      </c>
+      <c r="F15" t="n">
+        <v>19</v>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>Monarch HS</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>329 Campus Dr, Louisville, CO 80027</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>http://moh.bvsd.org/</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>Monarch High School</t>
         </is>
       </c>
-      <c r="K15" t="n">
+      <c r="M15" t="n">
         <v>39.9520220573069</v>
       </c>
-      <c r="L15" t="n">
+      <c r="N15" t="n">
         <v>-105.141776992356</v>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>http://moh.bvsd.org/</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>POINT (-105.141776992356 39.9520220573069)</t>
         </is>
@@ -1484,53 +1578,59 @@
       <c r="D16" t="n">
         <v>21</v>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E16" t="n">
+        <v>21</v>
+      </c>
+      <c r="F16" t="n">
+        <v>21</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>Nederland HS</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>597 Co Hwy 130, Nederland, CO 80466</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>https://neh.bvsd.org/</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>Nederland Middle/Senior High School</t>
         </is>
       </c>
-      <c r="K16" t="n">
+      <c r="M16" t="n">
         <v>39.95383849383303</v>
       </c>
-      <c r="L16" t="n">
+      <c r="N16" t="n">
         <v>-105.5233421126253</v>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="O16" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>https://neh.bvsd.org/</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>POINT (-105.5233421126253 39.95383849383303)</t>
         </is>
@@ -1553,45 +1653,51 @@
       <c r="D17" t="n">
         <v>22</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E17" t="n">
+        <v>22</v>
+      </c>
+      <c r="F17" t="n">
+        <v>22</v>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>New Vista</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>700 20th St, Boulder, CO 80302</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>http://nvh.bvsd.org/</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/mVZ7Cv3jx5iSPW3u9</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>New Vista High School</t>
         </is>
       </c>
-      <c r="K17" t="n">
+      <c r="M17" t="n">
         <v>40.0011978462681</v>
       </c>
-      <c r="L17" t="n">
+      <c r="N17" t="n">
         <v>-105.266504379284</v>
       </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr">
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr">
         <is>
           <t>POINT (-105.266504379284 40.0011978462681)</t>
         </is>
@@ -1614,53 +1720,59 @@
       <c r="D18" t="n">
         <v>23</v>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="E18" t="n">
+        <v>23</v>
+      </c>
+      <c r="F18" t="n">
+        <v>23</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>Niwot HS</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>8989 Niwot Rd, Niwot, CO 80503</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>https://nhs.svvsd.org/</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>Niwot High School</t>
         </is>
       </c>
-      <c r="K18" t="n">
+      <c r="M18" t="n">
         <v>40.10369506217272</v>
       </c>
-      <c r="L18" t="n">
+      <c r="N18" t="n">
         <v>-105.1442414652976</v>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="O18" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr">
+      <c r="P18" t="inlineStr">
         <is>
           <t>https://nhs.svvsd.org/</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
+      <c r="Q18" t="inlineStr">
         <is>
           <t>POINT (-105.1442414652976 40.10369506217272)</t>
         </is>
@@ -1683,53 +1795,59 @@
       <c r="D19" t="n">
         <v>25</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E19" t="n">
+        <v>25</v>
+      </c>
+      <c r="F19" t="n">
+        <v>25</v>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>Southern Hills MS</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>1500 Knox Dr, Boulder, CO 80305</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>http://shm.bvsd.org/</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="L19" t="inlineStr">
         <is>
           <t>Southern Hills Middle School</t>
         </is>
       </c>
-      <c r="K19" t="n">
+      <c r="M19" t="n">
         <v>39.97413389369987</v>
       </c>
-      <c r="L19" t="n">
+      <c r="N19" t="n">
         <v>-105.2452260530946</v>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="O19" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr">
+      <c r="P19" t="inlineStr">
         <is>
           <t>http://shm.bvsd.org/</t>
         </is>
       </c>
-      <c r="O19" t="inlineStr">
+      <c r="Q19" t="inlineStr">
         <is>
           <t>POINT (-105.2452260530946 39.97413389369987)</t>
         </is>
@@ -1752,53 +1870,59 @@
       <c r="D20" t="n">
         <v>28</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E20" t="n">
+        <v>28</v>
+      </c>
+      <c r="F20" t="n">
+        <v>28</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>Trail Ridge MS</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>1000 Button Rock Dr, Longmont, CO 80504</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>https://trms.svvsd.org/</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>Trail Ridge Middle School</t>
         </is>
       </c>
-      <c r="K20" t="n">
+      <c r="M20" t="n">
         <v>40.17693117783666</v>
       </c>
-      <c r="L20" t="n">
+      <c r="N20" t="n">
         <v>-105.0576162268638</v>
       </c>
-      <c r="M20" t="inlineStr">
+      <c r="O20" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
         </is>
       </c>
-      <c r="N20" t="inlineStr">
+      <c r="P20" t="inlineStr">
         <is>
           <t>https://trms.svvsd.org/</t>
         </is>
       </c>
-      <c r="O20" t="inlineStr">
+      <c r="Q20" t="inlineStr">
         <is>
           <t>POINT (-105.0576162268638 40.17693117783666)</t>
         </is>
@@ -1810,7 +1934,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Ward Private Home</t>
+          <t>Ward Community Center</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1818,36 +1942,20 @@
           <t>POLYGON ((-105.4661484313311 40.16510540791135, -105.46628891067 40.16510477709761, -105.470815740543 40.16518143398583, -105.4708146541582 40.16519354991458, -105.4707617910061 40.16578360363307, -105.4707617862852 40.16578366217297, -105.4705125686798 40.16856524699041, -105.4704672528061 40.1690710003927, -105.4704561694049 40.16919470380456, -105.4704014266738 40.1698729832864, -105.4703235422809 40.17083798352486, -105.4701471120568 40.17302390050776, -105.470147089627 40.17302417969756, -105.4701398981323 40.17311326375602, -105.4701498775658 40.17311351851009, -105.470200732758 40.17311482223527, -105.470709432716 40.1731278654992, -105.4711861857428 40.17314008889846, -105.471439289043 40.1731465768118, -105.4727391684574 40.17317988978623, -105.4749708600473 40.17323704782745, -105.4750032321987 40.1726821562563, -105.4750206722191 40.17238323337168, -105.4750210361202 40.17237698847438, -105.4752042504024 40.16923656802826, -105.479787691759 40.16935887360058, -105.4797873653326 40.16937091048318, -105.4797734359278 40.16988387259018, -105.4797733872597 40.16988566754004, -105.4796805373642 40.17330482726621, -105.4796240684069 40.17656529689094, -105.4796152483834 40.17796396985926, -105.4796026937846 40.17995501780022, -105.479611783183 40.17995483837693, -105.4809046495147 40.17992930563622, -105.4809104417855 40.17992919131213, -105.4821456944617 40.17990478346833, -105.4842904768209 40.17986236891954, -105.4842904845098 40.17987483273979, -105.4842905938626 40.18005209836011, -105.484290852698 40.18047691385383, -105.4842909836418 40.18069288673419, -105.4842919357208 40.18225457717938, -105.4842923359611 40.18291119120383, -105.4842927315417 40.18355750826427, -105.4843017355777 40.18355781209871, -105.4858596675139 40.18361035232417, -105.4887108236855 40.18370645233315, -105.4890342964373 40.18371735136233, -105.4913673103303 40.18380308278645, -105.4916169415424 40.18381225335324, -105.493803003558 40.18389564358236, -105.4938093397902 40.1838958852905, -105.4938123200268 40.18389599982997, -105.4938523169958 40.18035330559622, -105.4938523205461 40.18035299938223, -105.4942081234937 40.18036470973328, -105.4942254027887 40.18036558420872, -105.4988689323545 40.18060051532034, -105.5037971648563 40.18084965648772, -105.5066788071574 40.18091382279687, -105.5115988430433 40.18102320894966, -105.5138093385616 40.18107228813918, -105.5207705453987 40.18122672640443, -105.5208006874244 40.18122739465633, -105.522236754261 40.18127360796668, -105.5222435283211 40.18127382641728, -105.5222435741154 40.18127382730909, -105.522435320304 40.18127999739902, -105.5224377955276 40.18127643582816, -105.5224378823772 40.18127630972313, -105.523680357985 40.181292988343, -105.523688178229 40.1812930930153, -105.5236896753479 40.18129311342297, -105.5237041709683 40.18072051517435, -105.5237197330747 40.18010577977868, -105.5237413580885 40.17925150068127, -105.5237454789506 40.17908870192743, -105.5237510683669 40.17886786445666, -105.5237651645466 40.17831101269118, -105.5237857437776 40.17749800315436, -105.5238776530766 40.17387231186575, -105.5258247721261 40.17387231837259, -105.5258340931253 40.17387231809113, -105.5332652858553 40.17387203873018, -105.5332746068535 40.17387203604751, -105.5332742031089 40.1738843189681, -105.5331893193217 40.17646799626176, -105.5331568626344 40.17752450998029, -105.5331662580995 40.17752449827886, -105.5332269975165 40.17752442499798, -105.5332266806333 40.17753671869425, -105.5331269808046 40.18141083850799, -105.5330262556054 40.1837602446121, -105.532976230018 40.18492700366666, -105.5328963810823 40.18678931519381, -105.5328252778692 40.18844755645122, -105.5328252743849 40.18844763660821, -105.5328144473783 40.1887670954498, -105.5328026033848 40.18959315645375, -105.5327760272405 40.19144611821562, -105.5327628767569 40.19236313910528, -105.5327720701403 40.19236356970227, -105.5328092241853 40.19236530368316, -105.5328090737093 40.1923771568957, -105.5328019262174 40.19293933922767, -105.5328018956497 40.19294170518686, -105.5328006690869 40.1930380970772, -105.5328098787648 40.19303559882346, -105.5328294254024 40.19303029578, -105.5328935660998 40.19301413198865, -105.5329570730651 40.19299410915016, -105.5330083598834 40.19297567307023, -105.5330790606768 40.1929545853694, -105.5331549173888 40.1929269242624, -105.5332445784334 40.19289053114875, -105.5333357318797 40.19285139332066, -105.5334323856855 40.19282329373202, -105.5335304733625 40.19279520175227, -105.5336091149603 40.19277140683688, -105.5336459058447 40.19275785969391, -105.5336515583924 40.19275577849825, -105.533684251341 40.19274374108799, -105.5337565232855 40.19271606081569, -105.5338179414305 40.19269327228345, -105.533890165039 40.19266779307718, -105.5339501238616 40.19264610006633, -105.5340122329798 40.19262441809995, -105.5341047369489 40.19258913845898, -105.5341957862916 40.19255495433799, -105.5342200411473 40.19254790514945, -105.5342198678148 40.19256285923371, -105.5342193376537 40.19260852935302, -105.5342183473157 40.19269425235101, -105.5342183360385 40.19269518000148, -105.5342180715312 40.19271798939261, -105.5342271532779 40.19272517011618, -105.5343393829121 40.19281390637015, -105.5346356497051 40.19259680260618, -105.5348823209668 40.19251699672893, -105.5349371865247 40.19249180670148, -105.5349909777208 40.19246710871604, -105.537495561658 40.19258391871914, -105.5375025897888 40.19185229996346, -105.5375101454505 40.19106602720946, -105.5375433224156 40.1910399954814, -105.5375224677095 40.18937951494874, -105.5375223216064 40.1893679950532, -105.5372715249519 40.18934647278628, -105.537254321171 40.18934499589563, -105.5375677880135 40.18893092853408, -105.5375946466315 40.18889544853639, -105.541762862168 40.1891617345586, -105.5422569890588 40.18918897106952, -105.5422571009006 40.18920076026023, -105.5422758519701 40.1911640951709, -105.5422833975333 40.19195391480071, -105.5422833975938 40.19195401206859, -105.542297092536 40.19338773536003, -105.5422970925746 40.19338779750338, -105.5423024628827 40.19394992984792, -105.5423929265994 40.20341858732859, -105.542401834668 40.20341858226157, -105.5424019515685 40.20343087127191, -105.5471617411033 40.203428251832, -105.5471710649767 40.20342824622806, -105.5471762500321 40.20702449927905, -105.5471669256137 40.20702443013139, -105.5469038813974 40.20702247197197, -105.5423441045886 40.20698842150102, -105.5423441034594 40.20698849445215, -105.5422953313193 40.21055420708196, -105.5422860075863 40.21055412132916, -105.5404398525206 40.21053711938241, -105.5326909158406 40.21046358966055, -105.5326905760758 40.21136204136256, -105.5326905761208 40.21136213502758, -105.5326902668153 40.21217981128849, -105.5326894995797 40.21419262998702, -105.5326895026425 40.21419411331591, -105.5326985284376 40.21419413237972, -105.5422526119581 40.21421377049138, -105.5422524668593 40.21422603345813, -105.5422084115658 40.21794388539156, -105.5411373910101 40.21826779544625, -105.5398831425591 40.21944693342513, -105.5379809748795 40.21961963612427, -105.5379291219123 40.21962350240685, -105.5378566567431 40.21962890467403, -105.5364658151693 40.21975515971221, -105.5364659849748 40.21975632326548, -105.536469145231 40.2197779543675, -105.5364610049816 40.21977874858243, -105.5360297782496 40.21982080776719, -105.5360049453737 40.2214518136923, -105.5348769137664 40.22144872610919, -105.5338911592008 40.22144602273305, -105.5333207578963 40.22144445293673, -105.5326849358092 40.22144269979285, -105.5326849473221 40.2214446523428, -105.5326967674883 40.2233561262393, -105.5326825303639 40.22418840574673, -105.5326820404199 40.22504857987344, -105.5326910735317 40.22504859983672, -105.5344553890728 40.22505242161549, -105.5353538558136 40.22505402382836, -105.5360637775385 40.22505528352068, -105.5364251454815 40.22505592322528, -105.5364318357178 40.22505593462795, -105.536760204845 40.22505651522585, -105.5373800222655 40.2250576054056, -105.5374809703504 40.2250577834895, -105.5385255461858 40.22505961624928, -105.5405764553367 40.22506318763808, -105.5419484417806 40.22506555326001, -105.5419590751946 40.22506557191936, -105.5420808495041 40.22506765406047, -105.5420823229212 40.22506767874194, -105.5420822364319 40.22507980477056, -105.5420562713165 40.22872637531357, -105.542057627296 40.22872637662191, -105.5420429039838 40.2322667322377, -105.5418212665354 40.24069807142973, -105.5417703294095 40.24320999597101, -105.5417913293522 40.24484599488542, -105.5418693303538 40.25068399588682, -105.5419533310875 40.25691899504218, -105.5420123310872 40.26132699564431, -105.5420510583876 40.26143505394957, -105.5420511054112 40.26143505393247, -105.5420601092523 40.26143504165487, -105.546896776124 40.26142835486699, -105.5469164731246 40.26142832707124, -105.5488073098715 40.26142565841789, -105.5516765188264 40.26142154904153, -105.5516962275788 40.26142152042718, -105.5564490412647 40.26141455566594, -105.5564687629445 40.26141452623263, -105.5591675481954 40.26141048439985, -105.559187278102 40.26141045449919, -105.5591940095238 40.26141044475258, -105.5610087103939 40.26140744097114, -105.5795558249904 40.26109930837292, -105.5795753264785 40.2610990572043, -105.5951059878192 40.26090826365041, -105.5951255644495 40.26090802240864, -105.5978803250462 40.26087396174936, -105.5978999087103 40.26087372003241, -105.5990498899888 40.26085948275252, -105.5990694865891 40.26085924983279, -105.5995397909104 40.26085370200565, -105.5995593945634 40.26085347079817, -105.6024803232683 40.26081898919289, -105.6142594281275 40.26067918769429, -105.6159287966142 40.26065927760523, -105.6159484448253 40.26065904267666, -105.6183738399164 40.26063000678786, -105.6183934869193 40.2606297624392, -105.6213214042607 40.26059298525797, -105.6213410559414 40.26059273860285, -105.6230240548107 40.26057156630034, -105.6230437100057 40.26057131935239, -105.6277277549875 40.26051225854213, -105.627747425429 40.26051200987794, -105.632275471989 40.26045473382353, -105.6322951553285 40.26045448437176, -105.6333595672079 40.26044099555356, -105.6333792540661 40.26044074591335, -105.6336239250111 40.26043764207176, -105.6336436106918 40.26043739238794, -105.6344099544128 40.26042767444419, -105.6344296424389 40.26042742462398, -105.6344533637605 40.26042712418371, -105.6344730517862 40.26042687435609, -105.6370401114326 40.26039427547199, -105.6370598053172 40.2603940251974, -105.641661457955 40.26033544727563, -105.6416811682616 40.26033519529398, -105.6421922091127 40.26032867946999, -105.6422119170661 40.2603284283015, -105.6463212330816 40.26027594287727, -105.6463409574624 40.26027569098492, -105.6510511032203 40.26021535336445, -105.6510708369704 40.26021510065377, -105.653220247745 40.26018750197031, -105.6534108731882 40.2601810802276, -105.6533823627512 40.26010275780921, -105.6532830172156 40.25994882313275, -105.6532015168119 40.259833817446, -105.6530755380744 40.25970888806435, -105.653056450447 40.25969061631895, -105.6528639596007 40.25950741268624, -105.6526889307466 40.2593871624231, -105.652642514434 40.25935601447338, -105.6524271025182 40.25918859577206, -105.652112632482 40.25892918790828, -105.6518414912158 40.25866632340869, -105.6518412163808 40.2586659058817, -105.6518402220181 40.25866439414499, -105.6518249196642 40.25864111788805, -105.651683174363 40.25842552064559, -105.6516722710576 40.25840806831427, -105.6515514218632 40.25817243805065, -105.6515429003808 40.25815503662493, -105.6514243241588 40.25786656297638, -105.6514187228448 40.25784972511072, -105.6514055789766 40.25757162818682, -105.6513344204328 40.25729383767664, -105.6513306212376 40.25727751710651, -105.6512928566423 40.25697723763877, -105.6512494136496 40.25670131742907, -105.6512475526345 40.25668592286098, -105.6512481806062 40.25659521519253, -105.6512491443465 40.25645626717135, -105.6512492414307 40.25644232184331, -105.651250394949 40.25627562546527, -105.6512238153397 40.25580599850561, -105.6512233117349 40.25579151809188, -105.6512386810696 40.2554038107325, -105.6512392740317 40.25539031326282, -105.6512547967072 40.25511750050543, -105.651254798984 40.25511746717952, -105.6512556523308 40.25510424315733, -105.6512679930778 40.25496298995328, -105.651283544426 40.25478497372899, -105.6512465313483 40.25451425149574, -105.6510657606499 40.25415446368373, -105.651056843717 40.25413708614312, -105.6508969847668 40.25382258276831, -105.6505310873636 40.2534957431415, -105.6505198035114 40.25348589422141, -105.650277580469 40.25334159185142, -105.6502158172845 40.25330586876338, -105.6497508549943 40.25305330688136, -105.6493031225032 40.25278747457062, -105.6489024621259 40.25250204640531, -105.6485320184643 40.25224942820618, -105.648122926153 40.25197372674319, -105.6478519627375 40.25176733123399, -105.647595323896 40.2516000866161, -105.6474810359026 40.2515261922803, -105.6473040944805 40.25143101667013, -105.6471837932539 40.25136724816764, -105.6468534777815 40.25120486346038, -105.6466993803544 40.25114202354365, -105.6465010494459 40.25106199343578, -105.6463131316636 40.25101511518552, -105.6461854347542 40.25098444290174, -105.6459617149985 40.25091212623183, -105.645862718699 40.25086625543839, -105.6439109359637 40.24997257845546, -105.6439113906358 40.24997248152362, -105.6440326178304 40.24994670984607, -105.6460486209198 40.24951810932338, -105.6461040002026 40.24950599091284, -105.6461040377955 40.24950598185919, -105.6461837138841 40.24948586944218, -105.6461837538199 40.24948585678304, -105.6462761693258 40.24945621494909, -105.6462878338384 40.24945293635419, -105.6465034720074 40.2493933900957, -105.6465165544287 40.24939030511742, -105.6468338582291 40.24931722103709, -105.6468479730201 40.24931432744434, -105.6473447774411 40.24921444122509, -105.6473620074362 40.24921285670883, -105.6478251640483 40.24917729760249, -105.6478451563986 40.24917744047953, -105.6483876106674 40.24918924142482, -105.6484084764347 40.24918997028969, -105.6490580710522 40.24921440685837, -105.6490793598224 40.24921560338041, -105.6496621472309 40.24925061573745, -105.649857509743 40.24926235109255, -105.6498792923866 40.24926416375346, -105.6504807419691 40.24931712691847, -105.6505029278615 40.24931949642218, -105.6510873439726 40.249384258711, -105.6510876331863 40.24938428985514, -105.6517955093473 40.24946011446387, -105.6524384646635 40.24946103545784, -105.6532240381383 40.24939543248849, -105.6532429858952 40.24939464187201, -105.6540359245012 40.24936764317474, -105.6540561108867 40.24936779732936, -105.6547920954059 40.24937937171175, -105.6548135707898 40.24938089655689, -105.6553635528423 40.24942562557963, -105.6560772134397 40.2494691280667, -105.6560990989358 40.2494710970272, -105.6566697271875 40.24952454693272, -105.6572882420254 40.24953298344785, -105.6572884124538 40.2495329823156, -105.6577466825842 40.24952787256891, -105.6577468823637 40.24952785698604, -105.658364554839 40.24947889500469, -105.6583837733506 40.24947829771016, -105.658383836817 40.24947829582203, -105.6588610698823 40.24946552024045, -105.6593578213218 40.24936558880857, -105.6596740517714 40.24922577817019, -105.6598284918649 40.24908374683517, -105.6600357955445 40.24885510058633, -105.6601709350914 40.24869839282666, -105.6602180098776 40.24847606239258, -105.6602904669786 40.24808708989965, -105.6603197434563 40.24775706340495, -105.6603209213945 40.24774420990298, -105.6603381955352 40.24758479666077, -105.6603395938818 40.24757220763556, -105.6603473707779 40.24750678741342, -105.6603488540162 40.24749431264927, -105.6603658886433 40.24735099924052, -105.6603676534624 40.2473388122845, -105.6604413607002 40.24701574268065, -105.6604416576382 40.2466576694766, -105.660406673147 40.24625862093598, -105.6604060936211 40.24624414514405, -105.6604638791043 40.2458376972433, -105.6604423228038 40.24554413969873, -105.6604183656476 40.24532331789342, -105.6604176166594 40.24530874776879, -105.6604654929911 40.24502852130396, -105.6604680799253 40.24501810382434, -105.6606031082612 40.24480953958241, -105.6608380761308 40.24465551037683, -105.661090919282 40.24451736259382, -105.6614394345306 40.24425372862866, -105.6617972409519 40.24400229844849, -105.661993737268 40.24379598909656, -105.6622515148447 40.24354079687833, -105.6623638976777 40.24339320647818, -105.6623412545372 40.243148140186, -105.6622271542483 40.24289913312061, -105.6622212185086 40.24288262853066, -105.662246928383 40.24270330468485, -105.6622493009619 40.24269235519348, -105.6624203867668 40.24238932411787, -105.6626383198902 40.24217056212871, -105.6627478603099 40.2420858297572, -105.6628966257281 40.24188143849485, -105.6630035083658 40.2416272908031, -105.6630070175849 40.24161941982204, -105.6631343254574 40.24137469705771, -105.6632915945943 40.24121971764026, -105.6634577117512 40.24103557054804, -105.6636414775772 40.24080598165017, -105.6638605888681 40.24047958579609, -105.6641361334141 40.24008308784516, -105.6643937880334 40.23986345373206, -105.6646430665669 40.23956239662796, -105.6647837931359 40.23929073503575, -105.6649769754472 40.23895438237981, -105.6651788634559 40.23861149463966, -105.665323466031 40.23835513830205, -105.6653962474659 40.23809944644505, -105.665431211319 40.23766674878126, -105.6654329294115 40.23765467076841, -105.6655795293855 40.23730339632174, -105.6656516849346 40.23700392224806, -105.6655733758443 40.23677124300807, -105.6654192999047 40.23653663304073, -105.6652664880635 40.23634685679159, -105.6651081521364 40.23616363214872, -105.6650945635468 40.23614659102824, -105.6649503217293 40.23588669668948, -105.6649408301455 40.23586931017438, -105.6648173713558 40.23562903403352, -105.6648096253163 40.23561180533154, -105.6647862204469 40.23550442489909, -105.6647251887129 40.23522442147496, -105.6647251756337 40.23522435844993, -105.6646582848182 40.23494468934514, -105.6646546756029 40.23492852738642, -105.6645951132258 40.23457015220544, -105.6645927169959 40.23455456581809, -105.6645619404331 40.23428038048088, -105.6645609881937 40.23426566023956, -105.6646107631039 40.23381407701542, -105.6646123901615 40.23380175146494, -105.6646686018296 40.23352436399449, -105.6646712989217 40.23351378322931, -105.6648220164282 40.23318151580031, -105.6648255241641 40.23317475342208, -105.6650047084142 40.2329491006681, -105.6651964929561 40.2327528359099, -105.6654011529644 40.23258888212007, -105.6657063539013 40.23236997563181, -105.6659413331565 40.23217075944036, -105.6661675652812 40.23202312776482, -105.6663889616327 40.23191128709515, -105.6666810970455 40.23171510873143, -105.6666926686825 40.23171249465987, -105.6670132530934 40.23164008776747, -105.6670310503309 40.23163893539422, -105.6670310985044 40.23163893352346, -105.6671542201482 40.23163200282799, -105.6671543176415 40.23163198737654, -105.6673891053773 40.23159393428879, -105.6675672799185 40.23153819341664, -105.6677025916841 40.23133320802084, -105.6677681890939 40.23097816878754, -105.6677631503988 40.23075299479768, -105.6677483196333 40.23044769834121, -105.6677481743348 40.23043358126473, -105.6677741899327 40.2302316910987, -105.6677764100459 40.23022044448404, -105.6678022827057 40.23016966127873, -105.6679082388013 40.22996248731734, -105.6680695015121 40.2297791769222, -105.6682133000139 40.22966333765718, -105.6684010177816 40.22951487491294, -105.6685625454325 40.22935359900887, -105.6687415781404 40.22916824706451, -105.6688267008086 40.22894056836384, -105.6688429479812 40.22873624245703, -105.6688205696722 40.22852339716228, -105.6687613011443 40.22838176133099, -105.6686730393414 40.22821884274862, -105.6685174411165 40.22801933434805, -105.6683511792286 40.22783588408025, -105.6683375401028 40.22781896947912, -105.6682470624096 40.22761127111529, -105.6682416637716 40.22759486778096, -105.6682721112314 40.22737017614368, -105.6682739650483 40.22735817442233, -105.6683029921154 40.22722332576805, -105.6683058044111 40.2272130959819, -105.6683934966554 40.22704599071793, -105.6685196675831 40.22692074262096, -105.6687379630553 40.22675606758625, -105.6689083831121 40.22657508868081, -105.6690438599216 40.22640284891151, -105.6690758537972 40.22632072549793, -105.6690792556187 40.22631231949595, -105.6691903428408 40.22606427355334, -105.6692787329387 40.22583821434375, -105.6693278820078 40.22567399448331, -105.6693861052922 40.22544429847117, -105.669440759808 40.22514343033741, -105.66945233353 40.2249046090048, -105.6694532890332 40.22489151701731, -105.6694919852029 40.22466959399863, -105.6694915482502 40.22436290200361, -105.6693372707889 40.22410474212811, -105.6691337832986 40.22385606282835, -105.6689801460077 40.22368898447323, -105.6688367933033 40.22358134839062, -105.668820995009 40.22356996322452, -105.6686399339946 40.22346121020597, -105.66857070503 40.22342023718163, -105.6684063343704 40.22334358118142, -105.6683101888107 40.22329963458959, -105.6680685904649 40.22318068359311, -105.6678529537799 40.22304919374229, -105.6676002381706 40.22290378130718, -105.6674823272445 40.22284463958258, -105.6673437859818 40.22277593321919, -105.6672358734293 40.22272320634443, -105.6669856426672 40.22260732588539, -105.6667614982625 40.22246269083642, -105.6664857475077 40.222278601177, -105.6662919082906 40.22213095583463, -105.6661158510701 40.22201122023689, -105.6660285158423 40.22195229519745, -105.6659311617552 40.22189506412996, -105.6658563941644 40.22185175849506, -105.6656409412277 40.2217135933068, -105.6654520699702 40.22157582560256, -105.6653094536946 40.22148618217604, -105.6652393815789 40.22144276315675, -105.665179073635 40.2214088029338, -105.6650717714665 40.22134893480318, -105.6648732975747 40.22122908068761, -105.664797561422 40.22118791743397, -105.6646748951959 40.22112196728029, -105.6644591962295 40.22100981930868, -105.6642219518465 40.22087489948009, -105.6640011588874 40.22075494675638, -105.6639699494858 40.22073950563956, -105.6638033782239 40.22065749648416, -105.663644079153 40.22058103005954, -105.6635385751952 40.22048613622436, -105.6635385995102 40.22048598758672, -105.6635388206752 40.22048464173911, -105.6635459583738 40.22044129623704, -105.6635476333263 40.22043232723859, -105.663673564368 40.22034839813178, -105.6636823712486 40.22034252890084, -105.6636991629626 40.22034265464351, -105.6638131673268 40.22034350736083, -105.6638342814396 40.22034461134673, -105.66407395674 40.22035701730299, -105.6643249631576 40.22033462269664, -105.6643434378263 40.22033350759454, -105.6644807467734 40.22032595522565, -105.6644996202503 40.22032505838363, -105.664784009688 40.22031195569402, -105.6648041558022 40.22031213053535, -105.6650694737762 40.22031713167482, -105.665091824547 40.22032044650427, -105.665285107907 40.22035381967699, -105.6653082109339 40.22036160950015, -105.665453274059 40.22041584313852, -105.665476017825 40.22042613357929, -105.6656793835069 40.22052078736321, -105.666025019436 40.22065934213276, -105.6662109684469 40.22072644191363, -105.6665026809634 40.22079240572894, -105.6667602715467 40.22079269933909, -105.6670897912757 40.22075811984187, -105.6671100524527 40.2207586849872, -105.6675771648658 40.22078108328294, -105.6679161754167 40.22078667180477, -105.6679372613319 40.22078769222535, -105.6683273153827 40.22080907895852, -105.668349755364 40.22081223091617, -105.6686076023389 40.22085048682219, -105.6689434412469 40.22085470710499, -105.6689437513543 40.22085468143454, -105.6692620187301 40.22082685426683, -105.6692621514361 40.22082683155698, -105.6694877544554 40.22078559660721, -105.6697167316999 40.22070633274292, -105.670025529971 40.2205818739025, -105.6702602768931 40.22048289117972, -105.6704487179681 40.22038269732911, -105.6705318160145 40.22031142090378, -105.6706279297542 40.22020806563764, -105.6707634219981 40.22005296253833, -105.6709557580282 40.2198097498957, -105.6710802586927 40.2195102805907, -105.6711688587618 40.21926150827178, -105.6712223812788 40.21908071032284, -105.6712253346044 40.21907080716942, -105.6712666943526 40.21893789998065, -105.6712699602049 40.21892894021936, -105.6714498496281 40.21861495681172, -105.6715202551233 40.21847299480071, -105.671677961364 40.21823353650302, -105.6717915822289 40.21803192563492, -105.6718254444284 40.21785519677312, -105.6717553058992 40.21764151836187, -105.6717134573279 40.21753417629488, -105.6717077086626 40.21751735122088, -105.6716852102138 40.21736043335561, -105.6716834977097 40.21734524052872, -105.6716820255947 40.21698238032493, -105.6716342371114 40.21666497320453, -105.6716330510765 40.21665029385176, -105.6716974302847 40.21638855819683, -105.6716844886336 40.21617089596663, -105.6716031140915 40.21590230216545, -105.6715988975821 40.21588596024648, -105.6715868140986 40.21564834423229, -105.6715866363083 40.21563422447139, -105.671620006545 40.21537038231266, -105.6714720476905 40.21507356785254, -105.6713067369528 40.21484232290414, -105.6711008389497 40.21459721857093, -105.6708955791502 40.21438856038766, -105.6708818677844 40.2143719965027, -105.6707985907888 40.21404450838158, -105.6707963908123 40.21403062936756, -105.6710172976288 40.21375003597582, -105.6711798523966 40.21360484501722, -105.6713683785321 40.21343511289258, -105.6714650322431 40.21323580950317, -105.6715368673237 40.21305180125874, -105.6716108388324 40.21274444621527, -105.6716288543036 40.2124036293946, -105.6715814682046 40.21200177952105, -105.6714895341933 40.21156533862437, -105.671486455078 40.21154944621814, -105.6714344058856 40.21113793040745, -105.6714332596219 40.21112312849539, -105.6714547991578 40.21092602580006, -105.6714563055534 40.21091361022041, -105.6714980512335 40.21065270683239, -105.6715004847314 40.2106417939246, -105.6716179011028 40.21040545184155, -105.671664020672 40.21016743042685, -105.6716005492482 40.20992461097636, -105.6714341043355 40.20968414709365, -105.6714230068125 40.20966684897819, -105.6713526988938 40.20947998468864, -105.6712415442038 40.20922611109982, -105.6712343401312 40.20920897381667, -105.6711858342907 40.20906879448798, -105.671180227529 40.20905200698229, -105.6711120121573 40.20881812486911, -105.6711076268386 40.2088016985051, -105.6710679500579 40.20858059997141, -105.6710660945438 40.20856538390952, -105.6710951345212 40.20828515027478, -105.6710971069037 40.20827352295509, -105.6712490761915 40.20794918102887, -105.671252188425 40.20794333224706, -105.6714572507412 40.20776888574395, -105.671692983331 40.20760782260579, -105.671946837003 40.20746655576141, -105.6721096169302 40.20735484743265, -105.6723544287556 40.20722381706818, -105.6726600896722 40.20703938899105, -105.6728621527235 40.20688668559855, -105.6729976289071 40.20669015514054, -105.6730647160993 40.20644451025514, -105.6730678105499 40.20643499409206, -105.673206630464 40.20617431563913, -105.6733991767576 40.20599920259642, -105.6736513100163 40.20574410144964, -105.673799651054 40.20551870087024, -105.6739011514344 40.20534961296253, -105.6740954712419 40.20501136167052, -105.6742218988902 40.20476981641871, -105.674327059758 40.20462555292173, -105.6743913490012 40.20458955425074, -105.674406410934 40.20458814547064, -105.674457882481 40.20458362323701, -105.6744758279328 40.20458215786167, -105.6745819942282 40.20457132159748, -105.6747229798607 40.20452271252111, -105.6748448176996 40.20443287443803, -105.674994499918 40.20430770117226, -105.6751955721305 40.20415308938585, -105.6753971589113 40.20402163432263, -105.6756075566028 40.20390695053762, -105.6758225187993 40.20378210304028, -105.6760931932345 40.20362448291268, -105.6763292401676 40.20353687486897, -105.6763395737016 40.2035335024706, -105.6763396335542 40.2035334825655, -105.6766524176939 40.20343302824362, -105.6766648130916 40.20342984450046, -105.6769356120544 40.20336198784395, -105.6771745118465 40.20329083899474, -105.6774120088294 40.20319948890239, -105.6775459069634 40.20313382843321, -105.6778039324744 40.20302953190082, -105.6778152165018 40.20302631461814, -105.6780621159669 40.20295850286715, -105.6781938470535 40.20289104192163, -105.6782686189575 40.20277966302427, -105.6782330253896 40.20256177745768, -105.678146814832 40.20234917729157, -105.6780636463431 40.20218882324744, -105.6779048632146 40.20200063177179, -105.6778913430041 40.20198365230154, -105.6777848579481 40.20178683232973, -105.6777760633732 40.201769519553, -105.6776790023688 40.20151917503038, -105.6775820109331 40.20131543154896, -105.6774806636888 40.20113149318991, -105.677471925699 40.20111419741364, -105.6774135739281 40.20093048570482, -105.6774087103606 40.2009139179919, -105.6773746711299 40.20074969189098, -105.6773025737169 40.20067296439435, -105.6772870750698 40.20065833402217, -105.6772867405361 40.20065796437652, -105.6772855154855 40.20065661170868, -105.6772124247469 40.20057588058088, -105.6771303299135 40.20050091461442, -105.677110930098 40.20048379905398, -105.6769837093085 40.20036940590301, -105.6769828743263 40.20036854708027, -105.6769820711433 40.20036772153204, -105.6768967181972 40.20027993903021, -105.6768820765282 40.20026326826825, -105.6768159285832 40.20014339393698, -105.6768091210255 40.20012714709139, -105.6768556014762 40.19994812733729, -105.6768585909085 40.19993829059837, -105.67695172948 40.19973998451265, -105.676955236575 40.19973274799546, -105.6770774666019 40.19950071915762, -105.677191466394 40.19929860908254, -105.677309877271 40.19910291361013, -105.6774321865941 40.19887741471136, -105.6775502241474 40.19865534192194, -105.6776388836061 40.19850001203584, -105.6777664012934 40.19833084362219, -105.677859358288 40.19817902390867, -105.6779915239622 40.19802619180775, -105.6780673977488 40.19789303763628, -105.6780974597292 40.19781217787021, -105.678093610375 40.19765681352559, -105.6780492504934 40.19744129817882, -105.677985354926 40.19729188755628, -105.6779247261666 40.19718164024333, -105.6779174020624 40.19716501868773, -105.6779351602477 40.19701107739367, -105.6779372746921 40.1970000027021, -105.678004741952 40.19688982213197, -105.6780596499286 40.19671669514958, -105.678071926527 40.19656638369481, -105.6780735871556 40.19634390762809, -105.678074154487 40.19633047746711, -105.67810410177 40.19616573681866, -105.678122920101 40.19591730248069, -105.6781240986365 40.19590451082409, -105.6781697967753 40.19562028816761, -105.6781797409691 40.19534197737302, -105.6781803389271 40.19532859309427, -105.6781977556393 40.19513170030768, -105.6782070388807 40.19484594049832, -105.6782075650279 40.19483249508618, -105.6782244408778 40.19458256772621, -105.6782341424972 40.19434313834616, -105.6782347793217 40.19432980353974, -105.6782519002093 40.19410310032079, -105.6782529398048 40.19409019359268, -105.6782742489293 40.19386989909211, -105.6782875275536 40.19356417239761, -105.6782485732217 40.19336613348817, -105.6781494802977 40.19314990804275, -105.6781414339438 40.1931326985922, -105.6780370489998 40.19289911524799, -105.6780297956547 40.1928819919292, -105.6779584459529 40.19267161911222, -105.6779532208666 40.19265495198785, -105.6778824219966 40.19233396648192, -105.677879096605 40.19231799622053, -105.6778530901214 40.19216014855787, -105.6778259574849 40.19203372650452, -105.6778234235607 40.1920181666116, -105.6778331188409 40.19186483292374, -105.6778347578226 40.19185297810984, -105.6779274774696 40.19168121408297, -105.6780466278303 40.19153206643568, -105.6781600304808 40.19136463031327, -105.6781519689368 40.19109901984651, -105.6780483550102 40.19096721548783, -105.6780341644516 40.19095039284954, -105.6779374023908 40.19082985643251, -105.6779258125981 40.19081283344089, -105.6778831211533 40.19062535816793, -105.6778806803566 40.19060991791348, -105.6779063544293 40.19041914381376, -105.6779083317913 40.19040736953217, -105.677971367463 40.1901881086194, -105.6780090548469 40.18971784405401, -105.6779019323254 40.18925666184236, -105.677765546384 40.18893325343011, -105.6777584028516 40.18891617134472, -105.6776926608927 40.18874264792856, -105.6775924744353 40.18855230766899, -105.6774687696009 40.18834147264181, -105.6773329173417 40.18814377739658, -105.6773211596643 40.18812653754374, -105.6772256809055 40.18797639568763, -105.6770380712492 40.18774144196102, -105.6770246010461 40.1877244559753, -105.6768426188331 40.18747682323465, -105.6766742782837 40.18730812405553, -105.6765065596637 40.18717919733659, -105.6764839112511 40.18716219017327, -105.6764829605575 40.18716147652353, -105.6763959415487 40.18710202448237, -105.6763308014061 40.18705804967441, -105.6760992185649 40.18689566223739, -105.6759303858499 40.18679373368499, -105.6758363636698 40.18673768635443, -105.6755581622642 40.18657711774318, -105.6754319340273 40.18652047142681, -105.6753559905684 40.18648750826154, -105.6751336758973 40.18639575841871, -105.</t>
         </is>
       </c>
-      <c r="D21" t="n">
-        <v>29</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Ward Private Home</t>
-        </is>
-      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Ward private home</t>
-        </is>
-      </c>
-      <c r="K21" t="n">
-        <v>40.0733984409928</v>
-      </c>
-      <c r="L21" t="n">
-        <v>-105.506518983446</v>
-      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>POINT (-105.506518983446 40.0733984409928)</t>
-        </is>
-      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
refactor source and output files
</commit_message>
<xml_diff>
--- a/data/supersites_geom_2024.xlsx
+++ b/data/supersites_geom_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,70 +446,75 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 0.2</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 0.1</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Venue</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>address</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>organization</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>website</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>google_map_link</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>google_map_name</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>lat</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>lon</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>google_map_url</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>website_url</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>location_geom</t>
         </is>
@@ -538,49 +543,52 @@
       <c r="F2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>Allenspark Fire Station</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>14861 CO-7, Allenspark, CO 80510</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
         <is>
           <t>http://www.allensparkfire.com/</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Allenspark Fire Protection</t>
         </is>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>40.19712777610975</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>-105.5279141785934</v>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>http://www.allensparkfire.com/</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>POINT (-105.5279141785934 40.19712777610975)</t>
         </is>
@@ -609,53 +617,56 @@
       <c r="F3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Altona MS</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>4600 Clover Basin Dr, Longmont, CO 80503</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>https://ams.svvsd.org/</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Altona Middle School</t>
         </is>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>40.14448266991539</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>-105.1626179175455</v>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>https://ams.svvsd.org/</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>POINT (-105.1626179175455 40.14448266991539)</t>
         </is>
@@ -684,53 +695,56 @@
       <c r="F4" t="n">
         <v>4</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>Burlington Elementary</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>1051 S Pratt Pkwy, Longmont, CO 80501</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>http://bes.svvsd.org/</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>Burlington Elementary School</t>
         </is>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>40.1466539913149</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>-105.108633248163</v>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>http://bes.svvsd.org/</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>POINT (-105.108633248163 40.1466539913149)</t>
         </is>
@@ -759,53 +773,56 @@
       <c r="F5" t="n">
         <v>5</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>Casey MS</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>1301 High St, Boulder, CO 80304</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>http://cam.bvsd.org/</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>Casey Middle School</t>
         </is>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>40.0228711759357</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>-105.2791579470394</v>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>http://cam.bvsd.org/</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>POINT (-105.2791579470394 40.0228711759357)</t>
         </is>
@@ -834,53 +851,56 @@
       <c r="F6" t="n">
         <v>6</v>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" t="n">
+        <v>6</v>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>Centaurus HS</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>10300 W South Boulder Rd, Lafayette, CO 80026</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>http://ceh.bvsd.org/</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>Centaurus High School</t>
         </is>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>39.98635981263706</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>-105.1125276640655</v>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>http://ceh.bvsd.org/</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>POINT (-105.1125276640655 39.98635981263706)</t>
         </is>
@@ -909,53 +929,56 @@
       <c r="F7" t="n">
         <v>7</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" t="n">
+        <v>7</v>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>Centennial MS</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>2205 Norwood Ave, Boulder, CO 80304</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>http://cem.bvsd.org/</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="M7" t="inlineStr">
         <is>
           <t>Centennial Middle School</t>
         </is>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>40.04506796264024</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>-105.2671472290834</v>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>http://cem.bvsd.org/</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
+      <c r="R7" t="inlineStr">
         <is>
           <t>POINT (-105.2671472290834 40.04506796264024)</t>
         </is>
@@ -984,53 +1007,56 @@
       <c r="F8" t="n">
         <v>8</v>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" t="n">
+        <v>8</v>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>Eldorado K8</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>3351 S Indiana St, Superior, CO 80027</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>http://el8.bvsd.org/</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t>Eldorado K-8 School</t>
         </is>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>39.921698179021</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>-105.161197194222</v>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="Q8" t="inlineStr">
         <is>
           <t>http://el8.bvsd.org/</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
+      <c r="R8" t="inlineStr">
         <is>
           <t>POINT (-105.161197194222 39.921698179021)</t>
         </is>
@@ -1059,53 +1085,56 @@
       <c r="F9" t="n">
         <v>10</v>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>Erie MS</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>650 Main St, Erie, CO 80516</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>https://ems.svvsd.org/</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="M9" t="inlineStr">
         <is>
           <t>Erie Middle School</t>
         </is>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>40.05101707648438</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>-105.0529688258069</v>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>https://ems.svvsd.org/</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="R9" t="inlineStr">
         <is>
           <t>POINT (-105.0529688258069 40.05101707648438)</t>
         </is>
@@ -1134,53 +1163,56 @@
       <c r="F10" t="n">
         <v>12</v>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G10" t="n">
+        <v>12</v>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>Gold Hill School</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>890 Main St, Boulder, CO 80302</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>http://ghe.bvsd.org/</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>Gold Hill Elementary School</t>
         </is>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>40.063366273762</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>-105.412472825461</v>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="P10" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>http://ghe.bvsd.org/</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="R10" t="inlineStr">
         <is>
           <t>POINT (-105.412472825461 40.063366273762)</t>
         </is>
@@ -1209,53 +1241,56 @@
       <c r="F11" t="n">
         <v>14</v>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" t="n">
+        <v>14</v>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>Jamestown School</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>111 Mesa St, Jamestown, CO 80455</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>http://jae.bvsd.org/</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="M11" t="inlineStr">
         <is>
           <t>Jamestown Elementary School</t>
         </is>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>40.1164318137431</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>-105.387802261192</v>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>http://jae.bvsd.org/</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="R11" t="inlineStr">
         <is>
           <t>POINT (-105.387802261192 40.1164318137431)</t>
         </is>
@@ -1284,53 +1319,56 @@
       <c r="F12" t="n">
         <v>15</v>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" t="n">
+        <v>15</v>
+      </c>
+      <c r="H12" t="inlineStr">
         <is>
           <t>Longs Peak MS</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>1500 14th Ave, Longmont, CO 80501</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>http://lpms.svvsd.org/</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>Longs Peak Middle School</t>
         </is>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>40.18399195721774</v>
       </c>
-      <c r="N12" t="n">
+      <c r="O12" t="n">
         <v>-105.117518880356</v>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>http://lpms.svvsd.org/</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="R12" t="inlineStr">
         <is>
           <t>POINT (-105.117518880356 40.18399195721774)</t>
         </is>
@@ -1359,53 +1397,56 @@
       <c r="F13" t="n">
         <v>17</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" t="n">
+        <v>17</v>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t>Lyons Middle Senior</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>100 McConnell Dr, Lyons, CO 80540</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>https://lmshs.svvsd.org/</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t>Lyons Middle/Senior High School</t>
         </is>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>40.2147599852984</v>
       </c>
-      <c r="N13" t="n">
+      <c r="O13" t="n">
         <v>-105.264461148759</v>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>https://lmshs.svvsd.org/</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
+      <c r="R13" t="inlineStr">
         <is>
           <t>POINT (-105.264461148759 40.2147599852984)</t>
         </is>
@@ -1434,53 +1475,56 @@
       <c r="F14" t="n">
         <v>18</v>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" t="n">
+        <v>18</v>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>Manhattan MS</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>290 Manhattan Dr, Boulder, CO 80303</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>http://mam.bvsd.org/</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>Manhattan Middle School of Arts and Academics</t>
         </is>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>39.99410342530379</v>
       </c>
-      <c r="N14" t="n">
+      <c r="O14" t="n">
         <v>-105.2273572175253</v>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="P14" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="Q14" t="inlineStr">
         <is>
           <t>http://mam.bvsd.org/</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr">
+      <c r="R14" t="inlineStr">
         <is>
           <t>POINT (-105.2273572175253 39.99410342530379)</t>
         </is>
@@ -1509,53 +1553,56 @@
       <c r="F15" t="n">
         <v>19</v>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" t="n">
+        <v>19</v>
+      </c>
+      <c r="H15" t="inlineStr">
         <is>
           <t>Monarch HS</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>329 Campus Dr, Louisville, CO 80027</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>http://moh.bvsd.org/</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="M15" t="inlineStr">
         <is>
           <t>Monarch High School</t>
         </is>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>39.9520220573069</v>
       </c>
-      <c r="N15" t="n">
+      <c r="O15" t="n">
         <v>-105.141776992356</v>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>http://moh.bvsd.org/</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
+      <c r="R15" t="inlineStr">
         <is>
           <t>POINT (-105.141776992356 39.9520220573069)</t>
         </is>
@@ -1584,53 +1631,56 @@
       <c r="F16" t="n">
         <v>21</v>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" t="n">
+        <v>21</v>
+      </c>
+      <c r="H16" t="inlineStr">
         <is>
           <t>Nederland HS</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>597 Co Hwy 130, Nederland, CO 80466</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>https://neh.bvsd.org/</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="M16" t="inlineStr">
         <is>
           <t>Nederland Middle/Senior High School</t>
         </is>
       </c>
-      <c r="M16" t="n">
+      <c r="N16" t="n">
         <v>39.95383849383303</v>
       </c>
-      <c r="N16" t="n">
+      <c r="O16" t="n">
         <v>-105.5233421126253</v>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="P16" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="Q16" t="inlineStr">
         <is>
           <t>https://neh.bvsd.org/</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="R16" t="inlineStr">
         <is>
           <t>POINT (-105.5233421126253 39.95383849383303)</t>
         </is>
@@ -1659,45 +1709,48 @@
       <c r="F17" t="n">
         <v>22</v>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G17" t="n">
+        <v>22</v>
+      </c>
+      <c r="H17" t="inlineStr">
         <is>
           <t>New Vista</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>700 20th St, Boulder, CO 80302</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>http://nvh.bvsd.org/</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/mVZ7Cv3jx5iSPW3u9</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="M17" t="inlineStr">
         <is>
           <t>New Vista High School</t>
         </is>
       </c>
-      <c r="M17" t="n">
+      <c r="N17" t="n">
         <v>40.0011978462681</v>
       </c>
-      <c r="N17" t="n">
+      <c r="O17" t="n">
         <v>-105.266504379284</v>
       </c>
-      <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr">
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr">
         <is>
           <t>POINT (-105.266504379284 40.0011978462681)</t>
         </is>
@@ -1726,53 +1779,56 @@
       <c r="F18" t="n">
         <v>23</v>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" t="n">
+        <v>23</v>
+      </c>
+      <c r="H18" t="inlineStr">
         <is>
           <t>Niwot HS</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>8989 Niwot Rd, Niwot, CO 80503</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>https://nhs.svvsd.org/</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="M18" t="inlineStr">
         <is>
           <t>Niwot High School</t>
         </is>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>40.10369506217272</v>
       </c>
-      <c r="N18" t="n">
+      <c r="O18" t="n">
         <v>-105.1442414652976</v>
       </c>
-      <c r="O18" t="inlineStr">
+      <c r="P18" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr">
+      <c r="Q18" t="inlineStr">
         <is>
           <t>https://nhs.svvsd.org/</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr">
+      <c r="R18" t="inlineStr">
         <is>
           <t>POINT (-105.1442414652976 40.10369506217272)</t>
         </is>
@@ -1801,53 +1857,56 @@
       <c r="F19" t="n">
         <v>25</v>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G19" t="n">
+        <v>25</v>
+      </c>
+      <c r="H19" t="inlineStr">
         <is>
           <t>Southern Hills MS</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>1500 Knox Dr, Boulder, CO 80305</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>BVSD</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>http://shm.bvsd.org/</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="L19" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="M19" t="inlineStr">
         <is>
           <t>Southern Hills Middle School</t>
         </is>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>39.97413389369987</v>
       </c>
-      <c r="N19" t="n">
+      <c r="O19" t="n">
         <v>-105.2452260530946</v>
       </c>
-      <c r="O19" t="inlineStr">
+      <c r="P19" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr">
+      <c r="Q19" t="inlineStr">
         <is>
           <t>http://shm.bvsd.org/</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr">
+      <c r="R19" t="inlineStr">
         <is>
           <t>POINT (-105.2452260530946 39.97413389369987)</t>
         </is>
@@ -1876,53 +1935,56 @@
       <c r="F20" t="n">
         <v>28</v>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="G20" t="n">
+        <v>28</v>
+      </c>
+      <c r="H20" t="inlineStr">
         <is>
           <t>Trail Ridge MS</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>1000 Button Rock Dr, Longmont, CO 80504</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>SVVSD</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>https://trms.svvsd.org/</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
+      <c r="M20" t="inlineStr">
         <is>
           <t>Trail Ridge Middle School</t>
         </is>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>40.17693117783666</v>
       </c>
-      <c r="N20" t="n">
+      <c r="O20" t="n">
         <v>-105.0576162268638</v>
       </c>
-      <c r="O20" t="inlineStr">
+      <c r="P20" t="inlineStr">
         <is>
           <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr">
+      <c r="Q20" t="inlineStr">
         <is>
           <t>https://trms.svvsd.org/</t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr">
+      <c r="R20" t="inlineStr">
         <is>
           <t>POINT (-105.0576162268638 40.17693117783666)</t>
         </is>
@@ -1956,6 +2018,7 @@
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update Supersites from Judi's worksheet
</commit_message>
<xml_diff>
--- a/data/supersites_geom_2024.xlsx
+++ b/data/supersites_geom_2024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,75 +446,65 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.3</t>
+          <t>Unnamed: 0</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.2</t>
+          <t>Venue</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0.1</t>
+          <t>venue_code</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>address</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Venue</t>
+          <t>organization</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>address</t>
+          <t>website</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>organization</t>
+          <t>google_map_link</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>website</t>
+          <t>google_map_name</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>google_map_link</t>
+          <t>lat</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>google_map_name</t>
+          <t>lon</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>lat</t>
+          <t>google_map_url</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>lon</t>
+          <t>website_url</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>google_map_url</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>website_url</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>location_geom</t>
         </is>
@@ -537,58 +527,54 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Allenspark Fire Station</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ALLENSPFS</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>14861 CO-7, Allenspark, CO 80510</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>14861 CO-7, Allenspark, CO 80510</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr"/>
+          <t>http://www.allensparkfire.com/</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>Allenspark Fire Protection</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>40.19712777610975</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-105.5279141785934</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>http://www.allensparkfire.com/</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Allenspark Fire Protection</t>
-        </is>
-      </c>
-      <c r="N2" t="n">
-        <v>40.19712777610975</v>
-      </c>
-      <c r="O2" t="n">
-        <v>-105.5279141785934</v>
-      </c>
       <c r="P2" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/HYN1GYNb9yE4w4RL7</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>http://www.allensparkfire.com/</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
         <is>
           <t>POINT (-105.5279141785934 40.19712777610975)</t>
         </is>
@@ -611,62 +597,58 @@
       <c r="D3" t="n">
         <v>1</v>
       </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Altona MS</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>ALTONAMS</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>4600 Clover Basin Dr, Longmont, CO 80503</t>
+        </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Altona MS</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>4600 Clover Basin Dr, Longmont, CO 80503</t>
+          <t>https://ams.svvsd.org/</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>Altona Middle School</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>40.14448266991539</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-105.1626179175455</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
           <t>https://ams.svvsd.org/</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Altona Middle School</t>
-        </is>
-      </c>
-      <c r="N3" t="n">
-        <v>40.14448266991539</v>
-      </c>
-      <c r="O3" t="n">
-        <v>-105.1626179175455</v>
-      </c>
       <c r="P3" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/ew5ypnry93DZwFNj8</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>https://ams.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
         <is>
           <t>POINT (-105.1626179175455 40.14448266991539)</t>
         </is>
@@ -689,62 +671,58 @@
       <c r="D4" t="n">
         <v>4</v>
       </c>
-      <c r="E4" t="n">
-        <v>4</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4</v>
-      </c>
-      <c r="G4" t="n">
-        <v>4</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Burlington Elementary</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BURLINGES</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1051 S Pratt Pkwy, Longmont, CO 80501</t>
+        </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Burlington Elementary</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1051 S Pratt Pkwy, Longmont, CO 80501</t>
+          <t>http://bes.svvsd.org/</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
+          <t>Burlington Elementary School</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>40.1466539913149</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-105.108633248163</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
           <t>http://bes.svvsd.org/</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Burlington Elementary School</t>
-        </is>
-      </c>
-      <c r="N4" t="n">
-        <v>40.1466539913149</v>
-      </c>
-      <c r="O4" t="n">
-        <v>-105.108633248163</v>
-      </c>
       <c r="P4" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/QefhqxMskS5oyZY87</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>http://bes.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
         <is>
           <t>POINT (-105.108633248163 40.1466539913149)</t>
         </is>
@@ -767,62 +745,58 @@
       <c r="D5" t="n">
         <v>5</v>
       </c>
-      <c r="E5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F5" t="n">
-        <v>5</v>
-      </c>
-      <c r="G5" t="n">
-        <v>5</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Casey MS</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>CASEYMS</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1301 High St, Boulder, CO 80304</t>
+        </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Casey MS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1301 High St, Boulder, CO 80304</t>
+          <t>http://cam.bvsd.org/</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
+          <t>Casey Middle School</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>40.0228711759357</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-105.2791579470394</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
           <t>http://cam.bvsd.org/</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Casey Middle School</t>
-        </is>
-      </c>
-      <c r="N5" t="n">
-        <v>40.0228711759357</v>
-      </c>
-      <c r="O5" t="n">
-        <v>-105.2791579470394</v>
-      </c>
       <c r="P5" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/kqj3JEma8TPCRKWU9</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>http://cam.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
         <is>
           <t>POINT (-105.2791579470394 40.0228711759357)</t>
         </is>
@@ -845,62 +819,58 @@
       <c r="D6" t="n">
         <v>6</v>
       </c>
-      <c r="E6" t="n">
-        <v>6</v>
-      </c>
-      <c r="F6" t="n">
-        <v>6</v>
-      </c>
-      <c r="G6" t="n">
-        <v>6</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Centaurus HS</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>CENTAURHS</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>10300 W South Boulder Rd, Lafayette, CO 80026</t>
+        </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Centaurus HS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>10300 W South Boulder Rd, Lafayette, CO 80026</t>
+          <t>http://ceh.bvsd.org/</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
+          <t>Centaurus High School</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>39.98635981263706</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-105.1125276640655</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
           <t>http://ceh.bvsd.org/</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Centaurus High School</t>
-        </is>
-      </c>
-      <c r="N6" t="n">
-        <v>39.98635981263706</v>
-      </c>
-      <c r="O6" t="n">
-        <v>-105.1125276640655</v>
-      </c>
       <c r="P6" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/qmDEC4W3XTN7acfs9</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>http://ceh.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
         <is>
           <t>POINT (-105.1125276640655 39.98635981263706)</t>
         </is>
@@ -923,62 +893,58 @@
       <c r="D7" t="n">
         <v>7</v>
       </c>
-      <c r="E7" t="n">
-        <v>7</v>
-      </c>
-      <c r="F7" t="n">
-        <v>7</v>
-      </c>
-      <c r="G7" t="n">
-        <v>7</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Centennial MS</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>CENTENNMS</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2205 Norwood Ave, Boulder, CO 80304</t>
+        </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Centennial MS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2205 Norwood Ave, Boulder, CO 80304</t>
+          <t>http://cem.bvsd.org/</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
+          <t>Centennial Middle School</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>40.04506796264024</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-105.2671472290834</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
           <t>http://cem.bvsd.org/</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>Centennial Middle School</t>
-        </is>
-      </c>
-      <c r="N7" t="n">
-        <v>40.04506796264024</v>
-      </c>
-      <c r="O7" t="n">
-        <v>-105.2671472290834</v>
-      </c>
       <c r="P7" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/tKhhHtoniAvTfpPH9</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>http://cem.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
         <is>
           <t>POINT (-105.2671472290834 40.04506796264024)</t>
         </is>
@@ -1001,62 +967,58 @@
       <c r="D8" t="n">
         <v>8</v>
       </c>
-      <c r="E8" t="n">
-        <v>8</v>
-      </c>
-      <c r="F8" t="n">
-        <v>8</v>
-      </c>
-      <c r="G8" t="n">
-        <v>8</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Eldorado K8</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ELDORADOK8</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>3351 S Indiana St, Superior, CO 80027</t>
+        </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Eldorado K8</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3351 S Indiana St, Superior, CO 80027</t>
+          <t>http://el8.bvsd.org/</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
+          <t>Eldorado K-8 School</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>39.921698179021</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-105.161197194222</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
           <t>http://el8.bvsd.org/</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>Eldorado K-8 School</t>
-        </is>
-      </c>
-      <c r="N8" t="n">
-        <v>39.921698179021</v>
-      </c>
-      <c r="O8" t="n">
-        <v>-105.161197194222</v>
-      </c>
       <c r="P8" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/s2gJjfVYasWGLpMz7</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>http://el8.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
         <is>
           <t>POINT (-105.161197194222 39.921698179021)</t>
         </is>
@@ -1079,62 +1041,58 @@
       <c r="D9" t="n">
         <v>10</v>
       </c>
-      <c r="E9" t="n">
-        <v>10</v>
-      </c>
-      <c r="F9" t="n">
-        <v>10</v>
-      </c>
-      <c r="G9" t="n">
-        <v>10</v>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Erie MS</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>ERIEMS</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>650 Main St, Erie, CO 80516</t>
+        </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Erie MS</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>650 Main St, Erie, CO 80516</t>
+          <t>https://ems.svvsd.org/</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
+          <t>Erie Middle School</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>40.05101707648438</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-105.0529688258069</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
           <t>https://ems.svvsd.org/</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>Erie Middle School</t>
-        </is>
-      </c>
-      <c r="N9" t="n">
-        <v>40.05101707648438</v>
-      </c>
-      <c r="O9" t="n">
-        <v>-105.0529688258069</v>
-      </c>
       <c r="P9" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/A5evm4HRnAPM1aUp8</t>
-        </is>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>https://ems.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
         <is>
           <t>POINT (-105.0529688258069 40.05101707648438)</t>
         </is>
@@ -1157,62 +1115,58 @@
       <c r="D10" t="n">
         <v>12</v>
       </c>
-      <c r="E10" t="n">
-        <v>12</v>
-      </c>
-      <c r="F10" t="n">
-        <v>12</v>
-      </c>
-      <c r="G10" t="n">
-        <v>12</v>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Gold Hill School</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>GOLDHILLES</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>890 Main St, Boulder, CO 80302</t>
+        </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Gold Hill School</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>890 Main St, Boulder, CO 80302</t>
+          <t>http://ghe.bvsd.org/</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
+          <t>Gold Hill Elementary School</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>40.063366273762</v>
+      </c>
+      <c r="M10" t="n">
+        <v>-105.412472825461</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
           <t>http://ghe.bvsd.org/</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Gold Hill Elementary School</t>
-        </is>
-      </c>
-      <c r="N10" t="n">
-        <v>40.063366273762</v>
-      </c>
-      <c r="O10" t="n">
-        <v>-105.412472825461</v>
-      </c>
       <c r="P10" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/PZV28vuUvb8p7LJs6</t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>http://ghe.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
         <is>
           <t>POINT (-105.412472825461 40.063366273762)</t>
         </is>
@@ -1235,62 +1189,58 @@
       <c r="D11" t="n">
         <v>14</v>
       </c>
-      <c r="E11" t="n">
-        <v>14</v>
-      </c>
-      <c r="F11" t="n">
-        <v>14</v>
-      </c>
-      <c r="G11" t="n">
-        <v>14</v>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Jamestown School</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>JAMESTWNES</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>111 Mesa St, Jamestown, CO 80455</t>
+        </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Jamestown School</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>111 Mesa St, Jamestown, CO 80455</t>
+          <t>http://jae.bvsd.org/</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
+          <t>Jamestown Elementary School</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>40.1164318137431</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-105.387802261192</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
           <t>http://jae.bvsd.org/</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>Jamestown Elementary School</t>
-        </is>
-      </c>
-      <c r="N11" t="n">
-        <v>40.1164318137431</v>
-      </c>
-      <c r="O11" t="n">
-        <v>-105.387802261192</v>
-      </c>
       <c r="P11" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/xaKW9Ljh7VtMuQPf6</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>http://jae.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
         <is>
           <t>POINT (-105.387802261192 40.1164318137431)</t>
         </is>
@@ -1313,62 +1263,58 @@
       <c r="D12" t="n">
         <v>15</v>
       </c>
-      <c r="E12" t="n">
-        <v>15</v>
-      </c>
-      <c r="F12" t="n">
-        <v>15</v>
-      </c>
-      <c r="G12" t="n">
-        <v>15</v>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Longs Peak MS</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>LONGSPEAKMS</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1500 14th Ave, Longmont, CO 80501</t>
+        </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Longs Peak MS</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>1500 14th Ave, Longmont, CO 80501</t>
+          <t>http://lpms.svvsd.org/</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
+          <t>Longs Peak Middle School</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>40.18399195721774</v>
+      </c>
+      <c r="M12" t="n">
+        <v>-105.117518880356</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
           <t>http://lpms.svvsd.org/</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>Longs Peak Middle School</t>
-        </is>
-      </c>
-      <c r="N12" t="n">
-        <v>40.18399195721774</v>
-      </c>
-      <c r="O12" t="n">
-        <v>-105.117518880356</v>
-      </c>
       <c r="P12" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/44xqEDG33jkv1pN28</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>http://lpms.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
         <is>
           <t>POINT (-105.117518880356 40.18399195721774)</t>
         </is>
@@ -1391,62 +1337,58 @@
       <c r="D13" t="n">
         <v>17</v>
       </c>
-      <c r="E13" t="n">
-        <v>17</v>
-      </c>
-      <c r="F13" t="n">
-        <v>17</v>
-      </c>
-      <c r="G13" t="n">
-        <v>17</v>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Lyons Middle Senior</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>LYONSMS</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>100 McConnell Dr, Lyons, CO 80540</t>
+        </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Lyons Middle Senior</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>100 McConnell Dr, Lyons, CO 80540</t>
+          <t>https://lmshs.svvsd.org/</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
+          <t>Lyons Middle/Senior High School</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>40.2147599852984</v>
+      </c>
+      <c r="M13" t="n">
+        <v>-105.264461148759</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
           <t>https://lmshs.svvsd.org/</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>Lyons Middle/Senior High School</t>
-        </is>
-      </c>
-      <c r="N13" t="n">
-        <v>40.2147599852984</v>
-      </c>
-      <c r="O13" t="n">
-        <v>-105.264461148759</v>
-      </c>
       <c r="P13" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/ohTLL54wbPdkJNFA8</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>https://lmshs.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
         <is>
           <t>POINT (-105.264461148759 40.2147599852984)</t>
         </is>
@@ -1469,62 +1411,58 @@
       <c r="D14" t="n">
         <v>18</v>
       </c>
-      <c r="E14" t="n">
-        <v>18</v>
-      </c>
-      <c r="F14" t="n">
-        <v>18</v>
-      </c>
-      <c r="G14" t="n">
-        <v>18</v>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Manhattan MS</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>MANHATMS</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>290 Manhattan Dr, Boulder, CO 80303</t>
+        </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Manhattan MS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>290 Manhattan Dr, Boulder, CO 80303</t>
+          <t>http://mam.bvsd.org/</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
+          <t>Manhattan Middle School of Arts and Academics</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>39.99410342530379</v>
+      </c>
+      <c r="M14" t="n">
+        <v>-105.2273572175253</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
           <t>http://mam.bvsd.org/</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>Manhattan Middle School of Arts and Academics</t>
-        </is>
-      </c>
-      <c r="N14" t="n">
-        <v>39.99410342530379</v>
-      </c>
-      <c r="O14" t="n">
-        <v>-105.2273572175253</v>
-      </c>
       <c r="P14" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/pkEKK86Dh3tGgHz46</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>http://mam.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
         <is>
           <t>POINT (-105.2273572175253 39.99410342530379)</t>
         </is>
@@ -1547,62 +1485,58 @@
       <c r="D15" t="n">
         <v>19</v>
       </c>
-      <c r="E15" t="n">
-        <v>19</v>
-      </c>
-      <c r="F15" t="n">
-        <v>19</v>
-      </c>
-      <c r="G15" t="n">
-        <v>19</v>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Monarch HS</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>MONARCHHS</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>329 Campus Dr, Louisville, CO 80027</t>
+        </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Monarch HS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>329 Campus Dr, Louisville, CO 80027</t>
+          <t>http://moh.bvsd.org/</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
+          <t>Monarch High School</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>39.9520220573069</v>
+      </c>
+      <c r="M15" t="n">
+        <v>-105.141776992356</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
           <t>http://moh.bvsd.org/</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>Monarch High School</t>
-        </is>
-      </c>
-      <c r="N15" t="n">
-        <v>39.9520220573069</v>
-      </c>
-      <c r="O15" t="n">
-        <v>-105.141776992356</v>
-      </c>
       <c r="P15" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/GVkb3S8qP6y3d6Lc6</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>http://moh.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
         <is>
           <t>POINT (-105.141776992356 39.9520220573069)</t>
         </is>
@@ -1625,62 +1559,58 @@
       <c r="D16" t="n">
         <v>21</v>
       </c>
-      <c r="E16" t="n">
-        <v>21</v>
-      </c>
-      <c r="F16" t="n">
-        <v>21</v>
-      </c>
-      <c r="G16" t="n">
-        <v>21</v>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Nederland HS</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>NEDERLNDHS</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>597 Co Hwy 130, Nederland, CO 80466</t>
+        </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Nederland HS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>597 Co Hwy 130, Nederland, CO 80466</t>
+          <t>https://neh.bvsd.org/</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
+          <t>Nederland Middle/Senior High School</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>39.95383849383303</v>
+      </c>
+      <c r="M16" t="n">
+        <v>-105.5233421126253</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
           <t>https://neh.bvsd.org/</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>Nederland Middle/Senior High School</t>
-        </is>
-      </c>
-      <c r="N16" t="n">
-        <v>39.95383849383303</v>
-      </c>
-      <c r="O16" t="n">
-        <v>-105.5233421126253</v>
-      </c>
       <c r="P16" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/mVMWPW4o458ETfhw5</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>https://neh.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
         <is>
           <t>POINT (-105.5233421126253 39.95383849383303)</t>
         </is>
@@ -1703,54 +1633,50 @@
       <c r="D17" t="n">
         <v>22</v>
       </c>
-      <c r="E17" t="n">
-        <v>22</v>
-      </c>
-      <c r="F17" t="n">
-        <v>22</v>
-      </c>
-      <c r="G17" t="n">
-        <v>22</v>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>New Vista</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>NEWVISTAHS</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>700 20th St, Boulder, CO 80302</t>
+        </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>New Vista</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>700 20th St, Boulder, CO 80302</t>
+          <t>http://nvh.bvsd.org/</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/mVZ7Cv3jx5iSPW3u9</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>http://nvh.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/mVZ7Cv3jx5iSPW3u9</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
           <t>New Vista High School</t>
         </is>
       </c>
-      <c r="N17" t="n">
+      <c r="L17" t="n">
         <v>40.0011978462681</v>
       </c>
-      <c r="O17" t="n">
+      <c r="M17" t="n">
         <v>-105.266504379284</v>
       </c>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr">
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr">
         <is>
           <t>POINT (-105.266504379284 40.0011978462681)</t>
         </is>
@@ -1773,62 +1699,58 @@
       <c r="D18" t="n">
         <v>23</v>
       </c>
-      <c r="E18" t="n">
-        <v>23</v>
-      </c>
-      <c r="F18" t="n">
-        <v>23</v>
-      </c>
-      <c r="G18" t="n">
-        <v>23</v>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Niwot HS</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>NIWOTHS</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>8989 Niwot Rd, Niwot, CO 80503</t>
+        </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Niwot HS</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>8989 Niwot Rd, Niwot, CO 80503</t>
+          <t>https://nhs.svvsd.org/</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
+          <t>Niwot High School</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>40.10369506217272</v>
+      </c>
+      <c r="M18" t="n">
+        <v>-105.1442414652976</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
           <t>https://nhs.svvsd.org/</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>Niwot High School</t>
-        </is>
-      </c>
-      <c r="N18" t="n">
-        <v>40.10369506217272</v>
-      </c>
-      <c r="O18" t="n">
-        <v>-105.1442414652976</v>
-      </c>
       <c r="P18" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/VmRuiC4cCzQrbJPR7</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>https://nhs.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
         <is>
           <t>POINT (-105.1442414652976 40.10369506217272)</t>
         </is>
@@ -1851,62 +1773,58 @@
       <c r="D19" t="n">
         <v>25</v>
       </c>
-      <c r="E19" t="n">
-        <v>25</v>
-      </c>
-      <c r="F19" t="n">
-        <v>25</v>
-      </c>
-      <c r="G19" t="n">
-        <v>25</v>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Southern Hills MS</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>SOUTHILLMS</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>1500 Knox Dr, Boulder, CO 80305</t>
+        </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Southern Hills MS</t>
+          <t>BVSD</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>1500 Knox Dr, Boulder, CO 80305</t>
+          <t>http://shm.bvsd.org/</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>BVSD</t>
+          <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
+          <t>Southern Hills Middle School</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>39.97413389369987</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-105.2452260530946</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
           <t>http://shm.bvsd.org/</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Southern Hills Middle School</t>
-        </is>
-      </c>
-      <c r="N19" t="n">
-        <v>39.97413389369987</v>
-      </c>
-      <c r="O19" t="n">
-        <v>-105.2452260530946</v>
-      </c>
       <c r="P19" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/J5CQaiF7gt1pezXm8</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>http://shm.bvsd.org/</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
         <is>
           <t>POINT (-105.2452260530946 39.97413389369987)</t>
         </is>
@@ -1929,62 +1847,58 @@
       <c r="D20" t="n">
         <v>28</v>
       </c>
-      <c r="E20" t="n">
-        <v>28</v>
-      </c>
-      <c r="F20" t="n">
-        <v>28</v>
-      </c>
-      <c r="G20" t="n">
-        <v>28</v>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Trail Ridge MS</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>TRAILRIDGEMS</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1000 Button Rock Dr, Longmont, CO 80504</t>
+        </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Trail Ridge MS</t>
+          <t>SVVSD</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>1000 Button Rock Dr, Longmont, CO 80504</t>
+          <t>https://trms.svvsd.org/</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>SVVSD</t>
+          <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
+          <t>Trail Ridge Middle School</t>
+        </is>
+      </c>
+      <c r="L20" t="n">
+        <v>40.17693117783666</v>
+      </c>
+      <c r="M20" t="n">
+        <v>-105.0576162268638</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
           <t>https://trms.svvsd.org/</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>Trail Ridge Middle School</t>
-        </is>
-      </c>
-      <c r="N20" t="n">
-        <v>40.17693117783666</v>
-      </c>
-      <c r="O20" t="n">
-        <v>-105.0576162268638</v>
-      </c>
       <c r="P20" t="inlineStr">
-        <is>
-          <t>https://maps.app.goo.gl/jwrYoLXX3rzhtEFy7</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>https://trms.svvsd.org/</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
         <is>
           <t>POINT (-105.0576162268638 40.17693117783666)</t>
         </is>
@@ -2004,21 +1918,45 @@
           <t>POLYGON ((-105.4661484313311 40.16510540791135, -105.46628891067 40.16510477709761, -105.470815740543 40.16518143398583, -105.4708146541582 40.16519354991458, -105.4707617910061 40.16578360363307, -105.4707617862852 40.16578366217297, -105.4705125686798 40.16856524699041, -105.4704672528061 40.1690710003927, -105.4704561694049 40.16919470380456, -105.4704014266738 40.1698729832864, -105.4703235422809 40.17083798352486, -105.4701471120568 40.17302390050776, -105.470147089627 40.17302417969756, -105.4701398981323 40.17311326375602, -105.4701498775658 40.17311351851009, -105.470200732758 40.17311482223527, -105.470709432716 40.1731278654992, -105.4711861857428 40.17314008889846, -105.471439289043 40.1731465768118, -105.4727391684574 40.17317988978623, -105.4749708600473 40.17323704782745, -105.4750032321987 40.1726821562563, -105.4750206722191 40.17238323337168, -105.4750210361202 40.17237698847438, -105.4752042504024 40.16923656802826, -105.479787691759 40.16935887360058, -105.4797873653326 40.16937091048318, -105.4797734359278 40.16988387259018, -105.4797733872597 40.16988566754004, -105.4796805373642 40.17330482726621, -105.4796240684069 40.17656529689094, -105.4796152483834 40.17796396985926, -105.4796026937846 40.17995501780022, -105.479611783183 40.17995483837693, -105.4809046495147 40.17992930563622, -105.4809104417855 40.17992919131213, -105.4821456944617 40.17990478346833, -105.4842904768209 40.17986236891954, -105.4842904845098 40.17987483273979, -105.4842905938626 40.18005209836011, -105.484290852698 40.18047691385383, -105.4842909836418 40.18069288673419, -105.4842919357208 40.18225457717938, -105.4842923359611 40.18291119120383, -105.4842927315417 40.18355750826427, -105.4843017355777 40.18355781209871, -105.4858596675139 40.18361035232417, -105.4887108236855 40.18370645233315, -105.4890342964373 40.18371735136233, -105.4913673103303 40.18380308278645, -105.4916169415424 40.18381225335324, -105.493803003558 40.18389564358236, -105.4938093397902 40.1838958852905, -105.4938123200268 40.18389599982997, -105.4938523169958 40.18035330559622, -105.4938523205461 40.18035299938223, -105.4942081234937 40.18036470973328, -105.4942254027887 40.18036558420872, -105.4988689323545 40.18060051532034, -105.5037971648563 40.18084965648772, -105.5066788071574 40.18091382279687, -105.5115988430433 40.18102320894966, -105.5138093385616 40.18107228813918, -105.5207705453987 40.18122672640443, -105.5208006874244 40.18122739465633, -105.522236754261 40.18127360796668, -105.5222435283211 40.18127382641728, -105.5222435741154 40.18127382730909, -105.522435320304 40.18127999739902, -105.5224377955276 40.18127643582816, -105.5224378823772 40.18127630972313, -105.523680357985 40.181292988343, -105.523688178229 40.1812930930153, -105.5236896753479 40.18129311342297, -105.5237041709683 40.18072051517435, -105.5237197330747 40.18010577977868, -105.5237413580885 40.17925150068127, -105.5237454789506 40.17908870192743, -105.5237510683669 40.17886786445666, -105.5237651645466 40.17831101269118, -105.5237857437776 40.17749800315436, -105.5238776530766 40.17387231186575, -105.5258247721261 40.17387231837259, -105.5258340931253 40.17387231809113, -105.5332652858553 40.17387203873018, -105.5332746068535 40.17387203604751, -105.5332742031089 40.1738843189681, -105.5331893193217 40.17646799626176, -105.5331568626344 40.17752450998029, -105.5331662580995 40.17752449827886, -105.5332269975165 40.17752442499798, -105.5332266806333 40.17753671869425, -105.5331269808046 40.18141083850799, -105.5330262556054 40.1837602446121, -105.532976230018 40.18492700366666, -105.5328963810823 40.18678931519381, -105.5328252778692 40.18844755645122, -105.5328252743849 40.18844763660821, -105.5328144473783 40.1887670954498, -105.5328026033848 40.18959315645375, -105.5327760272405 40.19144611821562, -105.5327628767569 40.19236313910528, -105.5327720701403 40.19236356970227, -105.5328092241853 40.19236530368316, -105.5328090737093 40.1923771568957, -105.5328019262174 40.19293933922767, -105.5328018956497 40.19294170518686, -105.5328006690869 40.1930380970772, -105.5328098787648 40.19303559882346, -105.5328294254024 40.19303029578, -105.5328935660998 40.19301413198865, -105.5329570730651 40.19299410915016, -105.5330083598834 40.19297567307023, -105.5330790606768 40.1929545853694, -105.5331549173888 40.1929269242624, -105.5332445784334 40.19289053114875, -105.5333357318797 40.19285139332066, -105.5334323856855 40.19282329373202, -105.5335304733625 40.19279520175227, -105.5336091149603 40.19277140683688, -105.5336459058447 40.19275785969391, -105.5336515583924 40.19275577849825, -105.533684251341 40.19274374108799, -105.5337565232855 40.19271606081569, -105.5338179414305 40.19269327228345, -105.533890165039 40.19266779307718, -105.5339501238616 40.19264610006633, -105.5340122329798 40.19262441809995, -105.5341047369489 40.19258913845898, -105.5341957862916 40.19255495433799, -105.5342200411473 40.19254790514945, -105.5342198678148 40.19256285923371, -105.5342193376537 40.19260852935302, -105.5342183473157 40.19269425235101, -105.5342183360385 40.19269518000148, -105.5342180715312 40.19271798939261, -105.5342271532779 40.19272517011618, -105.5343393829121 40.19281390637015, -105.5346356497051 40.19259680260618, -105.5348823209668 40.19251699672893, -105.5349371865247 40.19249180670148, -105.5349909777208 40.19246710871604, -105.537495561658 40.19258391871914, -105.5375025897888 40.19185229996346, -105.5375101454505 40.19106602720946, -105.5375433224156 40.1910399954814, -105.5375224677095 40.18937951494874, -105.5375223216064 40.1893679950532, -105.5372715249519 40.18934647278628, -105.537254321171 40.18934499589563, -105.5375677880135 40.18893092853408, -105.5375946466315 40.18889544853639, -105.541762862168 40.1891617345586, -105.5422569890588 40.18918897106952, -105.5422571009006 40.18920076026023, -105.5422758519701 40.1911640951709, -105.5422833975333 40.19195391480071, -105.5422833975938 40.19195401206859, -105.542297092536 40.19338773536003, -105.5422970925746 40.19338779750338, -105.5423024628827 40.19394992984792, -105.5423929265994 40.20341858732859, -105.542401834668 40.20341858226157, -105.5424019515685 40.20343087127191, -105.5471617411033 40.203428251832, -105.5471710649767 40.20342824622806, -105.5471762500321 40.20702449927905, -105.5471669256137 40.20702443013139, -105.5469038813974 40.20702247197197, -105.5423441045886 40.20698842150102, -105.5423441034594 40.20698849445215, -105.5422953313193 40.21055420708196, -105.5422860075863 40.21055412132916, -105.5404398525206 40.21053711938241, -105.5326909158406 40.21046358966055, -105.5326905760758 40.21136204136256, -105.5326905761208 40.21136213502758, -105.5326902668153 40.21217981128849, -105.5326894995797 40.21419262998702, -105.5326895026425 40.21419411331591, -105.5326985284376 40.21419413237972, -105.5422526119581 40.21421377049138, -105.5422524668593 40.21422603345813, -105.5422084115658 40.21794388539156, -105.5411373910101 40.21826779544625, -105.5398831425591 40.21944693342513, -105.5379809748795 40.21961963612427, -105.5379291219123 40.21962350240685, -105.5378566567431 40.21962890467403, -105.5364658151693 40.21975515971221, -105.5364659849748 40.21975632326548, -105.536469145231 40.2197779543675, -105.5364610049816 40.21977874858243, -105.5360297782496 40.21982080776719, -105.5360049453737 40.2214518136923, -105.5348769137664 40.22144872610919, -105.5338911592008 40.22144602273305, -105.5333207578963 40.22144445293673, -105.5326849358092 40.22144269979285, -105.5326849473221 40.2214446523428, -105.5326967674883 40.2233561262393, -105.5326825303639 40.22418840574673, -105.5326820404199 40.22504857987344, -105.5326910735317 40.22504859983672, -105.5344553890728 40.22505242161549, -105.5353538558136 40.22505402382836, -105.5360637775385 40.22505528352068, -105.5364251454815 40.22505592322528, -105.5364318357178 40.22505593462795, -105.536760204845 40.22505651522585, -105.5373800222655 40.2250576054056, -105.5374809703504 40.2250577834895, -105.5385255461858 40.22505961624928, -105.5405764553367 40.22506318763808, -105.5419484417806 40.22506555326001, -105.5419590751946 40.22506557191936, -105.5420808495041 40.22506765406047, -105.5420823229212 40.22506767874194, -105.5420822364319 40.22507980477056, -105.5420562713165 40.22872637531357, -105.542057627296 40.22872637662191, -105.5420429039838 40.2322667322377, -105.5418212665354 40.24069807142973, -105.5417703294095 40.24320999597101, -105.5417913293522 40.24484599488542, -105.5418693303538 40.25068399588682, -105.5419533310875 40.25691899504218, -105.5420123310872 40.26132699564431, -105.5420510583876 40.26143505394957, -105.5420511054112 40.26143505393247, -105.5420601092523 40.26143504165487, -105.546896776124 40.26142835486699, -105.5469164731246 40.26142832707124, -105.5488073098715 40.26142565841789, -105.5516765188264 40.26142154904153, -105.5516962275788 40.26142152042718, -105.5564490412647 40.26141455566594, -105.5564687629445 40.26141452623263, -105.5591675481954 40.26141048439985, -105.559187278102 40.26141045449919, -105.5591940095238 40.26141044475258, -105.5610087103939 40.26140744097114, -105.5795558249904 40.26109930837292, -105.5795753264785 40.2610990572043, -105.5951059878192 40.26090826365041, -105.5951255644495 40.26090802240864, -105.5978803250462 40.26087396174936, -105.5978999087103 40.26087372003241, -105.5990498899888 40.26085948275252, -105.5990694865891 40.26085924983279, -105.5995397909104 40.26085370200565, -105.5995593945634 40.26085347079817, -105.6024803232683 40.26081898919289, -105.6142594281275 40.26067918769429, -105.6159287966142 40.26065927760523, -105.6159484448253 40.26065904267666, -105.6183738399164 40.26063000678786, -105.6183934869193 40.2606297624392, -105.6213214042607 40.26059298525797, -105.6213410559414 40.26059273860285, -105.6230240548107 40.26057156630034, -105.6230437100057 40.26057131935239, -105.6277277549875 40.26051225854213, -105.627747425429 40.26051200987794, -105.632275471989 40.26045473382353, -105.6322951553285 40.26045448437176, -105.6333595672079 40.26044099555356, -105.6333792540661 40.26044074591335, -105.6336239250111 40.26043764207176, -105.6336436106918 40.26043739238794, -105.6344099544128 40.26042767444419, -105.6344296424389 40.26042742462398, -105.6344533637605 40.26042712418371, -105.6344730517862 40.26042687435609, -105.6370401114326 40.26039427547199, -105.6370598053172 40.2603940251974, -105.641661457955 40.26033544727563, -105.6416811682616 40.26033519529398, -105.6421922091127 40.26032867946999, -105.6422119170661 40.2603284283015, -105.6463212330816 40.26027594287727, -105.6463409574624 40.26027569098492, -105.6510511032203 40.26021535336445, -105.6510708369704 40.26021510065377, -105.653220247745 40.26018750197031, -105.6534108731882 40.2601810802276, -105.6533823627512 40.26010275780921, -105.6532830172156 40.25994882313275, -105.6532015168119 40.259833817446, -105.6530755380744 40.25970888806435, -105.653056450447 40.25969061631895, -105.6528639596007 40.25950741268624, -105.6526889307466 40.2593871624231, -105.652642514434 40.25935601447338, -105.6524271025182 40.25918859577206, -105.652112632482 40.25892918790828, -105.6518414912158 40.25866632340869, -105.6518412163808 40.2586659058817, -105.6518402220181 40.25866439414499, -105.6518249196642 40.25864111788805, -105.651683174363 40.25842552064559, -105.6516722710576 40.25840806831427, -105.6515514218632 40.25817243805065, -105.6515429003808 40.25815503662493, -105.6514243241588 40.25786656297638, -105.6514187228448 40.25784972511072, -105.6514055789766 40.25757162818682, -105.6513344204328 40.25729383767664, -105.6513306212376 40.25727751710651, -105.6512928566423 40.25697723763877, -105.6512494136496 40.25670131742907, -105.6512475526345 40.25668592286098, -105.6512481806062 40.25659521519253, -105.6512491443465 40.25645626717135, -105.6512492414307 40.25644232184331, -105.651250394949 40.25627562546527, -105.6512238153397 40.25580599850561, -105.6512233117349 40.25579151809188, -105.6512386810696 40.2554038107325, -105.6512392740317 40.25539031326282, -105.6512547967072 40.25511750050543, -105.651254798984 40.25511746717952, -105.6512556523308 40.25510424315733, -105.6512679930778 40.25496298995328, -105.651283544426 40.25478497372899, -105.6512465313483 40.25451425149574, -105.6510657606499 40.25415446368373, -105.651056843717 40.25413708614312, -105.6508969847668 40.25382258276831, -105.6505310873636 40.2534957431415, -105.6505198035114 40.25348589422141, -105.650277580469 40.25334159185142, -105.6502158172845 40.25330586876338, -105.6497508549943 40.25305330688136, -105.6493031225032 40.25278747457062, -105.6489024621259 40.25250204640531, -105.6485320184643 40.25224942820618, -105.648122926153 40.25197372674319, -105.6478519627375 40.25176733123399, -105.647595323896 40.2516000866161, -105.6474810359026 40.2515261922803, -105.6473040944805 40.25143101667013, -105.6471837932539 40.25136724816764, -105.6468534777815 40.25120486346038, -105.6466993803544 40.25114202354365, -105.6465010494459 40.25106199343578, -105.6463131316636 40.25101511518552, -105.6461854347542 40.25098444290174, -105.6459617149985 40.25091212623183, -105.645862718699 40.25086625543839, -105.6439109359637 40.24997257845546, -105.6439113906358 40.24997248152362, -105.6440326178304 40.24994670984607, -105.6460486209198 40.24951810932338, -105.6461040002026 40.24950599091284, -105.6461040377955 40.24950598185919, -105.6461837138841 40.24948586944218, -105.6461837538199 40.24948585678304, -105.6462761693258 40.24945621494909, -105.6462878338384 40.24945293635419, -105.6465034720074 40.2493933900957, -105.6465165544287 40.24939030511742, -105.6468338582291 40.24931722103709, -105.6468479730201 40.24931432744434, -105.6473447774411 40.24921444122509, -105.6473620074362 40.24921285670883, -105.6478251640483 40.24917729760249, -105.6478451563986 40.24917744047953, -105.6483876106674 40.24918924142482, -105.6484084764347 40.24918997028969, -105.6490580710522 40.24921440685837, -105.6490793598224 40.24921560338041, -105.6496621472309 40.24925061573745, -105.649857509743 40.24926235109255, -105.6498792923866 40.24926416375346, -105.6504807419691 40.24931712691847, -105.6505029278615 40.24931949642218, -105.6510873439726 40.249384258711, -105.6510876331863 40.24938428985514, -105.6517955093473 40.24946011446387, -105.6524384646635 40.24946103545784, -105.6532240381383 40.24939543248849, -105.6532429858952 40.24939464187201, -105.6540359245012 40.24936764317474, -105.6540561108867 40.24936779732936, -105.6547920954059 40.24937937171175, -105.6548135707898 40.24938089655689, -105.6553635528423 40.24942562557963, -105.6560772134397 40.2494691280667, -105.6560990989358 40.2494710970272, -105.6566697271875 40.24952454693272, -105.6572882420254 40.24953298344785, -105.6572884124538 40.2495329823156, -105.6577466825842 40.24952787256891, -105.6577468823637 40.24952785698604, -105.658364554839 40.24947889500469, -105.6583837733506 40.24947829771016, -105.658383836817 40.24947829582203, -105.6588610698823 40.24946552024045, -105.6593578213218 40.24936558880857, -105.6596740517714 40.24922577817019, -105.6598284918649 40.24908374683517, -105.6600357955445 40.24885510058633, -105.6601709350914 40.24869839282666, -105.6602180098776 40.24847606239258, -105.6602904669786 40.24808708989965, -105.6603197434563 40.24775706340495, -105.6603209213945 40.24774420990298, -105.6603381955352 40.24758479666077, -105.6603395938818 40.24757220763556, -105.6603473707779 40.24750678741342, -105.6603488540162 40.24749431264927, -105.6603658886433 40.24735099924052, -105.6603676534624 40.2473388122845, -105.6604413607002 40.24701574268065, -105.6604416576382 40.2466576694766, -105.660406673147 40.24625862093598, -105.6604060936211 40.24624414514405, -105.6604638791043 40.2458376972433, -105.6604423228038 40.24554413969873, -105.6604183656476 40.24532331789342, -105.6604176166594 40.24530874776879, -105.6604654929911 40.24502852130396, -105.6604680799253 40.24501810382434, -105.6606031082612 40.24480953958241, -105.6608380761308 40.24465551037683, -105.661090919282 40.24451736259382, -105.6614394345306 40.24425372862866, -105.6617972409519 40.24400229844849, -105.661993737268 40.24379598909656, -105.6622515148447 40.24354079687833, -105.6623638976777 40.24339320647818, -105.6623412545372 40.243148140186, -105.6622271542483 40.24289913312061, -105.6622212185086 40.24288262853066, -105.662246928383 40.24270330468485, -105.6622493009619 40.24269235519348, -105.6624203867668 40.24238932411787, -105.6626383198902 40.24217056212871, -105.6627478603099 40.2420858297572, -105.6628966257281 40.24188143849485, -105.6630035083658 40.2416272908031, -105.6630070175849 40.24161941982204, -105.6631343254574 40.24137469705771, -105.6632915945943 40.24121971764026, -105.6634577117512 40.24103557054804, -105.6636414775772 40.24080598165017, -105.6638605888681 40.24047958579609, -105.6641361334141 40.24008308784516, -105.6643937880334 40.23986345373206, -105.6646430665669 40.23956239662796, -105.6647837931359 40.23929073503575, -105.6649769754472 40.23895438237981, -105.6651788634559 40.23861149463966, -105.665323466031 40.23835513830205, -105.6653962474659 40.23809944644505, -105.665431211319 40.23766674878126, -105.6654329294115 40.23765467076841, -105.6655795293855 40.23730339632174, -105.6656516849346 40.23700392224806, -105.6655733758443 40.23677124300807, -105.6654192999047 40.23653663304073, -105.6652664880635 40.23634685679159, -105.6651081521364 40.23616363214872, -105.6650945635468 40.23614659102824, -105.6649503217293 40.23588669668948, -105.6649408301455 40.23586931017438, -105.6648173713558 40.23562903403352, -105.6648096253163 40.23561180533154, -105.6647862204469 40.23550442489909, -105.6647251887129 40.23522442147496, -105.6647251756337 40.23522435844993, -105.6646582848182 40.23494468934514, -105.6646546756029 40.23492852738642, -105.6645951132258 40.23457015220544, -105.6645927169959 40.23455456581809, -105.6645619404331 40.23428038048088, -105.6645609881937 40.23426566023956, -105.6646107631039 40.23381407701542, -105.6646123901615 40.23380175146494, -105.6646686018296 40.23352436399449, -105.6646712989217 40.23351378322931, -105.6648220164282 40.23318151580031, -105.6648255241641 40.23317475342208, -105.6650047084142 40.2329491006681, -105.6651964929561 40.2327528359099, -105.6654011529644 40.23258888212007, -105.6657063539013 40.23236997563181, -105.6659413331565 40.23217075944036, -105.6661675652812 40.23202312776482, -105.6663889616327 40.23191128709515, -105.6666810970455 40.23171510873143, -105.6666926686825 40.23171249465987, -105.6670132530934 40.23164008776747, -105.6670310503309 40.23163893539422, -105.6670310985044 40.23163893352346, -105.6671542201482 40.23163200282799, -105.6671543176415 40.23163198737654, -105.6673891053773 40.23159393428879, -105.6675672799185 40.23153819341664, -105.6677025916841 40.23133320802084, -105.6677681890939 40.23097816878754, -105.6677631503988 40.23075299479768, -105.6677483196333 40.23044769834121, -105.6677481743348 40.23043358126473, -105.6677741899327 40.2302316910987, -105.6677764100459 40.23022044448404, -105.6678022827057 40.23016966127873, -105.6679082388013 40.22996248731734, -105.6680695015121 40.2297791769222, -105.6682133000139 40.22966333765718, -105.6684010177816 40.22951487491294, -105.6685625454325 40.22935359900887, -105.6687415781404 40.22916824706451, -105.6688267008086 40.22894056836384, -105.6688429479812 40.22873624245703, -105.6688205696722 40.22852339716228, -105.6687613011443 40.22838176133099, -105.6686730393414 40.22821884274862, -105.6685174411165 40.22801933434805, -105.6683511792286 40.22783588408025, -105.6683375401028 40.22781896947912, -105.6682470624096 40.22761127111529, -105.6682416637716 40.22759486778096, -105.6682721112314 40.22737017614368, -105.6682739650483 40.22735817442233, -105.6683029921154 40.22722332576805, -105.6683058044111 40.2272130959819, -105.6683934966554 40.22704599071793, -105.6685196675831 40.22692074262096, -105.6687379630553 40.22675606758625, -105.6689083831121 40.22657508868081, -105.6690438599216 40.22640284891151, -105.6690758537972 40.22632072549793, -105.6690792556187 40.22631231949595, -105.6691903428408 40.22606427355334, -105.6692787329387 40.22583821434375, -105.6693278820078 40.22567399448331, -105.6693861052922 40.22544429847117, -105.669440759808 40.22514343033741, -105.66945233353 40.2249046090048, -105.6694532890332 40.22489151701731, -105.6694919852029 40.22466959399863, -105.6694915482502 40.22436290200361, -105.6693372707889 40.22410474212811, -105.6691337832986 40.22385606282835, -105.6689801460077 40.22368898447323, -105.6688367933033 40.22358134839062, -105.668820995009 40.22356996322452, -105.6686399339946 40.22346121020597, -105.66857070503 40.22342023718163, -105.6684063343704 40.22334358118142, -105.6683101888107 40.22329963458959, -105.6680685904649 40.22318068359311, -105.6678529537799 40.22304919374229, -105.6676002381706 40.22290378130718, -105.6674823272445 40.22284463958258, -105.6673437859818 40.22277593321919, -105.6672358734293 40.22272320634443, -105.6669856426672 40.22260732588539, -105.6667614982625 40.22246269083642, -105.6664857475077 40.222278601177, -105.6662919082906 40.22213095583463, -105.6661158510701 40.22201122023689, -105.6660285158423 40.22195229519745, -105.6659311617552 40.22189506412996, -105.6658563941644 40.22185175849506, -105.6656409412277 40.2217135933068, -105.6654520699702 40.22157582560256, -105.6653094536946 40.22148618217604, -105.6652393815789 40.22144276315675, -105.665179073635 40.2214088029338, -105.6650717714665 40.22134893480318, -105.6648732975747 40.22122908068761, -105.664797561422 40.22118791743397, -105.6646748951959 40.22112196728029, -105.6644591962295 40.22100981930868, -105.6642219518465 40.22087489948009, -105.6640011588874 40.22075494675638, -105.6639699494858 40.22073950563956, -105.6638033782239 40.22065749648416, -105.663644079153 40.22058103005954, -105.6635385751952 40.22048613622436, -105.6635385995102 40.22048598758672, -105.6635388206752 40.22048464173911, -105.6635459583738 40.22044129623704, -105.6635476333263 40.22043232723859, -105.663673564368 40.22034839813178, -105.6636823712486 40.22034252890084, -105.6636991629626 40.22034265464351, -105.6638131673268 40.22034350736083, -105.6638342814396 40.22034461134673, -105.66407395674 40.22035701730299, -105.6643249631576 40.22033462269664, -105.6643434378263 40.22033350759454, -105.6644807467734 40.22032595522565, -105.6644996202503 40.22032505838363, -105.664784009688 40.22031195569402, -105.6648041558022 40.22031213053535, -105.6650694737762 40.22031713167482, -105.665091824547 40.22032044650427, -105.665285107907 40.22035381967699, -105.6653082109339 40.22036160950015, -105.665453274059 40.22041584313852, -105.665476017825 40.22042613357929, -105.6656793835069 40.22052078736321, -105.666025019436 40.22065934213276, -105.6662109684469 40.22072644191363, -105.6665026809634 40.22079240572894, -105.6667602715467 40.22079269933909, -105.6670897912757 40.22075811984187, -105.6671100524527 40.2207586849872, -105.6675771648658 40.22078108328294, -105.6679161754167 40.22078667180477, -105.6679372613319 40.22078769222535, -105.6683273153827 40.22080907895852, -105.668349755364 40.22081223091617, -105.6686076023389 40.22085048682219, -105.6689434412469 40.22085470710499, -105.6689437513543 40.22085468143454, -105.6692620187301 40.22082685426683, -105.6692621514361 40.22082683155698, -105.6694877544554 40.22078559660721, -105.6697167316999 40.22070633274292, -105.670025529971 40.2205818739025, -105.6702602768931 40.22048289117972, -105.6704487179681 40.22038269732911, -105.6705318160145 40.22031142090378, -105.6706279297542 40.22020806563764, -105.6707634219981 40.22005296253833, -105.6709557580282 40.2198097498957, -105.6710802586927 40.2195102805907, -105.6711688587618 40.21926150827178, -105.6712223812788 40.21908071032284, -105.6712253346044 40.21907080716942, -105.6712666943526 40.21893789998065, -105.6712699602049 40.21892894021936, -105.6714498496281 40.21861495681172, -105.6715202551233 40.21847299480071, -105.671677961364 40.21823353650302, -105.6717915822289 40.21803192563492, -105.6718254444284 40.21785519677312, -105.6717553058992 40.21764151836187, -105.6717134573279 40.21753417629488, -105.6717077086626 40.21751735122088, -105.6716852102138 40.21736043335561, -105.6716834977097 40.21734524052872, -105.6716820255947 40.21698238032493, -105.6716342371114 40.21666497320453, -105.6716330510765 40.21665029385176, -105.6716974302847 40.21638855819683, -105.6716844886336 40.21617089596663, -105.6716031140915 40.21590230216545, -105.6715988975821 40.21588596024648, -105.6715868140986 40.21564834423229, -105.6715866363083 40.21563422447139, -105.671620006545 40.21537038231266, -105.6714720476905 40.21507356785254, -105.6713067369528 40.21484232290414, -105.6711008389497 40.21459721857093, -105.6708955791502 40.21438856038766, -105.6708818677844 40.2143719965027, -105.6707985907888 40.21404450838158, -105.6707963908123 40.21403062936756, -105.6710172976288 40.21375003597582, -105.6711798523966 40.21360484501722, -105.6713683785321 40.21343511289258, -105.6714650322431 40.21323580950317, -105.6715368673237 40.21305180125874, -105.6716108388324 40.21274444621527, -105.6716288543036 40.2124036293946, -105.6715814682046 40.21200177952105, -105.6714895341933 40.21156533862437, -105.671486455078 40.21154944621814, -105.6714344058856 40.21113793040745, -105.6714332596219 40.21112312849539, -105.6714547991578 40.21092602580006, -105.6714563055534 40.21091361022041, -105.6714980512335 40.21065270683239, -105.6715004847314 40.2106417939246, -105.6716179011028 40.21040545184155, -105.671664020672 40.21016743042685, -105.6716005492482 40.20992461097636, -105.6714341043355 40.20968414709365, -105.6714230068125 40.20966684897819, -105.6713526988938 40.20947998468864, -105.6712415442038 40.20922611109982, -105.6712343401312 40.20920897381667, -105.6711858342907 40.20906879448798, -105.671180227529 40.20905200698229, -105.6711120121573 40.20881812486911, -105.6711076268386 40.2088016985051, -105.6710679500579 40.20858059997141, -105.6710660945438 40.20856538390952, -105.6710951345212 40.20828515027478, -105.6710971069037 40.20827352295509, -105.6712490761915 40.20794918102887, -105.671252188425 40.20794333224706, -105.6714572507412 40.20776888574395, -105.671692983331 40.20760782260579, -105.671946837003 40.20746655576141, -105.6721096169302 40.20735484743265, -105.6723544287556 40.20722381706818, -105.6726600896722 40.20703938899105, -105.6728621527235 40.20688668559855, -105.6729976289071 40.20669015514054, -105.6730647160993 40.20644451025514, -105.6730678105499 40.20643499409206, -105.673206630464 40.20617431563913, -105.6733991767576 40.20599920259642, -105.6736513100163 40.20574410144964, -105.673799651054 40.20551870087024, -105.6739011514344 40.20534961296253, -105.6740954712419 40.20501136167052, -105.6742218988902 40.20476981641871, -105.674327059758 40.20462555292173, -105.6743913490012 40.20458955425074, -105.674406410934 40.20458814547064, -105.674457882481 40.20458362323701, -105.6744758279328 40.20458215786167, -105.6745819942282 40.20457132159748, -105.6747229798607 40.20452271252111, -105.6748448176996 40.20443287443803, -105.674994499918 40.20430770117226, -105.6751955721305 40.20415308938585, -105.6753971589113 40.20402163432263, -105.6756075566028 40.20390695053762, -105.6758225187993 40.20378210304028, -105.6760931932345 40.20362448291268, -105.6763292401676 40.20353687486897, -105.6763395737016 40.2035335024706, -105.6763396335542 40.2035334825655, -105.6766524176939 40.20343302824362, -105.6766648130916 40.20342984450046, -105.6769356120544 40.20336198784395, -105.6771745118465 40.20329083899474, -105.6774120088294 40.20319948890239, -105.6775459069634 40.20313382843321, -105.6778039324744 40.20302953190082, -105.6778152165018 40.20302631461814, -105.6780621159669 40.20295850286715, -105.6781938470535 40.20289104192163, -105.6782686189575 40.20277966302427, -105.6782330253896 40.20256177745768, -105.678146814832 40.20234917729157, -105.6780636463431 40.20218882324744, -105.6779048632146 40.20200063177179, -105.6778913430041 40.20198365230154, -105.6777848579481 40.20178683232973, -105.6777760633732 40.201769519553, -105.6776790023688 40.20151917503038, -105.6775820109331 40.20131543154896, -105.6774806636888 40.20113149318991, -105.677471925699 40.20111419741364, -105.6774135739281 40.20093048570482, -105.6774087103606 40.2009139179919, -105.6773746711299 40.20074969189098, -105.6773025737169 40.20067296439435, -105.6772870750698 40.20065833402217, -105.6772867405361 40.20065796437652, -105.6772855154855 40.20065661170868, -105.6772124247469 40.20057588058088, -105.6771303299135 40.20050091461442, -105.677110930098 40.20048379905398, -105.6769837093085 40.20036940590301, -105.6769828743263 40.20036854708027, -105.6769820711433 40.20036772153204, -105.6768967181972 40.20027993903021, -105.6768820765282 40.20026326826825, -105.6768159285832 40.20014339393698, -105.6768091210255 40.20012714709139, -105.6768556014762 40.19994812733729, -105.6768585909085 40.19993829059837, -105.67695172948 40.19973998451265, -105.676955236575 40.19973274799546, -105.6770774666019 40.19950071915762, -105.677191466394 40.19929860908254, -105.677309877271 40.19910291361013, -105.6774321865941 40.19887741471136, -105.6775502241474 40.19865534192194, -105.6776388836061 40.19850001203584, -105.6777664012934 40.19833084362219, -105.677859358288 40.19817902390867, -105.6779915239622 40.19802619180775, -105.6780673977488 40.19789303763628, -105.6780974597292 40.19781217787021, -105.678093610375 40.19765681352559, -105.6780492504934 40.19744129817882, -105.677985354926 40.19729188755628, -105.6779247261666 40.19718164024333, -105.6779174020624 40.19716501868773, -105.6779351602477 40.19701107739367, -105.6779372746921 40.1970000027021, -105.678004741952 40.19688982213197, -105.6780596499286 40.19671669514958, -105.678071926527 40.19656638369481, -105.6780735871556 40.19634390762809, -105.678074154487 40.19633047746711, -105.67810410177 40.19616573681866, -105.678122920101 40.19591730248069, -105.6781240986365 40.19590451082409, -105.6781697967753 40.19562028816761, -105.6781797409691 40.19534197737302, -105.6781803389271 40.19532859309427, -105.6781977556393 40.19513170030768, -105.6782070388807 40.19484594049832, -105.6782075650279 40.19483249508618, -105.6782244408778 40.19458256772621, -105.6782341424972 40.19434313834616, -105.6782347793217 40.19432980353974, -105.6782519002093 40.19410310032079, -105.6782529398048 40.19409019359268, -105.6782742489293 40.19386989909211, -105.6782875275536 40.19356417239761, -105.6782485732217 40.19336613348817, -105.6781494802977 40.19314990804275, -105.6781414339438 40.1931326985922, -105.6780370489998 40.19289911524799, -105.6780297956547 40.1928819919292, -105.6779584459529 40.19267161911222, -105.6779532208666 40.19265495198785, -105.6778824219966 40.19233396648192, -105.677879096605 40.19231799622053, -105.6778530901214 40.19216014855787, -105.6778259574849 40.19203372650452, -105.6778234235607 40.1920181666116, -105.6778331188409 40.19186483292374, -105.6778347578226 40.19185297810984, -105.6779274774696 40.19168121408297, -105.6780466278303 40.19153206643568, -105.6781600304808 40.19136463031327, -105.6781519689368 40.19109901984651, -105.6780483550102 40.19096721548783, -105.6780341644516 40.19095039284954, -105.6779374023908 40.19082985643251, -105.6779258125981 40.19081283344089, -105.6778831211533 40.19062535816793, -105.6778806803566 40.19060991791348, -105.6779063544293 40.19041914381376, -105.6779083317913 40.19040736953217, -105.677971367463 40.1901881086194, -105.6780090548469 40.18971784405401, -105.6779019323254 40.18925666184236, -105.677765546384 40.18893325343011, -105.6777584028516 40.18891617134472, -105.6776926608927 40.18874264792856, -105.6775924744353 40.18855230766899, -105.6774687696009 40.18834147264181, -105.6773329173417 40.18814377739658, -105.6773211596643 40.18812653754374, -105.6772256809055 40.18797639568763, -105.6770380712492 40.18774144196102, -105.6770246010461 40.1877244559753, -105.6768426188331 40.18747682323465, -105.6766742782837 40.18730812405553, -105.6765065596637 40.18717919733659, -105.6764839112511 40.18716219017327, -105.6764829605575 40.18716147652353, -105.6763959415487 40.18710202448237, -105.6763308014061 40.18705804967441, -105.6760992185649 40.18689566223739, -105.6759303858499 40.18679373368499, -105.6758363636698 40.18673768635443, -105.6755581622642 40.18657711774318, -105.6754319340273 40.18652047142681, -105.6753559905684 40.18648750826154, -105.6751336758973 40.18639575841871, -105.</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
+      <c r="D21" t="n">
+        <v>29</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Ward Community Center</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>WARD</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1 Columbia St, Ward, CO 80481</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="L21" t="n">
+        <v>40.0733984409928</v>
+      </c>
+      <c r="M21" t="n">
+        <v>-105.506518983446</v>
+      </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>POINT (-105.506518983446 40.0733984409928)</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>